<commit_message>
Auto update photos 2025-11-26 09:46:42
</commit_message>
<xml_diff>
--- a/articles_summary.xlsx
+++ b/articles_summary.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Summary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,76 +441,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0026-2</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/0026-2/470.jpg,https://oleks-netizen.github.io/product-images/0026-2/471.jpg,https://oleks-netizen.github.io/product-images/0026-2/472.jpg,https://oleks-netizen.github.io/product-images/0026-2/473.jpg,https://oleks-netizen.github.io/product-images/0026-2/474.jpg</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>0026-3</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/0026-3/4648.jpg,https://oleks-netizen.github.io/product-images/0026-3/4649.jpg,https://oleks-netizen.github.io/product-images/0026-3/4650.jpg,https://oleks-netizen.github.io/product-images/0026-3/4651.jpg,https://oleks-netizen.github.io/product-images/0026-3/4652.jpg,https://oleks-netizen.github.io/product-images/0026-3/4653.jpg</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
           <t>005</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B2" t="inlineStr">
         <is>
           <t>https://oleks-netizen.github.io/product-images/005/2504.jpg,https://oleks-netizen.github.io/product-images/005/2505.jpg,https://oleks-netizen.github.io/product-images/005/2506.jpg,https://oleks-netizen.github.io/product-images/005/2507.jpg,https://oleks-netizen.github.io/product-images/005/2508.jpg,https://oleks-netizen.github.io/product-images/005/2509.jpg,https://oleks-netizen.github.io/product-images/005/2510.jpg</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="C2" t="n">
         <v>7</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>009-2</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/009-2/1144.jpg,https://oleks-netizen.github.io/product-images/009-2/1145.jpg,https://oleks-netizen.github.io/product-images/009-2/1146.jpg,https://oleks-netizen.github.io/product-images/009-2/1147.jpg,https://oleks-netizen.github.io/product-images/009-2/1148.jpg,https://oleks-netizen.github.io/product-images/009-2/1149.jpg</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>009-4</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/009-4/1769.jpg,https://oleks-netizen.github.io/product-images/009-4/1770.jpg,https://oleks-netizen.github.io/product-images/009-4/1771.jpg,https://oleks-netizen.github.io/product-images/009-4/1772.jpg,https://oleks-netizen.github.io/product-images/009-4/1773.jpg,https://oleks-netizen.github.io/product-images/009-4/1774.jpg</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update 2025-11-26 11:53:20
</commit_message>
<xml_diff>
--- a/articles_summary.xlsx
+++ b/articles_summary.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,33 +424,63 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Артикул</t>
+          <t>Article</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Посилання</t>
+          <t>Links</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Кількість фото</t>
+          <t>Count</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>005</t>
+          <t>7631-grey</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/005/2504.jpg,https://oleks-netizen.github.io/product-images/005/2505.jpg,https://oleks-netizen.github.io/product-images/005/2506.jpg,https://oleks-netizen.github.io/product-images/005/2507.jpg,https://oleks-netizen.github.io/product-images/005/2508.jpg,https://oleks-netizen.github.io/product-images/005/2509.jpg,https://oleks-netizen.github.io/product-images/005/2510.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/7631-grey/5081.jpg,https://oleks-netizen.github.io/product-images/7631-grey/5082.jpg,https://oleks-netizen.github.io/product-images/7631-grey/5083.jpg,https://oleks-netizen.github.io/product-images/7631-grey/5084.jpg,https://oleks-netizen.github.io/product-images/7631-grey/5085.jpg,https://oleks-netizen.github.io/product-images/7631-grey/5086.jpg,https://oleks-netizen.github.io/product-images/7631-grey/5087.jpg,https://oleks-netizen.github.io/product-images/7631-grey/5088.jpg,https://oleks-netizen.github.io/product-images/7631-grey/5089.jpg,https://oleks-netizen.github.io/product-images/7631-grey/5090.jpg</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>7683-black</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/7683-black/4183.jpg,https://oleks-netizen.github.io/product-images/7683-black/4185.jpg,https://oleks-netizen.github.io/product-images/7683-black/4186.jpg,https://oleks-netizen.github.io/product-images/7683-black/4187.jpg,https://oleks-netizen.github.io/product-images/7683-black/4188.jpg,https://oleks-netizen.github.io/product-images/7683-black/4189.jpg,https://oleks-netizen.github.io/product-images/7683-black/4190.jpg,https://oleks-netizen.github.io/product-images/7683-black/4191.jpg,https://oleks-netizen.github.io/product-images/7683-black/4192.jpg</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>7687-black</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/7687-black/1044.jpg,https://oleks-netizen.github.io/product-images/7687-black/1046.jpg,https://oleks-netizen.github.io/product-images/7687-black/1047.jpg,https://oleks-netizen.github.io/product-images/7687-black/1048.jpg,https://oleks-netizen.github.io/product-images/7687-black/1049.jpg,https://oleks-netizen.github.io/product-images/7687-black/1050.jpg,https://oleks-netizen.github.io/product-images/7687-black/1051.jpg,https://oleks-netizen.github.io/product-images/7687-black/1052.jpg,https://oleks-netizen.github.io/product-images/7687-black/1053.jpg</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update 2025-11-26 13:29:56
</commit_message>
<xml_diff>
--- a/articles_summary.xlsx
+++ b/articles_summary.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,63 +424,903 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Article</t>
+          <t>Артикул</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Links</t>
+          <t>Посилання</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Count</t>
+          <t>Кількість фото</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>7631-grey</t>
+          <t>3141A Вишнева</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/7631-grey/5081.jpg,https://oleks-netizen.github.io/product-images/7631-grey/5082.jpg,https://oleks-netizen.github.io/product-images/7631-grey/5083.jpg,https://oleks-netizen.github.io/product-images/7631-grey/5084.jpg,https://oleks-netizen.github.io/product-images/7631-grey/5085.jpg,https://oleks-netizen.github.io/product-images/7631-grey/5086.jpg,https://oleks-netizen.github.io/product-images/7631-grey/5087.jpg,https://oleks-netizen.github.io/product-images/7631-grey/5088.jpg,https://oleks-netizen.github.io/product-images/7631-grey/5089.jpg,https://oleks-netizen.github.io/product-images/7631-grey/5090.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/3141A Вишнева/407.jpg,https://oleks-netizen.github.io/product-images/3141A Вишнева/408.jpg,https://oleks-netizen.github.io/product-images/3141A Вишнева/409.jpg,https://oleks-netizen.github.io/product-images/3141A Вишнева/411.jpg,https://oleks-netizen.github.io/product-images/3141A Вишнева/412.jpg</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>7683-black</t>
+          <t>3141A Пурпурна</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/7683-black/4183.jpg,https://oleks-netizen.github.io/product-images/7683-black/4185.jpg,https://oleks-netizen.github.io/product-images/7683-black/4186.jpg,https://oleks-netizen.github.io/product-images/7683-black/4187.jpg,https://oleks-netizen.github.io/product-images/7683-black/4188.jpg,https://oleks-netizen.github.io/product-images/7683-black/4189.jpg,https://oleks-netizen.github.io/product-images/7683-black/4190.jpg,https://oleks-netizen.github.io/product-images/7683-black/4191.jpg,https://oleks-netizen.github.io/product-images/7683-black/4192.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/3141A Пурпурна/750.jpg,https://oleks-netizen.github.io/product-images/3141A Пурпурна/751.jpg,https://oleks-netizen.github.io/product-images/3141A Пурпурна/752.jpg,https://oleks-netizen.github.io/product-images/3141A Пурпурна/754.jpg,https://oleks-netizen.github.io/product-images/3141A Пурпурна/755.jpg</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>7687-black</t>
+          <t>3141A-1</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/7687-black/1044.jpg,https://oleks-netizen.github.io/product-images/7687-black/1046.jpg,https://oleks-netizen.github.io/product-images/7687-black/1047.jpg,https://oleks-netizen.github.io/product-images/7687-black/1048.jpg,https://oleks-netizen.github.io/product-images/7687-black/1049.jpg,https://oleks-netizen.github.io/product-images/7687-black/1050.jpg,https://oleks-netizen.github.io/product-images/7687-black/1051.jpg,https://oleks-netizen.github.io/product-images/7687-black/1052.jpg,https://oleks-netizen.github.io/product-images/7687-black/1053.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/3141A-1/5257.jpg,https://oleks-netizen.github.io/product-images/3141A-1/5258.jpg,https://oleks-netizen.github.io/product-images/3141A-1/5259.jpg,https://oleks-netizen.github.io/product-images/3141A-1/5261.jpg,https://oleks-netizen.github.io/product-images/3141A-1/5262.jpg,https://oleks-netizen.github.io/product-images/3141A-1/5265.jpg,https://oleks-netizen.github.io/product-images/3141A-1/5266.jpg</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>9</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>3148 Бордова</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3148 Бордова/1011.jpg,https://oleks-netizen.github.io/product-images/3148 Бордова/1012.jpg,https://oleks-netizen.github.io/product-images/3148 Бордова/1013.jpg,https://oleks-netizen.github.io/product-images/3148 Бордова/1015.jpg,https://oleks-netizen.github.io/product-images/3148 Бордова/1016.jpg</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>3148 Бузкова</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3148 Бузкова/174.jpg,https://oleks-netizen.github.io/product-images/3148 Бузкова/175.jpg,https://oleks-netizen.github.io/product-images/3148 Бузкова/176.jpg,https://oleks-netizen.github.io/product-images/3148 Бузкова/178.jpg,https://oleks-netizen.github.io/product-images/3148 Бузкова/179.jpg</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>3148 Жовта</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3148 Жовта/5894.jpg,https://oleks-netizen.github.io/product-images/3148 Жовта/5895.jpg,https://oleks-netizen.github.io/product-images/3148 Жовта/5896.jpg,https://oleks-netizen.github.io/product-images/3148 Жовта/5897.jpg,https://oleks-netizen.github.io/product-images/3148 Жовта/5898.jpg,https://oleks-netizen.github.io/product-images/3148 Жовта/5899.jpg,https://oleks-netizen.github.io/product-images/3148 Жовта/5900.jpg,https://oleks-netizen.github.io/product-images/3148 Жовта/5901.jpg,https://oleks-netizen.github.io/product-images/3148 Жовта/5902.jpg,https://oleks-netizen.github.io/product-images/3148 Жовта/5903.jpg</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>3148 Синя</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3148 Синя/6116.jpg,https://oleks-netizen.github.io/product-images/3148 Синя/6117.jpg,https://oleks-netizen.github.io/product-images/3148 Синя/6118.jpg,https://oleks-netizen.github.io/product-images/3148 Синя/6119.jpg,https://oleks-netizen.github.io/product-images/3148 Синя/6120.jpg,https://oleks-netizen.github.io/product-images/3148 Синя/6121.jpg,https://oleks-netizen.github.io/product-images/3148 Синя/6122.jpg,https://oleks-netizen.github.io/product-images/3148 Синя/6123.jpg,https://oleks-netizen.github.io/product-images/3148 Синя/6124.jpg,https://oleks-netizen.github.io/product-images/3148 Синя/6125.jpg</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>3148 Чорна</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3148 Чорна/3271.jpg,https://oleks-netizen.github.io/product-images/3148 Чорна/3272.jpg,https://oleks-netizen.github.io/product-images/3148 Чорна/3273.jpg,https://oleks-netizen.github.io/product-images/3148 Чорна/3274.jpg,https://oleks-netizen.github.io/product-images/3148 Чорна/3275.jpg,https://oleks-netizen.github.io/product-images/3148 Чорна/3276.jpg,https://oleks-netizen.github.io/product-images/3148 Чорна/3277.jpg,https://oleks-netizen.github.io/product-images/3148 Чорна/3278.jpg,https://oleks-netizen.github.io/product-images/3148 Чорна/3279.jpg,https://oleks-netizen.github.io/product-images/3148 Чорна/3280.jpg</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>3148-1</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3148-1/1412.jpg,https://oleks-netizen.github.io/product-images/3148-1/1413.jpg,https://oleks-netizen.github.io/product-images/3148-1/1414.jpg,https://oleks-netizen.github.io/product-images/3148-1/1415.jpg,https://oleks-netizen.github.io/product-images/3148-1/1416.jpg,https://oleks-netizen.github.io/product-images/3148-1/1417.jpg,https://oleks-netizen.github.io/product-images/3148-1/1418.jpg,https://oleks-netizen.github.io/product-images/3148-1/1419.jpg,https://oleks-netizen.github.io/product-images/3148-1/1420.jpg,https://oleks-netizen.github.io/product-images/3148-1/1421.jpg</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>3149 Paris</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3149 Paris/3008.jpg,https://oleks-netizen.github.io/product-images/3149 Paris/3009.jpg,https://oleks-netizen.github.io/product-images/3149 Paris/3010.jpg,https://oleks-netizen.github.io/product-images/3149 Paris/3011.jpg,https://oleks-netizen.github.io/product-images/3149 Paris/3012.jpg,https://oleks-netizen.github.io/product-images/3149 Paris/3013.jpg,https://oleks-netizen.github.io/product-images/3149 Paris/3014.jpg,https://oleks-netizen.github.io/product-images/3149 Paris/3015.jpg,https://oleks-netizen.github.io/product-images/3149 Paris/3016.jpg</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>3149 Ейфелева Вежа</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3149 Ейфелева Вежа/4878.jpg,https://oleks-netizen.github.io/product-images/3149 Ейфелева Вежа/4879.jpg,https://oleks-netizen.github.io/product-images/3149 Ейфелева Вежа/4880.jpg,https://oleks-netizen.github.io/product-images/3149 Ейфелева Вежа/4881.jpg,https://oleks-netizen.github.io/product-images/3149 Ейфелева Вежа/4882.jpg,https://oleks-netizen.github.io/product-images/3149 Ейфелева Вежа/4883.jpg,https://oleks-netizen.github.io/product-images/3149 Ейфелева Вежа/4884.jpg,https://oleks-netizen.github.io/product-images/3149 Ейфелева Вежа/4885.jpg</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>3149 Кіт</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3149 Кіт/640.jpg,https://oleks-netizen.github.io/product-images/3149 Кіт/641.jpg,https://oleks-netizen.github.io/product-images/3149 Кіт/642.jpg,https://oleks-netizen.github.io/product-images/3149 Кіт/643.jpg,https://oleks-netizen.github.io/product-images/3149 Кіт/644.jpg,https://oleks-netizen.github.io/product-images/3149 Кіт/645.jpg,https://oleks-netizen.github.io/product-images/3149 Кіт/646.jpg,https://oleks-netizen.github.io/product-images/3149 Кіт/647.jpg,https://oleks-netizen.github.io/product-images/3149 Кіт/648.jpg</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>3149 Кава в Парижі</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3149 Кава в Парижі/5019.jpg,https://oleks-netizen.github.io/product-images/3149 Кава в Парижі/5020.jpg,https://oleks-netizen.github.io/product-images/3149 Кава в Парижі/5021.jpg,https://oleks-netizen.github.io/product-images/3149 Кава в Парижі/5022.jpg,https://oleks-netizen.github.io/product-images/3149 Кава в Парижі/5023.jpg,https://oleks-netizen.github.io/product-images/3149 Кава в Парижі/5024.jpg,https://oleks-netizen.github.io/product-images/3149 Кава в Парижі/5025.jpg,https://oleks-netizen.github.io/product-images/3149 Кава в Парижі/5026.jpg,https://oleks-netizen.github.io/product-images/3149 Кава в Парижі/5027.jpg</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>3149 Слід</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3149 Слід/5808.jpg,https://oleks-netizen.github.io/product-images/3149 Слід/5809.jpg,https://oleks-netizen.github.io/product-images/3149 Слід/5810.jpg,https://oleks-netizen.github.io/product-images/3149 Слід/5811.jpg,https://oleks-netizen.github.io/product-images/3149 Слід/5812.jpg,https://oleks-netizen.github.io/product-images/3149 Слід/5813.jpg,https://oleks-netizen.github.io/product-images/3149 Слід/5814.jpg,https://oleks-netizen.github.io/product-images/3149 Слід/5815.jpg</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>3149-1</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3149-1/2024.jpg,https://oleks-netizen.github.io/product-images/3149-1/2025.jpg,https://oleks-netizen.github.io/product-images/3149-1/2026.jpg,https://oleks-netizen.github.io/product-images/3149-1/2027.jpg,https://oleks-netizen.github.io/product-images/3149-1/2028.jpg,https://oleks-netizen.github.io/product-images/3149-1/2029.jpg,https://oleks-netizen.github.io/product-images/3149-1/2030.jpg,https://oleks-netizen.github.io/product-images/3149-1/2031.jpg</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>3150 France</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3150 France/6150.jpg,https://oleks-netizen.github.io/product-images/3150 France/6151.jpg,https://oleks-netizen.github.io/product-images/3150 France/6152.jpg,https://oleks-netizen.github.io/product-images/3150 France/6153.jpg,https://oleks-netizen.github.io/product-images/3150 France/6154.jpg,https://oleks-netizen.github.io/product-images/3150 France/6155.jpg,https://oleks-netizen.github.io/product-images/3150 France/6156.jpg,https://oleks-netizen.github.io/product-images/3150 France/6157.jpg</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>3150 Paris</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3150 Paris/2825.jpg,https://oleks-netizen.github.io/product-images/3150 Paris/2826.jpg,https://oleks-netizen.github.io/product-images/3150 Paris/2827.jpg,https://oleks-netizen.github.io/product-images/3150 Paris/2828.jpg,https://oleks-netizen.github.io/product-images/3150 Paris/2829.jpg,https://oleks-netizen.github.io/product-images/3150 Paris/2830.jpg,https://oleks-netizen.github.io/product-images/3150 Paris/2831.jpg,https://oleks-netizen.github.io/product-images/3150 Paris/2832.jpg,https://oleks-netizen.github.io/product-images/3150 Paris/2833.jpg</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>3150 Прогулянка в Парижі</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3150 Прогулянка в Парижі/2015.jpg,https://oleks-netizen.github.io/product-images/3150 Прогулянка в Парижі/2016.jpg,https://oleks-netizen.github.io/product-images/3150 Прогулянка в Парижі/2017.jpg,https://oleks-netizen.github.io/product-images/3150 Прогулянка в Парижі/2018.jpg,https://oleks-netizen.github.io/product-images/3150 Прогулянка в Парижі/2019.jpg,https://oleks-netizen.github.io/product-images/3150 Прогулянка в Парижі/2020.jpg,https://oleks-netizen.github.io/product-images/3150 Прогулянка в Парижі/2021.jpg,https://oleks-netizen.github.io/product-images/3150 Прогулянка в Парижі/2022.jpg,https://oleks-netizen.github.io/product-images/3150 Прогулянка в Парижі/2023.jpg</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>3150 Сліди</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3150 Сліди/521.jpg,https://oleks-netizen.github.io/product-images/3150 Сліди/522.jpg,https://oleks-netizen.github.io/product-images/3150 Сліди/523.jpg,https://oleks-netizen.github.io/product-images/3150 Сліди/524.jpg,https://oleks-netizen.github.io/product-images/3150 Сліди/525.jpg,https://oleks-netizen.github.io/product-images/3150 Сліди/526.jpg,https://oleks-netizen.github.io/product-images/3150 Сліди/527.jpg,https://oleks-netizen.github.io/product-images/3150 Сліди/528.jpg,https://oleks-netizen.github.io/product-images/3150 Сліди/529.jpg</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>3150-1</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3150-1/4812.jpg,https://oleks-netizen.github.io/product-images/3150-1/4813.jpg,https://oleks-netizen.github.io/product-images/3150-1/4814.jpg,https://oleks-netizen.github.io/product-images/3150-1/4815.jpg,https://oleks-netizen.github.io/product-images/3150-1/4816.jpg,https://oleks-netizen.github.io/product-images/3150-1/4817.jpg,https://oleks-netizen.github.io/product-images/3150-1/4818.jpg,https://oleks-netizen.github.io/product-images/3150-1/4819.jpg,https://oleks-netizen.github.io/product-images/3150-1/4820.jpg</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>3225 Біла</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3225 Біла/1193.jpg,https://oleks-netizen.github.io/product-images/3225 Біла/1194.jpg,https://oleks-netizen.github.io/product-images/3225 Біла/1195.jpg,https://oleks-netizen.github.io/product-images/3225 Біла/1196.jpg,https://oleks-netizen.github.io/product-images/3225 Біла/1197.jpg,https://oleks-netizen.github.io/product-images/3225 Біла/1198.jpg,https://oleks-netizen.github.io/product-images/3225 Біла/1199.jpg,https://oleks-netizen.github.io/product-images/3225 Біла/1200.jpg,https://oleks-netizen.github.io/product-images/3225 Біла/1201.jpg</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>3225 Коралова</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3225 Коралова/669.jpg,https://oleks-netizen.github.io/product-images/3225 Коралова/670.jpg,https://oleks-netizen.github.io/product-images/3225 Коралова/671.jpg,https://oleks-netizen.github.io/product-images/3225 Коралова/672.jpg,https://oleks-netizen.github.io/product-images/3225 Коралова/673.jpg,https://oleks-netizen.github.io/product-images/3225 Коралова/674.jpg,https://oleks-netizen.github.io/product-images/3225 Коралова/675.jpg,https://oleks-netizen.github.io/product-images/3225 Коралова/676.jpg,https://oleks-netizen.github.io/product-images/3225 Коралова/677.jpg</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>3225 Кремова</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3225 Кремова/2692.jpg,https://oleks-netizen.github.io/product-images/3225 Кремова/2693.jpg,https://oleks-netizen.github.io/product-images/3225 Кремова/2694.jpg,https://oleks-netizen.github.io/product-images/3225 Кремова/2695.jpg,https://oleks-netizen.github.io/product-images/3225 Кремова/2696.jpg,https://oleks-netizen.github.io/product-images/3225 Кремова/2697.jpg,https://oleks-netizen.github.io/product-images/3225 Кремова/2698.jpg,https://oleks-netizen.github.io/product-images/3225 Кремова/2699.jpg,https://oleks-netizen.github.io/product-images/3225 Кремова/2700.jpg</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>3225 Сіро-блакитна</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3225 Сіро-блакитна/5120.jpg,https://oleks-netizen.github.io/product-images/3225 Сіро-блакитна/5121.jpg,https://oleks-netizen.github.io/product-images/3225 Сіро-блакитна/5122.jpg,https://oleks-netizen.github.io/product-images/3225 Сіро-блакитна/5123.jpg,https://oleks-netizen.github.io/product-images/3225 Сіро-блакитна/5124.jpg,https://oleks-netizen.github.io/product-images/3225 Сіро-блакитна/5125.jpg,https://oleks-netizen.github.io/product-images/3225 Сіро-блакитна/5126.jpg,https://oleks-netizen.github.io/product-images/3225 Сіро-блакитна/5127.jpg,https://oleks-netizen.github.io/product-images/3225 Сіро-блакитна/5128.jpg</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>3225 Синя</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3225 Синя/5867.jpg,https://oleks-netizen.github.io/product-images/3225 Синя/5868.jpg,https://oleks-netizen.github.io/product-images/3225 Синя/5869.jpg,https://oleks-netizen.github.io/product-images/3225 Синя/5870.jpg,https://oleks-netizen.github.io/product-images/3225 Синя/5871.jpg,https://oleks-netizen.github.io/product-images/3225 Синя/5872.jpg,https://oleks-netizen.github.io/product-images/3225 Синя/5873.jpg,https://oleks-netizen.github.io/product-images/3225 Синя/5874.jpg,https://oleks-netizen.github.io/product-images/3225 Синя/5875.jpg</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>3225 Фіолетова</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3225 Фіолетова/3700.jpg,https://oleks-netizen.github.io/product-images/3225 Фіолетова/3701.jpg,https://oleks-netizen.github.io/product-images/3225 Фіолетова/3702.jpg,https://oleks-netizen.github.io/product-images/3225 Фіолетова/3703.jpg,https://oleks-netizen.github.io/product-images/3225 Фіолетова/3704.jpg,https://oleks-netizen.github.io/product-images/3225 Фіолетова/3705.jpg,https://oleks-netizen.github.io/product-images/3225 Фіолетова/3706.jpg,https://oleks-netizen.github.io/product-images/3225 Фіолетова/3707.jpg,https://oleks-netizen.github.io/product-images/3225 Фіолетова/3708.jpg</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>3226 Paris</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3226 Paris/1974.jpg,https://oleks-netizen.github.io/product-images/3226 Paris/1975.jpg,https://oleks-netizen.github.io/product-images/3226 Paris/1976.jpg,https://oleks-netizen.github.io/product-images/3226 Paris/1977.jpg,https://oleks-netizen.github.io/product-images/3226 Paris/1978.jpg,https://oleks-netizen.github.io/product-images/3226 Paris/1979.jpg,https://oleks-netizen.github.io/product-images/3226 Paris/1980.jpg,https://oleks-netizen.github.io/product-images/3226 Paris/1981.jpg,https://oleks-netizen.github.io/product-images/3226 Paris/1982.jpg</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>3226 Зірки</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3226 Зірки/5825.jpg,https://oleks-netizen.github.io/product-images/3226 Зірки/5826.jpg,https://oleks-netizen.github.io/product-images/3226 Зірки/5827.jpg,https://oleks-netizen.github.io/product-images/3226 Зірки/5828.jpg,https://oleks-netizen.github.io/product-images/3226 Зірки/5829.jpg,https://oleks-netizen.github.io/product-images/3226 Зірки/5830.jpg,https://oleks-netizen.github.io/product-images/3226 Зірки/5831.jpg,https://oleks-netizen.github.io/product-images/3226 Зірки/5832.jpg,https://oleks-netizen.github.io/product-images/3226 Зірки/5833.jpg</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>3226 Кіт</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3226 Кіт/879.jpg,https://oleks-netizen.github.io/product-images/3226 Кіт/880.jpg,https://oleks-netizen.github.io/product-images/3226 Кіт/881.jpg,https://oleks-netizen.github.io/product-images/3226 Кіт/882.jpg,https://oleks-netizen.github.io/product-images/3226 Кіт/883.jpg,https://oleks-netizen.github.io/product-images/3226 Кіт/884.jpg,https://oleks-netizen.github.io/product-images/3226 Кіт/885.jpg,https://oleks-netizen.github.io/product-images/3226 Кіт/886.jpg</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>3226 Місто</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3226 Місто/2006.jpg,https://oleks-netizen.github.io/product-images/3226 Місто/2007.jpg,https://oleks-netizen.github.io/product-images/3226 Місто/2008.jpg,https://oleks-netizen.github.io/product-images/3226 Місто/2009.jpg,https://oleks-netizen.github.io/product-images/3226 Місто/2010.jpg,https://oleks-netizen.github.io/product-images/3226 Місто/2011.jpg,https://oleks-netizen.github.io/product-images/3226 Місто/2012.jpg,https://oleks-netizen.github.io/product-images/3226 Місто/2013.jpg,https://oleks-netizen.github.io/product-images/3226 Місто/2014.jpg</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>3226 Сніг</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3226 Сніг/1711.jpg,https://oleks-netizen.github.io/product-images/3226 Сніг/1712.jpg,https://oleks-netizen.github.io/product-images/3226 Сніг/1713.jpg,https://oleks-netizen.github.io/product-images/3226 Сніг/1714.jpg,https://oleks-netizen.github.io/product-images/3226 Сніг/1715.jpg,https://oleks-netizen.github.io/product-images/3226 Сніг/1716.jpg,https://oleks-netizen.github.io/product-images/3226 Сніг/1717.jpg,https://oleks-netizen.github.io/product-images/3226 Сніг/1718.jpg,https://oleks-netizen.github.io/product-images/3226 Сніг/1719.jpg</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>3226 Сяйво</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3226 Сяйво/5668.jpg,https://oleks-netizen.github.io/product-images/3226 Сяйво/5669.jpg,https://oleks-netizen.github.io/product-images/3226 Сяйво/5670.jpg,https://oleks-netizen.github.io/product-images/3226 Сяйво/5671.jpg,https://oleks-netizen.github.io/product-images/3226 Сяйво/5672.jpg,https://oleks-netizen.github.io/product-images/3226 Сяйво/5673.jpg,https://oleks-netizen.github.io/product-images/3226 Сяйво/5674.jpg,https://oleks-netizen.github.io/product-images/3226 Сяйво/5675.jpg,https://oleks-netizen.github.io/product-images/3226 Сяйво/5676.jpg</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>3305 Бордова</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3305 Бордова/4511.jpg,https://oleks-netizen.github.io/product-images/3305 Бордова/4512.jpg,https://oleks-netizen.github.io/product-images/3305 Бордова/4513.jpg,https://oleks-netizen.github.io/product-images/3305 Бордова/4514.jpg,https://oleks-netizen.github.io/product-images/3305 Бордова/4515.jpg</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>3305 Вишнева</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3305 Вишнева/2756.jpg,https://oleks-netizen.github.io/product-images/3305 Вишнева/2757.jpg,https://oleks-netizen.github.io/product-images/3305 Вишнева/2758.jpg,https://oleks-netizen.github.io/product-images/3305 Вишнева/2759.jpg,https://oleks-netizen.github.io/product-images/3305 Вишнева/2760.jpg</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>3305 Червона</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3305 Червона/4483.jpg,https://oleks-netizen.github.io/product-images/3305 Червона/4484.jpg,https://oleks-netizen.github.io/product-images/3305 Червона/4485.jpg,https://oleks-netizen.github.io/product-images/3305 Червона/4486.jpg,https://oleks-netizen.github.io/product-images/3305 Червона/4487.jpg</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>3306A Біла</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3306A Біла/2544.jpg,https://oleks-netizen.github.io/product-images/3306A Біла/2545.jpg,https://oleks-netizen.github.io/product-images/3306A Біла/2546.jpg,https://oleks-netizen.github.io/product-images/3306A Біла/2547.jpg,https://oleks-netizen.github.io/product-images/3306A Біла/2548.jpg,https://oleks-netizen.github.io/product-images/3306A Біла/2549.jpg,https://oleks-netizen.github.io/product-images/3306A Біла/2550.jpg,https://oleks-netizen.github.io/product-images/3306A Біла/2551.jpg,https://oleks-netizen.github.io/product-images/3306A Біла/2552.jpg</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>3306A Бордова</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3306A Бордова/4622.jpg,https://oleks-netizen.github.io/product-images/3306A Бордова/4623.jpg,https://oleks-netizen.github.io/product-images/3306A Бордова/4624.jpg,https://oleks-netizen.github.io/product-images/3306A Бордова/4625.jpg,https://oleks-netizen.github.io/product-images/3306A Бордова/4626.jpg,https://oleks-netizen.github.io/product-images/3306A Бордова/4627.jpg,https://oleks-netizen.github.io/product-images/3306A Бордова/4628.jpg,https://oleks-netizen.github.io/product-images/3306A Бордова/4629.jpg,https://oleks-netizen.github.io/product-images/3306A Бордова/4630.jpg</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>3306A Сіра</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3306A Сіра/5215.jpg,https://oleks-netizen.github.io/product-images/3306A Сіра/5216.jpg,https://oleks-netizen.github.io/product-images/3306A Сіра/5217.jpg,https://oleks-netizen.github.io/product-images/3306A Сіра/5218.jpg,https://oleks-netizen.github.io/product-images/3306A Сіра/5219.jpg,https://oleks-netizen.github.io/product-images/3306A Сіра/5220.jpg,https://oleks-netizen.github.io/product-images/3306A Сіра/5221.jpg,https://oleks-netizen.github.io/product-images/3306A Сіра/5222.jpg,https://oleks-netizen.github.io/product-images/3306A Сіра/5223.jpg</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>3306A Синя</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3306A Синя/4206.jpg,https://oleks-netizen.github.io/product-images/3306A Синя/4207.jpg,https://oleks-netizen.github.io/product-images/3306A Синя/4208.jpg,https://oleks-netizen.github.io/product-images/3306A Синя/4209.jpg,https://oleks-netizen.github.io/product-images/3306A Синя/4210.jpg,https://oleks-netizen.github.io/product-images/3306A Синя/4211.jpg,https://oleks-netizen.github.io/product-images/3306A Синя/4212.jpg,https://oleks-netizen.github.io/product-images/3306A Синя/4213.jpg</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>3306A Червона</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3306A Червона/832.jpg,https://oleks-netizen.github.io/product-images/3306A Червона/833.jpg,https://oleks-netizen.github.io/product-images/3306A Червона/834.jpg,https://oleks-netizen.github.io/product-images/3306A Червона/835.jpg,https://oleks-netizen.github.io/product-images/3306A Червона/836.jpg,https://oleks-netizen.github.io/product-images/3306A Червона/837.jpg,https://oleks-netizen.github.io/product-images/3306A Червона/838.jpg,https://oleks-netizen.github.io/product-images/3306A Червона/839.jpg,https://oleks-netizen.github.io/product-images/3306A Червона/840.jpg</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>3306A Чорний</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/3306A Чорний/5134.jpg,https://oleks-netizen.github.io/product-images/3306A Чорний/5135.jpg,https://oleks-netizen.github.io/product-images/3306A Чорний/5136.jpg,https://oleks-netizen.github.io/product-images/3306A Чорний/5137.jpg,https://oleks-netizen.github.io/product-images/3306A Чорний/5138.jpg,https://oleks-netizen.github.io/product-images/3306A Чорний/5139.jpg,https://oleks-netizen.github.io/product-images/3306A Чорний/5140.jpg,https://oleks-netizen.github.io/product-images/3306A Чорний/5141.jpg,https://oleks-netizen.github.io/product-images/3306A Чорний/5142.jpg</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>5302A Біла</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/5302A Біла/92.jpg,https://oleks-netizen.github.io/product-images/5302A Біла/93.jpg,https://oleks-netizen.github.io/product-images/5302A Біла/94.jpg,https://oleks-netizen.github.io/product-images/5302A Біла/95.jpg,https://oleks-netizen.github.io/product-images/5302A Біла/96.jpg,https://oleks-netizen.github.io/product-images/5302A Біла/97.jpg,https://oleks-netizen.github.io/product-images/5302A Біла/98.jpg,https://oleks-netizen.github.io/product-images/5302A Біла/99.jpg</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>5302A Бежева</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/5302A Бежева/1644.jpg,https://oleks-netizen.github.io/product-images/5302A Бежева/1645.jpg,https://oleks-netizen.github.io/product-images/5302A Бежева/1646.jpg,https://oleks-netizen.github.io/product-images/5302A Бежева/1647.jpg,https://oleks-netizen.github.io/product-images/5302A Бежева/1648.jpg,https://oleks-netizen.github.io/product-images/5302A Бежева/1649.jpg,https://oleks-netizen.github.io/product-images/5302A Бежева/1650.jpg,https://oleks-netizen.github.io/product-images/5302A Бежева/1651.jpg,https://oleks-netizen.github.io/product-images/5302A Бежева/1652.jpg</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>5302A Кольорова</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/5302A Кольорова/3662.jpg,https://oleks-netizen.github.io/product-images/5302A Кольорова/3663.jpg,https://oleks-netizen.github.io/product-images/5302A Кольорова/3664.jpg,https://oleks-netizen.github.io/product-images/5302A Кольорова/3665.jpg,https://oleks-netizen.github.io/product-images/5302A Кольорова/3666.jpg,https://oleks-netizen.github.io/product-images/5302A Кольорова/3667.jpg,https://oleks-netizen.github.io/product-images/5302A Кольорова/3668.jpg,https://oleks-netizen.github.io/product-images/5302A Кольорова/3669.jpg,https://oleks-netizen.github.io/product-images/5302A Кольорова/3670.jpg</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>5302A Синя</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/5302A Синя/3723.jpg,https://oleks-netizen.github.io/product-images/5302A Синя/3724.jpg,https://oleks-netizen.github.io/product-images/5302A Синя/3725.jpg,https://oleks-netizen.github.io/product-images/5302A Синя/3726.jpg,https://oleks-netizen.github.io/product-images/5302A Синя/3727.jpg,https://oleks-netizen.github.io/product-images/5302A Синя/3728.jpg,https://oleks-netizen.github.io/product-images/5302A Синя/3729.jpg,https://oleks-netizen.github.io/product-images/5302A Синя/3730.jpg,https://oleks-netizen.github.io/product-images/5302A Синя/3731.jpg</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>5302A Чорна</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/5302A Чорна/5241.jpg,https://oleks-netizen.github.io/product-images/5302A Чорна/5242.jpg,https://oleks-netizen.github.io/product-images/5302A Чорна/5243.jpg,https://oleks-netizen.github.io/product-images/5302A Чорна/5244.jpg,https://oleks-netizen.github.io/product-images/5302A Чорна/5245.jpg,https://oleks-netizen.github.io/product-images/5302A Чорна/5246.jpg,https://oleks-netizen.github.io/product-images/5302A Чорна/5247.jpg,https://oleks-netizen.github.io/product-images/5302A Чорна/5248.jpg,https://oleks-netizen.github.io/product-images/5302A Чорна/5249.jpg</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>5302A Чорно-біла</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/5302A Чорно-біла/849.jpg,https://oleks-netizen.github.io/product-images/5302A Чорно-біла/850.jpg,https://oleks-netizen.github.io/product-images/5302A Чорно-біла/851.jpg,https://oleks-netizen.github.io/product-images/5302A Чорно-біла/852.jpg,https://oleks-netizen.github.io/product-images/5302A Чорно-біла/853.jpg,https://oleks-netizen.github.io/product-images/5302A Чорно-біла/854.jpg,https://oleks-netizen.github.io/product-images/5302A Чорно-біла/855.jpg,https://oleks-netizen.github.io/product-images/5302A Чорно-біла/856.jpg</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>BV38171-1</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/BV38171-1/1396.jpg,https://oleks-netizen.github.io/product-images/BV38171-1/1397.jpg,https://oleks-netizen.github.io/product-images/BV38171-1/1398.jpg,https://oleks-netizen.github.io/product-images/BV38171-1/1399.jpg,https://oleks-netizen.github.io/product-images/BV38171-1/1400.jpg,https://oleks-netizen.github.io/product-images/BV38171-1/1401.jpg,https://oleks-netizen.github.io/product-images/BV38171-1/1402.jpg,https://oleks-netizen.github.io/product-images/BV38171-1/1403.jpg</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>BV38319-143</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/BV38319-143/1165.jpg,https://oleks-netizen.github.io/product-images/BV38319-143/1166.jpg,https://oleks-netizen.github.io/product-images/BV38319-143/1167.jpg,https://oleks-netizen.github.io/product-images/BV38319-143/1168.jpg,https://oleks-netizen.github.io/product-images/BV38319-143/1169.jpg,https://oleks-netizen.github.io/product-images/BV38319-143/1170.jpg</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>BV38321-1</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/BV38321-1/3655.jpg,https://oleks-netizen.github.io/product-images/BV38321-1/3656.jpg,https://oleks-netizen.github.io/product-images/BV38321-1/3657.jpg,https://oleks-netizen.github.io/product-images/BV38321-1/3658.jpg,https://oleks-netizen.github.io/product-images/BV38321-1/3659.jpg,https://oleks-netizen.github.io/product-images/BV38321-1/3660.jpg,https://oleks-netizen.github.io/product-images/BV38321-1/3661.jpg</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>BV38345-150</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/BV38345-150/655.jpg,https://oleks-netizen.github.io/product-images/BV38345-150/656.jpg,https://oleks-netizen.github.io/product-images/BV38345-150/657.jpg,https://oleks-netizen.github.io/product-images/BV38345-150/658.jpg,https://oleks-netizen.github.io/product-images/BV38345-150/659.jpg,https://oleks-netizen.github.io/product-images/BV38345-150/660.jpg</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>BV38345-210</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/BV38345-210/1745.jpg,https://oleks-netizen.github.io/product-images/BV38345-210/1746.jpg,https://oleks-netizen.github.io/product-images/BV38345-210/1747.jpg,https://oleks-netizen.github.io/product-images/BV38345-210/1748.jpg,https://oleks-netizen.github.io/product-images/BV38345-210/1749.jpg,https://oleks-netizen.github.io/product-images/BV38345-210/1750.jpg,https://oleks-netizen.github.io/product-images/BV38345-210/1751.jpg</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>BV38348-1</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/BV38348-1/207.jpg,https://oleks-netizen.github.io/product-images/BV38348-1/208.jpg,https://oleks-netizen.github.io/product-images/BV38348-1/209.jpg,https://oleks-netizen.github.io/product-images/BV38348-1/210.jpg,https://oleks-netizen.github.io/product-images/BV38348-1/211.jpg,https://oleks-netizen.github.io/product-images/BV38348-1/212.jpg,https://oleks-netizen.github.io/product-images/BV38348-1/213.jpg</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>BV38363-100</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/BV38363-100/810.jpg,https://oleks-netizen.github.io/product-images/BV38363-100/811.jpg,https://oleks-netizen.github.io/product-images/BV38363-100/812.jpg,https://oleks-netizen.github.io/product-images/BV38363-100/813.jpg,https://oleks-netizen.github.io/product-images/BV38363-100/814.jpg,https://oleks-netizen.github.io/product-images/BV38363-100/815.jpg</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>BV38363-143</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/BV38363-143/5955.jpg,https://oleks-netizen.github.io/product-images/BV38363-143/5956.jpg,https://oleks-netizen.github.io/product-images/BV38363-143/5957.jpg,https://oleks-netizen.github.io/product-images/BV38363-143/5958.jpg,https://oleks-netizen.github.io/product-images/BV38363-143/5959.jpg,https://oleks-netizen.github.io/product-images/BV38363-143/5960.jpg,https://oleks-netizen.github.io/product-images/BV38363-143/5961.jpg</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>BV38601-153</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/BV38601-153/5649.jpg,https://oleks-netizen.github.io/product-images/BV38601-153/5650.jpg,https://oleks-netizen.github.io/product-images/BV38601-153/5651.jpg,https://oleks-netizen.github.io/product-images/BV38601-153/5652.jpg,https://oleks-netizen.github.io/product-images/BV38601-153/5653.jpg,https://oleks-netizen.github.io/product-images/BV38601-153/5654.jpg</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>BV38601-2803</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/BV38601-2803/2790.jpg,https://oleks-netizen.github.io/product-images/BV38601-2803/2791.jpg,https://oleks-netizen.github.io/product-images/BV38601-2803/2792.jpg,https://oleks-netizen.github.io/product-images/BV38601-2803/2793.jpg,https://oleks-netizen.github.io/product-images/BV38601-2803/2794.jpg,https://oleks-netizen.github.io/product-images/BV38601-2803/2795.jpg</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>BV38629-100</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/BV38629-100/1829.jpg,https://oleks-netizen.github.io/product-images/BV38629-100/1830.jpg,https://oleks-netizen.github.io/product-images/BV38629-100/1831.jpg,https://oleks-netizen.github.io/product-images/BV38629-100/1832.jpg,https://oleks-netizen.github.io/product-images/BV38629-100/1833.jpg,https://oleks-netizen.github.io/product-images/BV38629-100/1834.jpg,https://oleks-netizen.github.io/product-images/BV38629-100/1835.jpg,https://oleks-netizen.github.io/product-images/BV38629-100/1836.jpg</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>BV38643-1</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/BV38643-1/6005.jpg,https://oleks-netizen.github.io/product-images/BV38643-1/6006.jpg,https://oleks-netizen.github.io/product-images/BV38643-1/6007.jpg,https://oleks-netizen.github.io/product-images/BV38643-1/6008.jpg,https://oleks-netizen.github.io/product-images/BV38643-1/6009.jpg,https://oleks-netizen.github.io/product-images/BV38643-1/6010.jpg,https://oleks-netizen.github.io/product-images/BV38643-1/6011.jpg</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update 2025-11-26 15:02:36
</commit_message>
<xml_diff>
--- a/articles_summary.xlsx
+++ b/articles_summary.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:C159"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,12 +441,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>3141A Вишнева</t>
+          <t>0026-2</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3141A Вишнева/407.jpg,https://oleks-netizen.github.io/product-images/3141A Вишнева/408.jpg,https://oleks-netizen.github.io/product-images/3141A Вишнева/409.jpg,https://oleks-netizen.github.io/product-images/3141A Вишнева/411.jpg,https://oleks-netizen.github.io/product-images/3141A Вишнева/412.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/0026-2/470.jpg,https://oleks-netizen.github.io/product-images/0026-2/471.jpg,https://oleks-netizen.github.io/product-images/0026-2/472.jpg,https://oleks-netizen.github.io/product-images/0026-2/473.jpg,https://oleks-netizen.github.io/product-images/0026-2/474.jpg</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -456,147 +456,147 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>3141A Пурпурна</t>
+          <t>0026-3</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3141A Пурпурна/750.jpg,https://oleks-netizen.github.io/product-images/3141A Пурпурна/751.jpg,https://oleks-netizen.github.io/product-images/3141A Пурпурна/752.jpg,https://oleks-netizen.github.io/product-images/3141A Пурпурна/754.jpg,https://oleks-netizen.github.io/product-images/3141A Пурпурна/755.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/0026-3/4648.jpg,https://oleks-netizen.github.io/product-images/0026-3/4649.jpg,https://oleks-netizen.github.io/product-images/0026-3/4650.jpg,https://oleks-netizen.github.io/product-images/0026-3/4651.jpg,https://oleks-netizen.github.io/product-images/0026-3/4652.jpg,https://oleks-netizen.github.io/product-images/0026-3/4653.jpg</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3141A-1</t>
+          <t>0026-4</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3141A-1/5257.jpg,https://oleks-netizen.github.io/product-images/3141A-1/5258.jpg,https://oleks-netizen.github.io/product-images/3141A-1/5259.jpg,https://oleks-netizen.github.io/product-images/3141A-1/5261.jpg,https://oleks-netizen.github.io/product-images/3141A-1/5262.jpg,https://oleks-netizen.github.io/product-images/3141A-1/5265.jpg,https://oleks-netizen.github.io/product-images/3141A-1/5266.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/0026-4/2038.jpg,https://oleks-netizen.github.io/product-images/0026-4/2039.jpg,https://oleks-netizen.github.io/product-images/0026-4/2040.jpg,https://oleks-netizen.github.io/product-images/0026-4/2041.jpg,https://oleks-netizen.github.io/product-images/0026-4/2042.jpg,https://oleks-netizen.github.io/product-images/0026-4/2043.jpg</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3148 Бордова</t>
+          <t>0026-5</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3148 Бордова/1011.jpg,https://oleks-netizen.github.io/product-images/3148 Бордова/1012.jpg,https://oleks-netizen.github.io/product-images/3148 Бордова/1013.jpg,https://oleks-netizen.github.io/product-images/3148 Бордова/1015.jpg,https://oleks-netizen.github.io/product-images/3148 Бордова/1016.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/0026-5/4516.jpg,https://oleks-netizen.github.io/product-images/0026-5/4517.jpg,https://oleks-netizen.github.io/product-images/0026-5/4518.jpg,https://oleks-netizen.github.io/product-images/0026-5/4519.jpg,https://oleks-netizen.github.io/product-images/0026-5/4520.jpg,https://oleks-netizen.github.io/product-images/0026-5/4521.jpg</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>3148 Бузкова</t>
+          <t>0026-6</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3148 Бузкова/174.jpg,https://oleks-netizen.github.io/product-images/3148 Бузкова/175.jpg,https://oleks-netizen.github.io/product-images/3148 Бузкова/176.jpg,https://oleks-netizen.github.io/product-images/3148 Бузкова/178.jpg,https://oleks-netizen.github.io/product-images/3148 Бузкова/179.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/0026-6/3717.jpg,https://oleks-netizen.github.io/product-images/0026-6/3718.jpg,https://oleks-netizen.github.io/product-images/0026-6/3719.jpg,https://oleks-netizen.github.io/product-images/0026-6/3720.jpg,https://oleks-netizen.github.io/product-images/0026-6/3721.jpg,https://oleks-netizen.github.io/product-images/0026-6/3722.jpg</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>3148 Жовта</t>
+          <t>0026-7</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3148 Жовта/5894.jpg,https://oleks-netizen.github.io/product-images/3148 Жовта/5895.jpg,https://oleks-netizen.github.io/product-images/3148 Жовта/5896.jpg,https://oleks-netizen.github.io/product-images/3148 Жовта/5897.jpg,https://oleks-netizen.github.io/product-images/3148 Жовта/5898.jpg,https://oleks-netizen.github.io/product-images/3148 Жовта/5899.jpg,https://oleks-netizen.github.io/product-images/3148 Жовта/5900.jpg,https://oleks-netizen.github.io/product-images/3148 Жовта/5901.jpg,https://oleks-netizen.github.io/product-images/3148 Жовта/5902.jpg,https://oleks-netizen.github.io/product-images/3148 Жовта/5903.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/0026-7/543.jpg,https://oleks-netizen.github.io/product-images/0026-7/544.jpg,https://oleks-netizen.github.io/product-images/0026-7/545.jpg,https://oleks-netizen.github.io/product-images/0026-7/546.jpg,https://oleks-netizen.github.io/product-images/0026-7/547.jpg,https://oleks-netizen.github.io/product-images/0026-7/548.jpg</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>3148 Синя</t>
+          <t>0039-3</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3148 Синя/6116.jpg,https://oleks-netizen.github.io/product-images/3148 Синя/6117.jpg,https://oleks-netizen.github.io/product-images/3148 Синя/6118.jpg,https://oleks-netizen.github.io/product-images/3148 Синя/6119.jpg,https://oleks-netizen.github.io/product-images/3148 Синя/6120.jpg,https://oleks-netizen.github.io/product-images/3148 Синя/6121.jpg,https://oleks-netizen.github.io/product-images/3148 Синя/6122.jpg,https://oleks-netizen.github.io/product-images/3148 Синя/6123.jpg,https://oleks-netizen.github.io/product-images/3148 Синя/6124.jpg,https://oleks-netizen.github.io/product-images/3148 Синя/6125.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/0039-3/5398.jpg,https://oleks-netizen.github.io/product-images/0039-3/5399.jpg,https://oleks-netizen.github.io/product-images/0039-3/5400.jpg,https://oleks-netizen.github.io/product-images/0039-3/5401.jpg,https://oleks-netizen.github.io/product-images/0039-3/5402.jpg,https://oleks-netizen.github.io/product-images/0039-3/5403.jpg</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>3148 Чорна</t>
+          <t>005</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3148 Чорна/3271.jpg,https://oleks-netizen.github.io/product-images/3148 Чорна/3272.jpg,https://oleks-netizen.github.io/product-images/3148 Чорна/3273.jpg,https://oleks-netizen.github.io/product-images/3148 Чорна/3274.jpg,https://oleks-netizen.github.io/product-images/3148 Чорна/3275.jpg,https://oleks-netizen.github.io/product-images/3148 Чорна/3276.jpg,https://oleks-netizen.github.io/product-images/3148 Чорна/3277.jpg,https://oleks-netizen.github.io/product-images/3148 Чорна/3278.jpg,https://oleks-netizen.github.io/product-images/3148 Чорна/3279.jpg,https://oleks-netizen.github.io/product-images/3148 Чорна/3280.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/005/2504.jpg,https://oleks-netizen.github.io/product-images/005/2505.jpg,https://oleks-netizen.github.io/product-images/005/2506.jpg,https://oleks-netizen.github.io/product-images/005/2507.jpg,https://oleks-netizen.github.io/product-images/005/2508.jpg,https://oleks-netizen.github.io/product-images/005/2509.jpg,https://oleks-netizen.github.io/product-images/005/2510.jpg</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>3148-1</t>
+          <t>009-2</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3148-1/1412.jpg,https://oleks-netizen.github.io/product-images/3148-1/1413.jpg,https://oleks-netizen.github.io/product-images/3148-1/1414.jpg,https://oleks-netizen.github.io/product-images/3148-1/1415.jpg,https://oleks-netizen.github.io/product-images/3148-1/1416.jpg,https://oleks-netizen.github.io/product-images/3148-1/1417.jpg,https://oleks-netizen.github.io/product-images/3148-1/1418.jpg,https://oleks-netizen.github.io/product-images/3148-1/1419.jpg,https://oleks-netizen.github.io/product-images/3148-1/1420.jpg,https://oleks-netizen.github.io/product-images/3148-1/1421.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/009-2/1144.jpg,https://oleks-netizen.github.io/product-images/009-2/1145.jpg,https://oleks-netizen.github.io/product-images/009-2/1146.jpg,https://oleks-netizen.github.io/product-images/009-2/1147.jpg,https://oleks-netizen.github.io/product-images/009-2/1148.jpg,https://oleks-netizen.github.io/product-images/009-2/1149.jpg</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>3149 Paris</t>
+          <t>009-4</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3149 Paris/3008.jpg,https://oleks-netizen.github.io/product-images/3149 Paris/3009.jpg,https://oleks-netizen.github.io/product-images/3149 Paris/3010.jpg,https://oleks-netizen.github.io/product-images/3149 Paris/3011.jpg,https://oleks-netizen.github.io/product-images/3149 Paris/3012.jpg,https://oleks-netizen.github.io/product-images/3149 Paris/3013.jpg,https://oleks-netizen.github.io/product-images/3149 Paris/3014.jpg,https://oleks-netizen.github.io/product-images/3149 Paris/3015.jpg,https://oleks-netizen.github.io/product-images/3149 Paris/3016.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/009-4/1769.jpg,https://oleks-netizen.github.io/product-images/009-4/1770.jpg,https://oleks-netizen.github.io/product-images/009-4/1771.jpg,https://oleks-netizen.github.io/product-images/009-4/1772.jpg,https://oleks-netizen.github.io/product-images/009-4/1773.jpg,https://oleks-netizen.github.io/product-images/009-4/1774.jpg</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>3149 Ейфелева Вежа</t>
+          <t>1809-black</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3149 Ейфелева Вежа/4878.jpg,https://oleks-netizen.github.io/product-images/3149 Ейфелева Вежа/4879.jpg,https://oleks-netizen.github.io/product-images/3149 Ейфелева Вежа/4880.jpg,https://oleks-netizen.github.io/product-images/3149 Ейфелева Вежа/4881.jpg,https://oleks-netizen.github.io/product-images/3149 Ейфелева Вежа/4882.jpg,https://oleks-netizen.github.io/product-images/3149 Ейфелева Вежа/4883.jpg,https://oleks-netizen.github.io/product-images/3149 Ейфелева Вежа/4884.jpg,https://oleks-netizen.github.io/product-images/3149 Ейфелева Вежа/4885.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/1809-black/5770.jpg,https://oleks-netizen.github.io/product-images/1809-black/5771.jpg,https://oleks-netizen.github.io/product-images/1809-black/5772.jpg,https://oleks-netizen.github.io/product-images/1809-black/5773.jpg,https://oleks-netizen.github.io/product-images/1809-black/5774.jpg,https://oleks-netizen.github.io/product-images/1809-black/5775.jpg,https://oleks-netizen.github.io/product-images/1809-black/5776.jpg,https://oleks-netizen.github.io/product-images/1809-black/5777.jpg</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -606,57 +606,57 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>3149 Кіт</t>
+          <t>1809-grey</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3149 Кіт/640.jpg,https://oleks-netizen.github.io/product-images/3149 Кіт/641.jpg,https://oleks-netizen.github.io/product-images/3149 Кіт/642.jpg,https://oleks-netizen.github.io/product-images/3149 Кіт/643.jpg,https://oleks-netizen.github.io/product-images/3149 Кіт/644.jpg,https://oleks-netizen.github.io/product-images/3149 Кіт/645.jpg,https://oleks-netizen.github.io/product-images/3149 Кіт/646.jpg,https://oleks-netizen.github.io/product-images/3149 Кіт/647.jpg,https://oleks-netizen.github.io/product-images/3149 Кіт/648.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/1809-grey/5152.jpg,https://oleks-netizen.github.io/product-images/1809-grey/5153.jpg,https://oleks-netizen.github.io/product-images/1809-grey/5154.jpg,https://oleks-netizen.github.io/product-images/1809-grey/5155.jpg,https://oleks-netizen.github.io/product-images/1809-grey/5156.jpg,https://oleks-netizen.github.io/product-images/1809-grey/5157.jpg,https://oleks-netizen.github.io/product-images/1809-grey/5158.jpg,https://oleks-netizen.github.io/product-images/1809-grey/5159.jpg</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>3149 Кава в Парижі</t>
+          <t>509-black</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3149 Кава в Парижі/5019.jpg,https://oleks-netizen.github.io/product-images/3149 Кава в Парижі/5020.jpg,https://oleks-netizen.github.io/product-images/3149 Кава в Парижі/5021.jpg,https://oleks-netizen.github.io/product-images/3149 Кава в Парижі/5022.jpg,https://oleks-netizen.github.io/product-images/3149 Кава в Парижі/5023.jpg,https://oleks-netizen.github.io/product-images/3149 Кава в Парижі/5024.jpg,https://oleks-netizen.github.io/product-images/3149 Кава в Парижі/5025.jpg,https://oleks-netizen.github.io/product-images/3149 Кава в Парижі/5026.jpg,https://oleks-netizen.github.io/product-images/3149 Кава в Парижі/5027.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/509-black/791.jpg,https://oleks-netizen.github.io/product-images/509-black/792.jpg,https://oleks-netizen.github.io/product-images/509-black/793.jpg,https://oleks-netizen.github.io/product-images/509-black/794.jpg,https://oleks-netizen.github.io/product-images/509-black/795.jpg,https://oleks-netizen.github.io/product-images/509-black/796.jpg,https://oleks-netizen.github.io/product-images/509-black/797.jpg</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>3149 Слід</t>
+          <t>509-green</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3149 Слід/5808.jpg,https://oleks-netizen.github.io/product-images/3149 Слід/5809.jpg,https://oleks-netizen.github.io/product-images/3149 Слід/5810.jpg,https://oleks-netizen.github.io/product-images/3149 Слід/5811.jpg,https://oleks-netizen.github.io/product-images/3149 Слід/5812.jpg,https://oleks-netizen.github.io/product-images/3149 Слід/5813.jpg,https://oleks-netizen.github.io/product-images/3149 Слід/5814.jpg,https://oleks-netizen.github.io/product-images/3149 Слід/5815.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/509-green/4476.jpg,https://oleks-netizen.github.io/product-images/509-green/4477.jpg,https://oleks-netizen.github.io/product-images/509-green/4478.jpg,https://oleks-netizen.github.io/product-images/509-green/4479.jpg,https://oleks-netizen.github.io/product-images/509-green/4480.jpg,https://oleks-netizen.github.io/product-images/509-green/4481.jpg,https://oleks-netizen.github.io/product-images/509-green/4482.jpg</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>3149-1</t>
+          <t>6098-black</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3149-1/2024.jpg,https://oleks-netizen.github.io/product-images/3149-1/2025.jpg,https://oleks-netizen.github.io/product-images/3149-1/2026.jpg,https://oleks-netizen.github.io/product-images/3149-1/2027.jpg,https://oleks-netizen.github.io/product-images/3149-1/2028.jpg,https://oleks-netizen.github.io/product-images/3149-1/2029.jpg,https://oleks-netizen.github.io/product-images/3149-1/2030.jpg,https://oleks-netizen.github.io/product-images/3149-1/2031.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/6098-black/4843.jpg,https://oleks-netizen.github.io/product-images/6098-black/4844.jpg,https://oleks-netizen.github.io/product-images/6098-black/4845.jpg,https://oleks-netizen.github.io/product-images/6098-black/4846.jpg,https://oleks-netizen.github.io/product-images/6098-black/4847.jpg,https://oleks-netizen.github.io/product-images/6098-black/4848.jpg,https://oleks-netizen.github.io/product-images/6098-black/4849.jpg,https://oleks-netizen.github.io/product-images/6098-black/4850.jpg</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -666,12 +666,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>3150 France</t>
+          <t>6098-green-kam</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3150 France/6150.jpg,https://oleks-netizen.github.io/product-images/3150 France/6151.jpg,https://oleks-netizen.github.io/product-images/3150 France/6152.jpg,https://oleks-netizen.github.io/product-images/3150 France/6153.jpg,https://oleks-netizen.github.io/product-images/3150 France/6154.jpg,https://oleks-netizen.github.io/product-images/3150 France/6155.jpg,https://oleks-netizen.github.io/product-images/3150 France/6156.jpg,https://oleks-netizen.github.io/product-images/3150 France/6157.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/6098-green-kam/3909.jpg,https://oleks-netizen.github.io/product-images/6098-green-kam/3910.jpg,https://oleks-netizen.github.io/product-images/6098-green-kam/3911.jpg,https://oleks-netizen.github.io/product-images/6098-green-kam/3912.jpg,https://oleks-netizen.github.io/product-images/6098-green-kam/3913.jpg,https://oleks-netizen.github.io/product-images/6098-green-kam/3914.jpg,https://oleks-netizen.github.io/product-images/6098-green-kam/3915.jpg,https://oleks-netizen.github.io/product-images/6098-green-kam/3916.jpg</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -681,12 +681,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>3150 Paris</t>
+          <t>6836-black</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3150 Paris/2825.jpg,https://oleks-netizen.github.io/product-images/3150 Paris/2826.jpg,https://oleks-netizen.github.io/product-images/3150 Paris/2827.jpg,https://oleks-netizen.github.io/product-images/3150 Paris/2828.jpg,https://oleks-netizen.github.io/product-images/3150 Paris/2829.jpg,https://oleks-netizen.github.io/product-images/3150 Paris/2830.jpg,https://oleks-netizen.github.io/product-images/3150 Paris/2831.jpg,https://oleks-netizen.github.io/product-images/3150 Paris/2832.jpg,https://oleks-netizen.github.io/product-images/3150 Paris/2833.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/6836-black/5143.jpg,https://oleks-netizen.github.io/product-images/6836-black/5144.jpg,https://oleks-netizen.github.io/product-images/6836-black/5145.jpg,https://oleks-netizen.github.io/product-images/6836-black/5146.jpg,https://oleks-netizen.github.io/product-images/6836-black/5147.jpg,https://oleks-netizen.github.io/product-images/6836-black/5148.jpg,https://oleks-netizen.github.io/product-images/6836-black/5149.jpg,https://oleks-netizen.github.io/product-images/6836-black/5150.jpg,https://oleks-netizen.github.io/product-images/6836-black/5151.jpg</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -696,12 +696,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>3150 Прогулянка в Парижі</t>
+          <t>7631-black</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3150 Прогулянка в Парижі/2015.jpg,https://oleks-netizen.github.io/product-images/3150 Прогулянка в Парижі/2016.jpg,https://oleks-netizen.github.io/product-images/3150 Прогулянка в Парижі/2017.jpg,https://oleks-netizen.github.io/product-images/3150 Прогулянка в Парижі/2018.jpg,https://oleks-netizen.github.io/product-images/3150 Прогулянка в Парижі/2019.jpg,https://oleks-netizen.github.io/product-images/3150 Прогулянка в Парижі/2020.jpg,https://oleks-netizen.github.io/product-images/3150 Прогулянка в Парижі/2021.jpg,https://oleks-netizen.github.io/product-images/3150 Прогулянка в Парижі/2022.jpg,https://oleks-netizen.github.io/product-images/3150 Прогулянка в Парижі/2023.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/7631-black/2368.jpg,https://oleks-netizen.github.io/product-images/7631-black/2369.jpg,https://oleks-netizen.github.io/product-images/7631-black/2370.jpg,https://oleks-netizen.github.io/product-images/7631-black/2371.jpg,https://oleks-netizen.github.io/product-images/7631-black/2372.jpg,https://oleks-netizen.github.io/product-images/7631-black/2373.jpg,https://oleks-netizen.github.io/product-images/7631-black/2374.jpg,https://oleks-netizen.github.io/product-images/7631-black/2375.jpg,https://oleks-netizen.github.io/product-images/7631-black/2376.jpg</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -711,207 +711,207 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>3150 Сліди</t>
+          <t>C-8460A-grey</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3150 Сліди/521.jpg,https://oleks-netizen.github.io/product-images/3150 Сліди/522.jpg,https://oleks-netizen.github.io/product-images/3150 Сліди/523.jpg,https://oleks-netizen.github.io/product-images/3150 Сліди/524.jpg,https://oleks-netizen.github.io/product-images/3150 Сліди/525.jpg,https://oleks-netizen.github.io/product-images/3150 Сліди/526.jpg,https://oleks-netizen.github.io/product-images/3150 Сліди/527.jpg,https://oleks-netizen.github.io/product-images/3150 Сліди/528.jpg,https://oleks-netizen.github.io/product-images/3150 Сліди/529.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C-8460A-grey/4594.jpg,https://oleks-netizen.github.io/product-images/C-8460A-grey/4595.jpg,https://oleks-netizen.github.io/product-images/C-8460A-grey/4596.jpg,https://oleks-netizen.github.io/product-images/C-8460A-grey/4597.jpg,https://oleks-netizen.github.io/product-images/C-8460A-grey/4598.jpg,https://oleks-netizen.github.io/product-images/C-8460A-grey/4599.jpg</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>3150-1</t>
+          <t>C-8460A-pink</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3150-1/4812.jpg,https://oleks-netizen.github.io/product-images/3150-1/4813.jpg,https://oleks-netizen.github.io/product-images/3150-1/4814.jpg,https://oleks-netizen.github.io/product-images/3150-1/4815.jpg,https://oleks-netizen.github.io/product-images/3150-1/4816.jpg,https://oleks-netizen.github.io/product-images/3150-1/4817.jpg,https://oleks-netizen.github.io/product-images/3150-1/4818.jpg,https://oleks-netizen.github.io/product-images/3150-1/4819.jpg,https://oleks-netizen.github.io/product-images/3150-1/4820.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C-8460A-pink/5728.jpg,https://oleks-netizen.github.io/product-images/C-8460A-pink/5729.jpg,https://oleks-netizen.github.io/product-images/C-8460A-pink/5730.jpg,https://oleks-netizen.github.io/product-images/C-8460A-pink/5731.jpg,https://oleks-netizen.github.io/product-images/C-8460A-pink/5732.jpg,https://oleks-netizen.github.io/product-images/C-8460A-pink/5733.jpg</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>3225 Біла</t>
+          <t>C-8460A-silvery-grey</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3225 Біла/1193.jpg,https://oleks-netizen.github.io/product-images/3225 Біла/1194.jpg,https://oleks-netizen.github.io/product-images/3225 Біла/1195.jpg,https://oleks-netizen.github.io/product-images/3225 Біла/1196.jpg,https://oleks-netizen.github.io/product-images/3225 Біла/1197.jpg,https://oleks-netizen.github.io/product-images/3225 Біла/1198.jpg,https://oleks-netizen.github.io/product-images/3225 Біла/1199.jpg,https://oleks-netizen.github.io/product-images/3225 Біла/1200.jpg,https://oleks-netizen.github.io/product-images/3225 Біла/1201.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C-8460A-silvery-grey/2183.jpg,https://oleks-netizen.github.io/product-images/C-8460A-silvery-grey/2184.jpg,https://oleks-netizen.github.io/product-images/C-8460A-silvery-grey/2185.jpg,https://oleks-netizen.github.io/product-images/C-8460A-silvery-grey/2186.jpg,https://oleks-netizen.github.io/product-images/C-8460A-silvery-grey/2187.jpg,https://oleks-netizen.github.io/product-images/C-8460A-silvery-grey/2188.jpg</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>3225 Коралова</t>
+          <t>C-8460B-black</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3225 Коралова/669.jpg,https://oleks-netizen.github.io/product-images/3225 Коралова/670.jpg,https://oleks-netizen.github.io/product-images/3225 Коралова/671.jpg,https://oleks-netizen.github.io/product-images/3225 Коралова/672.jpg,https://oleks-netizen.github.io/product-images/3225 Коралова/673.jpg,https://oleks-netizen.github.io/product-images/3225 Коралова/674.jpg,https://oleks-netizen.github.io/product-images/3225 Коралова/675.jpg,https://oleks-netizen.github.io/product-images/3225 Коралова/676.jpg,https://oleks-netizen.github.io/product-images/3225 Коралова/677.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C-8460B-black/1627.jpg,https://oleks-netizen.github.io/product-images/C-8460B-black/1628.jpg,https://oleks-netizen.github.io/product-images/C-8460B-black/1629.jpg,https://oleks-netizen.github.io/product-images/C-8460B-black/1630.jpg,https://oleks-netizen.github.io/product-images/C-8460B-black/1631.jpg,https://oleks-netizen.github.io/product-images/C-8460B-black/1632.jpg</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>3225 Кремова</t>
+          <t>C-8460B-green</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3225 Кремова/2692.jpg,https://oleks-netizen.github.io/product-images/3225 Кремова/2693.jpg,https://oleks-netizen.github.io/product-images/3225 Кремова/2694.jpg,https://oleks-netizen.github.io/product-images/3225 Кремова/2695.jpg,https://oleks-netizen.github.io/product-images/3225 Кремова/2696.jpg,https://oleks-netizen.github.io/product-images/3225 Кремова/2697.jpg,https://oleks-netizen.github.io/product-images/3225 Кремова/2698.jpg,https://oleks-netizen.github.io/product-images/3225 Кремова/2699.jpg,https://oleks-netizen.github.io/product-images/3225 Кремова/2700.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C-8460B-green/3881.jpg,https://oleks-netizen.github.io/product-images/C-8460B-green/3882.jpg,https://oleks-netizen.github.io/product-images/C-8460B-green/3883.jpg,https://oleks-netizen.github.io/product-images/C-8460B-green/3884.jpg,https://oleks-netizen.github.io/product-images/C-8460B-green/3885.jpg,https://oleks-netizen.github.io/product-images/C-8460B-green/3886.jpg</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>3225 Сіро-блакитна</t>
+          <t>C-8460B-grey</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3225 Сіро-блакитна/5120.jpg,https://oleks-netizen.github.io/product-images/3225 Сіро-блакитна/5121.jpg,https://oleks-netizen.github.io/product-images/3225 Сіро-блакитна/5122.jpg,https://oleks-netizen.github.io/product-images/3225 Сіро-блакитна/5123.jpg,https://oleks-netizen.github.io/product-images/3225 Сіро-блакитна/5124.jpg,https://oleks-netizen.github.io/product-images/3225 Сіро-блакитна/5125.jpg,https://oleks-netizen.github.io/product-images/3225 Сіро-блакитна/5126.jpg,https://oleks-netizen.github.io/product-images/3225 Сіро-блакитна/5127.jpg,https://oleks-netizen.github.io/product-images/3225 Сіро-блакитна/5128.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C-8460B-grey/5445.jpg,https://oleks-netizen.github.io/product-images/C-8460B-grey/5446.jpg,https://oleks-netizen.github.io/product-images/C-8460B-grey/5447.jpg,https://oleks-netizen.github.io/product-images/C-8460B-grey/5448.jpg,https://oleks-netizen.github.io/product-images/C-8460B-grey/5449.jpg,https://oleks-netizen.github.io/product-images/C-8460B-grey/5450.jpg</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>3225 Синя</t>
+          <t>C-8460B-khaki</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3225 Синя/5867.jpg,https://oleks-netizen.github.io/product-images/3225 Синя/5868.jpg,https://oleks-netizen.github.io/product-images/3225 Синя/5869.jpg,https://oleks-netizen.github.io/product-images/3225 Синя/5870.jpg,https://oleks-netizen.github.io/product-images/3225 Синя/5871.jpg,https://oleks-netizen.github.io/product-images/3225 Синя/5872.jpg,https://oleks-netizen.github.io/product-images/3225 Синя/5873.jpg,https://oleks-netizen.github.io/product-images/3225 Синя/5874.jpg,https://oleks-netizen.github.io/product-images/3225 Синя/5875.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C-8460B-khaki/4282.jpg,https://oleks-netizen.github.io/product-images/C-8460B-khaki/4283.jpg,https://oleks-netizen.github.io/product-images/C-8460B-khaki/4284.jpg,https://oleks-netizen.github.io/product-images/C-8460B-khaki/4285.jpg,https://oleks-netizen.github.io/product-images/C-8460B-khaki/4286.jpg,https://oleks-netizen.github.io/product-images/C-8460B-khaki/4287.jpg</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>3225 Фіолетова</t>
+          <t>C-8460B-red</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3225 Фіолетова/3700.jpg,https://oleks-netizen.github.io/product-images/3225 Фіолетова/3701.jpg,https://oleks-netizen.github.io/product-images/3225 Фіолетова/3702.jpg,https://oleks-netizen.github.io/product-images/3225 Фіолетова/3703.jpg,https://oleks-netizen.github.io/product-images/3225 Фіолетова/3704.jpg,https://oleks-netizen.github.io/product-images/3225 Фіолетова/3705.jpg,https://oleks-netizen.github.io/product-images/3225 Фіолетова/3706.jpg,https://oleks-netizen.github.io/product-images/3225 Фіолетова/3707.jpg,https://oleks-netizen.github.io/product-images/3225 Фіолетова/3708.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C-8460B-red/2231.jpg,https://oleks-netizen.github.io/product-images/C-8460B-red/2232.jpg,https://oleks-netizen.github.io/product-images/C-8460B-red/2233.jpg,https://oleks-netizen.github.io/product-images/C-8460B-red/2234.jpg,https://oleks-netizen.github.io/product-images/C-8460B-red/2235.jpg,https://oleks-netizen.github.io/product-images/C-8460B-red/2236.jpg</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>3226 Paris</t>
+          <t>C-8998-black</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3226 Paris/1974.jpg,https://oleks-netizen.github.io/product-images/3226 Paris/1975.jpg,https://oleks-netizen.github.io/product-images/3226 Paris/1976.jpg,https://oleks-netizen.github.io/product-images/3226 Paris/1977.jpg,https://oleks-netizen.github.io/product-images/3226 Paris/1978.jpg,https://oleks-netizen.github.io/product-images/3226 Paris/1979.jpg,https://oleks-netizen.github.io/product-images/3226 Paris/1980.jpg,https://oleks-netizen.github.io/product-images/3226 Paris/1981.jpg,https://oleks-netizen.github.io/product-images/3226 Paris/1982.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C-8998-black/3443.jpg,https://oleks-netizen.github.io/product-images/C-8998-black/3444.jpg,https://oleks-netizen.github.io/product-images/C-8998-black/3445.jpg,https://oleks-netizen.github.io/product-images/C-8998-black/3446.jpg,https://oleks-netizen.github.io/product-images/C-8998-black/3447.jpg</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>3226 Зірки</t>
+          <t>C-8998-dark-green</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3226 Зірки/5825.jpg,https://oleks-netizen.github.io/product-images/3226 Зірки/5826.jpg,https://oleks-netizen.github.io/product-images/3226 Зірки/5827.jpg,https://oleks-netizen.github.io/product-images/3226 Зірки/5828.jpg,https://oleks-netizen.github.io/product-images/3226 Зірки/5829.jpg,https://oleks-netizen.github.io/product-images/3226 Зірки/5830.jpg,https://oleks-netizen.github.io/product-images/3226 Зірки/5831.jpg,https://oleks-netizen.github.io/product-images/3226 Зірки/5832.jpg,https://oleks-netizen.github.io/product-images/3226 Зірки/5833.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C-8998-dark-green/4886.jpg,https://oleks-netizen.github.io/product-images/C-8998-dark-green/4887.jpg,https://oleks-netizen.github.io/product-images/C-8998-dark-green/4888.jpg,https://oleks-netizen.github.io/product-images/C-8998-dark-green/4889.jpg,https://oleks-netizen.github.io/product-images/C-8998-dark-green/4890.jpg,https://oleks-netizen.github.io/product-images/C-8998-dark-green/4891.jpg</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>3226 Кіт</t>
+          <t>C-8998-lime green</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3226 Кіт/879.jpg,https://oleks-netizen.github.io/product-images/3226 Кіт/880.jpg,https://oleks-netizen.github.io/product-images/3226 Кіт/881.jpg,https://oleks-netizen.github.io/product-images/3226 Кіт/882.jpg,https://oleks-netizen.github.io/product-images/3226 Кіт/883.jpg,https://oleks-netizen.github.io/product-images/3226 Кіт/884.jpg,https://oleks-netizen.github.io/product-images/3226 Кіт/885.jpg,https://oleks-netizen.github.io/product-images/3226 Кіт/886.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C-8998-lime green/1313.jpg,https://oleks-netizen.github.io/product-images/C-8998-lime green/1314.jpg,https://oleks-netizen.github.io/product-images/C-8998-lime green/1315.jpg,https://oleks-netizen.github.io/product-images/C-8998-lime green/1316.jpg,https://oleks-netizen.github.io/product-images/C-8998-lime green/1317.jpg</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>3226 Місто</t>
+          <t>C-8998-pink</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3226 Місто/2006.jpg,https://oleks-netizen.github.io/product-images/3226 Місто/2007.jpg,https://oleks-netizen.github.io/product-images/3226 Місто/2008.jpg,https://oleks-netizen.github.io/product-images/3226 Місто/2009.jpg,https://oleks-netizen.github.io/product-images/3226 Місто/2010.jpg,https://oleks-netizen.github.io/product-images/3226 Місто/2011.jpg,https://oleks-netizen.github.io/product-images/3226 Місто/2012.jpg,https://oleks-netizen.github.io/product-images/3226 Місто/2013.jpg,https://oleks-netizen.github.io/product-images/3226 Місто/2014.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C-8998-pink/5274.jpg,https://oleks-netizen.github.io/product-images/C-8998-pink/5275.jpg,https://oleks-netizen.github.io/product-images/C-8998-pink/5276.jpg,https://oleks-netizen.github.io/product-images/C-8998-pink/5277.jpg,https://oleks-netizen.github.io/product-images/C-8998-pink/5278.jpg,https://oleks-netizen.github.io/product-images/C-8998-pink/5279.jpg</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>3226 Сніг</t>
+          <t>DRL19001-1</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3226 Сніг/1711.jpg,https://oleks-netizen.github.io/product-images/3226 Сніг/1712.jpg,https://oleks-netizen.github.io/product-images/3226 Сніг/1713.jpg,https://oleks-netizen.github.io/product-images/3226 Сніг/1714.jpg,https://oleks-netizen.github.io/product-images/3226 Сніг/1715.jpg,https://oleks-netizen.github.io/product-images/3226 Сніг/1716.jpg,https://oleks-netizen.github.io/product-images/3226 Сніг/1717.jpg,https://oleks-netizen.github.io/product-images/3226 Сніг/1718.jpg,https://oleks-netizen.github.io/product-images/3226 Сніг/1719.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL19001-1/2864.jpg,https://oleks-netizen.github.io/product-images/DRL19001-1/2865.jpg,https://oleks-netizen.github.io/product-images/DRL19001-1/2866.jpg,https://oleks-netizen.github.io/product-images/DRL19001-1/2867.jpg,https://oleks-netizen.github.io/product-images/DRL19001-1/2868.jpg,https://oleks-netizen.github.io/product-images/DRL19001-1/2869.jpg,https://oleks-netizen.github.io/product-images/DRL19001-1/2870.jpg,https://oleks-netizen.github.io/product-images/DRL19001-1/2871.jpg</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>3226 Сяйво</t>
+          <t>DRL19012-1</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3226 Сяйво/5668.jpg,https://oleks-netizen.github.io/product-images/3226 Сяйво/5669.jpg,https://oleks-netizen.github.io/product-images/3226 Сяйво/5670.jpg,https://oleks-netizen.github.io/product-images/3226 Сяйво/5671.jpg,https://oleks-netizen.github.io/product-images/3226 Сяйво/5672.jpg,https://oleks-netizen.github.io/product-images/3226 Сяйво/5673.jpg,https://oleks-netizen.github.io/product-images/3226 Сяйво/5674.jpg,https://oleks-netizen.github.io/product-images/3226 Сяйво/5675.jpg,https://oleks-netizen.github.io/product-images/3226 Сяйво/5676.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL19012-1/5981.jpg,https://oleks-netizen.github.io/product-images/DRL19012-1/5982.jpg,https://oleks-netizen.github.io/product-images/DRL19012-1/5983.jpg,https://oleks-netizen.github.io/product-images/DRL19012-1/5984.jpg,https://oleks-netizen.github.io/product-images/DRL19012-1/5985.jpg,https://oleks-netizen.github.io/product-images/DRL19012-1/5986.jpg,https://oleks-netizen.github.io/product-images/DRL19012-1/5987.jpg,https://oleks-netizen.github.io/product-images/DRL19012-1/5988.jpg,https://oleks-netizen.github.io/product-images/DRL19012-1/5989.jpg</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -921,102 +921,102 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>3305 Бордова</t>
+          <t>DRL19077-1</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3305 Бордова/4511.jpg,https://oleks-netizen.github.io/product-images/3305 Бордова/4512.jpg,https://oleks-netizen.github.io/product-images/3305 Бордова/4513.jpg,https://oleks-netizen.github.io/product-images/3305 Бордова/4514.jpg,https://oleks-netizen.github.io/product-images/3305 Бордова/4515.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL19077-1/4120.jpg,https://oleks-netizen.github.io/product-images/DRL19077-1/4121.jpg,https://oleks-netizen.github.io/product-images/DRL19077-1/4122.jpg,https://oleks-netizen.github.io/product-images/DRL19077-1/4123.jpg,https://oleks-netizen.github.io/product-images/DRL19077-1/4124.jpg,https://oleks-netizen.github.io/product-images/DRL19077-1/4125.jpg,https://oleks-netizen.github.io/product-images/DRL19077-1/4126.jpg,https://oleks-netizen.github.io/product-images/DRL19077-1/4127.jpg</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>3305 Вишнева</t>
+          <t>DRL19092-1</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3305 Вишнева/2756.jpg,https://oleks-netizen.github.io/product-images/3305 Вишнева/2757.jpg,https://oleks-netizen.github.io/product-images/3305 Вишнева/2758.jpg,https://oleks-netizen.github.io/product-images/3305 Вишнева/2759.jpg,https://oleks-netizen.github.io/product-images/3305 Вишнева/2760.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL19092-1/4796.jpg,https://oleks-netizen.github.io/product-images/DRL19092-1/4797.jpg,https://oleks-netizen.github.io/product-images/DRL19092-1/4798.jpg,https://oleks-netizen.github.io/product-images/DRL19092-1/4799.jpg,https://oleks-netizen.github.io/product-images/DRL19092-1/4800.jpg,https://oleks-netizen.github.io/product-images/DRL19092-1/4801.jpg,https://oleks-netizen.github.io/product-images/DRL19092-1/4802.jpg,https://oleks-netizen.github.io/product-images/DRL19092-1/4803.jpg</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>3305 Червона</t>
+          <t>DRL19120-1</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3305 Червона/4483.jpg,https://oleks-netizen.github.io/product-images/3305 Червона/4484.jpg,https://oleks-netizen.github.io/product-images/3305 Червона/4485.jpg,https://oleks-netizen.github.io/product-images/3305 Червона/4486.jpg,https://oleks-netizen.github.io/product-images/3305 Червона/4487.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL19120-1/4710.jpg,https://oleks-netizen.github.io/product-images/DRL19120-1/4711.jpg,https://oleks-netizen.github.io/product-images/DRL19120-1/4712.jpg,https://oleks-netizen.github.io/product-images/DRL19120-1/4713.jpg,https://oleks-netizen.github.io/product-images/DRL19120-1/4714.jpg,https://oleks-netizen.github.io/product-images/DRL19120-1/4715.jpg,https://oleks-netizen.github.io/product-images/DRL19120-1/4716.jpg,https://oleks-netizen.github.io/product-images/DRL19120-1/4717.jpg,https://oleks-netizen.github.io/product-images/DRL19120-1/4718.jpg</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>3306A Біла</t>
+          <t>DRL19122-1</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3306A Біла/2544.jpg,https://oleks-netizen.github.io/product-images/3306A Біла/2545.jpg,https://oleks-netizen.github.io/product-images/3306A Біла/2546.jpg,https://oleks-netizen.github.io/product-images/3306A Біла/2547.jpg,https://oleks-netizen.github.io/product-images/3306A Біла/2548.jpg,https://oleks-netizen.github.io/product-images/3306A Біла/2549.jpg,https://oleks-netizen.github.io/product-images/3306A Біла/2550.jpg,https://oleks-netizen.github.io/product-images/3306A Біла/2551.jpg,https://oleks-netizen.github.io/product-images/3306A Біла/2552.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL19122-1/5841.jpg,https://oleks-netizen.github.io/product-images/DRL19122-1/5842.jpg,https://oleks-netizen.github.io/product-images/DRL19122-1/5843.jpg,https://oleks-netizen.github.io/product-images/DRL19122-1/5844.jpg,https://oleks-netizen.github.io/product-images/DRL19122-1/5845.jpg,https://oleks-netizen.github.io/product-images/DRL19122-1/5846.jpg,https://oleks-netizen.github.io/product-images/DRL19122-1/5847.jpg,https://oleks-netizen.github.io/product-images/DRL19122-1/5848.jpg</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>3306A Бордова</t>
+          <t>DRL19253-1</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3306A Бордова/4622.jpg,https://oleks-netizen.github.io/product-images/3306A Бордова/4623.jpg,https://oleks-netizen.github.io/product-images/3306A Бордова/4624.jpg,https://oleks-netizen.github.io/product-images/3306A Бордова/4625.jpg,https://oleks-netizen.github.io/product-images/3306A Бордова/4626.jpg,https://oleks-netizen.github.io/product-images/3306A Бордова/4627.jpg,https://oleks-netizen.github.io/product-images/3306A Бордова/4628.jpg,https://oleks-netizen.github.io/product-images/3306A Бордова/4629.jpg,https://oleks-netizen.github.io/product-images/3306A Бордова/4630.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL19253-1/4719.jpg,https://oleks-netizen.github.io/product-images/DRL19253-1/4720.jpg,https://oleks-netizen.github.io/product-images/DRL19253-1/4721.jpg,https://oleks-netizen.github.io/product-images/DRL19253-1/4722.jpg,https://oleks-netizen.github.io/product-images/DRL19253-1/4723.jpg,https://oleks-netizen.github.io/product-images/DRL19253-1/4724.jpg,https://oleks-netizen.github.io/product-images/DRL19253-1/4725.jpg,https://oleks-netizen.github.io/product-images/DRL19253-1/4726.jpg</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>3306A Сіра</t>
+          <t>DRL19520-1B</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3306A Сіра/5215.jpg,https://oleks-netizen.github.io/product-images/3306A Сіра/5216.jpg,https://oleks-netizen.github.io/product-images/3306A Сіра/5217.jpg,https://oleks-netizen.github.io/product-images/3306A Сіра/5218.jpg,https://oleks-netizen.github.io/product-images/3306A Сіра/5219.jpg,https://oleks-netizen.github.io/product-images/3306A Сіра/5220.jpg,https://oleks-netizen.github.io/product-images/3306A Сіра/5221.jpg,https://oleks-netizen.github.io/product-images/3306A Сіра/5222.jpg,https://oleks-netizen.github.io/product-images/3306A Сіра/5223.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL19520-1B/1447.jpg,https://oleks-netizen.github.io/product-images/DRL19520-1B/1448.jpg,https://oleks-netizen.github.io/product-images/DRL19520-1B/1449.jpg,https://oleks-netizen.github.io/product-images/DRL19520-1B/1450.jpg,https://oleks-netizen.github.io/product-images/DRL19520-1B/1451.jpg,https://oleks-netizen.github.io/product-images/DRL19520-1B/1452.jpg,https://oleks-netizen.github.io/product-images/DRL19520-1B/1453.jpg,https://oleks-netizen.github.io/product-images/DRL19520-1B/1454.jpg</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>3306A Синя</t>
+          <t>DRL19601-1</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3306A Синя/4206.jpg,https://oleks-netizen.github.io/product-images/3306A Синя/4207.jpg,https://oleks-netizen.github.io/product-images/3306A Синя/4208.jpg,https://oleks-netizen.github.io/product-images/3306A Синя/4209.jpg,https://oleks-netizen.github.io/product-images/3306A Синя/4210.jpg,https://oleks-netizen.github.io/product-images/3306A Синя/4211.jpg,https://oleks-netizen.github.io/product-images/3306A Синя/4212.jpg,https://oleks-netizen.github.io/product-images/3306A Синя/4213.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL19601-1/1021.jpg,https://oleks-netizen.github.io/product-images/DRL19601-1/1022.jpg,https://oleks-netizen.github.io/product-images/DRL19601-1/1023.jpg,https://oleks-netizen.github.io/product-images/DRL19601-1/1024.jpg,https://oleks-netizen.github.io/product-images/DRL19601-1/1025.jpg,https://oleks-netizen.github.io/product-images/DRL19601-1/1026.jpg,https://oleks-netizen.github.io/product-images/DRL19601-1/1027.jpg,https://oleks-netizen.github.io/product-images/DRL19601-1/1028.jpg</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -1026,12 +1026,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>3306A Червона</t>
+          <t>DRL19712-1</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3306A Червона/832.jpg,https://oleks-netizen.github.io/product-images/3306A Червона/833.jpg,https://oleks-netizen.github.io/product-images/3306A Червона/834.jpg,https://oleks-netizen.github.io/product-images/3306A Червона/835.jpg,https://oleks-netizen.github.io/product-images/3306A Червона/836.jpg,https://oleks-netizen.github.io/product-images/3306A Червона/837.jpg,https://oleks-netizen.github.io/product-images/3306A Червона/838.jpg,https://oleks-netizen.github.io/product-images/3306A Червона/839.jpg,https://oleks-netizen.github.io/product-images/3306A Червона/840.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL19712-1/2535.jpg,https://oleks-netizen.github.io/product-images/DRL19712-1/2536.jpg,https://oleks-netizen.github.io/product-images/DRL19712-1/2537.jpg,https://oleks-netizen.github.io/product-images/DRL19712-1/2538.jpg,https://oleks-netizen.github.io/product-images/DRL19712-1/2539.jpg,https://oleks-netizen.github.io/product-images/DRL19712-1/2540.jpg,https://oleks-netizen.github.io/product-images/DRL19712-1/2541.jpg,https://oleks-netizen.github.io/product-images/DRL19712-1/2542.jpg,https://oleks-netizen.github.io/product-images/DRL19712-1/2543.jpg</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -1041,237 +1041,237 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>3306A Чорний</t>
+          <t>DRL19818A-A</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3306A Чорний/5134.jpg,https://oleks-netizen.github.io/product-images/3306A Чорний/5135.jpg,https://oleks-netizen.github.io/product-images/3306A Чорний/5136.jpg,https://oleks-netizen.github.io/product-images/3306A Чорний/5137.jpg,https://oleks-netizen.github.io/product-images/3306A Чорний/5138.jpg,https://oleks-netizen.github.io/product-images/3306A Чорний/5139.jpg,https://oleks-netizen.github.io/product-images/3306A Чорний/5140.jpg,https://oleks-netizen.github.io/product-images/3306A Чорний/5141.jpg,https://oleks-netizen.github.io/product-images/3306A Чорний/5142.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL19818A-A/1404.jpg,https://oleks-netizen.github.io/product-images/DRL19818A-A/1405.jpg,https://oleks-netizen.github.io/product-images/DRL19818A-A/1406.jpg,https://oleks-netizen.github.io/product-images/DRL19818A-A/1407.jpg,https://oleks-netizen.github.io/product-images/DRL19818A-A/1408.jpg,https://oleks-netizen.github.io/product-images/DRL19818A-A/1409.jpg,https://oleks-netizen.github.io/product-images/DRL19818A-A/1410.jpg,https://oleks-netizen.github.io/product-images/DRL19818A-A/1411.jpg</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>5302A Біла</t>
+          <t>DRL19941-1</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/5302A Біла/92.jpg,https://oleks-netizen.github.io/product-images/5302A Біла/93.jpg,https://oleks-netizen.github.io/product-images/5302A Біла/94.jpg,https://oleks-netizen.github.io/product-images/5302A Біла/95.jpg,https://oleks-netizen.github.io/product-images/5302A Біла/96.jpg,https://oleks-netizen.github.io/product-images/5302A Біла/97.jpg,https://oleks-netizen.github.io/product-images/5302A Біла/98.jpg,https://oleks-netizen.github.io/product-images/5302A Біла/99.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL19941-1/741.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/742.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/743.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/744.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/745.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/746.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/747.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/748.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/749.jpg</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>5302A Бежева</t>
+          <t>DRL6601-1</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/5302A Бежева/1644.jpg,https://oleks-netizen.github.io/product-images/5302A Бежева/1645.jpg,https://oleks-netizen.github.io/product-images/5302A Бежева/1646.jpg,https://oleks-netizen.github.io/product-images/5302A Бежева/1647.jpg,https://oleks-netizen.github.io/product-images/5302A Бежева/1648.jpg,https://oleks-netizen.github.io/product-images/5302A Бежева/1649.jpg,https://oleks-netizen.github.io/product-images/5302A Бежева/1650.jpg,https://oleks-netizen.github.io/product-images/5302A Бежева/1651.jpg,https://oleks-netizen.github.io/product-images/5302A Бежева/1652.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL6601-1/816.jpg,https://oleks-netizen.github.io/product-images/DRL6601-1/817.jpg,https://oleks-netizen.github.io/product-images/DRL6601-1/818.jpg,https://oleks-netizen.github.io/product-images/DRL6601-1/819.jpg,https://oleks-netizen.github.io/product-images/DRL6601-1/820.jpg,https://oleks-netizen.github.io/product-images/DRL6601-1/821.jpg,https://oleks-netizen.github.io/product-images/DRL6601-1/822.jpg,https://oleks-netizen.github.io/product-images/DRL6601-1/823.jpg</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>5302A Кольорова</t>
+          <t>DRS16059-1</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/5302A Кольорова/3662.jpg,https://oleks-netizen.github.io/product-images/5302A Кольорова/3663.jpg,https://oleks-netizen.github.io/product-images/5302A Кольорова/3664.jpg,https://oleks-netizen.github.io/product-images/5302A Кольорова/3665.jpg,https://oleks-netizen.github.io/product-images/5302A Кольорова/3666.jpg,https://oleks-netizen.github.io/product-images/5302A Кольорова/3667.jpg,https://oleks-netizen.github.io/product-images/5302A Кольорова/3668.jpg,https://oleks-netizen.github.io/product-images/5302A Кольорова/3669.jpg,https://oleks-netizen.github.io/product-images/5302A Кольорова/3670.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRS16059-1/1854.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1855.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1856.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1857.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1858.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1859.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1860.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1861.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1862.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1863.jpg</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>5302A Синя</t>
+          <t>DRS16975-1</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/5302A Синя/3723.jpg,https://oleks-netizen.github.io/product-images/5302A Синя/3724.jpg,https://oleks-netizen.github.io/product-images/5302A Синя/3725.jpg,https://oleks-netizen.github.io/product-images/5302A Синя/3726.jpg,https://oleks-netizen.github.io/product-images/5302A Синя/3727.jpg,https://oleks-netizen.github.io/product-images/5302A Синя/3728.jpg,https://oleks-netizen.github.io/product-images/5302A Синя/3729.jpg,https://oleks-netizen.github.io/product-images/5302A Синя/3730.jpg,https://oleks-netizen.github.io/product-images/5302A Синя/3731.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRS16975-1/3087.jpg,https://oleks-netizen.github.io/product-images/DRS16975-1/3088.jpg,https://oleks-netizen.github.io/product-images/DRS16975-1/3089.jpg,https://oleks-netizen.github.io/product-images/DRS16975-1/3090.jpg,https://oleks-netizen.github.io/product-images/DRS16975-1/3091.jpg,https://oleks-netizen.github.io/product-images/DRS16975-1/3092.jpg</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>5302A Чорна</t>
+          <t>DRS17116-3</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/5302A Чорна/5241.jpg,https://oleks-netizen.github.io/product-images/5302A Чорна/5242.jpg,https://oleks-netizen.github.io/product-images/5302A Чорна/5243.jpg,https://oleks-netizen.github.io/product-images/5302A Чорна/5244.jpg,https://oleks-netizen.github.io/product-images/5302A Чорна/5245.jpg,https://oleks-netizen.github.io/product-images/5302A Чорна/5246.jpg,https://oleks-netizen.github.io/product-images/5302A Чорна/5247.jpg,https://oleks-netizen.github.io/product-images/5302A Чорна/5248.jpg,https://oleks-netizen.github.io/product-images/5302A Чорна/5249.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRS17116-3/2032.jpg,https://oleks-netizen.github.io/product-images/DRS17116-3/2033.jpg,https://oleks-netizen.github.io/product-images/DRS17116-3/2034.jpg,https://oleks-netizen.github.io/product-images/DRS17116-3/2035.jpg,https://oleks-netizen.github.io/product-images/DRS17116-3/2036.jpg,https://oleks-netizen.github.io/product-images/DRS17116-3/2037.jpg</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>5302A Чорно-біла</t>
+          <t>DRS17131-2</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/5302A Чорно-біла/849.jpg,https://oleks-netizen.github.io/product-images/5302A Чорно-біла/850.jpg,https://oleks-netizen.github.io/product-images/5302A Чорно-біла/851.jpg,https://oleks-netizen.github.io/product-images/5302A Чорно-біла/852.jpg,https://oleks-netizen.github.io/product-images/5302A Чорно-біла/853.jpg,https://oleks-netizen.github.io/product-images/5302A Чорно-біла/854.jpg,https://oleks-netizen.github.io/product-images/5302A Чорно-біла/855.jpg,https://oleks-netizen.github.io/product-images/5302A Чорно-біла/856.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRS17131-2/1936.jpg,https://oleks-netizen.github.io/product-images/DRS17131-2/1937.jpg,https://oleks-netizen.github.io/product-images/DRS17131-2/1938.jpg,https://oleks-netizen.github.io/product-images/DRS17131-2/1939.jpg,https://oleks-netizen.github.io/product-images/DRS17131-2/1940.jpg,https://oleks-netizen.github.io/product-images/DRS17131-2/1941.jpg,https://oleks-netizen.github.io/product-images/DRS17131-2/1942.jpg</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>BV38171-1</t>
+          <t>DRS17132-1</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BV38171-1/1396.jpg,https://oleks-netizen.github.io/product-images/BV38171-1/1397.jpg,https://oleks-netizen.github.io/product-images/BV38171-1/1398.jpg,https://oleks-netizen.github.io/product-images/BV38171-1/1399.jpg,https://oleks-netizen.github.io/product-images/BV38171-1/1400.jpg,https://oleks-netizen.github.io/product-images/BV38171-1/1401.jpg,https://oleks-netizen.github.io/product-images/BV38171-1/1402.jpg,https://oleks-netizen.github.io/product-images/BV38171-1/1403.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRS17132-1/4550.jpg,https://oleks-netizen.github.io/product-images/DRS17132-1/4551.jpg,https://oleks-netizen.github.io/product-images/DRS17132-1/4552.jpg,https://oleks-netizen.github.io/product-images/DRS17132-1/4553.jpg,https://oleks-netizen.github.io/product-images/DRS17132-1/4554.jpg,https://oleks-netizen.github.io/product-images/DRS17132-1/4555.jpg,https://oleks-netizen.github.io/product-images/DRS17132-1/4556.jpg</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>BV38319-143</t>
+          <t>DRS17203-1</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BV38319-143/1165.jpg,https://oleks-netizen.github.io/product-images/BV38319-143/1166.jpg,https://oleks-netizen.github.io/product-images/BV38319-143/1167.jpg,https://oleks-netizen.github.io/product-images/BV38319-143/1168.jpg,https://oleks-netizen.github.io/product-images/BV38319-143/1169.jpg,https://oleks-netizen.github.io/product-images/BV38319-143/1170.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRS17203-1/963.jpg,https://oleks-netizen.github.io/product-images/DRS17203-1/964.jpg,https://oleks-netizen.github.io/product-images/DRS17203-1/965.jpg,https://oleks-netizen.github.io/product-images/DRS17203-1/966.jpg,https://oleks-netizen.github.io/product-images/DRS17203-1/967.jpg,https://oleks-netizen.github.io/product-images/DRS17203-1/968.jpg,https://oleks-netizen.github.io/product-images/DRS17203-1/969.jpg,https://oleks-netizen.github.io/product-images/DRS17203-1/970.jpg</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>BV38321-1</t>
+          <t>DRS19023-2</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BV38321-1/3655.jpg,https://oleks-netizen.github.io/product-images/BV38321-1/3656.jpg,https://oleks-netizen.github.io/product-images/BV38321-1/3657.jpg,https://oleks-netizen.github.io/product-images/BV38321-1/3658.jpg,https://oleks-netizen.github.io/product-images/BV38321-1/3659.jpg,https://oleks-netizen.github.io/product-images/BV38321-1/3660.jpg,https://oleks-netizen.github.io/product-images/BV38321-1/3661.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRS19023-2/2966.jpg,https://oleks-netizen.github.io/product-images/DRS19023-2/2967.jpg,https://oleks-netizen.github.io/product-images/DRS19023-2/2968.jpg,https://oleks-netizen.github.io/product-images/DRS19023-2/2969.jpg,https://oleks-netizen.github.io/product-images/DRS19023-2/2970.jpg,https://oleks-netizen.github.io/product-images/DRS19023-2/2971.jpg</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>BV38345-150</t>
+          <t>DRS19353-1</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BV38345-150/655.jpg,https://oleks-netizen.github.io/product-images/BV38345-150/656.jpg,https://oleks-netizen.github.io/product-images/BV38345-150/657.jpg,https://oleks-netizen.github.io/product-images/BV38345-150/658.jpg,https://oleks-netizen.github.io/product-images/BV38345-150/659.jpg,https://oleks-netizen.github.io/product-images/BV38345-150/660.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRS19353-1/1892.jpg,https://oleks-netizen.github.io/product-images/DRS19353-1/1893.jpg,https://oleks-netizen.github.io/product-images/DRS19353-1/1894.jpg,https://oleks-netizen.github.io/product-images/DRS19353-1/1895.jpg,https://oleks-netizen.github.io/product-images/DRS19353-1/1896.jpg,https://oleks-netizen.github.io/product-images/DRS19353-1/1897.jpg,https://oleks-netizen.github.io/product-images/DRS19353-1/1898.jpg,https://oleks-netizen.github.io/product-images/DRS19353-1/1899.jpg</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>BV38345-210</t>
+          <t>DRS19800-1</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BV38345-210/1745.jpg,https://oleks-netizen.github.io/product-images/BV38345-210/1746.jpg,https://oleks-netizen.github.io/product-images/BV38345-210/1747.jpg,https://oleks-netizen.github.io/product-images/BV38345-210/1748.jpg,https://oleks-netizen.github.io/product-images/BV38345-210/1749.jpg,https://oleks-netizen.github.io/product-images/BV38345-210/1750.jpg,https://oleks-netizen.github.io/product-images/BV38345-210/1751.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRS19800-1/6032.jpg,https://oleks-netizen.github.io/product-images/DRS19800-1/6033.jpg,https://oleks-netizen.github.io/product-images/DRS19800-1/6034.jpg,https://oleks-netizen.github.io/product-images/DRS19800-1/6035.jpg,https://oleks-netizen.github.io/product-images/DRS19800-1/6036.jpg,https://oleks-netizen.github.io/product-images/DRS19800-1/6037.jpg</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>BV38348-1</t>
+          <t>DRS19802-1</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BV38348-1/207.jpg,https://oleks-netizen.github.io/product-images/BV38348-1/208.jpg,https://oleks-netizen.github.io/product-images/BV38348-1/209.jpg,https://oleks-netizen.github.io/product-images/BV38348-1/210.jpg,https://oleks-netizen.github.io/product-images/BV38348-1/211.jpg,https://oleks-netizen.github.io/product-images/BV38348-1/212.jpg,https://oleks-netizen.github.io/product-images/BV38348-1/213.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRS19802-1/5802.jpg,https://oleks-netizen.github.io/product-images/DRS19802-1/5803.jpg,https://oleks-netizen.github.io/product-images/DRS19802-1/5804.jpg,https://oleks-netizen.github.io/product-images/DRS19802-1/5805.jpg,https://oleks-netizen.github.io/product-images/DRS19802-1/5806.jpg,https://oleks-netizen.github.io/product-images/DRS19802-1/5807.jpg</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>BV38363-100</t>
+          <t>DS30002-023</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BV38363-100/810.jpg,https://oleks-netizen.github.io/product-images/BV38363-100/811.jpg,https://oleks-netizen.github.io/product-images/BV38363-100/812.jpg,https://oleks-netizen.github.io/product-images/BV38363-100/813.jpg,https://oleks-netizen.github.io/product-images/BV38363-100/814.jpg,https://oleks-netizen.github.io/product-images/BV38363-100/815.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DS30002-023/2441.jpg,https://oleks-netizen.github.io/product-images/DS30002-023/2442.jpg,https://oleks-netizen.github.io/product-images/DS30002-023/2443.jpg,https://oleks-netizen.github.io/product-images/DS30002-023/2444.jpg,https://oleks-netizen.github.io/product-images/DS30002-023/2445.jpg,https://oleks-netizen.github.io/product-images/DS30002-023/2446.jpg,https://oleks-netizen.github.io/product-images/DS30002-023/2448.jpg</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>BV38363-143</t>
+          <t>DS30002-025</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BV38363-143/5955.jpg,https://oleks-netizen.github.io/product-images/BV38363-143/5956.jpg,https://oleks-netizen.github.io/product-images/BV38363-143/5957.jpg,https://oleks-netizen.github.io/product-images/BV38363-143/5958.jpg,https://oleks-netizen.github.io/product-images/BV38363-143/5959.jpg,https://oleks-netizen.github.io/product-images/BV38363-143/5960.jpg,https://oleks-netizen.github.io/product-images/BV38363-143/5961.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DS30002-025/4055.jpg,https://oleks-netizen.github.io/product-images/DS30002-025/4056.jpg,https://oleks-netizen.github.io/product-images/DS30002-025/4057.jpg,https://oleks-netizen.github.io/product-images/DS30002-025/4058.jpg,https://oleks-netizen.github.io/product-images/DS30002-025/4059.jpg,https://oleks-netizen.github.io/product-images/DS30002-025/4062.jpg</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>BV38601-153</t>
+          <t>DS30002-112</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BV38601-153/5649.jpg,https://oleks-netizen.github.io/product-images/BV38601-153/5650.jpg,https://oleks-netizen.github.io/product-images/BV38601-153/5651.jpg,https://oleks-netizen.github.io/product-images/BV38601-153/5652.jpg,https://oleks-netizen.github.io/product-images/BV38601-153/5653.jpg,https://oleks-netizen.github.io/product-images/BV38601-153/5654.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DS30002-112/711.jpg,https://oleks-netizen.github.io/product-images/DS30002-112/712.jpg,https://oleks-netizen.github.io/product-images/DS30002-112/713.jpg,https://oleks-netizen.github.io/product-images/DS30002-112/714.jpg,https://oleks-netizen.github.io/product-images/DS30002-112/715.jpg,https://oleks-netizen.github.io/product-images/DS30002-112/718.jpg</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -1281,27 +1281,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>BV38601-2803</t>
+          <t>DS30002-132</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BV38601-2803/2790.jpg,https://oleks-netizen.github.io/product-images/BV38601-2803/2791.jpg,https://oleks-netizen.github.io/product-images/BV38601-2803/2792.jpg,https://oleks-netizen.github.io/product-images/BV38601-2803/2793.jpg,https://oleks-netizen.github.io/product-images/BV38601-2803/2794.jpg,https://oleks-netizen.github.io/product-images/BV38601-2803/2795.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DS30002-132/5381.jpg,https://oleks-netizen.github.io/product-images/DS30002-132/5382.jpg,https://oleks-netizen.github.io/product-images/DS30002-132/5383.jpg,https://oleks-netizen.github.io/product-images/DS30002-132/5384.jpg,https://oleks-netizen.github.io/product-images/DS30002-132/5385.jpg,https://oleks-netizen.github.io/product-images/DS30002-132/5386.jpg,https://oleks-netizen.github.io/product-images/DS30002-132/5387.jpg,https://oleks-netizen.github.io/product-images/DS30002-132/5388.jpg</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>BV38629-100</t>
+          <t>DS30002-162</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BV38629-100/1829.jpg,https://oleks-netizen.github.io/product-images/BV38629-100/1830.jpg,https://oleks-netizen.github.io/product-images/BV38629-100/1831.jpg,https://oleks-netizen.github.io/product-images/BV38629-100/1832.jpg,https://oleks-netizen.github.io/product-images/BV38629-100/1833.jpg,https://oleks-netizen.github.io/product-images/BV38629-100/1834.jpg,https://oleks-netizen.github.io/product-images/BV38629-100/1835.jpg,https://oleks-netizen.github.io/product-images/BV38629-100/1836.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DS30002-162/6176.jpg,https://oleks-netizen.github.io/product-images/DS30002-162/6177.jpg,https://oleks-netizen.github.io/product-images/DS30002-162/6178.jpg,https://oleks-netizen.github.io/product-images/DS30002-162/6179.jpg,https://oleks-netizen.github.io/product-images/DS30002-162/6180.jpg,https://oleks-netizen.github.io/product-images/DS30002-162/6181.jpg,https://oleks-netizen.github.io/product-images/DS30002-162/6182.jpg,https://oleks-netizen.github.io/product-images/DS30002-162/6183.jpg</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -1311,16 +1311,1501 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>BV38643-1</t>
+          <t>DS30002-287</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BV38643-1/6005.jpg,https://oleks-netizen.github.io/product-images/BV38643-1/6006.jpg,https://oleks-netizen.github.io/product-images/BV38643-1/6007.jpg,https://oleks-netizen.github.io/product-images/BV38643-1/6008.jpg,https://oleks-netizen.github.io/product-images/BV38643-1/6009.jpg,https://oleks-netizen.github.io/product-images/BV38643-1/6010.jpg,https://oleks-netizen.github.io/product-images/BV38643-1/6011.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DS30002-287/1738.jpg,https://oleks-netizen.github.io/product-images/DS30002-287/1739.jpg,https://oleks-netizen.github.io/product-images/DS30002-287/1740.jpg,https://oleks-netizen.github.io/product-images/DS30002-287/1741.jpg,https://oleks-netizen.github.io/product-images/DS30002-287/1742.jpg,https://oleks-netizen.github.io/product-images/DS30002-287/1743.jpg,https://oleks-netizen.github.io/product-images/DS30002-287/1744.jpg</t>
         </is>
       </c>
       <c r="C60" t="n">
         <v>7</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>DS30002-288</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/DS30002-288/4198.jpg,https://oleks-netizen.github.io/product-images/DS30002-288/4199.jpg,https://oleks-netizen.github.io/product-images/DS30002-288/4200.jpg,https://oleks-netizen.github.io/product-images/DS30002-288/4201.jpg,https://oleks-netizen.github.io/product-images/DS30002-288/4202.jpg,https://oleks-netizen.github.io/product-images/DS30002-288/4205.jpg</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>F20218-black</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/F20218-black/2169.jpg,https://oleks-netizen.github.io/product-images/F20218-black/2170.jpg,https://oleks-netizen.github.io/product-images/F20218-black/2171.jpg,https://oleks-netizen.github.io/product-images/F20218-black/2172.jpg,https://oleks-netizen.github.io/product-images/F20218-black/2173.jpg</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>FW-A2106-black</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/FW-A2106-black/2673.jpg,https://oleks-netizen.github.io/product-images/FW-A2106-black/2674.jpg,https://oleks-netizen.github.io/product-images/FW-A2106-black/2675.jpg,https://oleks-netizen.github.io/product-images/FW-A2106-black/2676.jpg,https://oleks-netizen.github.io/product-images/FW-A2106-black/2677.jpg</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>FW-A648-black</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/FW-A648-black/1543.jpg,https://oleks-netizen.github.io/product-images/FW-A648-black/1544.jpg,https://oleks-netizen.github.io/product-images/FW-A648-black/1545.jpg,https://oleks-netizen.github.io/product-images/FW-A648-black/1546.jpg,https://oleks-netizen.github.io/product-images/FW-A648-black/1547.jpg,https://oleks-netizen.github.io/product-images/FW-A648-black/1548.jpg</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>FW-A648-blue</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/FW-A648-blue/493.jpg,https://oleks-netizen.github.io/product-images/FW-A648-blue/494.jpg,https://oleks-netizen.github.io/product-images/FW-A648-blue/495.jpg,https://oleks-netizen.github.io/product-images/FW-A648-blue/496.jpg,https://oleks-netizen.github.io/product-images/FW-A648-blue/497.jpg,https://oleks-netizen.github.io/product-images/FW-A648-blue/498.jpg</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>FW-A648-green</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/FW-A648-green/6165.jpg,https://oleks-netizen.github.io/product-images/FW-A648-green/6166.jpg,https://oleks-netizen.github.io/product-images/FW-A648-green/6167.jpg,https://oleks-netizen.github.io/product-images/FW-A648-green/6168.jpg,https://oleks-netizen.github.io/product-images/FW-A648-green/6169.jpg,https://oleks-netizen.github.io/product-images/FW-A648-green/6170.jpg</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>FW-A648-purple</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/FW-A648-purple/2066.jpg,https://oleks-netizen.github.io/product-images/FW-A648-purple/2067.jpg,https://oleks-netizen.github.io/product-images/FW-A648-purple/2068.jpg,https://oleks-netizen.github.io/product-images/FW-A648-purple/2069.jpg,https://oleks-netizen.github.io/product-images/FW-A648-purple/2070.jpg,https://oleks-netizen.github.io/product-images/FW-A648-purple/2071.jpg</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>FW-A648-red</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/FW-A648-red/1241.jpg,https://oleks-netizen.github.io/product-images/FW-A648-red/1242.jpg,https://oleks-netizen.github.io/product-images/FW-A648-red/1243.jpg,https://oleks-netizen.github.io/product-images/FW-A648-red/1244.jpg,https://oleks-netizen.github.io/product-images/FW-A648-red/1245.jpg,https://oleks-netizen.github.io/product-images/FW-A648-red/1246.jpg</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>G2568-black</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/G2568-black/1298.jpg,https://oleks-netizen.github.io/product-images/G2568-black/1299.jpg,https://oleks-netizen.github.io/product-images/G2568-black/1300.jpg,https://oleks-netizen.github.io/product-images/G2568-black/1301.jpg,https://oleks-netizen.github.io/product-images/G2568-black/1302.jpg,https://oleks-netizen.github.io/product-images/G2568-black/1303.jpg,https://oleks-netizen.github.io/product-images/G2568-black/1304.jpg,https://oleks-netizen.github.io/product-images/G2568-black/1305.jpg</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>G2568-grey</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/G2568-grey/1752.jpg,https://oleks-netizen.github.io/product-images/G2568-grey/1753.jpg,https://oleks-netizen.github.io/product-images/G2568-grey/1754.jpg,https://oleks-netizen.github.io/product-images/G2568-grey/1755.jpg,https://oleks-netizen.github.io/product-images/G2568-grey/1756.jpg,https://oleks-netizen.github.io/product-images/G2568-grey/1757.jpg,https://oleks-netizen.github.io/product-images/G2568-grey/1758.jpg</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>H-2908-black</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/H-2908-black/5423.jpg,https://oleks-netizen.github.io/product-images/H-2908-black/5424.jpg,https://oleks-netizen.github.io/product-images/H-2908-black/5425.jpg,https://oleks-netizen.github.io/product-images/H-2908-black/5426.jpg,https://oleks-netizen.github.io/product-images/H-2908-black/5427.jpg</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>H-2908-red</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/H-2908-red/3159.jpg,https://oleks-netizen.github.io/product-images/H-2908-red/3160.jpg,https://oleks-netizen.github.io/product-images/H-2908-red/3161.jpg,https://oleks-netizen.github.io/product-images/H-2908-red/3162.jpg,https://oleks-netizen.github.io/product-images/H-2908-red/3163.jpg</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>L20001-22</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20001-22/955.jpg,https://oleks-netizen.github.io/product-images/L20001-22/956.jpg,https://oleks-netizen.github.io/product-images/L20001-22/957.jpg,https://oleks-netizen.github.io/product-images/L20001-22/958.jpg,https://oleks-netizen.github.io/product-images/L20001-22/959.jpg,https://oleks-netizen.github.io/product-images/L20001-22/960.jpg,https://oleks-netizen.github.io/product-images/L20001-22/961.jpg,https://oleks-netizen.github.io/product-images/L20001-22/962.jpg</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>L20011-1</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20011-1/3500.jpg,https://oleks-netizen.github.io/product-images/L20011-1/3501.jpg,https://oleks-netizen.github.io/product-images/L20011-1/3502.jpg,https://oleks-netizen.github.io/product-images/L20011-1/3503.jpg,https://oleks-netizen.github.io/product-images/L20011-1/3504.jpg,https://oleks-netizen.github.io/product-images/L20011-1/3505.jpg,https://oleks-netizen.github.io/product-images/L20011-1/3506.jpg,https://oleks-netizen.github.io/product-images/L20011-1/3507.jpg</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>L20011-22</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20011-22/6081.jpg,https://oleks-netizen.github.io/product-images/L20011-22/6082.jpg,https://oleks-netizen.github.io/product-images/L20011-22/6083.jpg,https://oleks-netizen.github.io/product-images/L20011-22/6084.jpg,https://oleks-netizen.github.io/product-images/L20011-22/6085.jpg,https://oleks-netizen.github.io/product-images/L20011-22/6086.jpg,https://oleks-netizen.github.io/product-images/L20011-22/6087.jpg,https://oleks-netizen.github.io/product-images/L20011-22/6088.jpg</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>L20011-56</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20011-56/5785.jpg,https://oleks-netizen.github.io/product-images/L20011-56/5786.jpg,https://oleks-netizen.github.io/product-images/L20011-56/5787.jpg,https://oleks-netizen.github.io/product-images/L20011-56/5788.jpg,https://oleks-netizen.github.io/product-images/L20011-56/5789.jpg,https://oleks-netizen.github.io/product-images/L20011-56/5790.jpg,https://oleks-netizen.github.io/product-images/L20011-56/5791.jpg,https://oleks-netizen.github.io/product-images/L20011-56/5792.jpg</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>L20030-1</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20030-1/4702.jpg,https://oleks-netizen.github.io/product-images/L20030-1/4703.jpg,https://oleks-netizen.github.io/product-images/L20030-1/4704.jpg,https://oleks-netizen.github.io/product-images/L20030-1/4705.jpg,https://oleks-netizen.github.io/product-images/L20030-1/4706.jpg,https://oleks-netizen.github.io/product-images/L20030-1/4707.jpg,https://oleks-netizen.github.io/product-images/L20030-1/4708.jpg,https://oleks-netizen.github.io/product-images/L20030-1/4709.jpg</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>L20030-56</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20030-56/3774.jpg,https://oleks-netizen.github.io/product-images/L20030-56/3775.jpg,https://oleks-netizen.github.io/product-images/L20030-56/3776.jpg,https://oleks-netizen.github.io/product-images/L20030-56/3777.jpg,https://oleks-netizen.github.io/product-images/L20030-56/3778.jpg,https://oleks-netizen.github.io/product-images/L20030-56/3779.jpg,https://oleks-netizen.github.io/product-images/L20030-56/3780.jpg,https://oleks-netizen.github.io/product-images/L20030-56/3781.jpg</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>L20036-1</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20036-1/3838.jpg,https://oleks-netizen.github.io/product-images/L20036-1/3839.jpg,https://oleks-netizen.github.io/product-images/L20036-1/3840.jpg,https://oleks-netizen.github.io/product-images/L20036-1/3841.jpg,https://oleks-netizen.github.io/product-images/L20036-1/3842.jpg,https://oleks-netizen.github.io/product-images/L20036-1/3843.jpg,https://oleks-netizen.github.io/product-images/L20036-1/3844.jpg,https://oleks-netizen.github.io/product-images/L20036-1/3845.jpg,https://oleks-netizen.github.io/product-images/L20036-1/3846.jpg</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>L20036-8</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20036-8/53.jpg,https://oleks-netizen.github.io/product-images/L20036-8/54.jpg,https://oleks-netizen.github.io/product-images/L20036-8/55.jpg,https://oleks-netizen.github.io/product-images/L20036-8/57.jpg,https://oleks-netizen.github.io/product-images/L20036-8/58.jpg,https://oleks-netizen.github.io/product-images/L20036-8/59.jpg,https://oleks-netizen.github.io/product-images/L20036-8/60.jpg</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>L20063-1</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20063-1/3093.jpg,https://oleks-netizen.github.io/product-images/L20063-1/3094.jpg,https://oleks-netizen.github.io/product-images/L20063-1/3095.jpg,https://oleks-netizen.github.io/product-images/L20063-1/3096.jpg,https://oleks-netizen.github.io/product-images/L20063-1/3097.jpg,https://oleks-netizen.github.io/product-images/L20063-1/3098.jpg,https://oleks-netizen.github.io/product-images/L20063-1/3099.jpg,https://oleks-netizen.github.io/product-images/L20063-1/3100.jpg,https://oleks-netizen.github.io/product-images/L20063-1/3101.jpg</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>L20063-8</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20063-8/896.jpg,https://oleks-netizen.github.io/product-images/L20063-8/897.jpg,https://oleks-netizen.github.io/product-images/L20063-8/898.jpg,https://oleks-netizen.github.io/product-images/L20063-8/899.jpg,https://oleks-netizen.github.io/product-images/L20063-8/900.jpg,https://oleks-netizen.github.io/product-images/L20063-8/901.jpg,https://oleks-netizen.github.io/product-images/L20063-8/902.jpg,https://oleks-netizen.github.io/product-images/L20063-8/903.jpg,https://oleks-netizen.github.io/product-images/L20063-8/904.jpg</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>L20633-78</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20633-78/1983.jpg,https://oleks-netizen.github.io/product-images/L20633-78/1984.jpg,https://oleks-netizen.github.io/product-images/L20633-78/1985.jpg,https://oleks-netizen.github.io/product-images/L20633-78/1986.jpg,https://oleks-netizen.github.io/product-images/L20633-78/1987.jpg,https://oleks-netizen.github.io/product-images/L20633-78/1988.jpg,https://oleks-netizen.github.io/product-images/L20633-78/1989.jpg,https://oleks-netizen.github.io/product-images/L20633-78/1990.jpg</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>L20633-90</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20633-90/3421.jpg,https://oleks-netizen.github.io/product-images/L20633-90/3422.jpg,https://oleks-netizen.github.io/product-images/L20633-90/3423.jpg,https://oleks-netizen.github.io/product-images/L20633-90/3424.jpg,https://oleks-netizen.github.io/product-images/L20633-90/3425.jpg,https://oleks-netizen.github.io/product-images/L20633-90/3426.jpg,https://oleks-netizen.github.io/product-images/L20633-90/3427.jpg,https://oleks-netizen.github.io/product-images/L20633-90/3428.jpg</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>L20680-1</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20680-1/3946.jpg,https://oleks-netizen.github.io/product-images/L20680-1/3947.jpg,https://oleks-netizen.github.io/product-images/L20680-1/3948.jpg,https://oleks-netizen.github.io/product-images/L20680-1/3949.jpg,https://oleks-netizen.github.io/product-images/L20680-1/3950.jpg,https://oleks-netizen.github.io/product-images/L20680-1/3951.jpg,https://oleks-netizen.github.io/product-images/L20680-1/3952.jpg,https://oleks-netizen.github.io/product-images/L20680-1/3953.jpg,https://oleks-netizen.github.io/product-images/L20680-1/3954.jpg</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>L20680-56</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20680-56/3017.jpg,https://oleks-netizen.github.io/product-images/L20680-56/3018.jpg,https://oleks-netizen.github.io/product-images/L20680-56/3019.jpg,https://oleks-netizen.github.io/product-images/L20680-56/3020.jpg,https://oleks-netizen.github.io/product-images/L20680-56/3021.jpg,https://oleks-netizen.github.io/product-images/L20680-56/3022.jpg,https://oleks-netizen.github.io/product-images/L20680-56/3023.jpg,https://oleks-netizen.github.io/product-images/L20680-56/3024.jpg,https://oleks-netizen.github.io/product-images/L20680-56/3025.jpg</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>L20680-58</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20680-58/5518.jpg,https://oleks-netizen.github.io/product-images/L20680-58/5519.jpg,https://oleks-netizen.github.io/product-images/L20680-58/5520.jpg,https://oleks-netizen.github.io/product-images/L20680-58/5521.jpg,https://oleks-netizen.github.io/product-images/L20680-58/5522.jpg,https://oleks-netizen.github.io/product-images/L20680-58/5523.jpg,https://oleks-netizen.github.io/product-images/L20680-58/5524.jpg,https://oleks-netizen.github.io/product-images/L20680-58/5525.jpg,https://oleks-netizen.github.io/product-images/L20680-58/5526.jpg</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>L20682-1</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20682-1/3026.jpg,https://oleks-netizen.github.io/product-images/L20682-1/3027.jpg,https://oleks-netizen.github.io/product-images/L20682-1/3028.jpg,https://oleks-netizen.github.io/product-images/L20682-1/3029.jpg,https://oleks-netizen.github.io/product-images/L20682-1/3030.jpg,https://oleks-netizen.github.io/product-images/L20682-1/3031.jpg,https://oleks-netizen.github.io/product-images/L20682-1/3032.jpg,https://oleks-netizen.github.io/product-images/L20682-1/3033.jpg</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>L20683-1</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20683-1/2684.jpg,https://oleks-netizen.github.io/product-images/L20683-1/2685.jpg,https://oleks-netizen.github.io/product-images/L20683-1/2686.jpg,https://oleks-netizen.github.io/product-images/L20683-1/2687.jpg,https://oleks-netizen.github.io/product-images/L20683-1/2688.jpg,https://oleks-netizen.github.io/product-images/L20683-1/2689.jpg,https://oleks-netizen.github.io/product-images/L20683-1/2690.jpg,https://oleks-netizen.github.io/product-images/L20683-1/2691.jpg</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>L20683-2</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20683-2/1370.jpg,https://oleks-netizen.github.io/product-images/L20683-2/1371.jpg,https://oleks-netizen.github.io/product-images/L20683-2/1372.jpg,https://oleks-netizen.github.io/product-images/L20683-2/1373.jpg,https://oleks-netizen.github.io/product-images/L20683-2/1374.jpg,https://oleks-netizen.github.io/product-images/L20683-2/1375.jpg,https://oleks-netizen.github.io/product-images/L20683-2/1376.jpg,https://oleks-netizen.github.io/product-images/L20683-2/1377.jpg</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>L20713-1</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20713-1/499.jpg,https://oleks-netizen.github.io/product-images/L20713-1/500.jpg,https://oleks-netizen.github.io/product-images/L20713-1/501.jpg,https://oleks-netizen.github.io/product-images/L20713-1/502.jpg,https://oleks-netizen.github.io/product-images/L20713-1/503.jpg,https://oleks-netizen.github.io/product-images/L20713-1/504.jpg,https://oleks-netizen.github.io/product-images/L20713-1/505.jpg,https://oleks-netizen.github.io/product-images/L20713-1/506.jpg,https://oleks-netizen.github.io/product-images/L20713-1/507.jpg</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>L20713-8</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20713-8/971.jpg,https://oleks-netizen.github.io/product-images/L20713-8/972.jpg,https://oleks-netizen.github.io/product-images/L20713-8/973.jpg,https://oleks-netizen.github.io/product-images/L20713-8/974.jpg,https://oleks-netizen.github.io/product-images/L20713-8/975.jpg,https://oleks-netizen.github.io/product-images/L20713-8/976.jpg,https://oleks-netizen.github.io/product-images/L20713-8/977.jpg,https://oleks-netizen.github.io/product-images/L20713-8/978.jpg,https://oleks-netizen.github.io/product-images/L20713-8/979.jpg</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>L20812-1</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20812-1/5035.jpg,https://oleks-netizen.github.io/product-images/L20812-1/5036.jpg,https://oleks-netizen.github.io/product-images/L20812-1/5037.jpg,https://oleks-netizen.github.io/product-images/L20812-1/5038.jpg,https://oleks-netizen.github.io/product-images/L20812-1/5039.jpg,https://oleks-netizen.github.io/product-images/L20812-1/5040.jpg,https://oleks-netizen.github.io/product-images/L20812-1/5041.jpg,https://oleks-netizen.github.io/product-images/L20812-1/5042.jpg,https://oleks-netizen.github.io/product-images/L20812-1/5043.jpg</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>L20812-10</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20812-10/2722.jpg,https://oleks-netizen.github.io/product-images/L20812-10/2723.jpg,https://oleks-netizen.github.io/product-images/L20812-10/2724.jpg,https://oleks-netizen.github.io/product-images/L20812-10/2725.jpg,https://oleks-netizen.github.io/product-images/L20812-10/2726.jpg,https://oleks-netizen.github.io/product-images/L20812-10/2727.jpg,https://oleks-netizen.github.io/product-images/L20812-10/2728.jpg,https://oleks-netizen.github.io/product-images/L20812-10/2729.jpg,https://oleks-netizen.github.io/product-images/L20812-10/2730.jpg</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>L20812-15</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20812-15/423.jpg,https://oleks-netizen.github.io/product-images/L20812-15/424.jpg,https://oleks-netizen.github.io/product-images/L20812-15/425.jpg,https://oleks-netizen.github.io/product-images/L20812-15/426.jpg,https://oleks-netizen.github.io/product-images/L20812-15/427.jpg,https://oleks-netizen.github.io/product-images/L20812-15/428.jpg,https://oleks-netizen.github.io/product-images/L20812-15/429.jpg,https://oleks-netizen.github.io/product-images/L20812-15/430.jpg,https://oleks-netizen.github.io/product-images/L20812-15/431.jpg</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>L20812-56</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20812-56/2102.jpg,https://oleks-netizen.github.io/product-images/L20812-56/2103.jpg,https://oleks-netizen.github.io/product-images/L20812-56/2104.jpg,https://oleks-netizen.github.io/product-images/L20812-56/2105.jpg,https://oleks-netizen.github.io/product-images/L20812-56/2106.jpg,https://oleks-netizen.github.io/product-images/L20812-56/2107.jpg,https://oleks-netizen.github.io/product-images/L20812-56/2109.jpg,https://oleks-netizen.github.io/product-images/L20812-56/2110.jpg</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>L20841-58</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20841-58/4355.jpg,https://oleks-netizen.github.io/product-images/L20841-58/4356.jpg,https://oleks-netizen.github.io/product-images/L20841-58/4357.jpg,https://oleks-netizen.github.io/product-images/L20841-58/4358.jpg,https://oleks-netizen.github.io/product-images/L20841-58/4359.jpg,https://oleks-netizen.github.io/product-images/L20841-58/4360.jpg,https://oleks-netizen.github.io/product-images/L20841-58/4361.jpg,https://oleks-netizen.github.io/product-images/L20841-58/4362.jpg</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>L20849-1</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20849-1/2311.jpg,https://oleks-netizen.github.io/product-images/L20849-1/2312.jpg,https://oleks-netizen.github.io/product-images/L20849-1/2313.jpg,https://oleks-netizen.github.io/product-images/L20849-1/2314.jpg,https://oleks-netizen.github.io/product-images/L20849-1/2315.jpg,https://oleks-netizen.github.io/product-images/L20849-1/2316.jpg,https://oleks-netizen.github.io/product-images/L20849-1/2317.jpg,https://oleks-netizen.github.io/product-images/L20849-1/2318.jpg</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>L20849-701</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20849-701/4239.jpg,https://oleks-netizen.github.io/product-images/L20849-701/4240.jpg,https://oleks-netizen.github.io/product-images/L20849-701/4241.jpg,https://oleks-netizen.github.io/product-images/L20849-701/4242.jpg,https://oleks-netizen.github.io/product-images/L20849-701/4243.jpg,https://oleks-netizen.github.io/product-images/L20849-701/4244.jpg,https://oleks-netizen.github.io/product-images/L20849-701/4245.jpg,https://oleks-netizen.github.io/product-images/L20849-701/4246.jpg</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>L20849-720</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20849-720/2360.jpg,https://oleks-netizen.github.io/product-images/L20849-720/2361.jpg,https://oleks-netizen.github.io/product-images/L20849-720/2362.jpg,https://oleks-netizen.github.io/product-images/L20849-720/2364.jpg</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>L20849-811</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20849-811/2606.jpg,https://oleks-netizen.github.io/product-images/L20849-811/2607.jpg,https://oleks-netizen.github.io/product-images/L20849-811/2608.jpg,https://oleks-netizen.github.io/product-images/L20849-811/2609.jpg,https://oleks-netizen.github.io/product-images/L20849-811/2610.jpg,https://oleks-netizen.github.io/product-images/L20849-811/2611.jpg,https://oleks-netizen.github.io/product-images/L20849-811/2612.jpg,https://oleks-netizen.github.io/product-images/L20849-811/2613.jpg</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>L20853-1</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20853-1/2927.jpg,https://oleks-netizen.github.io/product-images/L20853-1/2928.jpg,https://oleks-netizen.github.io/product-images/L20853-1/2929.jpg,https://oleks-netizen.github.io/product-images/L20853-1/2930.jpg,https://oleks-netizen.github.io/product-images/L20853-1/2931.jpg,https://oleks-netizen.github.io/product-images/L20853-1/2932.jpg,https://oleks-netizen.github.io/product-images/L20853-1/2933.jpg,https://oleks-netizen.github.io/product-images/L20853-1/2934.jpg,https://oleks-netizen.github.io/product-images/L20853-1/2935.jpg</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>L20993-1</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L20993-1/2913.jpg,https://oleks-netizen.github.io/product-images/L20993-1/2914.jpg,https://oleks-netizen.github.io/product-images/L20993-1/2915.jpg,https://oleks-netizen.github.io/product-images/L20993-1/2916.jpg,https://oleks-netizen.github.io/product-images/L20993-1/2917.jpg,https://oleks-netizen.github.io/product-images/L20993-1/2918.jpg,https://oleks-netizen.github.io/product-images/L20993-1/2920.jpg</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>L21019-1</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L21019-1/2834.jpg,https://oleks-netizen.github.io/product-images/L21019-1/2835.jpg,https://oleks-netizen.github.io/product-images/L21019-1/2836.jpg,https://oleks-netizen.github.io/product-images/L21019-1/2837.jpg,https://oleks-netizen.github.io/product-images/L21019-1/2838.jpg,https://oleks-netizen.github.io/product-images/L21019-1/2839.jpg,https://oleks-netizen.github.io/product-images/L21019-1/2840.jpg,https://oleks-netizen.github.io/product-images/L21019-1/2841.jpg</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>L21019-142</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L21019-142/4411.jpg,https://oleks-netizen.github.io/product-images/L21019-142/4412.jpg,https://oleks-netizen.github.io/product-images/L21019-142/4413.jpg,https://oleks-netizen.github.io/product-images/L21019-142/4414.jpg,https://oleks-netizen.github.io/product-images/L21019-142/4415.jpg,https://oleks-netizen.github.io/product-images/L21019-142/4416.jpg,https://oleks-netizen.github.io/product-images/L21019-142/4417.jpg,https://oleks-netizen.github.io/product-images/L21019-142/4418.jpg</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>L21035-101</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L21035-101/166.jpg,https://oleks-netizen.github.io/product-images/L21035-101/167.jpg,https://oleks-netizen.github.io/product-images/L21035-101/168.jpg,https://oleks-netizen.github.io/product-images/L21035-101/169.jpg,https://oleks-netizen.github.io/product-images/L21035-101/170.jpg,https://oleks-netizen.github.io/product-images/L21035-101/171.jpg,https://oleks-netizen.github.io/product-images/L21035-101/172.jpg</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>L21075-1</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L21075-1/4522.jpg,https://oleks-netizen.github.io/product-images/L21075-1/4523.jpg,https://oleks-netizen.github.io/product-images/L21075-1/4524.jpg,https://oleks-netizen.github.io/product-images/L21075-1/4525.jpg,https://oleks-netizen.github.io/product-images/L21075-1/4526.jpg,https://oleks-netizen.github.io/product-images/L21075-1/4527.jpg,https://oleks-netizen.github.io/product-images/L21075-1/4528.jpg,https://oleks-netizen.github.io/product-images/L21075-1/4529.jpg</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>L21209-1</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L21209-1/3247.jpg,https://oleks-netizen.github.io/product-images/L21209-1/3248.jpg,https://oleks-netizen.github.io/product-images/L21209-1/3249.jpg,https://oleks-netizen.github.io/product-images/L21209-1/3250.jpg,https://oleks-netizen.github.io/product-images/L21209-1/3251.jpg,https://oleks-netizen.github.io/product-images/L21209-1/3252.jpg,https://oleks-netizen.github.io/product-images/L21209-1/3253.jpg,https://oleks-netizen.github.io/product-images/L21209-1/3254.jpg,https://oleks-netizen.github.io/product-images/L21209-1/3255.jpg</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>L21209-25</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L21209-25/4488.jpg,https://oleks-netizen.github.io/product-images/L21209-25/4489.jpg,https://oleks-netizen.github.io/product-images/L21209-25/4490.jpg,https://oleks-netizen.github.io/product-images/L21209-25/4491.jpg,https://oleks-netizen.github.io/product-images/L21209-25/4492.jpg,https://oleks-netizen.github.io/product-images/L21209-25/4493.jpg,https://oleks-netizen.github.io/product-images/L21209-25/4494.jpg,https://oleks-netizen.github.io/product-images/L21209-25/4495.jpg,https://oleks-netizen.github.io/product-images/L21209-25/4496.jpg</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>L21511-101</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L21511-101/2804.jpg,https://oleks-netizen.github.io/product-images/L21511-101/2805.jpg,https://oleks-netizen.github.io/product-images/L21511-101/2806.jpg,https://oleks-netizen.github.io/product-images/L21511-101/2807.jpg,https://oleks-netizen.github.io/product-images/L21511-101/2808.jpg,https://oleks-netizen.github.io/product-images/L21511-101/2809.jpg,https://oleks-netizen.github.io/product-images/L21511-101/2810.jpg,https://oleks-netizen.github.io/product-images/L21511-101/2811.jpg</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>L21529-43</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L21529-43/1431.jpg,https://oleks-netizen.github.io/product-images/L21529-43/1432.jpg,https://oleks-netizen.github.io/product-images/L21529-43/1433.jpg,https://oleks-netizen.github.io/product-images/L21529-43/1434.jpg,https://oleks-netizen.github.io/product-images/L21529-43/1435.jpg,https://oleks-netizen.github.io/product-images/L21529-43/1436.jpg,https://oleks-netizen.github.io/product-images/L21529-43/1437.jpg,https://oleks-netizen.github.io/product-images/L21529-43/1438.jpg</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>L21531-1</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L21531-1/2951.jpg,https://oleks-netizen.github.io/product-images/L21531-1/2952.jpg,https://oleks-netizen.github.io/product-images/L21531-1/2953.jpg,https://oleks-netizen.github.io/product-images/L21531-1/2954.jpg,https://oleks-netizen.github.io/product-images/L21531-1/2955.jpg,https://oleks-netizen.github.io/product-images/L21531-1/2956.jpg,https://oleks-netizen.github.io/product-images/L21531-1/2957.jpg,https://oleks-netizen.github.io/product-images/L21531-1/2958.jpg</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>L21531-11</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L21531-11/2153.jpg,https://oleks-netizen.github.io/product-images/L21531-11/2154.jpg,https://oleks-netizen.github.io/product-images/L21531-11/2155.jpg,https://oleks-netizen.github.io/product-images/L21531-11/2156.jpg,https://oleks-netizen.github.io/product-images/L21531-11/2157.jpg,https://oleks-netizen.github.io/product-images/L21531-11/2158.jpg,https://oleks-netizen.github.io/product-images/L21531-11/2159.jpg,https://oleks-netizen.github.io/product-images/L21531-11/2160.jpg</t>
+        </is>
+      </c>
+      <c r="C113" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>L21545-1</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L21545-1/5389.jpg,https://oleks-netizen.github.io/product-images/L21545-1/5390.jpg,https://oleks-netizen.github.io/product-images/L21545-1/5391.jpg,https://oleks-netizen.github.io/product-images/L21545-1/5392.jpg,https://oleks-netizen.github.io/product-images/L21545-1/5393.jpg,https://oleks-netizen.github.io/product-images/L21545-1/5394.jpg,https://oleks-netizen.github.io/product-images/L21545-1/5395.jpg,https://oleks-netizen.github.io/product-images/L21545-1/5396.jpg,https://oleks-netizen.github.io/product-images/L21545-1/5397.jpg</t>
+        </is>
+      </c>
+      <c r="C114" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>L21545-175</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L21545-175/5996.jpg,https://oleks-netizen.github.io/product-images/L21545-175/5997.jpg,https://oleks-netizen.github.io/product-images/L21545-175/5998.jpg,https://oleks-netizen.github.io/product-images/L21545-175/5999.jpg,https://oleks-netizen.github.io/product-images/L21545-175/6000.jpg,https://oleks-netizen.github.io/product-images/L21545-175/6001.jpg,https://oleks-netizen.github.io/product-images/L21545-175/6002.jpg,https://oleks-netizen.github.io/product-images/L21545-175/6003.jpg,https://oleks-netizen.github.io/product-images/L21545-175/6004.jpg</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>L21547-64</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L21547-64/4631.jpg,https://oleks-netizen.github.io/product-images/L21547-64/4632.jpg,https://oleks-netizen.github.io/product-images/L21547-64/4633.jpg,https://oleks-netizen.github.io/product-images/L21547-64/4634.jpg,https://oleks-netizen.github.io/product-images/L21547-64/4635.jpg,https://oleks-netizen.github.io/product-images/L21547-64/4636.jpg,https://oleks-netizen.github.io/product-images/L21547-64/4637.jpg,https://oleks-netizen.github.io/product-images/L21547-64/4638.jpg</t>
+        </is>
+      </c>
+      <c r="C116" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>L21549-1</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L21549-1/4564.jpg,https://oleks-netizen.github.io/product-images/L21549-1/4565.jpg,https://oleks-netizen.github.io/product-images/L21549-1/4566.jpg,https://oleks-netizen.github.io/product-images/L21549-1/4567.jpg,https://oleks-netizen.github.io/product-images/L21549-1/4568.jpg,https://oleks-netizen.github.io/product-images/L21549-1/4569.jpg,https://oleks-netizen.github.io/product-images/L21549-1/4570.jpg,https://oleks-netizen.github.io/product-images/L21549-1/4571.jpg,https://oleks-netizen.github.io/product-images/L21549-1/4572.jpg</t>
+        </is>
+      </c>
+      <c r="C117" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>L21549-22</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L21549-22/2079.jpg,https://oleks-netizen.github.io/product-images/L21549-22/2080.jpg,https://oleks-netizen.github.io/product-images/L21549-22/2081.jpg,https://oleks-netizen.github.io/product-images/L21549-22/2082.jpg,https://oleks-netizen.github.io/product-images/L21549-22/2083.jpg,https://oleks-netizen.github.io/product-images/L21549-22/2084.jpg,https://oleks-netizen.github.io/product-images/L21549-22/2085.jpg,https://oleks-netizen.github.io/product-images/L21549-22/2086.jpg,https://oleks-netizen.github.io/product-images/L21549-22/2087.jpg</t>
+        </is>
+      </c>
+      <c r="C118" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>L21557-1</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L21557-1/3864.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3865.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3866.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3867.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3868.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3869.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3870.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3871.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3872.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3873.jpg</t>
+        </is>
+      </c>
+      <c r="C119" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>L21557-173</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L21557-173/3476.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3477.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3478.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3479.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3480.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3481.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3482.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3483.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3484.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3485.jpg</t>
+        </is>
+      </c>
+      <c r="C120" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>L21561-1</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L21561-1/2782.jpg,https://oleks-netizen.github.io/product-images/L21561-1/2783.jpg,https://oleks-netizen.github.io/product-images/L21561-1/2784.jpg,https://oleks-netizen.github.io/product-images/L21561-1/2785.jpg,https://oleks-netizen.github.io/product-images/L21561-1/2786.jpg,https://oleks-netizen.github.io/product-images/L21561-1/2787.jpg,https://oleks-netizen.github.io/product-images/L21561-1/2788.jpg,https://oleks-netizen.github.io/product-images/L21561-1/2789.jpg</t>
+        </is>
+      </c>
+      <c r="C121" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>L21561-25</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L21561-25/438.jpg,https://oleks-netizen.github.io/product-images/L21561-25/439.jpg,https://oleks-netizen.github.io/product-images/L21561-25/440.jpg,https://oleks-netizen.github.io/product-images/L21561-25/441.jpg,https://oleks-netizen.github.io/product-images/L21561-25/442.jpg,https://oleks-netizen.github.io/product-images/L21561-25/443.jpg,https://oleks-netizen.github.io/product-images/L21561-25/444.jpg,https://oleks-netizen.github.io/product-images/L21561-25/445.jpg</t>
+        </is>
+      </c>
+      <c r="C122" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>L22007-1K</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22007-1K/4694.jpg,https://oleks-netizen.github.io/product-images/L22007-1K/4695.jpg,https://oleks-netizen.github.io/product-images/L22007-1K/4696.jpg,https://oleks-netizen.github.io/product-images/L22007-1K/4697.jpg,https://oleks-netizen.github.io/product-images/L22007-1K/4698.jpg,https://oleks-netizen.github.io/product-images/L22007-1K/4699.jpg,https://oleks-netizen.github.io/product-images/L22007-1K/4700.jpg,https://oleks-netizen.github.io/product-images/L22007-1K/4701.jpg</t>
+        </is>
+      </c>
+      <c r="C123" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>L22007-3K</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22007-3K/1998.jpg,https://oleks-netizen.github.io/product-images/L22007-3K/1999.jpg,https://oleks-netizen.github.io/product-images/L22007-3K/2000.jpg,https://oleks-netizen.github.io/product-images/L22007-3K/2001.jpg,https://oleks-netizen.github.io/product-images/L22007-3K/2002.jpg,https://oleks-netizen.github.io/product-images/L22007-3K/2003.jpg,https://oleks-netizen.github.io/product-images/L22007-3K/2004.jpg,https://oleks-netizen.github.io/product-images/L22007-3K/2005.jpg</t>
+        </is>
+      </c>
+      <c r="C124" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>L22008-1</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22008-1/5288.jpg,https://oleks-netizen.github.io/product-images/L22008-1/5289.jpg,https://oleks-netizen.github.io/product-images/L22008-1/5290.jpg,https://oleks-netizen.github.io/product-images/L22008-1/5291.jpg,https://oleks-netizen.github.io/product-images/L22008-1/5292.jpg,https://oleks-netizen.github.io/product-images/L22008-1/5293.jpg,https://oleks-netizen.github.io/product-images/L22008-1/5294.jpg,https://oleks-netizen.github.io/product-images/L22008-1/5295.jpg</t>
+        </is>
+      </c>
+      <c r="C125" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>L22008-12</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22008-12/315.jpg,https://oleks-netizen.github.io/product-images/L22008-12/316.jpg,https://oleks-netizen.github.io/product-images/L22008-12/317.jpg,https://oleks-netizen.github.io/product-images/L22008-12/318.jpg,https://oleks-netizen.github.io/product-images/L22008-12/319.jpg,https://oleks-netizen.github.io/product-images/L22008-12/320.jpg,https://oleks-netizen.github.io/product-images/L22008-12/321.jpg</t>
+        </is>
+      </c>
+      <c r="C126" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>L22008-8</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22008-8/5347.jpg,https://oleks-netizen.github.io/product-images/L22008-8/5348.jpg,https://oleks-netizen.github.io/product-images/L22008-8/5349.jpg,https://oleks-netizen.github.io/product-images/L22008-8/5350.jpg,https://oleks-netizen.github.io/product-images/L22008-8/5351.jpg,https://oleks-netizen.github.io/product-images/L22008-8/5352.jpg,https://oleks-netizen.github.io/product-images/L22008-8/5353.jpg,https://oleks-netizen.github.io/product-images/L22008-8/5354.jpg</t>
+        </is>
+      </c>
+      <c r="C127" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>L22009-1</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22009-1/5232.jpg,https://oleks-netizen.github.io/product-images/L22009-1/5233.jpg,https://oleks-netizen.github.io/product-images/L22009-1/5234.jpg,https://oleks-netizen.github.io/product-images/L22009-1/5235.jpg,https://oleks-netizen.github.io/product-images/L22009-1/5236.jpg,https://oleks-netizen.github.io/product-images/L22009-1/5237.jpg,https://oleks-netizen.github.io/product-images/L22009-1/5238.jpg,https://oleks-netizen.github.io/product-images/L22009-1/5239.jpg,https://oleks-netizen.github.io/product-images/L22009-1/5240.jpg</t>
+        </is>
+      </c>
+      <c r="C128" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>L22009-35</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22009-35/2222.jpg,https://oleks-netizen.github.io/product-images/L22009-35/2223.jpg,https://oleks-netizen.github.io/product-images/L22009-35/2224.jpg,https://oleks-netizen.github.io/product-images/L22009-35/2225.jpg,https://oleks-netizen.github.io/product-images/L22009-35/2226.jpg,https://oleks-netizen.github.io/product-images/L22009-35/2227.jpg,https://oleks-netizen.github.io/product-images/L22009-35/2228.jpg,https://oleks-netizen.github.io/product-images/L22009-35/2229.jpg,https://oleks-netizen.github.io/product-images/L22009-35/2230.jpg</t>
+        </is>
+      </c>
+      <c r="C129" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>L22018-2W</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22018-2W/3764.jpg,https://oleks-netizen.github.io/product-images/L22018-2W/3765.jpg</t>
+        </is>
+      </c>
+      <c r="C130" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>L22098-1</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22098-1/2899.jpg,https://oleks-netizen.github.io/product-images/L22098-1/2900.jpg,https://oleks-netizen.github.io/product-images/L22098-1/2901.jpg,https://oleks-netizen.github.io/product-images/L22098-1/2902.jpg,https://oleks-netizen.github.io/product-images/L22098-1/2903.jpg,https://oleks-netizen.github.io/product-images/L22098-1/2904.jpg,https://oleks-netizen.github.io/product-images/L22098-1/2905.jpg</t>
+        </is>
+      </c>
+      <c r="C131" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>L22125-1</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22125-1/3847.jpg,https://oleks-netizen.github.io/product-images/L22125-1/3848.jpg,https://oleks-netizen.github.io/product-images/L22125-1/3849.jpg,https://oleks-netizen.github.io/product-images/L22125-1/3850.jpg,https://oleks-netizen.github.io/product-images/L22125-1/3851.jpg,https://oleks-netizen.github.io/product-images/L22125-1/3852.jpg,https://oleks-netizen.github.io/product-images/L22125-1/3853.jpg,https://oleks-netizen.github.io/product-images/L22125-1/3854.jpg</t>
+        </is>
+      </c>
+      <c r="C132" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>L22125-8</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22125-8/1000.jpg,https://oleks-netizen.github.io/product-images/L22125-8/1001.jpg,https://oleks-netizen.github.io/product-images/L22125-8/1002.jpg,https://oleks-netizen.github.io/product-images/L22125-8/1003.jpg,https://oleks-netizen.github.io/product-images/L22125-8/996.jpg,https://oleks-netizen.github.io/product-images/L22125-8/997.jpg,https://oleks-netizen.github.io/product-images/L22125-8/998.jpg,https://oleks-netizen.github.io/product-images/L22125-8/999.jpg</t>
+        </is>
+      </c>
+      <c r="C133" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>L22162-1W</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22162-1W/3944.jpg,https://oleks-netizen.github.io/product-images/L22162-1W/3945.jpg</t>
+        </is>
+      </c>
+      <c r="C134" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>L22187-1W</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22187-1W/2487.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/2488.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/2489.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/2490.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/2491.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/2492.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/2493.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/2494.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/2495.jpg</t>
+        </is>
+      </c>
+      <c r="C135" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>L22187-1X</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22187-1X/1184.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/1185.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/1186.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/1187.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/1188.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/1189.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/1190.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/1191.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/1192.jpg</t>
+        </is>
+      </c>
+      <c r="C136" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>L22322-01</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22322-01/2936.jpg,https://oleks-netizen.github.io/product-images/L22322-01/2937.jpg,https://oleks-netizen.github.io/product-images/L22322-01/2938.jpg,https://oleks-netizen.github.io/product-images/L22322-01/2939.jpg,https://oleks-netizen.github.io/product-images/L22322-01/2940.jpg,https://oleks-netizen.github.io/product-images/L22322-01/2941.jpg,https://oleks-netizen.github.io/product-images/L22322-01/2942.jpg,https://oleks-netizen.github.io/product-images/L22322-01/2943.jpg,https://oleks-netizen.github.io/product-images/L22322-01/2944.jpg</t>
+        </is>
+      </c>
+      <c r="C137" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>L22322-02</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22322-02/5568.jpg,https://oleks-netizen.github.io/product-images/L22322-02/5569.jpg,https://oleks-netizen.github.io/product-images/L22322-02/5570.jpg,https://oleks-netizen.github.io/product-images/L22322-02/5571.jpg,https://oleks-netizen.github.io/product-images/L22322-02/5572.jpg,https://oleks-netizen.github.io/product-images/L22322-02/5573.jpg,https://oleks-netizen.github.io/product-images/L22322-02/5574.jpg,https://oleks-netizen.github.io/product-images/L22322-02/5575.jpg,https://oleks-netizen.github.io/product-images/L22322-02/5576.jpg</t>
+        </is>
+      </c>
+      <c r="C138" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>L22322-1</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22322-1/2650.jpg,https://oleks-netizen.github.io/product-images/L22322-1/2651.jpg,https://oleks-netizen.github.io/product-images/L22322-1/2652.jpg,https://oleks-netizen.github.io/product-images/L22322-1/2653.jpg,https://oleks-netizen.github.io/product-images/L22322-1/2654.jpg,https://oleks-netizen.github.io/product-images/L22322-1/2655.jpg,https://oleks-netizen.github.io/product-images/L22322-1/2656.jpg,https://oleks-netizen.github.io/product-images/L22322-1/2657.jpg,https://oleks-netizen.github.io/product-images/L22322-1/2658.jpg</t>
+        </is>
+      </c>
+      <c r="C139" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>L22322-4</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22322-4/2244.jpg,https://oleks-netizen.github.io/product-images/L22322-4/2245.jpg,https://oleks-netizen.github.io/product-images/L22322-4/2246.jpg,https://oleks-netizen.github.io/product-images/L22322-4/2247.jpg,https://oleks-netizen.github.io/product-images/L22322-4/2248.jpg,https://oleks-netizen.github.io/product-images/L22322-4/2249.jpg,https://oleks-netizen.github.io/product-images/L22322-4/2250.jpg,https://oleks-netizen.github.io/product-images/L22322-4/2251.jpg,https://oleks-netizen.github.io/product-images/L22322-4/2252.jpg</t>
+        </is>
+      </c>
+      <c r="C140" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>L22532-01</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22532-01/760.jpg,https://oleks-netizen.github.io/product-images/L22532-01/761.jpg,https://oleks-netizen.github.io/product-images/L22532-01/762.jpg,https://oleks-netizen.github.io/product-images/L22532-01/763.jpg,https://oleks-netizen.github.io/product-images/L22532-01/764.jpg,https://oleks-netizen.github.io/product-images/L22532-01/765.jpg,https://oleks-netizen.github.io/product-images/L22532-01/766.jpg</t>
+        </is>
+      </c>
+      <c r="C141" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>L22532-03</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22532-03/4339.jpg,https://oleks-netizen.github.io/product-images/L22532-03/4340.jpg,https://oleks-netizen.github.io/product-images/L22532-03/4341.jpg,https://oleks-netizen.github.io/product-images/L22532-03/4342.jpg,https://oleks-netizen.github.io/product-images/L22532-03/4343.jpg,https://oleks-netizen.github.io/product-images/L22532-03/4344.jpg,https://oleks-netizen.github.io/product-images/L22532-03/4345.jpg,https://oleks-netizen.github.io/product-images/L22532-03/4346.jpg</t>
+        </is>
+      </c>
+      <c r="C142" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>L22537-179</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22537-179/4308.jpg,https://oleks-netizen.github.io/product-images/L22537-179/4310.jpg,https://oleks-netizen.github.io/product-images/L22537-179/4311.jpg,https://oleks-netizen.github.io/product-images/L22537-179/4312.jpg,https://oleks-netizen.github.io/product-images/L22537-179/4313.jpg,https://oleks-netizen.github.io/product-images/L22537-179/4314.jpg,https://oleks-netizen.github.io/product-images/L22537-179/4315.jpg</t>
+        </is>
+      </c>
+      <c r="C143" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>L22613-1</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22613-1/5577.jpg,https://oleks-netizen.github.io/product-images/L22613-1/5579.jpg,https://oleks-netizen.github.io/product-images/L22613-1/5580.jpg,https://oleks-netizen.github.io/product-images/L22613-1/5581.jpg,https://oleks-netizen.github.io/product-images/L22613-1/5582.jpg,https://oleks-netizen.github.io/product-images/L22613-1/5583.jpg,https://oleks-netizen.github.io/product-images/L22613-1/5584.jpg</t>
+        </is>
+      </c>
+      <c r="C144" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>L22613-2S</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22613-2S/5699.jpg,https://oleks-netizen.github.io/product-images/L22613-2S/5701.jpg,https://oleks-netizen.github.io/product-images/L22613-2S/5702.jpg,https://oleks-netizen.github.io/product-images/L22613-2S/5703.jpg,https://oleks-netizen.github.io/product-images/L22613-2S/5704.jpg,https://oleks-netizen.github.io/product-images/L22613-2S/5705.jpg</t>
+        </is>
+      </c>
+      <c r="C145" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>L22619-1X</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22619-1X/1422.jpg,https://oleks-netizen.github.io/product-images/L22619-1X/1424.jpg,https://oleks-netizen.github.io/product-images/L22619-1X/1425.jpg,https://oleks-netizen.github.io/product-images/L22619-1X/1426.jpg,https://oleks-netizen.github.io/product-images/L22619-1X/1427.jpg,https://oleks-netizen.github.io/product-images/L22619-1X/1428.jpg,https://oleks-netizen.github.io/product-images/L22619-1X/1429.jpg</t>
+        </is>
+      </c>
+      <c r="C146" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>L22661-1</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22661-1/573.jpg,https://oleks-netizen.github.io/product-images/L22661-1/575.jpg,https://oleks-netizen.github.io/product-images/L22661-1/576.jpg,https://oleks-netizen.github.io/product-images/L22661-1/577.jpg,https://oleks-netizen.github.io/product-images/L22661-1/578.jpg,https://oleks-netizen.github.io/product-images/L22661-1/579.jpg</t>
+        </is>
+      </c>
+      <c r="C147" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>L22808-1</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22808-1/145.jpg,https://oleks-netizen.github.io/product-images/L22808-1/147.jpg,https://oleks-netizen.github.io/product-images/L22808-1/148.jpg,https://oleks-netizen.github.io/product-images/L22808-1/149.jpg,https://oleks-netizen.github.io/product-images/L22808-1/150.jpg,https://oleks-netizen.github.io/product-images/L22808-1/151.jpg</t>
+        </is>
+      </c>
+      <c r="C148" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>L22808-1W</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22808-1W/5535.jpg,https://oleks-netizen.github.io/product-images/L22808-1W/5537.jpg,https://oleks-netizen.github.io/product-images/L22808-1W/5538.jpg,https://oleks-netizen.github.io/product-images/L22808-1W/5539.jpg,https://oleks-netizen.github.io/product-images/L22808-1W/5540.jpg,https://oleks-netizen.github.io/product-images/L22808-1W/5541.jpg</t>
+        </is>
+      </c>
+      <c r="C149" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>L22813-04S</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22813-04S/1952.jpg,https://oleks-netizen.github.io/product-images/L22813-04S/1954.jpg,https://oleks-netizen.github.io/product-images/L22813-04S/1955.jpg,https://oleks-netizen.github.io/product-images/L22813-04S/1956.jpg,https://oleks-netizen.github.io/product-images/L22813-04S/1957.jpg,https://oleks-netizen.github.io/product-images/L22813-04S/1958.jpg,https://oleks-netizen.github.io/product-images/L22813-04S/1959.jpg</t>
+        </is>
+      </c>
+      <c r="C150" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>L22813-05S</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22813-05S/2519.jpg,https://oleks-netizen.github.io/product-images/L22813-05S/2521.jpg,https://oleks-netizen.github.io/product-images/L22813-05S/2522.jpg,https://oleks-netizen.github.io/product-images/L22813-05S/2523.jpg,https://oleks-netizen.github.io/product-images/L22813-05S/2524.jpg,https://oleks-netizen.github.io/product-images/L22813-05S/2525.jpg,https://oleks-netizen.github.io/product-images/L22813-05S/2526.jpg</t>
+        </is>
+      </c>
+      <c r="C151" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>L22902-1C</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22902-1C/5543.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/5545.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/5546.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/5547.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/5548.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/5549.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/5550.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/5551.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/5552.jpg</t>
+        </is>
+      </c>
+      <c r="C152" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>L22916-5W</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L22916-5W/5707.jpg,https://oleks-netizen.github.io/product-images/L22916-5W/5710.jpg,https://oleks-netizen.github.io/product-images/L22916-5W/5711.jpg,https://oleks-netizen.github.io/product-images/L22916-5W/5712.jpg,https://oleks-netizen.github.io/product-images/L22916-5W/5713.jpg,https://oleks-netizen.github.io/product-images/L22916-5W/5714.jpg</t>
+        </is>
+      </c>
+      <c r="C153" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>L26003-1</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L26003-1/5192.jpg,https://oleks-netizen.github.io/product-images/L26003-1/5194.jpg,https://oleks-netizen.github.io/product-images/L26003-1/5195.jpg,https://oleks-netizen.github.io/product-images/L26003-1/5196.jpg,https://oleks-netizen.github.io/product-images/L26003-1/5197.jpg,https://oleks-netizen.github.io/product-images/L26003-1/5198.jpg</t>
+        </is>
+      </c>
+      <c r="C154" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>L26018-1</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L26018-1/4039.jpg,https://oleks-netizen.github.io/product-images/L26018-1/4041.jpg,https://oleks-netizen.github.io/product-images/L26018-1/4042.jpg,https://oleks-netizen.github.io/product-images/L26018-1/4043.jpg,https://oleks-netizen.github.io/product-images/L26018-1/4044.jpg,https://oleks-netizen.github.io/product-images/L26018-1/4045.jpg</t>
+        </is>
+      </c>
+      <c r="C155" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>L26290-005</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L26290-005/5655.jpg,https://oleks-netizen.github.io/product-images/L26290-005/5657.jpg,https://oleks-netizen.github.io/product-images/L26290-005/5658.jpg,https://oleks-netizen.github.io/product-images/L26290-005/5659.jpg</t>
+        </is>
+      </c>
+      <c r="C156" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>L26309-005</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L26309-005/4804.jpg,https://oleks-netizen.github.io/product-images/L26309-005/4806.jpg,https://oleks-netizen.github.io/product-images/L26309-005/4807.jpg,https://oleks-netizen.github.io/product-images/L26309-005/4808.jpg,https://oleks-netizen.github.io/product-images/L26309-005/4809.jpg</t>
+        </is>
+      </c>
+      <c r="C157" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>L26321-1</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L26321-1/4175.jpg,https://oleks-netizen.github.io/product-images/L26321-1/4177.jpg,https://oleks-netizen.github.io/product-images/L26321-1/4178.jpg,https://oleks-netizen.github.io/product-images/L26321-1/4179.jpg,https://oleks-netizen.github.io/product-images/L26321-1/4180.jpg,https://oleks-netizen.github.io/product-images/L26321-1/4181.jpg</t>
+        </is>
+      </c>
+      <c r="C158" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>L9902-3C</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L9902-3C/930.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/931.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/932.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/933.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/934.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/935.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/936.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/937.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/938.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/939.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/940.jpg</t>
+        </is>
+      </c>
+      <c r="C159" t="n">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update 2025-11-26 15:55:37
</commit_message>
<xml_diff>
--- a/articles_summary.xlsx
+++ b/articles_summary.xlsx
@@ -446,7 +446,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/0026-2/470.jpg,https://oleks-netizen.github.io/product-images/0026-2/471.jpg,https://oleks-netizen.github.io/product-images/0026-2/472.jpg,https://oleks-netizen.github.io/product-images/0026-2/473.jpg,https://oleks-netizen.github.io/product-images/0026-2/474.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/0026-2/1.jpg,https://oleks-netizen.github.io/product-images/0026-2/470.jpg,https://oleks-netizen.github.io/product-images/0026-2/471.jpg,https://oleks-netizen.github.io/product-images/0026-2/473.jpg,https://oleks-netizen.github.io/product-images/0026-2/474.jpg</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -461,7 +461,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/0026-3/4648.jpg,https://oleks-netizen.github.io/product-images/0026-3/4649.jpg,https://oleks-netizen.github.io/product-images/0026-3/4650.jpg,https://oleks-netizen.github.io/product-images/0026-3/4651.jpg,https://oleks-netizen.github.io/product-images/0026-3/4652.jpg,https://oleks-netizen.github.io/product-images/0026-3/4653.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/0026-3/1.jpg,https://oleks-netizen.github.io/product-images/0026-3/4648.jpg,https://oleks-netizen.github.io/product-images/0026-3/4649.jpg,https://oleks-netizen.github.io/product-images/0026-3/4651.jpg,https://oleks-netizen.github.io/product-images/0026-3/4652.jpg,https://oleks-netizen.github.io/product-images/0026-3/4653.jpg</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -476,7 +476,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/0026-4/2038.jpg,https://oleks-netizen.github.io/product-images/0026-4/2039.jpg,https://oleks-netizen.github.io/product-images/0026-4/2040.jpg,https://oleks-netizen.github.io/product-images/0026-4/2041.jpg,https://oleks-netizen.github.io/product-images/0026-4/2042.jpg,https://oleks-netizen.github.io/product-images/0026-4/2043.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/0026-4/1.jpg,https://oleks-netizen.github.io/product-images/0026-4/2038.jpg,https://oleks-netizen.github.io/product-images/0026-4/2039.jpg,https://oleks-netizen.github.io/product-images/0026-4/2041.jpg,https://oleks-netizen.github.io/product-images/0026-4/2042.jpg,https://oleks-netizen.github.io/product-images/0026-4/2043.jpg</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -491,7 +491,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/0026-5/4516.jpg,https://oleks-netizen.github.io/product-images/0026-5/4517.jpg,https://oleks-netizen.github.io/product-images/0026-5/4518.jpg,https://oleks-netizen.github.io/product-images/0026-5/4519.jpg,https://oleks-netizen.github.io/product-images/0026-5/4520.jpg,https://oleks-netizen.github.io/product-images/0026-5/4521.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/0026-5/1.jpg,https://oleks-netizen.github.io/product-images/0026-5/4516.jpg,https://oleks-netizen.github.io/product-images/0026-5/4517.jpg,https://oleks-netizen.github.io/product-images/0026-5/4519.jpg,https://oleks-netizen.github.io/product-images/0026-5/4520.jpg,https://oleks-netizen.github.io/product-images/0026-5/4521.jpg</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -506,7 +506,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/0026-6/3717.jpg,https://oleks-netizen.github.io/product-images/0026-6/3718.jpg,https://oleks-netizen.github.io/product-images/0026-6/3719.jpg,https://oleks-netizen.github.io/product-images/0026-6/3720.jpg,https://oleks-netizen.github.io/product-images/0026-6/3721.jpg,https://oleks-netizen.github.io/product-images/0026-6/3722.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/0026-6/1.jpg,https://oleks-netizen.github.io/product-images/0026-6/3717.jpg,https://oleks-netizen.github.io/product-images/0026-6/3718.jpg,https://oleks-netizen.github.io/product-images/0026-6/3720.jpg,https://oleks-netizen.github.io/product-images/0026-6/3721.jpg,https://oleks-netizen.github.io/product-images/0026-6/3722.jpg</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -521,7 +521,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/0026-7/543.jpg,https://oleks-netizen.github.io/product-images/0026-7/544.jpg,https://oleks-netizen.github.io/product-images/0026-7/545.jpg,https://oleks-netizen.github.io/product-images/0026-7/546.jpg,https://oleks-netizen.github.io/product-images/0026-7/547.jpg,https://oleks-netizen.github.io/product-images/0026-7/548.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/0026-7/1.jpg,https://oleks-netizen.github.io/product-images/0026-7/543.jpg,https://oleks-netizen.github.io/product-images/0026-7/544.jpg,https://oleks-netizen.github.io/product-images/0026-7/546.jpg,https://oleks-netizen.github.io/product-images/0026-7/547.jpg,https://oleks-netizen.github.io/product-images/0026-7/548.jpg</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -536,7 +536,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/0039-3/5398.jpg,https://oleks-netizen.github.io/product-images/0039-3/5399.jpg,https://oleks-netizen.github.io/product-images/0039-3/5400.jpg,https://oleks-netizen.github.io/product-images/0039-3/5401.jpg,https://oleks-netizen.github.io/product-images/0039-3/5402.jpg,https://oleks-netizen.github.io/product-images/0039-3/5403.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/0039-3/1.jpg,https://oleks-netizen.github.io/product-images/0039-3/5398.jpg,https://oleks-netizen.github.io/product-images/0039-3/5399.jpg,https://oleks-netizen.github.io/product-images/0039-3/5401.jpg,https://oleks-netizen.github.io/product-images/0039-3/5402.jpg,https://oleks-netizen.github.io/product-images/0039-3/5403.jpg</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -551,7 +551,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/005/2504.jpg,https://oleks-netizen.github.io/product-images/005/2505.jpg,https://oleks-netizen.github.io/product-images/005/2506.jpg,https://oleks-netizen.github.io/product-images/005/2507.jpg,https://oleks-netizen.github.io/product-images/005/2508.jpg,https://oleks-netizen.github.io/product-images/005/2509.jpg,https://oleks-netizen.github.io/product-images/005/2510.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/005/1.jpg,https://oleks-netizen.github.io/product-images/005/2504.jpg,https://oleks-netizen.github.io/product-images/005/2505.jpg,https://oleks-netizen.github.io/product-images/005/2507.jpg,https://oleks-netizen.github.io/product-images/005/2508.jpg,https://oleks-netizen.github.io/product-images/005/2509.jpg,https://oleks-netizen.github.io/product-images/005/2510.jpg</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -566,7 +566,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/009-2/1144.jpg,https://oleks-netizen.github.io/product-images/009-2/1145.jpg,https://oleks-netizen.github.io/product-images/009-2/1146.jpg,https://oleks-netizen.github.io/product-images/009-2/1147.jpg,https://oleks-netizen.github.io/product-images/009-2/1148.jpg,https://oleks-netizen.github.io/product-images/009-2/1149.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/009-2/1144.jpg,https://oleks-netizen.github.io/product-images/009-2/1145.jpg,https://oleks-netizen.github.io/product-images/009-2/1147.jpg,https://oleks-netizen.github.io/product-images/009-2/1148.jpg,https://oleks-netizen.github.io/product-images/009-2/1149.jpg,https://oleks-netizen.github.io/product-images/009-2/1.jpg</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -581,7 +581,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/009-4/1769.jpg,https://oleks-netizen.github.io/product-images/009-4/1770.jpg,https://oleks-netizen.github.io/product-images/009-4/1771.jpg,https://oleks-netizen.github.io/product-images/009-4/1772.jpg,https://oleks-netizen.github.io/product-images/009-4/1773.jpg,https://oleks-netizen.github.io/product-images/009-4/1774.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/009-4/1769.jpg,https://oleks-netizen.github.io/product-images/009-4/1770.jpg,https://oleks-netizen.github.io/product-images/009-4/1772.jpg,https://oleks-netizen.github.io/product-images/009-4/1773.jpg,https://oleks-netizen.github.io/product-images/009-4/1774.jpg,https://oleks-netizen.github.io/product-images/009-4/1.jpg</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -596,7 +596,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/1809-black/5770.jpg,https://oleks-netizen.github.io/product-images/1809-black/5771.jpg,https://oleks-netizen.github.io/product-images/1809-black/5772.jpg,https://oleks-netizen.github.io/product-images/1809-black/5773.jpg,https://oleks-netizen.github.io/product-images/1809-black/5774.jpg,https://oleks-netizen.github.io/product-images/1809-black/5775.jpg,https://oleks-netizen.github.io/product-images/1809-black/5776.jpg,https://oleks-netizen.github.io/product-images/1809-black/5777.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/1809-black/1.jpg,https://oleks-netizen.github.io/product-images/1809-black/5770.jpg,https://oleks-netizen.github.io/product-images/1809-black/5771.jpg,https://oleks-netizen.github.io/product-images/1809-black/5773.jpg,https://oleks-netizen.github.io/product-images/1809-black/5774.jpg,https://oleks-netizen.github.io/product-images/1809-black/5775.jpg,https://oleks-netizen.github.io/product-images/1809-black/5776.jpg,https://oleks-netizen.github.io/product-images/1809-black/5777.jpg</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -611,7 +611,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/1809-grey/5152.jpg,https://oleks-netizen.github.io/product-images/1809-grey/5153.jpg,https://oleks-netizen.github.io/product-images/1809-grey/5154.jpg,https://oleks-netizen.github.io/product-images/1809-grey/5155.jpg,https://oleks-netizen.github.io/product-images/1809-grey/5156.jpg,https://oleks-netizen.github.io/product-images/1809-grey/5157.jpg,https://oleks-netizen.github.io/product-images/1809-grey/5158.jpg,https://oleks-netizen.github.io/product-images/1809-grey/5159.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/1809-grey/1.jpg,https://oleks-netizen.github.io/product-images/1809-grey/5152.jpg,https://oleks-netizen.github.io/product-images/1809-grey/5153.jpg,https://oleks-netizen.github.io/product-images/1809-grey/5155.jpg,https://oleks-netizen.github.io/product-images/1809-grey/5156.jpg,https://oleks-netizen.github.io/product-images/1809-grey/5157.jpg,https://oleks-netizen.github.io/product-images/1809-grey/5158.jpg,https://oleks-netizen.github.io/product-images/1809-grey/5159.jpg</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -626,7 +626,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/509-black/791.jpg,https://oleks-netizen.github.io/product-images/509-black/792.jpg,https://oleks-netizen.github.io/product-images/509-black/793.jpg,https://oleks-netizen.github.io/product-images/509-black/794.jpg,https://oleks-netizen.github.io/product-images/509-black/795.jpg,https://oleks-netizen.github.io/product-images/509-black/796.jpg,https://oleks-netizen.github.io/product-images/509-black/797.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/509-black/1.jpg,https://oleks-netizen.github.io/product-images/509-black/791.jpg,https://oleks-netizen.github.io/product-images/509-black/792.jpg,https://oleks-netizen.github.io/product-images/509-black/794.jpg,https://oleks-netizen.github.io/product-images/509-black/795.jpg,https://oleks-netizen.github.io/product-images/509-black/796.jpg,https://oleks-netizen.github.io/product-images/509-black/797.jpg</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -641,7 +641,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/509-green/4476.jpg,https://oleks-netizen.github.io/product-images/509-green/4477.jpg,https://oleks-netizen.github.io/product-images/509-green/4478.jpg,https://oleks-netizen.github.io/product-images/509-green/4479.jpg,https://oleks-netizen.github.io/product-images/509-green/4480.jpg,https://oleks-netizen.github.io/product-images/509-green/4481.jpg,https://oleks-netizen.github.io/product-images/509-green/4482.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/509-green/1.jpg,https://oleks-netizen.github.io/product-images/509-green/4476.jpg,https://oleks-netizen.github.io/product-images/509-green/4477.jpg,https://oleks-netizen.github.io/product-images/509-green/4479.jpg,https://oleks-netizen.github.io/product-images/509-green/4480.jpg,https://oleks-netizen.github.io/product-images/509-green/4481.jpg,https://oleks-netizen.github.io/product-images/509-green/4482.jpg</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -656,7 +656,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/6098-black/4843.jpg,https://oleks-netizen.github.io/product-images/6098-black/4844.jpg,https://oleks-netizen.github.io/product-images/6098-black/4845.jpg,https://oleks-netizen.github.io/product-images/6098-black/4846.jpg,https://oleks-netizen.github.io/product-images/6098-black/4847.jpg,https://oleks-netizen.github.io/product-images/6098-black/4848.jpg,https://oleks-netizen.github.io/product-images/6098-black/4849.jpg,https://oleks-netizen.github.io/product-images/6098-black/4850.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/6098-black/1.jpg,https://oleks-netizen.github.io/product-images/6098-black/4843.jpg,https://oleks-netizen.github.io/product-images/6098-black/4844.jpg,https://oleks-netizen.github.io/product-images/6098-black/4846.jpg,https://oleks-netizen.github.io/product-images/6098-black/4847.jpg,https://oleks-netizen.github.io/product-images/6098-black/4848.jpg,https://oleks-netizen.github.io/product-images/6098-black/4849.jpg,https://oleks-netizen.github.io/product-images/6098-black/4850.jpg</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -671,7 +671,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/6098-green-kam/3909.jpg,https://oleks-netizen.github.io/product-images/6098-green-kam/3910.jpg,https://oleks-netizen.github.io/product-images/6098-green-kam/3911.jpg,https://oleks-netizen.github.io/product-images/6098-green-kam/3912.jpg,https://oleks-netizen.github.io/product-images/6098-green-kam/3913.jpg,https://oleks-netizen.github.io/product-images/6098-green-kam/3914.jpg,https://oleks-netizen.github.io/product-images/6098-green-kam/3915.jpg,https://oleks-netizen.github.io/product-images/6098-green-kam/3916.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/6098-green-kam/1.jpg,https://oleks-netizen.github.io/product-images/6098-green-kam/3909.jpg,https://oleks-netizen.github.io/product-images/6098-green-kam/3910.jpg,https://oleks-netizen.github.io/product-images/6098-green-kam/3912.jpg,https://oleks-netizen.github.io/product-images/6098-green-kam/3913.jpg,https://oleks-netizen.github.io/product-images/6098-green-kam/3914.jpg,https://oleks-netizen.github.io/product-images/6098-green-kam/3915.jpg,https://oleks-netizen.github.io/product-images/6098-green-kam/3916.jpg</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -686,7 +686,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/6836-black/5143.jpg,https://oleks-netizen.github.io/product-images/6836-black/5144.jpg,https://oleks-netizen.github.io/product-images/6836-black/5145.jpg,https://oleks-netizen.github.io/product-images/6836-black/5146.jpg,https://oleks-netizen.github.io/product-images/6836-black/5147.jpg,https://oleks-netizen.github.io/product-images/6836-black/5148.jpg,https://oleks-netizen.github.io/product-images/6836-black/5149.jpg,https://oleks-netizen.github.io/product-images/6836-black/5150.jpg,https://oleks-netizen.github.io/product-images/6836-black/5151.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/6836-black/1.jpg,https://oleks-netizen.github.io/product-images/6836-black/5143.jpg,https://oleks-netizen.github.io/product-images/6836-black/5144.jpg,https://oleks-netizen.github.io/product-images/6836-black/5146.jpg,https://oleks-netizen.github.io/product-images/6836-black/5147.jpg,https://oleks-netizen.github.io/product-images/6836-black/5148.jpg,https://oleks-netizen.github.io/product-images/6836-black/5149.jpg,https://oleks-netizen.github.io/product-images/6836-black/5150.jpg,https://oleks-netizen.github.io/product-images/6836-black/5151.jpg</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -701,7 +701,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/7631-black/2368.jpg,https://oleks-netizen.github.io/product-images/7631-black/2369.jpg,https://oleks-netizen.github.io/product-images/7631-black/2370.jpg,https://oleks-netizen.github.io/product-images/7631-black/2371.jpg,https://oleks-netizen.github.io/product-images/7631-black/2372.jpg,https://oleks-netizen.github.io/product-images/7631-black/2373.jpg,https://oleks-netizen.github.io/product-images/7631-black/2374.jpg,https://oleks-netizen.github.io/product-images/7631-black/2375.jpg,https://oleks-netizen.github.io/product-images/7631-black/2376.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/7631-black/1.jpg,https://oleks-netizen.github.io/product-images/7631-black/2368.jpg,https://oleks-netizen.github.io/product-images/7631-black/2369.jpg,https://oleks-netizen.github.io/product-images/7631-black/2371.jpg,https://oleks-netizen.github.io/product-images/7631-black/2372.jpg,https://oleks-netizen.github.io/product-images/7631-black/2373.jpg,https://oleks-netizen.github.io/product-images/7631-black/2374.jpg,https://oleks-netizen.github.io/product-images/7631-black/2375.jpg,https://oleks-netizen.github.io/product-images/7631-black/2376.jpg</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -716,7 +716,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C-8460A-grey/4594.jpg,https://oleks-netizen.github.io/product-images/C-8460A-grey/4595.jpg,https://oleks-netizen.github.io/product-images/C-8460A-grey/4596.jpg,https://oleks-netizen.github.io/product-images/C-8460A-grey/4597.jpg,https://oleks-netizen.github.io/product-images/C-8460A-grey/4598.jpg,https://oleks-netizen.github.io/product-images/C-8460A-grey/4599.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C-8460A-grey/1.jpg,https://oleks-netizen.github.io/product-images/C-8460A-grey/4594.jpg,https://oleks-netizen.github.io/product-images/C-8460A-grey/4596.jpg,https://oleks-netizen.github.io/product-images/C-8460A-grey/4597.jpg,https://oleks-netizen.github.io/product-images/C-8460A-grey/4598.jpg,https://oleks-netizen.github.io/product-images/C-8460A-grey/4599.jpg</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -731,7 +731,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C-8460A-pink/5728.jpg,https://oleks-netizen.github.io/product-images/C-8460A-pink/5729.jpg,https://oleks-netizen.github.io/product-images/C-8460A-pink/5730.jpg,https://oleks-netizen.github.io/product-images/C-8460A-pink/5731.jpg,https://oleks-netizen.github.io/product-images/C-8460A-pink/5732.jpg,https://oleks-netizen.github.io/product-images/C-8460A-pink/5733.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C-8460A-pink/1.jpg,https://oleks-netizen.github.io/product-images/C-8460A-pink/5728.jpg,https://oleks-netizen.github.io/product-images/C-8460A-pink/5730.jpg,https://oleks-netizen.github.io/product-images/C-8460A-pink/5731.jpg,https://oleks-netizen.github.io/product-images/C-8460A-pink/5732.jpg,https://oleks-netizen.github.io/product-images/C-8460A-pink/5733.jpg</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -746,7 +746,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C-8460A-silvery-grey/2183.jpg,https://oleks-netizen.github.io/product-images/C-8460A-silvery-grey/2184.jpg,https://oleks-netizen.github.io/product-images/C-8460A-silvery-grey/2185.jpg,https://oleks-netizen.github.io/product-images/C-8460A-silvery-grey/2186.jpg,https://oleks-netizen.github.io/product-images/C-8460A-silvery-grey/2187.jpg,https://oleks-netizen.github.io/product-images/C-8460A-silvery-grey/2188.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C-8460A-silvery-grey/1.jpg,https://oleks-netizen.github.io/product-images/C-8460A-silvery-grey/2183.jpg,https://oleks-netizen.github.io/product-images/C-8460A-silvery-grey/2185.jpg,https://oleks-netizen.github.io/product-images/C-8460A-silvery-grey/2186.jpg,https://oleks-netizen.github.io/product-images/C-8460A-silvery-grey/2187.jpg,https://oleks-netizen.github.io/product-images/C-8460A-silvery-grey/2188.jpg</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -761,7 +761,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C-8460B-black/1627.jpg,https://oleks-netizen.github.io/product-images/C-8460B-black/1628.jpg,https://oleks-netizen.github.io/product-images/C-8460B-black/1629.jpg,https://oleks-netizen.github.io/product-images/C-8460B-black/1630.jpg,https://oleks-netizen.github.io/product-images/C-8460B-black/1631.jpg,https://oleks-netizen.github.io/product-images/C-8460B-black/1632.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C-8460B-black/1627.jpg,https://oleks-netizen.github.io/product-images/C-8460B-black/1629.jpg,https://oleks-netizen.github.io/product-images/C-8460B-black/1630.jpg,https://oleks-netizen.github.io/product-images/C-8460B-black/1631.jpg,https://oleks-netizen.github.io/product-images/C-8460B-black/1632.jpg,https://oleks-netizen.github.io/product-images/C-8460B-black/1.jpg</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -776,7 +776,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C-8460B-green/3881.jpg,https://oleks-netizen.github.io/product-images/C-8460B-green/3882.jpg,https://oleks-netizen.github.io/product-images/C-8460B-green/3883.jpg,https://oleks-netizen.github.io/product-images/C-8460B-green/3884.jpg,https://oleks-netizen.github.io/product-images/C-8460B-green/3885.jpg,https://oleks-netizen.github.io/product-images/C-8460B-green/3886.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C-8460B-green/1.jpg,https://oleks-netizen.github.io/product-images/C-8460B-green/3881.jpg,https://oleks-netizen.github.io/product-images/C-8460B-green/3883.jpg,https://oleks-netizen.github.io/product-images/C-8460B-green/3884.jpg,https://oleks-netizen.github.io/product-images/C-8460B-green/3885.jpg,https://oleks-netizen.github.io/product-images/C-8460B-green/3886.jpg</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -791,7 +791,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C-8460B-grey/5445.jpg,https://oleks-netizen.github.io/product-images/C-8460B-grey/5446.jpg,https://oleks-netizen.github.io/product-images/C-8460B-grey/5447.jpg,https://oleks-netizen.github.io/product-images/C-8460B-grey/5448.jpg,https://oleks-netizen.github.io/product-images/C-8460B-grey/5449.jpg,https://oleks-netizen.github.io/product-images/C-8460B-grey/5450.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C-8460B-grey/1.jpg,https://oleks-netizen.github.io/product-images/C-8460B-grey/5445.jpg,https://oleks-netizen.github.io/product-images/C-8460B-grey/5447.jpg,https://oleks-netizen.github.io/product-images/C-8460B-grey/5448.jpg,https://oleks-netizen.github.io/product-images/C-8460B-grey/5449.jpg,https://oleks-netizen.github.io/product-images/C-8460B-grey/5450.jpg</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -806,7 +806,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C-8460B-khaki/4282.jpg,https://oleks-netizen.github.io/product-images/C-8460B-khaki/4283.jpg,https://oleks-netizen.github.io/product-images/C-8460B-khaki/4284.jpg,https://oleks-netizen.github.io/product-images/C-8460B-khaki/4285.jpg,https://oleks-netizen.github.io/product-images/C-8460B-khaki/4286.jpg,https://oleks-netizen.github.io/product-images/C-8460B-khaki/4287.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C-8460B-khaki/1.jpg,https://oleks-netizen.github.io/product-images/C-8460B-khaki/4282.jpg,https://oleks-netizen.github.io/product-images/C-8460B-khaki/4284.jpg,https://oleks-netizen.github.io/product-images/C-8460B-khaki/4285.jpg,https://oleks-netizen.github.io/product-images/C-8460B-khaki/4286.jpg,https://oleks-netizen.github.io/product-images/C-8460B-khaki/4287.jpg</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -821,7 +821,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C-8460B-red/2231.jpg,https://oleks-netizen.github.io/product-images/C-8460B-red/2232.jpg,https://oleks-netizen.github.io/product-images/C-8460B-red/2233.jpg,https://oleks-netizen.github.io/product-images/C-8460B-red/2234.jpg,https://oleks-netizen.github.io/product-images/C-8460B-red/2235.jpg,https://oleks-netizen.github.io/product-images/C-8460B-red/2236.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C-8460B-red/1.jpg,https://oleks-netizen.github.io/product-images/C-8460B-red/2231.jpg,https://oleks-netizen.github.io/product-images/C-8460B-red/2233.jpg,https://oleks-netizen.github.io/product-images/C-8460B-red/2234.jpg,https://oleks-netizen.github.io/product-images/C-8460B-red/2235.jpg,https://oleks-netizen.github.io/product-images/C-8460B-red/2236.jpg</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -836,7 +836,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C-8998-black/3443.jpg,https://oleks-netizen.github.io/product-images/C-8998-black/3444.jpg,https://oleks-netizen.github.io/product-images/C-8998-black/3445.jpg,https://oleks-netizen.github.io/product-images/C-8998-black/3446.jpg,https://oleks-netizen.github.io/product-images/C-8998-black/3447.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C-8998-black/1.jpg,https://oleks-netizen.github.io/product-images/C-8998-black/3444.jpg,https://oleks-netizen.github.io/product-images/C-8998-black/3445.jpg,https://oleks-netizen.github.io/product-images/C-8998-black/3446.jpg,https://oleks-netizen.github.io/product-images/C-8998-black/3447.jpg</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -851,7 +851,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C-8998-dark-green/4886.jpg,https://oleks-netizen.github.io/product-images/C-8998-dark-green/4887.jpg,https://oleks-netizen.github.io/product-images/C-8998-dark-green/4888.jpg,https://oleks-netizen.github.io/product-images/C-8998-dark-green/4889.jpg,https://oleks-netizen.github.io/product-images/C-8998-dark-green/4890.jpg,https://oleks-netizen.github.io/product-images/C-8998-dark-green/4891.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C-8998-dark-green/1.jpg,https://oleks-netizen.github.io/product-images/C-8998-dark-green/4886.jpg,https://oleks-netizen.github.io/product-images/C-8998-dark-green/4888.jpg,https://oleks-netizen.github.io/product-images/C-8998-dark-green/4889.jpg,https://oleks-netizen.github.io/product-images/C-8998-dark-green/4890.jpg,https://oleks-netizen.github.io/product-images/C-8998-dark-green/4891.jpg</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -866,7 +866,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C-8998-lime green/1313.jpg,https://oleks-netizen.github.io/product-images/C-8998-lime green/1314.jpg,https://oleks-netizen.github.io/product-images/C-8998-lime green/1315.jpg,https://oleks-netizen.github.io/product-images/C-8998-lime green/1316.jpg,https://oleks-netizen.github.io/product-images/C-8998-lime green/1317.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C-8998-lime green/1313.jpg,https://oleks-netizen.github.io/product-images/C-8998-lime green/1315.jpg,https://oleks-netizen.github.io/product-images/C-8998-lime green/1316.jpg,https://oleks-netizen.github.io/product-images/C-8998-lime green/1317.jpg,https://oleks-netizen.github.io/product-images/C-8998-lime green/1.jpg</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -881,7 +881,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C-8998-pink/5274.jpg,https://oleks-netizen.github.io/product-images/C-8998-pink/5275.jpg,https://oleks-netizen.github.io/product-images/C-8998-pink/5276.jpg,https://oleks-netizen.github.io/product-images/C-8998-pink/5277.jpg,https://oleks-netizen.github.io/product-images/C-8998-pink/5278.jpg,https://oleks-netizen.github.io/product-images/C-8998-pink/5279.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C-8998-pink/1.jpg,https://oleks-netizen.github.io/product-images/C-8998-pink/5275.jpg,https://oleks-netizen.github.io/product-images/C-8998-pink/5276.jpg,https://oleks-netizen.github.io/product-images/C-8998-pink/5277.jpg,https://oleks-netizen.github.io/product-images/C-8998-pink/5278.jpg,https://oleks-netizen.github.io/product-images/C-8998-pink/5279.jpg</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -896,7 +896,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DRL19001-1/2864.jpg,https://oleks-netizen.github.io/product-images/DRL19001-1/2865.jpg,https://oleks-netizen.github.io/product-images/DRL19001-1/2866.jpg,https://oleks-netizen.github.io/product-images/DRL19001-1/2867.jpg,https://oleks-netizen.github.io/product-images/DRL19001-1/2868.jpg,https://oleks-netizen.github.io/product-images/DRL19001-1/2869.jpg,https://oleks-netizen.github.io/product-images/DRL19001-1/2870.jpg,https://oleks-netizen.github.io/product-images/DRL19001-1/2871.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL19001-1/1.jpg,https://oleks-netizen.github.io/product-images/DRL19001-1/2864.jpg,https://oleks-netizen.github.io/product-images/DRL19001-1/2865.jpg,https://oleks-netizen.github.io/product-images/DRL19001-1/2867.jpg,https://oleks-netizen.github.io/product-images/DRL19001-1/2868.jpg,https://oleks-netizen.github.io/product-images/DRL19001-1/2869.jpg,https://oleks-netizen.github.io/product-images/DRL19001-1/2870.jpg,https://oleks-netizen.github.io/product-images/DRL19001-1/2871.jpg</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -911,7 +911,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DRL19012-1/5981.jpg,https://oleks-netizen.github.io/product-images/DRL19012-1/5982.jpg,https://oleks-netizen.github.io/product-images/DRL19012-1/5983.jpg,https://oleks-netizen.github.io/product-images/DRL19012-1/5984.jpg,https://oleks-netizen.github.io/product-images/DRL19012-1/5985.jpg,https://oleks-netizen.github.io/product-images/DRL19012-1/5986.jpg,https://oleks-netizen.github.io/product-images/DRL19012-1/5987.jpg,https://oleks-netizen.github.io/product-images/DRL19012-1/5988.jpg,https://oleks-netizen.github.io/product-images/DRL19012-1/5989.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL19012-1/1.jpg,https://oleks-netizen.github.io/product-images/DRL19012-1/5981.jpg,https://oleks-netizen.github.io/product-images/DRL19012-1/5982.jpg,https://oleks-netizen.github.io/product-images/DRL19012-1/5984.jpg,https://oleks-netizen.github.io/product-images/DRL19012-1/5985.jpg,https://oleks-netizen.github.io/product-images/DRL19012-1/5986.jpg,https://oleks-netizen.github.io/product-images/DRL19012-1/5987.jpg,https://oleks-netizen.github.io/product-images/DRL19012-1/5988.jpg,https://oleks-netizen.github.io/product-images/DRL19012-1/5989.jpg</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -926,7 +926,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DRL19077-1/4120.jpg,https://oleks-netizen.github.io/product-images/DRL19077-1/4121.jpg,https://oleks-netizen.github.io/product-images/DRL19077-1/4122.jpg,https://oleks-netizen.github.io/product-images/DRL19077-1/4123.jpg,https://oleks-netizen.github.io/product-images/DRL19077-1/4124.jpg,https://oleks-netizen.github.io/product-images/DRL19077-1/4125.jpg,https://oleks-netizen.github.io/product-images/DRL19077-1/4126.jpg,https://oleks-netizen.github.io/product-images/DRL19077-1/4127.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL19077-1/1.jpg,https://oleks-netizen.github.io/product-images/DRL19077-1/4120.jpg,https://oleks-netizen.github.io/product-images/DRL19077-1/4121.jpg,https://oleks-netizen.github.io/product-images/DRL19077-1/4123.jpg,https://oleks-netizen.github.io/product-images/DRL19077-1/4124.jpg,https://oleks-netizen.github.io/product-images/DRL19077-1/4125.jpg,https://oleks-netizen.github.io/product-images/DRL19077-1/4126.jpg,https://oleks-netizen.github.io/product-images/DRL19077-1/4127.jpg</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -941,7 +941,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DRL19092-1/4796.jpg,https://oleks-netizen.github.io/product-images/DRL19092-1/4797.jpg,https://oleks-netizen.github.io/product-images/DRL19092-1/4798.jpg,https://oleks-netizen.github.io/product-images/DRL19092-1/4799.jpg,https://oleks-netizen.github.io/product-images/DRL19092-1/4800.jpg,https://oleks-netizen.github.io/product-images/DRL19092-1/4801.jpg,https://oleks-netizen.github.io/product-images/DRL19092-1/4802.jpg,https://oleks-netizen.github.io/product-images/DRL19092-1/4803.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL19092-1/1.jpg,https://oleks-netizen.github.io/product-images/DRL19092-1/4796.jpg,https://oleks-netizen.github.io/product-images/DRL19092-1/4797.jpg,https://oleks-netizen.github.io/product-images/DRL19092-1/4799.jpg,https://oleks-netizen.github.io/product-images/DRL19092-1/4800.jpg,https://oleks-netizen.github.io/product-images/DRL19092-1/4801.jpg,https://oleks-netizen.github.io/product-images/DRL19092-1/4802.jpg,https://oleks-netizen.github.io/product-images/DRL19092-1/4803.jpg</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -956,7 +956,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DRL19120-1/4710.jpg,https://oleks-netizen.github.io/product-images/DRL19120-1/4711.jpg,https://oleks-netizen.github.io/product-images/DRL19120-1/4712.jpg,https://oleks-netizen.github.io/product-images/DRL19120-1/4713.jpg,https://oleks-netizen.github.io/product-images/DRL19120-1/4714.jpg,https://oleks-netizen.github.io/product-images/DRL19120-1/4715.jpg,https://oleks-netizen.github.io/product-images/DRL19120-1/4716.jpg,https://oleks-netizen.github.io/product-images/DRL19120-1/4717.jpg,https://oleks-netizen.github.io/product-images/DRL19120-1/4718.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL19120-1/1.jpg,https://oleks-netizen.github.io/product-images/DRL19120-1/4710.jpg,https://oleks-netizen.github.io/product-images/DRL19120-1/4711.jpg,https://oleks-netizen.github.io/product-images/DRL19120-1/4713.jpg,https://oleks-netizen.github.io/product-images/DRL19120-1/4714.jpg,https://oleks-netizen.github.io/product-images/DRL19120-1/4715.jpg,https://oleks-netizen.github.io/product-images/DRL19120-1/4716.jpg,https://oleks-netizen.github.io/product-images/DRL19120-1/4717.jpg,https://oleks-netizen.github.io/product-images/DRL19120-1/4718.jpg</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -971,7 +971,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DRL19122-1/5841.jpg,https://oleks-netizen.github.io/product-images/DRL19122-1/5842.jpg,https://oleks-netizen.github.io/product-images/DRL19122-1/5843.jpg,https://oleks-netizen.github.io/product-images/DRL19122-1/5844.jpg,https://oleks-netizen.github.io/product-images/DRL19122-1/5845.jpg,https://oleks-netizen.github.io/product-images/DRL19122-1/5846.jpg,https://oleks-netizen.github.io/product-images/DRL19122-1/5847.jpg,https://oleks-netizen.github.io/product-images/DRL19122-1/5848.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL19122-1/1.jpg,https://oleks-netizen.github.io/product-images/DRL19122-1/5841.jpg,https://oleks-netizen.github.io/product-images/DRL19122-1/5842.jpg,https://oleks-netizen.github.io/product-images/DRL19122-1/5844.jpg,https://oleks-netizen.github.io/product-images/DRL19122-1/5845.jpg,https://oleks-netizen.github.io/product-images/DRL19122-1/5846.jpg,https://oleks-netizen.github.io/product-images/DRL19122-1/5847.jpg,https://oleks-netizen.github.io/product-images/DRL19122-1/5848.jpg</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -986,7 +986,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DRL19253-1/4719.jpg,https://oleks-netizen.github.io/product-images/DRL19253-1/4720.jpg,https://oleks-netizen.github.io/product-images/DRL19253-1/4721.jpg,https://oleks-netizen.github.io/product-images/DRL19253-1/4722.jpg,https://oleks-netizen.github.io/product-images/DRL19253-1/4723.jpg,https://oleks-netizen.github.io/product-images/DRL19253-1/4724.jpg,https://oleks-netizen.github.io/product-images/DRL19253-1/4725.jpg,https://oleks-netizen.github.io/product-images/DRL19253-1/4726.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL19253-1/1.jpg,https://oleks-netizen.github.io/product-images/DRL19253-1/4719.jpg,https://oleks-netizen.github.io/product-images/DRL19253-1/4720.jpg,https://oleks-netizen.github.io/product-images/DRL19253-1/4722.jpg,https://oleks-netizen.github.io/product-images/DRL19253-1/4723.jpg,https://oleks-netizen.github.io/product-images/DRL19253-1/4724.jpg,https://oleks-netizen.github.io/product-images/DRL19253-1/4725.jpg,https://oleks-netizen.github.io/product-images/DRL19253-1/4726.jpg</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DRL19520-1B/1447.jpg,https://oleks-netizen.github.io/product-images/DRL19520-1B/1448.jpg,https://oleks-netizen.github.io/product-images/DRL19520-1B/1449.jpg,https://oleks-netizen.github.io/product-images/DRL19520-1B/1450.jpg,https://oleks-netizen.github.io/product-images/DRL19520-1B/1451.jpg,https://oleks-netizen.github.io/product-images/DRL19520-1B/1452.jpg,https://oleks-netizen.github.io/product-images/DRL19520-1B/1453.jpg,https://oleks-netizen.github.io/product-images/DRL19520-1B/1454.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL19520-1B/1447.jpg,https://oleks-netizen.github.io/product-images/DRL19520-1B/1448.jpg,https://oleks-netizen.github.io/product-images/DRL19520-1B/1450.jpg,https://oleks-netizen.github.io/product-images/DRL19520-1B/1451.jpg,https://oleks-netizen.github.io/product-images/DRL19520-1B/1452.jpg,https://oleks-netizen.github.io/product-images/DRL19520-1B/1453.jpg,https://oleks-netizen.github.io/product-images/DRL19520-1B/1454.jpg,https://oleks-netizen.github.io/product-images/DRL19520-1B/1.jpg</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -1016,7 +1016,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DRL19601-1/1021.jpg,https://oleks-netizen.github.io/product-images/DRL19601-1/1022.jpg,https://oleks-netizen.github.io/product-images/DRL19601-1/1023.jpg,https://oleks-netizen.github.io/product-images/DRL19601-1/1024.jpg,https://oleks-netizen.github.io/product-images/DRL19601-1/1025.jpg,https://oleks-netizen.github.io/product-images/DRL19601-1/1026.jpg,https://oleks-netizen.github.io/product-images/DRL19601-1/1027.jpg,https://oleks-netizen.github.io/product-images/DRL19601-1/1028.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL19601-1/1021.jpg,https://oleks-netizen.github.io/product-images/DRL19601-1/1022.jpg,https://oleks-netizen.github.io/product-images/DRL19601-1/1024.jpg,https://oleks-netizen.github.io/product-images/DRL19601-1/1025.jpg,https://oleks-netizen.github.io/product-images/DRL19601-1/1026.jpg,https://oleks-netizen.github.io/product-images/DRL19601-1/1027.jpg,https://oleks-netizen.github.io/product-images/DRL19601-1/1028.jpg,https://oleks-netizen.github.io/product-images/DRL19601-1/1.jpg</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -1031,7 +1031,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DRL19712-1/2535.jpg,https://oleks-netizen.github.io/product-images/DRL19712-1/2536.jpg,https://oleks-netizen.github.io/product-images/DRL19712-1/2537.jpg,https://oleks-netizen.github.io/product-images/DRL19712-1/2538.jpg,https://oleks-netizen.github.io/product-images/DRL19712-1/2539.jpg,https://oleks-netizen.github.io/product-images/DRL19712-1/2540.jpg,https://oleks-netizen.github.io/product-images/DRL19712-1/2541.jpg,https://oleks-netizen.github.io/product-images/DRL19712-1/2542.jpg,https://oleks-netizen.github.io/product-images/DRL19712-1/2543.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL19712-1/1.jpg,https://oleks-netizen.github.io/product-images/DRL19712-1/2535.jpg,https://oleks-netizen.github.io/product-images/DRL19712-1/2536.jpg,https://oleks-netizen.github.io/product-images/DRL19712-1/2538.jpg,https://oleks-netizen.github.io/product-images/DRL19712-1/2539.jpg,https://oleks-netizen.github.io/product-images/DRL19712-1/2540.jpg,https://oleks-netizen.github.io/product-images/DRL19712-1/2541.jpg,https://oleks-netizen.github.io/product-images/DRL19712-1/2542.jpg,https://oleks-netizen.github.io/product-images/DRL19712-1/2543.jpg</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DRL19818A-A/1404.jpg,https://oleks-netizen.github.io/product-images/DRL19818A-A/1405.jpg,https://oleks-netizen.github.io/product-images/DRL19818A-A/1406.jpg,https://oleks-netizen.github.io/product-images/DRL19818A-A/1407.jpg,https://oleks-netizen.github.io/product-images/DRL19818A-A/1408.jpg,https://oleks-netizen.github.io/product-images/DRL19818A-A/1409.jpg,https://oleks-netizen.github.io/product-images/DRL19818A-A/1410.jpg,https://oleks-netizen.github.io/product-images/DRL19818A-A/1411.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL19818A-A/1404.jpg,https://oleks-netizen.github.io/product-images/DRL19818A-A/1405.jpg,https://oleks-netizen.github.io/product-images/DRL19818A-A/1407.jpg,https://oleks-netizen.github.io/product-images/DRL19818A-A/1408.jpg,https://oleks-netizen.github.io/product-images/DRL19818A-A/1409.jpg,https://oleks-netizen.github.io/product-images/DRL19818A-A/1410.jpg,https://oleks-netizen.github.io/product-images/DRL19818A-A/1411.jpg,https://oleks-netizen.github.io/product-images/DRL19818A-A/1.jpg</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -1061,7 +1061,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DRL19941-1/741.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/742.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/743.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/744.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/745.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/746.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/747.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/748.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/749.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL19941-1/1.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/741.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/742.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/744.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/745.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/746.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/747.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/748.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/749.jpg</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -1076,7 +1076,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DRL6601-1/816.jpg,https://oleks-netizen.github.io/product-images/DRL6601-1/817.jpg,https://oleks-netizen.github.io/product-images/DRL6601-1/818.jpg,https://oleks-netizen.github.io/product-images/DRL6601-1/819.jpg,https://oleks-netizen.github.io/product-images/DRL6601-1/820.jpg,https://oleks-netizen.github.io/product-images/DRL6601-1/821.jpg,https://oleks-netizen.github.io/product-images/DRL6601-1/822.jpg,https://oleks-netizen.github.io/product-images/DRL6601-1/823.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL6601-1/1.jpg,https://oleks-netizen.github.io/product-images/DRL6601-1/816.jpg,https://oleks-netizen.github.io/product-images/DRL6601-1/817.jpg,https://oleks-netizen.github.io/product-images/DRL6601-1/819.jpg,https://oleks-netizen.github.io/product-images/DRL6601-1/820.jpg,https://oleks-netizen.github.io/product-images/DRL6601-1/821.jpg,https://oleks-netizen.github.io/product-images/DRL6601-1/822.jpg,https://oleks-netizen.github.io/product-images/DRL6601-1/823.jpg</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1091,7 +1091,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DRS16059-1/1854.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1855.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1856.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1857.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1858.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1859.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1860.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1861.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1862.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1863.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRS16059-1/1854.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1855.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1857.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1858.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1859.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1860.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1861.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1862.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1863.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1.jpg</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1106,7 +1106,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DRS16975-1/3087.jpg,https://oleks-netizen.github.io/product-images/DRS16975-1/3088.jpg,https://oleks-netizen.github.io/product-images/DRS16975-1/3089.jpg,https://oleks-netizen.github.io/product-images/DRS16975-1/3090.jpg,https://oleks-netizen.github.io/product-images/DRS16975-1/3091.jpg,https://oleks-netizen.github.io/product-images/DRS16975-1/3092.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRS16975-1/1.jpg,https://oleks-netizen.github.io/product-images/DRS16975-1/3087.jpg,https://oleks-netizen.github.io/product-images/DRS16975-1/3088.jpg,https://oleks-netizen.github.io/product-images/DRS16975-1/3090.jpg,https://oleks-netizen.github.io/product-images/DRS16975-1/3091.jpg,https://oleks-netizen.github.io/product-images/DRS16975-1/3092.jpg</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DRS17116-3/2032.jpg,https://oleks-netizen.github.io/product-images/DRS17116-3/2033.jpg,https://oleks-netizen.github.io/product-images/DRS17116-3/2034.jpg,https://oleks-netizen.github.io/product-images/DRS17116-3/2035.jpg,https://oleks-netizen.github.io/product-images/DRS17116-3/2036.jpg,https://oleks-netizen.github.io/product-images/DRS17116-3/2037.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRS17116-3/1.jpg,https://oleks-netizen.github.io/product-images/DRS17116-3/2032.jpg,https://oleks-netizen.github.io/product-images/DRS17116-3/2033.jpg,https://oleks-netizen.github.io/product-images/DRS17116-3/2035.jpg,https://oleks-netizen.github.io/product-images/DRS17116-3/2036.jpg,https://oleks-netizen.github.io/product-images/DRS17116-3/2037.jpg</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1136,7 +1136,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DRS17131-2/1936.jpg,https://oleks-netizen.github.io/product-images/DRS17131-2/1937.jpg,https://oleks-netizen.github.io/product-images/DRS17131-2/1938.jpg,https://oleks-netizen.github.io/product-images/DRS17131-2/1939.jpg,https://oleks-netizen.github.io/product-images/DRS17131-2/1940.jpg,https://oleks-netizen.github.io/product-images/DRS17131-2/1941.jpg,https://oleks-netizen.github.io/product-images/DRS17131-2/1942.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRS17131-2/1936.jpg,https://oleks-netizen.github.io/product-images/DRS17131-2/1937.jpg,https://oleks-netizen.github.io/product-images/DRS17131-2/1938.jpg,https://oleks-netizen.github.io/product-images/DRS17131-2/1940.jpg,https://oleks-netizen.github.io/product-images/DRS17131-2/1941.jpg,https://oleks-netizen.github.io/product-images/DRS17131-2/1942.jpg,https://oleks-netizen.github.io/product-images/DRS17131-2/1.jpg</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1151,7 +1151,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DRS17132-1/4550.jpg,https://oleks-netizen.github.io/product-images/DRS17132-1/4551.jpg,https://oleks-netizen.github.io/product-images/DRS17132-1/4552.jpg,https://oleks-netizen.github.io/product-images/DRS17132-1/4553.jpg,https://oleks-netizen.github.io/product-images/DRS17132-1/4554.jpg,https://oleks-netizen.github.io/product-images/DRS17132-1/4555.jpg,https://oleks-netizen.github.io/product-images/DRS17132-1/4556.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRS17132-1/1.jpg,https://oleks-netizen.github.io/product-images/DRS17132-1/4550.jpg,https://oleks-netizen.github.io/product-images/DRS17132-1/4551.jpg,https://oleks-netizen.github.io/product-images/DRS17132-1/4552.jpg,https://oleks-netizen.github.io/product-images/DRS17132-1/4554.jpg,https://oleks-netizen.github.io/product-images/DRS17132-1/4555.jpg,https://oleks-netizen.github.io/product-images/DRS17132-1/4556.jpg</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1166,7 +1166,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DRS17203-1/963.jpg,https://oleks-netizen.github.io/product-images/DRS17203-1/964.jpg,https://oleks-netizen.github.io/product-images/DRS17203-1/965.jpg,https://oleks-netizen.github.io/product-images/DRS17203-1/966.jpg,https://oleks-netizen.github.io/product-images/DRS17203-1/967.jpg,https://oleks-netizen.github.io/product-images/DRS17203-1/968.jpg,https://oleks-netizen.github.io/product-images/DRS17203-1/969.jpg,https://oleks-netizen.github.io/product-images/DRS17203-1/970.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRS17203-1/1.jpg,https://oleks-netizen.github.io/product-images/DRS17203-1/963.jpg,https://oleks-netizen.github.io/product-images/DRS17203-1/964.jpg,https://oleks-netizen.github.io/product-images/DRS17203-1/965.jpg,https://oleks-netizen.github.io/product-images/DRS17203-1/967.jpg,https://oleks-netizen.github.io/product-images/DRS17203-1/968.jpg,https://oleks-netizen.github.io/product-images/DRS17203-1/969.jpg,https://oleks-netizen.github.io/product-images/DRS17203-1/970.jpg</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DRS19023-2/2966.jpg,https://oleks-netizen.github.io/product-images/DRS19023-2/2967.jpg,https://oleks-netizen.github.io/product-images/DRS19023-2/2968.jpg,https://oleks-netizen.github.io/product-images/DRS19023-2/2969.jpg,https://oleks-netizen.github.io/product-images/DRS19023-2/2970.jpg,https://oleks-netizen.github.io/product-images/DRS19023-2/2971.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRS19023-2/1.jpg,https://oleks-netizen.github.io/product-images/DRS19023-2/2966.jpg,https://oleks-netizen.github.io/product-images/DRS19023-2/2967.jpg,https://oleks-netizen.github.io/product-images/DRS19023-2/2969.jpg,https://oleks-netizen.github.io/product-images/DRS19023-2/2970.jpg,https://oleks-netizen.github.io/product-images/DRS19023-2/2971.jpg</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1196,7 +1196,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DRS19353-1/1892.jpg,https://oleks-netizen.github.io/product-images/DRS19353-1/1893.jpg,https://oleks-netizen.github.io/product-images/DRS19353-1/1894.jpg,https://oleks-netizen.github.io/product-images/DRS19353-1/1895.jpg,https://oleks-netizen.github.io/product-images/DRS19353-1/1896.jpg,https://oleks-netizen.github.io/product-images/DRS19353-1/1897.jpg,https://oleks-netizen.github.io/product-images/DRS19353-1/1898.jpg,https://oleks-netizen.github.io/product-images/DRS19353-1/1899.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRS19353-1/1892.jpg,https://oleks-netizen.github.io/product-images/DRS19353-1/1893.jpg,https://oleks-netizen.github.io/product-images/DRS19353-1/1895.jpg,https://oleks-netizen.github.io/product-images/DRS19353-1/1896.jpg,https://oleks-netizen.github.io/product-images/DRS19353-1/1897.jpg,https://oleks-netizen.github.io/product-images/DRS19353-1/1898.jpg,https://oleks-netizen.github.io/product-images/DRS19353-1/1899.jpg,https://oleks-netizen.github.io/product-images/DRS19353-1/1.jpg</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1211,7 +1211,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DRS19800-1/6032.jpg,https://oleks-netizen.github.io/product-images/DRS19800-1/6033.jpg,https://oleks-netizen.github.io/product-images/DRS19800-1/6034.jpg,https://oleks-netizen.github.io/product-images/DRS19800-1/6035.jpg,https://oleks-netizen.github.io/product-images/DRS19800-1/6036.jpg,https://oleks-netizen.github.io/product-images/DRS19800-1/6037.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRS19800-1/1.jpg,https://oleks-netizen.github.io/product-images/DRS19800-1/6032.jpg,https://oleks-netizen.github.io/product-images/DRS19800-1/6033.jpg,https://oleks-netizen.github.io/product-images/DRS19800-1/6035.jpg,https://oleks-netizen.github.io/product-images/DRS19800-1/6036.jpg,https://oleks-netizen.github.io/product-images/DRS19800-1/6037.jpg</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DRS19802-1/5802.jpg,https://oleks-netizen.github.io/product-images/DRS19802-1/5803.jpg,https://oleks-netizen.github.io/product-images/DRS19802-1/5804.jpg,https://oleks-netizen.github.io/product-images/DRS19802-1/5805.jpg,https://oleks-netizen.github.io/product-images/DRS19802-1/5806.jpg,https://oleks-netizen.github.io/product-images/DRS19802-1/5807.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRS19802-1/1.jpg,https://oleks-netizen.github.io/product-images/DRS19802-1/5802.jpg,https://oleks-netizen.github.io/product-images/DRS19802-1/5803.jpg,https://oleks-netizen.github.io/product-images/DRS19802-1/5805.jpg,https://oleks-netizen.github.io/product-images/DRS19802-1/5806.jpg,https://oleks-netizen.github.io/product-images/DRS19802-1/5807.jpg</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DS30002-023/2441.jpg,https://oleks-netizen.github.io/product-images/DS30002-023/2442.jpg,https://oleks-netizen.github.io/product-images/DS30002-023/2443.jpg,https://oleks-netizen.github.io/product-images/DS30002-023/2444.jpg,https://oleks-netizen.github.io/product-images/DS30002-023/2445.jpg,https://oleks-netizen.github.io/product-images/DS30002-023/2446.jpg,https://oleks-netizen.github.io/product-images/DS30002-023/2448.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DS30002-023/1.jpg,https://oleks-netizen.github.io/product-images/DS30002-023/2441.jpg,https://oleks-netizen.github.io/product-images/DS30002-023/2442.jpg,https://oleks-netizen.github.io/product-images/DS30002-023/2444.jpg,https://oleks-netizen.github.io/product-images/DS30002-023/2445.jpg,https://oleks-netizen.github.io/product-images/DS30002-023/2446.jpg,https://oleks-netizen.github.io/product-images/DS30002-023/2448.jpg</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -1256,7 +1256,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DS30002-025/4055.jpg,https://oleks-netizen.github.io/product-images/DS30002-025/4056.jpg,https://oleks-netizen.github.io/product-images/DS30002-025/4057.jpg,https://oleks-netizen.github.io/product-images/DS30002-025/4058.jpg,https://oleks-netizen.github.io/product-images/DS30002-025/4059.jpg,https://oleks-netizen.github.io/product-images/DS30002-025/4062.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DS30002-025/1.jpg,https://oleks-netizen.github.io/product-images/DS30002-025/4055.jpg,https://oleks-netizen.github.io/product-images/DS30002-025/4056.jpg,https://oleks-netizen.github.io/product-images/DS30002-025/4058.jpg,https://oleks-netizen.github.io/product-images/DS30002-025/4059.jpg,https://oleks-netizen.github.io/product-images/DS30002-025/4062.jpg</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -1271,7 +1271,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DS30002-112/711.jpg,https://oleks-netizen.github.io/product-images/DS30002-112/712.jpg,https://oleks-netizen.github.io/product-images/DS30002-112/713.jpg,https://oleks-netizen.github.io/product-images/DS30002-112/714.jpg,https://oleks-netizen.github.io/product-images/DS30002-112/715.jpg,https://oleks-netizen.github.io/product-images/DS30002-112/718.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DS30002-112/1.jpg,https://oleks-netizen.github.io/product-images/DS30002-112/711.jpg,https://oleks-netizen.github.io/product-images/DS30002-112/712.jpg,https://oleks-netizen.github.io/product-images/DS30002-112/714.jpg,https://oleks-netizen.github.io/product-images/DS30002-112/715.jpg,https://oleks-netizen.github.io/product-images/DS30002-112/718.jpg</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -1286,7 +1286,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DS30002-132/5381.jpg,https://oleks-netizen.github.io/product-images/DS30002-132/5382.jpg,https://oleks-netizen.github.io/product-images/DS30002-132/5383.jpg,https://oleks-netizen.github.io/product-images/DS30002-132/5384.jpg,https://oleks-netizen.github.io/product-images/DS30002-132/5385.jpg,https://oleks-netizen.github.io/product-images/DS30002-132/5386.jpg,https://oleks-netizen.github.io/product-images/DS30002-132/5387.jpg,https://oleks-netizen.github.io/product-images/DS30002-132/5388.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DS30002-132/1.jpg,https://oleks-netizen.github.io/product-images/DS30002-132/5381.jpg,https://oleks-netizen.github.io/product-images/DS30002-132/5382.jpg,https://oleks-netizen.github.io/product-images/DS30002-132/5384.jpg,https://oleks-netizen.github.io/product-images/DS30002-132/5385.jpg,https://oleks-netizen.github.io/product-images/DS30002-132/5386.jpg,https://oleks-netizen.github.io/product-images/DS30002-132/5387.jpg,https://oleks-netizen.github.io/product-images/DS30002-132/5388.jpg</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -1301,7 +1301,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DS30002-162/6176.jpg,https://oleks-netizen.github.io/product-images/DS30002-162/6177.jpg,https://oleks-netizen.github.io/product-images/DS30002-162/6178.jpg,https://oleks-netizen.github.io/product-images/DS30002-162/6179.jpg,https://oleks-netizen.github.io/product-images/DS30002-162/6180.jpg,https://oleks-netizen.github.io/product-images/DS30002-162/6181.jpg,https://oleks-netizen.github.io/product-images/DS30002-162/6182.jpg,https://oleks-netizen.github.io/product-images/DS30002-162/6183.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DS30002-162/1.jpg,https://oleks-netizen.github.io/product-images/DS30002-162/6176.jpg,https://oleks-netizen.github.io/product-images/DS30002-162/6177.jpg,https://oleks-netizen.github.io/product-images/DS30002-162/6179.jpg,https://oleks-netizen.github.io/product-images/DS30002-162/6180.jpg,https://oleks-netizen.github.io/product-images/DS30002-162/6181.jpg,https://oleks-netizen.github.io/product-images/DS30002-162/6182.jpg,https://oleks-netizen.github.io/product-images/DS30002-162/6183.jpg</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -1316,7 +1316,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DS30002-287/1738.jpg,https://oleks-netizen.github.io/product-images/DS30002-287/1739.jpg,https://oleks-netizen.github.io/product-images/DS30002-287/1740.jpg,https://oleks-netizen.github.io/product-images/DS30002-287/1741.jpg,https://oleks-netizen.github.io/product-images/DS30002-287/1742.jpg,https://oleks-netizen.github.io/product-images/DS30002-287/1743.jpg,https://oleks-netizen.github.io/product-images/DS30002-287/1744.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DS30002-287/1738.jpg,https://oleks-netizen.github.io/product-images/DS30002-287/1739.jpg,https://oleks-netizen.github.io/product-images/DS30002-287/1741.jpg,https://oleks-netizen.github.io/product-images/DS30002-287/1742.jpg,https://oleks-netizen.github.io/product-images/DS30002-287/1743.jpg,https://oleks-netizen.github.io/product-images/DS30002-287/1744.jpg,https://oleks-netizen.github.io/product-images/DS30002-287/1.jpg</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -1331,7 +1331,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DS30002-288/4198.jpg,https://oleks-netizen.github.io/product-images/DS30002-288/4199.jpg,https://oleks-netizen.github.io/product-images/DS30002-288/4200.jpg,https://oleks-netizen.github.io/product-images/DS30002-288/4201.jpg,https://oleks-netizen.github.io/product-images/DS30002-288/4202.jpg,https://oleks-netizen.github.io/product-images/DS30002-288/4205.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DS30002-288/1.jpg,https://oleks-netizen.github.io/product-images/DS30002-288/4198.jpg,https://oleks-netizen.github.io/product-images/DS30002-288/4199.jpg,https://oleks-netizen.github.io/product-images/DS30002-288/4201.jpg,https://oleks-netizen.github.io/product-images/DS30002-288/4202.jpg,https://oleks-netizen.github.io/product-images/DS30002-288/4205.jpg</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -1346,7 +1346,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/F20218-black/2169.jpg,https://oleks-netizen.github.io/product-images/F20218-black/2170.jpg,https://oleks-netizen.github.io/product-images/F20218-black/2171.jpg,https://oleks-netizen.github.io/product-images/F20218-black/2172.jpg,https://oleks-netizen.github.io/product-images/F20218-black/2173.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/F20218-black/1.jpg,https://oleks-netizen.github.io/product-images/F20218-black/2169.jpg,https://oleks-netizen.github.io/product-images/F20218-black/2171.jpg,https://oleks-netizen.github.io/product-images/F20218-black/2172.jpg,https://oleks-netizen.github.io/product-images/F20218-black/2173.jpg</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -1361,7 +1361,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/FW-A2106-black/2673.jpg,https://oleks-netizen.github.io/product-images/FW-A2106-black/2674.jpg,https://oleks-netizen.github.io/product-images/FW-A2106-black/2675.jpg,https://oleks-netizen.github.io/product-images/FW-A2106-black/2676.jpg,https://oleks-netizen.github.io/product-images/FW-A2106-black/2677.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/FW-A2106-black/1.jpg,https://oleks-netizen.github.io/product-images/FW-A2106-black/2674.jpg,https://oleks-netizen.github.io/product-images/FW-A2106-black/2675.jpg,https://oleks-netizen.github.io/product-images/FW-A2106-black/2676.jpg,https://oleks-netizen.github.io/product-images/FW-A2106-black/2677.jpg</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -1376,7 +1376,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/FW-A648-black/1543.jpg,https://oleks-netizen.github.io/product-images/FW-A648-black/1544.jpg,https://oleks-netizen.github.io/product-images/FW-A648-black/1545.jpg,https://oleks-netizen.github.io/product-images/FW-A648-black/1546.jpg,https://oleks-netizen.github.io/product-images/FW-A648-black/1547.jpg,https://oleks-netizen.github.io/product-images/FW-A648-black/1548.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/FW-A648-black/1543.jpg,https://oleks-netizen.github.io/product-images/FW-A648-black/1545.jpg,https://oleks-netizen.github.io/product-images/FW-A648-black/1546.jpg,https://oleks-netizen.github.io/product-images/FW-A648-black/1547.jpg,https://oleks-netizen.github.io/product-images/FW-A648-black/1548.jpg,https://oleks-netizen.github.io/product-images/FW-A648-black/1.jpg</t>
         </is>
       </c>
       <c r="C64" t="n">
@@ -1391,7 +1391,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/FW-A648-blue/493.jpg,https://oleks-netizen.github.io/product-images/FW-A648-blue/494.jpg,https://oleks-netizen.github.io/product-images/FW-A648-blue/495.jpg,https://oleks-netizen.github.io/product-images/FW-A648-blue/496.jpg,https://oleks-netizen.github.io/product-images/FW-A648-blue/497.jpg,https://oleks-netizen.github.io/product-images/FW-A648-blue/498.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/FW-A648-blue/1.jpg,https://oleks-netizen.github.io/product-images/FW-A648-blue/493.jpg,https://oleks-netizen.github.io/product-images/FW-A648-blue/495.jpg,https://oleks-netizen.github.io/product-images/FW-A648-blue/496.jpg,https://oleks-netizen.github.io/product-images/FW-A648-blue/497.jpg,https://oleks-netizen.github.io/product-images/FW-A648-blue/498.jpg</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -1406,7 +1406,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/FW-A648-green/6165.jpg,https://oleks-netizen.github.io/product-images/FW-A648-green/6166.jpg,https://oleks-netizen.github.io/product-images/FW-A648-green/6167.jpg,https://oleks-netizen.github.io/product-images/FW-A648-green/6168.jpg,https://oleks-netizen.github.io/product-images/FW-A648-green/6169.jpg,https://oleks-netizen.github.io/product-images/FW-A648-green/6170.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/FW-A648-green/1.jpg,https://oleks-netizen.github.io/product-images/FW-A648-green/6165.jpg,https://oleks-netizen.github.io/product-images/FW-A648-green/6167.jpg,https://oleks-netizen.github.io/product-images/FW-A648-green/6168.jpg,https://oleks-netizen.github.io/product-images/FW-A648-green/6169.jpg,https://oleks-netizen.github.io/product-images/FW-A648-green/6170.jpg</t>
         </is>
       </c>
       <c r="C66" t="n">
@@ -1421,7 +1421,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/FW-A648-purple/2066.jpg,https://oleks-netizen.github.io/product-images/FW-A648-purple/2067.jpg,https://oleks-netizen.github.io/product-images/FW-A648-purple/2068.jpg,https://oleks-netizen.github.io/product-images/FW-A648-purple/2069.jpg,https://oleks-netizen.github.io/product-images/FW-A648-purple/2070.jpg,https://oleks-netizen.github.io/product-images/FW-A648-purple/2071.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/FW-A648-purple/1.jpg,https://oleks-netizen.github.io/product-images/FW-A648-purple/2066.jpg,https://oleks-netizen.github.io/product-images/FW-A648-purple/2068.jpg,https://oleks-netizen.github.io/product-images/FW-A648-purple/2069.jpg,https://oleks-netizen.github.io/product-images/FW-A648-purple/2070.jpg,https://oleks-netizen.github.io/product-images/FW-A648-purple/2071.jpg</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -1436,7 +1436,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/FW-A648-red/1241.jpg,https://oleks-netizen.github.io/product-images/FW-A648-red/1242.jpg,https://oleks-netizen.github.io/product-images/FW-A648-red/1243.jpg,https://oleks-netizen.github.io/product-images/FW-A648-red/1244.jpg,https://oleks-netizen.github.io/product-images/FW-A648-red/1245.jpg,https://oleks-netizen.github.io/product-images/FW-A648-red/1246.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/FW-A648-red/1241.jpg,https://oleks-netizen.github.io/product-images/FW-A648-red/1243.jpg,https://oleks-netizen.github.io/product-images/FW-A648-red/1244.jpg,https://oleks-netizen.github.io/product-images/FW-A648-red/1245.jpg,https://oleks-netizen.github.io/product-images/FW-A648-red/1246.jpg,https://oleks-netizen.github.io/product-images/FW-A648-red/1.jpg</t>
         </is>
       </c>
       <c r="C68" t="n">
@@ -1451,7 +1451,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/G2568-black/1298.jpg,https://oleks-netizen.github.io/product-images/G2568-black/1299.jpg,https://oleks-netizen.github.io/product-images/G2568-black/1300.jpg,https://oleks-netizen.github.io/product-images/G2568-black/1301.jpg,https://oleks-netizen.github.io/product-images/G2568-black/1302.jpg,https://oleks-netizen.github.io/product-images/G2568-black/1303.jpg,https://oleks-netizen.github.io/product-images/G2568-black/1304.jpg,https://oleks-netizen.github.io/product-images/G2568-black/1305.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/G2568-black/1298.jpg,https://oleks-netizen.github.io/product-images/G2568-black/1299.jpg,https://oleks-netizen.github.io/product-images/G2568-black/1301.jpg,https://oleks-netizen.github.io/product-images/G2568-black/1302.jpg,https://oleks-netizen.github.io/product-images/G2568-black/1303.jpg,https://oleks-netizen.github.io/product-images/G2568-black/1304.jpg,https://oleks-netizen.github.io/product-images/G2568-black/1305.jpg,https://oleks-netizen.github.io/product-images/G2568-black/1.jpg</t>
         </is>
       </c>
       <c r="C69" t="n">
@@ -1466,7 +1466,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/G2568-grey/1752.jpg,https://oleks-netizen.github.io/product-images/G2568-grey/1753.jpg,https://oleks-netizen.github.io/product-images/G2568-grey/1754.jpg,https://oleks-netizen.github.io/product-images/G2568-grey/1755.jpg,https://oleks-netizen.github.io/product-images/G2568-grey/1756.jpg,https://oleks-netizen.github.io/product-images/G2568-grey/1757.jpg,https://oleks-netizen.github.io/product-images/G2568-grey/1758.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/G2568-grey/1752.jpg,https://oleks-netizen.github.io/product-images/G2568-grey/1753.jpg,https://oleks-netizen.github.io/product-images/G2568-grey/1755.jpg,https://oleks-netizen.github.io/product-images/G2568-grey/1756.jpg,https://oleks-netizen.github.io/product-images/G2568-grey/1757.jpg,https://oleks-netizen.github.io/product-images/G2568-grey/1758.jpg,https://oleks-netizen.github.io/product-images/G2568-grey/1.jpg</t>
         </is>
       </c>
       <c r="C70" t="n">
@@ -1481,7 +1481,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/H-2908-black/5423.jpg,https://oleks-netizen.github.io/product-images/H-2908-black/5424.jpg,https://oleks-netizen.github.io/product-images/H-2908-black/5425.jpg,https://oleks-netizen.github.io/product-images/H-2908-black/5426.jpg,https://oleks-netizen.github.io/product-images/H-2908-black/5427.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/H-2908-black/1.jpg,https://oleks-netizen.github.io/product-images/H-2908-black/5423.jpg,https://oleks-netizen.github.io/product-images/H-2908-black/5425.jpg,https://oleks-netizen.github.io/product-images/H-2908-black/5426.jpg,https://oleks-netizen.github.io/product-images/H-2908-black/5427.jpg</t>
         </is>
       </c>
       <c r="C71" t="n">
@@ -1496,7 +1496,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/H-2908-red/3159.jpg,https://oleks-netizen.github.io/product-images/H-2908-red/3160.jpg,https://oleks-netizen.github.io/product-images/H-2908-red/3161.jpg,https://oleks-netizen.github.io/product-images/H-2908-red/3162.jpg,https://oleks-netizen.github.io/product-images/H-2908-red/3163.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/H-2908-red/1.jpg,https://oleks-netizen.github.io/product-images/H-2908-red/3159.jpg,https://oleks-netizen.github.io/product-images/H-2908-red/3161.jpg,https://oleks-netizen.github.io/product-images/H-2908-red/3162.jpg,https://oleks-netizen.github.io/product-images/H-2908-red/3163.jpg</t>
         </is>
       </c>
       <c r="C72" t="n">
@@ -1511,7 +1511,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20001-22/955.jpg,https://oleks-netizen.github.io/product-images/L20001-22/956.jpg,https://oleks-netizen.github.io/product-images/L20001-22/957.jpg,https://oleks-netizen.github.io/product-images/L20001-22/958.jpg,https://oleks-netizen.github.io/product-images/L20001-22/959.jpg,https://oleks-netizen.github.io/product-images/L20001-22/960.jpg,https://oleks-netizen.github.io/product-images/L20001-22/961.jpg,https://oleks-netizen.github.io/product-images/L20001-22/962.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20001-22/1.jpg,https://oleks-netizen.github.io/product-images/L20001-22/955.jpg,https://oleks-netizen.github.io/product-images/L20001-22/956.jpg,https://oleks-netizen.github.io/product-images/L20001-22/958.jpg,https://oleks-netizen.github.io/product-images/L20001-22/959.jpg,https://oleks-netizen.github.io/product-images/L20001-22/960.jpg,https://oleks-netizen.github.io/product-images/L20001-22/961.jpg,https://oleks-netizen.github.io/product-images/L20001-22/962.jpg</t>
         </is>
       </c>
       <c r="C73" t="n">
@@ -1526,7 +1526,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20011-1/3500.jpg,https://oleks-netizen.github.io/product-images/L20011-1/3501.jpg,https://oleks-netizen.github.io/product-images/L20011-1/3502.jpg,https://oleks-netizen.github.io/product-images/L20011-1/3503.jpg,https://oleks-netizen.github.io/product-images/L20011-1/3504.jpg,https://oleks-netizen.github.io/product-images/L20011-1/3505.jpg,https://oleks-netizen.github.io/product-images/L20011-1/3506.jpg,https://oleks-netizen.github.io/product-images/L20011-1/3507.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20011-1/1.jpg,https://oleks-netizen.github.io/product-images/L20011-1/3500.jpg,https://oleks-netizen.github.io/product-images/L20011-1/3501.jpg,https://oleks-netizen.github.io/product-images/L20011-1/3503.jpg,https://oleks-netizen.github.io/product-images/L20011-1/3504.jpg,https://oleks-netizen.github.io/product-images/L20011-1/3505.jpg,https://oleks-netizen.github.io/product-images/L20011-1/3506.jpg,https://oleks-netizen.github.io/product-images/L20011-1/3507.jpg</t>
         </is>
       </c>
       <c r="C74" t="n">
@@ -1541,7 +1541,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20011-22/6081.jpg,https://oleks-netizen.github.io/product-images/L20011-22/6082.jpg,https://oleks-netizen.github.io/product-images/L20011-22/6083.jpg,https://oleks-netizen.github.io/product-images/L20011-22/6084.jpg,https://oleks-netizen.github.io/product-images/L20011-22/6085.jpg,https://oleks-netizen.github.io/product-images/L20011-22/6086.jpg,https://oleks-netizen.github.io/product-images/L20011-22/6087.jpg,https://oleks-netizen.github.io/product-images/L20011-22/6088.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20011-22/1.jpg,https://oleks-netizen.github.io/product-images/L20011-22/6081.jpg,https://oleks-netizen.github.io/product-images/L20011-22/6082.jpg,https://oleks-netizen.github.io/product-images/L20011-22/6084.jpg,https://oleks-netizen.github.io/product-images/L20011-22/6085.jpg,https://oleks-netizen.github.io/product-images/L20011-22/6086.jpg,https://oleks-netizen.github.io/product-images/L20011-22/6087.jpg,https://oleks-netizen.github.io/product-images/L20011-22/6088.jpg</t>
         </is>
       </c>
       <c r="C75" t="n">
@@ -1556,7 +1556,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20011-56/5785.jpg,https://oleks-netizen.github.io/product-images/L20011-56/5786.jpg,https://oleks-netizen.github.io/product-images/L20011-56/5787.jpg,https://oleks-netizen.github.io/product-images/L20011-56/5788.jpg,https://oleks-netizen.github.io/product-images/L20011-56/5789.jpg,https://oleks-netizen.github.io/product-images/L20011-56/5790.jpg,https://oleks-netizen.github.io/product-images/L20011-56/5791.jpg,https://oleks-netizen.github.io/product-images/L20011-56/5792.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20011-56/1.jpg,https://oleks-netizen.github.io/product-images/L20011-56/5785.jpg,https://oleks-netizen.github.io/product-images/L20011-56/5786.jpg,https://oleks-netizen.github.io/product-images/L20011-56/5788.jpg,https://oleks-netizen.github.io/product-images/L20011-56/5789.jpg,https://oleks-netizen.github.io/product-images/L20011-56/5790.jpg,https://oleks-netizen.github.io/product-images/L20011-56/5791.jpg,https://oleks-netizen.github.io/product-images/L20011-56/5792.jpg</t>
         </is>
       </c>
       <c r="C76" t="n">
@@ -1571,7 +1571,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20030-1/4702.jpg,https://oleks-netizen.github.io/product-images/L20030-1/4703.jpg,https://oleks-netizen.github.io/product-images/L20030-1/4704.jpg,https://oleks-netizen.github.io/product-images/L20030-1/4705.jpg,https://oleks-netizen.github.io/product-images/L20030-1/4706.jpg,https://oleks-netizen.github.io/product-images/L20030-1/4707.jpg,https://oleks-netizen.github.io/product-images/L20030-1/4708.jpg,https://oleks-netizen.github.io/product-images/L20030-1/4709.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20030-1/1.jpg,https://oleks-netizen.github.io/product-images/L20030-1/4702.jpg,https://oleks-netizen.github.io/product-images/L20030-1/4703.jpg,https://oleks-netizen.github.io/product-images/L20030-1/4704.jpg,https://oleks-netizen.github.io/product-images/L20030-1/4706.jpg,https://oleks-netizen.github.io/product-images/L20030-1/4707.jpg,https://oleks-netizen.github.io/product-images/L20030-1/4708.jpg,https://oleks-netizen.github.io/product-images/L20030-1/4709.jpg</t>
         </is>
       </c>
       <c r="C77" t="n">
@@ -1586,7 +1586,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20030-56/3774.jpg,https://oleks-netizen.github.io/product-images/L20030-56/3775.jpg,https://oleks-netizen.github.io/product-images/L20030-56/3776.jpg,https://oleks-netizen.github.io/product-images/L20030-56/3777.jpg,https://oleks-netizen.github.io/product-images/L20030-56/3778.jpg,https://oleks-netizen.github.io/product-images/L20030-56/3779.jpg,https://oleks-netizen.github.io/product-images/L20030-56/3780.jpg,https://oleks-netizen.github.io/product-images/L20030-56/3781.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20030-56/1.jpg,https://oleks-netizen.github.io/product-images/L20030-56/3774.jpg,https://oleks-netizen.github.io/product-images/L20030-56/3775.jpg,https://oleks-netizen.github.io/product-images/L20030-56/3776.jpg,https://oleks-netizen.github.io/product-images/L20030-56/3778.jpg,https://oleks-netizen.github.io/product-images/L20030-56/3779.jpg,https://oleks-netizen.github.io/product-images/L20030-56/3780.jpg,https://oleks-netizen.github.io/product-images/L20030-56/3781.jpg</t>
         </is>
       </c>
       <c r="C78" t="n">
@@ -1601,7 +1601,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20036-1/3838.jpg,https://oleks-netizen.github.io/product-images/L20036-1/3839.jpg,https://oleks-netizen.github.io/product-images/L20036-1/3840.jpg,https://oleks-netizen.github.io/product-images/L20036-1/3841.jpg,https://oleks-netizen.github.io/product-images/L20036-1/3842.jpg,https://oleks-netizen.github.io/product-images/L20036-1/3843.jpg,https://oleks-netizen.github.io/product-images/L20036-1/3844.jpg,https://oleks-netizen.github.io/product-images/L20036-1/3845.jpg,https://oleks-netizen.github.io/product-images/L20036-1/3846.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20036-1/1.jpg,https://oleks-netizen.github.io/product-images/L20036-1/3838.jpg,https://oleks-netizen.github.io/product-images/L20036-1/3839.jpg,https://oleks-netizen.github.io/product-images/L20036-1/3841.jpg,https://oleks-netizen.github.io/product-images/L20036-1/3842.jpg,https://oleks-netizen.github.io/product-images/L20036-1/3843.jpg,https://oleks-netizen.github.io/product-images/L20036-1/3844.jpg,https://oleks-netizen.github.io/product-images/L20036-1/3845.jpg,https://oleks-netizen.github.io/product-images/L20036-1/3846.jpg</t>
         </is>
       </c>
       <c r="C79" t="n">
@@ -1616,7 +1616,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20036-8/53.jpg,https://oleks-netizen.github.io/product-images/L20036-8/54.jpg,https://oleks-netizen.github.io/product-images/L20036-8/55.jpg,https://oleks-netizen.github.io/product-images/L20036-8/57.jpg,https://oleks-netizen.github.io/product-images/L20036-8/58.jpg,https://oleks-netizen.github.io/product-images/L20036-8/59.jpg,https://oleks-netizen.github.io/product-images/L20036-8/60.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20036-8/1.jpg,https://oleks-netizen.github.io/product-images/L20036-8/53.jpg,https://oleks-netizen.github.io/product-images/L20036-8/54.jpg,https://oleks-netizen.github.io/product-images/L20036-8/57.jpg,https://oleks-netizen.github.io/product-images/L20036-8/58.jpg,https://oleks-netizen.github.io/product-images/L20036-8/59.jpg,https://oleks-netizen.github.io/product-images/L20036-8/60.jpg</t>
         </is>
       </c>
       <c r="C80" t="n">
@@ -1631,7 +1631,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20063-1/3093.jpg,https://oleks-netizen.github.io/product-images/L20063-1/3094.jpg,https://oleks-netizen.github.io/product-images/L20063-1/3095.jpg,https://oleks-netizen.github.io/product-images/L20063-1/3096.jpg,https://oleks-netizen.github.io/product-images/L20063-1/3097.jpg,https://oleks-netizen.github.io/product-images/L20063-1/3098.jpg,https://oleks-netizen.github.io/product-images/L20063-1/3099.jpg,https://oleks-netizen.github.io/product-images/L20063-1/3100.jpg,https://oleks-netizen.github.io/product-images/L20063-1/3101.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20063-1/1.jpg,https://oleks-netizen.github.io/product-images/L20063-1/3093.jpg,https://oleks-netizen.github.io/product-images/L20063-1/3094.jpg,https://oleks-netizen.github.io/product-images/L20063-1/3096.jpg,https://oleks-netizen.github.io/product-images/L20063-1/3097.jpg,https://oleks-netizen.github.io/product-images/L20063-1/3098.jpg,https://oleks-netizen.github.io/product-images/L20063-1/3099.jpg,https://oleks-netizen.github.io/product-images/L20063-1/3100.jpg,https://oleks-netizen.github.io/product-images/L20063-1/3101.jpg</t>
         </is>
       </c>
       <c r="C81" t="n">
@@ -1646,7 +1646,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20063-8/896.jpg,https://oleks-netizen.github.io/product-images/L20063-8/897.jpg,https://oleks-netizen.github.io/product-images/L20063-8/898.jpg,https://oleks-netizen.github.io/product-images/L20063-8/899.jpg,https://oleks-netizen.github.io/product-images/L20063-8/900.jpg,https://oleks-netizen.github.io/product-images/L20063-8/901.jpg,https://oleks-netizen.github.io/product-images/L20063-8/902.jpg,https://oleks-netizen.github.io/product-images/L20063-8/903.jpg,https://oleks-netizen.github.io/product-images/L20063-8/904.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20063-8/1.jpg,https://oleks-netizen.github.io/product-images/L20063-8/896.jpg,https://oleks-netizen.github.io/product-images/L20063-8/897.jpg,https://oleks-netizen.github.io/product-images/L20063-8/899.jpg,https://oleks-netizen.github.io/product-images/L20063-8/900.jpg,https://oleks-netizen.github.io/product-images/L20063-8/901.jpg,https://oleks-netizen.github.io/product-images/L20063-8/902.jpg,https://oleks-netizen.github.io/product-images/L20063-8/903.jpg,https://oleks-netizen.github.io/product-images/L20063-8/904.jpg</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -1661,7 +1661,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20633-78/1983.jpg,https://oleks-netizen.github.io/product-images/L20633-78/1984.jpg,https://oleks-netizen.github.io/product-images/L20633-78/1985.jpg,https://oleks-netizen.github.io/product-images/L20633-78/1986.jpg,https://oleks-netizen.github.io/product-images/L20633-78/1987.jpg,https://oleks-netizen.github.io/product-images/L20633-78/1988.jpg,https://oleks-netizen.github.io/product-images/L20633-78/1989.jpg,https://oleks-netizen.github.io/product-images/L20633-78/1990.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20633-78/1983.jpg,https://oleks-netizen.github.io/product-images/L20633-78/1984.jpg,https://oleks-netizen.github.io/product-images/L20633-78/1986.jpg,https://oleks-netizen.github.io/product-images/L20633-78/1987.jpg,https://oleks-netizen.github.io/product-images/L20633-78/1988.jpg,https://oleks-netizen.github.io/product-images/L20633-78/1989.jpg,https://oleks-netizen.github.io/product-images/L20633-78/1990.jpg,https://oleks-netizen.github.io/product-images/L20633-78/1.jpg</t>
         </is>
       </c>
       <c r="C83" t="n">
@@ -1676,7 +1676,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20633-90/3421.jpg,https://oleks-netizen.github.io/product-images/L20633-90/3422.jpg,https://oleks-netizen.github.io/product-images/L20633-90/3423.jpg,https://oleks-netizen.github.io/product-images/L20633-90/3424.jpg,https://oleks-netizen.github.io/product-images/L20633-90/3425.jpg,https://oleks-netizen.github.io/product-images/L20633-90/3426.jpg,https://oleks-netizen.github.io/product-images/L20633-90/3427.jpg,https://oleks-netizen.github.io/product-images/L20633-90/3428.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20633-90/1.jpg,https://oleks-netizen.github.io/product-images/L20633-90/3421.jpg,https://oleks-netizen.github.io/product-images/L20633-90/3422.jpg,https://oleks-netizen.github.io/product-images/L20633-90/3424.jpg,https://oleks-netizen.github.io/product-images/L20633-90/3425.jpg,https://oleks-netizen.github.io/product-images/L20633-90/3426.jpg,https://oleks-netizen.github.io/product-images/L20633-90/3427.jpg,https://oleks-netizen.github.io/product-images/L20633-90/3428.jpg</t>
         </is>
       </c>
       <c r="C84" t="n">
@@ -1691,7 +1691,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20680-1/3946.jpg,https://oleks-netizen.github.io/product-images/L20680-1/3947.jpg,https://oleks-netizen.github.io/product-images/L20680-1/3948.jpg,https://oleks-netizen.github.io/product-images/L20680-1/3949.jpg,https://oleks-netizen.github.io/product-images/L20680-1/3950.jpg,https://oleks-netizen.github.io/product-images/L20680-1/3951.jpg,https://oleks-netizen.github.io/product-images/L20680-1/3952.jpg,https://oleks-netizen.github.io/product-images/L20680-1/3953.jpg,https://oleks-netizen.github.io/product-images/L20680-1/3954.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20680-1/1.jpg,https://oleks-netizen.github.io/product-images/L20680-1/3946.jpg,https://oleks-netizen.github.io/product-images/L20680-1/3947.jpg,https://oleks-netizen.github.io/product-images/L20680-1/3949.jpg,https://oleks-netizen.github.io/product-images/L20680-1/3950.jpg,https://oleks-netizen.github.io/product-images/L20680-1/3951.jpg,https://oleks-netizen.github.io/product-images/L20680-1/3952.jpg,https://oleks-netizen.github.io/product-images/L20680-1/3953.jpg,https://oleks-netizen.github.io/product-images/L20680-1/3954.jpg</t>
         </is>
       </c>
       <c r="C85" t="n">
@@ -1706,7 +1706,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20680-56/3017.jpg,https://oleks-netizen.github.io/product-images/L20680-56/3018.jpg,https://oleks-netizen.github.io/product-images/L20680-56/3019.jpg,https://oleks-netizen.github.io/product-images/L20680-56/3020.jpg,https://oleks-netizen.github.io/product-images/L20680-56/3021.jpg,https://oleks-netizen.github.io/product-images/L20680-56/3022.jpg,https://oleks-netizen.github.io/product-images/L20680-56/3023.jpg,https://oleks-netizen.github.io/product-images/L20680-56/3024.jpg,https://oleks-netizen.github.io/product-images/L20680-56/3025.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20680-56/1.jpg,https://oleks-netizen.github.io/product-images/L20680-56/3017.jpg,https://oleks-netizen.github.io/product-images/L20680-56/3018.jpg,https://oleks-netizen.github.io/product-images/L20680-56/3020.jpg,https://oleks-netizen.github.io/product-images/L20680-56/3021.jpg,https://oleks-netizen.github.io/product-images/L20680-56/3022.jpg,https://oleks-netizen.github.io/product-images/L20680-56/3023.jpg,https://oleks-netizen.github.io/product-images/L20680-56/3024.jpg,https://oleks-netizen.github.io/product-images/L20680-56/3025.jpg</t>
         </is>
       </c>
       <c r="C86" t="n">
@@ -1721,7 +1721,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20680-58/5518.jpg,https://oleks-netizen.github.io/product-images/L20680-58/5519.jpg,https://oleks-netizen.github.io/product-images/L20680-58/5520.jpg,https://oleks-netizen.github.io/product-images/L20680-58/5521.jpg,https://oleks-netizen.github.io/product-images/L20680-58/5522.jpg,https://oleks-netizen.github.io/product-images/L20680-58/5523.jpg,https://oleks-netizen.github.io/product-images/L20680-58/5524.jpg,https://oleks-netizen.github.io/product-images/L20680-58/5525.jpg,https://oleks-netizen.github.io/product-images/L20680-58/5526.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20680-58/1.jpg,https://oleks-netizen.github.io/product-images/L20680-58/5518.jpg,https://oleks-netizen.github.io/product-images/L20680-58/5519.jpg,https://oleks-netizen.github.io/product-images/L20680-58/5521.jpg,https://oleks-netizen.github.io/product-images/L20680-58/5522.jpg,https://oleks-netizen.github.io/product-images/L20680-58/5523.jpg,https://oleks-netizen.github.io/product-images/L20680-58/5524.jpg,https://oleks-netizen.github.io/product-images/L20680-58/5525.jpg,https://oleks-netizen.github.io/product-images/L20680-58/5526.jpg</t>
         </is>
       </c>
       <c r="C87" t="n">
@@ -1736,7 +1736,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20682-1/3026.jpg,https://oleks-netizen.github.io/product-images/L20682-1/3027.jpg,https://oleks-netizen.github.io/product-images/L20682-1/3028.jpg,https://oleks-netizen.github.io/product-images/L20682-1/3029.jpg,https://oleks-netizen.github.io/product-images/L20682-1/3030.jpg,https://oleks-netizen.github.io/product-images/L20682-1/3031.jpg,https://oleks-netizen.github.io/product-images/L20682-1/3032.jpg,https://oleks-netizen.github.io/product-images/L20682-1/3033.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20682-1/1.jpg,https://oleks-netizen.github.io/product-images/L20682-1/3026.jpg,https://oleks-netizen.github.io/product-images/L20682-1/3027.jpg,https://oleks-netizen.github.io/product-images/L20682-1/3029.jpg,https://oleks-netizen.github.io/product-images/L20682-1/3030.jpg,https://oleks-netizen.github.io/product-images/L20682-1/3031.jpg,https://oleks-netizen.github.io/product-images/L20682-1/3032.jpg,https://oleks-netizen.github.io/product-images/L20682-1/3033.jpg</t>
         </is>
       </c>
       <c r="C88" t="n">
@@ -1751,7 +1751,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20683-1/2684.jpg,https://oleks-netizen.github.io/product-images/L20683-1/2685.jpg,https://oleks-netizen.github.io/product-images/L20683-1/2686.jpg,https://oleks-netizen.github.io/product-images/L20683-1/2687.jpg,https://oleks-netizen.github.io/product-images/L20683-1/2688.jpg,https://oleks-netizen.github.io/product-images/L20683-1/2689.jpg,https://oleks-netizen.github.io/product-images/L20683-1/2690.jpg,https://oleks-netizen.github.io/product-images/L20683-1/2691.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20683-1/1.jpg,https://oleks-netizen.github.io/product-images/L20683-1/2684.jpg,https://oleks-netizen.github.io/product-images/L20683-1/2685.jpg,https://oleks-netizen.github.io/product-images/L20683-1/2687.jpg,https://oleks-netizen.github.io/product-images/L20683-1/2688.jpg,https://oleks-netizen.github.io/product-images/L20683-1/2689.jpg,https://oleks-netizen.github.io/product-images/L20683-1/2690.jpg,https://oleks-netizen.github.io/product-images/L20683-1/2691.jpg</t>
         </is>
       </c>
       <c r="C89" t="n">
@@ -1766,7 +1766,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20683-2/1370.jpg,https://oleks-netizen.github.io/product-images/L20683-2/1371.jpg,https://oleks-netizen.github.io/product-images/L20683-2/1372.jpg,https://oleks-netizen.github.io/product-images/L20683-2/1373.jpg,https://oleks-netizen.github.io/product-images/L20683-2/1374.jpg,https://oleks-netizen.github.io/product-images/L20683-2/1375.jpg,https://oleks-netizen.github.io/product-images/L20683-2/1376.jpg,https://oleks-netizen.github.io/product-images/L20683-2/1377.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20683-2/1370.jpg,https://oleks-netizen.github.io/product-images/L20683-2/1371.jpg,https://oleks-netizen.github.io/product-images/L20683-2/1373.jpg,https://oleks-netizen.github.io/product-images/L20683-2/1374.jpg,https://oleks-netizen.github.io/product-images/L20683-2/1375.jpg,https://oleks-netizen.github.io/product-images/L20683-2/1376.jpg,https://oleks-netizen.github.io/product-images/L20683-2/1377.jpg,https://oleks-netizen.github.io/product-images/L20683-2/1.jpg</t>
         </is>
       </c>
       <c r="C90" t="n">
@@ -1781,7 +1781,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20713-1/499.jpg,https://oleks-netizen.github.io/product-images/L20713-1/500.jpg,https://oleks-netizen.github.io/product-images/L20713-1/501.jpg,https://oleks-netizen.github.io/product-images/L20713-1/502.jpg,https://oleks-netizen.github.io/product-images/L20713-1/503.jpg,https://oleks-netizen.github.io/product-images/L20713-1/504.jpg,https://oleks-netizen.github.io/product-images/L20713-1/505.jpg,https://oleks-netizen.github.io/product-images/L20713-1/506.jpg,https://oleks-netizen.github.io/product-images/L20713-1/507.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20713-1/1.jpg,https://oleks-netizen.github.io/product-images/L20713-1/499.jpg,https://oleks-netizen.github.io/product-images/L20713-1/500.jpg,https://oleks-netizen.github.io/product-images/L20713-1/502.jpg,https://oleks-netizen.github.io/product-images/L20713-1/503.jpg,https://oleks-netizen.github.io/product-images/L20713-1/504.jpg,https://oleks-netizen.github.io/product-images/L20713-1/505.jpg,https://oleks-netizen.github.io/product-images/L20713-1/506.jpg,https://oleks-netizen.github.io/product-images/L20713-1/507.jpg</t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -1796,7 +1796,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20713-8/971.jpg,https://oleks-netizen.github.io/product-images/L20713-8/972.jpg,https://oleks-netizen.github.io/product-images/L20713-8/973.jpg,https://oleks-netizen.github.io/product-images/L20713-8/974.jpg,https://oleks-netizen.github.io/product-images/L20713-8/975.jpg,https://oleks-netizen.github.io/product-images/L20713-8/976.jpg,https://oleks-netizen.github.io/product-images/L20713-8/977.jpg,https://oleks-netizen.github.io/product-images/L20713-8/978.jpg,https://oleks-netizen.github.io/product-images/L20713-8/979.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20713-8/1.jpg,https://oleks-netizen.github.io/product-images/L20713-8/971.jpg,https://oleks-netizen.github.io/product-images/L20713-8/972.jpg,https://oleks-netizen.github.io/product-images/L20713-8/974.jpg,https://oleks-netizen.github.io/product-images/L20713-8/975.jpg,https://oleks-netizen.github.io/product-images/L20713-8/976.jpg,https://oleks-netizen.github.io/product-images/L20713-8/977.jpg,https://oleks-netizen.github.io/product-images/L20713-8/978.jpg,https://oleks-netizen.github.io/product-images/L20713-8/979.jpg</t>
         </is>
       </c>
       <c r="C92" t="n">
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20812-1/5035.jpg,https://oleks-netizen.github.io/product-images/L20812-1/5036.jpg,https://oleks-netizen.github.io/product-images/L20812-1/5037.jpg,https://oleks-netizen.github.io/product-images/L20812-1/5038.jpg,https://oleks-netizen.github.io/product-images/L20812-1/5039.jpg,https://oleks-netizen.github.io/product-images/L20812-1/5040.jpg,https://oleks-netizen.github.io/product-images/L20812-1/5041.jpg,https://oleks-netizen.github.io/product-images/L20812-1/5042.jpg,https://oleks-netizen.github.io/product-images/L20812-1/5043.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20812-1/1.jpg,https://oleks-netizen.github.io/product-images/L20812-1/5035.jpg,https://oleks-netizen.github.io/product-images/L20812-1/5036.jpg,https://oleks-netizen.github.io/product-images/L20812-1/5038.jpg,https://oleks-netizen.github.io/product-images/L20812-1/5039.jpg,https://oleks-netizen.github.io/product-images/L20812-1/5040.jpg,https://oleks-netizen.github.io/product-images/L20812-1/5041.jpg,https://oleks-netizen.github.io/product-images/L20812-1/5042.jpg,https://oleks-netizen.github.io/product-images/L20812-1/5043.jpg</t>
         </is>
       </c>
       <c r="C93" t="n">
@@ -1826,7 +1826,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20812-10/2722.jpg,https://oleks-netizen.github.io/product-images/L20812-10/2723.jpg,https://oleks-netizen.github.io/product-images/L20812-10/2724.jpg,https://oleks-netizen.github.io/product-images/L20812-10/2725.jpg,https://oleks-netizen.github.io/product-images/L20812-10/2726.jpg,https://oleks-netizen.github.io/product-images/L20812-10/2727.jpg,https://oleks-netizen.github.io/product-images/L20812-10/2728.jpg,https://oleks-netizen.github.io/product-images/L20812-10/2729.jpg,https://oleks-netizen.github.io/product-images/L20812-10/2730.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20812-10/1.jpg,https://oleks-netizen.github.io/product-images/L20812-10/2722.jpg,https://oleks-netizen.github.io/product-images/L20812-10/2723.jpg,https://oleks-netizen.github.io/product-images/L20812-10/2725.jpg,https://oleks-netizen.github.io/product-images/L20812-10/2726.jpg,https://oleks-netizen.github.io/product-images/L20812-10/2727.jpg,https://oleks-netizen.github.io/product-images/L20812-10/2728.jpg,https://oleks-netizen.github.io/product-images/L20812-10/2729.jpg,https://oleks-netizen.github.io/product-images/L20812-10/2730.jpg</t>
         </is>
       </c>
       <c r="C94" t="n">
@@ -1841,7 +1841,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20812-15/423.jpg,https://oleks-netizen.github.io/product-images/L20812-15/424.jpg,https://oleks-netizen.github.io/product-images/L20812-15/425.jpg,https://oleks-netizen.github.io/product-images/L20812-15/426.jpg,https://oleks-netizen.github.io/product-images/L20812-15/427.jpg,https://oleks-netizen.github.io/product-images/L20812-15/428.jpg,https://oleks-netizen.github.io/product-images/L20812-15/429.jpg,https://oleks-netizen.github.io/product-images/L20812-15/430.jpg,https://oleks-netizen.github.io/product-images/L20812-15/431.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20812-15/1.jpg,https://oleks-netizen.github.io/product-images/L20812-15/423.jpg,https://oleks-netizen.github.io/product-images/L20812-15/424.jpg,https://oleks-netizen.github.io/product-images/L20812-15/426.jpg,https://oleks-netizen.github.io/product-images/L20812-15/427.jpg,https://oleks-netizen.github.io/product-images/L20812-15/428.jpg,https://oleks-netizen.github.io/product-images/L20812-15/429.jpg,https://oleks-netizen.github.io/product-images/L20812-15/430.jpg,https://oleks-netizen.github.io/product-images/L20812-15/431.jpg</t>
         </is>
       </c>
       <c r="C95" t="n">
@@ -1856,7 +1856,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20812-56/2102.jpg,https://oleks-netizen.github.io/product-images/L20812-56/2103.jpg,https://oleks-netizen.github.io/product-images/L20812-56/2104.jpg,https://oleks-netizen.github.io/product-images/L20812-56/2105.jpg,https://oleks-netizen.github.io/product-images/L20812-56/2106.jpg,https://oleks-netizen.github.io/product-images/L20812-56/2107.jpg,https://oleks-netizen.github.io/product-images/L20812-56/2109.jpg,https://oleks-netizen.github.io/product-images/L20812-56/2110.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20812-56/1.jpg,https://oleks-netizen.github.io/product-images/L20812-56/2102.jpg,https://oleks-netizen.github.io/product-images/L20812-56/2103.jpg,https://oleks-netizen.github.io/product-images/L20812-56/2105.jpg,https://oleks-netizen.github.io/product-images/L20812-56/2106.jpg,https://oleks-netizen.github.io/product-images/L20812-56/2107.jpg,https://oleks-netizen.github.io/product-images/L20812-56/2109.jpg,https://oleks-netizen.github.io/product-images/L20812-56/2110.jpg</t>
         </is>
       </c>
       <c r="C96" t="n">
@@ -1871,7 +1871,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20841-58/4355.jpg,https://oleks-netizen.github.io/product-images/L20841-58/4356.jpg,https://oleks-netizen.github.io/product-images/L20841-58/4357.jpg,https://oleks-netizen.github.io/product-images/L20841-58/4358.jpg,https://oleks-netizen.github.io/product-images/L20841-58/4359.jpg,https://oleks-netizen.github.io/product-images/L20841-58/4360.jpg,https://oleks-netizen.github.io/product-images/L20841-58/4361.jpg,https://oleks-netizen.github.io/product-images/L20841-58/4362.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20841-58/1.jpg,https://oleks-netizen.github.io/product-images/L20841-58/4355.jpg,https://oleks-netizen.github.io/product-images/L20841-58/4356.jpg,https://oleks-netizen.github.io/product-images/L20841-58/4358.jpg,https://oleks-netizen.github.io/product-images/L20841-58/4359.jpg,https://oleks-netizen.github.io/product-images/L20841-58/4360.jpg,https://oleks-netizen.github.io/product-images/L20841-58/4361.jpg,https://oleks-netizen.github.io/product-images/L20841-58/4362.jpg</t>
         </is>
       </c>
       <c r="C97" t="n">
@@ -1886,7 +1886,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20849-1/2311.jpg,https://oleks-netizen.github.io/product-images/L20849-1/2312.jpg,https://oleks-netizen.github.io/product-images/L20849-1/2313.jpg,https://oleks-netizen.github.io/product-images/L20849-1/2314.jpg,https://oleks-netizen.github.io/product-images/L20849-1/2315.jpg,https://oleks-netizen.github.io/product-images/L20849-1/2316.jpg,https://oleks-netizen.github.io/product-images/L20849-1/2317.jpg,https://oleks-netizen.github.io/product-images/L20849-1/2318.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20849-1/1.jpg,https://oleks-netizen.github.io/product-images/L20849-1/2311.jpg,https://oleks-netizen.github.io/product-images/L20849-1/2312.jpg,https://oleks-netizen.github.io/product-images/L20849-1/2314.jpg,https://oleks-netizen.github.io/product-images/L20849-1/2315.jpg,https://oleks-netizen.github.io/product-images/L20849-1/2316.jpg,https://oleks-netizen.github.io/product-images/L20849-1/2317.jpg,https://oleks-netizen.github.io/product-images/L20849-1/2318.jpg</t>
         </is>
       </c>
       <c r="C98" t="n">
@@ -1901,7 +1901,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20849-701/4239.jpg,https://oleks-netizen.github.io/product-images/L20849-701/4240.jpg,https://oleks-netizen.github.io/product-images/L20849-701/4241.jpg,https://oleks-netizen.github.io/product-images/L20849-701/4242.jpg,https://oleks-netizen.github.io/product-images/L20849-701/4243.jpg,https://oleks-netizen.github.io/product-images/L20849-701/4244.jpg,https://oleks-netizen.github.io/product-images/L20849-701/4245.jpg,https://oleks-netizen.github.io/product-images/L20849-701/4246.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20849-701/1.jpg,https://oleks-netizen.github.io/product-images/L20849-701/4239.jpg,https://oleks-netizen.github.io/product-images/L20849-701/4240.jpg,https://oleks-netizen.github.io/product-images/L20849-701/4242.jpg,https://oleks-netizen.github.io/product-images/L20849-701/4243.jpg,https://oleks-netizen.github.io/product-images/L20849-701/4244.jpg,https://oleks-netizen.github.io/product-images/L20849-701/4245.jpg,https://oleks-netizen.github.io/product-images/L20849-701/4246.jpg</t>
         </is>
       </c>
       <c r="C99" t="n">
@@ -1916,7 +1916,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20849-720/2360.jpg,https://oleks-netizen.github.io/product-images/L20849-720/2361.jpg,https://oleks-netizen.github.io/product-images/L20849-720/2362.jpg,https://oleks-netizen.github.io/product-images/L20849-720/2364.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20849-720/1.jpg,https://oleks-netizen.github.io/product-images/L20849-720/2360.jpg,https://oleks-netizen.github.io/product-images/L20849-720/2361.jpg,https://oleks-netizen.github.io/product-images/L20849-720/2364.jpg</t>
         </is>
       </c>
       <c r="C100" t="n">
@@ -1931,7 +1931,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20849-811/2606.jpg,https://oleks-netizen.github.io/product-images/L20849-811/2607.jpg,https://oleks-netizen.github.io/product-images/L20849-811/2608.jpg,https://oleks-netizen.github.io/product-images/L20849-811/2609.jpg,https://oleks-netizen.github.io/product-images/L20849-811/2610.jpg,https://oleks-netizen.github.io/product-images/L20849-811/2611.jpg,https://oleks-netizen.github.io/product-images/L20849-811/2612.jpg,https://oleks-netizen.github.io/product-images/L20849-811/2613.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20849-811/1.jpg,https://oleks-netizen.github.io/product-images/L20849-811/2606.jpg,https://oleks-netizen.github.io/product-images/L20849-811/2607.jpg,https://oleks-netizen.github.io/product-images/L20849-811/2609.jpg,https://oleks-netizen.github.io/product-images/L20849-811/2610.jpg,https://oleks-netizen.github.io/product-images/L20849-811/2611.jpg,https://oleks-netizen.github.io/product-images/L20849-811/2612.jpg,https://oleks-netizen.github.io/product-images/L20849-811/2613.jpg</t>
         </is>
       </c>
       <c r="C101" t="n">
@@ -1946,7 +1946,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20853-1/2927.jpg,https://oleks-netizen.github.io/product-images/L20853-1/2928.jpg,https://oleks-netizen.github.io/product-images/L20853-1/2929.jpg,https://oleks-netizen.github.io/product-images/L20853-1/2930.jpg,https://oleks-netizen.github.io/product-images/L20853-1/2931.jpg,https://oleks-netizen.github.io/product-images/L20853-1/2932.jpg,https://oleks-netizen.github.io/product-images/L20853-1/2933.jpg,https://oleks-netizen.github.io/product-images/L20853-1/2934.jpg,https://oleks-netizen.github.io/product-images/L20853-1/2935.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20853-1/1.jpg,https://oleks-netizen.github.io/product-images/L20853-1/2927.jpg,https://oleks-netizen.github.io/product-images/L20853-1/2928.jpg,https://oleks-netizen.github.io/product-images/L20853-1/2929.jpg,https://oleks-netizen.github.io/product-images/L20853-1/2931.jpg,https://oleks-netizen.github.io/product-images/L20853-1/2932.jpg,https://oleks-netizen.github.io/product-images/L20853-1/2933.jpg,https://oleks-netizen.github.io/product-images/L20853-1/2934.jpg,https://oleks-netizen.github.io/product-images/L20853-1/2935.jpg</t>
         </is>
       </c>
       <c r="C102" t="n">
@@ -1961,7 +1961,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20993-1/2913.jpg,https://oleks-netizen.github.io/product-images/L20993-1/2914.jpg,https://oleks-netizen.github.io/product-images/L20993-1/2915.jpg,https://oleks-netizen.github.io/product-images/L20993-1/2916.jpg,https://oleks-netizen.github.io/product-images/L20993-1/2917.jpg,https://oleks-netizen.github.io/product-images/L20993-1/2918.jpg,https://oleks-netizen.github.io/product-images/L20993-1/2920.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20993-1/1.jpg,https://oleks-netizen.github.io/product-images/L20993-1/2913.jpg,https://oleks-netizen.github.io/product-images/L20993-1/2914.jpg,https://oleks-netizen.github.io/product-images/L20993-1/2916.jpg,https://oleks-netizen.github.io/product-images/L20993-1/2917.jpg,https://oleks-netizen.github.io/product-images/L20993-1/2918.jpg,https://oleks-netizen.github.io/product-images/L20993-1/2920.jpg</t>
         </is>
       </c>
       <c r="C103" t="n">
@@ -1976,7 +1976,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21019-1/2834.jpg,https://oleks-netizen.github.io/product-images/L21019-1/2835.jpg,https://oleks-netizen.github.io/product-images/L21019-1/2836.jpg,https://oleks-netizen.github.io/product-images/L21019-1/2837.jpg,https://oleks-netizen.github.io/product-images/L21019-1/2838.jpg,https://oleks-netizen.github.io/product-images/L21019-1/2839.jpg,https://oleks-netizen.github.io/product-images/L21019-1/2840.jpg,https://oleks-netizen.github.io/product-images/L21019-1/2841.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21019-1/1.jpg,https://oleks-netizen.github.io/product-images/L21019-1/2834.jpg,https://oleks-netizen.github.io/product-images/L21019-1/2835.jpg,https://oleks-netizen.github.io/product-images/L21019-1/2837.jpg,https://oleks-netizen.github.io/product-images/L21019-1/2838.jpg,https://oleks-netizen.github.io/product-images/L21019-1/2839.jpg,https://oleks-netizen.github.io/product-images/L21019-1/2840.jpg,https://oleks-netizen.github.io/product-images/L21019-1/2841.jpg</t>
         </is>
       </c>
       <c r="C104" t="n">
@@ -1991,7 +1991,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21019-142/4411.jpg,https://oleks-netizen.github.io/product-images/L21019-142/4412.jpg,https://oleks-netizen.github.io/product-images/L21019-142/4413.jpg,https://oleks-netizen.github.io/product-images/L21019-142/4414.jpg,https://oleks-netizen.github.io/product-images/L21019-142/4415.jpg,https://oleks-netizen.github.io/product-images/L21019-142/4416.jpg,https://oleks-netizen.github.io/product-images/L21019-142/4417.jpg,https://oleks-netizen.github.io/product-images/L21019-142/4418.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21019-142/1.jpg,https://oleks-netizen.github.io/product-images/L21019-142/4411.jpg,https://oleks-netizen.github.io/product-images/L21019-142/4412.jpg,https://oleks-netizen.github.io/product-images/L21019-142/4414.jpg,https://oleks-netizen.github.io/product-images/L21019-142/4415.jpg,https://oleks-netizen.github.io/product-images/L21019-142/4416.jpg,https://oleks-netizen.github.io/product-images/L21019-142/4417.jpg,https://oleks-netizen.github.io/product-images/L21019-142/4418.jpg</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -2006,7 +2006,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21035-101/166.jpg,https://oleks-netizen.github.io/product-images/L21035-101/167.jpg,https://oleks-netizen.github.io/product-images/L21035-101/168.jpg,https://oleks-netizen.github.io/product-images/L21035-101/169.jpg,https://oleks-netizen.github.io/product-images/L21035-101/170.jpg,https://oleks-netizen.github.io/product-images/L21035-101/171.jpg,https://oleks-netizen.github.io/product-images/L21035-101/172.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21035-101/166.jpg,https://oleks-netizen.github.io/product-images/L21035-101/167.jpg,https://oleks-netizen.github.io/product-images/L21035-101/169.jpg,https://oleks-netizen.github.io/product-images/L21035-101/170.jpg,https://oleks-netizen.github.io/product-images/L21035-101/171.jpg,https://oleks-netizen.github.io/product-images/L21035-101/172.jpg,https://oleks-netizen.github.io/product-images/L21035-101/1.jpg</t>
         </is>
       </c>
       <c r="C106" t="n">
@@ -2021,7 +2021,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21075-1/4522.jpg,https://oleks-netizen.github.io/product-images/L21075-1/4523.jpg,https://oleks-netizen.github.io/product-images/L21075-1/4524.jpg,https://oleks-netizen.github.io/product-images/L21075-1/4525.jpg,https://oleks-netizen.github.io/product-images/L21075-1/4526.jpg,https://oleks-netizen.github.io/product-images/L21075-1/4527.jpg,https://oleks-netizen.github.io/product-images/L21075-1/4528.jpg,https://oleks-netizen.github.io/product-images/L21075-1/4529.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21075-1/1.jpg,https://oleks-netizen.github.io/product-images/L21075-1/4522.jpg,https://oleks-netizen.github.io/product-images/L21075-1/4523.jpg,https://oleks-netizen.github.io/product-images/L21075-1/4525.jpg,https://oleks-netizen.github.io/product-images/L21075-1/4526.jpg,https://oleks-netizen.github.io/product-images/L21075-1/4527.jpg,https://oleks-netizen.github.io/product-images/L21075-1/4528.jpg,https://oleks-netizen.github.io/product-images/L21075-1/4529.jpg</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -2036,7 +2036,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21209-1/3247.jpg,https://oleks-netizen.github.io/product-images/L21209-1/3248.jpg,https://oleks-netizen.github.io/product-images/L21209-1/3249.jpg,https://oleks-netizen.github.io/product-images/L21209-1/3250.jpg,https://oleks-netizen.github.io/product-images/L21209-1/3251.jpg,https://oleks-netizen.github.io/product-images/L21209-1/3252.jpg,https://oleks-netizen.github.io/product-images/L21209-1/3253.jpg,https://oleks-netizen.github.io/product-images/L21209-1/3254.jpg,https://oleks-netizen.github.io/product-images/L21209-1/3255.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21209-1/1.jpg,https://oleks-netizen.github.io/product-images/L21209-1/3247.jpg,https://oleks-netizen.github.io/product-images/L21209-1/3248.jpg,https://oleks-netizen.github.io/product-images/L21209-1/3250.jpg,https://oleks-netizen.github.io/product-images/L21209-1/3251.jpg,https://oleks-netizen.github.io/product-images/L21209-1/3252.jpg,https://oleks-netizen.github.io/product-images/L21209-1/3253.jpg,https://oleks-netizen.github.io/product-images/L21209-1/3254.jpg,https://oleks-netizen.github.io/product-images/L21209-1/3255.jpg</t>
         </is>
       </c>
       <c r="C108" t="n">
@@ -2051,7 +2051,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21209-25/4488.jpg,https://oleks-netizen.github.io/product-images/L21209-25/4489.jpg,https://oleks-netizen.github.io/product-images/L21209-25/4490.jpg,https://oleks-netizen.github.io/product-images/L21209-25/4491.jpg,https://oleks-netizen.github.io/product-images/L21209-25/4492.jpg,https://oleks-netizen.github.io/product-images/L21209-25/4493.jpg,https://oleks-netizen.github.io/product-images/L21209-25/4494.jpg,https://oleks-netizen.github.io/product-images/L21209-25/4495.jpg,https://oleks-netizen.github.io/product-images/L21209-25/4496.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21209-25/1.jpg,https://oleks-netizen.github.io/product-images/L21209-25/4488.jpg,https://oleks-netizen.github.io/product-images/L21209-25/4489.jpg,https://oleks-netizen.github.io/product-images/L21209-25/4491.jpg,https://oleks-netizen.github.io/product-images/L21209-25/4492.jpg,https://oleks-netizen.github.io/product-images/L21209-25/4493.jpg,https://oleks-netizen.github.io/product-images/L21209-25/4494.jpg,https://oleks-netizen.github.io/product-images/L21209-25/4495.jpg,https://oleks-netizen.github.io/product-images/L21209-25/4496.jpg</t>
         </is>
       </c>
       <c r="C109" t="n">
@@ -2066,7 +2066,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21511-101/2804.jpg,https://oleks-netizen.github.io/product-images/L21511-101/2805.jpg,https://oleks-netizen.github.io/product-images/L21511-101/2806.jpg,https://oleks-netizen.github.io/product-images/L21511-101/2807.jpg,https://oleks-netizen.github.io/product-images/L21511-101/2808.jpg,https://oleks-netizen.github.io/product-images/L21511-101/2809.jpg,https://oleks-netizen.github.io/product-images/L21511-101/2810.jpg,https://oleks-netizen.github.io/product-images/L21511-101/2811.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21511-101/1.jpg,https://oleks-netizen.github.io/product-images/L21511-101/2804.jpg,https://oleks-netizen.github.io/product-images/L21511-101/2805.jpg,https://oleks-netizen.github.io/product-images/L21511-101/2807.jpg,https://oleks-netizen.github.io/product-images/L21511-101/2808.jpg,https://oleks-netizen.github.io/product-images/L21511-101/2809.jpg,https://oleks-netizen.github.io/product-images/L21511-101/2810.jpg,https://oleks-netizen.github.io/product-images/L21511-101/2811.jpg</t>
         </is>
       </c>
       <c r="C110" t="n">
@@ -2081,7 +2081,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21529-43/1431.jpg,https://oleks-netizen.github.io/product-images/L21529-43/1432.jpg,https://oleks-netizen.github.io/product-images/L21529-43/1433.jpg,https://oleks-netizen.github.io/product-images/L21529-43/1434.jpg,https://oleks-netizen.github.io/product-images/L21529-43/1435.jpg,https://oleks-netizen.github.io/product-images/L21529-43/1436.jpg,https://oleks-netizen.github.io/product-images/L21529-43/1437.jpg,https://oleks-netizen.github.io/product-images/L21529-43/1438.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21529-43/1431.jpg,https://oleks-netizen.github.io/product-images/L21529-43/1432.jpg,https://oleks-netizen.github.io/product-images/L21529-43/1434.jpg,https://oleks-netizen.github.io/product-images/L21529-43/1435.jpg,https://oleks-netizen.github.io/product-images/L21529-43/1436.jpg,https://oleks-netizen.github.io/product-images/L21529-43/1437.jpg,https://oleks-netizen.github.io/product-images/L21529-43/1438.jpg,https://oleks-netizen.github.io/product-images/L21529-43/1.jpg</t>
         </is>
       </c>
       <c r="C111" t="n">
@@ -2096,7 +2096,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21531-1/2951.jpg,https://oleks-netizen.github.io/product-images/L21531-1/2952.jpg,https://oleks-netizen.github.io/product-images/L21531-1/2953.jpg,https://oleks-netizen.github.io/product-images/L21531-1/2954.jpg,https://oleks-netizen.github.io/product-images/L21531-1/2955.jpg,https://oleks-netizen.github.io/product-images/L21531-1/2956.jpg,https://oleks-netizen.github.io/product-images/L21531-1/2957.jpg,https://oleks-netizen.github.io/product-images/L21531-1/2958.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21531-1/1.jpg,https://oleks-netizen.github.io/product-images/L21531-1/2951.jpg,https://oleks-netizen.github.io/product-images/L21531-1/2952.jpg,https://oleks-netizen.github.io/product-images/L21531-1/2954.jpg,https://oleks-netizen.github.io/product-images/L21531-1/2955.jpg,https://oleks-netizen.github.io/product-images/L21531-1/2956.jpg,https://oleks-netizen.github.io/product-images/L21531-1/2957.jpg,https://oleks-netizen.github.io/product-images/L21531-1/2958.jpg</t>
         </is>
       </c>
       <c r="C112" t="n">
@@ -2111,7 +2111,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21531-11/2153.jpg,https://oleks-netizen.github.io/product-images/L21531-11/2154.jpg,https://oleks-netizen.github.io/product-images/L21531-11/2155.jpg,https://oleks-netizen.github.io/product-images/L21531-11/2156.jpg,https://oleks-netizen.github.io/product-images/L21531-11/2157.jpg,https://oleks-netizen.github.io/product-images/L21531-11/2158.jpg,https://oleks-netizen.github.io/product-images/L21531-11/2159.jpg,https://oleks-netizen.github.io/product-images/L21531-11/2160.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21531-11/1.jpg,https://oleks-netizen.github.io/product-images/L21531-11/2153.jpg,https://oleks-netizen.github.io/product-images/L21531-11/2154.jpg,https://oleks-netizen.github.io/product-images/L21531-11/2156.jpg,https://oleks-netizen.github.io/product-images/L21531-11/2157.jpg,https://oleks-netizen.github.io/product-images/L21531-11/2158.jpg,https://oleks-netizen.github.io/product-images/L21531-11/2159.jpg,https://oleks-netizen.github.io/product-images/L21531-11/2160.jpg</t>
         </is>
       </c>
       <c r="C113" t="n">
@@ -2126,7 +2126,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21545-1/5389.jpg,https://oleks-netizen.github.io/product-images/L21545-1/5390.jpg,https://oleks-netizen.github.io/product-images/L21545-1/5391.jpg,https://oleks-netizen.github.io/product-images/L21545-1/5392.jpg,https://oleks-netizen.github.io/product-images/L21545-1/5393.jpg,https://oleks-netizen.github.io/product-images/L21545-1/5394.jpg,https://oleks-netizen.github.io/product-images/L21545-1/5395.jpg,https://oleks-netizen.github.io/product-images/L21545-1/5396.jpg,https://oleks-netizen.github.io/product-images/L21545-1/5397.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21545-1/1.jpg,https://oleks-netizen.github.io/product-images/L21545-1/5389.jpg,https://oleks-netizen.github.io/product-images/L21545-1/5390.jpg,https://oleks-netizen.github.io/product-images/L21545-1/5392.jpg,https://oleks-netizen.github.io/product-images/L21545-1/5393.jpg,https://oleks-netizen.github.io/product-images/L21545-1/5394.jpg,https://oleks-netizen.github.io/product-images/L21545-1/5395.jpg,https://oleks-netizen.github.io/product-images/L21545-1/5396.jpg,https://oleks-netizen.github.io/product-images/L21545-1/5397.jpg</t>
         </is>
       </c>
       <c r="C114" t="n">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21545-175/5996.jpg,https://oleks-netizen.github.io/product-images/L21545-175/5997.jpg,https://oleks-netizen.github.io/product-images/L21545-175/5998.jpg,https://oleks-netizen.github.io/product-images/L21545-175/5999.jpg,https://oleks-netizen.github.io/product-images/L21545-175/6000.jpg,https://oleks-netizen.github.io/product-images/L21545-175/6001.jpg,https://oleks-netizen.github.io/product-images/L21545-175/6002.jpg,https://oleks-netizen.github.io/product-images/L21545-175/6003.jpg,https://oleks-netizen.github.io/product-images/L21545-175/6004.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21545-175/1.jpg,https://oleks-netizen.github.io/product-images/L21545-175/5996.jpg,https://oleks-netizen.github.io/product-images/L21545-175/5997.jpg,https://oleks-netizen.github.io/product-images/L21545-175/5999.jpg,https://oleks-netizen.github.io/product-images/L21545-175/6000.jpg,https://oleks-netizen.github.io/product-images/L21545-175/6001.jpg,https://oleks-netizen.github.io/product-images/L21545-175/6002.jpg,https://oleks-netizen.github.io/product-images/L21545-175/6003.jpg,https://oleks-netizen.github.io/product-images/L21545-175/6004.jpg</t>
         </is>
       </c>
       <c r="C115" t="n">
@@ -2156,7 +2156,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21547-64/4631.jpg,https://oleks-netizen.github.io/product-images/L21547-64/4632.jpg,https://oleks-netizen.github.io/product-images/L21547-64/4633.jpg,https://oleks-netizen.github.io/product-images/L21547-64/4634.jpg,https://oleks-netizen.github.io/product-images/L21547-64/4635.jpg,https://oleks-netizen.github.io/product-images/L21547-64/4636.jpg,https://oleks-netizen.github.io/product-images/L21547-64/4637.jpg,https://oleks-netizen.github.io/product-images/L21547-64/4638.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21547-64/1.jpg,https://oleks-netizen.github.io/product-images/L21547-64/4631.jpg,https://oleks-netizen.github.io/product-images/L21547-64/4632.jpg,https://oleks-netizen.github.io/product-images/L21547-64/4634.jpg,https://oleks-netizen.github.io/product-images/L21547-64/4635.jpg,https://oleks-netizen.github.io/product-images/L21547-64/4636.jpg,https://oleks-netizen.github.io/product-images/L21547-64/4637.jpg,https://oleks-netizen.github.io/product-images/L21547-64/4638.jpg</t>
         </is>
       </c>
       <c r="C116" t="n">
@@ -2171,7 +2171,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21549-1/4564.jpg,https://oleks-netizen.github.io/product-images/L21549-1/4565.jpg,https://oleks-netizen.github.io/product-images/L21549-1/4566.jpg,https://oleks-netizen.github.io/product-images/L21549-1/4567.jpg,https://oleks-netizen.github.io/product-images/L21549-1/4568.jpg,https://oleks-netizen.github.io/product-images/L21549-1/4569.jpg,https://oleks-netizen.github.io/product-images/L21549-1/4570.jpg,https://oleks-netizen.github.io/product-images/L21549-1/4571.jpg,https://oleks-netizen.github.io/product-images/L21549-1/4572.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21549-1/1.jpg,https://oleks-netizen.github.io/product-images/L21549-1/4564.jpg,https://oleks-netizen.github.io/product-images/L21549-1/4565.jpg,https://oleks-netizen.github.io/product-images/L21549-1/4566.jpg,https://oleks-netizen.github.io/product-images/L21549-1/4568.jpg,https://oleks-netizen.github.io/product-images/L21549-1/4569.jpg,https://oleks-netizen.github.io/product-images/L21549-1/4570.jpg,https://oleks-netizen.github.io/product-images/L21549-1/4571.jpg,https://oleks-netizen.github.io/product-images/L21549-1/4572.jpg</t>
         </is>
       </c>
       <c r="C117" t="n">
@@ -2186,7 +2186,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21549-22/2079.jpg,https://oleks-netizen.github.io/product-images/L21549-22/2080.jpg,https://oleks-netizen.github.io/product-images/L21549-22/2081.jpg,https://oleks-netizen.github.io/product-images/L21549-22/2082.jpg,https://oleks-netizen.github.io/product-images/L21549-22/2083.jpg,https://oleks-netizen.github.io/product-images/L21549-22/2084.jpg,https://oleks-netizen.github.io/product-images/L21549-22/2085.jpg,https://oleks-netizen.github.io/product-images/L21549-22/2086.jpg,https://oleks-netizen.github.io/product-images/L21549-22/2087.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21549-22/1.jpg,https://oleks-netizen.github.io/product-images/L21549-22/2079.jpg,https://oleks-netizen.github.io/product-images/L21549-22/2080.jpg,https://oleks-netizen.github.io/product-images/L21549-22/2081.jpg,https://oleks-netizen.github.io/product-images/L21549-22/2083.jpg,https://oleks-netizen.github.io/product-images/L21549-22/2084.jpg,https://oleks-netizen.github.io/product-images/L21549-22/2085.jpg,https://oleks-netizen.github.io/product-images/L21549-22/2086.jpg,https://oleks-netizen.github.io/product-images/L21549-22/2087.jpg</t>
         </is>
       </c>
       <c r="C118" t="n">
@@ -2201,7 +2201,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21557-1/3864.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3865.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3866.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3867.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3868.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3869.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3870.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3871.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3872.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3873.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21557-1/1.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3864.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3865.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3866.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3868.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3869.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3870.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3871.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3872.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3873.jpg</t>
         </is>
       </c>
       <c r="C119" t="n">
@@ -2216,7 +2216,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21557-173/3476.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3477.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3478.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3479.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3480.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3481.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3482.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3483.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3484.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3485.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21557-173/1.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3476.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3477.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3478.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3480.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3481.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3482.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3483.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3484.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3485.jpg</t>
         </is>
       </c>
       <c r="C120" t="n">
@@ -2231,7 +2231,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21561-1/2782.jpg,https://oleks-netizen.github.io/product-images/L21561-1/2783.jpg,https://oleks-netizen.github.io/product-images/L21561-1/2784.jpg,https://oleks-netizen.github.io/product-images/L21561-1/2785.jpg,https://oleks-netizen.github.io/product-images/L21561-1/2786.jpg,https://oleks-netizen.github.io/product-images/L21561-1/2787.jpg,https://oleks-netizen.github.io/product-images/L21561-1/2788.jpg,https://oleks-netizen.github.io/product-images/L21561-1/2789.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21561-1/1.jpg,https://oleks-netizen.github.io/product-images/L21561-1/2782.jpg,https://oleks-netizen.github.io/product-images/L21561-1/2783.jpg,https://oleks-netizen.github.io/product-images/L21561-1/2785.jpg,https://oleks-netizen.github.io/product-images/L21561-1/2786.jpg,https://oleks-netizen.github.io/product-images/L21561-1/2787.jpg,https://oleks-netizen.github.io/product-images/L21561-1/2788.jpg,https://oleks-netizen.github.io/product-images/L21561-1/2789.jpg</t>
         </is>
       </c>
       <c r="C121" t="n">
@@ -2246,7 +2246,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21561-25/438.jpg,https://oleks-netizen.github.io/product-images/L21561-25/439.jpg,https://oleks-netizen.github.io/product-images/L21561-25/440.jpg,https://oleks-netizen.github.io/product-images/L21561-25/441.jpg,https://oleks-netizen.github.io/product-images/L21561-25/442.jpg,https://oleks-netizen.github.io/product-images/L21561-25/443.jpg,https://oleks-netizen.github.io/product-images/L21561-25/444.jpg,https://oleks-netizen.github.io/product-images/L21561-25/445.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21561-25/1.jpg,https://oleks-netizen.github.io/product-images/L21561-25/438.jpg,https://oleks-netizen.github.io/product-images/L21561-25/439.jpg,https://oleks-netizen.github.io/product-images/L21561-25/441.jpg,https://oleks-netizen.github.io/product-images/L21561-25/442.jpg,https://oleks-netizen.github.io/product-images/L21561-25/443.jpg,https://oleks-netizen.github.io/product-images/L21561-25/444.jpg,https://oleks-netizen.github.io/product-images/L21561-25/445.jpg</t>
         </is>
       </c>
       <c r="C122" t="n">
@@ -2261,7 +2261,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22007-1K/4694.jpg,https://oleks-netizen.github.io/product-images/L22007-1K/4695.jpg,https://oleks-netizen.github.io/product-images/L22007-1K/4696.jpg,https://oleks-netizen.github.io/product-images/L22007-1K/4697.jpg,https://oleks-netizen.github.io/product-images/L22007-1K/4698.jpg,https://oleks-netizen.github.io/product-images/L22007-1K/4699.jpg,https://oleks-netizen.github.io/product-images/L22007-1K/4700.jpg,https://oleks-netizen.github.io/product-images/L22007-1K/4701.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22007-1K/1.jpg,https://oleks-netizen.github.io/product-images/L22007-1K/4694.jpg,https://oleks-netizen.github.io/product-images/L22007-1K/4695.jpg,https://oleks-netizen.github.io/product-images/L22007-1K/4697.jpg,https://oleks-netizen.github.io/product-images/L22007-1K/4698.jpg,https://oleks-netizen.github.io/product-images/L22007-1K/4699.jpg,https://oleks-netizen.github.io/product-images/L22007-1K/4700.jpg,https://oleks-netizen.github.io/product-images/L22007-1K/4701.jpg</t>
         </is>
       </c>
       <c r="C123" t="n">
@@ -2276,7 +2276,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22007-3K/1998.jpg,https://oleks-netizen.github.io/product-images/L22007-3K/1999.jpg,https://oleks-netizen.github.io/product-images/L22007-3K/2000.jpg,https://oleks-netizen.github.io/product-images/L22007-3K/2001.jpg,https://oleks-netizen.github.io/product-images/L22007-3K/2002.jpg,https://oleks-netizen.github.io/product-images/L22007-3K/2003.jpg,https://oleks-netizen.github.io/product-images/L22007-3K/2004.jpg,https://oleks-netizen.github.io/product-images/L22007-3K/2005.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22007-3K/1998.jpg,https://oleks-netizen.github.io/product-images/L22007-3K/1999.jpg,https://oleks-netizen.github.io/product-images/L22007-3K/1.jpg,https://oleks-netizen.github.io/product-images/L22007-3K/2001.jpg,https://oleks-netizen.github.io/product-images/L22007-3K/2002.jpg,https://oleks-netizen.github.io/product-images/L22007-3K/2003.jpg,https://oleks-netizen.github.io/product-images/L22007-3K/2004.jpg,https://oleks-netizen.github.io/product-images/L22007-3K/2005.jpg</t>
         </is>
       </c>
       <c r="C124" t="n">
@@ -2291,7 +2291,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22008-1/5288.jpg,https://oleks-netizen.github.io/product-images/L22008-1/5289.jpg,https://oleks-netizen.github.io/product-images/L22008-1/5290.jpg,https://oleks-netizen.github.io/product-images/L22008-1/5291.jpg,https://oleks-netizen.github.io/product-images/L22008-1/5292.jpg,https://oleks-netizen.github.io/product-images/L22008-1/5293.jpg,https://oleks-netizen.github.io/product-images/L22008-1/5294.jpg,https://oleks-netizen.github.io/product-images/L22008-1/5295.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22008-1/1.jpg,https://oleks-netizen.github.io/product-images/L22008-1/5288.jpg,https://oleks-netizen.github.io/product-images/L22008-1/5289.jpg,https://oleks-netizen.github.io/product-images/L22008-1/5291.jpg,https://oleks-netizen.github.io/product-images/L22008-1/5292.jpg,https://oleks-netizen.github.io/product-images/L22008-1/5293.jpg,https://oleks-netizen.github.io/product-images/L22008-1/5294.jpg,https://oleks-netizen.github.io/product-images/L22008-1/5295.jpg</t>
         </is>
       </c>
       <c r="C125" t="n">
@@ -2306,7 +2306,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22008-12/315.jpg,https://oleks-netizen.github.io/product-images/L22008-12/316.jpg,https://oleks-netizen.github.io/product-images/L22008-12/317.jpg,https://oleks-netizen.github.io/product-images/L22008-12/318.jpg,https://oleks-netizen.github.io/product-images/L22008-12/319.jpg,https://oleks-netizen.github.io/product-images/L22008-12/320.jpg,https://oleks-netizen.github.io/product-images/L22008-12/321.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22008-12/1.jpg,https://oleks-netizen.github.io/product-images/L22008-12/315.jpg,https://oleks-netizen.github.io/product-images/L22008-12/316.jpg,https://oleks-netizen.github.io/product-images/L22008-12/318.jpg,https://oleks-netizen.github.io/product-images/L22008-12/319.jpg,https://oleks-netizen.github.io/product-images/L22008-12/320.jpg,https://oleks-netizen.github.io/product-images/L22008-12/321.jpg</t>
         </is>
       </c>
       <c r="C126" t="n">
@@ -2321,7 +2321,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22008-8/5347.jpg,https://oleks-netizen.github.io/product-images/L22008-8/5348.jpg,https://oleks-netizen.github.io/product-images/L22008-8/5349.jpg,https://oleks-netizen.github.io/product-images/L22008-8/5350.jpg,https://oleks-netizen.github.io/product-images/L22008-8/5351.jpg,https://oleks-netizen.github.io/product-images/L22008-8/5352.jpg,https://oleks-netizen.github.io/product-images/L22008-8/5353.jpg,https://oleks-netizen.github.io/product-images/L22008-8/5354.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22008-8/1.jpg,https://oleks-netizen.github.io/product-images/L22008-8/5347.jpg,https://oleks-netizen.github.io/product-images/L22008-8/5348.jpg,https://oleks-netizen.github.io/product-images/L22008-8/5350.jpg,https://oleks-netizen.github.io/product-images/L22008-8/5351.jpg,https://oleks-netizen.github.io/product-images/L22008-8/5352.jpg,https://oleks-netizen.github.io/product-images/L22008-8/5353.jpg,https://oleks-netizen.github.io/product-images/L22008-8/5354.jpg</t>
         </is>
       </c>
       <c r="C127" t="n">
@@ -2336,7 +2336,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22009-1/5232.jpg,https://oleks-netizen.github.io/product-images/L22009-1/5233.jpg,https://oleks-netizen.github.io/product-images/L22009-1/5234.jpg,https://oleks-netizen.github.io/product-images/L22009-1/5235.jpg,https://oleks-netizen.github.io/product-images/L22009-1/5236.jpg,https://oleks-netizen.github.io/product-images/L22009-1/5237.jpg,https://oleks-netizen.github.io/product-images/L22009-1/5238.jpg,https://oleks-netizen.github.io/product-images/L22009-1/5239.jpg,https://oleks-netizen.github.io/product-images/L22009-1/5240.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22009-1/1.jpg,https://oleks-netizen.github.io/product-images/L22009-1/5232.jpg,https://oleks-netizen.github.io/product-images/L22009-1/5233.jpg,https://oleks-netizen.github.io/product-images/L22009-1/5235.jpg,https://oleks-netizen.github.io/product-images/L22009-1/5236.jpg,https://oleks-netizen.github.io/product-images/L22009-1/5237.jpg,https://oleks-netizen.github.io/product-images/L22009-1/5238.jpg,https://oleks-netizen.github.io/product-images/L22009-1/5239.jpg,https://oleks-netizen.github.io/product-images/L22009-1/5240.jpg</t>
         </is>
       </c>
       <c r="C128" t="n">
@@ -2351,7 +2351,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22009-35/2222.jpg,https://oleks-netizen.github.io/product-images/L22009-35/2223.jpg,https://oleks-netizen.github.io/product-images/L22009-35/2224.jpg,https://oleks-netizen.github.io/product-images/L22009-35/2225.jpg,https://oleks-netizen.github.io/product-images/L22009-35/2226.jpg,https://oleks-netizen.github.io/product-images/L22009-35/2227.jpg,https://oleks-netizen.github.io/product-images/L22009-35/2228.jpg,https://oleks-netizen.github.io/product-images/L22009-35/2229.jpg,https://oleks-netizen.github.io/product-images/L22009-35/2230.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22009-35/1.jpg,https://oleks-netizen.github.io/product-images/L22009-35/2222.jpg,https://oleks-netizen.github.io/product-images/L22009-35/2223.jpg,https://oleks-netizen.github.io/product-images/L22009-35/2225.jpg,https://oleks-netizen.github.io/product-images/L22009-35/2226.jpg,https://oleks-netizen.github.io/product-images/L22009-35/2227.jpg,https://oleks-netizen.github.io/product-images/L22009-35/2228.jpg,https://oleks-netizen.github.io/product-images/L22009-35/2229.jpg,https://oleks-netizen.github.io/product-images/L22009-35/2230.jpg</t>
         </is>
       </c>
       <c r="C129" t="n">
@@ -2366,7 +2366,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22018-2W/3764.jpg,https://oleks-netizen.github.io/product-images/L22018-2W/3765.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22018-2W/1.jpg,https://oleks-netizen.github.io/product-images/L22018-2W/3764.jpg</t>
         </is>
       </c>
       <c r="C130" t="n">
@@ -2381,7 +2381,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22098-1/2899.jpg,https://oleks-netizen.github.io/product-images/L22098-1/2900.jpg,https://oleks-netizen.github.io/product-images/L22098-1/2901.jpg,https://oleks-netizen.github.io/product-images/L22098-1/2902.jpg,https://oleks-netizen.github.io/product-images/L22098-1/2903.jpg,https://oleks-netizen.github.io/product-images/L22098-1/2904.jpg,https://oleks-netizen.github.io/product-images/L22098-1/2905.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22098-1/1.jpg,https://oleks-netizen.github.io/product-images/L22098-1/2899.jpg,https://oleks-netizen.github.io/product-images/L22098-1/2901.jpg,https://oleks-netizen.github.io/product-images/L22098-1/2902.jpg,https://oleks-netizen.github.io/product-images/L22098-1/2903.jpg,https://oleks-netizen.github.io/product-images/L22098-1/2904.jpg,https://oleks-netizen.github.io/product-images/L22098-1/2905.jpg</t>
         </is>
       </c>
       <c r="C131" t="n">
@@ -2396,7 +2396,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22125-1/3847.jpg,https://oleks-netizen.github.io/product-images/L22125-1/3848.jpg,https://oleks-netizen.github.io/product-images/L22125-1/3849.jpg,https://oleks-netizen.github.io/product-images/L22125-1/3850.jpg,https://oleks-netizen.github.io/product-images/L22125-1/3851.jpg,https://oleks-netizen.github.io/product-images/L22125-1/3852.jpg,https://oleks-netizen.github.io/product-images/L22125-1/3853.jpg,https://oleks-netizen.github.io/product-images/L22125-1/3854.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22125-1/1.jpg,https://oleks-netizen.github.io/product-images/L22125-1/3847.jpg,https://oleks-netizen.github.io/product-images/L22125-1/3848.jpg,https://oleks-netizen.github.io/product-images/L22125-1/3850.jpg,https://oleks-netizen.github.io/product-images/L22125-1/3851.jpg,https://oleks-netizen.github.io/product-images/L22125-1/3852.jpg,https://oleks-netizen.github.io/product-images/L22125-1/3853.jpg,https://oleks-netizen.github.io/product-images/L22125-1/3854.jpg</t>
         </is>
       </c>
       <c r="C132" t="n">
@@ -2411,7 +2411,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22125-8/1000.jpg,https://oleks-netizen.github.io/product-images/L22125-8/1001.jpg,https://oleks-netizen.github.io/product-images/L22125-8/1002.jpg,https://oleks-netizen.github.io/product-images/L22125-8/1003.jpg,https://oleks-netizen.github.io/product-images/L22125-8/996.jpg,https://oleks-netizen.github.io/product-images/L22125-8/997.jpg,https://oleks-netizen.github.io/product-images/L22125-8/998.jpg,https://oleks-netizen.github.io/product-images/L22125-8/999.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22125-8/1000.jpg,https://oleks-netizen.github.io/product-images/L22125-8/1001.jpg,https://oleks-netizen.github.io/product-images/L22125-8/1002.jpg,https://oleks-netizen.github.io/product-images/L22125-8/1003.jpg,https://oleks-netizen.github.io/product-images/L22125-8/1.jpg,https://oleks-netizen.github.io/product-images/L22125-8/996.jpg,https://oleks-netizen.github.io/product-images/L22125-8/997.jpg,https://oleks-netizen.github.io/product-images/L22125-8/999.jpg</t>
         </is>
       </c>
       <c r="C133" t="n">
@@ -2426,7 +2426,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22162-1W/3944.jpg,https://oleks-netizen.github.io/product-images/L22162-1W/3945.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22162-1W/1.jpg,https://oleks-netizen.github.io/product-images/L22162-1W/3944.jpg</t>
         </is>
       </c>
       <c r="C134" t="n">
@@ -2441,7 +2441,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22187-1W/2487.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/2488.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/2489.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/2490.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/2491.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/2492.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/2493.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/2494.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/2495.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22187-1W/1.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/2487.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/2488.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/2490.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/2491.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/2492.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/2493.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/2494.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/2495.jpg</t>
         </is>
       </c>
       <c r="C135" t="n">
@@ -2456,7 +2456,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22187-1X/1184.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/1185.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/1186.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/1187.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/1188.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/1189.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/1190.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/1191.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/1192.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22187-1X/1184.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/1185.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/1187.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/1188.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/1189.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/1190.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/1191.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/1192.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/1.jpg</t>
         </is>
       </c>
       <c r="C136" t="n">
@@ -2471,7 +2471,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22322-01/2936.jpg,https://oleks-netizen.github.io/product-images/L22322-01/2937.jpg,https://oleks-netizen.github.io/product-images/L22322-01/2938.jpg,https://oleks-netizen.github.io/product-images/L22322-01/2939.jpg,https://oleks-netizen.github.io/product-images/L22322-01/2940.jpg,https://oleks-netizen.github.io/product-images/L22322-01/2941.jpg,https://oleks-netizen.github.io/product-images/L22322-01/2942.jpg,https://oleks-netizen.github.io/product-images/L22322-01/2943.jpg,https://oleks-netizen.github.io/product-images/L22322-01/2944.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22322-01/1.jpg,https://oleks-netizen.github.io/product-images/L22322-01/2936.jpg,https://oleks-netizen.github.io/product-images/L22322-01/2937.jpg,https://oleks-netizen.github.io/product-images/L22322-01/2939.jpg,https://oleks-netizen.github.io/product-images/L22322-01/2940.jpg,https://oleks-netizen.github.io/product-images/L22322-01/2941.jpg,https://oleks-netizen.github.io/product-images/L22322-01/2942.jpg,https://oleks-netizen.github.io/product-images/L22322-01/2943.jpg,https://oleks-netizen.github.io/product-images/L22322-01/2944.jpg</t>
         </is>
       </c>
       <c r="C137" t="n">
@@ -2486,7 +2486,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22322-02/5568.jpg,https://oleks-netizen.github.io/product-images/L22322-02/5569.jpg,https://oleks-netizen.github.io/product-images/L22322-02/5570.jpg,https://oleks-netizen.github.io/product-images/L22322-02/5571.jpg,https://oleks-netizen.github.io/product-images/L22322-02/5572.jpg,https://oleks-netizen.github.io/product-images/L22322-02/5573.jpg,https://oleks-netizen.github.io/product-images/L22322-02/5574.jpg,https://oleks-netizen.github.io/product-images/L22322-02/5575.jpg,https://oleks-netizen.github.io/product-images/L22322-02/5576.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22322-02/1.jpg,https://oleks-netizen.github.io/product-images/L22322-02/5568.jpg,https://oleks-netizen.github.io/product-images/L22322-02/5569.jpg,https://oleks-netizen.github.io/product-images/L22322-02/5571.jpg,https://oleks-netizen.github.io/product-images/L22322-02/5572.jpg,https://oleks-netizen.github.io/product-images/L22322-02/5573.jpg,https://oleks-netizen.github.io/product-images/L22322-02/5574.jpg,https://oleks-netizen.github.io/product-images/L22322-02/5575.jpg,https://oleks-netizen.github.io/product-images/L22322-02/5576.jpg</t>
         </is>
       </c>
       <c r="C138" t="n">
@@ -2501,7 +2501,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22322-1/2650.jpg,https://oleks-netizen.github.io/product-images/L22322-1/2651.jpg,https://oleks-netizen.github.io/product-images/L22322-1/2652.jpg,https://oleks-netizen.github.io/product-images/L22322-1/2653.jpg,https://oleks-netizen.github.io/product-images/L22322-1/2654.jpg,https://oleks-netizen.github.io/product-images/L22322-1/2655.jpg,https://oleks-netizen.github.io/product-images/L22322-1/2656.jpg,https://oleks-netizen.github.io/product-images/L22322-1/2657.jpg,https://oleks-netizen.github.io/product-images/L22322-1/2658.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22322-1/1.jpg,https://oleks-netizen.github.io/product-images/L22322-1/2650.jpg,https://oleks-netizen.github.io/product-images/L22322-1/2651.jpg,https://oleks-netizen.github.io/product-images/L22322-1/2653.jpg,https://oleks-netizen.github.io/product-images/L22322-1/2654.jpg,https://oleks-netizen.github.io/product-images/L22322-1/2655.jpg,https://oleks-netizen.github.io/product-images/L22322-1/2656.jpg,https://oleks-netizen.github.io/product-images/L22322-1/2657.jpg,https://oleks-netizen.github.io/product-images/L22322-1/2658.jpg</t>
         </is>
       </c>
       <c r="C139" t="n">
@@ -2516,7 +2516,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22322-4/2244.jpg,https://oleks-netizen.github.io/product-images/L22322-4/2245.jpg,https://oleks-netizen.github.io/product-images/L22322-4/2246.jpg,https://oleks-netizen.github.io/product-images/L22322-4/2247.jpg,https://oleks-netizen.github.io/product-images/L22322-4/2248.jpg,https://oleks-netizen.github.io/product-images/L22322-4/2249.jpg,https://oleks-netizen.github.io/product-images/L22322-4/2250.jpg,https://oleks-netizen.github.io/product-images/L22322-4/2251.jpg,https://oleks-netizen.github.io/product-images/L22322-4/2252.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22322-4/1.jpg,https://oleks-netizen.github.io/product-images/L22322-4/2244.jpg,https://oleks-netizen.github.io/product-images/L22322-4/2245.jpg,https://oleks-netizen.github.io/product-images/L22322-4/2247.jpg,https://oleks-netizen.github.io/product-images/L22322-4/2248.jpg,https://oleks-netizen.github.io/product-images/L22322-4/2249.jpg,https://oleks-netizen.github.io/product-images/L22322-4/2250.jpg,https://oleks-netizen.github.io/product-images/L22322-4/2251.jpg,https://oleks-netizen.github.io/product-images/L22322-4/2252.jpg</t>
         </is>
       </c>
       <c r="C140" t="n">
@@ -2531,7 +2531,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22532-01/760.jpg,https://oleks-netizen.github.io/product-images/L22532-01/761.jpg,https://oleks-netizen.github.io/product-images/L22532-01/762.jpg,https://oleks-netizen.github.io/product-images/L22532-01/763.jpg,https://oleks-netizen.github.io/product-images/L22532-01/764.jpg,https://oleks-netizen.github.io/product-images/L22532-01/765.jpg,https://oleks-netizen.github.io/product-images/L22532-01/766.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22532-01/1.jpg,https://oleks-netizen.github.io/product-images/L22532-01/760.jpg,https://oleks-netizen.github.io/product-images/L22532-01/762.jpg,https://oleks-netizen.github.io/product-images/L22532-01/763.jpg,https://oleks-netizen.github.io/product-images/L22532-01/764.jpg,https://oleks-netizen.github.io/product-images/L22532-01/765.jpg,https://oleks-netizen.github.io/product-images/L22532-01/766.jpg</t>
         </is>
       </c>
       <c r="C141" t="n">
@@ -2546,7 +2546,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22532-03/4339.jpg,https://oleks-netizen.github.io/product-images/L22532-03/4340.jpg,https://oleks-netizen.github.io/product-images/L22532-03/4341.jpg,https://oleks-netizen.github.io/product-images/L22532-03/4342.jpg,https://oleks-netizen.github.io/product-images/L22532-03/4343.jpg,https://oleks-netizen.github.io/product-images/L22532-03/4344.jpg,https://oleks-netizen.github.io/product-images/L22532-03/4345.jpg,https://oleks-netizen.github.io/product-images/L22532-03/4346.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22532-03/1.jpg,https://oleks-netizen.github.io/product-images/L22532-03/4339.jpg,https://oleks-netizen.github.io/product-images/L22532-03/4341.jpg,https://oleks-netizen.github.io/product-images/L22532-03/4342.jpg,https://oleks-netizen.github.io/product-images/L22532-03/4343.jpg,https://oleks-netizen.github.io/product-images/L22532-03/4344.jpg,https://oleks-netizen.github.io/product-images/L22532-03/4345.jpg,https://oleks-netizen.github.io/product-images/L22532-03/4346.jpg</t>
         </is>
       </c>
       <c r="C142" t="n">
@@ -2561,7 +2561,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22537-179/4308.jpg,https://oleks-netizen.github.io/product-images/L22537-179/4310.jpg,https://oleks-netizen.github.io/product-images/L22537-179/4311.jpg,https://oleks-netizen.github.io/product-images/L22537-179/4312.jpg,https://oleks-netizen.github.io/product-images/L22537-179/4313.jpg,https://oleks-netizen.github.io/product-images/L22537-179/4314.jpg,https://oleks-netizen.github.io/product-images/L22537-179/4315.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22537-179/1.jpg,https://oleks-netizen.github.io/product-images/L22537-179/4308.jpg,https://oleks-netizen.github.io/product-images/L22537-179/4311.jpg,https://oleks-netizen.github.io/product-images/L22537-179/4312.jpg,https://oleks-netizen.github.io/product-images/L22537-179/4313.jpg,https://oleks-netizen.github.io/product-images/L22537-179/4314.jpg,https://oleks-netizen.github.io/product-images/L22537-179/4315.jpg</t>
         </is>
       </c>
       <c r="C143" t="n">
@@ -2576,7 +2576,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22613-1/5577.jpg,https://oleks-netizen.github.io/product-images/L22613-1/5579.jpg,https://oleks-netizen.github.io/product-images/L22613-1/5580.jpg,https://oleks-netizen.github.io/product-images/L22613-1/5581.jpg,https://oleks-netizen.github.io/product-images/L22613-1/5582.jpg,https://oleks-netizen.github.io/product-images/L22613-1/5583.jpg,https://oleks-netizen.github.io/product-images/L22613-1/5584.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22613-1/1.jpg,https://oleks-netizen.github.io/product-images/L22613-1/5577.jpg,https://oleks-netizen.github.io/product-images/L22613-1/5580.jpg,https://oleks-netizen.github.io/product-images/L22613-1/5581.jpg,https://oleks-netizen.github.io/product-images/L22613-1/5582.jpg,https://oleks-netizen.github.io/product-images/L22613-1/5583.jpg,https://oleks-netizen.github.io/product-images/L22613-1/5584.jpg</t>
         </is>
       </c>
       <c r="C144" t="n">
@@ -2591,7 +2591,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22613-2S/5699.jpg,https://oleks-netizen.github.io/product-images/L22613-2S/5701.jpg,https://oleks-netizen.github.io/product-images/L22613-2S/5702.jpg,https://oleks-netizen.github.io/product-images/L22613-2S/5703.jpg,https://oleks-netizen.github.io/product-images/L22613-2S/5704.jpg,https://oleks-netizen.github.io/product-images/L22613-2S/5705.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22613-2S/1.jpg,https://oleks-netizen.github.io/product-images/L22613-2S/5699.jpg,https://oleks-netizen.github.io/product-images/L22613-2S/5702.jpg,https://oleks-netizen.github.io/product-images/L22613-2S/5703.jpg,https://oleks-netizen.github.io/product-images/L22613-2S/5704.jpg,https://oleks-netizen.github.io/product-images/L22613-2S/5705.jpg</t>
         </is>
       </c>
       <c r="C145" t="n">
@@ -2606,7 +2606,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22619-1X/1422.jpg,https://oleks-netizen.github.io/product-images/L22619-1X/1424.jpg,https://oleks-netizen.github.io/product-images/L22619-1X/1425.jpg,https://oleks-netizen.github.io/product-images/L22619-1X/1426.jpg,https://oleks-netizen.github.io/product-images/L22619-1X/1427.jpg,https://oleks-netizen.github.io/product-images/L22619-1X/1428.jpg,https://oleks-netizen.github.io/product-images/L22619-1X/1429.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22619-1X/1422.jpg,https://oleks-netizen.github.io/product-images/L22619-1X/1425.jpg,https://oleks-netizen.github.io/product-images/L22619-1X/1426.jpg,https://oleks-netizen.github.io/product-images/L22619-1X/1427.jpg,https://oleks-netizen.github.io/product-images/L22619-1X/1428.jpg,https://oleks-netizen.github.io/product-images/L22619-1X/1429.jpg,https://oleks-netizen.github.io/product-images/L22619-1X/1.jpg</t>
         </is>
       </c>
       <c r="C146" t="n">
@@ -2621,7 +2621,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22661-1/573.jpg,https://oleks-netizen.github.io/product-images/L22661-1/575.jpg,https://oleks-netizen.github.io/product-images/L22661-1/576.jpg,https://oleks-netizen.github.io/product-images/L22661-1/577.jpg,https://oleks-netizen.github.io/product-images/L22661-1/578.jpg,https://oleks-netizen.github.io/product-images/L22661-1/579.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22661-1/1.jpg,https://oleks-netizen.github.io/product-images/L22661-1/573.jpg,https://oleks-netizen.github.io/product-images/L22661-1/576.jpg,https://oleks-netizen.github.io/product-images/L22661-1/577.jpg,https://oleks-netizen.github.io/product-images/L22661-1/578.jpg,https://oleks-netizen.github.io/product-images/L22661-1/579.jpg</t>
         </is>
       </c>
       <c r="C147" t="n">
@@ -2636,7 +2636,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22808-1/145.jpg,https://oleks-netizen.github.io/product-images/L22808-1/147.jpg,https://oleks-netizen.github.io/product-images/L22808-1/148.jpg,https://oleks-netizen.github.io/product-images/L22808-1/149.jpg,https://oleks-netizen.github.io/product-images/L22808-1/150.jpg,https://oleks-netizen.github.io/product-images/L22808-1/151.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22808-1/145.jpg,https://oleks-netizen.github.io/product-images/L22808-1/148.jpg,https://oleks-netizen.github.io/product-images/L22808-1/149.jpg,https://oleks-netizen.github.io/product-images/L22808-1/150.jpg,https://oleks-netizen.github.io/product-images/L22808-1/151.jpg,https://oleks-netizen.github.io/product-images/L22808-1/1.jpg</t>
         </is>
       </c>
       <c r="C148" t="n">
@@ -2651,7 +2651,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22808-1W/5535.jpg,https://oleks-netizen.github.io/product-images/L22808-1W/5537.jpg,https://oleks-netizen.github.io/product-images/L22808-1W/5538.jpg,https://oleks-netizen.github.io/product-images/L22808-1W/5539.jpg,https://oleks-netizen.github.io/product-images/L22808-1W/5540.jpg,https://oleks-netizen.github.io/product-images/L22808-1W/5541.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22808-1W/1.jpg,https://oleks-netizen.github.io/product-images/L22808-1W/5535.jpg,https://oleks-netizen.github.io/product-images/L22808-1W/5538.jpg,https://oleks-netizen.github.io/product-images/L22808-1W/5539.jpg,https://oleks-netizen.github.io/product-images/L22808-1W/5540.jpg,https://oleks-netizen.github.io/product-images/L22808-1W/5541.jpg</t>
         </is>
       </c>
       <c r="C149" t="n">
@@ -2666,7 +2666,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22813-04S/1952.jpg,https://oleks-netizen.github.io/product-images/L22813-04S/1954.jpg,https://oleks-netizen.github.io/product-images/L22813-04S/1955.jpg,https://oleks-netizen.github.io/product-images/L22813-04S/1956.jpg,https://oleks-netizen.github.io/product-images/L22813-04S/1957.jpg,https://oleks-netizen.github.io/product-images/L22813-04S/1958.jpg,https://oleks-netizen.github.io/product-images/L22813-04S/1959.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22813-04S/1952.jpg,https://oleks-netizen.github.io/product-images/L22813-04S/1955.jpg,https://oleks-netizen.github.io/product-images/L22813-04S/1956.jpg,https://oleks-netizen.github.io/product-images/L22813-04S/1957.jpg,https://oleks-netizen.github.io/product-images/L22813-04S/1958.jpg,https://oleks-netizen.github.io/product-images/L22813-04S/1959.jpg,https://oleks-netizen.github.io/product-images/L22813-04S/1.jpg</t>
         </is>
       </c>
       <c r="C150" t="n">
@@ -2681,7 +2681,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22813-05S/2519.jpg,https://oleks-netizen.github.io/product-images/L22813-05S/2521.jpg,https://oleks-netizen.github.io/product-images/L22813-05S/2522.jpg,https://oleks-netizen.github.io/product-images/L22813-05S/2523.jpg,https://oleks-netizen.github.io/product-images/L22813-05S/2524.jpg,https://oleks-netizen.github.io/product-images/L22813-05S/2525.jpg,https://oleks-netizen.github.io/product-images/L22813-05S/2526.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22813-05S/1.jpg,https://oleks-netizen.github.io/product-images/L22813-05S/2519.jpg,https://oleks-netizen.github.io/product-images/L22813-05S/2522.jpg,https://oleks-netizen.github.io/product-images/L22813-05S/2523.jpg,https://oleks-netizen.github.io/product-images/L22813-05S/2524.jpg,https://oleks-netizen.github.io/product-images/L22813-05S/2525.jpg,https://oleks-netizen.github.io/product-images/L22813-05S/2526.jpg</t>
         </is>
       </c>
       <c r="C151" t="n">
@@ -2696,7 +2696,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22902-1C/5543.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/5545.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/5546.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/5547.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/5548.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/5549.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/5550.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/5551.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/5552.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22902-1C/1.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/5543.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/5546.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/5547.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/5548.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/5549.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/5550.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/5551.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/5552.jpg</t>
         </is>
       </c>
       <c r="C152" t="n">
@@ -2711,7 +2711,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22916-5W/5707.jpg,https://oleks-netizen.github.io/product-images/L22916-5W/5710.jpg,https://oleks-netizen.github.io/product-images/L22916-5W/5711.jpg,https://oleks-netizen.github.io/product-images/L22916-5W/5712.jpg,https://oleks-netizen.github.io/product-images/L22916-5W/5713.jpg,https://oleks-netizen.github.io/product-images/L22916-5W/5714.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22916-5W/1.jpg,https://oleks-netizen.github.io/product-images/L22916-5W/5707.jpg,https://oleks-netizen.github.io/product-images/L22916-5W/5711.jpg,https://oleks-netizen.github.io/product-images/L22916-5W/5712.jpg,https://oleks-netizen.github.io/product-images/L22916-5W/5713.jpg,https://oleks-netizen.github.io/product-images/L22916-5W/5714.jpg</t>
         </is>
       </c>
       <c r="C153" t="n">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L26003-1/5192.jpg,https://oleks-netizen.github.io/product-images/L26003-1/5194.jpg,https://oleks-netizen.github.io/product-images/L26003-1/5195.jpg,https://oleks-netizen.github.io/product-images/L26003-1/5196.jpg,https://oleks-netizen.github.io/product-images/L26003-1/5197.jpg,https://oleks-netizen.github.io/product-images/L26003-1/5198.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L26003-1/1.jpg,https://oleks-netizen.github.io/product-images/L26003-1/5192.jpg,https://oleks-netizen.github.io/product-images/L26003-1/5195.jpg,https://oleks-netizen.github.io/product-images/L26003-1/5196.jpg,https://oleks-netizen.github.io/product-images/L26003-1/5197.jpg,https://oleks-netizen.github.io/product-images/L26003-1/5198.jpg</t>
         </is>
       </c>
       <c r="C154" t="n">
@@ -2741,7 +2741,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L26018-1/4039.jpg,https://oleks-netizen.github.io/product-images/L26018-1/4041.jpg,https://oleks-netizen.github.io/product-images/L26018-1/4042.jpg,https://oleks-netizen.github.io/product-images/L26018-1/4043.jpg,https://oleks-netizen.github.io/product-images/L26018-1/4044.jpg,https://oleks-netizen.github.io/product-images/L26018-1/4045.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L26018-1/1.jpg,https://oleks-netizen.github.io/product-images/L26018-1/4039.jpg,https://oleks-netizen.github.io/product-images/L26018-1/4042.jpg,https://oleks-netizen.github.io/product-images/L26018-1/4043.jpg,https://oleks-netizen.github.io/product-images/L26018-1/4044.jpg,https://oleks-netizen.github.io/product-images/L26018-1/4045.jpg</t>
         </is>
       </c>
       <c r="C155" t="n">
@@ -2756,7 +2756,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L26290-005/5655.jpg,https://oleks-netizen.github.io/product-images/L26290-005/5657.jpg,https://oleks-netizen.github.io/product-images/L26290-005/5658.jpg,https://oleks-netizen.github.io/product-images/L26290-005/5659.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L26290-005/1.jpg,https://oleks-netizen.github.io/product-images/L26290-005/5655.jpg,https://oleks-netizen.github.io/product-images/L26290-005/5658.jpg,https://oleks-netizen.github.io/product-images/L26290-005/5659.jpg</t>
         </is>
       </c>
       <c r="C156" t="n">
@@ -2771,7 +2771,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L26309-005/4804.jpg,https://oleks-netizen.github.io/product-images/L26309-005/4806.jpg,https://oleks-netizen.github.io/product-images/L26309-005/4807.jpg,https://oleks-netizen.github.io/product-images/L26309-005/4808.jpg,https://oleks-netizen.github.io/product-images/L26309-005/4809.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L26309-005/1.jpg,https://oleks-netizen.github.io/product-images/L26309-005/4804.jpg,https://oleks-netizen.github.io/product-images/L26309-005/4807.jpg,https://oleks-netizen.github.io/product-images/L26309-005/4808.jpg,https://oleks-netizen.github.io/product-images/L26309-005/4809.jpg</t>
         </is>
       </c>
       <c r="C157" t="n">
@@ -2786,7 +2786,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L26321-1/4175.jpg,https://oleks-netizen.github.io/product-images/L26321-1/4177.jpg,https://oleks-netizen.github.io/product-images/L26321-1/4178.jpg,https://oleks-netizen.github.io/product-images/L26321-1/4179.jpg,https://oleks-netizen.github.io/product-images/L26321-1/4180.jpg,https://oleks-netizen.github.io/product-images/L26321-1/4181.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L26321-1/1.jpg,https://oleks-netizen.github.io/product-images/L26321-1/4175.jpg,https://oleks-netizen.github.io/product-images/L26321-1/4178.jpg,https://oleks-netizen.github.io/product-images/L26321-1/4179.jpg,https://oleks-netizen.github.io/product-images/L26321-1/4180.jpg,https://oleks-netizen.github.io/product-images/L26321-1/4181.jpg</t>
         </is>
       </c>
       <c r="C158" t="n">
@@ -2801,7 +2801,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L9902-3C/930.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/931.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/932.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/933.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/934.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/935.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/936.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/937.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/938.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/939.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/940.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L9902-3C/1.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/930.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/931.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/933.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/934.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/935.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/936.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/937.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/938.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/939.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/940.jpg</t>
         </is>
       </c>
       <c r="C159" t="n">

</xml_diff>

<commit_message>
Auto update 2025-11-27 12:07:59
</commit_message>
<xml_diff>
--- a/articles_summary.xlsx
+++ b/articles_summary.xlsx
@@ -446,7 +446,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/0026-2/1.jpg,https://oleks-netizen.github.io/product-images/0026-2/2.jpg,https://oleks-netizen.github.io/product-images/0026-2/4.jpg,https://oleks-netizen.github.io/product-images/0026-2/5.jpg,https://oleks-netizen.github.io/product-images/0026-2/6.jpg,https://oleks-netizen.github.io/product-images/0026-2/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/0026-2/1.jpg,https://oleks-netizen.github.io/product-images/0026-2/2.jpg,https://oleks-netizen.github.io/product-images/0026-2/3.jpg,https://oleks-netizen.github.io/product-images/0026-2/5.jpg,https://oleks-netizen.github.io/product-images/0026-2/6.jpg,https://oleks-netizen.github.io/product-images/0026-2/7.jpg</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -461,7 +461,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/0026-3/1.jpg,https://oleks-netizen.github.io/product-images/0026-3/2.jpg,https://oleks-netizen.github.io/product-images/0026-3/4.jpg,https://oleks-netizen.github.io/product-images/0026-3/5.jpg,https://oleks-netizen.github.io/product-images/0026-3/6.jpg,https://oleks-netizen.github.io/product-images/0026-3/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/0026-3/1.jpg,https://oleks-netizen.github.io/product-images/0026-3/2.jpg,https://oleks-netizen.github.io/product-images/0026-3/3.jpg,https://oleks-netizen.github.io/product-images/0026-3/5.jpg,https://oleks-netizen.github.io/product-images/0026-3/6.jpg,https://oleks-netizen.github.io/product-images/0026-3/7.jpg</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -476,7 +476,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/0026-4/1.jpg,https://oleks-netizen.github.io/product-images/0026-4/2.jpg,https://oleks-netizen.github.io/product-images/0026-4/4.jpg,https://oleks-netizen.github.io/product-images/0026-4/5.jpg,https://oleks-netizen.github.io/product-images/0026-4/6.jpg,https://oleks-netizen.github.io/product-images/0026-4/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/0026-4/1.jpg,https://oleks-netizen.github.io/product-images/0026-4/2.jpg,https://oleks-netizen.github.io/product-images/0026-4/3.jpg,https://oleks-netizen.github.io/product-images/0026-4/5.jpg,https://oleks-netizen.github.io/product-images/0026-4/6.jpg,https://oleks-netizen.github.io/product-images/0026-4/7.jpg</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -491,7 +491,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/0026-5/1.jpg,https://oleks-netizen.github.io/product-images/0026-5/2.jpg,https://oleks-netizen.github.io/product-images/0026-5/4.jpg,https://oleks-netizen.github.io/product-images/0026-5/5.jpg,https://oleks-netizen.github.io/product-images/0026-5/6.jpg,https://oleks-netizen.github.io/product-images/0026-5/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/0026-5/1.jpg,https://oleks-netizen.github.io/product-images/0026-5/2.jpg,https://oleks-netizen.github.io/product-images/0026-5/3.jpg,https://oleks-netizen.github.io/product-images/0026-5/5.jpg,https://oleks-netizen.github.io/product-images/0026-5/6.jpg,https://oleks-netizen.github.io/product-images/0026-5/7.jpg</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -506,7 +506,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/0026-6/1.jpg,https://oleks-netizen.github.io/product-images/0026-6/2.jpg,https://oleks-netizen.github.io/product-images/0026-6/4.jpg,https://oleks-netizen.github.io/product-images/0026-6/5.jpg,https://oleks-netizen.github.io/product-images/0026-6/6.jpg,https://oleks-netizen.github.io/product-images/0026-6/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/0026-6/1.jpg,https://oleks-netizen.github.io/product-images/0026-6/2.jpg,https://oleks-netizen.github.io/product-images/0026-6/3.jpg,https://oleks-netizen.github.io/product-images/0026-6/5.jpg,https://oleks-netizen.github.io/product-images/0026-6/6.jpg,https://oleks-netizen.github.io/product-images/0026-6/7.jpg</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -521,7 +521,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/0026-7/1.jpg,https://oleks-netizen.github.io/product-images/0026-7/2.jpg,https://oleks-netizen.github.io/product-images/0026-7/4.jpg,https://oleks-netizen.github.io/product-images/0026-7/5.jpg,https://oleks-netizen.github.io/product-images/0026-7/6.jpg,https://oleks-netizen.github.io/product-images/0026-7/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/0026-7/1.jpg,https://oleks-netizen.github.io/product-images/0026-7/2.jpg,https://oleks-netizen.github.io/product-images/0026-7/3.jpg,https://oleks-netizen.github.io/product-images/0026-7/5.jpg,https://oleks-netizen.github.io/product-images/0026-7/6.jpg,https://oleks-netizen.github.io/product-images/0026-7/7.jpg</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -536,7 +536,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/0039-3/1.jpg,https://oleks-netizen.github.io/product-images/0039-3/2.jpg,https://oleks-netizen.github.io/product-images/0039-3/4.jpg,https://oleks-netizen.github.io/product-images/0039-3/5.jpg,https://oleks-netizen.github.io/product-images/0039-3/6.jpg,https://oleks-netizen.github.io/product-images/0039-3/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/0039-3/1.jpg,https://oleks-netizen.github.io/product-images/0039-3/3.jpg,https://oleks-netizen.github.io/product-images/0039-3/4.jpg,https://oleks-netizen.github.io/product-images/0039-3/5.jpg,https://oleks-netizen.github.io/product-images/0039-3/6.jpg,https://oleks-netizen.github.io/product-images/0039-3/7.jpg</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -551,7 +551,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/005/1.jpg,https://oleks-netizen.github.io/product-images/005/2.jpg,https://oleks-netizen.github.io/product-images/005/4.jpg,https://oleks-netizen.github.io/product-images/005/5.jpg,https://oleks-netizen.github.io/product-images/005/6.jpg,https://oleks-netizen.github.io/product-images/005/7.jpg,https://oleks-netizen.github.io/product-images/005/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/005/1.jpg,https://oleks-netizen.github.io/product-images/005/3.jpg,https://oleks-netizen.github.io/product-images/005/4.jpg,https://oleks-netizen.github.io/product-images/005/5.jpg,https://oleks-netizen.github.io/product-images/005/6.jpg,https://oleks-netizen.github.io/product-images/005/7.jpg,https://oleks-netizen.github.io/product-images/005/8.jpg</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -566,7 +566,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/009-2/1.jpg,https://oleks-netizen.github.io/product-images/009-2/2.jpg,https://oleks-netizen.github.io/product-images/009-2/4.jpg,https://oleks-netizen.github.io/product-images/009-2/5.jpg,https://oleks-netizen.github.io/product-images/009-2/6.jpg,https://oleks-netizen.github.io/product-images/009-2/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/009-2/1.jpg,https://oleks-netizen.github.io/product-images/009-2/2.jpg,https://oleks-netizen.github.io/product-images/009-2/3.jpg,https://oleks-netizen.github.io/product-images/009-2/5.jpg,https://oleks-netizen.github.io/product-images/009-2/6.jpg,https://oleks-netizen.github.io/product-images/009-2/7.jpg</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -581,7 +581,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/009-4/1.jpg,https://oleks-netizen.github.io/product-images/009-4/2.jpg,https://oleks-netizen.github.io/product-images/009-4/4.jpg,https://oleks-netizen.github.io/product-images/009-4/5.jpg,https://oleks-netizen.github.io/product-images/009-4/6.jpg,https://oleks-netizen.github.io/product-images/009-4/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/009-4/1.jpg,https://oleks-netizen.github.io/product-images/009-4/3.jpg,https://oleks-netizen.github.io/product-images/009-4/4.jpg,https://oleks-netizen.github.io/product-images/009-4/5.jpg,https://oleks-netizen.github.io/product-images/009-4/6.jpg,https://oleks-netizen.github.io/product-images/009-4/7.jpg</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -596,7 +596,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/1203A Сіра/1.jpg,https://oleks-netizen.github.io/product-images/1203A Сіра/3.jpg,https://oleks-netizen.github.io/product-images/1203A Сіра/4.jpg,https://oleks-netizen.github.io/product-images/1203A Сіра/5.jpg,https://oleks-netizen.github.io/product-images/1203A Сіра/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/1203A Сіра/1.jpg,https://oleks-netizen.github.io/product-images/1203A Сіра/6.jpg,https://oleks-netizen.github.io/product-images/1203A Сіра/3.jpg,https://oleks-netizen.github.io/product-images/1203A Сіра/4.jpg,https://oleks-netizen.github.io/product-images/1203A Сіра/5.jpg</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -611,7 +611,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/1203A Синя/1.jpg,https://oleks-netizen.github.io/product-images/1203A Синя/3.jpg,https://oleks-netizen.github.io/product-images/1203A Синя/4.jpg,https://oleks-netizen.github.io/product-images/1203A Синя/5.jpg,https://oleks-netizen.github.io/product-images/1203A Синя/6.jpg,https://oleks-netizen.github.io/product-images/1203A Синя/7.jpg,https://oleks-netizen.github.io/product-images/1203A Синя/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/1203A Синя/1.jpg,https://oleks-netizen.github.io/product-images/1203A Синя/3.jpg,https://oleks-netizen.github.io/product-images/1203A Синя/8.jpg,https://oleks-netizen.github.io/product-images/1203A Синя/4.jpg,https://oleks-netizen.github.io/product-images/1203A Синя/5.jpg,https://oleks-netizen.github.io/product-images/1203A Синя/6.jpg,https://oleks-netizen.github.io/product-images/1203A Синя/7.jpg</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -626,7 +626,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/1203A Чорна/1.jpg,https://oleks-netizen.github.io/product-images/1203A Чорна/3.jpg,https://oleks-netizen.github.io/product-images/1203A Чорна/4.jpg,https://oleks-netizen.github.io/product-images/1203A Чорна/5.jpg,https://oleks-netizen.github.io/product-images/1203A Чорна/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/1203A Чорна/1.jpg,https://oleks-netizen.github.io/product-images/1203A Чорна/2.jpg,https://oleks-netizen.github.io/product-images/1203A Чорна/3.jpg,https://oleks-netizen.github.io/product-images/1203A Чорна/4.jpg,https://oleks-netizen.github.io/product-images/1203A Чорна/5.jpg</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -641,7 +641,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/1204/10.jpg,https://oleks-netizen.github.io/product-images/1204/11.jpg,https://oleks-netizen.github.io/product-images/1204/12.jpg,https://oleks-netizen.github.io/product-images/1204/1.jpg,https://oleks-netizen.github.io/product-images/1204/3.jpg,https://oleks-netizen.github.io/product-images/1204/4.jpg,https://oleks-netizen.github.io/product-images/1204/5.jpg,https://oleks-netizen.github.io/product-images/1204/6.jpg,https://oleks-netizen.github.io/product-images/1204/7.jpg,https://oleks-netizen.github.io/product-images/1204/8.jpg,https://oleks-netizen.github.io/product-images/1204/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/1204/1.jpg,https://oleks-netizen.github.io/product-images/1204/2.jpg,https://oleks-netizen.github.io/product-images/1204/10.jpg,https://oleks-netizen.github.io/product-images/1204/11.jpg,https://oleks-netizen.github.io/product-images/1204/3.jpg,https://oleks-netizen.github.io/product-images/1204/4.jpg,https://oleks-netizen.github.io/product-images/1204/5.jpg,https://oleks-netizen.github.io/product-images/1204/6.jpg,https://oleks-netizen.github.io/product-images/1204/7.jpg,https://oleks-netizen.github.io/product-images/1204/8.jpg,https://oleks-netizen.github.io/product-images/1204/9.jpg</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -686,7 +686,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3114/1.jpg,https://oleks-netizen.github.io/product-images/3114/2.jpg,https://oleks-netizen.github.io/product-images/3114/4.jpg,https://oleks-netizen.github.io/product-images/3114/5.jpg,https://oleks-netizen.github.io/product-images/3114/6.jpg,https://oleks-netizen.github.io/product-images/3114/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/3114/1.jpg,https://oleks-netizen.github.io/product-images/3114/2.jpg,https://oleks-netizen.github.io/product-images/3114/3.jpg,https://oleks-netizen.github.io/product-images/3114/4.jpg,https://oleks-netizen.github.io/product-images/3114/5.jpg,https://oleks-netizen.github.io/product-images/3114/6.jpg</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -746,7 +746,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3131/1.jpg,https://oleks-netizen.github.io/product-images/3131/2.jpg,https://oleks-netizen.github.io/product-images/3131/4.jpg,https://oleks-netizen.github.io/product-images/3131/5.jpg,https://oleks-netizen.github.io/product-images/3131/6.jpg,https://oleks-netizen.github.io/product-images/3131/7.jpg,https://oleks-netizen.github.io/product-images/3131/8.jpg,https://oleks-netizen.github.io/product-images/3131/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/3131/1.jpg,https://oleks-netizen.github.io/product-images/3131/2.jpg,https://oleks-netizen.github.io/product-images/3131/3.jpg,https://oleks-netizen.github.io/product-images/3131/4.jpg,https://oleks-netizen.github.io/product-images/3131/5.jpg,https://oleks-netizen.github.io/product-images/3131/6.jpg,https://oleks-netizen.github.io/product-images/3131/7.jpg,https://oleks-netizen.github.io/product-images/3131/8.jpg</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -806,7 +806,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3135/1.jpg,https://oleks-netizen.github.io/product-images/3135/3.jpg,https://oleks-netizen.github.io/product-images/3135/4.jpg,https://oleks-netizen.github.io/product-images/3135/5.jpg,https://oleks-netizen.github.io/product-images/3135/6.jpg,https://oleks-netizen.github.io/product-images/3135/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/3135/1.jpg,https://oleks-netizen.github.io/product-images/3135/2.jpg,https://oleks-netizen.github.io/product-images/3135/3.jpg,https://oleks-netizen.github.io/product-images/3135/4.jpg,https://oleks-netizen.github.io/product-images/3135/5.jpg,https://oleks-netizen.github.io/product-images/3135/6.jpg</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -851,7 +851,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3141 Коралова/1.jpg,https://oleks-netizen.github.io/product-images/3141 Коралова/2.jpg,https://oleks-netizen.github.io/product-images/3141 Коралова/3.jpg,https://oleks-netizen.github.io/product-images/3141 Коралова/4.jpg,https://oleks-netizen.github.io/product-images/3141 Коралова/5.jpg,https://oleks-netizen.github.io/product-images/3141 Коралова/6.jpg,https://oleks-netizen.github.io/product-images/3141 Коралова/7.jpg,https://oleks-netizen.github.io/product-images/3141 Коралова/8.jpg,https://oleks-netizen.github.io/product-images/3141 Коралова/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/3141 Коралова/1.jpg,https://oleks-netizen.github.io/product-images/3141 Коралова/2.jpg,https://oleks-netizen.github.io/product-images/3141 Коралова/10.jpg,https://oleks-netizen.github.io/product-images/3141 Коралова/4.jpg,https://oleks-netizen.github.io/product-images/3141 Коралова/5.jpg,https://oleks-netizen.github.io/product-images/3141 Коралова/6.jpg,https://oleks-netizen.github.io/product-images/3141 Коралова/7.jpg,https://oleks-netizen.github.io/product-images/3141 Коралова/8.jpg,https://oleks-netizen.github.io/product-images/3141 Коралова/9.jpg</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -866,7 +866,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3141 Рожева/1.jpg,https://oleks-netizen.github.io/product-images/3141 Рожева/2.jpg,https://oleks-netizen.github.io/product-images/3141 Рожева/3.jpg,https://oleks-netizen.github.io/product-images/3141 Рожева/4.jpg,https://oleks-netizen.github.io/product-images/3141 Рожева/5.jpg,https://oleks-netizen.github.io/product-images/3141 Рожева/6.jpg,https://oleks-netizen.github.io/product-images/3141 Рожева/7.jpg,https://oleks-netizen.github.io/product-images/3141 Рожева/8.jpg,https://oleks-netizen.github.io/product-images/3141 Рожева/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/3141 Рожева/1.jpg,https://oleks-netizen.github.io/product-images/3141 Рожева/2.jpg,https://oleks-netizen.github.io/product-images/3141 Рожева/10.jpg,https://oleks-netizen.github.io/product-images/3141 Рожева/4.jpg,https://oleks-netizen.github.io/product-images/3141 Рожева/5.jpg,https://oleks-netizen.github.io/product-images/3141 Рожева/6.jpg,https://oleks-netizen.github.io/product-images/3141 Рожева/7.jpg,https://oleks-netizen.github.io/product-images/3141 Рожева/8.jpg,https://oleks-netizen.github.io/product-images/3141 Рожева/9.jpg</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -881,7 +881,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3142-2/10.jpg,https://oleks-netizen.github.io/product-images/3142-2/1.jpg,https://oleks-netizen.github.io/product-images/3142-2/2.jpg,https://oleks-netizen.github.io/product-images/3142-2/3.jpg,https://oleks-netizen.github.io/product-images/3142-2/4.jpg,https://oleks-netizen.github.io/product-images/3142-2/5.jpg,https://oleks-netizen.github.io/product-images/3142-2/6.jpg,https://oleks-netizen.github.io/product-images/3142-2/7.jpg,https://oleks-netizen.github.io/product-images/3142-2/8.jpg,https://oleks-netizen.github.io/product-images/3142-2/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/3142-2/1.jpg,https://oleks-netizen.github.io/product-images/3142-2/2.jpg,https://oleks-netizen.github.io/product-images/3142-2/11.jpg,https://oleks-netizen.github.io/product-images/3142-2/3.jpg,https://oleks-netizen.github.io/product-images/3142-2/4.jpg,https://oleks-netizen.github.io/product-images/3142-2/5.jpg,https://oleks-netizen.github.io/product-images/3142-2/6.jpg,https://oleks-netizen.github.io/product-images/3142-2/7.jpg,https://oleks-netizen.github.io/product-images/3142-2/8.jpg,https://oleks-netizen.github.io/product-images/3142-2/9.jpg</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -896,7 +896,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3145 Hello, Paris/10.jpg,https://oleks-netizen.github.io/product-images/3145 Hello, Paris/1.jpg,https://oleks-netizen.github.io/product-images/3145 Hello, Paris/2.jpg,https://oleks-netizen.github.io/product-images/3145 Hello, Paris/3.jpg,https://oleks-netizen.github.io/product-images/3145 Hello, Paris/4.jpg,https://oleks-netizen.github.io/product-images/3145 Hello, Paris/5.jpg,https://oleks-netizen.github.io/product-images/3145 Hello, Paris/6.jpg,https://oleks-netizen.github.io/product-images/3145 Hello, Paris/7.jpg,https://oleks-netizen.github.io/product-images/3145 Hello, Paris/8.jpg,https://oleks-netizen.github.io/product-images/3145 Hello, Paris/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/3145 Hello, Paris/1.jpg,https://oleks-netizen.github.io/product-images/3145 Hello, Paris/2.jpg,https://oleks-netizen.github.io/product-images/3145 Hello, Paris/10.jpg,https://oleks-netizen.github.io/product-images/3145 Hello, Paris/3.jpg,https://oleks-netizen.github.io/product-images/3145 Hello, Paris/4.jpg,https://oleks-netizen.github.io/product-images/3145 Hello, Paris/5.jpg,https://oleks-netizen.github.io/product-images/3145 Hello, Paris/6.jpg,https://oleks-netizen.github.io/product-images/3145 Hello, Paris/7.jpg,https://oleks-netizen.github.io/product-images/3145 Hello, Paris/8.jpg,https://oleks-netizen.github.io/product-images/3145 Hello, Paris/9.jpg</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -911,7 +911,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3145-1/10.jpg,https://oleks-netizen.github.io/product-images/3145-1/1.jpg,https://oleks-netizen.github.io/product-images/3145-1/2.jpg,https://oleks-netizen.github.io/product-images/3145-1/3.jpg,https://oleks-netizen.github.io/product-images/3145-1/4.jpg,https://oleks-netizen.github.io/product-images/3145-1/5.jpg,https://oleks-netizen.github.io/product-images/3145-1/6.jpg,https://oleks-netizen.github.io/product-images/3145-1/7.jpg,https://oleks-netizen.github.io/product-images/3145-1/8.jpg,https://oleks-netizen.github.io/product-images/3145-1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/3145-1/1.jpg,https://oleks-netizen.github.io/product-images/3145-1/2.jpg,https://oleks-netizen.github.io/product-images/3145-1/10.jpg,https://oleks-netizen.github.io/product-images/3145-1/3.jpg,https://oleks-netizen.github.io/product-images/3145-1/4.jpg,https://oleks-netizen.github.io/product-images/3145-1/5.jpg,https://oleks-netizen.github.io/product-images/3145-1/6.jpg,https://oleks-netizen.github.io/product-images/3145-1/7.jpg,https://oleks-netizen.github.io/product-images/3145-1/8.jpg,https://oleks-netizen.github.io/product-images/3145-1/9.jpg</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -926,7 +926,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3145-2/10.jpg,https://oleks-netizen.github.io/product-images/3145-2/1.jpg,https://oleks-netizen.github.io/product-images/3145-2/2.jpg,https://oleks-netizen.github.io/product-images/3145-2/3.jpg,https://oleks-netizen.github.io/product-images/3145-2/4.jpg,https://oleks-netizen.github.io/product-images/3145-2/5.jpg,https://oleks-netizen.github.io/product-images/3145-2/6.jpg,https://oleks-netizen.github.io/product-images/3145-2/7.jpg,https://oleks-netizen.github.io/product-images/3145-2/8.jpg,https://oleks-netizen.github.io/product-images/3145-2/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/3145-2/1.jpg,https://oleks-netizen.github.io/product-images/3145-2/2.jpg,https://oleks-netizen.github.io/product-images/3145-2/10.jpg,https://oleks-netizen.github.io/product-images/3145-2/3.jpg,https://oleks-netizen.github.io/product-images/3145-2/4.jpg,https://oleks-netizen.github.io/product-images/3145-2/5.jpg,https://oleks-netizen.github.io/product-images/3145-2/6.jpg,https://oleks-netizen.github.io/product-images/3145-2/7.jpg,https://oleks-netizen.github.io/product-images/3145-2/8.jpg,https://oleks-netizen.github.io/product-images/3145-2/9.jpg</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -941,7 +941,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3146/10.jpg,https://oleks-netizen.github.io/product-images/3146/1.jpg,https://oleks-netizen.github.io/product-images/3146/2.jpg,https://oleks-netizen.github.io/product-images/3146/4.jpg,https://oleks-netizen.github.io/product-images/3146/5.jpg,https://oleks-netizen.github.io/product-images/3146/6.jpg,https://oleks-netizen.github.io/product-images/3146/7.jpg,https://oleks-netizen.github.io/product-images/3146/8.jpg,https://oleks-netizen.github.io/product-images/3146/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/3146/1.jpg,https://oleks-netizen.github.io/product-images/3146/10.jpg,https://oleks-netizen.github.io/product-images/3146/2.jpg,https://oleks-netizen.github.io/product-images/3146/4.jpg,https://oleks-netizen.github.io/product-images/3146/5.jpg,https://oleks-netizen.github.io/product-images/3146/6.jpg,https://oleks-netizen.github.io/product-images/3146/7.jpg,https://oleks-netizen.github.io/product-images/3146/8.jpg,https://oleks-netizen.github.io/product-images/3146/9.jpg</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -971,7 +971,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3219 Квіти/10.jpg,https://oleks-netizen.github.io/product-images/3219 Квіти/1.jpg,https://oleks-netizen.github.io/product-images/3219 Квіти/2.jpg,https://oleks-netizen.github.io/product-images/3219 Квіти/3.jpg,https://oleks-netizen.github.io/product-images/3219 Квіти/4.jpg,https://oleks-netizen.github.io/product-images/3219 Квіти/5.jpg,https://oleks-netizen.github.io/product-images/3219 Квіти/6.jpg,https://oleks-netizen.github.io/product-images/3219 Квіти/7.jpg,https://oleks-netizen.github.io/product-images/3219 Квіти/8.jpg,https://oleks-netizen.github.io/product-images/3219 Квіти/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/3219 Квіти/1.jpg,https://oleks-netizen.github.io/product-images/3219 Квіти/2.jpg,https://oleks-netizen.github.io/product-images/3219 Квіти/10.jpg,https://oleks-netizen.github.io/product-images/3219 Квіти/3.jpg,https://oleks-netizen.github.io/product-images/3219 Квіти/4.jpg,https://oleks-netizen.github.io/product-images/3219 Квіти/5.jpg,https://oleks-netizen.github.io/product-images/3219 Квіти/6.jpg,https://oleks-netizen.github.io/product-images/3219 Квіти/7.jpg,https://oleks-netizen.github.io/product-images/3219 Квіти/8.jpg,https://oleks-netizen.github.io/product-images/3219 Квіти/9.jpg</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -986,7 +986,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3220 Синя/10.jpg,https://oleks-netizen.github.io/product-images/3220 Синя/1.jpg,https://oleks-netizen.github.io/product-images/3220 Синя/2.jpg,https://oleks-netizen.github.io/product-images/3220 Синя/3.jpg,https://oleks-netizen.github.io/product-images/3220 Синя/4.jpg,https://oleks-netizen.github.io/product-images/3220 Синя/5.jpg,https://oleks-netizen.github.io/product-images/3220 Синя/6.jpg,https://oleks-netizen.github.io/product-images/3220 Синя/7.jpg,https://oleks-netizen.github.io/product-images/3220 Синя/8.jpg,https://oleks-netizen.github.io/product-images/3220 Синя/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/3220 Синя/1.jpg,https://oleks-netizen.github.io/product-images/3220 Синя/2.jpg,https://oleks-netizen.github.io/product-images/3220 Синя/10.jpg,https://oleks-netizen.github.io/product-images/3220 Синя/3.jpg,https://oleks-netizen.github.io/product-images/3220 Синя/4.jpg,https://oleks-netizen.github.io/product-images/3220 Синя/5.jpg,https://oleks-netizen.github.io/product-images/3220 Синя/6.jpg,https://oleks-netizen.github.io/product-images/3220 Синя/7.jpg,https://oleks-netizen.github.io/product-images/3220 Синя/8.jpg,https://oleks-netizen.github.io/product-images/3220 Синя/9.jpg</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3220 Червона/10.jpg,https://oleks-netizen.github.io/product-images/3220 Червона/11.jpg,https://oleks-netizen.github.io/product-images/3220 Червона/1.jpg,https://oleks-netizen.github.io/product-images/3220 Червона/2.jpg,https://oleks-netizen.github.io/product-images/3220 Червона/3.jpg,https://oleks-netizen.github.io/product-images/3220 Червона/4.jpg,https://oleks-netizen.github.io/product-images/3220 Червона/5.jpg,https://oleks-netizen.github.io/product-images/3220 Червона/6.jpg,https://oleks-netizen.github.io/product-images/3220 Червона/7.jpg,https://oleks-netizen.github.io/product-images/3220 Червона/8.jpg,https://oleks-netizen.github.io/product-images/3220 Червона/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/3220 Червона/1.jpg,https://oleks-netizen.github.io/product-images/3220 Червона/2.jpg,https://oleks-netizen.github.io/product-images/3220 Червона/10.jpg,https://oleks-netizen.github.io/product-images/3220 Червона/11.jpg,https://oleks-netizen.github.io/product-images/3220 Червона/3.jpg,https://oleks-netizen.github.io/product-images/3220 Червона/4.jpg,https://oleks-netizen.github.io/product-images/3220 Червона/5.jpg,https://oleks-netizen.github.io/product-images/3220 Червона/6.jpg,https://oleks-netizen.github.io/product-images/3220 Червона/7.jpg,https://oleks-netizen.github.io/product-images/3220 Червона/8.jpg,https://oleks-netizen.github.io/product-images/3220 Червона/9.jpg</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -1076,7 +1076,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3224/10.jpg,https://oleks-netizen.github.io/product-images/3224/1.jpg,https://oleks-netizen.github.io/product-images/3224/2.jpg,https://oleks-netizen.github.io/product-images/3224/4.jpg,https://oleks-netizen.github.io/product-images/3224/5.jpg,https://oleks-netizen.github.io/product-images/3224/6.jpg,https://oleks-netizen.github.io/product-images/3224/7.jpg,https://oleks-netizen.github.io/product-images/3224/8.jpg,https://oleks-netizen.github.io/product-images/3224/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/3224/1.jpg,https://oleks-netizen.github.io/product-images/3224/2.jpg,https://oleks-netizen.github.io/product-images/3224/3.jpg,https://oleks-netizen.github.io/product-images/3224/4.jpg,https://oleks-netizen.github.io/product-images/3224/5.jpg,https://oleks-netizen.github.io/product-images/3224/6.jpg,https://oleks-netizen.github.io/product-images/3224/7.jpg,https://oleks-netizen.github.io/product-images/3224/8.jpg,https://oleks-netizen.github.io/product-images/3224/9.jpg</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3307/10.jpg,https://oleks-netizen.github.io/product-images/3307/11.jpg,https://oleks-netizen.github.io/product-images/3307/1.jpg,https://oleks-netizen.github.io/product-images/3307/2.jpg,https://oleks-netizen.github.io/product-images/3307/4.jpg,https://oleks-netizen.github.io/product-images/3307/5.jpg,https://oleks-netizen.github.io/product-images/3307/6.jpg,https://oleks-netizen.github.io/product-images/3307/7.jpg,https://oleks-netizen.github.io/product-images/3307/8.jpg,https://oleks-netizen.github.io/product-images/3307/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/3307/1.jpg,https://oleks-netizen.github.io/product-images/3307/2.jpg,https://oleks-netizen.github.io/product-images/3307/3.jpg,https://oleks-netizen.github.io/product-images/3307/10.jpg,https://oleks-netizen.github.io/product-images/3307/4.jpg,https://oleks-netizen.github.io/product-images/3307/5.jpg,https://oleks-netizen.github.io/product-images/3307/6.jpg,https://oleks-netizen.github.io/product-images/3307/7.jpg,https://oleks-netizen.github.io/product-images/3307/8.jpg,https://oleks-netizen.github.io/product-images/3307/9.jpg</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1286,7 +1286,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/5302 Червона/10.jpg,https://oleks-netizen.github.io/product-images/5302 Червона/1.jpg,https://oleks-netizen.github.io/product-images/5302 Червона/2.jpg,https://oleks-netizen.github.io/product-images/5302 Червона/3.jpg,https://oleks-netizen.github.io/product-images/5302 Червона/4.jpg,https://oleks-netizen.github.io/product-images/5302 Червона/5.jpg,https://oleks-netizen.github.io/product-images/5302 Червона/6.jpg,https://oleks-netizen.github.io/product-images/5302 Червона/7.jpg,https://oleks-netizen.github.io/product-images/5302 Червона/8.jpg,https://oleks-netizen.github.io/product-images/5302 Червона/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/5302 Червона/1.jpg,https://oleks-netizen.github.io/product-images/5302 Червона/2.jpg,https://oleks-netizen.github.io/product-images/5302 Червона/10.jpg,https://oleks-netizen.github.io/product-images/5302 Червона/3.jpg,https://oleks-netizen.github.io/product-images/5302 Червона/4.jpg,https://oleks-netizen.github.io/product-images/5302 Червона/5.jpg,https://oleks-netizen.github.io/product-images/5302 Червона/6.jpg,https://oleks-netizen.github.io/product-images/5302 Червона/7.jpg,https://oleks-netizen.github.io/product-images/5302 Червона/8.jpg,https://oleks-netizen.github.io/product-images/5302 Червона/9.jpg</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -1391,7 +1391,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/6836-black/10.jpg,https://oleks-netizen.github.io/product-images/6836-black/1.jpg,https://oleks-netizen.github.io/product-images/6836-black/2.jpg,https://oleks-netizen.github.io/product-images/6836-black/4.jpg,https://oleks-netizen.github.io/product-images/6836-black/5.jpg,https://oleks-netizen.github.io/product-images/6836-black/6.jpg,https://oleks-netizen.github.io/product-images/6836-black/7.jpg,https://oleks-netizen.github.io/product-images/6836-black/8.jpg,https://oleks-netizen.github.io/product-images/6836-black/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/6836-black/1.jpg,https://oleks-netizen.github.io/product-images/6836-black/2.jpg,https://oleks-netizen.github.io/product-images/6836-black/10.jpg,https://oleks-netizen.github.io/product-images/6836-black/4.jpg,https://oleks-netizen.github.io/product-images/6836-black/5.jpg,https://oleks-netizen.github.io/product-images/6836-black/6.jpg,https://oleks-netizen.github.io/product-images/6836-black/7.jpg,https://oleks-netizen.github.io/product-images/6836-black/8.jpg,https://oleks-netizen.github.io/product-images/6836-black/9.jpg</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -1406,7 +1406,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/7631-black/10.jpg,https://oleks-netizen.github.io/product-images/7631-black/1.jpg,https://oleks-netizen.github.io/product-images/7631-black/2.jpg,https://oleks-netizen.github.io/product-images/7631-black/4.jpg,https://oleks-netizen.github.io/product-images/7631-black/5.jpg,https://oleks-netizen.github.io/product-images/7631-black/6.jpg,https://oleks-netizen.github.io/product-images/7631-black/7.jpg,https://oleks-netizen.github.io/product-images/7631-black/8.jpg,https://oleks-netizen.github.io/product-images/7631-black/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/7631-black/1.jpg,https://oleks-netizen.github.io/product-images/7631-black/2.jpg,https://oleks-netizen.github.io/product-images/7631-black/10.jpg,https://oleks-netizen.github.io/product-images/7631-black/4.jpg,https://oleks-netizen.github.io/product-images/7631-black/5.jpg,https://oleks-netizen.github.io/product-images/7631-black/6.jpg,https://oleks-netizen.github.io/product-images/7631-black/7.jpg,https://oleks-netizen.github.io/product-images/7631-black/8.jpg,https://oleks-netizen.github.io/product-images/7631-black/9.jpg</t>
         </is>
       </c>
       <c r="C66" t="n">
@@ -1421,7 +1421,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/7631-grey/10.jpg,https://oleks-netizen.github.io/product-images/7631-grey/11.jpg,https://oleks-netizen.github.io/product-images/7631-grey/1.jpg,https://oleks-netizen.github.io/product-images/7631-grey/2.jpg,https://oleks-netizen.github.io/product-images/7631-grey/4.jpg,https://oleks-netizen.github.io/product-images/7631-grey/5.jpg,https://oleks-netizen.github.io/product-images/7631-grey/6.jpg,https://oleks-netizen.github.io/product-images/7631-grey/7.jpg,https://oleks-netizen.github.io/product-images/7631-grey/8.jpg,https://oleks-netizen.github.io/product-images/7631-grey/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/7631-grey/1.jpg,https://oleks-netizen.github.io/product-images/7631-grey/2.jpg,https://oleks-netizen.github.io/product-images/7631-grey/10.jpg,https://oleks-netizen.github.io/product-images/7631-grey/11.jpg,https://oleks-netizen.github.io/product-images/7631-grey/4.jpg,https://oleks-netizen.github.io/product-images/7631-grey/5.jpg,https://oleks-netizen.github.io/product-images/7631-grey/6.jpg,https://oleks-netizen.github.io/product-images/7631-grey/7.jpg,https://oleks-netizen.github.io/product-images/7631-grey/8.jpg,https://oleks-netizen.github.io/product-images/7631-grey/9.jpg</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -1436,7 +1436,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/7683-black/10.jpg,https://oleks-netizen.github.io/product-images/7683-black/1.jpg,https://oleks-netizen.github.io/product-images/7683-black/3.jpg,https://oleks-netizen.github.io/product-images/7683-black/4.jpg,https://oleks-netizen.github.io/product-images/7683-black/5.jpg,https://oleks-netizen.github.io/product-images/7683-black/6.jpg,https://oleks-netizen.github.io/product-images/7683-black/7.jpg,https://oleks-netizen.github.io/product-images/7683-black/8.jpg,https://oleks-netizen.github.io/product-images/7683-black/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/7683-black/1.jpg,https://oleks-netizen.github.io/product-images/7683-black/2.jpg,https://oleks-netizen.github.io/product-images/7683-black/10.jpg,https://oleks-netizen.github.io/product-images/7683-black/4.jpg,https://oleks-netizen.github.io/product-images/7683-black/5.jpg,https://oleks-netizen.github.io/product-images/7683-black/6.jpg,https://oleks-netizen.github.io/product-images/7683-black/7.jpg,https://oleks-netizen.github.io/product-images/7683-black/8.jpg,https://oleks-netizen.github.io/product-images/7683-black/9.jpg</t>
         </is>
       </c>
       <c r="C68" t="n">
@@ -1451,7 +1451,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/7687-black/10.jpg,https://oleks-netizen.github.io/product-images/7687-black/1.jpg,https://oleks-netizen.github.io/product-images/7687-black/3.jpg,https://oleks-netizen.github.io/product-images/7687-black/4.jpg,https://oleks-netizen.github.io/product-images/7687-black/5.jpg,https://oleks-netizen.github.io/product-images/7687-black/6.jpg,https://oleks-netizen.github.io/product-images/7687-black/7.jpg,https://oleks-netizen.github.io/product-images/7687-black/8.jpg,https://oleks-netizen.github.io/product-images/7687-black/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/7687-black/1.jpg,https://oleks-netizen.github.io/product-images/7687-black/2.jpg,https://oleks-netizen.github.io/product-images/7687-black/10.jpg,https://oleks-netizen.github.io/product-images/7687-black/4.jpg,https://oleks-netizen.github.io/product-images/7687-black/5.jpg,https://oleks-netizen.github.io/product-images/7687-black/6.jpg,https://oleks-netizen.github.io/product-images/7687-black/7.jpg,https://oleks-netizen.github.io/product-images/7687-black/8.jpg,https://oleks-netizen.github.io/product-images/7687-black/9.jpg</t>
         </is>
       </c>
       <c r="C69" t="n">
@@ -1466,7 +1466,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/7687-grey/10.jpg,https://oleks-netizen.github.io/product-images/7687-grey/1.jpg,https://oleks-netizen.github.io/product-images/7687-grey/3.jpg,https://oleks-netizen.github.io/product-images/7687-grey/4.jpg,https://oleks-netizen.github.io/product-images/7687-grey/5.jpg,https://oleks-netizen.github.io/product-images/7687-grey/6.jpg,https://oleks-netizen.github.io/product-images/7687-grey/7.jpg,https://oleks-netizen.github.io/product-images/7687-grey/8.jpg,https://oleks-netizen.github.io/product-images/7687-grey/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/7687-grey/1.jpg,https://oleks-netizen.github.io/product-images/7687-grey/2.jpg,https://oleks-netizen.github.io/product-images/7687-grey/10.jpg,https://oleks-netizen.github.io/product-images/7687-grey/4.jpg,https://oleks-netizen.github.io/product-images/7687-grey/5.jpg,https://oleks-netizen.github.io/product-images/7687-grey/6.jpg,https://oleks-netizen.github.io/product-images/7687-grey/7.jpg,https://oleks-netizen.github.io/product-images/7687-grey/8.jpg,https://oleks-netizen.github.io/product-images/7687-grey/9.jpg</t>
         </is>
       </c>
       <c r="C70" t="n">
@@ -1481,7 +1481,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/7688-black/10.jpg,https://oleks-netizen.github.io/product-images/7688-black/1.jpg,https://oleks-netizen.github.io/product-images/7688-black/3.jpg,https://oleks-netizen.github.io/product-images/7688-black/4.jpg,https://oleks-netizen.github.io/product-images/7688-black/5.jpg,https://oleks-netizen.github.io/product-images/7688-black/6.jpg,https://oleks-netizen.github.io/product-images/7688-black/7.jpg,https://oleks-netizen.github.io/product-images/7688-black/8.jpg,https://oleks-netizen.github.io/product-images/7688-black/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/7688-black/1.jpg,https://oleks-netizen.github.io/product-images/7688-black/2.jpg,https://oleks-netizen.github.io/product-images/7688-black/10.jpg,https://oleks-netizen.github.io/product-images/7688-black/4.jpg,https://oleks-netizen.github.io/product-images/7688-black/5.jpg,https://oleks-netizen.github.io/product-images/7688-black/6.jpg,https://oleks-netizen.github.io/product-images/7688-black/7.jpg,https://oleks-netizen.github.io/product-images/7688-black/8.jpg,https://oleks-netizen.github.io/product-images/7688-black/9.jpg</t>
         </is>
       </c>
       <c r="C71" t="n">
@@ -1496,7 +1496,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/7688-grey/10.jpg,https://oleks-netizen.github.io/product-images/7688-grey/1.jpg,https://oleks-netizen.github.io/product-images/7688-grey/3.jpg,https://oleks-netizen.github.io/product-images/7688-grey/4.jpg,https://oleks-netizen.github.io/product-images/7688-grey/5.jpg,https://oleks-netizen.github.io/product-images/7688-grey/6.jpg,https://oleks-netizen.github.io/product-images/7688-grey/7.jpg,https://oleks-netizen.github.io/product-images/7688-grey/8.jpg,https://oleks-netizen.github.io/product-images/7688-grey/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/7688-grey/1.jpg,https://oleks-netizen.github.io/product-images/7688-grey/2.jpg,https://oleks-netizen.github.io/product-images/7688-grey/10.jpg,https://oleks-netizen.github.io/product-images/7688-grey/4.jpg,https://oleks-netizen.github.io/product-images/7688-grey/5.jpg,https://oleks-netizen.github.io/product-images/7688-grey/6.jpg,https://oleks-netizen.github.io/product-images/7688-grey/7.jpg,https://oleks-netizen.github.io/product-images/7688-grey/8.jpg,https://oleks-netizen.github.io/product-images/7688-grey/9.jpg</t>
         </is>
       </c>
       <c r="C72" t="n">
@@ -1661,7 +1661,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/8825-green-pixel/10.jpg,https://oleks-netizen.github.io/product-images/8825-green-pixel/11.jpg,https://oleks-netizen.github.io/product-images/8825-green-pixel/12.jpg,https://oleks-netizen.github.io/product-images/8825-green-pixel/13.jpg,https://oleks-netizen.github.io/product-images/8825-green-pixel/1.jpg,https://oleks-netizen.github.io/product-images/8825-green-pixel/2.jpg,https://oleks-netizen.github.io/product-images/8825-green-pixel/3.jpg,https://oleks-netizen.github.io/product-images/8825-green-pixel/5.jpg,https://oleks-netizen.github.io/product-images/8825-green-pixel/6.jpg,https://oleks-netizen.github.io/product-images/8825-green-pixel/7.jpg,https://oleks-netizen.github.io/product-images/8825-green-pixel/8.jpg,https://oleks-netizen.github.io/product-images/8825-green-pixel/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/8825-green-pixel/1.jpg,https://oleks-netizen.github.io/product-images/8825-green-pixel/2.jpg,https://oleks-netizen.github.io/product-images/8825-green-pixel/4.jpg,https://oleks-netizen.github.io/product-images/8825-green-pixel/13.jpg,https://oleks-netizen.github.io/product-images/8825-green-pixel/10.jpg,https://oleks-netizen.github.io/product-images/8825-green-pixel/11.jpg,https://oleks-netizen.github.io/product-images/8825-green-pixel/12.jpg,https://oleks-netizen.github.io/product-images/8825-green-pixel/5.jpg,https://oleks-netizen.github.io/product-images/8825-green-pixel/6.jpg,https://oleks-netizen.github.io/product-images/8825-green-pixel/7.jpg,https://oleks-netizen.github.io/product-images/8825-green-pixel/8.jpg,https://oleks-netizen.github.io/product-images/8825-green-pixel/9.jpg</t>
         </is>
       </c>
       <c r="C83" t="n">
@@ -1676,7 +1676,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/8825-khaki/10.jpg,https://oleks-netizen.github.io/product-images/8825-khaki/11.jpg,https://oleks-netizen.github.io/product-images/8825-khaki/12.jpg,https://oleks-netizen.github.io/product-images/8825-khaki/13.jpg,https://oleks-netizen.github.io/product-images/8825-khaki/14.jpg,https://oleks-netizen.github.io/product-images/8825-khaki/1.jpg,https://oleks-netizen.github.io/product-images/8825-khaki/2.jpg,https://oleks-netizen.github.io/product-images/8825-khaki/3.jpg,https://oleks-netizen.github.io/product-images/8825-khaki/5.jpg,https://oleks-netizen.github.io/product-images/8825-khaki/6.jpg,https://oleks-netizen.github.io/product-images/8825-khaki/7.jpg,https://oleks-netizen.github.io/product-images/8825-khaki/8.jpg,https://oleks-netizen.github.io/product-images/8825-khaki/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/8825-khaki/1.jpg,https://oleks-netizen.github.io/product-images/8825-khaki/2.jpg,https://oleks-netizen.github.io/product-images/8825-khaki/4.jpg,https://oleks-netizen.github.io/product-images/8825-khaki/14.jpg,https://oleks-netizen.github.io/product-images/8825-khaki/10.jpg,https://oleks-netizen.github.io/product-images/8825-khaki/11.jpg,https://oleks-netizen.github.io/product-images/8825-khaki/12.jpg,https://oleks-netizen.github.io/product-images/8825-khaki/13.jpg,https://oleks-netizen.github.io/product-images/8825-khaki/3.jpg,https://oleks-netizen.github.io/product-images/8825-khaki/5.jpg,https://oleks-netizen.github.io/product-images/8825-khaki/6.jpg,https://oleks-netizen.github.io/product-images/8825-khaki/7.jpg,https://oleks-netizen.github.io/product-images/8825-khaki/9.jpg</t>
         </is>
       </c>
       <c r="C84" t="n">
@@ -1691,7 +1691,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/8825-pesok-pixel/10.jpg,https://oleks-netizen.github.io/product-images/8825-pesok-pixel/11.jpg,https://oleks-netizen.github.io/product-images/8825-pesok-pixel/12.jpg,https://oleks-netizen.github.io/product-images/8825-pesok-pixel/1.jpg,https://oleks-netizen.github.io/product-images/8825-pesok-pixel/2.jpg,https://oleks-netizen.github.io/product-images/8825-pesok-pixel/3.jpg,https://oleks-netizen.github.io/product-images/8825-pesok-pixel/4.jpg,https://oleks-netizen.github.io/product-images/8825-pesok-pixel/5.jpg,https://oleks-netizen.github.io/product-images/8825-pesok-pixel/6.jpg,https://oleks-netizen.github.io/product-images/8825-pesok-pixel/7.jpg,https://oleks-netizen.github.io/product-images/8825-pesok-pixel/8.jpg,https://oleks-netizen.github.io/product-images/8825-pesok-pixel/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/8825-pesok-pixel/1.jpg,https://oleks-netizen.github.io/product-images/8825-pesok-pixel/2.jpg,https://oleks-netizen.github.io/product-images/8825-pesok-pixel/4.jpg,https://oleks-netizen.github.io/product-images/8825-pesok-pixel/13.jpg,https://oleks-netizen.github.io/product-images/8825-pesok-pixel/10.jpg,https://oleks-netizen.github.io/product-images/8825-pesok-pixel/11.jpg,https://oleks-netizen.github.io/product-images/8825-pesok-pixel/12.jpg,https://oleks-netizen.github.io/product-images/8825-pesok-pixel/5.jpg,https://oleks-netizen.github.io/product-images/8825-pesok-pixel/6.jpg,https://oleks-netizen.github.io/product-images/8825-pesok-pixel/7.jpg,https://oleks-netizen.github.io/product-images/8825-pesok-pixel/8.jpg,https://oleks-netizen.github.io/product-images/8825-pesok-pixel/9.jpg</t>
         </is>
       </c>
       <c r="C85" t="n">
@@ -1706,7 +1706,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/9065-black/10.jpg,https://oleks-netizen.github.io/product-images/9065-black/1.jpg,https://oleks-netizen.github.io/product-images/9065-black/2.jpg,https://oleks-netizen.github.io/product-images/9065-black/3.jpg,https://oleks-netizen.github.io/product-images/9065-black/5.jpg,https://oleks-netizen.github.io/product-images/9065-black/6.jpg,https://oleks-netizen.github.io/product-images/9065-black/7.jpg,https://oleks-netizen.github.io/product-images/9065-black/8.jpg,https://oleks-netizen.github.io/product-images/9065-black/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/9065-black/1.jpg,https://oleks-netizen.github.io/product-images/9065-black/2.jpg,https://oleks-netizen.github.io/product-images/9065-black/10.jpg,https://oleks-netizen.github.io/product-images/9065-black/3.jpg,https://oleks-netizen.github.io/product-images/9065-black/5.jpg,https://oleks-netizen.github.io/product-images/9065-black/6.jpg,https://oleks-netizen.github.io/product-images/9065-black/7.jpg,https://oleks-netizen.github.io/product-images/9065-black/8.jpg,https://oleks-netizen.github.io/product-images/9065-black/9.jpg</t>
         </is>
       </c>
       <c r="C86" t="n">
@@ -1721,7 +1721,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/9065-green/10.jpg,https://oleks-netizen.github.io/product-images/9065-green/1.jpg,https://oleks-netizen.github.io/product-images/9065-green/2.jpg,https://oleks-netizen.github.io/product-images/9065-green/3.jpg,https://oleks-netizen.github.io/product-images/9065-green/5.jpg,https://oleks-netizen.github.io/product-images/9065-green/6.jpg,https://oleks-netizen.github.io/product-images/9065-green/7.jpg,https://oleks-netizen.github.io/product-images/9065-green/8.jpg,https://oleks-netizen.github.io/product-images/9065-green/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/9065-green/1.jpg,https://oleks-netizen.github.io/product-images/9065-green/2.jpg,https://oleks-netizen.github.io/product-images/9065-green/10.jpg,https://oleks-netizen.github.io/product-images/9065-green/3.jpg,https://oleks-netizen.github.io/product-images/9065-green/5.jpg,https://oleks-netizen.github.io/product-images/9065-green/6.jpg,https://oleks-netizen.github.io/product-images/9065-green/7.jpg,https://oleks-netizen.github.io/product-images/9065-green/8.jpg,https://oleks-netizen.github.io/product-images/9065-green/9.jpg</t>
         </is>
       </c>
       <c r="C87" t="n">
@@ -1736,7 +1736,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/9065-grey-kam/10.jpg,https://oleks-netizen.github.io/product-images/9065-grey-kam/1.jpg,https://oleks-netizen.github.io/product-images/9065-grey-kam/2.jpg,https://oleks-netizen.github.io/product-images/9065-grey-kam/3.jpg,https://oleks-netizen.github.io/product-images/9065-grey-kam/5.jpg,https://oleks-netizen.github.io/product-images/9065-grey-kam/6.jpg,https://oleks-netizen.github.io/product-images/9065-grey-kam/7.jpg,https://oleks-netizen.github.io/product-images/9065-grey-kam/8.jpg,https://oleks-netizen.github.io/product-images/9065-grey-kam/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/9065-grey-kam/1.jpg,https://oleks-netizen.github.io/product-images/9065-grey-kam/2.jpg,https://oleks-netizen.github.io/product-images/9065-grey-kam/10.jpg,https://oleks-netizen.github.io/product-images/9065-grey-kam/3.jpg,https://oleks-netizen.github.io/product-images/9065-grey-kam/5.jpg,https://oleks-netizen.github.io/product-images/9065-grey-kam/6.jpg,https://oleks-netizen.github.io/product-images/9065-grey-kam/7.jpg,https://oleks-netizen.github.io/product-images/9065-grey-kam/8.jpg,https://oleks-netizen.github.io/product-images/9065-grey-kam/9.jpg</t>
         </is>
       </c>
       <c r="C88" t="n">
@@ -1796,7 +1796,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BV12374-011-24/10.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-24/11.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-24/12.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-24/13.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-24/14.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-24/15.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-24/1.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-24/3.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-24/4.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-24/5.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-24/6.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-24/7.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-24/8.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-24/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BV12374-011-24/1.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-24/2.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-24/10.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-24/11.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-24/12.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-24/13.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-24/14.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-24/15.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-24/3.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-24/5.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-24/6.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-24/7.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-24/8.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-24/9.jpg</t>
         </is>
       </c>
       <c r="C92" t="n">
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BV12374-011-28/10.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-28/11.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-28/12.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-28/13.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-28/14.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-28/15.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-28/1.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-28/3.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-28/4.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-28/5.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-28/6.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-28/7.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-28/8.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-28/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BV12374-011-28/1.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-28/2.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-28/10.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-28/11.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-28/12.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-28/13.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-28/14.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-28/15.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-28/3.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-28/5.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-28/6.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-28/7.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-28/8.jpg,https://oleks-netizen.github.io/product-images/BV12374-011-28/9.jpg</t>
         </is>
       </c>
       <c r="C93" t="n">
@@ -1826,7 +1826,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BV12374-012-24/10.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-24/11.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-24/12.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-24/13.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-24/14.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-24/15.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-24/1.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-24/3.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-24/4.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-24/5.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-24/6.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-24/7.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-24/8.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-24/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BV12374-012-24/1.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-24/2.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-24/10.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-24/11.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-24/12.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-24/13.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-24/14.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-24/15.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-24/3.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-24/5.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-24/6.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-24/7.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-24/8.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-24/9.jpg</t>
         </is>
       </c>
       <c r="C94" t="n">
@@ -1841,7 +1841,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BV12374-012-28/10.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-28/11.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-28/12.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-28/13.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-28/14.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-28/15.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-28/1.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-28/3.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-28/4.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-28/5.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-28/6.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-28/7.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-28/8.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-28/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BV12374-012-28/1.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-28/2.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-28/10.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-28/11.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-28/12.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-28/13.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-28/14.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-28/15.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-28/3.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-28/4.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-28/6.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-28/7.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-28/8.jpg,https://oleks-netizen.github.io/product-images/BV12374-012-28/9.jpg</t>
         </is>
       </c>
       <c r="C95" t="n">
@@ -2306,7 +2306,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BV38655-1/10.jpg,https://oleks-netizen.github.io/product-images/BV38655-1/1.jpg,https://oleks-netizen.github.io/product-images/BV38655-1/2.jpg,https://oleks-netizen.github.io/product-images/BV38655-1/4.jpg,https://oleks-netizen.github.io/product-images/BV38655-1/5.jpg,https://oleks-netizen.github.io/product-images/BV38655-1/6.jpg,https://oleks-netizen.github.io/product-images/BV38655-1/7.jpg,https://oleks-netizen.github.io/product-images/BV38655-1/8.jpg,https://oleks-netizen.github.io/product-images/BV38655-1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BV38655-1/1.jpg,https://oleks-netizen.github.io/product-images/BV38655-1/2.jpg,https://oleks-netizen.github.io/product-images/BV38655-1/10.jpg,https://oleks-netizen.github.io/product-images/BV38655-1/4.jpg,https://oleks-netizen.github.io/product-images/BV38655-1/5.jpg,https://oleks-netizen.github.io/product-images/BV38655-1/6.jpg,https://oleks-netizen.github.io/product-images/BV38655-1/7.jpg,https://oleks-netizen.github.io/product-images/BV38655-1/8.jpg,https://oleks-netizen.github.io/product-images/BV38655-1/9.jpg</t>
         </is>
       </c>
       <c r="C126" t="n">
@@ -2321,7 +2321,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BV38655-153/10.jpg,https://oleks-netizen.github.io/product-images/BV38655-153/1.jpg,https://oleks-netizen.github.io/product-images/BV38655-153/2.jpg,https://oleks-netizen.github.io/product-images/BV38655-153/4.jpg,https://oleks-netizen.github.io/product-images/BV38655-153/5.jpg,https://oleks-netizen.github.io/product-images/BV38655-153/6.jpg,https://oleks-netizen.github.io/product-images/BV38655-153/7.jpg,https://oleks-netizen.github.io/product-images/BV38655-153/8.jpg,https://oleks-netizen.github.io/product-images/BV38655-153/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BV38655-153/1.jpg,https://oleks-netizen.github.io/product-images/BV38655-153/2.jpg,https://oleks-netizen.github.io/product-images/BV38655-153/10.jpg,https://oleks-netizen.github.io/product-images/BV38655-153/4.jpg,https://oleks-netizen.github.io/product-images/BV38655-153/5.jpg,https://oleks-netizen.github.io/product-images/BV38655-153/6.jpg,https://oleks-netizen.github.io/product-images/BV38655-153/7.jpg,https://oleks-netizen.github.io/product-images/BV38655-153/8.jpg,https://oleks-netizen.github.io/product-images/BV38655-153/9.jpg</t>
         </is>
       </c>
       <c r="C127" t="n">
@@ -3701,7 +3701,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DRL19941-1/10.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/1.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/2.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/4.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/5.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/6.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/7.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/8.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRL19941-1/1.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/2.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/10.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/4.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/5.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/6.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/7.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/8.jpg,https://oleks-netizen.github.io/product-images/DRL19941-1/9.jpg</t>
         </is>
       </c>
       <c r="C219" t="n">
@@ -3731,7 +3731,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DRS16059-1/10.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/11.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/1.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/2.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/4.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/5.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/6.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/7.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/8.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DRS16059-1/1.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/2.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/10.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/11.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/4.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/5.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/6.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/7.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/8.jpg,https://oleks-netizen.github.io/product-images/DRS16059-1/9.jpg</t>
         </is>
       </c>
       <c r="C221" t="n">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/DS23873-230/1.jpg,https://oleks-netizen.github.io/product-images/DS23873-230/2.jpg,https://oleks-netizen.github.io/product-images/DS23873-230/3.jpg,https://oleks-netizen.github.io/product-images/DS23873-230/5.jpg,https://oleks-netizen.github.io/product-images/DS23873-230/6.jpg,https://oleks-netizen.github.io/product-images/DS23873-230/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/DS23873-230/1.jpg,https://oleks-netizen.github.io/product-images/DS23873-230/2.jpg,https://oleks-netizen.github.io/product-images/DS23873-230/4.jpg,https://oleks-netizen.github.io/product-images/DS23873-230/3.jpg,https://oleks-netizen.github.io/product-images/DS23873-230/5.jpg,https://oleks-netizen.github.io/product-images/DS23873-230/6.jpg</t>
         </is>
       </c>
       <c r="C231" t="n">
@@ -4166,7 +4166,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-grey/10.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-grey/1.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-grey/2.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-grey/3.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-grey/4.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-grey/6.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-grey/7.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-grey/8.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-grey/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-grey/1.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-grey/2.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-grey/5.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-grey/10.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-grey/3.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-grey/4.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-grey/6.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-grey/7.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-grey/9.jpg</t>
         </is>
       </c>
       <c r="C250" t="n">
@@ -4181,7 +4181,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-purple/10.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-purple/1.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-purple/2.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-purple/3.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-purple/4.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-purple/6.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-purple/7.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-purple/8.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-purple/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-purple/1.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-purple/2.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-purple/5.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-purple/10.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-purple/3.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-purple/4.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-purple/6.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-purple/7.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-dark-purple/9.jpg</t>
         </is>
       </c>
       <c r="C251" t="n">
@@ -4196,7 +4196,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/ICE-2314-20-khaki/10.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-khaki/1.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-khaki/2.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-khaki/3.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-khaki/4.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-khaki/6.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-khaki/7.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-khaki/8.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-khaki/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/ICE-2314-20-khaki/1.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-khaki/2.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-khaki/5.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-khaki/10.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-khaki/3.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-khaki/4.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-khaki/6.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-khaki/7.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-khaki/9.jpg</t>
         </is>
       </c>
       <c r="C252" t="n">
@@ -4211,7 +4211,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/ICE-2314-20-rose-gold/10.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-rose-gold/1.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-rose-gold/2.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-rose-gold/3.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-rose-gold/4.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-rose-gold/6.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-rose-gold/7.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-rose-gold/8.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-rose-gold/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/ICE-2314-20-rose-gold/1.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-rose-gold/2.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-rose-gold/5.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-rose-gold/10.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-rose-gold/3.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-rose-gold/4.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-rose-gold/6.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-rose-gold/7.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-20-rose-gold/9.jpg</t>
         </is>
       </c>
       <c r="C253" t="n">
@@ -4226,7 +4226,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-grey/1.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-grey/2.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-grey/3.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-grey/4.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-grey/5.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-grey/6.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-grey/8.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-grey/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-grey/1.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-grey/2.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-grey/7.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-grey/3.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-grey/5.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-grey/6.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-grey/8.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-grey/9.jpg</t>
         </is>
       </c>
       <c r="C254" t="n">
@@ -4241,7 +4241,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-purple/1.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-purple/2.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-purple/3.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-purple/4.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-purple/5.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-purple/6.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-purple/8.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-purple/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-purple/1.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-purple/2.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-purple/7.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-purple/3.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-purple/4.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-purple/5.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-purple/6.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-dark-purple/9.jpg</t>
         </is>
       </c>
       <c r="C255" t="n">
@@ -4256,7 +4256,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/ICE-2314-24-rose-gold/1.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-rose-gold/2.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-rose-gold/3.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-rose-gold/4.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-rose-gold/5.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-rose-gold/6.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-rose-gold/8.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-rose-gold/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/ICE-2314-24-rose-gold/1.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-rose-gold/2.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-rose-gold/7.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-rose-gold/3.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-rose-gold/4.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-rose-gold/5.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-rose-gold/6.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-24-rose-gold/9.jpg</t>
         </is>
       </c>
       <c r="C256" t="n">
@@ -4271,7 +4271,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-grey/1.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-grey/2.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-grey/3.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-grey/4.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-grey/5.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-grey/6.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-grey/8.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-grey/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-grey/1.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-grey/2.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-grey/7.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-grey/3.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-grey/4.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-grey/5.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-grey/6.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-grey/9.jpg</t>
         </is>
       </c>
       <c r="C257" t="n">
@@ -4286,7 +4286,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-purple/1.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-purple/2.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-purple/3.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-purple/4.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-purple/5.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-purple/6.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-purple/8.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-purple/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-purple/1.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-purple/2.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-purple/7.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-purple/3.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-purple/5.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-purple/6.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-purple/8.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-dark-purple/9.jpg</t>
         </is>
       </c>
       <c r="C258" t="n">
@@ -4301,7 +4301,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/ICE-2314-28-rose-gold/1.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-rose-gold/2.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-rose-gold/3.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-rose-gold/4.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-rose-gold/5.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-rose-gold/6.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-rose-gold/8.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-rose-gold/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/ICE-2314-28-rose-gold/1.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-rose-gold/2.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-rose-gold/7.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-rose-gold/3.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-rose-gold/5.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-rose-gold/6.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-rose-gold/8.jpg,https://oleks-netizen.github.io/product-images/ICE-2314-28-rose-gold/9.jpg</t>
         </is>
       </c>
       <c r="C259" t="n">
@@ -4406,7 +4406,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20036-1/10.jpg,https://oleks-netizen.github.io/product-images/L20036-1/1.jpg,https://oleks-netizen.github.io/product-images/L20036-1/2.jpg,https://oleks-netizen.github.io/product-images/L20036-1/4.jpg,https://oleks-netizen.github.io/product-images/L20036-1/5.jpg,https://oleks-netizen.github.io/product-images/L20036-1/6.jpg,https://oleks-netizen.github.io/product-images/L20036-1/7.jpg,https://oleks-netizen.github.io/product-images/L20036-1/8.jpg,https://oleks-netizen.github.io/product-images/L20036-1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20036-1/1.jpg,https://oleks-netizen.github.io/product-images/L20036-1/2.jpg,https://oleks-netizen.github.io/product-images/L20036-1/10.jpg,https://oleks-netizen.github.io/product-images/L20036-1/4.jpg,https://oleks-netizen.github.io/product-images/L20036-1/5.jpg,https://oleks-netizen.github.io/product-images/L20036-1/6.jpg,https://oleks-netizen.github.io/product-images/L20036-1/7.jpg,https://oleks-netizen.github.io/product-images/L20036-1/8.jpg,https://oleks-netizen.github.io/product-images/L20036-1/9.jpg</t>
         </is>
       </c>
       <c r="C266" t="n">
@@ -4436,7 +4436,7 @@
       </c>
       <c r="B268" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20063-1/10.jpg,https://oleks-netizen.github.io/product-images/L20063-1/1.jpg,https://oleks-netizen.github.io/product-images/L20063-1/2.jpg,https://oleks-netizen.github.io/product-images/L20063-1/4.jpg,https://oleks-netizen.github.io/product-images/L20063-1/5.jpg,https://oleks-netizen.github.io/product-images/L20063-1/6.jpg,https://oleks-netizen.github.io/product-images/L20063-1/7.jpg,https://oleks-netizen.github.io/product-images/L20063-1/8.jpg,https://oleks-netizen.github.io/product-images/L20063-1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20063-1/1.jpg,https://oleks-netizen.github.io/product-images/L20063-1/2.jpg,https://oleks-netizen.github.io/product-images/L20063-1/10.jpg,https://oleks-netizen.github.io/product-images/L20063-1/4.jpg,https://oleks-netizen.github.io/product-images/L20063-1/5.jpg,https://oleks-netizen.github.io/product-images/L20063-1/6.jpg,https://oleks-netizen.github.io/product-images/L20063-1/7.jpg,https://oleks-netizen.github.io/product-images/L20063-1/8.jpg,https://oleks-netizen.github.io/product-images/L20063-1/9.jpg</t>
         </is>
       </c>
       <c r="C268" t="n">
@@ -4451,7 +4451,7 @@
       </c>
       <c r="B269" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20063-8/10.jpg,https://oleks-netizen.github.io/product-images/L20063-8/1.jpg,https://oleks-netizen.github.io/product-images/L20063-8/2.jpg,https://oleks-netizen.github.io/product-images/L20063-8/4.jpg,https://oleks-netizen.github.io/product-images/L20063-8/5.jpg,https://oleks-netizen.github.io/product-images/L20063-8/6.jpg,https://oleks-netizen.github.io/product-images/L20063-8/7.jpg,https://oleks-netizen.github.io/product-images/L20063-8/8.jpg,https://oleks-netizen.github.io/product-images/L20063-8/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20063-8/1.jpg,https://oleks-netizen.github.io/product-images/L20063-8/2.jpg,https://oleks-netizen.github.io/product-images/L20063-8/10.jpg,https://oleks-netizen.github.io/product-images/L20063-8/4.jpg,https://oleks-netizen.github.io/product-images/L20063-8/5.jpg,https://oleks-netizen.github.io/product-images/L20063-8/6.jpg,https://oleks-netizen.github.io/product-images/L20063-8/7.jpg,https://oleks-netizen.github.io/product-images/L20063-8/8.jpg,https://oleks-netizen.github.io/product-images/L20063-8/9.jpg</t>
         </is>
       </c>
       <c r="C269" t="n">
@@ -4511,7 +4511,7 @@
       </c>
       <c r="B273" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20680-1/10.jpg,https://oleks-netizen.github.io/product-images/L20680-1/1.jpg,https://oleks-netizen.github.io/product-images/L20680-1/2.jpg,https://oleks-netizen.github.io/product-images/L20680-1/4.jpg,https://oleks-netizen.github.io/product-images/L20680-1/5.jpg,https://oleks-netizen.github.io/product-images/L20680-1/6.jpg,https://oleks-netizen.github.io/product-images/L20680-1/7.jpg,https://oleks-netizen.github.io/product-images/L20680-1/8.jpg,https://oleks-netizen.github.io/product-images/L20680-1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20680-1/1.jpg,https://oleks-netizen.github.io/product-images/L20680-1/2.jpg,https://oleks-netizen.github.io/product-images/L20680-1/10.jpg,https://oleks-netizen.github.io/product-images/L20680-1/4.jpg,https://oleks-netizen.github.io/product-images/L20680-1/5.jpg,https://oleks-netizen.github.io/product-images/L20680-1/6.jpg,https://oleks-netizen.github.io/product-images/L20680-1/7.jpg,https://oleks-netizen.github.io/product-images/L20680-1/8.jpg,https://oleks-netizen.github.io/product-images/L20680-1/9.jpg</t>
         </is>
       </c>
       <c r="C273" t="n">
@@ -4526,7 +4526,7 @@
       </c>
       <c r="B274" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20680-56/10.jpg,https://oleks-netizen.github.io/product-images/L20680-56/1.jpg,https://oleks-netizen.github.io/product-images/L20680-56/2.jpg,https://oleks-netizen.github.io/product-images/L20680-56/4.jpg,https://oleks-netizen.github.io/product-images/L20680-56/5.jpg,https://oleks-netizen.github.io/product-images/L20680-56/6.jpg,https://oleks-netizen.github.io/product-images/L20680-56/7.jpg,https://oleks-netizen.github.io/product-images/L20680-56/8.jpg,https://oleks-netizen.github.io/product-images/L20680-56/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20680-56/1.jpg,https://oleks-netizen.github.io/product-images/L20680-56/2.jpg,https://oleks-netizen.github.io/product-images/L20680-56/10.jpg,https://oleks-netizen.github.io/product-images/L20680-56/4.jpg,https://oleks-netizen.github.io/product-images/L20680-56/5.jpg,https://oleks-netizen.github.io/product-images/L20680-56/6.jpg,https://oleks-netizen.github.io/product-images/L20680-56/7.jpg,https://oleks-netizen.github.io/product-images/L20680-56/8.jpg,https://oleks-netizen.github.io/product-images/L20680-56/9.jpg</t>
         </is>
       </c>
       <c r="C274" t="n">
@@ -4541,7 +4541,7 @@
       </c>
       <c r="B275" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20680-58/10.jpg,https://oleks-netizen.github.io/product-images/L20680-58/1.jpg,https://oleks-netizen.github.io/product-images/L20680-58/2.jpg,https://oleks-netizen.github.io/product-images/L20680-58/4.jpg,https://oleks-netizen.github.io/product-images/L20680-58/5.jpg,https://oleks-netizen.github.io/product-images/L20680-58/6.jpg,https://oleks-netizen.github.io/product-images/L20680-58/7.jpg,https://oleks-netizen.github.io/product-images/L20680-58/8.jpg,https://oleks-netizen.github.io/product-images/L20680-58/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20680-58/1.jpg,https://oleks-netizen.github.io/product-images/L20680-58/2.jpg,https://oleks-netizen.github.io/product-images/L20680-58/10.jpg,https://oleks-netizen.github.io/product-images/L20680-58/4.jpg,https://oleks-netizen.github.io/product-images/L20680-58/5.jpg,https://oleks-netizen.github.io/product-images/L20680-58/6.jpg,https://oleks-netizen.github.io/product-images/L20680-58/7.jpg,https://oleks-netizen.github.io/product-images/L20680-58/8.jpg,https://oleks-netizen.github.io/product-images/L20680-58/9.jpg</t>
         </is>
       </c>
       <c r="C275" t="n">
@@ -4601,7 +4601,7 @@
       </c>
       <c r="B279" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20713-1/10.jpg,https://oleks-netizen.github.io/product-images/L20713-1/1.jpg,https://oleks-netizen.github.io/product-images/L20713-1/2.jpg,https://oleks-netizen.github.io/product-images/L20713-1/4.jpg,https://oleks-netizen.github.io/product-images/L20713-1/5.jpg,https://oleks-netizen.github.io/product-images/L20713-1/6.jpg,https://oleks-netizen.github.io/product-images/L20713-1/7.jpg,https://oleks-netizen.github.io/product-images/L20713-1/8.jpg,https://oleks-netizen.github.io/product-images/L20713-1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20713-1/1.jpg,https://oleks-netizen.github.io/product-images/L20713-1/2.jpg,https://oleks-netizen.github.io/product-images/L20713-1/10.jpg,https://oleks-netizen.github.io/product-images/L20713-1/4.jpg,https://oleks-netizen.github.io/product-images/L20713-1/5.jpg,https://oleks-netizen.github.io/product-images/L20713-1/6.jpg,https://oleks-netizen.github.io/product-images/L20713-1/7.jpg,https://oleks-netizen.github.io/product-images/L20713-1/8.jpg,https://oleks-netizen.github.io/product-images/L20713-1/9.jpg</t>
         </is>
       </c>
       <c r="C279" t="n">
@@ -4616,7 +4616,7 @@
       </c>
       <c r="B280" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20713-8/10.jpg,https://oleks-netizen.github.io/product-images/L20713-8/1.jpg,https://oleks-netizen.github.io/product-images/L20713-8/2.jpg,https://oleks-netizen.github.io/product-images/L20713-8/4.jpg,https://oleks-netizen.github.io/product-images/L20713-8/5.jpg,https://oleks-netizen.github.io/product-images/L20713-8/6.jpg,https://oleks-netizen.github.io/product-images/L20713-8/7.jpg,https://oleks-netizen.github.io/product-images/L20713-8/8.jpg,https://oleks-netizen.github.io/product-images/L20713-8/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20713-8/1.jpg,https://oleks-netizen.github.io/product-images/L20713-8/2.jpg,https://oleks-netizen.github.io/product-images/L20713-8/10.jpg,https://oleks-netizen.github.io/product-images/L20713-8/4.jpg,https://oleks-netizen.github.io/product-images/L20713-8/5.jpg,https://oleks-netizen.github.io/product-images/L20713-8/6.jpg,https://oleks-netizen.github.io/product-images/L20713-8/7.jpg,https://oleks-netizen.github.io/product-images/L20713-8/8.jpg,https://oleks-netizen.github.io/product-images/L20713-8/9.jpg</t>
         </is>
       </c>
       <c r="C280" t="n">
@@ -4631,7 +4631,7 @@
       </c>
       <c r="B281" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20812-1/10.jpg,https://oleks-netizen.github.io/product-images/L20812-1/1.jpg,https://oleks-netizen.github.io/product-images/L20812-1/2.jpg,https://oleks-netizen.github.io/product-images/L20812-1/4.jpg,https://oleks-netizen.github.io/product-images/L20812-1/5.jpg,https://oleks-netizen.github.io/product-images/L20812-1/6.jpg,https://oleks-netizen.github.io/product-images/L20812-1/7.jpg,https://oleks-netizen.github.io/product-images/L20812-1/8.jpg,https://oleks-netizen.github.io/product-images/L20812-1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20812-1/1.jpg,https://oleks-netizen.github.io/product-images/L20812-1/2.jpg,https://oleks-netizen.github.io/product-images/L20812-1/10.jpg,https://oleks-netizen.github.io/product-images/L20812-1/4.jpg,https://oleks-netizen.github.io/product-images/L20812-1/5.jpg,https://oleks-netizen.github.io/product-images/L20812-1/6.jpg,https://oleks-netizen.github.io/product-images/L20812-1/7.jpg,https://oleks-netizen.github.io/product-images/L20812-1/8.jpg,https://oleks-netizen.github.io/product-images/L20812-1/9.jpg</t>
         </is>
       </c>
       <c r="C281" t="n">
@@ -4646,7 +4646,7 @@
       </c>
       <c r="B282" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20812-10/10.jpg,https://oleks-netizen.github.io/product-images/L20812-10/1.jpg,https://oleks-netizen.github.io/product-images/L20812-10/2.jpg,https://oleks-netizen.github.io/product-images/L20812-10/4.jpg,https://oleks-netizen.github.io/product-images/L20812-10/5.jpg,https://oleks-netizen.github.io/product-images/L20812-10/6.jpg,https://oleks-netizen.github.io/product-images/L20812-10/7.jpg,https://oleks-netizen.github.io/product-images/L20812-10/8.jpg,https://oleks-netizen.github.io/product-images/L20812-10/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20812-10/1.jpg,https://oleks-netizen.github.io/product-images/L20812-10/2.jpg,https://oleks-netizen.github.io/product-images/L20812-10/10.jpg,https://oleks-netizen.github.io/product-images/L20812-10/4.jpg,https://oleks-netizen.github.io/product-images/L20812-10/5.jpg,https://oleks-netizen.github.io/product-images/L20812-10/6.jpg,https://oleks-netizen.github.io/product-images/L20812-10/7.jpg,https://oleks-netizen.github.io/product-images/L20812-10/8.jpg,https://oleks-netizen.github.io/product-images/L20812-10/9.jpg</t>
         </is>
       </c>
       <c r="C282" t="n">
@@ -4661,7 +4661,7 @@
       </c>
       <c r="B283" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20812-15/10.jpg,https://oleks-netizen.github.io/product-images/L20812-15/1.jpg,https://oleks-netizen.github.io/product-images/L20812-15/2.jpg,https://oleks-netizen.github.io/product-images/L20812-15/4.jpg,https://oleks-netizen.github.io/product-images/L20812-15/5.jpg,https://oleks-netizen.github.io/product-images/L20812-15/6.jpg,https://oleks-netizen.github.io/product-images/L20812-15/7.jpg,https://oleks-netizen.github.io/product-images/L20812-15/8.jpg,https://oleks-netizen.github.io/product-images/L20812-15/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20812-15/1.jpg,https://oleks-netizen.github.io/product-images/L20812-15/2.jpg,https://oleks-netizen.github.io/product-images/L20812-15/10.jpg,https://oleks-netizen.github.io/product-images/L20812-15/4.jpg,https://oleks-netizen.github.io/product-images/L20812-15/5.jpg,https://oleks-netizen.github.io/product-images/L20812-15/6.jpg,https://oleks-netizen.github.io/product-images/L20812-15/7.jpg,https://oleks-netizen.github.io/product-images/L20812-15/8.jpg,https://oleks-netizen.github.io/product-images/L20812-15/9.jpg</t>
         </is>
       </c>
       <c r="C283" t="n">
@@ -4766,7 +4766,7 @@
       </c>
       <c r="B290" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20853-1/10.jpg,https://oleks-netizen.github.io/product-images/L20853-1/1.jpg,https://oleks-netizen.github.io/product-images/L20853-1/2.jpg,https://oleks-netizen.github.io/product-images/L20853-1/4.jpg,https://oleks-netizen.github.io/product-images/L20853-1/5.jpg,https://oleks-netizen.github.io/product-images/L20853-1/6.jpg,https://oleks-netizen.github.io/product-images/L20853-1/7.jpg,https://oleks-netizen.github.io/product-images/L20853-1/8.jpg,https://oleks-netizen.github.io/product-images/L20853-1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20853-1/2.jpg,https://oleks-netizen.github.io/product-images/L20853-1/4.jpg,https://oleks-netizen.github.io/product-images/L20853-1/11.jpg,https://oleks-netizen.github.io/product-images/L20853-1/10.jpg,https://oleks-netizen.github.io/product-images/L20853-1/5.jpg,https://oleks-netizen.github.io/product-images/L20853-1/6.jpg,https://oleks-netizen.github.io/product-images/L20853-1/7.jpg,https://oleks-netizen.github.io/product-images/L20853-1/8.jpg,https://oleks-netizen.github.io/product-images/L20853-1/9.jpg</t>
         </is>
       </c>
       <c r="C290" t="n">
@@ -4856,7 +4856,7 @@
       </c>
       <c r="B296" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21209-1/10.jpg,https://oleks-netizen.github.io/product-images/L21209-1/1.jpg,https://oleks-netizen.github.io/product-images/L21209-1/2.jpg,https://oleks-netizen.github.io/product-images/L21209-1/4.jpg,https://oleks-netizen.github.io/product-images/L21209-1/5.jpg,https://oleks-netizen.github.io/product-images/L21209-1/6.jpg,https://oleks-netizen.github.io/product-images/L21209-1/7.jpg,https://oleks-netizen.github.io/product-images/L21209-1/8.jpg,https://oleks-netizen.github.io/product-images/L21209-1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21209-1/1.jpg,https://oleks-netizen.github.io/product-images/L21209-1/2.jpg,https://oleks-netizen.github.io/product-images/L21209-1/10.jpg,https://oleks-netizen.github.io/product-images/L21209-1/4.jpg,https://oleks-netizen.github.io/product-images/L21209-1/5.jpg,https://oleks-netizen.github.io/product-images/L21209-1/6.jpg,https://oleks-netizen.github.io/product-images/L21209-1/7.jpg,https://oleks-netizen.github.io/product-images/L21209-1/8.jpg,https://oleks-netizen.github.io/product-images/L21209-1/9.jpg</t>
         </is>
       </c>
       <c r="C296" t="n">
@@ -4871,7 +4871,7 @@
       </c>
       <c r="B297" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21209-25/10.jpg,https://oleks-netizen.github.io/product-images/L21209-25/1.jpg,https://oleks-netizen.github.io/product-images/L21209-25/2.jpg,https://oleks-netizen.github.io/product-images/L21209-25/4.jpg,https://oleks-netizen.github.io/product-images/L21209-25/5.jpg,https://oleks-netizen.github.io/product-images/L21209-25/6.jpg,https://oleks-netizen.github.io/product-images/L21209-25/7.jpg,https://oleks-netizen.github.io/product-images/L21209-25/8.jpg,https://oleks-netizen.github.io/product-images/L21209-25/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21209-25/1.jpg,https://oleks-netizen.github.io/product-images/L21209-25/2.jpg,https://oleks-netizen.github.io/product-images/L21209-25/10.jpg,https://oleks-netizen.github.io/product-images/L21209-25/4.jpg,https://oleks-netizen.github.io/product-images/L21209-25/5.jpg,https://oleks-netizen.github.io/product-images/L21209-25/6.jpg,https://oleks-netizen.github.io/product-images/L21209-25/7.jpg,https://oleks-netizen.github.io/product-images/L21209-25/8.jpg,https://oleks-netizen.github.io/product-images/L21209-25/9.jpg</t>
         </is>
       </c>
       <c r="C297" t="n">
@@ -4946,7 +4946,7 @@
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21545-1/10.jpg,https://oleks-netizen.github.io/product-images/L21545-1/1.jpg,https://oleks-netizen.github.io/product-images/L21545-1/2.jpg,https://oleks-netizen.github.io/product-images/L21545-1/4.jpg,https://oleks-netizen.github.io/product-images/L21545-1/5.jpg,https://oleks-netizen.github.io/product-images/L21545-1/6.jpg,https://oleks-netizen.github.io/product-images/L21545-1/7.jpg,https://oleks-netizen.github.io/product-images/L21545-1/8.jpg,https://oleks-netizen.github.io/product-images/L21545-1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21545-1/1.jpg,https://oleks-netizen.github.io/product-images/L21545-1/2.jpg,https://oleks-netizen.github.io/product-images/L21545-1/10.jpg,https://oleks-netizen.github.io/product-images/L21545-1/4.jpg,https://oleks-netizen.github.io/product-images/L21545-1/5.jpg,https://oleks-netizen.github.io/product-images/L21545-1/6.jpg,https://oleks-netizen.github.io/product-images/L21545-1/7.jpg,https://oleks-netizen.github.io/product-images/L21545-1/8.jpg,https://oleks-netizen.github.io/product-images/L21545-1/9.jpg</t>
         </is>
       </c>
       <c r="C302" t="n">
@@ -4961,7 +4961,7 @@
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21545-175/10.jpg,https://oleks-netizen.github.io/product-images/L21545-175/1.jpg,https://oleks-netizen.github.io/product-images/L21545-175/2.jpg,https://oleks-netizen.github.io/product-images/L21545-175/4.jpg,https://oleks-netizen.github.io/product-images/L21545-175/5.jpg,https://oleks-netizen.github.io/product-images/L21545-175/6.jpg,https://oleks-netizen.github.io/product-images/L21545-175/7.jpg,https://oleks-netizen.github.io/product-images/L21545-175/8.jpg,https://oleks-netizen.github.io/product-images/L21545-175/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21545-175/1.jpg,https://oleks-netizen.github.io/product-images/L21545-175/2.jpg,https://oleks-netizen.github.io/product-images/L21545-175/10.jpg,https://oleks-netizen.github.io/product-images/L21545-175/4.jpg,https://oleks-netizen.github.io/product-images/L21545-175/5.jpg,https://oleks-netizen.github.io/product-images/L21545-175/6.jpg,https://oleks-netizen.github.io/product-images/L21545-175/7.jpg,https://oleks-netizen.github.io/product-images/L21545-175/8.jpg,https://oleks-netizen.github.io/product-images/L21545-175/9.jpg</t>
         </is>
       </c>
       <c r="C303" t="n">
@@ -4991,7 +4991,7 @@
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21549-1/10.jpg,https://oleks-netizen.github.io/product-images/L21549-1/1.jpg,https://oleks-netizen.github.io/product-images/L21549-1/2.jpg,https://oleks-netizen.github.io/product-images/L21549-1/3.jpg,https://oleks-netizen.github.io/product-images/L21549-1/5.jpg,https://oleks-netizen.github.io/product-images/L21549-1/6.jpg,https://oleks-netizen.github.io/product-images/L21549-1/7.jpg,https://oleks-netizen.github.io/product-images/L21549-1/8.jpg,https://oleks-netizen.github.io/product-images/L21549-1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21549-1/1.jpg,https://oleks-netizen.github.io/product-images/L21549-1/2.jpg,https://oleks-netizen.github.io/product-images/L21549-1/10.jpg,https://oleks-netizen.github.io/product-images/L21549-1/3.jpg,https://oleks-netizen.github.io/product-images/L21549-1/5.jpg,https://oleks-netizen.github.io/product-images/L21549-1/6.jpg,https://oleks-netizen.github.io/product-images/L21549-1/7.jpg,https://oleks-netizen.github.io/product-images/L21549-1/8.jpg,https://oleks-netizen.github.io/product-images/L21549-1/9.jpg</t>
         </is>
       </c>
       <c r="C305" t="n">
@@ -5006,7 +5006,7 @@
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21549-22/10.jpg,https://oleks-netizen.github.io/product-images/L21549-22/1.jpg,https://oleks-netizen.github.io/product-images/L21549-22/2.jpg,https://oleks-netizen.github.io/product-images/L21549-22/3.jpg,https://oleks-netizen.github.io/product-images/L21549-22/5.jpg,https://oleks-netizen.github.io/product-images/L21549-22/6.jpg,https://oleks-netizen.github.io/product-images/L21549-22/7.jpg,https://oleks-netizen.github.io/product-images/L21549-22/8.jpg,https://oleks-netizen.github.io/product-images/L21549-22/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21549-22/1.jpg,https://oleks-netizen.github.io/product-images/L21549-22/2.jpg,https://oleks-netizen.github.io/product-images/L21549-22/10.jpg,https://oleks-netizen.github.io/product-images/L21549-22/3.jpg,https://oleks-netizen.github.io/product-images/L21549-22/5.jpg,https://oleks-netizen.github.io/product-images/L21549-22/6.jpg,https://oleks-netizen.github.io/product-images/L21549-22/7.jpg,https://oleks-netizen.github.io/product-images/L21549-22/8.jpg,https://oleks-netizen.github.io/product-images/L21549-22/9.jpg</t>
         </is>
       </c>
       <c r="C306" t="n">
@@ -5021,7 +5021,7 @@
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21557-1/10.jpg,https://oleks-netizen.github.io/product-images/L21557-1/11.jpg,https://oleks-netizen.github.io/product-images/L21557-1/1.jpg,https://oleks-netizen.github.io/product-images/L21557-1/2.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3.jpg,https://oleks-netizen.github.io/product-images/L21557-1/5.jpg,https://oleks-netizen.github.io/product-images/L21557-1/6.jpg,https://oleks-netizen.github.io/product-images/L21557-1/7.jpg,https://oleks-netizen.github.io/product-images/L21557-1/8.jpg,https://oleks-netizen.github.io/product-images/L21557-1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21557-1/1.jpg,https://oleks-netizen.github.io/product-images/L21557-1/2.jpg,https://oleks-netizen.github.io/product-images/L21557-1/10.jpg,https://oleks-netizen.github.io/product-images/L21557-1/11.jpg,https://oleks-netizen.github.io/product-images/L21557-1/3.jpg,https://oleks-netizen.github.io/product-images/L21557-1/5.jpg,https://oleks-netizen.github.io/product-images/L21557-1/6.jpg,https://oleks-netizen.github.io/product-images/L21557-1/7.jpg,https://oleks-netizen.github.io/product-images/L21557-1/8.jpg,https://oleks-netizen.github.io/product-images/L21557-1/9.jpg</t>
         </is>
       </c>
       <c r="C307" t="n">
@@ -5036,7 +5036,7 @@
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21557-173/10.jpg,https://oleks-netizen.github.io/product-images/L21557-173/11.jpg,https://oleks-netizen.github.io/product-images/L21557-173/1.jpg,https://oleks-netizen.github.io/product-images/L21557-173/2.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3.jpg,https://oleks-netizen.github.io/product-images/L21557-173/5.jpg,https://oleks-netizen.github.io/product-images/L21557-173/6.jpg,https://oleks-netizen.github.io/product-images/L21557-173/7.jpg,https://oleks-netizen.github.io/product-images/L21557-173/8.jpg,https://oleks-netizen.github.io/product-images/L21557-173/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21557-173/1.jpg,https://oleks-netizen.github.io/product-images/L21557-173/2.jpg,https://oleks-netizen.github.io/product-images/L21557-173/10.jpg,https://oleks-netizen.github.io/product-images/L21557-173/11.jpg,https://oleks-netizen.github.io/product-images/L21557-173/3.jpg,https://oleks-netizen.github.io/product-images/L21557-173/5.jpg,https://oleks-netizen.github.io/product-images/L21557-173/6.jpg,https://oleks-netizen.github.io/product-images/L21557-173/7.jpg,https://oleks-netizen.github.io/product-images/L21557-173/8.jpg,https://oleks-netizen.github.io/product-images/L21557-173/9.jpg</t>
         </is>
       </c>
       <c r="C308" t="n">
@@ -5156,7 +5156,7 @@
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22009-1/10.jpg,https://oleks-netizen.github.io/product-images/L22009-1/1.jpg,https://oleks-netizen.github.io/product-images/L22009-1/2.jpg,https://oleks-netizen.github.io/product-images/L22009-1/4.jpg,https://oleks-netizen.github.io/product-images/L22009-1/5.jpg,https://oleks-netizen.github.io/product-images/L22009-1/6.jpg,https://oleks-netizen.github.io/product-images/L22009-1/7.jpg,https://oleks-netizen.github.io/product-images/L22009-1/8.jpg,https://oleks-netizen.github.io/product-images/L22009-1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22009-1/1.jpg,https://oleks-netizen.github.io/product-images/L22009-1/2.jpg,https://oleks-netizen.github.io/product-images/L22009-1/10.jpg,https://oleks-netizen.github.io/product-images/L22009-1/4.jpg,https://oleks-netizen.github.io/product-images/L22009-1/5.jpg,https://oleks-netizen.github.io/product-images/L22009-1/6.jpg,https://oleks-netizen.github.io/product-images/L22009-1/7.jpg,https://oleks-netizen.github.io/product-images/L22009-1/8.jpg,https://oleks-netizen.github.io/product-images/L22009-1/9.jpg</t>
         </is>
       </c>
       <c r="C316" t="n">
@@ -5171,7 +5171,7 @@
       </c>
       <c r="B317" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22009-35/10.jpg,https://oleks-netizen.github.io/product-images/L22009-35/1.jpg,https://oleks-netizen.github.io/product-images/L22009-35/2.jpg,https://oleks-netizen.github.io/product-images/L22009-35/4.jpg,https://oleks-netizen.github.io/product-images/L22009-35/5.jpg,https://oleks-netizen.github.io/product-images/L22009-35/6.jpg,https://oleks-netizen.github.io/product-images/L22009-35/7.jpg,https://oleks-netizen.github.io/product-images/L22009-35/8.jpg,https://oleks-netizen.github.io/product-images/L22009-35/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22009-35/1.jpg,https://oleks-netizen.github.io/product-images/L22009-35/2.jpg,https://oleks-netizen.github.io/product-images/L22009-35/10.jpg,https://oleks-netizen.github.io/product-images/L22009-35/4.jpg,https://oleks-netizen.github.io/product-images/L22009-35/5.jpg,https://oleks-netizen.github.io/product-images/L22009-35/6.jpg,https://oleks-netizen.github.io/product-images/L22009-35/7.jpg,https://oleks-netizen.github.io/product-images/L22009-35/8.jpg,https://oleks-netizen.github.io/product-images/L22009-35/9.jpg</t>
         </is>
       </c>
       <c r="C317" t="n">
@@ -5231,7 +5231,7 @@
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22187-1W/10.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/1.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/2.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/4.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/5.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/6.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/7.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/8.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22187-1W/1.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/2.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/10.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/4.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/5.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/6.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/7.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/8.jpg,https://oleks-netizen.github.io/product-images/L22187-1W/9.jpg</t>
         </is>
       </c>
       <c r="C321" t="n">
@@ -5246,7 +5246,7 @@
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22187-1X/10.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/1.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/2.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/4.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/5.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/6.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/7.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/8.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22187-1X/1.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/2.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/10.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/4.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/5.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/6.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/7.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/8.jpg,https://oleks-netizen.github.io/product-images/L22187-1X/9.jpg</t>
         </is>
       </c>
       <c r="C322" t="n">
@@ -5261,7 +5261,7 @@
       </c>
       <c r="B323" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22322-01/10.jpg,https://oleks-netizen.github.io/product-images/L22322-01/1.jpg,https://oleks-netizen.github.io/product-images/L22322-01/2.jpg,https://oleks-netizen.github.io/product-images/L22322-01/4.jpg,https://oleks-netizen.github.io/product-images/L22322-01/5.jpg,https://oleks-netizen.github.io/product-images/L22322-01/6.jpg,https://oleks-netizen.github.io/product-images/L22322-01/7.jpg,https://oleks-netizen.github.io/product-images/L22322-01/8.jpg,https://oleks-netizen.github.io/product-images/L22322-01/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22322-01/1.jpg,https://oleks-netizen.github.io/product-images/L22322-01/2.jpg,https://oleks-netizen.github.io/product-images/L22322-01/10.jpg,https://oleks-netizen.github.io/product-images/L22322-01/4.jpg,https://oleks-netizen.github.io/product-images/L22322-01/5.jpg,https://oleks-netizen.github.io/product-images/L22322-01/6.jpg,https://oleks-netizen.github.io/product-images/L22322-01/7.jpg,https://oleks-netizen.github.io/product-images/L22322-01/8.jpg,https://oleks-netizen.github.io/product-images/L22322-01/9.jpg</t>
         </is>
       </c>
       <c r="C323" t="n">
@@ -5276,7 +5276,7 @@
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22322-02/10.jpg,https://oleks-netizen.github.io/product-images/L22322-02/1.jpg,https://oleks-netizen.github.io/product-images/L22322-02/2.jpg,https://oleks-netizen.github.io/product-images/L22322-02/4.jpg,https://oleks-netizen.github.io/product-images/L22322-02/5.jpg,https://oleks-netizen.github.io/product-images/L22322-02/6.jpg,https://oleks-netizen.github.io/product-images/L22322-02/7.jpg,https://oleks-netizen.github.io/product-images/L22322-02/8.jpg,https://oleks-netizen.github.io/product-images/L22322-02/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22322-02/1.jpg,https://oleks-netizen.github.io/product-images/L22322-02/2.jpg,https://oleks-netizen.github.io/product-images/L22322-02/10.jpg,https://oleks-netizen.github.io/product-images/L22322-02/4.jpg,https://oleks-netizen.github.io/product-images/L22322-02/5.jpg,https://oleks-netizen.github.io/product-images/L22322-02/6.jpg,https://oleks-netizen.github.io/product-images/L22322-02/7.jpg,https://oleks-netizen.github.io/product-images/L22322-02/8.jpg,https://oleks-netizen.github.io/product-images/L22322-02/9.jpg</t>
         </is>
       </c>
       <c r="C324" t="n">
@@ -5291,7 +5291,7 @@
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22322-1/10.jpg,https://oleks-netizen.github.io/product-images/L22322-1/1.jpg,https://oleks-netizen.github.io/product-images/L22322-1/2.jpg,https://oleks-netizen.github.io/product-images/L22322-1/4.jpg,https://oleks-netizen.github.io/product-images/L22322-1/5.jpg,https://oleks-netizen.github.io/product-images/L22322-1/6.jpg,https://oleks-netizen.github.io/product-images/L22322-1/7.jpg,https://oleks-netizen.github.io/product-images/L22322-1/8.jpg,https://oleks-netizen.github.io/product-images/L22322-1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22322-1/1.jpg,https://oleks-netizen.github.io/product-images/L22322-1/2.jpg,https://oleks-netizen.github.io/product-images/L22322-1/10.jpg,https://oleks-netizen.github.io/product-images/L22322-1/4.jpg,https://oleks-netizen.github.io/product-images/L22322-1/5.jpg,https://oleks-netizen.github.io/product-images/L22322-1/6.jpg,https://oleks-netizen.github.io/product-images/L22322-1/7.jpg,https://oleks-netizen.github.io/product-images/L22322-1/8.jpg,https://oleks-netizen.github.io/product-images/L22322-1/9.jpg</t>
         </is>
       </c>
       <c r="C325" t="n">
@@ -5306,7 +5306,7 @@
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22322-4/10.jpg,https://oleks-netizen.github.io/product-images/L22322-4/1.jpg,https://oleks-netizen.github.io/product-images/L22322-4/3.jpg,https://oleks-netizen.github.io/product-images/L22322-4/4.jpg,https://oleks-netizen.github.io/product-images/L22322-4/5.jpg,https://oleks-netizen.github.io/product-images/L22322-4/6.jpg,https://oleks-netizen.github.io/product-images/L22322-4/7.jpg,https://oleks-netizen.github.io/product-images/L22322-4/8.jpg,https://oleks-netizen.github.io/product-images/L22322-4/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22322-4/1.jpg,https://oleks-netizen.github.io/product-images/L22322-4/2.jpg,https://oleks-netizen.github.io/product-images/L22322-4/10.jpg,https://oleks-netizen.github.io/product-images/L22322-4/4.jpg,https://oleks-netizen.github.io/product-images/L22322-4/5.jpg,https://oleks-netizen.github.io/product-images/L22322-4/6.jpg,https://oleks-netizen.github.io/product-images/L22322-4/7.jpg,https://oleks-netizen.github.io/product-images/L22322-4/8.jpg,https://oleks-netizen.github.io/product-images/L22322-4/9.jpg</t>
         </is>
       </c>
       <c r="C326" t="n">
@@ -5486,7 +5486,7 @@
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L22902-1C/10.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/1.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/3.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/4.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/5.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/6.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/7.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/8.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L22902-1C/1.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/2.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/10.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/4.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/5.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/6.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/7.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/8.jpg,https://oleks-netizen.github.io/product-images/L22902-1C/9.jpg</t>
         </is>
       </c>
       <c r="C338" t="n">
@@ -5906,7 +5906,7 @@
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L9902-3C/10.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/11.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/12.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/1.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/2.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/4.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/5.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/6.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/7.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/8.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L9902-3C/1.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/2.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/3.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/10.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/11.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/4.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/5.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/6.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/7.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/8.jpg,https://oleks-netizen.github.io/product-images/L9902-3C/9.jpg</t>
         </is>
       </c>
       <c r="C366" t="n">
@@ -6191,7 +6191,7 @@
       </c>
       <c r="B385" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC47168-30/1.jpg,https://oleks-netizen.github.io/product-images/LC47168-30/3.jpg,https://oleks-netizen.github.io/product-images/LC47168-30/4.jpg,https://oleks-netizen.github.io/product-images/LC47168-30/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC47168-30/1.jpg,https://oleks-netizen.github.io/product-images/LC47168-30/2.jpg,https://oleks-netizen.github.io/product-images/LC47168-30/3.jpg,https://oleks-netizen.github.io/product-images/LC47168-30/5.jpg</t>
         </is>
       </c>
       <c r="C385" t="n">

</xml_diff>

<commit_message>
Auto update 2025-12-13 09:14:17
</commit_message>
<xml_diff>
--- a/articles_summary.xlsx
+++ b/articles_summary.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,102 +471,102 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>125v1genav37-black</t>
+          <t>14669</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/125v1genav37-black/1.jpg,https://oleks-netizen.github.io/product-images/125v1genav37-black/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14669/1.jpg,https://oleks-netizen.github.io/product-images/14669/14.jpg,https://oleks-netizen.github.io/product-images/14669/10.jpg,https://oleks-netizen.github.io/product-images/14669/11.jpg,https://oleks-netizen.github.io/product-images/14669/12.jpg,https://oleks-netizen.github.io/product-images/14669/13.jpg,https://oleks-netizen.github.io/product-images/14669/2.jpg,https://oleks-netizen.github.io/product-images/14669/3.jpg,https://oleks-netizen.github.io/product-images/14669/4.jpg,https://oleks-netizen.github.io/product-images/14669/5.jpg,https://oleks-netizen.github.io/product-images/14669/7.jpg,https://oleks-netizen.github.io/product-images/14669/8.jpg,https://oleks-netizen.github.io/product-images/14669/9.jpg</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>14669</t>
+          <t>20658</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14669/1.jpg,https://oleks-netizen.github.io/product-images/14669/14.jpg,https://oleks-netizen.github.io/product-images/14669/10.jpg,https://oleks-netizen.github.io/product-images/14669/11.jpg,https://oleks-netizen.github.io/product-images/14669/12.jpg,https://oleks-netizen.github.io/product-images/14669/13.jpg,https://oleks-netizen.github.io/product-images/14669/2.jpg,https://oleks-netizen.github.io/product-images/14669/3.jpg,https://oleks-netizen.github.io/product-images/14669/4.jpg,https://oleks-netizen.github.io/product-images/14669/5.jpg,https://oleks-netizen.github.io/product-images/14669/7.jpg,https://oleks-netizen.github.io/product-images/14669/8.jpg,https://oleks-netizen.github.io/product-images/14669/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20658/1.jpg,https://oleks-netizen.github.io/product-images/20658/10.jpg,https://oleks-netizen.github.io/product-images/20658/2.jpg,https://oleks-netizen.github.io/product-images/20658/3.jpg,https://oleks-netizen.github.io/product-images/20658/4.jpg,https://oleks-netizen.github.io/product-images/20658/5.jpg,https://oleks-netizen.github.io/product-images/20658/6.jpg,https://oleks-netizen.github.io/product-images/20658/7.jpg,https://oleks-netizen.github.io/product-images/20658/8.jpg,https://oleks-netizen.github.io/product-images/20658/9.jpg</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>20658</t>
+          <t>532660</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20658/1.jpg,https://oleks-netizen.github.io/product-images/20658/10.jpg,https://oleks-netizen.github.io/product-images/20658/2.jpg,https://oleks-netizen.github.io/product-images/20658/3.jpg,https://oleks-netizen.github.io/product-images/20658/4.jpg,https://oleks-netizen.github.io/product-images/20658/5.jpg,https://oleks-netizen.github.io/product-images/20658/6.jpg,https://oleks-netizen.github.io/product-images/20658/7.jpg,https://oleks-netizen.github.io/product-images/20658/8.jpg,https://oleks-netizen.github.io/product-images/20658/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/532660/1.jpg,https://oleks-netizen.github.io/product-images/532660/2.jpg,https://oleks-netizen.github.io/product-images/532660/3.jpg,https://oleks-netizen.github.io/product-images/532660/4.jpg,https://oleks-netizen.github.io/product-images/532660/5.jpg</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>532660</t>
+          <t>84045 BRN</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/532660/1.jpg,https://oleks-netizen.github.io/product-images/532660/2.jpg,https://oleks-netizen.github.io/product-images/532660/3.jpg,https://oleks-netizen.github.io/product-images/532660/4.jpg,https://oleks-netizen.github.io/product-images/532660/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/84045 BRN/1.jpg</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>84045 BRN</t>
+          <t>BN-BAG-33-iz</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/84045 BRN/1.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/1.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/2.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/3.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/4.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/5.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/6.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/7.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/8.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/9.jpg</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>BN-BAG-33-iz</t>
+          <t>BN-KLATCH-3-g-kr</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/1.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/2.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/3.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/4.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/5.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/6.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/7.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/8.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/10.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/1.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/2.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/3.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/4.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/5.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/6.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/7.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/8.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/9.jpg</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>BN-KLATCH-3-g-kr</t>
+          <t>BN-OP-7-3-k-kr</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/10.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/1.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/2.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/3.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/4.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/5.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/6.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/7.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/8.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/10.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/1.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/2.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/3.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/4.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/5.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/6.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/7.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/8.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/9.jpg</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -576,240 +576,225 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>BN-OP-7-3-k-kr</t>
+          <t>Cv1zk-153br-brown</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/10.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/1.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/2.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/3.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/4.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/5.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/6.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/7.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/8.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/Cv1zk-153br-brown/1.jpg,https://oleks-netizen.github.io/product-images/Cv1zk-153br-brown/2.jpg</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Cv1zk-153br-brown</t>
+          <t>K10122bl-black</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/Cv1zk-153br-brown/1.jpg,https://oleks-netizen.github.io/product-images/Cv1zk-153br-brown/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K10122bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K10122bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K10122bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K10122bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K10122bl-black/5.jpg,https://oleks-netizen.github.io/product-images/K10122bl-black/6.jpg</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>K10122bl-black</t>
+          <t>K17859-black</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K10122bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K10122bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K10122bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K10122bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K10122bl-black/5.jpg,https://oleks-netizen.github.io/product-images/K10122bl-black/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K17859-black/1.jpg,https://oleks-netizen.github.io/product-images/K17859-black/2.jpg,https://oleks-netizen.github.io/product-images/K17859-black/3.jpg,https://oleks-netizen.github.io/product-images/K17859-black/4.jpg,https://oleks-netizen.github.io/product-images/K17859-black/5.jpg,https://oleks-netizen.github.io/product-images/K17859-black/6.jpg,https://oleks-netizen.github.io/product-images/K17859-black/7.jpg,https://oleks-netizen.github.io/product-images/K17859-black/8.jpg</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>K17859-black</t>
+          <t>K18123bl-black</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K17859-black/1.jpg,https://oleks-netizen.github.io/product-images/K17859-black/2.jpg,https://oleks-netizen.github.io/product-images/K17859-black/3.jpg,https://oleks-netizen.github.io/product-images/K17859-black/4.jpg,https://oleks-netizen.github.io/product-images/K17859-black/5.jpg,https://oleks-netizen.github.io/product-images/K17859-black/6.jpg,https://oleks-netizen.github.io/product-images/K17859-black/7.jpg,https://oleks-netizen.github.io/product-images/K17859-black/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K18123bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K18123bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K18123bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K18123bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K18123bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>K18123bl-black</t>
+          <t>K49 CHESTNUT</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K18123bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K18123bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K18123bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K18123bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K18123bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K49 CHESTNUT/1.jpg,https://oleks-netizen.github.io/product-images/K49 CHESTNUT/2.jpg,https://oleks-netizen.github.io/product-images/K49 CHESTNUT/3.jpg,https://oleks-netizen.github.io/product-images/K49 CHESTNUT/4.jpg,https://oleks-netizen.github.io/product-images/K49 CHESTNUT/5.jpg,https://oleks-netizen.github.io/product-images/K49 CHESTNUT/6.jpg,https://oleks-netizen.github.io/product-images/K49 CHESTNUT/7.jpg</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>K49 CHESTNUT</t>
+          <t>L87202-F0</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K49 CHESTNUT/1.jpg,https://oleks-netizen.github.io/product-images/K49 CHESTNUT/2.jpg,https://oleks-netizen.github.io/product-images/K49 CHESTNUT/3.jpg,https://oleks-netizen.github.io/product-images/K49 CHESTNUT/4.jpg,https://oleks-netizen.github.io/product-images/K49 CHESTNUT/5.jpg,https://oleks-netizen.github.io/product-images/K49 CHESTNUT/6.jpg,https://oleks-netizen.github.io/product-images/K49 CHESTNUT/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L87202-F0/1.jpg,https://oleks-netizen.github.io/product-images/L87202-F0/2.jpg,https://oleks-netizen.github.io/product-images/L87202-F0/3.jpg,https://oleks-netizen.github.io/product-images/L87202-F0/4.jpg,https://oleks-netizen.github.io/product-images/L87202-F0/5.jpg,https://oleks-netizen.github.io/product-images/L87202-F0/6.jpg,https://oleks-netizen.github.io/product-images/L87202-F0/7.jpg,https://oleks-netizen.github.io/product-images/L87202-F0/8.jpg,https://oleks-netizen.github.io/product-images/L87202-F0/9.jpg</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>L87202-F0</t>
+          <t>L87606-1</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L87202-F0/1.jpg,https://oleks-netizen.github.io/product-images/L87202-F0/2.jpg,https://oleks-netizen.github.io/product-images/L87202-F0/3.jpg,https://oleks-netizen.github.io/product-images/L87202-F0/4.jpg,https://oleks-netizen.github.io/product-images/L87202-F0/5.jpg,https://oleks-netizen.github.io/product-images/L87202-F0/6.jpg,https://oleks-netizen.github.io/product-images/L87202-F0/7.jpg,https://oleks-netizen.github.io/product-images/L87202-F0/8.jpg,https://oleks-netizen.github.io/product-images/L87202-F0/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L87606-1/10.jpg,https://oleks-netizen.github.io/product-images/L87606-1/1.jpg,https://oleks-netizen.github.io/product-images/L87606-1/2.jpg,https://oleks-netizen.github.io/product-images/L87606-1/3.jpg,https://oleks-netizen.github.io/product-images/L87606-1/4.jpg,https://oleks-netizen.github.io/product-images/L87606-1/5.jpg,https://oleks-netizen.github.io/product-images/L87606-1/6.jpg,https://oleks-netizen.github.io/product-images/L87606-1/7.jpg,https://oleks-netizen.github.io/product-images/L87606-1/8.jpg,https://oleks-netizen.github.io/product-images/L87606-1/9.jpg</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>L87606-1</t>
+          <t>Lim-3992RH</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L87606-1/10.jpg,https://oleks-netizen.github.io/product-images/L87606-1/1.jpg,https://oleks-netizen.github.io/product-images/L87606-1/2.jpg,https://oleks-netizen.github.io/product-images/L87606-1/3.jpg,https://oleks-netizen.github.io/product-images/L87606-1/4.jpg,https://oleks-netizen.github.io/product-images/L87606-1/5.jpg,https://oleks-netizen.github.io/product-images/L87606-1/6.jpg,https://oleks-netizen.github.io/product-images/L87606-1/7.jpg,https://oleks-netizen.github.io/product-images/L87606-1/8.jpg,https://oleks-netizen.github.io/product-images/L87606-1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/Lim-3992RH/1.jpg,https://oleks-netizen.github.io/product-images/Lim-3992RH/2.jpg,https://oleks-netizen.github.io/product-images/Lim-3992RH/3.jpg,https://oleks-netizen.github.io/product-images/Lim-3992RH/4.jpg,https://oleks-netizen.github.io/product-images/Lim-3992RH/5.jpg,https://oleks-netizen.github.io/product-images/Lim-3992RH/6.jpg</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Lim-3992RH</t>
+          <t>RC-0010-4lx</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/Lim-3992RH/1.jpg,https://oleks-netizen.github.io/product-images/Lim-3992RH/2.jpg,https://oleks-netizen.github.io/product-images/Lim-3992RH/3.jpg,https://oleks-netizen.github.io/product-images/Lim-3992RH/4.jpg,https://oleks-netizen.github.io/product-images/Lim-3992RH/5.jpg,https://oleks-netizen.github.io/product-images/Lim-3992RH/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/RC-0010-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RC-0010-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RC-0010-4lx/3.jpg,https://oleks-netizen.github.io/product-images/RC-0010-4lx/4.jpg,https://oleks-netizen.github.io/product-images/RC-0010-4lx/5.jpg,https://oleks-netizen.github.io/product-images/RC-0010-4lx/6.jpg,https://oleks-netizen.github.io/product-images/RC-0010-4lx/7.jpg,https://oleks-netizen.github.io/product-images/RC-0010-4lx/8.jpg</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>RC-0010-4lx</t>
+          <t>T-B3142</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RC-0010-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RC-0010-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RC-0010-4lx/3.jpg,https://oleks-netizen.github.io/product-images/RC-0010-4lx/4.jpg,https://oleks-netizen.github.io/product-images/RC-0010-4lx/5.jpg,https://oleks-netizen.github.io/product-images/RC-0010-4lx/6.jpg,https://oleks-netizen.github.io/product-images/RC-0010-4lx/7.jpg,https://oleks-netizen.github.io/product-images/RC-0010-4lx/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/T-B3142/1.jpg,https://oleks-netizen.github.io/product-images/T-B3142/2.jpg,https://oleks-netizen.github.io/product-images/T-B3142/3.jpg,https://oleks-netizen.github.io/product-images/T-B3142/4.jpg</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>T-B3142</t>
+          <t>TW-Avenue-dark-beige-flo</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/T-B3142/1.jpg,https://oleks-netizen.github.io/product-images/T-B3142/2.jpg,https://oleks-netizen.github.io/product-images/T-B3142/3.jpg,https://oleks-netizen.github.io/product-images/T-B3142/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/10.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/1.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/2.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/3.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/4.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/5.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/6.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/7.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/8.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/9.jpg</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>TW-Avenue-dark-beige-flo</t>
+          <t>TW-Rubby-small-blue</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/10.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/1.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/2.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/3.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/4.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/5.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/6.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/7.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/8.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/TW-Rubby-small-blue/1.jpg,https://oleks-netizen.github.io/product-images/TW-Rubby-small-blue/2.jpg,https://oleks-netizen.github.io/product-images/TW-Rubby-small-blue/3.jpg,https://oleks-netizen.github.io/product-images/TW-Rubby-small-blue/4.jpg,https://oleks-netizen.github.io/product-images/TW-Rubby-small-blue/5.jpg,https://oleks-netizen.github.io/product-images/TW-Rubby-small-blue/6.jpg,https://oleks-netizen.github.io/product-images/TW-Rubby-small-blue/7.jpg,https://oleks-netizen.github.io/product-images/TW-Rubby-small-blue/8.jpg</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>TW-Rubby-small-blue</t>
+          <t>V1125FX02-black</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-Rubby-small-blue/1.jpg,https://oleks-netizen.github.io/product-images/TW-Rubby-small-blue/2.jpg,https://oleks-netizen.github.io/product-images/TW-Rubby-small-blue/3.jpg,https://oleks-netizen.github.io/product-images/TW-Rubby-small-blue/4.jpg,https://oleks-netizen.github.io/product-images/TW-Rubby-small-blue/5.jpg,https://oleks-netizen.github.io/product-images/TW-Rubby-small-blue/6.jpg,https://oleks-netizen.github.io/product-images/TW-Rubby-small-blue/7.jpg,https://oleks-netizen.github.io/product-images/TW-Rubby-small-blue/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/V1125FX02-black/1.jpg,https://oleks-netizen.github.io/product-images/V1125FX02-black/2.jpg</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>V1125FX02-black</t>
+          <t>V1T123-H33-BE-black</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/V1125FX02-black/1.jpg,https://oleks-netizen.github.io/product-images/V1125FX02-black/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/V1T123-H33-BE-black/1.jpg,https://oleks-netizen.github.io/product-images/V1T123-H33-BE-black/2.jpg,https://oleks-netizen.github.io/product-images/V1T123-H33-BE-black/3.jpg,https://oleks-netizen.github.io/product-images/V1T123-H33-BE-black/4.jpg,https://oleks-netizen.github.io/product-images/V1T123-H33-BE-black/5.jpg,https://oleks-netizen.github.io/product-images/V1T123-H33-BE-black/6.jpg</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>V1T123-H33-BE-black</t>
+          <t>VC02807cognac</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/V1T123-H33-BE-black/1.jpg,https://oleks-netizen.github.io/product-images/V1T123-H33-BE-black/2.jpg,https://oleks-netizen.github.io/product-images/V1T123-H33-BE-black/3.jpg,https://oleks-netizen.github.io/product-images/V1T123-H33-BE-black/4.jpg,https://oleks-netizen.github.io/product-images/V1T123-H33-BE-black/5.jpg,https://oleks-netizen.github.io/product-images/V1T123-H33-BE-black/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/VC02807cognac/10.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/1.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/2.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/3.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/4.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/5.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/6.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/7.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/8.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/9.jpg</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>VC02807cognac</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/VC02807cognac/10.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/1.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/2.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/3.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/4.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/5.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/6.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/7.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/8.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/9.jpg</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update 2025-12-17 07:58:20
</commit_message>
<xml_diff>
--- a/articles_summary.xlsx
+++ b/articles_summary.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,12 +441,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>11136</t>
+          <t>40236112</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/11136/1.jpg,https://oleks-netizen.github.io/product-images/11136/2.jpg,https://oleks-netizen.github.io/product-images/11136/3.jpg,https://oleks-netizen.github.io/product-images/11136/4.jpg,https://oleks-netizen.github.io/product-images/11136/5.jpg,https://oleks-netizen.github.io/product-images/11136/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/40236112/1.jpg,https://oleks-netizen.github.io/product-images/40236112/7.jpg,https://oleks-netizen.github.io/product-images/40236112/2.jpg,https://oleks-netizen.github.io/product-images/40236112/4.jpg,https://oleks-netizen.github.io/product-images/40236112/5.jpg,https://oleks-netizen.github.io/product-images/40236112/6.jpg</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -456,72 +456,72 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>11560</t>
+          <t>BN-GC-14-1-o-felt-d-Photoroom</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/11560/1.jpg,https://oleks-netizen.github.io/product-images/11560/10.jpg,https://oleks-netizen.github.io/product-images/11560/11.jpg,https://oleks-netizen.github.io/product-images/11560/2.jpg,https://oleks-netizen.github.io/product-images/11560/3.jpg,https://oleks-netizen.github.io/product-images/11560/4.jpg,https://oleks-netizen.github.io/product-images/11560/5.jpg,https://oleks-netizen.github.io/product-images/11560/6.jpg,https://oleks-netizen.github.io/product-images/11560/7.jpg,https://oleks-netizen.github.io/product-images/11560/8.jpg,https://oleks-netizen.github.io/product-images/11560/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BN-GC-14-1-o-felt-d-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/BN-GC-14-1-o-felt-d-Photoroom/2.jpg,https://oleks-netizen.github.io/product-images/BN-GC-14-1-o-felt-d-Photoroom/3.jpg</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>14669</t>
+          <t>BN-GC-14-1-o-felt-d</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14669/1.jpg,https://oleks-netizen.github.io/product-images/14669/14.jpg,https://oleks-netizen.github.io/product-images/14669/10.jpg,https://oleks-netizen.github.io/product-images/14669/11.jpg,https://oleks-netizen.github.io/product-images/14669/12.jpg,https://oleks-netizen.github.io/product-images/14669/13.jpg,https://oleks-netizen.github.io/product-images/14669/2.jpg,https://oleks-netizen.github.io/product-images/14669/3.jpg,https://oleks-netizen.github.io/product-images/14669/4.jpg,https://oleks-netizen.github.io/product-images/14669/5.jpg,https://oleks-netizen.github.io/product-images/14669/7.jpg,https://oleks-netizen.github.io/product-images/14669/8.jpg,https://oleks-netizen.github.io/product-images/14669/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BN-GC-14-1-o-felt-d/6.jpg</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>20658</t>
+          <t>BN-GC-16-1-o-felt-d-Photoroom</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20658/1.jpg,https://oleks-netizen.github.io/product-images/20658/10.jpg,https://oleks-netizen.github.io/product-images/20658/2.jpg,https://oleks-netizen.github.io/product-images/20658/3.jpg,https://oleks-netizen.github.io/product-images/20658/4.jpg,https://oleks-netizen.github.io/product-images/20658/5.jpg,https://oleks-netizen.github.io/product-images/20658/6.jpg,https://oleks-netizen.github.io/product-images/20658/7.jpg,https://oleks-netizen.github.io/product-images/20658/8.jpg,https://oleks-netizen.github.io/product-images/20658/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BN-GC-16-1-o-felt-d-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/BN-GC-16-1-o-felt-d-Photoroom/2.jpg,https://oleks-netizen.github.io/product-images/BN-GC-16-1-o-felt-d-Photoroom/3.jpg</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>532660</t>
+          <t>BN-GC-16-1-o-felt-d</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/532660/1.jpg,https://oleks-netizen.github.io/product-images/532660/2.jpg,https://oleks-netizen.github.io/product-images/532660/3.jpg,https://oleks-netizen.github.io/product-images/532660/4.jpg,https://oleks-netizen.github.io/product-images/532660/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BN-GC-16-1-o-felt-d/6.jpg</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>84045 BRN</t>
+          <t>BN-OP-12-g-kr</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/84045 BRN/1.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BN-OP-12-g-kr/1.jpg</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -531,237 +531,237 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BN-BAG-33-iz</t>
+          <t>BN-OP-12-g-kr-Photoroom</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/1.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/2.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/3.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/4.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/5.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/6.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/7.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/8.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-33-iz/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BN-OP-12-g-kr-Photoroom/2.jpg,https://oleks-netizen.github.io/product-images/BN-OP-12-g-kr-Photoroom/3.jpg</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>BN-KLATCH-3-g-kr</t>
+          <t>BN-SB-13-k</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/10.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/1.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/2.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/3.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/4.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/5.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/6.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/7.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/8.jpg,https://oleks-netizen.github.io/product-images/BN-KLATCH-3-g-kr/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BN-SB-13-k/1.jpg</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>BN-OP-7-3-k-kr</t>
+          <t>BN-SB-13-k-Photoroom</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/10.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/1.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/2.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/3.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/4.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/5.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/6.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/7.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/8.jpg,https://oleks-netizen.github.io/product-images/BN-OP-7-3-k-kr/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BN-SB-13-k-Photoroom/2.jpg,https://oleks-netizen.github.io/product-images/BN-SB-13-k-Photoroom/3.jpg</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Cv1zk-153br-brown</t>
+          <t>BN-SB-13-vin</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/Cv1zk-153br-brown/1.jpg,https://oleks-netizen.github.io/product-images/Cv1zk-153br-brown/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BN-SB-13-vin/1.jpg</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>K10122bl-black</t>
+          <t>BN-SB-13-vin-Photoroom</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K10122bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K10122bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K10122bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K10122bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K10122bl-black/5.jpg,https://oleks-netizen.github.io/product-images/K10122bl-black/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BN-SB-13-vin-Photoroom/2.jpg,https://oleks-netizen.github.io/product-images/BN-SB-13-vin-Photoroom/3.jpg</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>K17859-black</t>
+          <t>BN-SB-6_073926907251</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K17859-black/1.jpg,https://oleks-netizen.github.io/product-images/K17859-black/2.jpg,https://oleks-netizen.github.io/product-images/K17859-black/3.jpg,https://oleks-netizen.github.io/product-images/K17859-black/4.jpg,https://oleks-netizen.github.io/product-images/K17859-black/5.jpg,https://oleks-netizen.github.io/product-images/K17859-black/6.jpg,https://oleks-netizen.github.io/product-images/K17859-black/7.jpg,https://oleks-netizen.github.io/product-images/K17859-black/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BN-SB-6_073926907251/1.jpg</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>K18123bl-black</t>
+          <t>BN-SB-6_073926337432-Photoroom</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K18123bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K18123bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K18123bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K18123bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K18123bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BN-SB-6_073926337432-Photoroom/2.jpg</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>K49 CHESTNUT</t>
+          <t>BN-SB-6_073926493725-Photoroom</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K49 CHESTNUT/1.jpg,https://oleks-netizen.github.io/product-images/K49 CHESTNUT/2.jpg,https://oleks-netizen.github.io/product-images/K49 CHESTNUT/3.jpg,https://oleks-netizen.github.io/product-images/K49 CHESTNUT/4.jpg,https://oleks-netizen.github.io/product-images/K49 CHESTNUT/5.jpg,https://oleks-netizen.github.io/product-images/K49 CHESTNUT/6.jpg,https://oleks-netizen.github.io/product-images/K49 CHESTNUT/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BN-SB-6_073926493725-Photoroom/3.jpg</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>L87202-F0</t>
+          <t>BN-SB-6_073926689097-Photoroom</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L87202-F0/1.jpg,https://oleks-netizen.github.io/product-images/L87202-F0/2.jpg,https://oleks-netizen.github.io/product-images/L87202-F0/3.jpg,https://oleks-netizen.github.io/product-images/L87202-F0/4.jpg,https://oleks-netizen.github.io/product-images/L87202-F0/5.jpg,https://oleks-netizen.github.io/product-images/L87202-F0/6.jpg,https://oleks-netizen.github.io/product-images/L87202-F0/7.jpg,https://oleks-netizen.github.io/product-images/L87202-F0/8.jpg,https://oleks-netizen.github.io/product-images/L87202-F0/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BN-SB-6_073926689097-Photoroom/4.jpg</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>L87606-1</t>
+          <t>HB10032_3044</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L87606-1/10.jpg,https://oleks-netizen.github.io/product-images/L87606-1/1.jpg,https://oleks-netizen.github.io/product-images/L87606-1/2.jpg,https://oleks-netizen.github.io/product-images/L87606-1/3.jpg,https://oleks-netizen.github.io/product-images/L87606-1/4.jpg,https://oleks-netizen.github.io/product-images/L87606-1/5.jpg,https://oleks-netizen.github.io/product-images/L87606-1/6.jpg,https://oleks-netizen.github.io/product-images/L87606-1/7.jpg,https://oleks-netizen.github.io/product-images/L87606-1/8.jpg,https://oleks-netizen.github.io/product-images/L87606-1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/HB10032_3044/1.jpg,https://oleks-netizen.github.io/product-images/HB10032_3044/5.jpg,https://oleks-netizen.github.io/product-images/HB10032_3044/3.jpg,https://oleks-netizen.github.io/product-images/HB10032_3044/4.jpg</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Lim-3992RH</t>
+          <t>RB63 LIME M</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/Lim-3992RH/1.jpg,https://oleks-netizen.github.io/product-images/Lim-3992RH/2.jpg,https://oleks-netizen.github.io/product-images/Lim-3992RH/3.jpg,https://oleks-netizen.github.io/product-images/Lim-3992RH/4.jpg,https://oleks-netizen.github.io/product-images/Lim-3992RH/5.jpg,https://oleks-netizen.github.io/product-images/Lim-3992RH/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/RB63 LIME M/1.jpg,https://oleks-netizen.github.io/product-images/RB63 LIME M/5.jpg,https://oleks-netizen.github.io/product-images/RB63 LIME M/2.jpg,https://oleks-netizen.github.io/product-images/RB63 LIME M/3.jpg</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>RC-0010-4lx</t>
+          <t>TW-PH-beige-ksr</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RC-0010-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RC-0010-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RC-0010-4lx/3.jpg,https://oleks-netizen.github.io/product-images/RC-0010-4lx/4.jpg,https://oleks-netizen.github.io/product-images/RC-0010-4lx/5.jpg,https://oleks-netizen.github.io/product-images/RC-0010-4lx/6.jpg,https://oleks-netizen.github.io/product-images/RC-0010-4lx/7.jpg,https://oleks-netizen.github.io/product-images/RC-0010-4lx/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/TW-PH-beige-ksr/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-beige-ksr/3.jpg</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>T-B3142</t>
+          <t>TW-PH-black-ksr-Photoroom</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/T-B3142/1.jpg,https://oleks-netizen.github.io/product-images/T-B3142/2.jpg,https://oleks-netizen.github.io/product-images/T-B3142/3.jpg,https://oleks-netizen.github.io/product-images/T-B3142/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/TW-PH-black-ksr-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-black-ksr-Photoroom/4.jpg</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>TW-Avenue-dark-beige-flo</t>
+          <t>TW-PH-black-ksr</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/10.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/1.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/2.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/3.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/4.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/5.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/6.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/7.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/8.jpg,https://oleks-netizen.github.io/product-images/TW-Avenue-dark-beige-flo/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/TW-PH-black-ksr/6.jpg,https://oleks-netizen.github.io/product-images/TW-PH-black-ksr/3.jpg,https://oleks-netizen.github.io/product-images/TW-PH-black-ksr/5.jpg</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>TW-Rubby-small-blue</t>
+          <t>TW-PH-dark-blue</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-Rubby-small-blue/1.jpg,https://oleks-netizen.github.io/product-images/TW-Rubby-small-blue/2.jpg,https://oleks-netizen.github.io/product-images/TW-Rubby-small-blue/3.jpg,https://oleks-netizen.github.io/product-images/TW-Rubby-small-blue/4.jpg,https://oleks-netizen.github.io/product-images/TW-Rubby-small-blue/5.jpg,https://oleks-netizen.github.io/product-images/TW-Rubby-small-blue/6.jpg,https://oleks-netizen.github.io/product-images/TW-Rubby-small-blue/7.jpg,https://oleks-netizen.github.io/product-images/TW-Rubby-small-blue/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/TW-PH-dark-blue/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-dark-blue/3.jpg</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>V1125FX02-black</t>
+          <t>TW-PH-kon-crz</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/V1125FX02-black/1.jpg,https://oleks-netizen.github.io/product-images/V1125FX02-black/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/TW-PH-kon-crz/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-kon-crz/3.jpg</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -771,31 +771,46 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>V1T123-H33-BE-black</t>
+          <t>TW-PH-kon-ksr</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/V1T123-H33-BE-black/1.jpg,https://oleks-netizen.github.io/product-images/V1T123-H33-BE-black/2.jpg,https://oleks-netizen.github.io/product-images/V1T123-H33-BE-black/3.jpg,https://oleks-netizen.github.io/product-images/V1T123-H33-BE-black/4.jpg,https://oleks-netizen.github.io/product-images/V1T123-H33-BE-black/5.jpg,https://oleks-netizen.github.io/product-images/V1T123-H33-BE-black/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/TW-PH-kon-ksr/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-kon-ksr/3.jpg</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>VC02807cognac</t>
+          <t>TW-PH-mars-ksr</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/VC02807cognac/10.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/1.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/2.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/3.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/4.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/5.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/6.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/7.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/8.jpg,https://oleks-netizen.github.io/product-images/VC02807cognac/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/TW-PH-mars-ksr/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-mars-ksr/3.jpg</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>10</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>TW-PH-red-saf</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-PH-red-saf/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-red-saf/3.jpg</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update 2025-12-17 08:06:12
</commit_message>
<xml_diff>
--- a/articles_summary.xlsx
+++ b/articles_summary.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,376 +441,31 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>40236112</t>
+          <t>BN-GC-14-1-o-felt-d-Photoroom</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/40236112/1.jpg,https://oleks-netizen.github.io/product-images/40236112/7.jpg,https://oleks-netizen.github.io/product-images/40236112/2.jpg,https://oleks-netizen.github.io/product-images/40236112/4.jpg,https://oleks-netizen.github.io/product-images/40236112/5.jpg,https://oleks-netizen.github.io/product-images/40236112/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BN-GC-14-1-o-felt-d-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/BN-GC-14-1-o-felt-d-Photoroom/2.jpg,https://oleks-netizen.github.io/product-images/BN-GC-14-1-o-felt-d-Photoroom/3.jpg</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BN-GC-14-1-o-felt-d-Photoroom</t>
+          <t>BN-GC-14-1-o-felt-d</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-GC-14-1-o-felt-d-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/BN-GC-14-1-o-felt-d-Photoroom/2.jpg,https://oleks-netizen.github.io/product-images/BN-GC-14-1-o-felt-d-Photoroom/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BN-GC-14-1-o-felt-d/6.jpg</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>BN-GC-14-1-o-felt-d</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-GC-14-1-o-felt-d/6.jpg</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
         <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>BN-GC-16-1-o-felt-d-Photoroom</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-GC-16-1-o-felt-d-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/BN-GC-16-1-o-felt-d-Photoroom/2.jpg,https://oleks-netizen.github.io/product-images/BN-GC-16-1-o-felt-d-Photoroom/3.jpg</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>BN-GC-16-1-o-felt-d</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-GC-16-1-o-felt-d/6.jpg</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>BN-OP-12-g-kr</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-OP-12-g-kr/1.jpg</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>BN-OP-12-g-kr-Photoroom</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-OP-12-g-kr-Photoroom/2.jpg,https://oleks-netizen.github.io/product-images/BN-OP-12-g-kr-Photoroom/3.jpg</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>BN-SB-13-k</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-SB-13-k/1.jpg</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>BN-SB-13-k-Photoroom</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-SB-13-k-Photoroom/2.jpg,https://oleks-netizen.github.io/product-images/BN-SB-13-k-Photoroom/3.jpg</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>BN-SB-13-vin</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-SB-13-vin/1.jpg</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>BN-SB-13-vin-Photoroom</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-SB-13-vin-Photoroom/2.jpg,https://oleks-netizen.github.io/product-images/BN-SB-13-vin-Photoroom/3.jpg</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>BN-SB-6_073926907251</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-SB-6_073926907251/1.jpg</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>BN-SB-6_073926337432-Photoroom</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-SB-6_073926337432-Photoroom/2.jpg</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>BN-SB-6_073926493725-Photoroom</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-SB-6_073926493725-Photoroom/3.jpg</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>BN-SB-6_073926689097-Photoroom</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-SB-6_073926689097-Photoroom/4.jpg</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>HB10032_3044</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/HB10032_3044/1.jpg,https://oleks-netizen.github.io/product-images/HB10032_3044/5.jpg,https://oleks-netizen.github.io/product-images/HB10032_3044/3.jpg,https://oleks-netizen.github.io/product-images/HB10032_3044/4.jpg</t>
-        </is>
-      </c>
-      <c r="C17" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>RB63 LIME M</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/RB63 LIME M/1.jpg,https://oleks-netizen.github.io/product-images/RB63 LIME M/5.jpg,https://oleks-netizen.github.io/product-images/RB63 LIME M/2.jpg,https://oleks-netizen.github.io/product-images/RB63 LIME M/3.jpg</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>TW-PH-beige-ksr</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-PH-beige-ksr/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-beige-ksr/3.jpg</t>
-        </is>
-      </c>
-      <c r="C19" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>TW-PH-black-ksr-Photoroom</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-PH-black-ksr-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-black-ksr-Photoroom/4.jpg</t>
-        </is>
-      </c>
-      <c r="C20" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>TW-PH-black-ksr</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-PH-black-ksr/6.jpg,https://oleks-netizen.github.io/product-images/TW-PH-black-ksr/3.jpg,https://oleks-netizen.github.io/product-images/TW-PH-black-ksr/5.jpg</t>
-        </is>
-      </c>
-      <c r="C21" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>TW-PH-dark-blue</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-PH-dark-blue/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-dark-blue/3.jpg</t>
-        </is>
-      </c>
-      <c r="C22" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>TW-PH-kon-crz</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-PH-kon-crz/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-kon-crz/3.jpg</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>TW-PH-kon-ksr</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-PH-kon-ksr/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-kon-ksr/3.jpg</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>TW-PH-mars-ksr</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-PH-mars-ksr/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-mars-ksr/3.jpg</t>
-        </is>
-      </c>
-      <c r="C25" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>TW-PH-red-saf</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-PH-red-saf/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-red-saf/3.jpg</t>
-        </is>
-      </c>
-      <c r="C26" t="n">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update 2025-12-17 08:44:01
</commit_message>
<xml_diff>
--- a/articles_summary.xlsx
+++ b/articles_summary.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,16 +441,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BN-GC-14-1-o-felt-d-Photoroom</t>
+          <t>40236112</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-GC-14-1-o-felt-d-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/BN-GC-14-1-o-felt-d-Photoroom/2.jpg,https://oleks-netizen.github.io/product-images/BN-GC-14-1-o-felt-d-Photoroom/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/40236112/1.jpg,https://oleks-netizen.github.io/product-images/40236112/7.jpg,https://oleks-netizen.github.io/product-images/40236112/2.jpg,https://oleks-netizen.github.io/product-images/40236112/4.jpg,https://oleks-netizen.github.io/product-images/40236112/5.jpg,https://oleks-netizen.github.io/product-images/40236112/6.jpg</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -461,11 +461,266 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-GC-14-1-o-felt-d/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BN-GC-14-1-o-felt-d/1.jpg,https://oleks-netizen.github.io/product-images/BN-GC-14-1-o-felt-d/2.jpg,https://oleks-netizen.github.io/product-images/BN-GC-14-1-o-felt-d/3.jpg,https://oleks-netizen.github.io/product-images/BN-GC-14-1-o-felt-d/6.jpg</t>
         </is>
       </c>
       <c r="C3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>BN-GC-16-1-o-felt-d</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/BN-GC-16-1-o-felt-d/1.jpg,https://oleks-netizen.github.io/product-images/BN-GC-16-1-o-felt-d/2.jpg,https://oleks-netizen.github.io/product-images/BN-GC-16-1-o-felt-d/3.jpg,https://oleks-netizen.github.io/product-images/BN-GC-16-1-o-felt-d/6.jpg</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>BN-OP-12-g-kr</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/BN-OP-12-g-kr/1.jpg,https://oleks-netizen.github.io/product-images/BN-OP-12-g-kr/2.jpg,https://oleks-netizen.github.io/product-images/BN-OP-12-g-kr/3.jpg</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>BN-SB-13-k</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/BN-SB-13-k/1.jpg,https://oleks-netizen.github.io/product-images/BN-SB-13-k/2.jpg,https://oleks-netizen.github.io/product-images/BN-SB-13-k/3.jpg</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>BN-SB-13-vin</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/BN-SB-13-vin/1.jpg,https://oleks-netizen.github.io/product-images/BN-SB-13-vin/2.jpg,https://oleks-netizen.github.io/product-images/BN-SB-13-vin/3.jpg</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>BN-SB-6_073926907251</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/BN-SB-6_073926907251/1.jpg</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>BN-SB-6_073926337432</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/BN-SB-6_073926337432/2.jpg</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>BN-SB-6_073926493725</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/BN-SB-6_073926493725/3.jpg</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>BN-SB-6_073926689097</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/BN-SB-6_073926689097/4.jpg</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>HB10032_3044</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/HB10032_3044/1.jpg,https://oleks-netizen.github.io/product-images/HB10032_3044/5.jpg,https://oleks-netizen.github.io/product-images/HB10032_3044/3.jpg,https://oleks-netizen.github.io/product-images/HB10032_3044/4.jpg</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>RB63 LIME M</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/RB63 LIME M/1.jpg,https://oleks-netizen.github.io/product-images/RB63 LIME M/5.jpg,https://oleks-netizen.github.io/product-images/RB63 LIME M/2.jpg,https://oleks-netizen.github.io/product-images/RB63 LIME M/3.jpg</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>TW-PH-beige-ksr</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-PH-beige-ksr/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-beige-ksr/3.jpg</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>TW-PH-black-ksr</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-PH-black-ksr/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-black-ksr/6.jpg,https://oleks-netizen.github.io/product-images/TW-PH-black-ksr/3.jpg,https://oleks-netizen.github.io/product-images/TW-PH-black-ksr/4.jpg,https://oleks-netizen.github.io/product-images/TW-PH-black-ksr/5.jpg</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>TW-PH-dark-blue</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-PH-dark-blue/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-dark-blue/3.jpg</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>TW-PH-kon-crz</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-PH-kon-crz/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-kon-crz/3.jpg</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>TW-PH-kon-ksr</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-PH-kon-ksr/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-kon-ksr/3.jpg</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>TW-PH-mars-ksr</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-PH-mars-ksr/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-mars-ksr/3.jpg</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>TW-PH-red-saf</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-PH-red-saf/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-red-saf/3.jpg</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update 2025-12-21 19:47:09
</commit_message>
<xml_diff>
--- a/articles_summary.xlsx
+++ b/articles_summary.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,42 +441,42 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>40236112</t>
+          <t>1733_1_1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/40236112/1.jpg,https://oleks-netizen.github.io/product-images/40236112/7.jpg,https://oleks-netizen.github.io/product-images/40236112/2.jpg,https://oleks-netizen.github.io/product-images/40236112/4.jpg,https://oleks-netizen.github.io/product-images/40236112/5.jpg,https://oleks-netizen.github.io/product-images/40236112/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/1733_1_1/1.jpg</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BN-GC-14-1-o-felt-d</t>
+          <t>206120</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-GC-14-1-o-felt-d/1.jpg,https://oleks-netizen.github.io/product-images/BN-GC-14-1-o-felt-d/2.jpg,https://oleks-netizen.github.io/product-images/BN-GC-14-1-o-felt-d/3.jpg,https://oleks-netizen.github.io/product-images/BN-GC-14-1-o-felt-d/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/206120/1.jpg,https://oleks-netizen.github.io/product-images/206120/2.jpg</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BN-GC-16-1-o-felt-d</t>
+          <t>224420</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-GC-16-1-o-felt-d/1.jpg,https://oleks-netizen.github.io/product-images/BN-GC-16-1-o-felt-d/2.jpg,https://oleks-netizen.github.io/product-images/BN-GC-16-1-o-felt-d/3.jpg,https://oleks-netizen.github.io/product-images/BN-GC-16-1-o-felt-d/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/224420/1.jpg,https://oleks-netizen.github.io/product-images/224420/5.jpg,https://oleks-netizen.github.io/product-images/224420/2.jpg,https://oleks-netizen.github.io/product-images/224420/3.jpg</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -486,42 +486,42 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BN-OP-12-g-kr</t>
+          <t>2459_1_6</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-OP-12-g-kr/1.jpg,https://oleks-netizen.github.io/product-images/BN-OP-12-g-kr/2.jpg,https://oleks-netizen.github.io/product-images/BN-OP-12-g-kr/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/2459_1_6/1.jpg</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BN-SB-13-k</t>
+          <t>30127445</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-SB-13-k/1.jpg,https://oleks-netizen.github.io/product-images/BN-SB-13-k/2.jpg,https://oleks-netizen.github.io/product-images/BN-SB-13-k/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/30127445/1.jpg,https://oleks-netizen.github.io/product-images/30127445/2.jpg,https://oleks-netizen.github.io/product-images/30127445/3.jpg,https://oleks-netizen.github.io/product-images/30127445/4.jpg,https://oleks-netizen.github.io/product-images/30127445/5.jpg</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BN-SB-13-vin</t>
+          <t>303660</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-SB-13-vin/1.jpg,https://oleks-netizen.github.io/product-images/BN-SB-13-vin/2.jpg,https://oleks-netizen.github.io/product-images/BN-SB-13-vin/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/303660/1.jpg,https://oleks-netizen.github.io/product-images/303660/4.jpg,https://oleks-netizen.github.io/product-images/303660/3.jpg</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -531,196 +531,1666 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BN-SB-6_073926907251</t>
+          <t>5210401</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-SB-6_073926907251/1.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/5210401/1.jpg,https://oleks-netizen.github.io/product-images/5210401/10.jpg,https://oleks-netizen.github.io/product-images/5210401/2.jpg,https://oleks-netizen.github.io/product-images/5210401/3.jpg,https://oleks-netizen.github.io/product-images/5210401/4.jpg,https://oleks-netizen.github.io/product-images/5210401/5.jpg,https://oleks-netizen.github.io/product-images/5210401/6.jpg,https://oleks-netizen.github.io/product-images/5210401/7.jpg,https://oleks-netizen.github.io/product-images/5210401/8.jpg,https://oleks-netizen.github.io/product-images/5210401/9.jpg</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>BN-SB-6_073926337432</t>
+          <t>5218101</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-SB-6_073926337432/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/5218101/1.jpg,https://oleks-netizen.github.io/product-images/5218101/11.jpg,https://oleks-netizen.github.io/product-images/5218101/10.jpg,https://oleks-netizen.github.io/product-images/5218101/2.jpg,https://oleks-netizen.github.io/product-images/5218101/3.jpg,https://oleks-netizen.github.io/product-images/5218101/5.jpg,https://oleks-netizen.github.io/product-images/5218101/6.jpg,https://oleks-netizen.github.io/product-images/5218101/7.jpg,https://oleks-netizen.github.io/product-images/5218101/8.jpg,https://oleks-netizen.github.io/product-images/5218101/9.jpg</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>BN-SB-6_073926493725</t>
+          <t>5221401</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-SB-6_073926493725/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/5221401/1.jpg,https://oleks-netizen.github.io/product-images/5221401/11.jpg,https://oleks-netizen.github.io/product-images/5221401/10.jpg,https://oleks-netizen.github.io/product-images/5221401/3.jpg,https://oleks-netizen.github.io/product-images/5221401/4.jpg,https://oleks-netizen.github.io/product-images/5221401/5.jpg,https://oleks-netizen.github.io/product-images/5221401/6.jpg,https://oleks-netizen.github.io/product-images/5221401/7.jpg,https://oleks-netizen.github.io/product-images/5221401/8.jpg,https://oleks-netizen.github.io/product-images/5221401/9.jpg</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>BN-SB-6_073926689097</t>
+          <t>5225501</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-SB-6_073926689097/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/5225501/1.jpg,https://oleks-netizen.github.io/product-images/5225501/11.jpg,https://oleks-netizen.github.io/product-images/5225501/10.jpg,https://oleks-netizen.github.io/product-images/5225501/3.jpg,https://oleks-netizen.github.io/product-images/5225501/4.jpg,https://oleks-netizen.github.io/product-images/5225501/5.jpg,https://oleks-netizen.github.io/product-images/5225501/6.jpg,https://oleks-netizen.github.io/product-images/5225501/7.jpg,https://oleks-netizen.github.io/product-images/5225501/8.jpg,https://oleks-netizen.github.io/product-images/5225501/9.jpg</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>HB10032_3044</t>
+          <t>522623</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/HB10032_3044/1.jpg,https://oleks-netizen.github.io/product-images/HB10032_3044/5.jpg,https://oleks-netizen.github.io/product-images/HB10032_3044/3.jpg,https://oleks-netizen.github.io/product-images/HB10032_3044/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/522623/1.jpg,https://oleks-netizen.github.io/product-images/522623/2.jpg</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>RB63 LIME M</t>
+          <t>522660</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RB63 LIME M/1.jpg,https://oleks-netizen.github.io/product-images/RB63 LIME M/5.jpg,https://oleks-netizen.github.io/product-images/RB63 LIME M/2.jpg,https://oleks-netizen.github.io/product-images/RB63 LIME M/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/522660/1.jpg,https://oleks-netizen.github.io/product-images/522660/2.jpg</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>TW-PH-beige-ksr</t>
+          <t>5241901</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-PH-beige-ksr/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-beige-ksr/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/5241901/1.jpg,https://oleks-netizen.github.io/product-images/5241901/10.jpg,https://oleks-netizen.github.io/product-images/5241901/2.jpg,https://oleks-netizen.github.io/product-images/5241901/3.jpg,https://oleks-netizen.github.io/product-images/5241901/4.jpg,https://oleks-netizen.github.io/product-images/5241901/5.jpg,https://oleks-netizen.github.io/product-images/5241901/6.jpg,https://oleks-netizen.github.io/product-images/5241901/7.jpg,https://oleks-netizen.github.io/product-images/5241901/8.jpg,https://oleks-netizen.github.io/product-images/5241901/9.jpg</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>TW-PH-black-ksr</t>
+          <t>5244701</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-PH-black-ksr/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-black-ksr/6.jpg,https://oleks-netizen.github.io/product-images/TW-PH-black-ksr/3.jpg,https://oleks-netizen.github.io/product-images/TW-PH-black-ksr/4.jpg,https://oleks-netizen.github.io/product-images/TW-PH-black-ksr/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/5244701/1.jpg,https://oleks-netizen.github.io/product-images/5244701/11.jpg,https://oleks-netizen.github.io/product-images/5244701/10.jpg,https://oleks-netizen.github.io/product-images/5244701/3.jpg,https://oleks-netizen.github.io/product-images/5244701/4.jpg,https://oleks-netizen.github.io/product-images/5244701/5.jpg,https://oleks-netizen.github.io/product-images/5244701/6.jpg,https://oleks-netizen.github.io/product-images/5244701/7.jpg,https://oleks-netizen.github.io/product-images/5244701/8.jpg,https://oleks-netizen.github.io/product-images/5244701/9.jpg</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>TW-PH-dark-blue</t>
+          <t>62725</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-PH-dark-blue/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-dark-blue/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/62725/1.jpg,https://oleks-netizen.github.io/product-images/62725/8.jpg,https://oleks-netizen.github.io/product-images/62725/2.jpg,https://oleks-netizen.github.io/product-images/62725/4.jpg,https://oleks-netizen.github.io/product-images/62725/5.jpg,https://oleks-netizen.github.io/product-images/62725/6.jpg,https://oleks-netizen.github.io/product-images/62725/7.jpg</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>TW-PH-kon-crz</t>
+          <t>62726</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-PH-kon-crz/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-kon-crz/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/62726/1.jpg,https://oleks-netizen.github.io/product-images/62726/8.jpg,https://oleks-netizen.github.io/product-images/62726/2.jpg,https://oleks-netizen.github.io/product-images/62726/4.jpg,https://oleks-netizen.github.io/product-images/62726/5.jpg,https://oleks-netizen.github.io/product-images/62726/6.jpg,https://oleks-netizen.github.io/product-images/62726/7.jpg</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>TW-PH-kon-ksr</t>
+          <t>62727</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-PH-kon-ksr/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-kon-ksr/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/62727/1.jpg,https://oleks-netizen.github.io/product-images/62727/8.jpg,https://oleks-netizen.github.io/product-images/62727/2.jpg,https://oleks-netizen.github.io/product-images/62727/4.jpg,https://oleks-netizen.github.io/product-images/62727/5.jpg,https://oleks-netizen.github.io/product-images/62727/6.jpg,https://oleks-netizen.github.io/product-images/62727/7.jpg</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>TW-PH-mars-ksr</t>
+          <t>701661</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-PH-mars-ksr/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-mars-ksr/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/701661/1.jpg,https://oleks-netizen.github.io/product-images/701661/2.jpg,https://oleks-netizen.github.io/product-images/701661/3.jpg,https://oleks-netizen.github.io/product-images/701661/4.jpg</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>TW-PH-red-saf</t>
+          <t>746710</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-PH-red-saf/1.jpg,https://oleks-netizen.github.io/product-images/TW-PH-red-saf/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/746710/1.jpg,https://oleks-netizen.github.io/product-images/746710/2.jpg,https://oleks-netizen.github.io/product-images/746710/3.jpg,https://oleks-netizen.github.io/product-images/746710/4.jpg,https://oleks-netizen.github.io/product-images/746710/5.jpg</t>
         </is>
       </c>
       <c r="C20" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>746743</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/746743/1.jpg,https://oleks-netizen.github.io/product-images/746743/6.jpg,https://oleks-netizen.github.io/product-images/746743/2.jpg,https://oleks-netizen.github.io/product-images/746743/3.jpg,https://oleks-netizen.github.io/product-images/746743/5.jpg</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>75_1_1</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/75_1_1/1.jpg</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>77266101</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/77266101/1.jpg,https://oleks-netizen.github.io/product-images/77266101/2.jpg,https://oleks-netizen.github.io/product-images/77266101/3.jpg,https://oleks-netizen.github.io/product-images/77266101/4.jpg,https://oleks-netizen.github.io/product-images/77266101/5.jpg,https://oleks-netizen.github.io/product-images/77266101/6.jpg,https://oleks-netizen.github.io/product-images/77266101/7.jpg</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>B10-434A</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/B10-434A/1.jpg,https://oleks-netizen.github.io/product-images/B10-434A/6.jpg,https://oleks-netizen.github.io/product-images/B10-434A/2.jpg,https://oleks-netizen.github.io/product-images/B10-434A/4.jpg,https://oleks-netizen.github.io/product-images/B10-434A/5.jpg</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>BB80701-50</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/BB80701-50/1.jpg,https://oleks-netizen.github.io/product-images/BB80701-50/2.jpg,https://oleks-netizen.github.io/product-images/BB80701-50/3.jpg,https://oleks-netizen.github.io/product-images/BB80701-50/4.jpg,https://oleks-netizen.github.io/product-images/BB80701-50/5.jpg,https://oleks-netizen.github.io/product-images/BB80701-50/6.jpg</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>BB81251-02</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/BB81251-02/1.jpg,https://oleks-netizen.github.io/product-images/BB81251-02/2.jpg,https://oleks-netizen.github.io/product-images/BB81251-02/3.jpg,https://oleks-netizen.github.io/product-images/BB81251-02/4.jpg,https://oleks-netizen.github.io/product-images/BB81251-02/5.jpg,https://oleks-netizen.github.io/product-images/BB81251-02/6.jpg</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>BN-SB-2-st-red</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/BN-SB-2-st-red/1.jpg,https://oleks-netizen.github.io/product-images/BN-SB-2-st-red/2.jpg,https://oleks-netizen.github.io/product-images/BN-SB-2-st-red/3.jpg,https://oleks-netizen.github.io/product-images/BN-SB-2-st-red/6.jpg</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>BS70106-01</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/BS70106-01/1.jpg,https://oleks-netizen.github.io/product-images/BS70106-01/2.jpg,https://oleks-netizen.github.io/product-images/BS70106-01/3.jpg,https://oleks-netizen.github.io/product-images/BS70106-01/4.jpg,https://oleks-netizen.github.io/product-images/BS70106-01/5.jpg,https://oleks-netizen.github.io/product-images/BS70106-01/6.jpg</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>BS80401-01</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/BS80401-01/1.jpg,https://oleks-netizen.github.io/product-images/BS80401-01/2.jpg,https://oleks-netizen.github.io/product-images/BS80401-01/3.jpg,https://oleks-netizen.github.io/product-images/BS80401-01/4.jpg,https://oleks-netizen.github.io/product-images/BS80401-01/5.jpg,https://oleks-netizen.github.io/product-images/BS80401-01/6.jpg</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>bx050a</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/bx050a/1.jpg,https://oleks-netizen.github.io/product-images/bx050a/7.jpg,https://oleks-netizen.github.io/product-images/bx050a/2.jpg,https://oleks-netizen.github.io/product-images/bx050a/4.jpg,https://oleks-netizen.github.io/product-images/bx050a/5.jpg,https://oleks-netizen.github.io/product-images/bx050a/6.jpg</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>bx050c</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/bx050c/1.jpg,https://oleks-netizen.github.io/product-images/bx050c/2.jpg,https://oleks-netizen.github.io/product-images/bx050c/3.jpg,https://oleks-netizen.github.io/product-images/bx050c/4.jpg,https://oleks-netizen.github.io/product-images/bx050c/5.jpg</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>bx9020</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/bx9020/1.jpg,https://oleks-netizen.github.io/product-images/bx9020/2.jpg,https://oleks-netizen.github.io/product-images/bx9020/3.jpg,https://oleks-netizen.github.io/product-images/bx9020/4.jpg,https://oleks-netizen.github.io/product-images/bx9020/5.jpg,https://oleks-netizen.github.io/product-images/bx9020/6.jpg,https://oleks-netizen.github.io/product-images/bx9020/7.jpg,https://oleks-netizen.github.io/product-images/bx9020/8.jpg</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>CrH-1294-4lx</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/CrH-1294-4lx/1.jpg,https://oleks-netizen.github.io/product-images/CrH-1294-4lx/10.jpg,https://oleks-netizen.github.io/product-images/CrH-1294-4lx/2.jpg,https://oleks-netizen.github.io/product-images/CrH-1294-4lx/3.jpg,https://oleks-netizen.github.io/product-images/CrH-1294-4lx/4.jpg,https://oleks-netizen.github.io/product-images/CrH-1294-4lx/5.jpg,https://oleks-netizen.github.io/product-images/CrH-1294-4lx/6.jpg,https://oleks-netizen.github.io/product-images/CrH-1294-4lx/7.jpg,https://oleks-netizen.github.io/product-images/CrH-1294-4lx/8.jpg,https://oleks-netizen.github.io/product-images/CrH-1294-4lx/9.jpg</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>DRL19158-2</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/DRL19158-2/1.jpg,https://oleks-netizen.github.io/product-images/DRL19158-2/7.jpg,https://oleks-netizen.github.io/product-images/DRL19158-2/2.jpg,https://oleks-netizen.github.io/product-images/DRL19158-2/4.jpg,https://oleks-netizen.github.io/product-images/DRL19158-2/5.jpg,https://oleks-netizen.github.io/product-images/DRL19158-2/6.jpg</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Elit-2020-4lx</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/Elit-2020-4lx/1.jpg,https://oleks-netizen.github.io/product-images/Elit-2020-4lx/11.jpg,https://oleks-netizen.github.io/product-images/Elit-2020-4lx/10.jpg,https://oleks-netizen.github.io/product-images/Elit-2020-4lx/3.jpg,https://oleks-netizen.github.io/product-images/Elit-2020-4lx/4.jpg,https://oleks-netizen.github.io/product-images/Elit-2020-4lx/5.jpg,https://oleks-netizen.github.io/product-images/Elit-2020-4lx/6.jpg,https://oleks-netizen.github.io/product-images/Elit-2020-4lx/7.jpg,https://oleks-netizen.github.io/product-images/Elit-2020-4lx/8.jpg,https://oleks-netizen.github.io/product-images/Elit-2020-4lx/9.jpg</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Elit-2022-4lx</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/Elit-2022-4lx/1.jpg,https://oleks-netizen.github.io/product-images/Elit-2022-4lx/11.jpg,https://oleks-netizen.github.io/product-images/Elit-2022-4lx/10.jpg,https://oleks-netizen.github.io/product-images/Elit-2022-4lx/3.jpg,https://oleks-netizen.github.io/product-images/Elit-2022-4lx/4.jpg,https://oleks-netizen.github.io/product-images/Elit-2022-4lx/5.jpg,https://oleks-netizen.github.io/product-images/Elit-2022-4lx/6.jpg,https://oleks-netizen.github.io/product-images/Elit-2022-4lx/7.jpg,https://oleks-netizen.github.io/product-images/Elit-2022-4lx/8.jpg,https://oleks-netizen.github.io/product-images/Elit-2022-4lx/9.jpg</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Elit-2023-4lx</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/Elit-2023-4lx/1.jpg,https://oleks-netizen.github.io/product-images/Elit-2023-4lx/10.jpg,https://oleks-netizen.github.io/product-images/Elit-2023-4lx/3.jpg,https://oleks-netizen.github.io/product-images/Elit-2023-4lx/4.jpg,https://oleks-netizen.github.io/product-images/Elit-2023-4lx/5.jpg,https://oleks-netizen.github.io/product-images/Elit-2023-4lx/6.jpg,https://oleks-netizen.github.io/product-images/Elit-2023-4lx/7.jpg,https://oleks-netizen.github.io/product-images/Elit-2023-4lx/8.jpg,https://oleks-netizen.github.io/product-images/Elit-2023-4lx/9.jpg</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>fz118545</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/fz118545/1.jpg,https://oleks-netizen.github.io/product-images/fz118545/2.jpg,https://oleks-netizen.github.io/product-images/fz118545/3.jpg,https://oleks-netizen.github.io/product-images/fz118545/4.jpg,https://oleks-netizen.github.io/product-images/fz118545/5.jpg,https://oleks-netizen.github.io/product-images/fz118545/6.jpg,https://oleks-netizen.github.io/product-images/fz118545/7.jpg,https://oleks-netizen.github.io/product-images/fz118545/8.jpg</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>fz1896103</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/fz1896103/1.jpg,https://oleks-netizen.github.io/product-images/fz1896103/11.jpg,https://oleks-netizen.github.io/product-images/fz1896103/2.jpg,https://oleks-netizen.github.io/product-images/fz1896103/3.jpg,https://oleks-netizen.github.io/product-images/fz1896103/4.jpg,https://oleks-netizen.github.io/product-images/fz1896103/5.jpg,https://oleks-netizen.github.io/product-images/fz1896103/6.jpg,https://oleks-netizen.github.io/product-images/fz1896103/7.jpg,https://oleks-netizen.github.io/product-images/fz1896103/8.jpg,https://oleks-netizen.github.io/product-images/fz1896103/9.jpg</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>fz189645</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/fz189645/1.jpg,https://oleks-netizen.github.io/product-images/fz189645/11.jpg,https://oleks-netizen.github.io/product-images/fz189645/10.jpg,https://oleks-netizen.github.io/product-images/fz189645/3.jpg,https://oleks-netizen.github.io/product-images/fz189645/4.jpg,https://oleks-netizen.github.io/product-images/fz189645/5.jpg,https://oleks-netizen.github.io/product-images/fz189645/6.jpg,https://oleks-netizen.github.io/product-images/fz189645/7.jpg,https://oleks-netizen.github.io/product-images/fz189645/8.jpg,https://oleks-netizen.github.io/product-images/fz189645/9.jpg</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>GA-0307-4lx</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/GA-0307-4lx/1.jpg,https://oleks-netizen.github.io/product-images/GA-0307-4lx/2.jpg,https://oleks-netizen.github.io/product-images/GA-0307-4lx/3.jpg,https://oleks-netizen.github.io/product-images/GA-0307-4lx/4.jpg,https://oleks-netizen.github.io/product-images/GA-0307-4lx/5.jpg,https://oleks-netizen.github.io/product-images/GA-0307-4lx/6.jpg,https://oleks-netizen.github.io/product-images/GA-0307-4lx/7.jpg,https://oleks-netizen.github.io/product-images/GA-0307-4lx/8.jpg,https://oleks-netizen.github.io/product-images/GA-0307-4lx/9.jpg</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>GYalc-5565-4lx</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/GYalc-5565-4lx/1.jpg,https://oleks-netizen.github.io/product-images/GYalc-5565-4lx/8.jpg,https://oleks-netizen.github.io/product-images/GYalc-5565-4lx/2.jpg,https://oleks-netizen.github.io/product-images/GYalc-5565-4lx/3.jpg,https://oleks-netizen.github.io/product-images/GYalc-5565-4lx/4.jpg,https://oleks-netizen.github.io/product-images/GYalc-5565-4lx/5.jpg,https://oleks-netizen.github.io/product-images/GYalc-5565-4lx/7.jpg</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>HB3095</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/HB3095/1.jpg,https://oleks-netizen.github.io/product-images/HB3095/2.jpg,https://oleks-netizen.github.io/product-images/HB3095/3.jpg,https://oleks-netizen.github.io/product-images/HB3095/4.jpg</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>HB3628R</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/HB3628R/1.jpg,https://oleks-netizen.github.io/product-images/HB3628R/8.jpg,https://oleks-netizen.github.io/product-images/HB3628R/2.jpg,https://oleks-netizen.github.io/product-images/HB3628R/4.jpg,https://oleks-netizen.github.io/product-images/HB3628R/5.jpg,https://oleks-netizen.github.io/product-images/HB3628R/6.jpg,https://oleks-netizen.github.io/product-images/HB3628R/7.jpg</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>K1617f-black</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/K1617f-black/1.jpg,https://oleks-netizen.github.io/product-images/K1617f-black/2.jpg,https://oleks-netizen.github.io/product-images/K1617f-black/3.jpg,https://oleks-netizen.github.io/product-images/K1617f-black/4.jpg,https://oleks-netizen.github.io/product-images/K1617f-black/5.jpg</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>L28001-1</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L28001-1/1.jpg,https://oleks-netizen.github.io/product-images/L28001-1/8.jpg,https://oleks-netizen.github.io/product-images/L28001-1/2.jpg,https://oleks-netizen.github.io/product-images/L28001-1/4.jpg,https://oleks-netizen.github.io/product-images/L28001-1/5.jpg,https://oleks-netizen.github.io/product-images/L28001-1/6.jpg,https://oleks-netizen.github.io/product-images/L28001-1/7.jpg</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>L28001-2</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L28001-2/1.jpg,https://oleks-netizen.github.io/product-images/L28001-2/2.jpg,https://oleks-netizen.github.io/product-images/L28001-2/4.jpg,https://oleks-netizen.github.io/product-images/L28001-2/5.jpg,https://oleks-netizen.github.io/product-images/L28001-2/6.jpg,https://oleks-netizen.github.io/product-images/L28001-2/7.jpg</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>L28001-3</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L28001-3/1.jpg,https://oleks-netizen.github.io/product-images/L28001-3/6.jpg,https://oleks-netizen.github.io/product-images/L28001-3/2.jpg,https://oleks-netizen.github.io/product-images/L28001-3/4.jpg,https://oleks-netizen.github.io/product-images/L28001-3/5.jpg,https://oleks-netizen.github.io/product-images/L28001-3/7.jpg</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>L28001-4</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L28001-4/1.jpg,https://oleks-netizen.github.io/product-images/L28001-4/8.jpg,https://oleks-netizen.github.io/product-images/L28001-4/2.jpg,https://oleks-netizen.github.io/product-images/L28001-4/4.jpg,https://oleks-netizen.github.io/product-images/L28001-4/5.jpg,https://oleks-netizen.github.io/product-images/L28001-4/6.jpg,https://oleks-netizen.github.io/product-images/L28001-4/7.jpg</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>L28028-1</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L28028-1/1.jpg,https://oleks-netizen.github.io/product-images/L28028-1/9.jpg,https://oleks-netizen.github.io/product-images/L28028-1/2.jpg,https://oleks-netizen.github.io/product-images/L28028-1/4.jpg,https://oleks-netizen.github.io/product-images/L28028-1/5.jpg,https://oleks-netizen.github.io/product-images/L28028-1/6.jpg,https://oleks-netizen.github.io/product-images/L28028-1/7.jpg,https://oleks-netizen.github.io/product-images/L28028-1/8.jpg</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>L28028-2</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L28028-2/1.jpg,https://oleks-netizen.github.io/product-images/L28028-2/9.jpg,https://oleks-netizen.github.io/product-images/L28028-2/2.jpg,https://oleks-netizen.github.io/product-images/L28028-2/4.jpg,https://oleks-netizen.github.io/product-images/L28028-2/5.jpg,https://oleks-netizen.github.io/product-images/L28028-2/6.jpg,https://oleks-netizen.github.io/product-images/L28028-2/7.jpg,https://oleks-netizen.github.io/product-images/L28028-2/8.jpg</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>L28028-3</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L28028-3/1.jpg,https://oleks-netizen.github.io/product-images/L28028-3/9.jpg,https://oleks-netizen.github.io/product-images/L28028-3/2.jpg,https://oleks-netizen.github.io/product-images/L28028-3/4.jpg,https://oleks-netizen.github.io/product-images/L28028-3/5.jpg,https://oleks-netizen.github.io/product-images/L28028-3/6.jpg,https://oleks-netizen.github.io/product-images/L28028-3/7.jpg,https://oleks-netizen.github.io/product-images/L28028-3/8.jpg</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>L28029-1</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L28029-1/1.jpg,https://oleks-netizen.github.io/product-images/L28029-1/9.jpg,https://oleks-netizen.github.io/product-images/L28029-1/2.jpg,https://oleks-netizen.github.io/product-images/L28029-1/4.jpg,https://oleks-netizen.github.io/product-images/L28029-1/5.jpg,https://oleks-netizen.github.io/product-images/L28029-1/6.jpg,https://oleks-netizen.github.io/product-images/L28029-1/7.jpg,https://oleks-netizen.github.io/product-images/L28029-1/8.jpg</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>L28029-2</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L28029-2/1.jpg,https://oleks-netizen.github.io/product-images/L28029-2/9.jpg,https://oleks-netizen.github.io/product-images/L28029-2/2.jpg,https://oleks-netizen.github.io/product-images/L28029-2/4.jpg,https://oleks-netizen.github.io/product-images/L28029-2/5.jpg,https://oleks-netizen.github.io/product-images/L28029-2/6.jpg,https://oleks-netizen.github.io/product-images/L28029-2/7.jpg,https://oleks-netizen.github.io/product-images/L28029-2/8.jpg</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>L28029-3</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L28029-3/1.jpg,https://oleks-netizen.github.io/product-images/L28029-3/9.jpg,https://oleks-netizen.github.io/product-images/L28029-3/2.jpg,https://oleks-netizen.github.io/product-images/L28029-3/4.jpg,https://oleks-netizen.github.io/product-images/L28029-3/5.jpg,https://oleks-netizen.github.io/product-images/L28029-3/6.jpg,https://oleks-netizen.github.io/product-images/L28029-3/7.jpg,https://oleks-netizen.github.io/product-images/L28029-3/8.jpg</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>L87229-1</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L87229-1/1.jpg,https://oleks-netizen.github.io/product-images/L87229-1/9.jpg,https://oleks-netizen.github.io/product-images/L87229-1/3.jpg,https://oleks-netizen.github.io/product-images/L87229-1/4.jpg,https://oleks-netizen.github.io/product-images/L87229-1/5.jpg,https://oleks-netizen.github.io/product-images/L87229-1/6.jpg,https://oleks-netizen.github.io/product-images/L87229-1/7.jpg,https://oleks-netizen.github.io/product-images/L87229-1/8.jpg</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>L88003-32</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L88003-32/1.jpg,https://oleks-netizen.github.io/product-images/L88003-32/8.jpg,https://oleks-netizen.github.io/product-images/L88003-32/2.jpg,https://oleks-netizen.github.io/product-images/L88003-32/4.jpg,https://oleks-netizen.github.io/product-images/L88003-32/5.jpg,https://oleks-netizen.github.io/product-images/L88003-32/6.jpg,https://oleks-netizen.github.io/product-images/L88003-32/7.jpg</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>LC47208K-1</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/LC47208K-1/1.jpg,https://oleks-netizen.github.io/product-images/LC47208K-1/7.jpg,https://oleks-netizen.github.io/product-images/LC47208K-1/2.jpg,https://oleks-netizen.github.io/product-images/LC47208K-1/3.jpg,https://oleks-netizen.github.io/product-images/LC47208K-1/5.jpg,https://oleks-netizen.github.io/product-images/LC47208K-1/6.jpg</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>LC47208K-1X</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/LC47208K-1X/1.jpg,https://oleks-netizen.github.io/product-images/LC47208K-1X/9.jpg,https://oleks-netizen.github.io/product-images/LC47208K-1X/2.jpg,https://oleks-netizen.github.io/product-images/LC47208K-1X/3.jpg,https://oleks-netizen.github.io/product-images/LC47208K-1X/5.jpg,https://oleks-netizen.github.io/product-images/LC47208K-1X/6.jpg,https://oleks-netizen.github.io/product-images/LC47208K-1X/7.jpg,https://oleks-netizen.github.io/product-images/LC47208K-1X/8.jpg</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>LC47208K-92</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/LC47208K-92/1.jpg,https://oleks-netizen.github.io/product-images/LC47208K-92/7.jpg,https://oleks-netizen.github.io/product-images/LC47208K-92/2.jpg,https://oleks-netizen.github.io/product-images/LC47208K-92/3.jpg,https://oleks-netizen.github.io/product-images/LC47208K-92/5.jpg,https://oleks-netizen.github.io/product-images/LC47208K-92/6.jpg</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>LC47210-1</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/LC47210-1/1.jpg,https://oleks-netizen.github.io/product-images/LC47210-1/6.jpg,https://oleks-netizen.github.io/product-images/LC47210-1/2.jpg,https://oleks-netizen.github.io/product-images/LC47210-1/4.jpg,https://oleks-netizen.github.io/product-images/LC47210-1/5.jpg</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>LC47210-1X</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/LC47210-1X/1.jpg,https://oleks-netizen.github.io/product-images/LC47210-1X/2.jpg,https://oleks-netizen.github.io/product-images/LC47210-1X/3.jpg,https://oleks-netizen.github.io/product-images/LC47210-1X/4.jpg,https://oleks-netizen.github.io/product-images/LC47210-1X/5.jpg,https://oleks-netizen.github.io/product-images/LC47210-1X/6.jpg</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>LC47210-92</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/LC47210-92/1.jpg,https://oleks-netizen.github.io/product-images/LC47210-92/8.jpg,https://oleks-netizen.github.io/product-images/LC47210-92/2.jpg,https://oleks-netizen.github.io/product-images/LC47210-92/4.jpg,https://oleks-netizen.github.io/product-images/LC47210-92/5.jpg,https://oleks-netizen.github.io/product-images/LC47210-92/6.jpg,https://oleks-netizen.github.io/product-images/LC47210-92/7.jpg</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>LC47240W-1</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/LC47240W-1/1.jpg,https://oleks-netizen.github.io/product-images/LC47240W-1/7.jpg,https://oleks-netizen.github.io/product-images/LC47240W-1/2.jpg,https://oleks-netizen.github.io/product-images/LC47240W-1/4.jpg,https://oleks-netizen.github.io/product-images/LC47240W-1/5.jpg,https://oleks-netizen.github.io/product-images/LC47240W-1/6.jpg</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>LC47240W-1X</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/LC47240W-1X/1.jpg,https://oleks-netizen.github.io/product-images/LC47240W-1X/7.jpg,https://oleks-netizen.github.io/product-images/LC47240W-1X/2.jpg,https://oleks-netizen.github.io/product-images/LC47240W-1X/4.jpg,https://oleks-netizen.github.io/product-images/LC47240W-1X/5.jpg,https://oleks-netizen.github.io/product-images/LC47240W-1X/6.jpg</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>LC47240W-92</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/LC47240W-92/1.jpg,https://oleks-netizen.github.io/product-images/LC47240W-92/8.jpg,https://oleks-netizen.github.io/product-images/LC47240W-92/2.jpg,https://oleks-netizen.github.io/product-images/LC47240W-92/3.jpg,https://oleks-netizen.github.io/product-images/LC47240W-92/5.jpg,https://oleks-netizen.github.io/product-images/LC47240W-92/6.jpg,https://oleks-netizen.github.io/product-images/LC47240W-92/7.jpg</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>LC47539-1</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/LC47539-1/1.jpg,https://oleks-netizen.github.io/product-images/LC47539-1/6.jpg,https://oleks-netizen.github.io/product-images/LC47539-1/2.jpg,https://oleks-netizen.github.io/product-images/LC47539-1/4.jpg,https://oleks-netizen.github.io/product-images/LC47539-1/5.jpg</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>LC47539-92</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/LC47539-92/1.jpg,https://oleks-netizen.github.io/product-images/LC47539-92/8.jpg,https://oleks-netizen.github.io/product-images/LC47539-92/2.jpg,https://oleks-netizen.github.io/product-images/LC47539-92/3.jpg,https://oleks-netizen.github.io/product-images/LC47539-92/5.jpg,https://oleks-netizen.github.io/product-images/LC47539-92/6.jpg,https://oleks-netizen.github.io/product-images/LC47539-92/7.jpg</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>LC47632F-1</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/LC47632F-1/1.jpg,https://oleks-netizen.github.io/product-images/LC47632F-1/7.jpg,https://oleks-netizen.github.io/product-images/LC47632F-1/2.jpg,https://oleks-netizen.github.io/product-images/LC47632F-1/4.jpg,https://oleks-netizen.github.io/product-images/LC47632F-1/5.jpg,https://oleks-netizen.github.io/product-images/LC47632F-1/6.jpg</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>LC47632F-92</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/LC47632F-92/1.jpg,https://oleks-netizen.github.io/product-images/LC47632F-92/8.jpg,https://oleks-netizen.github.io/product-images/LC47632F-92/2.jpg,https://oleks-netizen.github.io/product-images/LC47632F-92/3.jpg,https://oleks-netizen.github.io/product-images/LC47632F-92/5.jpg,https://oleks-netizen.github.io/product-images/LC47632F-92/6.jpg,https://oleks-netizen.github.io/product-images/LC47632F-92/7.jpg</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>LC47695-1</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/LC47695-1/1.jpg,https://oleks-netizen.github.io/product-images/LC47695-1/10.jpg,https://oleks-netizen.github.io/product-images/LC47695-1/2.jpg,https://oleks-netizen.github.io/product-images/LC47695-1/3.jpg,https://oleks-netizen.github.io/product-images/LC47695-1/5.jpg,https://oleks-netizen.github.io/product-images/LC47695-1/6.jpg,https://oleks-netizen.github.io/product-images/LC47695-1/7.jpg,https://oleks-netizen.github.io/product-images/LC47695-1/8.jpg,https://oleks-netizen.github.io/product-images/LC47695-1/9.jpg</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>LC47832-1</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/LC47832-1/1.jpg,https://oleks-netizen.github.io/product-images/LC47832-1/8.jpg,https://oleks-netizen.github.io/product-images/LC47832-1/2.jpg,https://oleks-netizen.github.io/product-images/LC47832-1/3.jpg,https://oleks-netizen.github.io/product-images/LC47832-1/5.jpg,https://oleks-netizen.github.io/product-images/LC47832-1/6.jpg,https://oleks-netizen.github.io/product-images/LC47832-1/7.jpg</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>LC47832-92</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/LC47832-92/1.jpg,https://oleks-netizen.github.io/product-images/LC47832-92/8.jpg,https://oleks-netizen.github.io/product-images/LC47832-92/2.jpg,https://oleks-netizen.github.io/product-images/LC47832-92/3.jpg,https://oleks-netizen.github.io/product-images/LC47832-92/5.jpg,https://oleks-netizen.github.io/product-images/LC47832-92/6.jpg,https://oleks-netizen.github.io/product-images/LC47832-92/7.jpg</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>LC47891-1</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/LC47891-1/1.jpg,https://oleks-netizen.github.io/product-images/LC47891-1/7.jpg,https://oleks-netizen.github.io/product-images/LC47891-1/2.jpg,https://oleks-netizen.github.io/product-images/LC47891-1/4.jpg,https://oleks-netizen.github.io/product-images/LC47891-1/5.jpg,https://oleks-netizen.github.io/product-images/LC47891-1/6.jpg</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>LC47891-92</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/LC47891-92/1.jpg,https://oleks-netizen.github.io/product-images/LC47891-92/8.jpg,https://oleks-netizen.github.io/product-images/LC47891-92/2.jpg,https://oleks-netizen.github.io/product-images/LC47891-92/3.jpg,https://oleks-netizen.github.io/product-images/LC47891-92/5.jpg,https://oleks-netizen.github.io/product-images/LC47891-92/6.jpg,https://oleks-netizen.github.io/product-images/LC47891-92/7.jpg</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>LC47991-1A</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/LC47991-1A/1.jpg,https://oleks-netizen.github.io/product-images/LC47991-1A/6.jpg,https://oleks-netizen.github.io/product-images/LC47991-1A/2.jpg,https://oleks-netizen.github.io/product-images/LC47991-1A/4.jpg,https://oleks-netizen.github.io/product-images/LC47991-1A/5.jpg</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>LC47991-92</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/LC47991-92/1.jpg,https://oleks-netizen.github.io/product-images/LC47991-92/8.jpg,https://oleks-netizen.github.io/product-images/LC47991-92/2.jpg,https://oleks-netizen.github.io/product-images/LC47991-92/3.jpg,https://oleks-netizen.github.io/product-images/LC47991-92/5.jpg,https://oleks-netizen.github.io/product-images/LC47991-92/6.jpg,https://oleks-netizen.github.io/product-images/LC47991-92/7.jpg</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>lim-22-115</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/lim-22-115/1.jpg,https://oleks-netizen.github.io/product-images/lim-22-115/2.jpg,https://oleks-netizen.github.io/product-images/lim-22-115/3.jpg,https://oleks-netizen.github.io/product-images/lim-22-115/4.jpg</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>RA-1342-3md</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/RA-1342-3md/1.jpg,https://oleks-netizen.github.io/product-images/RA-1342-3md/6.jpg,https://oleks-netizen.github.io/product-images/RA-1342-3md/3.jpg,https://oleks-netizen.github.io/product-images/RA-1342-3md/4.jpg,https://oleks-netizen.github.io/product-images/RA-1342-3md/5.jpg</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>RB-7340-3md</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/RB-7340-3md/1.jpg,https://oleks-netizen.github.io/product-images/RB-7340-3md/10.jpg,https://oleks-netizen.github.io/product-images/RB-7340-3md/2.jpg,https://oleks-netizen.github.io/product-images/RB-7340-3md/3.jpg,https://oleks-netizen.github.io/product-images/RB-7340-3md/4.jpg,https://oleks-netizen.github.io/product-images/RB-7340-3md/5.jpg,https://oleks-netizen.github.io/product-images/RB-7340-3md/6.jpg,https://oleks-netizen.github.io/product-images/RB-7340-3md/7.jpg,https://oleks-netizen.github.io/product-images/RB-7340-3md/8.jpg,https://oleks-netizen.github.io/product-images/RB-7340-3md/9.jpg</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>RC-7122-3mdL</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/RC-7122-3mdL/1.jpg,https://oleks-netizen.github.io/product-images/RC-7122-3mdL/7.jpg,https://oleks-netizen.github.io/product-images/RC-7122-3mdL/2.jpg,https://oleks-netizen.github.io/product-images/RC-7122-3mdL/3.jpg,https://oleks-netizen.github.io/product-images/RC-7122-3mdL/5.jpg,https://oleks-netizen.github.io/product-images/RC-7122-3mdL/6.jpg</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>RC-7340-3md</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/RC-7340-3md/1.jpg,https://oleks-netizen.github.io/product-images/RC-7340-3md/11.jpg,https://oleks-netizen.github.io/product-images/RC-7340-3md/10.jpg,https://oleks-netizen.github.io/product-images/RC-7340-3md/2.jpg,https://oleks-netizen.github.io/product-images/RC-7340-3md/4.jpg,https://oleks-netizen.github.io/product-images/RC-7340-3md/5.jpg,https://oleks-netizen.github.io/product-images/RC-7340-3md/6.jpg,https://oleks-netizen.github.io/product-images/RC-7340-3md/7.jpg,https://oleks-netizen.github.io/product-images/RC-7340-3md/8.jpg,https://oleks-netizen.github.io/product-images/RC-7340-3md/9.jpg</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>RCC-3920-3md</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/RCC-3920-3md/1.jpg,https://oleks-netizen.github.io/product-images/RCC-3920-3md/10.jpg,https://oleks-netizen.github.io/product-images/RCC-3920-3md/2.jpg,https://oleks-netizen.github.io/product-images/RCC-3920-3md/3.jpg,https://oleks-netizen.github.io/product-images/RCC-3920-3md/5.jpg,https://oleks-netizen.github.io/product-images/RCC-3920-3md/6.jpg,https://oleks-netizen.github.io/product-images/RCC-3920-3md/7.jpg,https://oleks-netizen.github.io/product-images/RCC-3920-3md/8.jpg,https://oleks-netizen.github.io/product-images/RCC-3920-3md/9.jpg</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>RCk-3420-3md</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/RCk-3420-3md/1.jpg,https://oleks-netizen.github.io/product-images/RCk-3420-3md/2.jpg,https://oleks-netizen.github.io/product-images/RCk-3420-3md/3.jpg,https://oleks-netizen.github.io/product-images/RCk-3420-3md/4.jpg,https://oleks-netizen.github.io/product-images/RCk-3420-3md/5.jpg,https://oleks-netizen.github.io/product-images/RCk-3420-3md/6.jpg,https://oleks-netizen.github.io/product-images/RCk-3420-3md/7.jpg,https://oleks-netizen.github.io/product-images/RCk-3420-3md/8.jpg</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>RYw-3027-4lx</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/RYw-3027-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RYw-3027-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RYw-3027-4lx/3.jpg,https://oleks-netizen.github.io/product-images/RYw-3027-4lx/4.jpg,https://oleks-netizen.github.io/product-images/RYw-3027-4lx/5.jpg,https://oleks-netizen.github.io/product-images/RYw-3027-4lx/6.jpg</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>RС-1342-3md</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/RС-1342-3md/1.jpg,https://oleks-netizen.github.io/product-images/RС-1342-3md/6.jpg,https://oleks-netizen.github.io/product-images/RС-1342-3md/3.jpg,https://oleks-netizen.github.io/product-images/RС-1342-3md/4.jpg,https://oleks-netizen.github.io/product-images/RС-1342-3md/5.jpg</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>TA-5664-4lx</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TA-5664-4lx/1.jpg,https://oleks-netizen.github.io/product-images/TA-5664-4lx/2.jpg,https://oleks-netizen.github.io/product-images/TA-5664-4lx/3.jpg,https://oleks-netizen.github.io/product-images/TA-5664-4lx/4.jpg,https://oleks-netizen.github.io/product-images/TA-5664-4lx/5.jpg,https://oleks-netizen.github.io/product-images/TA-5664-4lx/6.jpg,https://oleks-netizen.github.io/product-images/TA-5664-4lx/7.jpg,https://oleks-netizen.github.io/product-images/TA-5664-4lx/8.jpg</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>TW-Bella-dark-brown</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-Bella-dark-brown/1.jpg,https://oleks-netizen.github.io/product-images/TW-Bella-dark-brown/2.jpg,https://oleks-netizen.github.io/product-images/TW-Bella-dark-brown/3.jpg,https://oleks-netizen.github.io/product-images/TW-Bella-dark-brown/4.jpg</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>TW-Bella-mokko</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-Bella-mokko/1.jpg,https://oleks-netizen.github.io/product-images/TW-Bella-mokko/7.jpg,https://oleks-netizen.github.io/product-images/TW-Bella-mokko/3.jpg,https://oleks-netizen.github.io/product-images/TW-Bella-mokko/4.jpg,https://oleks-netizen.github.io/product-images/TW-Bella-mokko/5.jpg,https://oleks-netizen.github.io/product-images/TW-Bella-mokko/6.jpg</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>TW-Bella-olive</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-Bella-olive/1.jpg,https://oleks-netizen.github.io/product-images/TW-Bella-olive/2.jpg,https://oleks-netizen.github.io/product-images/TW-Bella-olive/3.jpg,https://oleks-netizen.github.io/product-images/TW-Bella-olive/4.jpg,https://oleks-netizen.github.io/product-images/TW-Bella-olive/5.jpg</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>TW-Bella-red</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-Bella-red/1.jpg,https://oleks-netizen.github.io/product-images/TW-Bella-red/5.jpg,https://oleks-netizen.github.io/product-images/TW-Bella-red/3.jpg,https://oleks-netizen.github.io/product-images/TW-Bella-red/4.jpg</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>TW-Bridget-white</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-Bridget-white/1.jpg,https://oleks-netizen.github.io/product-images/TW-Bridget-white/5.jpg,https://oleks-netizen.github.io/product-images/TW-Bridget-white/3.jpg,https://oleks-netizen.github.io/product-images/TW-Bridget-white/4.jpg</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>TW-Business-black</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-Business-black/1.jpg,https://oleks-netizen.github.io/product-images/TW-Business-black/4.jpg,https://oleks-netizen.github.io/product-images/TW-Business-black/3.jpg</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>TW-Business-dark-blue</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-Business-dark-blue/1.jpg,https://oleks-netizen.github.io/product-images/TW-Business-dark-blue/2.jpg,https://oleks-netizen.github.io/product-images/TW-Business-dark-blue/3.jpg,https://oleks-netizen.github.io/product-images/TW-Business-dark-blue/4.jpg</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>TW-Business-mars</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-Business-mars/1.jpg,https://oleks-netizen.github.io/product-images/TW-Business-mars/2.jpg,https://oleks-netizen.github.io/product-images/TW-Business-mars/3.jpg,https://oleks-netizen.github.io/product-images/TW-Business-mars/4.jpg,https://oleks-netizen.github.io/product-images/TW-Business-mars/5.jpg</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>TW-CB-8-black</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-CB-8-black/1.jpg,https://oleks-netizen.github.io/product-images/TW-CB-8-black/2.jpg,https://oleks-netizen.github.io/product-images/TW-CB-8-black/3.jpg,https://oleks-netizen.github.io/product-images/TW-CB-8-black/4.jpg</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>TW-CB-8-light-beige</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-CB-8-light-beige/1.jpg,https://oleks-netizen.github.io/product-images/TW-CB-8-light-beige/2.jpg,https://oleks-netizen.github.io/product-images/TW-CB-8-light-beige/3.jpg,https://oleks-netizen.github.io/product-images/TW-CB-8-light-beige/4.jpg</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>TW-CB-8-mars</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-CB-8-mars/1.jpg,https://oleks-netizen.github.io/product-images/TW-CB-8-mars/2.jpg,https://oleks-netizen.github.io/product-images/TW-CB-8-mars/3.jpg,https://oleks-netizen.github.io/product-images/TW-CB-8-mars/4.jpg</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>TW-CB-8-mokko</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-CB-8-mokko/1.jpg,https://oleks-netizen.github.io/product-images/TW-CB-8-mokko/2.jpg,https://oleks-netizen.github.io/product-images/TW-CB-8-mokko/3.jpg,https://oleks-netizen.github.io/product-images/TW-CB-8-mokko/4.jpg</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>TW-CB-8-pink</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-CB-8-pink/1.jpg,https://oleks-netizen.github.io/product-images/TW-CB-8-pink/2.jpg,https://oleks-netizen.github.io/product-images/TW-CB-8-pink/3.jpg,https://oleks-netizen.github.io/product-images/TW-CB-8-pink/4.jpg</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>TW-CB-8-red</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-CB-8-red/1.jpg,https://oleks-netizen.github.io/product-images/TW-CB-8-red/4.jpg,https://oleks-netizen.github.io/product-images/TW-CB-8-red/2.jpg</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>TW-GC-1-black</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-GC-1-black/1.jpg,https://oleks-netizen.github.io/product-images/TW-GC-1-black/2.jpg,https://oleks-netizen.github.io/product-images/TW-GC-1-black/3.jpg</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>TW-GC-1-mars</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-GC-1-mars/1.jpg,https://oleks-netizen.github.io/product-images/TW-GC-1-mars/2.jpg,https://oleks-netizen.github.io/product-images/TW-GC-1-mars/3.jpg</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>TW-GC-1-red</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-GC-1-red/1.jpg,https://oleks-netizen.github.io/product-images/TW-GC-1-red/2.jpg,https://oleks-netizen.github.io/product-images/TW-GC-1-red/3.jpg</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>TW-Jill-caramel</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-Jill-caramel/1.jpg,https://oleks-netizen.github.io/product-images/TW-Jill-caramel/6.jpg,https://oleks-netizen.github.io/product-images/TW-Jill-caramel/2.jpg,https://oleks-netizen.github.io/product-images/TW-Jill-caramel/4.jpg,https://oleks-netizen.github.io/product-images/TW-Jill-caramel/5.jpg</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>TW-Jill-red</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-Jill-red/1.jpg,https://oleks-netizen.github.io/product-images/TW-Jill-red/3.jpg</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>TW-KL-5-mars</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-KL-5-mars/1.jpg,https://oleks-netizen.github.io/product-images/TW-KL-5-mars/6.jpg,https://oleks-netizen.github.io/product-images/TW-KL-5-mars/2.jpg,https://oleks-netizen.github.io/product-images/TW-KL-5-mars/4.jpg,https://oleks-netizen.github.io/product-images/TW-KL-5-mars/5.jpg</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>TW-Nona-2-k</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-Nona-2-k/1.jpg,https://oleks-netizen.github.io/product-images/TW-Nona-2-k/5.jpg,https://oleks-netizen.github.io/product-images/TW-Nona-2-k/3.jpg,https://oleks-netizen.github.io/product-images/TW-Nona-2-k/4.jpg</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>TW-Nona-2-pink</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-Nona-2-pink/1.jpg,https://oleks-netizen.github.io/product-images/TW-Nona-2-pink/4.jpg,https://oleks-netizen.github.io/product-images/TW-Nona-2-pink/3.jpg</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>TW-OP-1-black</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-OP-1-black/1.jpg,https://oleks-netizen.github.io/product-images/TW-OP-1-black/2.jpg,https://oleks-netizen.github.io/product-images/TW-OP-1-black/3.jpg</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>TW-OP-1-dark-blue</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-OP-1-dark-blue/1.jpg,https://oleks-netizen.github.io/product-images/TW-OP-1-dark-blue/2.jpg,https://oleks-netizen.github.io/product-images/TW-OP-1-dark-blue/3.jpg</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>TW-OP-1-mars</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-OP-1-mars/1.jpg,https://oleks-netizen.github.io/product-images/TW-OP-1-mars/2.jpg,https://oleks-netizen.github.io/product-images/TW-OP-1-mars/3.jpg</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>TW-PM-Classic-mars</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-PM-Classic-mars/1.jpg,https://oleks-netizen.github.io/product-images/TW-PM-Classic-mars/2.jpg,https://oleks-netizen.github.io/product-images/TW-PM-Classic-mars/3.jpg,https://oleks-netizen.github.io/product-images/TW-PM-Classic-mars/4.jpg</t>
+        </is>
+      </c>
+      <c r="C113" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>TW-PM-Classic-red</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-PM-Classic-red/1.jpg,https://oleks-netizen.github.io/product-images/TW-PM-Classic-red/2.jpg,https://oleks-netizen.github.io/product-images/TW-PM-Classic-red/3.jpg,https://oleks-netizen.github.io/product-images/TW-PM-Classic-red/4.jpg</t>
+        </is>
+      </c>
+      <c r="C114" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>TW-Style-black</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-Style-black/1.jpg,https://oleks-netizen.github.io/product-images/TW-Style-black/2.jpg,https://oleks-netizen.github.io/product-images/TW-Style-black/3.jpg,https://oleks-netizen.github.io/product-images/TW-Style-black/4.jpg,https://oleks-netizen.github.io/product-images/TW-Style-black/5.jpg</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>TW-Style-kon</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TW-Style-kon/1.jpg,https://oleks-netizen.github.io/product-images/TW-Style-kon/5.jpg,https://oleks-netizen.github.io/product-images/TW-Style-kon/2.jpg,https://oleks-netizen.github.io/product-images/TW-Style-kon/3.jpg</t>
+        </is>
+      </c>
+      <c r="C116" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>vc001A-orange</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/vc001A-orange/1.jpg,https://oleks-netizen.github.io/product-images/vc001A-orange/2.jpg,https://oleks-netizen.github.io/product-images/vc001A-orange/3.jpg,https://oleks-netizen.github.io/product-images/vc001A-orange/4.jpg</t>
+        </is>
+      </c>
+      <c r="C117" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>vc001a-red</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/vc001a-red/1.jpg,https://oleks-netizen.github.io/product-images/vc001a-red/2.jpg,https://oleks-netizen.github.io/product-images/vc001a-red/3.jpg,https://oleks-netizen.github.io/product-images/vc001a-red/4.jpg</t>
+        </is>
+      </c>
+      <c r="C118" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update 2026-02-04 16:27:10
</commit_message>
<xml_diff>
--- a/articles_summary.xlsx
+++ b/articles_summary.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,31 +441,31 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>3edfff52020ebe32c91adc248efd2ba1-Photoroom</t>
+          <t>20869_1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/3edfff52020ebe32c91adc248efd2ba1-Photoroom/1.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20869_1/1.jpg,https://oleks-netizen.github.io/product-images/20869_1/2.jpg,https://oleks-netizen.github.io/product-images/20869_1/11.jpg,https://oleks-netizen.github.io/product-images/20869_1/3.jpg,https://oleks-netizen.github.io/product-images/20869_1/4.jpg,https://oleks-netizen.github.io/product-images/20869_1/5.jpg,https://oleks-netizen.github.io/product-images/20869_1/6.jpg,https://oleks-netizen.github.io/product-images/20869_1/7.jpg,https://oleks-netizen.github.io/product-images/20869_1/8.jpg</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>20869_1</t>
+          <t>20869_1_20869_1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20869_1/2.jpg,https://oleks-netizen.github.io/product-images/20869_1/11.jpg,https://oleks-netizen.github.io/product-images/20869_1/3.jpg,https://oleks-netizen.github.io/product-images/20869_1/4.jpg,https://oleks-netizen.github.io/product-images/20869_1/5.jpg,https://oleks-netizen.github.io/product-images/20869_1/6.jpg,https://oleks-netizen.github.io/product-images/20869_1/7.jpg,https://oleks-netizen.github.io/product-images/20869_1/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20869_1_20869_1/10.jpg</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -476,37 +476,37 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20871_1/1.jpg,https://oleks-netizen.github.io/product-images/20871_1/12.jpg,https://oleks-netizen.github.io/product-images/20871_1/11.jpg,https://oleks-netizen.github.io/product-images/20871_1/3.jpg,https://oleks-netizen.github.io/product-images/20871_1/4.jpg,https://oleks-netizen.github.io/product-images/20871_1/5.jpg,https://oleks-netizen.github.io/product-images/20871_1/6.jpg,https://oleks-netizen.github.io/product-images/20871_1/7.jpg,https://oleks-netizen.github.io/product-images/20871_1/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20871_1/1.jpg,https://oleks-netizen.github.io/product-images/20871_1/2.jpg,https://oleks-netizen.github.io/product-images/20871_1/12.jpg,https://oleks-netizen.github.io/product-images/20871_1/11.jpg,https://oleks-netizen.github.io/product-images/20871_1/3.jpg,https://oleks-netizen.github.io/product-images/20871_1/4.jpg,https://oleks-netizen.github.io/product-images/20871_1/5.jpg,https://oleks-netizen.github.io/product-images/20871_1/6.jpg,https://oleks-netizen.github.io/product-images/20871_1/7.jpg,https://oleks-netizen.github.io/product-images/20871_1/8.jpg</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>20871_1-Photoroom</t>
+          <t>20871_1_20871_1</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20871_1-Photoroom/2.jpg,https://oleks-netizen.github.io/product-images/20871_1-Photoroom/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20871_1_20871_1/10.jpg</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>23148-Photoroom</t>
+          <t>23148_23148-Photoroom</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/23148-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/23148-Photoroom/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/23148_23148-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/23148_23148-Photoroom/2.jpg</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -531,132 +531,132 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>23150-Photoroom</t>
+          <t>23150</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/23150-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/23150-Photoroom/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/23150/1.jpg,https://oleks-netizen.github.io/product-images/23150/2.jpg,https://oleks-netizen.github.io/product-images/23150/11.jpg,https://oleks-netizen.github.io/product-images/23150/3.jpg,https://oleks-netizen.github.io/product-images/23150/4.jpg,https://oleks-netizen.github.io/product-images/23150/5.jpg,https://oleks-netizen.github.io/product-images/23150/6.jpg,https://oleks-netizen.github.io/product-images/23150/7.jpg,https://oleks-netizen.github.io/product-images/23150/8.jpg</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>23150</t>
+          <t>23152</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/23150/11.jpg,https://oleks-netizen.github.io/product-images/23150/3.jpg,https://oleks-netizen.github.io/product-images/23150/4.jpg,https://oleks-netizen.github.io/product-images/23150/5.jpg,https://oleks-netizen.github.io/product-images/23150/6.jpg,https://oleks-netizen.github.io/product-images/23150/7.jpg,https://oleks-netizen.github.io/product-images/23150/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/23152/1.jpg,https://oleks-netizen.github.io/product-images/23152/2.jpg,https://oleks-netizen.github.io/product-images/23152/9.jpg,https://oleks-netizen.github.io/product-images/23152/11.jpg,https://oleks-netizen.github.io/product-images/23152/3.jpg,https://oleks-netizen.github.io/product-images/23152/4.jpg,https://oleks-netizen.github.io/product-images/23152/5.jpg,https://oleks-netizen.github.io/product-images/23152/6.jpg,https://oleks-netizen.github.io/product-images/23152/7.jpg,https://oleks-netizen.github.io/product-images/23152/8.jpg</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>23152-Photoroom</t>
+          <t>51411030m</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/23152-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/23152-Photoroom/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/51411030m/1.jpg,https://oleks-netizen.github.io/product-images/51411030m/3.jpg,https://oleks-netizen.github.io/product-images/51411030m/7.jpg,https://oleks-netizen.github.io/product-images/51411030m/4.jpg,https://oleks-netizen.github.io/product-images/51411030m/5.jpg,https://oleks-netizen.github.io/product-images/51411030m/6.jpg</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>23152</t>
+          <t>C1HS1890bl-black</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/23152/9.jpg,https://oleks-netizen.github.io/product-images/23152/11.jpg,https://oleks-netizen.github.io/product-images/23152/3.jpg,https://oleks-netizen.github.io/product-images/23152/4.jpg,https://oleks-netizen.github.io/product-images/23152/5.jpg,https://oleks-netizen.github.io/product-images/23152/6.jpg,https://oleks-netizen.github.io/product-images/23152/7.jpg,https://oleks-netizen.github.io/product-images/23152/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C1HS1890bl-black/1.jpg,https://oleks-netizen.github.io/product-images/C1HS1890bl-black/2.jpg,https://oleks-netizen.github.io/product-images/C1HS1890bl-black/6.jpg,https://oleks-netizen.github.io/product-images/C1HS1890bl-black/3.jpg,https://oleks-netizen.github.io/product-images/C1HS1890bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>51411030m</t>
+          <t>C1HSSA0546bl-black</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/51411030m/1.jpg,https://oleks-netizen.github.io/product-images/51411030m/2.jpg,https://oleks-netizen.github.io/product-images/51411030m/3.jpg,https://oleks-netizen.github.io/product-images/51411030m/4.jpg,https://oleks-netizen.github.io/product-images/51411030m/5.jpg,https://oleks-netizen.github.io/product-images/51411030m/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C1HSSA0546bl-black/1.jpg,https://oleks-netizen.github.io/product-images/C1HSSA0546bl-black/3.jpg,https://oleks-netizen.github.io/product-images/C1HSSA0546bl-black/5.jpg,https://oleks-netizen.github.io/product-images/C1HSSA0546bl-black/4.jpg</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>C1HS1890bl-black</t>
+          <t>C1HSSA0546gr-green</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C1HS1890bl-black/1.jpg,https://oleks-netizen.github.io/product-images/C1HS1890bl-black/2.jpg,https://oleks-netizen.github.io/product-images/C1HS1890bl-black/3.jpg,https://oleks-netizen.github.io/product-images/C1HS1890bl-black/4.jpg,https://oleks-netizen.github.io/product-images/C1HS1890bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C1HSSA0546gr-green/1.jpg,https://oleks-netizen.github.io/product-images/C1HSSA0546gr-green/5.jpg,https://oleks-netizen.github.io/product-images/C1HSSA0546gr-green/3.jpg,https://oleks-netizen.github.io/product-images/C1HSSA0546gr-green/4.jpg</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>C1HSSA0546bl-black</t>
+          <t>C1HSSA6020bl-black</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C1HSSA0546bl-black/1.jpg,https://oleks-netizen.github.io/product-images/C1HSSA0546bl-black/2.jpg,https://oleks-netizen.github.io/product-images/C1HSSA0546bl-black/3.jpg,https://oleks-netizen.github.io/product-images/C1HSSA0546bl-black/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C1HSSA6020bl-black/1.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020bl-black/2.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020bl-black/6.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020bl-black/3.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>C1HSSA0546gr-green</t>
+          <t>C1HSSA6020gr-green</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C1HSSA0546gr-green/1.jpg,https://oleks-netizen.github.io/product-images/C1HSSA0546gr-green/2.jpg,https://oleks-netizen.github.io/product-images/C1HSSA0546gr-green/3.jpg,https://oleks-netizen.github.io/product-images/C1HSSA0546gr-green/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C1HSSA6020gr-green/1.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020gr-green/2.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020gr-green/3.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020gr-green/4.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020gr-green/6.jpg</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>C1HSSA6020bl-black</t>
+          <t>C1SA6019bl-black</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C1HSSA6020bl-black/1.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020bl-black/2.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020bl-black/3.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020bl-black/4.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C1SA6019bl-black/1.jpg,https://oleks-netizen.github.io/product-images/C1SA6019bl-black/2.jpg,https://oleks-netizen.github.io/product-images/C1SA6019bl-black/4.jpg,https://oleks-netizen.github.io/product-images/C1SA6019bl-black/6.jpg,https://oleks-netizen.github.io/product-images/C1SA6019bl-black/3.jpg</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -666,27 +666,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>C1HSSA6020gr-green</t>
+          <t>C1SA9208bl-black</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C1HSSA6020gr-green/1.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020gr-green/2.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020gr-green/3.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020gr-green/4.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020gr-green/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C1SA9208bl-black/1.jpg,https://oleks-netizen.github.io/product-images/C1SA9208bl-black/2.jpg,https://oleks-netizen.github.io/product-images/C1SA9208bl-black/3.jpg,https://oleks-netizen.github.io/product-images/C1SA9208bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>C1SA6019bl-black</t>
+          <t>C1YM1725bl-black</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C1SA6019bl-black/1.jpg,https://oleks-netizen.github.io/product-images/C1SA6019bl-black/2.jpg,https://oleks-netizen.github.io/product-images/C1SA6019bl-black/3.jpg,https://oleks-netizen.github.io/product-images/C1SA6019bl-black/4.jpg,https://oleks-netizen.github.io/product-images/C1SA6019bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C1YM1725bl-black/1.jpg,https://oleks-netizen.github.io/product-images/C1YM1725bl-black/2.jpg,https://oleks-netizen.github.io/product-images/C1YM1725bl-black/3.jpg,https://oleks-netizen.github.io/product-images/C1YM1725bl-black/6.jpg,https://oleks-netizen.github.io/product-images/C1YM1725bl-black/4.jpg</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -696,117 +696,117 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>C1SA9208bl-black</t>
+          <t>FA-7122-4x</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C1SA9208bl-black/1.jpg,https://oleks-netizen.github.io/product-images/C1SA9208bl-black/2.jpg,https://oleks-netizen.github.io/product-images/C1SA9208bl-black/3.jpg,https://oleks-netizen.github.io/product-images/C1SA9208bl-black/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/FA-7122-4x/1.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/2.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/3.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/4.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/10.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/6.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/7.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/8.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/9.jpg</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>C1YM1725bl-black</t>
+          <t>JD7348A</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C1YM1725bl-black/1.jpg,https://oleks-netizen.github.io/product-images/C1YM1725bl-black/2.jpg,https://oleks-netizen.github.io/product-images/C1YM1725bl-black/3.jpg,https://oleks-netizen.github.io/product-images/C1YM1725bl-black/4.jpg,https://oleks-netizen.github.io/product-images/C1YM1725bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/JD7348A/2.jpg,https://oleks-netizen.github.io/product-images/JD7348A/3.jpg,https://oleks-netizen.github.io/product-images/JD7348A/5.jpg,https://oleks-netizen.github.io/product-images/JD7348A/4.jpg,https://oleks-netizen.github.io/product-images/JD7348A/6.jpg,https://oleks-netizen.github.io/product-images/JD7348A/7.jpg,https://oleks-netizen.github.io/product-images/JD7348A/9.jpg</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>FA-7122-4x</t>
+          <t>K1266-1bl-black</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/FA-7122-4x/1.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/2.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/3.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/11.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/10.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/5.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/6.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/7.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/8.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K1266-1bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K1266-1bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K1266-1bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K1266-1bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K1266-1bl-black/3.jpg</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>JD7348A</t>
+          <t>K1266-2bl-black</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/JD7348A/1.jpg,https://oleks-netizen.github.io/product-images/JD7348A/2.jpg,https://oleks-netizen.github.io/product-images/JD7348A/10.jpg,https://oleks-netizen.github.io/product-images/JD7348A/3.jpg,https://oleks-netizen.github.io/product-images/JD7348A/4.jpg,https://oleks-netizen.github.io/product-images/JD7348A/6.jpg,https://oleks-netizen.github.io/product-images/JD7348A/7.jpg,https://oleks-netizen.github.io/product-images/JD7348A/8.jpg,https://oleks-netizen.github.io/product-images/JD7348A/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K1266-2bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K1266-2bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K1266-2bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K1266-2bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K1266-2bl-black/4.jpg</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>K1266-1bl-black</t>
+          <t>K1426f-black</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K1266-1bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K1266-1bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K1266-1bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K1266-1bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K1266-1bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K1426f-black/1.jpg,https://oleks-netizen.github.io/product-images/K1426f-black/2.jpg,https://oleks-netizen.github.io/product-images/K1426f-black/5.jpg,https://oleks-netizen.github.io/product-images/K1426f-black/4.jpg</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>K1266-2bl-black</t>
+          <t>K1428f-black</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K1266-2bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K1266-2bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K1266-2bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K1266-2bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K1266-2bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K1428f-black/2.jpg,https://oleks-netizen.github.io/product-images/K1428f-black/3.jpg,https://oleks-netizen.github.io/product-images/K1428f-black/5.jpg,https://oleks-netizen.github.io/product-images/K1428f-black/4.jpg</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>K1426f-black</t>
+          <t>K166030bl-black</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K1426f-black/1.jpg,https://oleks-netizen.github.io/product-images/K1426f-black/2.jpg,https://oleks-netizen.github.io/product-images/K1426f-black/3.jpg,https://oleks-netizen.github.io/product-images/K1426f-black/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K166030bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K166030bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K166030bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K166030bl-black/5.jpg,https://oleks-netizen.github.io/product-images/K166030bl-black/6.jpg</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>K1428f-black</t>
+          <t>K166317bl-black</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K1428f-black/1.jpg,https://oleks-netizen.github.io/product-images/K1428f-black/2.jpg,https://oleks-netizen.github.io/product-images/K1428f-black/3.jpg,https://oleks-netizen.github.io/product-images/K1428f-black/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K166317bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K166317bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K166317bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K166317bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -816,12 +816,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>K166030bl-black</t>
+          <t>K166365bl-black</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K166030bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K166030bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K166030bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K166030bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K166030bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K166365bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K166365bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K166365bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K166365bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K166365bl-black/4.jpg</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -831,27 +831,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>K166317bl-black</t>
+          <t>K16685-1bl-black</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K166317bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K166317bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K166317bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K166317bl-black/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K16685-1bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K16685-1bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K16685-1bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K16685-1bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K16685-1bl-black/4.jpg</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>K166365bl-black</t>
+          <t>K16685-3bl-black</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K166365bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K166365bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K166365bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K166365bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K166365bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K16685-3bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K16685-3bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K16685-3bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K16685-3bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K16685-3bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -861,12 +861,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>K16685-1bl-black</t>
+          <t>K19803-1bl-black</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K16685-1bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K16685-1bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K16685-1bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K16685-1bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K16685-1bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K19803-1bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K19803-1bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K19803-1bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K19803-1bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K19803-1bl-black/6.jpg</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -876,12 +876,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>K16685-3bl-black</t>
+          <t>K19803-1br-brown</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K16685-3bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K16685-3bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K16685-3bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K16685-3bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K16685-3bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K19803-1br-brown/1.jpg,https://oleks-netizen.github.io/product-images/K19803-1br-brown/2.jpg,https://oleks-netizen.github.io/product-images/K19803-1br-brown/3.jpg,https://oleks-netizen.github.io/product-images/K19803-1br-brown/6.jpg,https://oleks-netizen.github.io/product-images/K19803-1br-brown/4.jpg</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -891,12 +891,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>K19803-1bl-black</t>
+          <t>K19803-2bl-black</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K19803-1bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K19803-1bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K19803-1bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K19803-1bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K19803-1bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K19803-2bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K19803-2bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K19803-2bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K19803-2bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K19803-2bl-black/6.jpg</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -906,27 +906,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>K19803-1br-brown</t>
+          <t>LB105 GRY</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K19803-1br-brown/1.jpg,https://oleks-netizen.github.io/product-images/K19803-1br-brown/2.jpg,https://oleks-netizen.github.io/product-images/K19803-1br-brown/3.jpg,https://oleks-netizen.github.io/product-images/K19803-1br-brown/4.jpg,https://oleks-netizen.github.io/product-images/K19803-1br-brown/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LB105 GRY/1.jpg,https://oleks-netizen.github.io/product-images/LB105 GRY/2.jpg,https://oleks-netizen.github.io/product-images/LB105 GRY/3.jpg,https://oleks-netizen.github.io/product-images/LB105 GRY/4.jpg,https://oleks-netizen.github.io/product-images/LB105 GRY/5.jpg,https://oleks-netizen.github.io/product-images/LB105 GRY/6.jpg,https://oleks-netizen.github.io/product-images/LB105 GRY/7.jpg</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>K19803-2bl-black</t>
+          <t>LBJX010013</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K19803-2bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K19803-2bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K19803-2bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K19803-2bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K19803-2bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LBJX010013/2.jpg,https://oleks-netizen.github.io/product-images/LBJX010013/3.jpg,https://oleks-netizen.github.io/product-images/LBJX010013/5.jpg,https://oleks-netizen.github.io/product-images/LBJX010013/6.jpg,https://oleks-netizen.github.io/product-images/LBJX010013/4.jpg</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -936,60 +936,30 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>LB105 GRY</t>
+          <t>RE-3079-3md</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LB105 GRY/1.jpg,https://oleks-netizen.github.io/product-images/LB105 GRY/2.jpg,https://oleks-netizen.github.io/product-images/LB105 GRY/3.jpg,https://oleks-netizen.github.io/product-images/LB105 GRY/4.jpg,https://oleks-netizen.github.io/product-images/LB105 GRY/5.jpg,https://oleks-netizen.github.io/product-images/LB105 GRY/6.jpg,https://oleks-netizen.github.io/product-images/LB105 GRY/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/RE-3079-3md/2.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/4.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/11.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/10.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/3.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/5.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/6.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/7.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/8.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/9.jpg</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>LBJX010013</t>
+          <t>RH-1811-4lx</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LBJX010013/1.jpg,https://oleks-netizen.github.io/product-images/LBJX010013/2.jpg,https://oleks-netizen.github.io/product-images/LBJX010013/6.jpg,https://oleks-netizen.github.io/product-images/LBJX010013/3.jpg,https://oleks-netizen.github.io/product-images/LBJX010013/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/RH-1811-4lx/1.jpg</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>RE-3079-3md</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/RE-3079-3md/1.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/2.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/10.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/3.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/4.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/5.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/6.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/7.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/8.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/9.jpg</t>
-        </is>
-      </c>
-      <c r="C37" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>RH-1811-4lx</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/RH-1811-4lx/1.jpg</t>
-        </is>
-      </c>
-      <c r="C38" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update 2026-02-04 16:32:24
</commit_message>
<xml_diff>
--- a/articles_summary.xlsx
+++ b/articles_summary.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,322 +446,322 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20869_1/1.jpg,https://oleks-netizen.github.io/product-images/20869_1/2.jpg,https://oleks-netizen.github.io/product-images/20869_1/11.jpg,https://oleks-netizen.github.io/product-images/20869_1/3.jpg,https://oleks-netizen.github.io/product-images/20869_1/4.jpg,https://oleks-netizen.github.io/product-images/20869_1/5.jpg,https://oleks-netizen.github.io/product-images/20869_1/6.jpg,https://oleks-netizen.github.io/product-images/20869_1/7.jpg,https://oleks-netizen.github.io/product-images/20869_1/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20869_1/1.jpg,https://oleks-netizen.github.io/product-images/20869_1/2.jpg,https://oleks-netizen.github.io/product-images/20869_1/2.jpg,https://oleks-netizen.github.io/product-images/20869_1/10.jpg,https://oleks-netizen.github.io/product-images/20869_1/11.jpg,https://oleks-netizen.github.io/product-images/20869_1/3.jpg,https://oleks-netizen.github.io/product-images/20869_1/4.jpg,https://oleks-netizen.github.io/product-images/20869_1/5.jpg,https://oleks-netizen.github.io/product-images/20869_1/6.jpg,https://oleks-netizen.github.io/product-images/20869_1/7.jpg,https://oleks-netizen.github.io/product-images/20869_1/8.jpg</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>20869_1_20869_1</t>
+          <t>20871_1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20869_1_20869_1/10.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20871_1/1.jpg,https://oleks-netizen.github.io/product-images/20871_1/2.jpg,https://oleks-netizen.github.io/product-images/20871_1/10.jpg,https://oleks-netizen.github.io/product-images/20871_1/12.jpg,https://oleks-netizen.github.io/product-images/20871_1/11.jpg,https://oleks-netizen.github.io/product-images/20871_1/3.jpg,https://oleks-netizen.github.io/product-images/20871_1/4.jpg,https://oleks-netizen.github.io/product-images/20871_1/5.jpg,https://oleks-netizen.github.io/product-images/20871_1/6.jpg,https://oleks-netizen.github.io/product-images/20871_1/7.jpg,https://oleks-netizen.github.io/product-images/20871_1/8.jpg</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>20871_1</t>
+          <t>23148</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20871_1/1.jpg,https://oleks-netizen.github.io/product-images/20871_1/2.jpg,https://oleks-netizen.github.io/product-images/20871_1/12.jpg,https://oleks-netizen.github.io/product-images/20871_1/11.jpg,https://oleks-netizen.github.io/product-images/20871_1/3.jpg,https://oleks-netizen.github.io/product-images/20871_1/4.jpg,https://oleks-netizen.github.io/product-images/20871_1/5.jpg,https://oleks-netizen.github.io/product-images/20871_1/6.jpg,https://oleks-netizen.github.io/product-images/20871_1/7.jpg,https://oleks-netizen.github.io/product-images/20871_1/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/23148/1.jpg,https://oleks-netizen.github.io/product-images/23148/2.jpg,https://oleks-netizen.github.io/product-images/23148/9.jpg,https://oleks-netizen.github.io/product-images/23148/12.jpg,https://oleks-netizen.github.io/product-images/23148/11.jpg,https://oleks-netizen.github.io/product-images/23148/3.jpg,https://oleks-netizen.github.io/product-images/23148/4.jpg,https://oleks-netizen.github.io/product-images/23148/5.jpg,https://oleks-netizen.github.io/product-images/23148/6.jpg,https://oleks-netizen.github.io/product-images/23148/7.jpg,https://oleks-netizen.github.io/product-images/23148/8.jpg</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>20871_1_20871_1</t>
+          <t>23150</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20871_1_20871_1/10.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/23150/1.jpg,https://oleks-netizen.github.io/product-images/23150/2.jpg,https://oleks-netizen.github.io/product-images/23150/11.jpg,https://oleks-netizen.github.io/product-images/23150/3.jpg,https://oleks-netizen.github.io/product-images/23150/4.jpg,https://oleks-netizen.github.io/product-images/23150/5.jpg,https://oleks-netizen.github.io/product-images/23150/6.jpg,https://oleks-netizen.github.io/product-images/23150/7.jpg,https://oleks-netizen.github.io/product-images/23150/8.jpg</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>23148_23148-Photoroom</t>
+          <t>23152</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/23148_23148-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/23148_23148-Photoroom/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/23152/1.jpg,https://oleks-netizen.github.io/product-images/23152/2.jpg,https://oleks-netizen.github.io/product-images/23152/9.jpg,https://oleks-netizen.github.io/product-images/23152/11.jpg,https://oleks-netizen.github.io/product-images/23152/3.jpg,https://oleks-netizen.github.io/product-images/23152/4.jpg,https://oleks-netizen.github.io/product-images/23152/5.jpg,https://oleks-netizen.github.io/product-images/23152/6.jpg,https://oleks-netizen.github.io/product-images/23152/7.jpg,https://oleks-netizen.github.io/product-images/23152/8.jpg</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>23148</t>
+          <t>51411030m</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/23148/9.jpg,https://oleks-netizen.github.io/product-images/23148/12.jpg,https://oleks-netizen.github.io/product-images/23148/11.jpg,https://oleks-netizen.github.io/product-images/23148/3.jpg,https://oleks-netizen.github.io/product-images/23148/4.jpg,https://oleks-netizen.github.io/product-images/23148/5.jpg,https://oleks-netizen.github.io/product-images/23148/6.jpg,https://oleks-netizen.github.io/product-images/23148/7.jpg,https://oleks-netizen.github.io/product-images/23148/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/51411030m/1.jpg,https://oleks-netizen.github.io/product-images/51411030m/3.jpg,https://oleks-netizen.github.io/product-images/51411030m/3.jpg,https://oleks-netizen.github.io/product-images/51411030m/7.jpg,https://oleks-netizen.github.io/product-images/51411030m/7.jpg,https://oleks-netizen.github.io/product-images/51411030m/4.jpg,https://oleks-netizen.github.io/product-images/51411030m/5.jpg,https://oleks-netizen.github.io/product-images/51411030m/6.jpg</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>23150</t>
+          <t>C1HS1890bl-black</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/23150/1.jpg,https://oleks-netizen.github.io/product-images/23150/2.jpg,https://oleks-netizen.github.io/product-images/23150/11.jpg,https://oleks-netizen.github.io/product-images/23150/3.jpg,https://oleks-netizen.github.io/product-images/23150/4.jpg,https://oleks-netizen.github.io/product-images/23150/5.jpg,https://oleks-netizen.github.io/product-images/23150/6.jpg,https://oleks-netizen.github.io/product-images/23150/7.jpg,https://oleks-netizen.github.io/product-images/23150/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C1HS1890bl-black/1.jpg,https://oleks-netizen.github.io/product-images/C1HS1890bl-black/2.jpg,https://oleks-netizen.github.io/product-images/C1HS1890bl-black/6.jpg,https://oleks-netizen.github.io/product-images/C1HS1890bl-black/3.jpg,https://oleks-netizen.github.io/product-images/C1HS1890bl-black/5.jpg,https://oleks-netizen.github.io/product-images/C1HS1890bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>23152</t>
+          <t>C1HSSA0546bl-black</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/23152/1.jpg,https://oleks-netizen.github.io/product-images/23152/2.jpg,https://oleks-netizen.github.io/product-images/23152/9.jpg,https://oleks-netizen.github.io/product-images/23152/11.jpg,https://oleks-netizen.github.io/product-images/23152/3.jpg,https://oleks-netizen.github.io/product-images/23152/4.jpg,https://oleks-netizen.github.io/product-images/23152/5.jpg,https://oleks-netizen.github.io/product-images/23152/6.jpg,https://oleks-netizen.github.io/product-images/23152/7.jpg,https://oleks-netizen.github.io/product-images/23152/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C1HSSA0546bl-black/1.jpg,https://oleks-netizen.github.io/product-images/C1HSSA0546bl-black/3.jpg,https://oleks-netizen.github.io/product-images/C1HSSA0546bl-black/3.jpg,https://oleks-netizen.github.io/product-images/C1HSSA0546bl-black/5.jpg,https://oleks-netizen.github.io/product-images/C1HSSA0546bl-black/4.jpg</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>51411030m</t>
+          <t>C1HSSA0546gr-green</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/51411030m/1.jpg,https://oleks-netizen.github.io/product-images/51411030m/3.jpg,https://oleks-netizen.github.io/product-images/51411030m/7.jpg,https://oleks-netizen.github.io/product-images/51411030m/4.jpg,https://oleks-netizen.github.io/product-images/51411030m/5.jpg,https://oleks-netizen.github.io/product-images/51411030m/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C1HSSA0546gr-green/1.jpg,https://oleks-netizen.github.io/product-images/C1HSSA0546gr-green/5.jpg,https://oleks-netizen.github.io/product-images/C1HSSA0546gr-green/5.jpg,https://oleks-netizen.github.io/product-images/C1HSSA0546gr-green/3.jpg,https://oleks-netizen.github.io/product-images/C1HSSA0546gr-green/4.jpg</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>C1HS1890bl-black</t>
+          <t>C1HSSA6020bl-black</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C1HS1890bl-black/1.jpg,https://oleks-netizen.github.io/product-images/C1HS1890bl-black/2.jpg,https://oleks-netizen.github.io/product-images/C1HS1890bl-black/6.jpg,https://oleks-netizen.github.io/product-images/C1HS1890bl-black/3.jpg,https://oleks-netizen.github.io/product-images/C1HS1890bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C1HSSA6020bl-black/1.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020bl-black/2.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020bl-black/2.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020bl-black/6.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020bl-black/6.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020bl-black/3.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020bl-black/5.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>C1HSSA0546bl-black</t>
+          <t>C1HSSA6020gr-green</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C1HSSA0546bl-black/1.jpg,https://oleks-netizen.github.io/product-images/C1HSSA0546bl-black/3.jpg,https://oleks-netizen.github.io/product-images/C1HSSA0546bl-black/5.jpg,https://oleks-netizen.github.io/product-images/C1HSSA0546bl-black/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C1HSSA6020gr-green/1.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020gr-green/2.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020gr-green/2.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020gr-green/3.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020gr-green/3.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020gr-green/4.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020gr-green/6.jpg</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>C1HSSA0546gr-green</t>
+          <t>C1SA6019bl-black</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C1HSSA0546gr-green/1.jpg,https://oleks-netizen.github.io/product-images/C1HSSA0546gr-green/5.jpg,https://oleks-netizen.github.io/product-images/C1HSSA0546gr-green/3.jpg,https://oleks-netizen.github.io/product-images/C1HSSA0546gr-green/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C1SA6019bl-black/1.jpg,https://oleks-netizen.github.io/product-images/C1SA6019bl-black/2.jpg,https://oleks-netizen.github.io/product-images/C1SA6019bl-black/2.jpg,https://oleks-netizen.github.io/product-images/C1SA6019bl-black/4.jpg,https://oleks-netizen.github.io/product-images/C1SA6019bl-black/6.jpg,https://oleks-netizen.github.io/product-images/C1SA6019bl-black/3.jpg</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>C1HSSA6020bl-black</t>
+          <t>C1SA9208bl-black</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C1HSSA6020bl-black/1.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020bl-black/2.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020bl-black/6.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020bl-black/3.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C1SA9208bl-black/1.jpg,https://oleks-netizen.github.io/product-images/C1SA9208bl-black/2.jpg,https://oleks-netizen.github.io/product-images/C1SA9208bl-black/3.jpg,https://oleks-netizen.github.io/product-images/C1SA9208bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>C1HSSA6020gr-green</t>
+          <t>C1YM1725bl-black</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C1HSSA6020gr-green/1.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020gr-green/2.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020gr-green/3.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020gr-green/4.jpg,https://oleks-netizen.github.io/product-images/C1HSSA6020gr-green/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C1YM1725bl-black/1.jpg,https://oleks-netizen.github.io/product-images/C1YM1725bl-black/2.jpg,https://oleks-netizen.github.io/product-images/C1YM1725bl-black/2.jpg,https://oleks-netizen.github.io/product-images/C1YM1725bl-black/3.jpg,https://oleks-netizen.github.io/product-images/C1YM1725bl-black/6.jpg,https://oleks-netizen.github.io/product-images/C1YM1725bl-black/4.jpg</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>C1SA6019bl-black</t>
+          <t>FA-7122-4x</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C1SA6019bl-black/1.jpg,https://oleks-netizen.github.io/product-images/C1SA6019bl-black/2.jpg,https://oleks-netizen.github.io/product-images/C1SA6019bl-black/4.jpg,https://oleks-netizen.github.io/product-images/C1SA6019bl-black/6.jpg,https://oleks-netizen.github.io/product-images/C1SA6019bl-black/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/FA-7122-4x/1.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/2.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/3.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/4.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/10.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/6.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/7.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/8.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/9.jpg</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>C1SA9208bl-black</t>
+          <t>JD7348A</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C1SA9208bl-black/1.jpg,https://oleks-netizen.github.io/product-images/C1SA9208bl-black/2.jpg,https://oleks-netizen.github.io/product-images/C1SA9208bl-black/3.jpg,https://oleks-netizen.github.io/product-images/C1SA9208bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/JD7348A/2.jpg,https://oleks-netizen.github.io/product-images/JD7348A/3.jpg,https://oleks-netizen.github.io/product-images/JD7348A/5.jpg,https://oleks-netizen.github.io/product-images/JD7348A/4.jpg,https://oleks-netizen.github.io/product-images/JD7348A/6.jpg,https://oleks-netizen.github.io/product-images/JD7348A/7.jpg,https://oleks-netizen.github.io/product-images/JD7348A/9.jpg</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>C1YM1725bl-black</t>
+          <t>K1266-1bl-black</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C1YM1725bl-black/1.jpg,https://oleks-netizen.github.io/product-images/C1YM1725bl-black/2.jpg,https://oleks-netizen.github.io/product-images/C1YM1725bl-black/3.jpg,https://oleks-netizen.github.io/product-images/C1YM1725bl-black/6.jpg,https://oleks-netizen.github.io/product-images/C1YM1725bl-black/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K1266-1bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K1266-1bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K1266-1bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K1266-1bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K1266-1bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K1266-1bl-black/3.jpg</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>FA-7122-4x</t>
+          <t>K1266-2bl-black</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/FA-7122-4x/1.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/2.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/3.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/4.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/10.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/6.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/7.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/8.jpg,https://oleks-netizen.github.io/product-images/FA-7122-4x/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K1266-2bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K1266-2bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K1266-2bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K1266-2bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K1266-2bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K1266-2bl-black/4.jpg</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>JD7348A</t>
+          <t>K1426f-black</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/JD7348A/2.jpg,https://oleks-netizen.github.io/product-images/JD7348A/3.jpg,https://oleks-netizen.github.io/product-images/JD7348A/5.jpg,https://oleks-netizen.github.io/product-images/JD7348A/4.jpg,https://oleks-netizen.github.io/product-images/JD7348A/6.jpg,https://oleks-netizen.github.io/product-images/JD7348A/7.jpg,https://oleks-netizen.github.io/product-images/JD7348A/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K1426f-black/1.jpg,https://oleks-netizen.github.io/product-images/K1426f-black/2.jpg,https://oleks-netizen.github.io/product-images/K1426f-black/5.jpg,https://oleks-netizen.github.io/product-images/K1426f-black/4.jpg</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>K1266-1bl-black</t>
+          <t>K1428f-black</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K1266-1bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K1266-1bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K1266-1bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K1266-1bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K1266-1bl-black/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K1428f-black/2.jpg,https://oleks-netizen.github.io/product-images/K1428f-black/3.jpg,https://oleks-netizen.github.io/product-images/K1428f-black/5.jpg,https://oleks-netizen.github.io/product-images/K1428f-black/4.jpg</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>K1266-2bl-black</t>
+          <t>K166030bl-black</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K1266-2bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K1266-2bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K1266-2bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K1266-2bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K1266-2bl-black/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K166030bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K166030bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K166030bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K166030bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K166030bl-black/5.jpg,https://oleks-netizen.github.io/product-images/K166030bl-black/6.jpg</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>K1426f-black</t>
+          <t>K166317bl-black</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K1426f-black/1.jpg,https://oleks-netizen.github.io/product-images/K1426f-black/2.jpg,https://oleks-netizen.github.io/product-images/K1426f-black/5.jpg,https://oleks-netizen.github.io/product-images/K1426f-black/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K166317bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K166317bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K166317bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K166317bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -771,117 +771,117 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>K1428f-black</t>
+          <t>K166365bl-black</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K1428f-black/2.jpg,https://oleks-netizen.github.io/product-images/K1428f-black/3.jpg,https://oleks-netizen.github.io/product-images/K1428f-black/5.jpg,https://oleks-netizen.github.io/product-images/K1428f-black/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K166365bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K166365bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K166365bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K166365bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K166365bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K166365bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K166365bl-black/4.jpg</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>K166030bl-black</t>
+          <t>K16685-1bl-black</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K166030bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K166030bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K166030bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K166030bl-black/5.jpg,https://oleks-netizen.github.io/product-images/K166030bl-black/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K16685-1bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K16685-1bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K16685-1bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K16685-1bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K16685-1bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K16685-1bl-black/4.jpg</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>K166317bl-black</t>
+          <t>K16685-3bl-black</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K166317bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K166317bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K166317bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K166317bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K16685-3bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K16685-3bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K16685-3bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K16685-3bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K16685-3bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K16685-3bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>K166365bl-black</t>
+          <t>K19803-1bl-black</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K166365bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K166365bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K166365bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K166365bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K166365bl-black/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K19803-1bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K19803-1bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K19803-1bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K19803-1bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K19803-1bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K19803-1bl-black/6.jpg</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>K16685-1bl-black</t>
+          <t>K19803-1br-brown</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K16685-1bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K16685-1bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K16685-1bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K16685-1bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K16685-1bl-black/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K19803-1br-brown/1.jpg,https://oleks-netizen.github.io/product-images/K19803-1br-brown/2.jpg,https://oleks-netizen.github.io/product-images/K19803-1br-brown/2.jpg,https://oleks-netizen.github.io/product-images/K19803-1br-brown/3.jpg,https://oleks-netizen.github.io/product-images/K19803-1br-brown/6.jpg,https://oleks-netizen.github.io/product-images/K19803-1br-brown/4.jpg</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>K16685-3bl-black</t>
+          <t>K19803-2bl-black</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K16685-3bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K16685-3bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K16685-3bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K16685-3bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K16685-3bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K19803-2bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K19803-2bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K19803-2bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K19803-2bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K19803-2bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K19803-2bl-black/6.jpg</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>K19803-1bl-black</t>
+          <t>LB105 GRY</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K19803-1bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K19803-1bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K19803-1bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K19803-1bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K19803-1bl-black/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LB105 GRY/1.jpg,https://oleks-netizen.github.io/product-images/LB105 GRY/2.jpg,https://oleks-netizen.github.io/product-images/LB105 GRY/3.jpg,https://oleks-netizen.github.io/product-images/LB105 GRY/4.jpg,https://oleks-netizen.github.io/product-images/LB105 GRY/5.jpg,https://oleks-netizen.github.io/product-images/LB105 GRY/6.jpg,https://oleks-netizen.github.io/product-images/LB105 GRY/7.jpg</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>K19803-1br-brown</t>
+          <t>LBJX010013</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K19803-1br-brown/1.jpg,https://oleks-netizen.github.io/product-images/K19803-1br-brown/2.jpg,https://oleks-netizen.github.io/product-images/K19803-1br-brown/3.jpg,https://oleks-netizen.github.io/product-images/K19803-1br-brown/6.jpg,https://oleks-netizen.github.io/product-images/K19803-1br-brown/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LBJX010013/2.jpg,https://oleks-netizen.github.io/product-images/LBJX010013/3.jpg,https://oleks-netizen.github.io/product-images/LBJX010013/5.jpg,https://oleks-netizen.github.io/product-images/LBJX010013/6.jpg,https://oleks-netizen.github.io/product-images/LBJX010013/4.jpg</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -891,75 +891,30 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>K19803-2bl-black</t>
+          <t>RE-3079-3md</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K19803-2bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K19803-2bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K19803-2bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K19803-2bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K19803-2bl-black/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/RE-3079-3md/2.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/4.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/11.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/10.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/3.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/5.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/6.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/7.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/8.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/9.jpg</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>LB105 GRY</t>
+          <t>RH-1811-4lx</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LB105 GRY/1.jpg,https://oleks-netizen.github.io/product-images/LB105 GRY/2.jpg,https://oleks-netizen.github.io/product-images/LB105 GRY/3.jpg,https://oleks-netizen.github.io/product-images/LB105 GRY/4.jpg,https://oleks-netizen.github.io/product-images/LB105 GRY/5.jpg,https://oleks-netizen.github.io/product-images/LB105 GRY/6.jpg,https://oleks-netizen.github.io/product-images/LB105 GRY/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/RH-1811-4lx/1.jpg</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>LBJX010013</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/LBJX010013/2.jpg,https://oleks-netizen.github.io/product-images/LBJX010013/3.jpg,https://oleks-netizen.github.io/product-images/LBJX010013/5.jpg,https://oleks-netizen.github.io/product-images/LBJX010013/6.jpg,https://oleks-netizen.github.io/product-images/LBJX010013/4.jpg</t>
-        </is>
-      </c>
-      <c r="C34" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>RE-3079-3md</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/RE-3079-3md/2.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/4.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/11.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/10.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/3.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/5.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/6.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/7.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/8.jpg,https://oleks-netizen.github.io/product-images/RE-3079-3md/9.jpg</t>
-        </is>
-      </c>
-      <c r="C35" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>RH-1811-4lx</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/RH-1811-4lx/1.jpg</t>
-        </is>
-      </c>
-      <c r="C36" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update 2026-02-18 19:39:16
</commit_message>
<xml_diff>
--- a/articles_summary.xlsx
+++ b/articles_summary.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C141"/>
+  <dimension ref="A1:C128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1191,12 +1191,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>BN-BAG-12-choko-Photoroom</t>
+          <t>BN-BAG-12-choko</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-BAG-12-choko-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-12-choko-Photoroom/2.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-12-choko-Photoroom/5.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-12-choko-Photoroom/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BN-BAG-12-choko/1.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-12-choko/2.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-12-choko/5.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-12-choko/3.jpg</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1206,12 +1206,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>BN-BAG-17-choko-Photoroom</t>
+          <t>BN-BAG-17-choko</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-BAG-17-choko-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-17-choko-Photoroom/2.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-17-choko-Photoroom/6.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-17-choko-Photoroom/4.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-17-choko-Photoroom/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BN-BAG-17-choko/1.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-17-choko/2.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-17-choko/6.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-17-choko/4.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-17-choko/5.jpg</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1326,102 +1326,102 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>BN-BAG-63-p-choko-Photoroom</t>
+          <t>BN-BAG-63-p-choko</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko-Photoroom/2.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko-Photoroom/3.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko-Photoroom/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko/1.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko/2.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko/10.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko/3.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko/5.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko/6.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko/7.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko/8.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko/9.jpg</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>BN-BAG-63-p-choko</t>
+          <t>BN-GC-34-choko</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko/10.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko/5.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko/6.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko/7.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BN-GC-34-choko/2.jpg,https://oleks-netizen.github.io/product-images/BN-GC-34-choko/10.jpg,https://oleks-netizen.github.io/product-images/BN-GC-34-choko/3.jpg,https://oleks-netizen.github.io/product-images/BN-GC-34-choko/4.jpg,https://oleks-netizen.github.io/product-images/BN-GC-34-choko/5.jpg,https://oleks-netizen.github.io/product-images/BN-GC-34-choko/6.jpg,https://oleks-netizen.github.io/product-images/BN-GC-34-choko/7.jpg,https://oleks-netizen.github.io/product-images/BN-GC-34-choko/8.jpg,https://oleks-netizen.github.io/product-images/BN-GC-34-choko/9.jpg</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>BN-GC-34-choko</t>
+          <t>BN-KK-11-nn</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-GC-34-choko/2.jpg,https://oleks-netizen.github.io/product-images/BN-GC-34-choko/10.jpg,https://oleks-netizen.github.io/product-images/BN-GC-34-choko/3.jpg,https://oleks-netizen.github.io/product-images/BN-GC-34-choko/4.jpg,https://oleks-netizen.github.io/product-images/BN-GC-34-choko/5.jpg,https://oleks-netizen.github.io/product-images/BN-GC-34-choko/6.jpg,https://oleks-netizen.github.io/product-images/BN-GC-34-choko/7.jpg,https://oleks-netizen.github.io/product-images/BN-GC-34-choko/8.jpg,https://oleks-netizen.github.io/product-images/BN-GC-34-choko/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BN-KK-11-nn/1.jpg,https://oleks-netizen.github.io/product-images/BN-KK-11-nn/2.jpg,https://oleks-netizen.github.io/product-images/BN-KK-11-nn/9.jpg,https://oleks-netizen.github.io/product-images/BN-KK-11-nn/3.jpg,https://oleks-netizen.github.io/product-images/BN-KK-11-nn/4.jpg,https://oleks-netizen.github.io/product-images/BN-KK-11-nn/6.jpg,https://oleks-netizen.github.io/product-images/BN-KK-11-nn/7.jpg,https://oleks-netizen.github.io/product-images/BN-KK-11-nn/8.jpg</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>BN-KK-11-nn-Photoroom</t>
+          <t>BN-KL-7-g-kr</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-KK-11-nn-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/BN-KK-11-nn-Photoroom/2.jpg,https://oleks-netizen.github.io/product-images/BN-KK-11-nn-Photoroom/3.jpg,https://oleks-netizen.github.io/product-images/BN-KK-11-nn-Photoroom/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BN-KL-7-g-kr/1.jpg,https://oleks-netizen.github.io/product-images/BN-KL-7-g-kr/2.jpg,https://oleks-netizen.github.io/product-images/BN-KL-7-g-kr/3.jpg</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>BN-KK-11-nn</t>
+          <t>CC602_BN</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-KK-11-nn/9.jpg,https://oleks-netizen.github.io/product-images/BN-KK-11-nn/6.jpg,https://oleks-netizen.github.io/product-images/BN-KK-11-nn/7.jpg,https://oleks-netizen.github.io/product-images/BN-KK-11-nn/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/CC602_BN/1.jpg,https://oleks-netizen.github.io/product-images/CC602_BN/2.jpg,https://oleks-netizen.github.io/product-images/CC602_BN/7.jpg,https://oleks-netizen.github.io/product-images/CC602_BN/4.jpg,https://oleks-netizen.github.io/product-images/CC602_BN/5.jpg,https://oleks-netizen.github.io/product-images/CC602_BN/6.jpg</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>BN-KL-7-g-kr</t>
+          <t>CC602_CR_BRN</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-KL-7-g-kr/1.jpg,https://oleks-netizen.github.io/product-images/BN-KL-7-g-kr/2.jpg,https://oleks-netizen.github.io/product-images/BN-KL-7-g-kr/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/CC602_CR_BRN/1.jpg,https://oleks-netizen.github.io/product-images/CC602_CR_BRN/2.jpg,https://oleks-netizen.github.io/product-images/CC602_CR_BRN/4.jpg,https://oleks-netizen.github.io/product-images/CC602_CR_BRN/8.jpg,https://oleks-netizen.github.io/product-images/CC602_CR_BRN/5.jpg,https://oleks-netizen.github.io/product-images/CC602_CR_BRN/6.jpg,https://oleks-netizen.github.io/product-images/CC602_CR_BRN/7.jpg</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>CC602_BN</t>
+          <t>CC607_NPA_BLK</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/CC602_BN/1.jpg,https://oleks-netizen.github.io/product-images/CC602_BN/2.jpg,https://oleks-netizen.github.io/product-images/CC602_BN/7.jpg,https://oleks-netizen.github.io/product-images/CC602_BN/4.jpg,https://oleks-netizen.github.io/product-images/CC602_BN/5.jpg,https://oleks-netizen.github.io/product-images/CC602_BN/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/CC607_NPA_BLK/1.jpg,https://oleks-netizen.github.io/product-images/CC607_NPA_BLK/2.jpg,https://oleks-netizen.github.io/product-images/CC607_NPA_BLK/7.jpg,https://oleks-netizen.github.io/product-images/CC607_NPA_BLK/4.jpg,https://oleks-netizen.github.io/product-images/CC607_NPA_BLK/5.jpg,https://oleks-netizen.github.io/product-images/CC607_NPA_BLK/6.jpg</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -1431,12 +1431,12 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>CC602_CR_BRN</t>
+          <t>FA-7778-4lx</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/CC602_CR_BRN/1.jpg,https://oleks-netizen.github.io/product-images/CC602_CR_BRN/2.jpg,https://oleks-netizen.github.io/product-images/CC602_CR_BRN/4.jpg,https://oleks-netizen.github.io/product-images/CC602_CR_BRN/8.jpg,https://oleks-netizen.github.io/product-images/CC602_CR_BRN/5.jpg,https://oleks-netizen.github.io/product-images/CC602_CR_BRN/6.jpg,https://oleks-netizen.github.io/product-images/CC602_CR_BRN/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/FA-7778-4lx/1.jpg,https://oleks-netizen.github.io/product-images/FA-7778-4lx/2.jpg,https://oleks-netizen.github.io/product-images/FA-7778-4lx/8.jpg,https://oleks-netizen.github.io/product-images/FA-7778-4lx/4.jpg,https://oleks-netizen.github.io/product-images/FA-7778-4lx/5.jpg,https://oleks-netizen.github.io/product-images/FA-7778-4lx/6.jpg,https://oleks-netizen.github.io/product-images/FA-7778-4lx/7.jpg</t>
         </is>
       </c>
       <c r="C68" t="n">
@@ -1446,87 +1446,87 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>CC607_NPA_BLK</t>
+          <t>FC-1819-3md</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/CC607_NPA_BLK/1.jpg,https://oleks-netizen.github.io/product-images/CC607_NPA_BLK/2.jpg,https://oleks-netizen.github.io/product-images/CC607_NPA_BLK/7.jpg,https://oleks-netizen.github.io/product-images/CC607_NPA_BLK/4.jpg,https://oleks-netizen.github.io/product-images/CC607_NPA_BLK/5.jpg,https://oleks-netizen.github.io/product-images/CC607_NPA_BLK/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/FC-1819-3md/1.jpg,https://oleks-netizen.github.io/product-images/FC-1819-3md/2.jpg,https://oleks-netizen.github.io/product-images/FC-1819-3md/3.jpg,https://oleks-netizen.github.io/product-images/FC-1819-3md/6.jpg,https://oleks-netizen.github.io/product-images/FC-1819-3md/5.jpg</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>FA-7778-4lx</t>
+          <t>GC-0041-4lx</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/FA-7778-4lx/1.jpg,https://oleks-netizen.github.io/product-images/FA-7778-4lx/2.jpg,https://oleks-netizen.github.io/product-images/FA-7778-4lx/8.jpg,https://oleks-netizen.github.io/product-images/FA-7778-4lx/4.jpg,https://oleks-netizen.github.io/product-images/FA-7778-4lx/5.jpg,https://oleks-netizen.github.io/product-images/FA-7778-4lx/6.jpg,https://oleks-netizen.github.io/product-images/FA-7778-4lx/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/GC-0041-4lx/1.jpg,https://oleks-netizen.github.io/product-images/GC-0041-4lx/2.jpg,https://oleks-netizen.github.io/product-images/GC-0041-4lx/10.jpg,https://oleks-netizen.github.io/product-images/GC-0041-4lx/4.jpg,https://oleks-netizen.github.io/product-images/GC-0041-4lx/5.jpg,https://oleks-netizen.github.io/product-images/GC-0041-4lx/6.jpg,https://oleks-netizen.github.io/product-images/GC-0041-4lx/7.jpg,https://oleks-netizen.github.io/product-images/GC-0041-4lx/8.jpg,https://oleks-netizen.github.io/product-images/GC-0041-4lx/9.jpg</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>FC-1819-3md</t>
+          <t>JCBBP 71 BLK_YELLOW</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/FC-1819-3md/1.jpg,https://oleks-netizen.github.io/product-images/FC-1819-3md/2.jpg,https://oleks-netizen.github.io/product-images/FC-1819-3md/3.jpg,https://oleks-netizen.github.io/product-images/FC-1819-3md/6.jpg,https://oleks-netizen.github.io/product-images/FC-1819-3md/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/1.jpg,https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/2.jpg,https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/4.jpg,https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/10.jpg,https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/3.jpg,https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/6.jpg,https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/7.jpg,https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/8.jpg,https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/9.jpg</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>GC-0041-4lx</t>
+          <t>L21065-010</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/GC-0041-4lx/1.jpg,https://oleks-netizen.github.io/product-images/GC-0041-4lx/2.jpg,https://oleks-netizen.github.io/product-images/GC-0041-4lx/10.jpg,https://oleks-netizen.github.io/product-images/GC-0041-4lx/4.jpg,https://oleks-netizen.github.io/product-images/GC-0041-4lx/5.jpg,https://oleks-netizen.github.io/product-images/GC-0041-4lx/6.jpg,https://oleks-netizen.github.io/product-images/GC-0041-4lx/7.jpg,https://oleks-netizen.github.io/product-images/GC-0041-4lx/8.jpg,https://oleks-netizen.github.io/product-images/GC-0041-4lx/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21065-010/1.jpg,https://oleks-netizen.github.io/product-images/L21065-010/2.jpg,https://oleks-netizen.github.io/product-images/L21065-010/8.jpg,https://oleks-netizen.github.io/product-images/L21065-010/4.jpg,https://oleks-netizen.github.io/product-images/L21065-010/5.jpg,https://oleks-netizen.github.io/product-images/L21065-010/6.jpg,https://oleks-netizen.github.io/product-images/L21065-010/7.jpg</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>JCBBP 71 BLK_YELLOW</t>
+          <t>L21065-038</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/1.jpg,https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/2.jpg,https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/4.jpg,https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/10.jpg,https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/3.jpg,https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/6.jpg,https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/7.jpg,https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/8.jpg,https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21065-038/1.jpg,https://oleks-netizen.github.io/product-images/L21065-038/2.jpg,https://oleks-netizen.github.io/product-images/L21065-038/8.jpg,https://oleks-netizen.github.io/product-images/L21065-038/4.jpg,https://oleks-netizen.github.io/product-images/L21065-038/5.jpg,https://oleks-netizen.github.io/product-images/L21065-038/6.jpg,https://oleks-netizen.github.io/product-images/L21065-038/7.jpg</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>L21065-010</t>
+          <t>L21065-056</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21065-010/1.jpg,https://oleks-netizen.github.io/product-images/L21065-010/2.jpg,https://oleks-netizen.github.io/product-images/L21065-010/8.jpg,https://oleks-netizen.github.io/product-images/L21065-010/4.jpg,https://oleks-netizen.github.io/product-images/L21065-010/5.jpg,https://oleks-netizen.github.io/product-images/L21065-010/6.jpg,https://oleks-netizen.github.io/product-images/L21065-010/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21065-056/1.jpg,https://oleks-netizen.github.io/product-images/L21065-056/2.jpg,https://oleks-netizen.github.io/product-images/L21065-056/8.jpg,https://oleks-netizen.github.io/product-images/L21065-056/4.jpg,https://oleks-netizen.github.io/product-images/L21065-056/5.jpg,https://oleks-netizen.github.io/product-images/L21065-056/6.jpg,https://oleks-netizen.github.io/product-images/L21065-056/7.jpg</t>
         </is>
       </c>
       <c r="C74" t="n">
@@ -1536,12 +1536,12 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>L21065-038</t>
+          <t>L21065-058</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21065-038/1.jpg,https://oleks-netizen.github.io/product-images/L21065-038/2.jpg,https://oleks-netizen.github.io/product-images/L21065-038/8.jpg,https://oleks-netizen.github.io/product-images/L21065-038/4.jpg,https://oleks-netizen.github.io/product-images/L21065-038/5.jpg,https://oleks-netizen.github.io/product-images/L21065-038/6.jpg,https://oleks-netizen.github.io/product-images/L21065-038/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21065-058/1.jpg,https://oleks-netizen.github.io/product-images/L21065-058/2.jpg,https://oleks-netizen.github.io/product-images/L21065-058/8.jpg,https://oleks-netizen.github.io/product-images/L21065-058/4.jpg,https://oleks-netizen.github.io/product-images/L21065-058/5.jpg,https://oleks-netizen.github.io/product-images/L21065-058/6.jpg,https://oleks-netizen.github.io/product-images/L21065-058/7.jpg</t>
         </is>
       </c>
       <c r="C75" t="n">
@@ -1551,12 +1551,12 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>L21065-056</t>
+          <t>L21567-010</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21065-056/1.jpg,https://oleks-netizen.github.io/product-images/L21065-056/2.jpg,https://oleks-netizen.github.io/product-images/L21065-056/8.jpg,https://oleks-netizen.github.io/product-images/L21065-056/4.jpg,https://oleks-netizen.github.io/product-images/L21065-056/5.jpg,https://oleks-netizen.github.io/product-images/L21065-056/6.jpg,https://oleks-netizen.github.io/product-images/L21065-056/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21567-010/1.jpg,https://oleks-netizen.github.io/product-images/L21567-010/2.jpg,https://oleks-netizen.github.io/product-images/L21567-010/8.jpg,https://oleks-netizen.github.io/product-images/L21567-010/4.jpg,https://oleks-netizen.github.io/product-images/L21567-010/5.jpg,https://oleks-netizen.github.io/product-images/L21567-010/6.jpg,https://oleks-netizen.github.io/product-images/L21567-010/7.jpg</t>
         </is>
       </c>
       <c r="C76" t="n">
@@ -1566,12 +1566,12 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>L21065-058</t>
+          <t>L21567-025</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21065-058/1.jpg,https://oleks-netizen.github.io/product-images/L21065-058/2.jpg,https://oleks-netizen.github.io/product-images/L21065-058/8.jpg,https://oleks-netizen.github.io/product-images/L21065-058/4.jpg,https://oleks-netizen.github.io/product-images/L21065-058/5.jpg,https://oleks-netizen.github.io/product-images/L21065-058/6.jpg,https://oleks-netizen.github.io/product-images/L21065-058/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21567-025/1.jpg,https://oleks-netizen.github.io/product-images/L21567-025/2.jpg,https://oleks-netizen.github.io/product-images/L21567-025/8.jpg,https://oleks-netizen.github.io/product-images/L21567-025/4.jpg,https://oleks-netizen.github.io/product-images/L21567-025/5.jpg,https://oleks-netizen.github.io/product-images/L21567-025/6.jpg,https://oleks-netizen.github.io/product-images/L21567-025/7.jpg</t>
         </is>
       </c>
       <c r="C77" t="n">
@@ -1581,72 +1581,72 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>L21567-010-Photoroom</t>
+          <t>L21575-010</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21567-010-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/L21567-010-Photoroom/8.jpg,https://oleks-netizen.github.io/product-images/L21567-010-Photoroom/4.jpg,https://oleks-netizen.github.io/product-images/L21567-010-Photoroom/5.jpg,https://oleks-netizen.github.io/product-images/L21567-010-Photoroom/6.jpg,https://oleks-netizen.github.io/product-images/L21567-010-Photoroom/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21575-010/1.jpg,https://oleks-netizen.github.io/product-images/L21575-010/2.jpg,https://oleks-netizen.github.io/product-images/L21575-010/8.jpg,https://oleks-netizen.github.io/product-images/L21575-010/4.jpg,https://oleks-netizen.github.io/product-images/L21575-010/5.jpg,https://oleks-netizen.github.io/product-images/L21575-010/6.jpg,https://oleks-netizen.github.io/product-images/L21575-010/7.jpg</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>L21567-010</t>
+          <t>L21575-038</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21567-010/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21575-038/1.jpg,https://oleks-netizen.github.io/product-images/L21575-038/2.jpg,https://oleks-netizen.github.io/product-images/L21575-038/8.jpg,https://oleks-netizen.github.io/product-images/L21575-038/4.jpg,https://oleks-netizen.github.io/product-images/L21575-038/5.jpg,https://oleks-netizen.github.io/product-images/L21575-038/6.jpg,https://oleks-netizen.github.io/product-images/L21575-038/7.jpg</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>L21567-025-Photoroom</t>
+          <t>L21586-010</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21567-025-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/L21567-025-Photoroom/8.jpg,https://oleks-netizen.github.io/product-images/L21567-025-Photoroom/4.jpg,https://oleks-netizen.github.io/product-images/L21567-025-Photoroom/5.jpg,https://oleks-netizen.github.io/product-images/L21567-025-Photoroom/6.jpg,https://oleks-netizen.github.io/product-images/L21567-025-Photoroom/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21586-010/1.jpg,https://oleks-netizen.github.io/product-images/L21586-010/2.jpg,https://oleks-netizen.github.io/product-images/L21586-010/8.jpg,https://oleks-netizen.github.io/product-images/L21586-010/4.jpg,https://oleks-netizen.github.io/product-images/L21586-010/5.jpg,https://oleks-netizen.github.io/product-images/L21586-010/6.jpg,https://oleks-netizen.github.io/product-images/L21586-010/7.jpg</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>L21567-025</t>
+          <t>L21586-025</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21567-025/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21586-025/1.jpg,https://oleks-netizen.github.io/product-images/L21586-025/2.jpg,https://oleks-netizen.github.io/product-images/L21586-025/8.jpg,https://oleks-netizen.github.io/product-images/L21586-025/4.jpg,https://oleks-netizen.github.io/product-images/L21586-025/5.jpg,https://oleks-netizen.github.io/product-images/L21586-025/6.jpg,https://oleks-netizen.github.io/product-images/L21586-025/7.jpg</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>L21575-010</t>
+          <t>L21586-097</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21575-010/1.jpg,https://oleks-netizen.github.io/product-images/L21575-010/2.jpg,https://oleks-netizen.github.io/product-images/L21575-010/8.jpg,https://oleks-netizen.github.io/product-images/L21575-010/4.jpg,https://oleks-netizen.github.io/product-images/L21575-010/5.jpg,https://oleks-netizen.github.io/product-images/L21575-010/6.jpg,https://oleks-netizen.github.io/product-images/L21575-010/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L21586-097/1.jpg,https://oleks-netizen.github.io/product-images/L21586-097/2.jpg,https://oleks-netizen.github.io/product-images/L21586-097/8.jpg,https://oleks-netizen.github.io/product-images/L21586-097/4.jpg,https://oleks-netizen.github.io/product-images/L21586-097/5.jpg,https://oleks-netizen.github.io/product-images/L21586-097/6.jpg,https://oleks-netizen.github.io/product-images/L21586-097/7.jpg</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -1656,312 +1656,312 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>L21575-038-Photoroom</t>
+          <t>LC69004-01</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21575-038-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/L21575-038-Photoroom/8.jpg,https://oleks-netizen.github.io/product-images/L21575-038-Photoroom/4.jpg,https://oleks-netizen.github.io/product-images/L21575-038-Photoroom/5.jpg,https://oleks-netizen.github.io/product-images/L21575-038-Photoroom/6.jpg,https://oleks-netizen.github.io/product-images/L21575-038-Photoroom/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC69004-01/1.jpg,https://oleks-netizen.github.io/product-images/LC69004-01/2.jpg,https://oleks-netizen.github.io/product-images/LC69004-01/9.jpg,https://oleks-netizen.github.io/product-images/LC69004-01/4.jpg,https://oleks-netizen.github.io/product-images/LC69004-01/5.jpg,https://oleks-netizen.github.io/product-images/LC69004-01/6.jpg,https://oleks-netizen.github.io/product-images/LC69004-01/7.jpg,https://oleks-netizen.github.io/product-images/LC69004-01/8.jpg</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>L21575-038</t>
+          <t>LC69004-02</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21575-038/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC69004-02/1.jpg,https://oleks-netizen.github.io/product-images/LC69004-02/2.jpg,https://oleks-netizen.github.io/product-images/LC69004-02/9.jpg,https://oleks-netizen.github.io/product-images/LC69004-02/4.jpg,https://oleks-netizen.github.io/product-images/LC69004-02/5.jpg,https://oleks-netizen.github.io/product-images/LC69004-02/6.jpg,https://oleks-netizen.github.io/product-images/LC69004-02/7.jpg,https://oleks-netizen.github.io/product-images/LC69004-02/8.jpg</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>L21586-010-Photoroom</t>
+          <t>LC69004-03</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21586-010-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/L21586-010-Photoroom/8.jpg,https://oleks-netizen.github.io/product-images/L21586-010-Photoroom/4.jpg,https://oleks-netizen.github.io/product-images/L21586-010-Photoroom/5.jpg,https://oleks-netizen.github.io/product-images/L21586-010-Photoroom/6.jpg,https://oleks-netizen.github.io/product-images/L21586-010-Photoroom/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC69004-03/1.jpg,https://oleks-netizen.github.io/product-images/LC69004-03/2.jpg,https://oleks-netizen.github.io/product-images/LC69004-03/9.jpg,https://oleks-netizen.github.io/product-images/LC69004-03/4.jpg,https://oleks-netizen.github.io/product-images/LC69004-03/5.jpg,https://oleks-netizen.github.io/product-images/LC69004-03/6.jpg,https://oleks-netizen.github.io/product-images/LC69004-03/7.jpg,https://oleks-netizen.github.io/product-images/LC69004-03/8.jpg</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>L21586-010</t>
+          <t>LC69004-04</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21586-010/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC69004-04/1.jpg,https://oleks-netizen.github.io/product-images/LC69004-04/2.jpg,https://oleks-netizen.github.io/product-images/LC69004-04/9.jpg,https://oleks-netizen.github.io/product-images/LC69004-04/4.jpg,https://oleks-netizen.github.io/product-images/LC69004-04/5.jpg,https://oleks-netizen.github.io/product-images/LC69004-04/6.jpg,https://oleks-netizen.github.io/product-images/LC69004-04/7.jpg,https://oleks-netizen.github.io/product-images/LC69004-04/8.jpg</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>L21586-025</t>
+          <t>LC69033-01</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21586-025/1.jpg,https://oleks-netizen.github.io/product-images/L21586-025/2.jpg,https://oleks-netizen.github.io/product-images/L21586-025/8.jpg,https://oleks-netizen.github.io/product-images/L21586-025/4.jpg,https://oleks-netizen.github.io/product-images/L21586-025/5.jpg,https://oleks-netizen.github.io/product-images/L21586-025/6.jpg,https://oleks-netizen.github.io/product-images/L21586-025/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC69033-01/1.jpg,https://oleks-netizen.github.io/product-images/LC69033-01/2.jpg,https://oleks-netizen.github.io/product-images/LC69033-01/9.jpg,https://oleks-netizen.github.io/product-images/LC69033-01/4.jpg,https://oleks-netizen.github.io/product-images/LC69033-01/5.jpg,https://oleks-netizen.github.io/product-images/LC69033-01/6.jpg,https://oleks-netizen.github.io/product-images/LC69033-01/7.jpg,https://oleks-netizen.github.io/product-images/LC69033-01/8.jpg</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>L21586-097-Photoroom</t>
+          <t>LC69033-05</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21586-097-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/L21586-097-Photoroom/8.jpg,https://oleks-netizen.github.io/product-images/L21586-097-Photoroom/4.jpg,https://oleks-netizen.github.io/product-images/L21586-097-Photoroom/5.jpg,https://oleks-netizen.github.io/product-images/L21586-097-Photoroom/6.jpg,https://oleks-netizen.github.io/product-images/L21586-097-Photoroom/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC69033-05/1.jpg,https://oleks-netizen.github.io/product-images/LC69033-05/2.jpg,https://oleks-netizen.github.io/product-images/LC69033-05/9.jpg,https://oleks-netizen.github.io/product-images/LC69033-05/4.jpg,https://oleks-netizen.github.io/product-images/LC69033-05/5.jpg,https://oleks-netizen.github.io/product-images/LC69033-05/6.jpg,https://oleks-netizen.github.io/product-images/LC69033-05/7.jpg,https://oleks-netizen.github.io/product-images/LC69033-05/8.jpg</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>L21586-097</t>
+          <t>LC69033-28</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21586-097/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC69033-28/1.jpg,https://oleks-netizen.github.io/product-images/LC69033-28/2.jpg,https://oleks-netizen.github.io/product-images/LC69033-28/3.jpg,https://oleks-netizen.github.io/product-images/LC69033-28/4.jpg,https://oleks-netizen.github.io/product-images/LC69033-28/5.jpg,https://oleks-netizen.github.io/product-images/LC69033-28/6.jpg,https://oleks-netizen.github.io/product-images/LC69033-28/8.jpg</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>LC69004-01-Photoroom</t>
+          <t>LC69033-41</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69004-01-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/LC69004-01-Photoroom/9.jpg,https://oleks-netizen.github.io/product-images/LC69004-01-Photoroom/4.jpg,https://oleks-netizen.github.io/product-images/LC69004-01-Photoroom/5.jpg,https://oleks-netizen.github.io/product-images/LC69004-01-Photoroom/6.jpg,https://oleks-netizen.github.io/product-images/LC69004-01-Photoroom/7.jpg,https://oleks-netizen.github.io/product-images/LC69004-01-Photoroom/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC69033-41/1.jpg,https://oleks-netizen.github.io/product-images/LC69033-41/2.jpg,https://oleks-netizen.github.io/product-images/LC69033-41/9.jpg,https://oleks-netizen.github.io/product-images/LC69033-41/4.jpg,https://oleks-netizen.github.io/product-images/LC69033-41/5.jpg,https://oleks-netizen.github.io/product-images/LC69033-41/6.jpg,https://oleks-netizen.github.io/product-images/LC69033-41/7.jpg,https://oleks-netizen.github.io/product-images/LC69033-41/8.jpg</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>LC69004-01</t>
+          <t>LC69033-71</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69004-01/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC69033-71/1.jpg,https://oleks-netizen.github.io/product-images/LC69033-71/2.jpg,https://oleks-netizen.github.io/product-images/LC69033-71/3.jpg,https://oleks-netizen.github.io/product-images/LC69033-71/9.jpg,https://oleks-netizen.github.io/product-images/LC69033-71/4.jpg,https://oleks-netizen.github.io/product-images/LC69033-71/5.jpg,https://oleks-netizen.github.io/product-images/LC69033-71/6.jpg,https://oleks-netizen.github.io/product-images/LC69033-71/8.jpg</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>LC69004-02-Photoroom</t>
+          <t>LC69052-2035</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69004-02-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/LC69004-02-Photoroom/9.jpg,https://oleks-netizen.github.io/product-images/LC69004-02-Photoroom/4.jpg,https://oleks-netizen.github.io/product-images/LC69004-02-Photoroom/5.jpg,https://oleks-netizen.github.io/product-images/LC69004-02-Photoroom/6.jpg,https://oleks-netizen.github.io/product-images/LC69004-02-Photoroom/7.jpg,https://oleks-netizen.github.io/product-images/LC69004-02-Photoroom/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC69052-2035/1.jpg,https://oleks-netizen.github.io/product-images/LC69052-2035/2.jpg,https://oleks-netizen.github.io/product-images/LC69052-2035/3.jpg,https://oleks-netizen.github.io/product-images/LC69052-2035/9.jpg,https://oleks-netizen.github.io/product-images/LC69052-2035/4.jpg,https://oleks-netizen.github.io/product-images/LC69052-2035/5.jpg,https://oleks-netizen.github.io/product-images/LC69052-2035/6.jpg,https://oleks-netizen.github.io/product-images/LC69052-2035/8.jpg</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>LC69004-02</t>
+          <t>LC69052-2036</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69004-02/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC69052-2036/1.jpg,https://oleks-netizen.github.io/product-images/LC69052-2036/2.jpg,https://oleks-netizen.github.io/product-images/LC69052-2036/3.jpg,https://oleks-netizen.github.io/product-images/LC69052-2036/9.jpg,https://oleks-netizen.github.io/product-images/LC69052-2036/4.jpg,https://oleks-netizen.github.io/product-images/LC69052-2036/5.jpg,https://oleks-netizen.github.io/product-images/LC69052-2036/6.jpg,https://oleks-netizen.github.io/product-images/LC69052-2036/8.jpg</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>LC69004-03-Photoroom</t>
+          <t>LC69052-2058</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69004-03-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/LC69004-03-Photoroom/9.jpg,https://oleks-netizen.github.io/product-images/LC69004-03-Photoroom/4.jpg,https://oleks-netizen.github.io/product-images/LC69004-03-Photoroom/5.jpg,https://oleks-netizen.github.io/product-images/LC69004-03-Photoroom/6.jpg,https://oleks-netizen.github.io/product-images/LC69004-03-Photoroom/7.jpg,https://oleks-netizen.github.io/product-images/LC69004-03-Photoroom/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC69052-2058/1.jpg,https://oleks-netizen.github.io/product-images/LC69052-2058/2.jpg,https://oleks-netizen.github.io/product-images/LC69052-2058/3.jpg,https://oleks-netizen.github.io/product-images/LC69052-2058/9.jpg,https://oleks-netizen.github.io/product-images/LC69052-2058/4.jpg,https://oleks-netizen.github.io/product-images/LC69052-2058/5.jpg,https://oleks-netizen.github.io/product-images/LC69052-2058/6.jpg,https://oleks-netizen.github.io/product-images/LC69052-2058/8.jpg</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>LC69004-03</t>
+          <t>LC69052-2259</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69004-03/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC69052-2259/1.jpg,https://oleks-netizen.github.io/product-images/LC69052-2259/2.jpg,https://oleks-netizen.github.io/product-images/LC69052-2259/3.jpg,https://oleks-netizen.github.io/product-images/LC69052-2259/9.jpg,https://oleks-netizen.github.io/product-images/LC69052-2259/4.jpg,https://oleks-netizen.github.io/product-images/LC69052-2259/5.jpg,https://oleks-netizen.github.io/product-images/LC69052-2259/6.jpg,https://oleks-netizen.github.io/product-images/LC69052-2259/8.jpg</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>LC69004-04-Photoroom</t>
+          <t>LC69055-01</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69004-04-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/LC69004-04-Photoroom/9.jpg,https://oleks-netizen.github.io/product-images/LC69004-04-Photoroom/4.jpg,https://oleks-netizen.github.io/product-images/LC69004-04-Photoroom/5.jpg,https://oleks-netizen.github.io/product-images/LC69004-04-Photoroom/6.jpg,https://oleks-netizen.github.io/product-images/LC69004-04-Photoroom/7.jpg,https://oleks-netizen.github.io/product-images/LC69004-04-Photoroom/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC69055-01/1.jpg,https://oleks-netizen.github.io/product-images/LC69055-01/2.jpg,https://oleks-netizen.github.io/product-images/LC69055-01/3.jpg,https://oleks-netizen.github.io/product-images/LC69055-01/9.jpg,https://oleks-netizen.github.io/product-images/LC69055-01/4.jpg,https://oleks-netizen.github.io/product-images/LC69055-01/5.jpg,https://oleks-netizen.github.io/product-images/LC69055-01/6.jpg,https://oleks-netizen.github.io/product-images/LC69055-01/8.jpg</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>LC69004-04</t>
+          <t>LC69055-26</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69004-04/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC69055-26/1.jpg,https://oleks-netizen.github.io/product-images/LC69055-26/2.jpg,https://oleks-netizen.github.io/product-images/LC69055-26/9.jpg,https://oleks-netizen.github.io/product-images/LC69055-26/3.jpg,https://oleks-netizen.github.io/product-images/LC69055-26/4.jpg,https://oleks-netizen.github.io/product-images/LC69055-26/5.jpg,https://oleks-netizen.github.io/product-images/LC69055-26/6.jpg,https://oleks-netizen.github.io/product-images/LC69055-26/8.jpg</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>LC69033-01-Photoroom</t>
+          <t>LC69055-71</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69033-01-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/LC69033-01-Photoroom/9.jpg,https://oleks-netizen.github.io/product-images/LC69033-01-Photoroom/4.jpg,https://oleks-netizen.github.io/product-images/LC69033-01-Photoroom/5.jpg,https://oleks-netizen.github.io/product-images/LC69033-01-Photoroom/6.jpg,https://oleks-netizen.github.io/product-images/LC69033-01-Photoroom/7.jpg,https://oleks-netizen.github.io/product-images/LC69033-01-Photoroom/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC69055-71/1.jpg,https://oleks-netizen.github.io/product-images/LC69055-71/2.jpg,https://oleks-netizen.github.io/product-images/LC69055-71/9.jpg,https://oleks-netizen.github.io/product-images/LC69055-71/3.jpg,https://oleks-netizen.github.io/product-images/LC69055-71/4.jpg,https://oleks-netizen.github.io/product-images/LC69055-71/5.jpg,https://oleks-netizen.github.io/product-images/LC69055-71/6.jpg,https://oleks-netizen.github.io/product-images/LC69055-71/8.jpg</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>LC69033-01</t>
+          <t>LC69055-76</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69033-01/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC69055-76/1.jpg,https://oleks-netizen.github.io/product-images/LC69055-76/2.jpg,https://oleks-netizen.github.io/product-images/LC69055-76/9.jpg,https://oleks-netizen.github.io/product-images/LC69055-76/3.jpg,https://oleks-netizen.github.io/product-images/LC69055-76/4.jpg,https://oleks-netizen.github.io/product-images/LC69055-76/5.jpg,https://oleks-netizen.github.io/product-images/LC69055-76/6.jpg,https://oleks-netizen.github.io/product-images/LC69055-76/8.jpg</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>LC69033-05-Photoroom</t>
+          <t>LC69055-84</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69033-05-Photoroom/1.jpg,https://oleks-netizen.github.io/product-images/LC69033-05-Photoroom/9.jpg,https://oleks-netizen.github.io/product-images/LC69033-05-Photoroom/4.jpg,https://oleks-netizen.github.io/product-images/LC69033-05-Photoroom/5.jpg,https://oleks-netizen.github.io/product-images/LC69033-05-Photoroom/6.jpg,https://oleks-netizen.github.io/product-images/LC69033-05-Photoroom/7.jpg,https://oleks-netizen.github.io/product-images/LC69033-05-Photoroom/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC69055-84/1.jpg,https://oleks-netizen.github.io/product-images/LC69055-84/2.jpg,https://oleks-netizen.github.io/product-images/LC69055-84/9.jpg,https://oleks-netizen.github.io/product-images/LC69055-84/3.jpg,https://oleks-netizen.github.io/product-images/LC69055-84/4.jpg,https://oleks-netizen.github.io/product-images/LC69055-84/5.jpg,https://oleks-netizen.github.io/product-images/LC69055-84/6.jpg,https://oleks-netizen.github.io/product-images/LC69055-84/8.jpg</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>LC69033-05</t>
+          <t>LC69802-01</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69033-05/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC69802-01/1.jpg,https://oleks-netizen.github.io/product-images/LC69802-01/2.jpg,https://oleks-netizen.github.io/product-images/LC69802-01/3.jpg,https://oleks-netizen.github.io/product-images/LC69802-01/9.jpg,https://oleks-netizen.github.io/product-images/LC69802-01/4.jpg,https://oleks-netizen.github.io/product-images/LC69802-01/5.jpg,https://oleks-netizen.github.io/product-images/LC69802-01/6.jpg,https://oleks-netizen.github.io/product-images/LC69802-01/8.jpg</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>LC69033-28</t>
+          <t>LC69802-12</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69033-28/1.jpg,https://oleks-netizen.github.io/product-images/LC69033-28/2.jpg,https://oleks-netizen.github.io/product-images/LC69033-28/3.jpg,https://oleks-netizen.github.io/product-images/LC69033-28/4.jpg,https://oleks-netizen.github.io/product-images/LC69033-28/5.jpg,https://oleks-netizen.github.io/product-images/LC69033-28/6.jpg,https://oleks-netizen.github.io/product-images/LC69033-28/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC69802-12/1.jpg,https://oleks-netizen.github.io/product-images/LC69802-12/2.jpg,https://oleks-netizen.github.io/product-images/LC69802-12/3.jpg,https://oleks-netizen.github.io/product-images/LC69802-12/9.jpg,https://oleks-netizen.github.io/product-images/LC69802-12/4.jpg,https://oleks-netizen.github.io/product-images/LC69802-12/5.jpg,https://oleks-netizen.github.io/product-images/LC69802-12/6.jpg,https://oleks-netizen.github.io/product-images/LC69802-12/8.jpg</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>LC69033-41</t>
+          <t>LC69802-25</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69033-41/1.jpg,https://oleks-netizen.github.io/product-images/LC69033-41/2.jpg,https://oleks-netizen.github.io/product-images/LC69033-41/9.jpg,https://oleks-netizen.github.io/product-images/LC69033-41/4.jpg,https://oleks-netizen.github.io/product-images/LC69033-41/5.jpg,https://oleks-netizen.github.io/product-images/LC69033-41/6.jpg,https://oleks-netizen.github.io/product-images/LC69033-41/7.jpg,https://oleks-netizen.github.io/product-images/LC69033-41/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC69802-25/1.jpg,https://oleks-netizen.github.io/product-images/LC69802-25/2.jpg,https://oleks-netizen.github.io/product-images/LC69802-25/9.jpg,https://oleks-netizen.github.io/product-images/LC69802-25/4.jpg,https://oleks-netizen.github.io/product-images/LC69802-25/5.jpg,https://oleks-netizen.github.io/product-images/LC69802-25/6.jpg,https://oleks-netizen.github.io/product-images/LC69802-25/7.jpg,https://oleks-netizen.github.io/product-images/LC69802-25/8.jpg</t>
         </is>
       </c>
       <c r="C103" t="n">
@@ -1971,12 +1971,12 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>LC69033-71</t>
+          <t>LC69802-71</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69033-71/1.jpg,https://oleks-netizen.github.io/product-images/LC69033-71/2.jpg,https://oleks-netizen.github.io/product-images/LC69033-71/3.jpg,https://oleks-netizen.github.io/product-images/LC69033-71/9.jpg,https://oleks-netizen.github.io/product-images/LC69033-71/4.jpg,https://oleks-netizen.github.io/product-images/LC69033-71/5.jpg,https://oleks-netizen.github.io/product-images/LC69033-71/6.jpg,https://oleks-netizen.github.io/product-images/LC69033-71/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC69802-71/1.jpg,https://oleks-netizen.github.io/product-images/LC69802-71/2.jpg,https://oleks-netizen.github.io/product-images/LC69802-71/3.jpg,https://oleks-netizen.github.io/product-images/LC69802-71/9.jpg,https://oleks-netizen.github.io/product-images/LC69802-71/4.jpg,https://oleks-netizen.github.io/product-images/LC69802-71/5.jpg,https://oleks-netizen.github.io/product-images/LC69802-71/6.jpg,https://oleks-netizen.github.io/product-images/LC69802-71/8.jpg</t>
         </is>
       </c>
       <c r="C104" t="n">
@@ -1986,12 +1986,12 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>LC69052-2035</t>
+          <t>LC69855-2058</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69052-2035/1.jpg,https://oleks-netizen.github.io/product-images/LC69052-2035/2.jpg,https://oleks-netizen.github.io/product-images/LC69052-2035/3.jpg,https://oleks-netizen.github.io/product-images/LC69052-2035/9.jpg,https://oleks-netizen.github.io/product-images/LC69052-2035/4.jpg,https://oleks-netizen.github.io/product-images/LC69052-2035/5.jpg,https://oleks-netizen.github.io/product-images/LC69052-2035/6.jpg,https://oleks-netizen.github.io/product-images/LC69052-2035/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC69855-2058/1.jpg,https://oleks-netizen.github.io/product-images/LC69855-2058/2.jpg,https://oleks-netizen.github.io/product-images/LC69855-2058/3.jpg,https://oleks-netizen.github.io/product-images/LC69855-2058/9.jpg,https://oleks-netizen.github.io/product-images/LC69855-2058/4.jpg,https://oleks-netizen.github.io/product-images/LC69855-2058/5.jpg,https://oleks-netizen.github.io/product-images/LC69855-2058/6.jpg,https://oleks-netizen.github.io/product-images/LC69855-2058/8.jpg</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -2001,27 +2001,27 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>LC69052-2036</t>
+          <t>LC69855-2259</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69052-2036/1.jpg,https://oleks-netizen.github.io/product-images/LC69052-2036/2.jpg,https://oleks-netizen.github.io/product-images/LC69052-2036/3.jpg,https://oleks-netizen.github.io/product-images/LC69052-2036/9.jpg,https://oleks-netizen.github.io/product-images/LC69052-2036/4.jpg,https://oleks-netizen.github.io/product-images/LC69052-2036/5.jpg,https://oleks-netizen.github.io/product-images/LC69052-2036/6.jpg,https://oleks-netizen.github.io/product-images/LC69052-2036/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC69855-2259/1.jpg,https://oleks-netizen.github.io/product-images/LC69855-2259/2.jpg,https://oleks-netizen.github.io/product-images/LC69855-2259/8.jpg,https://oleks-netizen.github.io/product-images/LC69855-2259/4.jpg,https://oleks-netizen.github.io/product-images/LC69855-2259/5.jpg,https://oleks-netizen.github.io/product-images/LC69855-2259/6.jpg,https://oleks-netizen.github.io/product-images/LC69855-2259/7.jpg</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>LC69052-2058</t>
+          <t>LC69855-2291</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69052-2058/1.jpg,https://oleks-netizen.github.io/product-images/LC69052-2058/2.jpg,https://oleks-netizen.github.io/product-images/LC69052-2058/3.jpg,https://oleks-netizen.github.io/product-images/LC69052-2058/9.jpg,https://oleks-netizen.github.io/product-images/LC69052-2058/4.jpg,https://oleks-netizen.github.io/product-images/LC69052-2058/5.jpg,https://oleks-netizen.github.io/product-images/LC69052-2058/6.jpg,https://oleks-netizen.github.io/product-images/LC69052-2058/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC69855-2291/1.jpg,https://oleks-netizen.github.io/product-images/LC69855-2291/2.jpg,https://oleks-netizen.github.io/product-images/LC69855-2291/9.jpg,https://oleks-netizen.github.io/product-images/LC69855-2291/4.jpg,https://oleks-netizen.github.io/product-images/LC69855-2291/5.jpg,https://oleks-netizen.github.io/product-images/LC69855-2291/6.jpg,https://oleks-netizen.github.io/product-images/LC69855-2291/7.jpg,https://oleks-netizen.github.io/product-images/LC69855-2291/8.jpg</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -2031,117 +2031,117 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>LC69052-2259</t>
+          <t>RB-8033-4lx</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69052-2259/1.jpg,https://oleks-netizen.github.io/product-images/LC69052-2259/2.jpg,https://oleks-netizen.github.io/product-images/LC69052-2259/3.jpg,https://oleks-netizen.github.io/product-images/LC69052-2259/9.jpg,https://oleks-netizen.github.io/product-images/LC69052-2259/4.jpg,https://oleks-netizen.github.io/product-images/LC69052-2259/5.jpg,https://oleks-netizen.github.io/product-images/LC69052-2259/6.jpg,https://oleks-netizen.github.io/product-images/LC69052-2259/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/RB-8033-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RB-8033-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RB-8033-4lx/6.jpg,https://oleks-netizen.github.io/product-images/RB-8033-4lx/4.jpg,https://oleks-netizen.github.io/product-images/RB-8033-4lx/5.jpg</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>LC69055-01</t>
+          <t>RC-3990-3md</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69055-01/1.jpg,https://oleks-netizen.github.io/product-images/LC69055-01/2.jpg,https://oleks-netizen.github.io/product-images/LC69055-01/3.jpg,https://oleks-netizen.github.io/product-images/LC69055-01/9.jpg,https://oleks-netizen.github.io/product-images/LC69055-01/4.jpg,https://oleks-netizen.github.io/product-images/LC69055-01/5.jpg,https://oleks-netizen.github.io/product-images/LC69055-01/6.jpg,https://oleks-netizen.github.io/product-images/LC69055-01/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/RC-3990-3md/1.jpg,https://oleks-netizen.github.io/product-images/RC-3990-3md/2.jpg,https://oleks-netizen.github.io/product-images/RC-3990-3md/4.jpg,https://oleks-netizen.github.io/product-images/RC-3990-3md/10.jpg,https://oleks-netizen.github.io/product-images/RC-3990-3md/5.jpg,https://oleks-netizen.github.io/product-images/RC-3990-3md/6.jpg,https://oleks-netizen.github.io/product-images/RC-3990-3md/7.jpg,https://oleks-netizen.github.io/product-images/RC-3990-3md/8.jpg,https://oleks-netizen.github.io/product-images/RC-3990-3md/9.jpg</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>LC69055-26</t>
+          <t>RC-60125-3md</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69055-26/1.jpg,https://oleks-netizen.github.io/product-images/LC69055-26/2.jpg,https://oleks-netizen.github.io/product-images/LC69055-26/9.jpg,https://oleks-netizen.github.io/product-images/LC69055-26/3.jpg,https://oleks-netizen.github.io/product-images/LC69055-26/4.jpg,https://oleks-netizen.github.io/product-images/LC69055-26/5.jpg,https://oleks-netizen.github.io/product-images/LC69055-26/6.jpg,https://oleks-netizen.github.io/product-images/LC69055-26/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/RC-60125-3md/1.jpg,https://oleks-netizen.github.io/product-images/RC-60125-3md/2.jpg,https://oleks-netizen.github.io/product-images/RC-60125-3md/7.jpg,https://oleks-netizen.github.io/product-images/RC-60125-3md/4.jpg,https://oleks-netizen.github.io/product-images/RC-60125-3md/5.jpg,https://oleks-netizen.github.io/product-images/RC-60125-3md/6.jpg</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>LC69055-71</t>
+          <t>RCc-1313-4lx</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69055-71/1.jpg,https://oleks-netizen.github.io/product-images/LC69055-71/2.jpg,https://oleks-netizen.github.io/product-images/LC69055-71/9.jpg,https://oleks-netizen.github.io/product-images/LC69055-71/3.jpg,https://oleks-netizen.github.io/product-images/LC69055-71/4.jpg,https://oleks-netizen.github.io/product-images/LC69055-71/5.jpg,https://oleks-netizen.github.io/product-images/LC69055-71/6.jpg,https://oleks-netizen.github.io/product-images/LC69055-71/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/RCc-1313-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RCc-1313-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RCc-1313-4lx/8.jpg,https://oleks-netizen.github.io/product-images/RCc-1313-4lx/3.jpg,https://oleks-netizen.github.io/product-images/RCc-1313-4lx/4.jpg,https://oleks-netizen.github.io/product-images/RCc-1313-4lx/5.jpg,https://oleks-netizen.github.io/product-images/RCc-1313-4lx/6.jpg</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>LC69055-76</t>
+          <t>RCh-1313-4lx</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69055-76/1.jpg,https://oleks-netizen.github.io/product-images/LC69055-76/2.jpg,https://oleks-netizen.github.io/product-images/LC69055-76/9.jpg,https://oleks-netizen.github.io/product-images/LC69055-76/3.jpg,https://oleks-netizen.github.io/product-images/LC69055-76/4.jpg,https://oleks-netizen.github.io/product-images/LC69055-76/5.jpg,https://oleks-netizen.github.io/product-images/LC69055-76/6.jpg,https://oleks-netizen.github.io/product-images/LC69055-76/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/RCh-1313-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RCh-1313-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RCh-1313-4lx/6.jpg,https://oleks-netizen.github.io/product-images/RCh-1313-4lx/3.jpg,https://oleks-netizen.github.io/product-images/RCh-1313-4lx/4.jpg</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>LC69055-84</t>
+          <t>RCj-0320-4lx</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69055-84/1.jpg,https://oleks-netizen.github.io/product-images/LC69055-84/2.jpg,https://oleks-netizen.github.io/product-images/LC69055-84/9.jpg,https://oleks-netizen.github.io/product-images/LC69055-84/3.jpg,https://oleks-netizen.github.io/product-images/LC69055-84/4.jpg,https://oleks-netizen.github.io/product-images/LC69055-84/5.jpg,https://oleks-netizen.github.io/product-images/LC69055-84/6.jpg,https://oleks-netizen.github.io/product-images/LC69055-84/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/RCj-0320-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RCj-0320-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RCj-0320-4lx/6.jpg,https://oleks-netizen.github.io/product-images/RCj-0320-4lx/4.jpg,https://oleks-netizen.github.io/product-images/RCj-0320-4lx/5.jpg</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>LC69802-01</t>
+          <t>RCj-1313-4lx</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69802-01/1.jpg,https://oleks-netizen.github.io/product-images/LC69802-01/2.jpg,https://oleks-netizen.github.io/product-images/LC69802-01/3.jpg,https://oleks-netizen.github.io/product-images/LC69802-01/9.jpg,https://oleks-netizen.github.io/product-images/LC69802-01/4.jpg,https://oleks-netizen.github.io/product-images/LC69802-01/5.jpg,https://oleks-netizen.github.io/product-images/LC69802-01/6.jpg,https://oleks-netizen.github.io/product-images/LC69802-01/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/RCj-1313-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RCj-1313-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RCj-1313-4lx/6.jpg,https://oleks-netizen.github.io/product-images/RCj-1313-4lx/3.jpg,https://oleks-netizen.github.io/product-images/RCj-1313-4lx/4.jpg</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>LC69802-12</t>
+          <t>RE-0001-4lx</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69802-12/1.jpg,https://oleks-netizen.github.io/product-images/LC69802-12/2.jpg,https://oleks-netizen.github.io/product-images/LC69802-12/3.jpg,https://oleks-netizen.github.io/product-images/LC69802-12/9.jpg,https://oleks-netizen.github.io/product-images/LC69802-12/4.jpg,https://oleks-netizen.github.io/product-images/LC69802-12/5.jpg,https://oleks-netizen.github.io/product-images/LC69802-12/6.jpg,https://oleks-netizen.github.io/product-images/LC69802-12/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/RE-0001-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RE-0001-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RE-0001-4lx/9.jpg,https://oleks-netizen.github.io/product-images/RE-0001-4lx/4.jpg,https://oleks-netizen.github.io/product-images/RE-0001-4lx/5.jpg,https://oleks-netizen.github.io/product-images/RE-0001-4lx/6.jpg,https://oleks-netizen.github.io/product-images/RE-0001-4lx/7.jpg,https://oleks-netizen.github.io/product-images/RE-0001-4lx/8.jpg</t>
         </is>
       </c>
       <c r="C115" t="n">
@@ -2151,72 +2151,72 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>LC69802-25</t>
+          <t>RE-60125-3md</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69802-25/1.jpg,https://oleks-netizen.github.io/product-images/LC69802-25/2.jpg,https://oleks-netizen.github.io/product-images/LC69802-25/9.jpg,https://oleks-netizen.github.io/product-images/LC69802-25/4.jpg,https://oleks-netizen.github.io/product-images/LC69802-25/5.jpg,https://oleks-netizen.github.io/product-images/LC69802-25/6.jpg,https://oleks-netizen.github.io/product-images/LC69802-25/7.jpg,https://oleks-netizen.github.io/product-images/LC69802-25/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/RE-60125-3md/1.jpg,https://oleks-netizen.github.io/product-images/RE-60125-3md/2.jpg,https://oleks-netizen.github.io/product-images/RE-60125-3md/7.jpg,https://oleks-netizen.github.io/product-images/RE-60125-3md/3.jpg,https://oleks-netizen.github.io/product-images/RE-60125-3md/4.jpg,https://oleks-netizen.github.io/product-images/RE-60125-3md/5.jpg</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>LC69802-71</t>
+          <t>RK-60125-3md</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69802-71/1.jpg,https://oleks-netizen.github.io/product-images/LC69802-71/2.jpg,https://oleks-netizen.github.io/product-images/LC69802-71/3.jpg,https://oleks-netizen.github.io/product-images/LC69802-71/9.jpg,https://oleks-netizen.github.io/product-images/LC69802-71/4.jpg,https://oleks-netizen.github.io/product-images/LC69802-71/5.jpg,https://oleks-netizen.github.io/product-images/LC69802-71/6.jpg,https://oleks-netizen.github.io/product-images/LC69802-71/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/RK-60125-3md/1.jpg,https://oleks-netizen.github.io/product-images/RK-60125-3md/2.jpg,https://oleks-netizen.github.io/product-images/RK-60125-3md/7.jpg,https://oleks-netizen.github.io/product-images/RK-60125-3md/4.jpg,https://oleks-netizen.github.io/product-images/RK-60125-3md/5.jpg,https://oleks-netizen.github.io/product-images/RK-60125-3md/6.jpg</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>LC69855-2058</t>
+          <t>RY-1819-3md</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69855-2058/1.jpg,https://oleks-netizen.github.io/product-images/LC69855-2058/2.jpg,https://oleks-netizen.github.io/product-images/LC69855-2058/3.jpg,https://oleks-netizen.github.io/product-images/LC69855-2058/9.jpg,https://oleks-netizen.github.io/product-images/LC69855-2058/4.jpg,https://oleks-netizen.github.io/product-images/LC69855-2058/5.jpg,https://oleks-netizen.github.io/product-images/LC69855-2058/6.jpg,https://oleks-netizen.github.io/product-images/LC69855-2058/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/RY-1819-3md/1.jpg,https://oleks-netizen.github.io/product-images/RY-1819-3md/7.jpg,https://oleks-netizen.github.io/product-images/RY-1819-3md/8.jpg,https://oleks-netizen.github.io/product-images/RY-1819-3md/3.jpg,https://oleks-netizen.github.io/product-images/RY-1819-3md/4.jpg,https://oleks-netizen.github.io/product-images/RY-1819-3md/5.jpg,https://oleks-netizen.github.io/product-images/RY-1819-3md/6.jpg</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>LC69855-2259</t>
+          <t>RА-60121-3md</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69855-2259/1.jpg,https://oleks-netizen.github.io/product-images/LC69855-2259/2.jpg,https://oleks-netizen.github.io/product-images/LC69855-2259/8.jpg,https://oleks-netizen.github.io/product-images/LC69855-2259/4.jpg,https://oleks-netizen.github.io/product-images/LC69855-2259/5.jpg,https://oleks-netizen.github.io/product-images/LC69855-2259/6.jpg,https://oleks-netizen.github.io/product-images/LC69855-2259/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/RА-60121-3md/1.jpg,https://oleks-netizen.github.io/product-images/RА-60121-3md/2.jpg,https://oleks-netizen.github.io/product-images/RА-60121-3md/5.jpg,https://oleks-netizen.github.io/product-images/RА-60121-3md/9.jpg,https://oleks-netizen.github.io/product-images/RА-60121-3md/3.jpg,https://oleks-netizen.github.io/product-images/RА-60121-3md/4.jpg,https://oleks-netizen.github.io/product-images/RА-60121-3md/6.jpg,https://oleks-netizen.github.io/product-images/RА-60121-3md/7.jpg</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>LC69855-2291</t>
+          <t>RЕ-60121-3md</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69855-2291/1.jpg,https://oleks-netizen.github.io/product-images/LC69855-2291/2.jpg,https://oleks-netizen.github.io/product-images/LC69855-2291/9.jpg,https://oleks-netizen.github.io/product-images/LC69855-2291/4.jpg,https://oleks-netizen.github.io/product-images/LC69855-2291/5.jpg,https://oleks-netizen.github.io/product-images/LC69855-2291/6.jpg,https://oleks-netizen.github.io/product-images/LC69855-2291/7.jpg,https://oleks-netizen.github.io/product-images/LC69855-2291/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/RЕ-60121-3md/1.jpg,https://oleks-netizen.github.io/product-images/RЕ-60121-3md/2.jpg,https://oleks-netizen.github.io/product-images/RЕ-60121-3md/5.jpg,https://oleks-netizen.github.io/product-images/RЕ-60121-3md/9.jpg,https://oleks-netizen.github.io/product-images/RЕ-60121-3md/3.jpg,https://oleks-netizen.github.io/product-images/RЕ-60121-3md/4.jpg,https://oleks-netizen.github.io/product-images/RЕ-60121-3md/6.jpg,https://oleks-netizen.github.io/product-images/RЕ-60121-3md/7.jpg</t>
         </is>
       </c>
       <c r="C120" t="n">
@@ -2226,315 +2226,120 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>RB-8033-4lx</t>
+          <t>RК-60121-3md</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RB-8033-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RB-8033-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RB-8033-4lx/6.jpg,https://oleks-netizen.github.io/product-images/RB-8033-4lx/4.jpg,https://oleks-netizen.github.io/product-images/RB-8033-4lx/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/RК-60121-3md/1.jpg,https://oleks-netizen.github.io/product-images/RК-60121-3md/2.jpg,https://oleks-netizen.github.io/product-images/RК-60121-3md/5.jpg,https://oleks-netizen.github.io/product-images/RК-60121-3md/9.jpg,https://oleks-netizen.github.io/product-images/RК-60121-3md/3.jpg,https://oleks-netizen.github.io/product-images/RК-60121-3md/4.jpg,https://oleks-netizen.github.io/product-images/RК-60121-3md/6.jpg,https://oleks-netizen.github.io/product-images/RК-60121-3md/7.jpg</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>RC-3990-3md</t>
+          <t>TW-Explorer-S-brown</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RC-3990-3md/1.jpg,https://oleks-netizen.github.io/product-images/RC-3990-3md/2.jpg,https://oleks-netizen.github.io/product-images/RC-3990-3md/4.jpg,https://oleks-netizen.github.io/product-images/RC-3990-3md/10.jpg,https://oleks-netizen.github.io/product-images/RC-3990-3md/5.jpg,https://oleks-netizen.github.io/product-images/RC-3990-3md/6.jpg,https://oleks-netizen.github.io/product-images/RC-3990-3md/7.jpg,https://oleks-netizen.github.io/product-images/RC-3990-3md/8.jpg,https://oleks-netizen.github.io/product-images/RC-3990-3md/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/TW-Explorer-S-brown/1.jpg,https://oleks-netizen.github.io/product-images/TW-Explorer-S-brown/2.jpg,https://oleks-netizen.github.io/product-images/TW-Explorer-S-brown/5.jpg,https://oleks-netizen.github.io/product-images/TW-Explorer-S-brown/3.jpg</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>RC-60125-3md</t>
+          <t>TW-Explorer-S-dark-blue</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RC-60125-3md/1.jpg,https://oleks-netizen.github.io/product-images/RC-60125-3md/2.jpg,https://oleks-netizen.github.io/product-images/RC-60125-3md/7.jpg,https://oleks-netizen.github.io/product-images/RC-60125-3md/4.jpg,https://oleks-netizen.github.io/product-images/RC-60125-3md/5.jpg,https://oleks-netizen.github.io/product-images/RC-60125-3md/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/TW-Explorer-S-dark-blue/1.jpg,https://oleks-netizen.github.io/product-images/TW-Explorer-S-dark-blue/2.jpg,https://oleks-netizen.github.io/product-images/TW-Explorer-S-dark-blue/5.jpg,https://oleks-netizen.github.io/product-images/TW-Explorer-S-dark-blue/3.jpg</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>RCc-1313-4lx</t>
+          <t>TW-Lina-black-flo</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RCc-1313-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RCc-1313-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RCc-1313-4lx/8.jpg,https://oleks-netizen.github.io/product-images/RCc-1313-4lx/3.jpg,https://oleks-netizen.github.io/product-images/RCc-1313-4lx/4.jpg,https://oleks-netizen.github.io/product-images/RCc-1313-4lx/5.jpg,https://oleks-netizen.github.io/product-images/RCc-1313-4lx/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/TW-Lina-black-flo/1.jpg,https://oleks-netizen.github.io/product-images/TW-Lina-black-flo/9.jpg,https://oleks-netizen.github.io/product-images/TW-Lina-black-flo/3.jpg,https://oleks-netizen.github.io/product-images/TW-Lina-black-flo/4.jpg,https://oleks-netizen.github.io/product-images/TW-Lina-black-flo/5.jpg,https://oleks-netizen.github.io/product-images/TW-Lina-black-flo/6.jpg,https://oleks-netizen.github.io/product-images/TW-Lina-black-flo/7.jpg,https://oleks-netizen.github.io/product-images/TW-Lina-black-flo/8.jpg</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>RCh-1313-4lx</t>
+          <t>TW-Mini-bag-m-black</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RCh-1313-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RCh-1313-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RCh-1313-4lx/6.jpg,https://oleks-netizen.github.io/product-images/RCh-1313-4lx/3.jpg,https://oleks-netizen.github.io/product-images/RCh-1313-4lx/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/TW-Mini-bag-m-black/1.jpg</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>RCj-0320-4lx</t>
+          <t>TW-Nancy-1-caramel</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RCj-0320-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RCj-0320-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RCj-0320-4lx/6.jpg,https://oleks-netizen.github.io/product-images/RCj-0320-4lx/4.jpg,https://oleks-netizen.github.io/product-images/RCj-0320-4lx/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/TW-Nancy-1-caramel/1.jpg,https://oleks-netizen.github.io/product-images/TW-Nancy-1-caramel/2.jpg,https://oleks-netizen.github.io/product-images/TW-Nancy-1-caramel/7.jpg,https://oleks-netizen.github.io/product-images/TW-Nancy-1-caramel/3.jpg,https://oleks-netizen.github.io/product-images/TW-Nancy-1-caramel/4.jpg,https://oleks-netizen.github.io/product-images/TW-Nancy-1-caramel/5.jpg</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>RCj-1313-4lx</t>
+          <t>TW-Walker-mokko</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RCj-1313-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RCj-1313-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RCj-1313-4lx/6.jpg,https://oleks-netizen.github.io/product-images/RCj-1313-4lx/3.jpg,https://oleks-netizen.github.io/product-images/RCj-1313-4lx/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/TW-Walker-mokko/1.jpg,https://oleks-netizen.github.io/product-images/TW-Walker-mokko/2.jpg,https://oleks-netizen.github.io/product-images/TW-Walker-mokko/5.jpg,https://oleks-netizen.github.io/product-images/TW-Walker-mokko/3.jpg</t>
         </is>
       </c>
       <c r="C127" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>RE-0001-4lx</t>
+          <t>Y1311 45</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RE-0001-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RE-0001-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RE-0001-4lx/9.jpg,https://oleks-netizen.github.io/product-images/RE-0001-4lx/4.jpg,https://oleks-netizen.github.io/product-images/RE-0001-4lx/5.jpg,https://oleks-netizen.github.io/product-images/RE-0001-4lx/6.jpg,https://oleks-netizen.github.io/product-images/RE-0001-4lx/7.jpg,https://oleks-netizen.github.io/product-images/RE-0001-4lx/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/Y1311 45/1.jpg,https://oleks-netizen.github.io/product-images/Y1311 45/2.jpg,https://oleks-netizen.github.io/product-images/Y1311 45/5.jpg,https://oleks-netizen.github.io/product-images/Y1311 45/3.jpg</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" t="inlineStr">
-        <is>
-          <t>RE-60125-3md</t>
-        </is>
-      </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/RE-60125-3md/1.jpg,https://oleks-netizen.github.io/product-images/RE-60125-3md/2.jpg,https://oleks-netizen.github.io/product-images/RE-60125-3md/7.jpg,https://oleks-netizen.github.io/product-images/RE-60125-3md/3.jpg,https://oleks-netizen.github.io/product-images/RE-60125-3md/4.jpg,https://oleks-netizen.github.io/product-images/RE-60125-3md/5.jpg</t>
-        </is>
-      </c>
-      <c r="C129" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" t="inlineStr">
-        <is>
-          <t>RK-60125-3md</t>
-        </is>
-      </c>
-      <c r="B130" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/RK-60125-3md/1.jpg,https://oleks-netizen.github.io/product-images/RK-60125-3md/2.jpg,https://oleks-netizen.github.io/product-images/RK-60125-3md/7.jpg,https://oleks-netizen.github.io/product-images/RK-60125-3md/4.jpg,https://oleks-netizen.github.io/product-images/RK-60125-3md/5.jpg,https://oleks-netizen.github.io/product-images/RK-60125-3md/6.jpg</t>
-        </is>
-      </c>
-      <c r="C130" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" t="inlineStr">
-        <is>
-          <t>RY-1819-3md</t>
-        </is>
-      </c>
-      <c r="B131" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/RY-1819-3md/1.jpg,https://oleks-netizen.github.io/product-images/RY-1819-3md/7.jpg,https://oleks-netizen.github.io/product-images/RY-1819-3md/8.jpg,https://oleks-netizen.github.io/product-images/RY-1819-3md/3.jpg,https://oleks-netizen.github.io/product-images/RY-1819-3md/4.jpg,https://oleks-netizen.github.io/product-images/RY-1819-3md/5.jpg,https://oleks-netizen.github.io/product-images/RY-1819-3md/6.jpg</t>
-        </is>
-      </c>
-      <c r="C131" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" t="inlineStr">
-        <is>
-          <t>RА-60121-3md</t>
-        </is>
-      </c>
-      <c r="B132" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/RА-60121-3md/1.jpg,https://oleks-netizen.github.io/product-images/RА-60121-3md/2.jpg,https://oleks-netizen.github.io/product-images/RА-60121-3md/5.jpg,https://oleks-netizen.github.io/product-images/RА-60121-3md/9.jpg,https://oleks-netizen.github.io/product-images/RА-60121-3md/3.jpg,https://oleks-netizen.github.io/product-images/RА-60121-3md/4.jpg,https://oleks-netizen.github.io/product-images/RА-60121-3md/6.jpg,https://oleks-netizen.github.io/product-images/RА-60121-3md/7.jpg</t>
-        </is>
-      </c>
-      <c r="C132" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" t="inlineStr">
-        <is>
-          <t>RЕ-60121-3md</t>
-        </is>
-      </c>
-      <c r="B133" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/RЕ-60121-3md/1.jpg,https://oleks-netizen.github.io/product-images/RЕ-60121-3md/2.jpg,https://oleks-netizen.github.io/product-images/RЕ-60121-3md/5.jpg,https://oleks-netizen.github.io/product-images/RЕ-60121-3md/9.jpg,https://oleks-netizen.github.io/product-images/RЕ-60121-3md/3.jpg,https://oleks-netizen.github.io/product-images/RЕ-60121-3md/4.jpg,https://oleks-netizen.github.io/product-images/RЕ-60121-3md/6.jpg,https://oleks-netizen.github.io/product-images/RЕ-60121-3md/7.jpg</t>
-        </is>
-      </c>
-      <c r="C133" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" t="inlineStr">
-        <is>
-          <t>RК-60121-3md</t>
-        </is>
-      </c>
-      <c r="B134" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/RК-60121-3md/1.jpg,https://oleks-netizen.github.io/product-images/RК-60121-3md/2.jpg,https://oleks-netizen.github.io/product-images/RК-60121-3md/5.jpg,https://oleks-netizen.github.io/product-images/RК-60121-3md/9.jpg,https://oleks-netizen.github.io/product-images/RК-60121-3md/3.jpg,https://oleks-netizen.github.io/product-images/RК-60121-3md/4.jpg,https://oleks-netizen.github.io/product-images/RК-60121-3md/6.jpg,https://oleks-netizen.github.io/product-images/RК-60121-3md/7.jpg</t>
-        </is>
-      </c>
-      <c r="C134" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" t="inlineStr">
-        <is>
-          <t>TW-Explorer-S-brown</t>
-        </is>
-      </c>
-      <c r="B135" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-Explorer-S-brown/1.jpg,https://oleks-netizen.github.io/product-images/TW-Explorer-S-brown/2.jpg,https://oleks-netizen.github.io/product-images/TW-Explorer-S-brown/5.jpg,https://oleks-netizen.github.io/product-images/TW-Explorer-S-brown/3.jpg</t>
-        </is>
-      </c>
-      <c r="C135" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" t="inlineStr">
-        <is>
-          <t>TW-Explorer-S-dark-blue</t>
-        </is>
-      </c>
-      <c r="B136" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-Explorer-S-dark-blue/1.jpg,https://oleks-netizen.github.io/product-images/TW-Explorer-S-dark-blue/2.jpg,https://oleks-netizen.github.io/product-images/TW-Explorer-S-dark-blue/5.jpg,https://oleks-netizen.github.io/product-images/TW-Explorer-S-dark-blue/3.jpg</t>
-        </is>
-      </c>
-      <c r="C136" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" t="inlineStr">
-        <is>
-          <t>TW-Lina-black-flo</t>
-        </is>
-      </c>
-      <c r="B137" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-Lina-black-flo/1.jpg,https://oleks-netizen.github.io/product-images/TW-Lina-black-flo/9.jpg,https://oleks-netizen.github.io/product-images/TW-Lina-black-flo/3.jpg,https://oleks-netizen.github.io/product-images/TW-Lina-black-flo/4.jpg,https://oleks-netizen.github.io/product-images/TW-Lina-black-flo/5.jpg,https://oleks-netizen.github.io/product-images/TW-Lina-black-flo/6.jpg,https://oleks-netizen.github.io/product-images/TW-Lina-black-flo/7.jpg,https://oleks-netizen.github.io/product-images/TW-Lina-black-flo/8.jpg</t>
-        </is>
-      </c>
-      <c r="C137" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" t="inlineStr">
-        <is>
-          <t>TW-Mini-bag-m-black</t>
-        </is>
-      </c>
-      <c r="B138" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-Mini-bag-m-black/1.jpg</t>
-        </is>
-      </c>
-      <c r="C138" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" t="inlineStr">
-        <is>
-          <t>TW-Nancy-1-caramel</t>
-        </is>
-      </c>
-      <c r="B139" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-Nancy-1-caramel/1.jpg,https://oleks-netizen.github.io/product-images/TW-Nancy-1-caramel/2.jpg,https://oleks-netizen.github.io/product-images/TW-Nancy-1-caramel/7.jpg,https://oleks-netizen.github.io/product-images/TW-Nancy-1-caramel/3.jpg,https://oleks-netizen.github.io/product-images/TW-Nancy-1-caramel/4.jpg,https://oleks-netizen.github.io/product-images/TW-Nancy-1-caramel/5.jpg</t>
-        </is>
-      </c>
-      <c r="C139" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" t="inlineStr">
-        <is>
-          <t>TW-Walker-mokko</t>
-        </is>
-      </c>
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-Walker-mokko/1.jpg,https://oleks-netizen.github.io/product-images/TW-Walker-mokko/2.jpg,https://oleks-netizen.github.io/product-images/TW-Walker-mokko/5.jpg,https://oleks-netizen.github.io/product-images/TW-Walker-mokko/3.jpg</t>
-        </is>
-      </c>
-      <c r="C140" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" t="inlineStr">
-        <is>
-          <t>Y1311 45</t>
-        </is>
-      </c>
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>https://oleks-netizen.github.io/product-images/Y1311 45/1.jpg,https://oleks-netizen.github.io/product-images/Y1311 45/2.jpg,https://oleks-netizen.github.io/product-images/Y1311 45/5.jpg,https://oleks-netizen.github.io/product-images/Y1311 45/3.jpg</t>
-        </is>
-      </c>
-      <c r="C141" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update 2026-02-27 16:44:37
</commit_message>
<xml_diff>
--- a/articles_summary.xlsx
+++ b/articles_summary.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C128"/>
+  <dimension ref="A1:C163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,957 +441,957 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1110_1_128</t>
+          <t>11711719</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/1110_1_128/1.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/11711719/1.jpg,https://oleks-netizen.github.io/product-images/11711719/2.jpg,https://oleks-netizen.github.io/product-images/11711719/3.jpg,https://oleks-netizen.github.io/product-images/11711719/11.jpg,https://oleks-netizen.github.io/product-images/11711719/10.jpg,https://oleks-netizen.github.io/product-images/11711719/4.jpg,https://oleks-netizen.github.io/product-images/11711719/5.jpg,https://oleks-netizen.github.io/product-images/11711719/6.jpg,https://oleks-netizen.github.io/product-images/11711719/8.jpg,https://oleks-netizen.github.io/product-images/11711719/9.jpg</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1121820891</t>
+          <t>11711719m</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/1121820891/1.jpg,https://oleks-netizen.github.io/product-images/1121820891/2.jpg,https://oleks-netizen.github.io/product-images/1121820891/3.jpg,https://oleks-netizen.github.io/product-images/1121820891/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/11711719m/1.jpg,https://oleks-netizen.github.io/product-images/11711719m/2.jpg,https://oleks-netizen.github.io/product-images/11711719m/9.jpg,https://oleks-netizen.github.io/product-images/11711719m/3.jpg,https://oleks-netizen.github.io/product-images/11711719m/4.jpg,https://oleks-netizen.github.io/product-images/11711719m/5.jpg,https://oleks-netizen.github.io/product-images/11711719m/7.jpg,https://oleks-netizen.github.io/product-images/11711719m/8.jpg</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1121820892</t>
+          <t>11nero</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/1121820892/1.jpg,https://oleks-netizen.github.io/product-images/1121820892/2.jpg,https://oleks-netizen.github.io/product-images/1121820892/3.jpg,https://oleks-netizen.github.io/product-images/1121820892/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/11nero/1.jpg,https://oleks-netizen.github.io/product-images/11nero/2.jpg</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1121820894</t>
+          <t>1352_1_2</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/1121820894/1.jpg,https://oleks-netizen.github.io/product-images/1121820894/2.jpg,https://oleks-netizen.github.io/product-images/1121820894/3.jpg,https://oleks-netizen.github.io/product-images/1121820894/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/1352_1_2/1.jpg</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1144-05-32</t>
+          <t>1531_1_4</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/1144-05-32/1.jpg,https://oleks-netizen.github.io/product-images/1144-05-32/2.jpg,https://oleks-netizen.github.io/product-images/1144-05-32/6.jpg,https://oleks-netizen.github.io/product-images/1144-05-32/3.jpg,https://oleks-netizen.github.io/product-images/1144-05-32/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/1531_1_4/1.jpg</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1144-06-32</t>
+          <t>1602060006</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/1144-06-32/1.jpg,https://oleks-netizen.github.io/product-images/1144-06-32/2.jpg,https://oleks-netizen.github.io/product-images/1144-06-32/6.jpg,https://oleks-netizen.github.io/product-images/1144-06-32/3.jpg,https://oleks-netizen.github.io/product-images/1144-06-32/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/1602060006/1.jpg,https://oleks-netizen.github.io/product-images/1602060006/2.jpg</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1144-11-32</t>
+          <t>25000030m</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/1144-11-32/1.jpg,https://oleks-netizen.github.io/product-images/1144-11-32/2.jpg,https://oleks-netizen.github.io/product-images/1144-11-32/6.jpg,https://oleks-netizen.github.io/product-images/1144-11-32/3.jpg,https://oleks-netizen.github.io/product-images/1144-11-32/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/25000030m/1.jpg,https://oleks-netizen.github.io/product-images/25000030m/2.jpg,https://oleks-netizen.github.io/product-images/25000030m/16.jpg,https://oleks-netizen.github.io/product-images/25000030m/10.jpg,https://oleks-netizen.github.io/product-images/25000030m/11.jpg,https://oleks-netizen.github.io/product-images/25000030m/12.jpg,https://oleks-netizen.github.io/product-images/25000030m/13.jpg,https://oleks-netizen.github.io/product-images/25000030m/14.jpg,https://oleks-netizen.github.io/product-images/25000030m/15.jpg,https://oleks-netizen.github.io/product-images/25000030m/3.jpg,https://oleks-netizen.github.io/product-images/25000030m/4.jpg,https://oleks-netizen.github.io/product-images/25000030m/5.jpg,https://oleks-netizen.github.io/product-images/25000030m/6.jpg,https://oleks-netizen.github.io/product-images/25000030m/8.jpg,https://oleks-netizen.github.io/product-images/25000030m/9.jpg</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1144-27-32</t>
+          <t>4041nero</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/1144-27-32/1.jpg,https://oleks-netizen.github.io/product-images/1144-27-32/2.jpg,https://oleks-netizen.github.io/product-images/1144-27-32/6.jpg,https://oleks-netizen.github.io/product-images/1144-27-32/3.jpg,https://oleks-netizen.github.io/product-images/1144-27-32/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/4041nero/1.jpg,https://oleks-netizen.github.io/product-images/4041nero/2.jpg</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1631_1_6</t>
+          <t>5196801</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/1631_1_6/1.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/5196801/1.jpg,https://oleks-netizen.github.io/product-images/5196801/2.jpg,https://oleks-netizen.github.io/product-images/5196801/7.jpg,https://oleks-netizen.github.io/product-images/5196801/11.jpg,https://oleks-netizen.github.io/product-images/5196801/10.jpg,https://oleks-netizen.github.io/product-images/5196801/4.jpg,https://oleks-netizen.github.io/product-images/5196801/5.jpg,https://oleks-netizen.github.io/product-images/5196801/6.jpg,https://oleks-netizen.github.io/product-images/5196801/8.jpg,https://oleks-netizen.github.io/product-images/5196801/9.jpg</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1728_1_2</t>
+          <t>5228201</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/1728_1_2/1.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/5228201/1.jpg,https://oleks-netizen.github.io/product-images/5228201/2.jpg,https://oleks-netizen.github.io/product-images/5228201/5.jpg,https://oleks-netizen.github.io/product-images/5228201/11.jpg,https://oleks-netizen.github.io/product-images/5228201/3.jpg,https://oleks-netizen.github.io/product-images/5228201/4.jpg,https://oleks-netizen.github.io/product-images/5228201/6.jpg,https://oleks-netizen.github.io/product-images/5228201/7.jpg,https://oleks-netizen.github.io/product-images/5228201/8.jpg,https://oleks-netizen.github.io/product-images/5228201/9.jpg</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>20875_1</t>
+          <t>533670</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20875_1/1.jpg,https://oleks-netizen.github.io/product-images/20875_1/2.jpg,https://oleks-netizen.github.io/product-images/20875_1/13.jpg,https://oleks-netizen.github.io/product-images/20875_1/10.jpg,https://oleks-netizen.github.io/product-images/20875_1/11.jpg,https://oleks-netizen.github.io/product-images/20875_1/12.jpg,https://oleks-netizen.github.io/product-images/20875_1/3.jpg,https://oleks-netizen.github.io/product-images/20875_1/4.jpg,https://oleks-netizen.github.io/product-images/20875_1/5.jpg,https://oleks-netizen.github.io/product-images/20875_1/6.jpg,https://oleks-netizen.github.io/product-images/20875_1/7.jpg,https://oleks-netizen.github.io/product-images/20875_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/533670/1.jpg,https://oleks-netizen.github.io/product-images/533670/2.jpg,https://oleks-netizen.github.io/product-images/533670/7.jpg,https://oleks-netizen.github.io/product-images/533670/8.jpg,https://oleks-netizen.github.io/product-images/533670/3.jpg,https://oleks-netizen.github.io/product-images/533670/4.jpg,https://oleks-netizen.github.io/product-images/533670/5.jpg</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>20876_1</t>
+          <t>538610</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20876_1/1.jpg,https://oleks-netizen.github.io/product-images/20876_1/2.jpg,https://oleks-netizen.github.io/product-images/20876_1/11.jpg,https://oleks-netizen.github.io/product-images/20876_1/10.jpg,https://oleks-netizen.github.io/product-images/20876_1/3.jpg,https://oleks-netizen.github.io/product-images/20876_1/4.jpg,https://oleks-netizen.github.io/product-images/20876_1/5.jpg,https://oleks-netizen.github.io/product-images/20876_1/6.jpg,https://oleks-netizen.github.io/product-images/20876_1/8.jpg,https://oleks-netizen.github.io/product-images/20876_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/538610/1.jpg,https://oleks-netizen.github.io/product-images/538610/2.jpg,https://oleks-netizen.github.io/product-images/538610/8.jpg,https://oleks-netizen.github.io/product-images/538610/3.jpg,https://oleks-netizen.github.io/product-images/538610/4.jpg,https://oleks-netizen.github.io/product-images/538610/6.jpg,https://oleks-netizen.github.io/product-images/538610/7.jpg</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>20877_1</t>
+          <t>77266501</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20877_1/1.jpg,https://oleks-netizen.github.io/product-images/20877_1/2.jpg,https://oleks-netizen.github.io/product-images/20877_1/12.jpg,https://oleks-netizen.github.io/product-images/20877_1/10.jpg,https://oleks-netizen.github.io/product-images/20877_1/11.jpg,https://oleks-netizen.github.io/product-images/20877_1/3.jpg,https://oleks-netizen.github.io/product-images/20877_1/4.jpg,https://oleks-netizen.github.io/product-images/20877_1/5.jpg,https://oleks-netizen.github.io/product-images/20877_1/6.jpg,https://oleks-netizen.github.io/product-images/20877_1/7.jpg,https://oleks-netizen.github.io/product-images/20877_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/77266501/1.jpg</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>20878_1</t>
+          <t>80460064m</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20878_1/1.jpg,https://oleks-netizen.github.io/product-images/20878_1/2.jpg,https://oleks-netizen.github.io/product-images/20878_1/14.jpg,https://oleks-netizen.github.io/product-images/20878_1/10.jpg,https://oleks-netizen.github.io/product-images/20878_1/11.jpg,https://oleks-netizen.github.io/product-images/20878_1/12.jpg,https://oleks-netizen.github.io/product-images/20878_1/13.jpg,https://oleks-netizen.github.io/product-images/20878_1/3.jpg,https://oleks-netizen.github.io/product-images/20878_1/4.jpg,https://oleks-netizen.github.io/product-images/20878_1/5.jpg,https://oleks-netizen.github.io/product-images/20878_1/6.jpg,https://oleks-netizen.github.io/product-images/20878_1/7.jpg,https://oleks-netizen.github.io/product-images/20878_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/80460064m/1.jpg,https://oleks-netizen.github.io/product-images/80460064m/2.jpg,https://oleks-netizen.github.io/product-images/80460064m/8.jpg,https://oleks-netizen.github.io/product-images/80460064m/15.jpg,https://oleks-netizen.github.io/product-images/80460064m/10.jpg,https://oleks-netizen.github.io/product-images/80460064m/11.jpg,https://oleks-netizen.github.io/product-images/80460064m/12.jpg,https://oleks-netizen.github.io/product-images/80460064m/13.jpg,https://oleks-netizen.github.io/product-images/80460064m/14.jpg,https://oleks-netizen.github.io/product-images/80460064m/3.jpg,https://oleks-netizen.github.io/product-images/80460064m/4.jpg,https://oleks-netizen.github.io/product-images/80460064m/5.jpg,https://oleks-netizen.github.io/product-images/80460064m/7.jpg,https://oleks-netizen.github.io/product-images/80460064m/9.jpg</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>20879_1</t>
+          <t>80460101m</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20879_1/1.jpg,https://oleks-netizen.github.io/product-images/20879_1/2.jpg,https://oleks-netizen.github.io/product-images/20879_1/13.jpg,https://oleks-netizen.github.io/product-images/20879_1/10.jpg,https://oleks-netizen.github.io/product-images/20879_1/11.jpg,https://oleks-netizen.github.io/product-images/20879_1/12.jpg,https://oleks-netizen.github.io/product-images/20879_1/3.jpg,https://oleks-netizen.github.io/product-images/20879_1/4.jpg,https://oleks-netizen.github.io/product-images/20879_1/6.jpg,https://oleks-netizen.github.io/product-images/20879_1/7.jpg,https://oleks-netizen.github.io/product-images/20879_1/8.jpg,https://oleks-netizen.github.io/product-images/20879_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/80460101m/1.jpg,https://oleks-netizen.github.io/product-images/80460101m/2.jpg,https://oleks-netizen.github.io/product-images/80460101m/8.jpg,https://oleks-netizen.github.io/product-images/80460101m/17.jpg,https://oleks-netizen.github.io/product-images/80460101m/10.jpg,https://oleks-netizen.github.io/product-images/80460101m/11.jpg,https://oleks-netizen.github.io/product-images/80460101m/12.jpg,https://oleks-netizen.github.io/product-images/80460101m/13.jpg,https://oleks-netizen.github.io/product-images/80460101m/14.jpg,https://oleks-netizen.github.io/product-images/80460101m/15.jpg,https://oleks-netizen.github.io/product-images/80460101m/16.jpg,https://oleks-netizen.github.io/product-images/80460101m/3.jpg,https://oleks-netizen.github.io/product-images/80460101m/4.jpg,https://oleks-netizen.github.io/product-images/80460101m/5.jpg,https://oleks-netizen.github.io/product-images/80460101m/7.jpg,https://oleks-netizen.github.io/product-images/80460101m/9.jpg</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>20880_1</t>
+          <t>90421065m</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20880_1/1.jpg,https://oleks-netizen.github.io/product-images/20880_1/2.jpg,https://oleks-netizen.github.io/product-images/20880_1/6.jpg,https://oleks-netizen.github.io/product-images/20880_1/12.jpg,https://oleks-netizen.github.io/product-images/20880_1/10.jpg,https://oleks-netizen.github.io/product-images/20880_1/11.jpg,https://oleks-netizen.github.io/product-images/20880_1/3.jpg,https://oleks-netizen.github.io/product-images/20880_1/4.jpg,https://oleks-netizen.github.io/product-images/20880_1/5.jpg,https://oleks-netizen.github.io/product-images/20880_1/7.jpg,https://oleks-netizen.github.io/product-images/20880_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/90421065m/1.jpg,https://oleks-netizen.github.io/product-images/90421065m/2.jpg,https://oleks-netizen.github.io/product-images/90421065m/15.jpg,https://oleks-netizen.github.io/product-images/90421065m/10.jpg,https://oleks-netizen.github.io/product-images/90421065m/11.jpg,https://oleks-netizen.github.io/product-images/90421065m/12.jpg,https://oleks-netizen.github.io/product-images/90421065m/13.jpg,https://oleks-netizen.github.io/product-images/90421065m/14.jpg,https://oleks-netizen.github.io/product-images/90421065m/3.jpg,https://oleks-netizen.github.io/product-images/90421065m/4.jpg,https://oleks-netizen.github.io/product-images/90421065m/6.jpg,https://oleks-netizen.github.io/product-images/90421065m/7.jpg,https://oleks-netizen.github.io/product-images/90421065m/8.jpg,https://oleks-netizen.github.io/product-images/90421065m/9.jpg</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>20881_1</t>
+          <t>Accademia1139nero</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20881_1/1.jpg,https://oleks-netizen.github.io/product-images/20881_1/2.jpg,https://oleks-netizen.github.io/product-images/20881_1/12.jpg,https://oleks-netizen.github.io/product-images/20881_1/10.jpg,https://oleks-netizen.github.io/product-images/20881_1/11.jpg,https://oleks-netizen.github.io/product-images/20881_1/3.jpg,https://oleks-netizen.github.io/product-images/20881_1/4.jpg,https://oleks-netizen.github.io/product-images/20881_1/5.jpg,https://oleks-netizen.github.io/product-images/20881_1/6.jpg,https://oleks-netizen.github.io/product-images/20881_1/7.jpg,https://oleks-netizen.github.io/product-images/20881_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/Accademia1139nero/1.jpg,https://oleks-netizen.github.io/product-images/Accademia1139nero/2.jpg,https://oleks-netizen.github.io/product-images/Accademia1139nero/3.jpg</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>20882_1</t>
+          <t>ButC-1404-4lx</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20882_1/1.jpg,https://oleks-netizen.github.io/product-images/20882_1/2.jpg,https://oleks-netizen.github.io/product-images/20882_1/14.jpg,https://oleks-netizen.github.io/product-images/20882_1/11.jpg,https://oleks-netizen.github.io/product-images/20882_1/12.jpg,https://oleks-netizen.github.io/product-images/20882_1/13.jpg,https://oleks-netizen.github.io/product-images/20882_1/3.jpg,https://oleks-netizen.github.io/product-images/20882_1/4.jpg,https://oleks-netizen.github.io/product-images/20882_1/5.jpg,https://oleks-netizen.github.io/product-images/20882_1/6.jpg,https://oleks-netizen.github.io/product-images/20882_1/7.jpg,https://oleks-netizen.github.io/product-images/20882_1/8.jpg,https://oleks-netizen.github.io/product-images/20882_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/ButC-1404-4lx/1.jpg,https://oleks-netizen.github.io/product-images/ButC-1404-4lx/2.jpg,https://oleks-netizen.github.io/product-images/ButC-1404-4lx/7.jpg,https://oleks-netizen.github.io/product-images/ButC-1404-4lx/4.jpg,https://oleks-netizen.github.io/product-images/ButC-1404-4lx/5.jpg,https://oleks-netizen.github.io/product-images/ButC-1404-4lx/6.jpg</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>20883_1</t>
+          <t>BV38416-153</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20883_1/1.jpg,https://oleks-netizen.github.io/product-images/20883_1/2.jpg,https://oleks-netizen.github.io/product-images/20883_1/13.jpg,https://oleks-netizen.github.io/product-images/20883_1/10.jpg,https://oleks-netizen.github.io/product-images/20883_1/11.jpg,https://oleks-netizen.github.io/product-images/20883_1/12.jpg,https://oleks-netizen.github.io/product-images/20883_1/3.jpg,https://oleks-netizen.github.io/product-images/20883_1/4.jpg,https://oleks-netizen.github.io/product-images/20883_1/5.jpg,https://oleks-netizen.github.io/product-images/20883_1/6.jpg,https://oleks-netizen.github.io/product-images/20883_1/7.jpg,https://oleks-netizen.github.io/product-images/20883_1/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BV38416-153/1.jpg,https://oleks-netizen.github.io/product-images/BV38416-153/2.jpg,https://oleks-netizen.github.io/product-images/BV38416-153/3.jpg,https://oleks-netizen.github.io/product-images/BV38416-153/8.jpg,https://oleks-netizen.github.io/product-images/BV38416-153/5.jpg,https://oleks-netizen.github.io/product-images/BV38416-153/6.jpg,https://oleks-netizen.github.io/product-images/BV38416-153/7.jpg</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20884_1</t>
+          <t>BV38601-1</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20884_1/1.jpg,https://oleks-netizen.github.io/product-images/20884_1/2.jpg,https://oleks-netizen.github.io/product-images/20884_1/12.jpg,https://oleks-netizen.github.io/product-images/20884_1/10.jpg,https://oleks-netizen.github.io/product-images/20884_1/11.jpg,https://oleks-netizen.github.io/product-images/20884_1/3.jpg,https://oleks-netizen.github.io/product-images/20884_1/5.jpg,https://oleks-netizen.github.io/product-images/20884_1/6.jpg,https://oleks-netizen.github.io/product-images/20884_1/7.jpg,https://oleks-netizen.github.io/product-images/20884_1/8.jpg,https://oleks-netizen.github.io/product-images/20884_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BV38601-1/1.jpg,https://oleks-netizen.github.io/product-images/BV38601-1/2.jpg,https://oleks-netizen.github.io/product-images/BV38601-1/6.jpg,https://oleks-netizen.github.io/product-images/BV38601-1/4.jpg,https://oleks-netizen.github.io/product-images/BV38601-1/5.jpg</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>20885_1</t>
+          <t>BV38753-1</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20885_1/1.jpg,https://oleks-netizen.github.io/product-images/20885_1/2.jpg,https://oleks-netizen.github.io/product-images/20885_1/11.jpg,https://oleks-netizen.github.io/product-images/20885_1/10.jpg,https://oleks-netizen.github.io/product-images/20885_1/3.jpg,https://oleks-netizen.github.io/product-images/20885_1/4.jpg,https://oleks-netizen.github.io/product-images/20885_1/5.jpg,https://oleks-netizen.github.io/product-images/20885_1/7.jpg,https://oleks-netizen.github.io/product-images/20885_1/8.jpg,https://oleks-netizen.github.io/product-images/20885_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/BV38753-1/1.jpg,https://oleks-netizen.github.io/product-images/BV38753-1/2.jpg,https://oleks-netizen.github.io/product-images/BV38753-1/8.jpg,https://oleks-netizen.github.io/product-images/BV38753-1/4.jpg,https://oleks-netizen.github.io/product-images/BV38753-1/5.jpg,https://oleks-netizen.github.io/product-images/BV38753-1/6.jpg,https://oleks-netizen.github.io/product-images/BV38753-1/7.jpg</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>20886_1</t>
+          <t>C-3079A-black</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20886_1/1.jpg,https://oleks-netizen.github.io/product-images/20886_1/2.jpg,https://oleks-netizen.github.io/product-images/20886_1/12.jpg,https://oleks-netizen.github.io/product-images/20886_1/10.jpg,https://oleks-netizen.github.io/product-images/20886_1/11.jpg,https://oleks-netizen.github.io/product-images/20886_1/3.jpg,https://oleks-netizen.github.io/product-images/20886_1/4.jpg,https://oleks-netizen.github.io/product-images/20886_1/5.jpg,https://oleks-netizen.github.io/product-images/20886_1/6.jpg,https://oleks-netizen.github.io/product-images/20886_1/8.jpg,https://oleks-netizen.github.io/product-images/20886_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/C-3079A-black/1.jpg,https://oleks-netizen.github.io/product-images/C-3079A-black/2.jpg,https://oleks-netizen.github.io/product-images/C-3079A-black/6.jpg,https://oleks-netizen.github.io/product-images/C-3079A-black/3.jpg,https://oleks-netizen.github.io/product-images/C-3079A-black/5.jpg</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>20887_1</t>
+          <t>Contatto9148nero</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20887_1/1.jpg,https://oleks-netizen.github.io/product-images/20887_1/2.jpg,https://oleks-netizen.github.io/product-images/20887_1/12.jpg,https://oleks-netizen.github.io/product-images/20887_1/10.jpg,https://oleks-netizen.github.io/product-images/20887_1/11.jpg,https://oleks-netizen.github.io/product-images/20887_1/3.jpg,https://oleks-netizen.github.io/product-images/20887_1/4.jpg,https://oleks-netizen.github.io/product-images/20887_1/5.jpg,https://oleks-netizen.github.io/product-images/20887_1/6.jpg,https://oleks-netizen.github.io/product-images/20887_1/8.jpg,https://oleks-netizen.github.io/product-images/20887_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/Contatto9148nero/1.jpg,https://oleks-netizen.github.io/product-images/Contatto9148nero/2.jpg,https://oleks-netizen.github.io/product-images/Contatto9148nero/3.jpg</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>20888_1</t>
+          <t>Cortina5051nero</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20888_1/1.jpg,https://oleks-netizen.github.io/product-images/20888_1/2.jpg,https://oleks-netizen.github.io/product-images/20888_1/10.jpg,https://oleks-netizen.github.io/product-images/20888_1/3.jpg,https://oleks-netizen.github.io/product-images/20888_1/4.jpg,https://oleks-netizen.github.io/product-images/20888_1/5.jpg,https://oleks-netizen.github.io/product-images/20888_1/6.jpg,https://oleks-netizen.github.io/product-images/20888_1/8.jpg,https://oleks-netizen.github.io/product-images/20888_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/Cortina5051nero/1.jpg,https://oleks-netizen.github.io/product-images/Cortina5051nero/2.jpg,https://oleks-netizen.github.io/product-images/Cortina5051nero/3.jpg</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>20889_1</t>
+          <t>Elit-1404-4lx</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20889_1/1.jpg,https://oleks-netizen.github.io/product-images/20889_1/2.jpg,https://oleks-netizen.github.io/product-images/20889_1/11.jpg,https://oleks-netizen.github.io/product-images/20889_1/10.jpg,https://oleks-netizen.github.io/product-images/20889_1/3.jpg,https://oleks-netizen.github.io/product-images/20889_1/4.jpg,https://oleks-netizen.github.io/product-images/20889_1/5.jpg,https://oleks-netizen.github.io/product-images/20889_1/6.jpg,https://oleks-netizen.github.io/product-images/20889_1/8.jpg,https://oleks-netizen.github.io/product-images/20889_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/Elit-1404-4lx/1.jpg,https://oleks-netizen.github.io/product-images/Elit-1404-4lx/2.jpg,https://oleks-netizen.github.io/product-images/Elit-1404-4lx/7.jpg,https://oleks-netizen.github.io/product-images/Elit-1404-4lx/4.jpg,https://oleks-netizen.github.io/product-images/Elit-1404-4lx/5.jpg,https://oleks-netizen.github.io/product-images/Elit-1404-4lx/6.jpg</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>20890_1</t>
+          <t>FA-1819-3md</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20890_1/1.jpg,https://oleks-netizen.github.io/product-images/20890_1/2.jpg,https://oleks-netizen.github.io/product-images/20890_1/10.jpg,https://oleks-netizen.github.io/product-images/20890_1/3.jpg,https://oleks-netizen.github.io/product-images/20890_1/4.jpg,https://oleks-netizen.github.io/product-images/20890_1/6.jpg,https://oleks-netizen.github.io/product-images/20890_1/7.jpg,https://oleks-netizen.github.io/product-images/20890_1/8.jpg,https://oleks-netizen.github.io/product-images/20890_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/FA-1819-3md/1.jpg,https://oleks-netizen.github.io/product-images/FA-1819-3md/2.jpg,https://oleks-netizen.github.io/product-images/FA-1819-3md/6.jpg,https://oleks-netizen.github.io/product-images/FA-1819-3md/4.jpg,https://oleks-netizen.github.io/product-images/FA-1819-3md/5.jpg</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>20891_1</t>
+          <t>FA-8033-4lx</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20891_1/1.jpg,https://oleks-netizen.github.io/product-images/20891_1/2.jpg,https://oleks-netizen.github.io/product-images/20891_1/10.jpg,https://oleks-netizen.github.io/product-images/20891_1/3.jpg,https://oleks-netizen.github.io/product-images/20891_1/4.jpg,https://oleks-netizen.github.io/product-images/20891_1/5.jpg,https://oleks-netizen.github.io/product-images/20891_1/7.jpg,https://oleks-netizen.github.io/product-images/20891_1/8.jpg,https://oleks-netizen.github.io/product-images/20891_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/FA-8033-4lx/1.jpg,https://oleks-netizen.github.io/product-images/FA-8033-4lx/2.jpg,https://oleks-netizen.github.io/product-images/FA-8033-4lx/6.jpg,https://oleks-netizen.github.io/product-images/FA-8033-4lx/4.jpg,https://oleks-netizen.github.io/product-images/FA-8033-4lx/5.jpg</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>20892_1</t>
+          <t>GA-1504-3md</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20892_1/1.jpg,https://oleks-netizen.github.io/product-images/20892_1/2.jpg,https://oleks-netizen.github.io/product-images/20892_1/11.jpg,https://oleks-netizen.github.io/product-images/20892_1/10.jpg,https://oleks-netizen.github.io/product-images/20892_1/3.jpg,https://oleks-netizen.github.io/product-images/20892_1/4.jpg,https://oleks-netizen.github.io/product-images/20892_1/5.jpg,https://oleks-netizen.github.io/product-images/20892_1/7.jpg,https://oleks-netizen.github.io/product-images/20892_1/8.jpg,https://oleks-netizen.github.io/product-images/20892_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/GA-1504-3md/1.jpg,https://oleks-netizen.github.io/product-images/GA-1504-3md/2.jpg,https://oleks-netizen.github.io/product-images/GA-1504-3md/5.jpg,https://oleks-netizen.github.io/product-images/GA-1504-3md/7.jpg,https://oleks-netizen.github.io/product-images/GA-1504-3md/4.jpg,https://oleks-netizen.github.io/product-images/GA-1504-3md/6.jpg</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>20893_1</t>
+          <t>GB-1302-3md</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20893_1/1.jpg,https://oleks-netizen.github.io/product-images/20893_1/2.jpg,https://oleks-netizen.github.io/product-images/20893_1/13.jpg,https://oleks-netizen.github.io/product-images/20893_1/10.jpg,https://oleks-netizen.github.io/product-images/20893_1/11.jpg,https://oleks-netizen.github.io/product-images/20893_1/12.jpg,https://oleks-netizen.github.io/product-images/20893_1/3.jpg,https://oleks-netizen.github.io/product-images/20893_1/4.jpg,https://oleks-netizen.github.io/product-images/20893_1/5.jpg,https://oleks-netizen.github.io/product-images/20893_1/6.jpg,https://oleks-netizen.github.io/product-images/20893_1/8.jpg,https://oleks-netizen.github.io/product-images/20893_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/GB-1302-3md/1.jpg,https://oleks-netizen.github.io/product-images/GB-1302-3md/2.jpg,https://oleks-netizen.github.io/product-images/GB-1302-3md/4.jpg,https://oleks-netizen.github.io/product-images/GB-1302-3md/7.jpg,https://oleks-netizen.github.io/product-images/GB-1302-3md/3.jpg,https://oleks-netizen.github.io/product-images/GB-1302-3md/5.jpg</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>20894_1</t>
+          <t>GC-1304-4lx</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20894_1/1.jpg,https://oleks-netizen.github.io/product-images/20894_1/2.jpg,https://oleks-netizen.github.io/product-images/20894_1/10.jpg,https://oleks-netizen.github.io/product-images/20894_1/3.jpg,https://oleks-netizen.github.io/product-images/20894_1/4.jpg,https://oleks-netizen.github.io/product-images/20894_1/5.jpg,https://oleks-netizen.github.io/product-images/20894_1/7.jpg,https://oleks-netizen.github.io/product-images/20894_1/8.jpg,https://oleks-netizen.github.io/product-images/20894_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/GC-1304-4lx/1.jpg,https://oleks-netizen.github.io/product-images/GC-1304-4lx/2.jpg,https://oleks-netizen.github.io/product-images/GC-1304-4lx/5.jpg,https://oleks-netizen.github.io/product-images/GC-1304-4lx/7.jpg,https://oleks-netizen.github.io/product-images/GC-1304-4lx/4.jpg,https://oleks-netizen.github.io/product-images/GC-1304-4lx/6.jpg</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>20895_1</t>
+          <t>GE-3104-2lx</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20895_1/1.jpg,https://oleks-netizen.github.io/product-images/20895_1/2.jpg,https://oleks-netizen.github.io/product-images/20895_1/12.jpg,https://oleks-netizen.github.io/product-images/20895_1/10.jpg,https://oleks-netizen.github.io/product-images/20895_1/11.jpg,https://oleks-netizen.github.io/product-images/20895_1/3.jpg,https://oleks-netizen.github.io/product-images/20895_1/4.jpg,https://oleks-netizen.github.io/product-images/20895_1/5.jpg,https://oleks-netizen.github.io/product-images/20895_1/7.jpg,https://oleks-netizen.github.io/product-images/20895_1/8.jpg,https://oleks-netizen.github.io/product-images/20895_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/GE-3104-2lx/1.jpg,https://oleks-netizen.github.io/product-images/GE-3104-2lx/2.jpg,https://oleks-netizen.github.io/product-images/GE-3104-2lx/3.jpg,https://oleks-netizen.github.io/product-images/GE-3104-2lx/6.jpg,https://oleks-netizen.github.io/product-images/GE-3104-2lx/5.jpg</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>20896_1</t>
+          <t>GX-8137-4lx</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20896_1/1.jpg,https://oleks-netizen.github.io/product-images/20896_1/2.jpg,https://oleks-netizen.github.io/product-images/20896_1/12.jpg,https://oleks-netizen.github.io/product-images/20896_1/10.jpg,https://oleks-netizen.github.io/product-images/20896_1/11.jpg,https://oleks-netizen.github.io/product-images/20896_1/3.jpg,https://oleks-netizen.github.io/product-images/20896_1/4.jpg,https://oleks-netizen.github.io/product-images/20896_1/5.jpg,https://oleks-netizen.github.io/product-images/20896_1/6.jpg,https://oleks-netizen.github.io/product-images/20896_1/7.jpg,https://oleks-netizen.github.io/product-images/20896_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/GX-8137-4lx/1.jpg,https://oleks-netizen.github.io/product-images/GX-8137-4lx/2.jpg,https://oleks-netizen.github.io/product-images/GX-8137-4lx/9.jpg,https://oleks-netizen.github.io/product-images/GX-8137-4lx/3.jpg,https://oleks-netizen.github.io/product-images/GX-8137-4lx/4.jpg,https://oleks-netizen.github.io/product-images/GX-8137-4lx/5.jpg,https://oleks-netizen.github.io/product-images/GX-8137-4lx/7.jpg,https://oleks-netizen.github.io/product-images/GX-8137-4lx/8.jpg</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>20897_1</t>
+          <t>HB03334</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20897_1/1.jpg,https://oleks-netizen.github.io/product-images/20897_1/2.jpg,https://oleks-netizen.github.io/product-images/20897_1/11.jpg,https://oleks-netizen.github.io/product-images/20897_1/10.jpg,https://oleks-netizen.github.io/product-images/20897_1/3.jpg,https://oleks-netizen.github.io/product-images/20897_1/4.jpg,https://oleks-netizen.github.io/product-images/20897_1/5.jpg,https://oleks-netizen.github.io/product-images/20897_1/7.jpg,https://oleks-netizen.github.io/product-images/20897_1/8.jpg,https://oleks-netizen.github.io/product-images/20897_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/HB03334/1.jpg,https://oleks-netizen.github.io/product-images/HB03334/2.jpg,https://oleks-netizen.github.io/product-images/HB03334/3.jpg,https://oleks-netizen.github.io/product-images/HB03334/7.jpg,https://oleks-netizen.github.io/product-images/HB03334/4.jpg,https://oleks-netizen.github.io/product-images/HB03334/6.jpg</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>20898_1</t>
+          <t>Italico109nero</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20898_1/1.jpg,https://oleks-netizen.github.io/product-images/20898_1/2.jpg,https://oleks-netizen.github.io/product-images/20898_1/11.jpg,https://oleks-netizen.github.io/product-images/20898_1/10.jpg,https://oleks-netizen.github.io/product-images/20898_1/3.jpg,https://oleks-netizen.github.io/product-images/20898_1/4.jpg,https://oleks-netizen.github.io/product-images/20898_1/5.jpg,https://oleks-netizen.github.io/product-images/20898_1/7.jpg,https://oleks-netizen.github.io/product-images/20898_1/8.jpg,https://oleks-netizen.github.io/product-images/20898_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/Italico109nero/1.jpg,https://oleks-netizen.github.io/product-images/Italico109nero/4.jpg,https://oleks-netizen.github.io/product-images/Italico109nero/3.jpg</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>20899_1</t>
+          <t>Italico1636cognac</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20899_1/1.jpg,https://oleks-netizen.github.io/product-images/20899_1/2.jpg,https://oleks-netizen.github.io/product-images/20899_1/12.jpg,https://oleks-netizen.github.io/product-images/20899_1/10.jpg,https://oleks-netizen.github.io/product-images/20899_1/11.jpg,https://oleks-netizen.github.io/product-images/20899_1/3.jpg,https://oleks-netizen.github.io/product-images/20899_1/4.jpg,https://oleks-netizen.github.io/product-images/20899_1/6.jpg,https://oleks-netizen.github.io/product-images/20899_1/7.jpg,https://oleks-netizen.github.io/product-images/20899_1/8.jpg,https://oleks-netizen.github.io/product-images/20899_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/Italico1636cognac/1.jpg,https://oleks-netizen.github.io/product-images/Italico1636cognac/2.jpg,https://oleks-netizen.github.io/product-images/Italico1636cognac/4.jpg</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>20900_1</t>
+          <t>Italico2367moro</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20900_1/1.jpg,https://oleks-netizen.github.io/product-images/20900_1/2.jpg,https://oleks-netizen.github.io/product-images/20900_1/9.jpg,https://oleks-netizen.github.io/product-images/20900_1/3.jpg,https://oleks-netizen.github.io/product-images/20900_1/4.jpg,https://oleks-netizen.github.io/product-images/20900_1/6.jpg,https://oleks-netizen.github.io/product-images/20900_1/7.jpg,https://oleks-netizen.github.io/product-images/20900_1/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/Italico2367moro/1.jpg,https://oleks-netizen.github.io/product-images/Italico2367moro/2.jpg,https://oleks-netizen.github.io/product-images/Italico2367moro/5.jpg,https://oleks-netizen.github.io/product-images/Italico2367moro/3.jpg</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>20901_1</t>
+          <t>Italico9188nero</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20901_1/1.jpg,https://oleks-netizen.github.io/product-images/20901_1/2.jpg,https://oleks-netizen.github.io/product-images/20901_1/11.jpg,https://oleks-netizen.github.io/product-images/20901_1/10.jpg,https://oleks-netizen.github.io/product-images/20901_1/3.jpg,https://oleks-netizen.github.io/product-images/20901_1/4.jpg,https://oleks-netizen.github.io/product-images/20901_1/5.jpg,https://oleks-netizen.github.io/product-images/20901_1/7.jpg,https://oleks-netizen.github.io/product-images/20901_1/8.jpg,https://oleks-netizen.github.io/product-images/20901_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/Italico9188nero/1.jpg,https://oleks-netizen.github.io/product-images/Italico9188nero/2.jpg,https://oleks-netizen.github.io/product-images/Italico9188nero/5.jpg,https://oleks-netizen.github.io/product-images/Italico9188nero/3.jpg</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>20902_1</t>
+          <t>Italico9405nero</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20902_1/1.jpg,https://oleks-netizen.github.io/product-images/20902_1/2.jpg,https://oleks-netizen.github.io/product-images/20902_1/12.jpg,https://oleks-netizen.github.io/product-images/20902_1/10.jpg,https://oleks-netizen.github.io/product-images/20902_1/11.jpg,https://oleks-netizen.github.io/product-images/20902_1/3.jpg,https://oleks-netizen.github.io/product-images/20902_1/4.jpg,https://oleks-netizen.github.io/product-images/20902_1/5.jpg,https://oleks-netizen.github.io/product-images/20902_1/7.jpg,https://oleks-netizen.github.io/product-images/20902_1/8.jpg,https://oleks-netizen.github.io/product-images/20902_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/Italico9405nero/1.jpg,https://oleks-netizen.github.io/product-images/Italico9405nero/2.jpg,https://oleks-netizen.github.io/product-images/Italico9405nero/5.jpg,https://oleks-netizen.github.io/product-images/Italico9405nero/4.jpg</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>20903_1</t>
+          <t>Italico954622moro</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20903_1/1.jpg,https://oleks-netizen.github.io/product-images/20903_1/2.jpg,https://oleks-netizen.github.io/product-images/20903_1/14.jpg,https://oleks-netizen.github.io/product-images/20903_1/10.jpg,https://oleks-netizen.github.io/product-images/20903_1/11.jpg,https://oleks-netizen.github.io/product-images/20903_1/12.jpg,https://oleks-netizen.github.io/product-images/20903_1/13.jpg,https://oleks-netizen.github.io/product-images/20903_1/3.jpg,https://oleks-netizen.github.io/product-images/20903_1/4.jpg,https://oleks-netizen.github.io/product-images/20903_1/5.jpg,https://oleks-netizen.github.io/product-images/20903_1/6.jpg,https://oleks-netizen.github.io/product-images/20903_1/8.jpg,https://oleks-netizen.github.io/product-images/20903_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/Italico954622moro/1.jpg,https://oleks-netizen.github.io/product-images/Italico954622moro/2.jpg,https://oleks-netizen.github.io/product-images/Italico954622moro/5.jpg,https://oleks-netizen.github.io/product-images/Italico954622moro/3.jpg</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>20904_1</t>
+          <t>JD1072A</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20904_1/1.jpg,https://oleks-netizen.github.io/product-images/20904_1/2.jpg,https://oleks-netizen.github.io/product-images/20904_1/12.jpg,https://oleks-netizen.github.io/product-images/20904_1/10.jpg,https://oleks-netizen.github.io/product-images/20904_1/11.jpg,https://oleks-netizen.github.io/product-images/20904_1/3.jpg,https://oleks-netizen.github.io/product-images/20904_1/4.jpg,https://oleks-netizen.github.io/product-images/20904_1/5.jpg,https://oleks-netizen.github.io/product-images/20904_1/6.jpg,https://oleks-netizen.github.io/product-images/20904_1/7.jpg,https://oleks-netizen.github.io/product-images/20904_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/JD1072A/1.jpg,https://oleks-netizen.github.io/product-images/JD1072A/2.jpg</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>20905_1</t>
+          <t>JD1072R</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20905_1/1.jpg,https://oleks-netizen.github.io/product-images/20905_1/2.jpg,https://oleks-netizen.github.io/product-images/20905_1/12.jpg,https://oleks-netizen.github.io/product-images/20905_1/10.jpg,https://oleks-netizen.github.io/product-images/20905_1/11.jpg,https://oleks-netizen.github.io/product-images/20905_1/3.jpg,https://oleks-netizen.github.io/product-images/20905_1/4.jpg,https://oleks-netizen.github.io/product-images/20905_1/5.jpg,https://oleks-netizen.github.io/product-images/20905_1/6.jpg,https://oleks-netizen.github.io/product-images/20905_1/8.jpg,https://oleks-netizen.github.io/product-images/20905_1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/JD1072R/1.jpg</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2140_1_5</t>
+          <t>JD1094A</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/2140_1_5/1.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/JD1094A/1.jpg,https://oleks-netizen.github.io/product-images/JD1094A/2.jpg,https://oleks-netizen.github.io/product-images/JD1094A/6.jpg,https://oleks-netizen.github.io/product-images/JD1094A/3.jpg,https://oleks-netizen.github.io/product-images/JD1094A/4.jpg</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>53300067</t>
+          <t>JD1097A</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/53300067/1.jpg,https://oleks-netizen.github.io/product-images/53300067/2.jpg,https://oleks-netizen.github.io/product-images/53300067/5.jpg,https://oleks-netizen.github.io/product-images/53300067/13.jpg,https://oleks-netizen.github.io/product-images/53300067/10.jpg,https://oleks-netizen.github.io/product-images/53300067/11.jpg,https://oleks-netizen.github.io/product-images/53300067/12.jpg,https://oleks-netizen.github.io/product-images/53300067/3.jpg,https://oleks-netizen.github.io/product-images/53300067/4.jpg,https://oleks-netizen.github.io/product-images/53300067/6.jpg,https://oleks-netizen.github.io/product-images/53300067/7.jpg,https://oleks-netizen.github.io/product-images/53300067/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/JD1097A/1.jpg,https://oleks-netizen.github.io/product-images/JD1097A/2.jpg,https://oleks-netizen.github.io/product-images/JD1097A/5.jpg,https://oleks-netizen.github.io/product-images/JD1097A/3.jpg</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>53300068</t>
+          <t>JD1097C</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/53300068/1.jpg,https://oleks-netizen.github.io/product-images/53300068/2.jpg,https://oleks-netizen.github.io/product-images/53300068/4.jpg,https://oleks-netizen.github.io/product-images/53300068/12.jpg,https://oleks-netizen.github.io/product-images/53300068/11.jpg,https://oleks-netizen.github.io/product-images/53300068/3.jpg,https://oleks-netizen.github.io/product-images/53300068/5.jpg,https://oleks-netizen.github.io/product-images/53300068/6.jpg,https://oleks-netizen.github.io/product-images/53300068/7.jpg,https://oleks-netizen.github.io/product-images/53300068/8.jpg,https://oleks-netizen.github.io/product-images/53300068/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/JD1097C/1.jpg,https://oleks-netizen.github.io/product-images/JD1097C/2.jpg,https://oleks-netizen.github.io/product-images/JD1097C/5.jpg,https://oleks-netizen.github.io/product-images/JD1097C/4.jpg</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>53330067</t>
+          <t>JD1105AL</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/53330067/1.jpg,https://oleks-netizen.github.io/product-images/53330067/2.jpg,https://oleks-netizen.github.io/product-images/53330067/9.jpg,https://oleks-netizen.github.io/product-images/53330067/14.jpg,https://oleks-netizen.github.io/product-images/53330067/10.jpg,https://oleks-netizen.github.io/product-images/53330067/11.jpg,https://oleks-netizen.github.io/product-images/53330067/12.jpg,https://oleks-netizen.github.io/product-images/53330067/13.jpg,https://oleks-netizen.github.io/product-images/53330067/3.jpg,https://oleks-netizen.github.io/product-images/53330067/4.jpg,https://oleks-netizen.github.io/product-images/53330067/5.jpg,https://oleks-netizen.github.io/product-images/53330067/6.jpg,https://oleks-netizen.github.io/product-images/53330067/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/JD1105AL/1.jpg,https://oleks-netizen.github.io/product-images/JD1105AL/2.jpg,https://oleks-netizen.github.io/product-images/JD1105AL/4.jpg</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>80460064</t>
+          <t>JD1105AS</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/80460064/1.jpg,https://oleks-netizen.github.io/product-images/80460064/2.jpg,https://oleks-netizen.github.io/product-images/80460064/6.jpg,https://oleks-netizen.github.io/product-images/80460064/14.jpg,https://oleks-netizen.github.io/product-images/80460064/10.jpg,https://oleks-netizen.github.io/product-images/80460064/11.jpg,https://oleks-netizen.github.io/product-images/80460064/12.jpg,https://oleks-netizen.github.io/product-images/80460064/13.jpg,https://oleks-netizen.github.io/product-images/80460064/3.jpg,https://oleks-netizen.github.io/product-images/80460064/4.jpg,https://oleks-netizen.github.io/product-images/80460064/7.jpg,https://oleks-netizen.github.io/product-images/80460064/8.jpg,https://oleks-netizen.github.io/product-images/80460064/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/JD1105AS/1.jpg,https://oleks-netizen.github.io/product-images/JD1105AS/2.jpg,https://oleks-netizen.github.io/product-images/JD1105AS/4.jpg</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>80460120</t>
+          <t>JD1107A</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/80460120/1.jpg,https://oleks-netizen.github.io/product-images/80460120/2.jpg,https://oleks-netizen.github.io/product-images/80460120/14.jpg,https://oleks-netizen.github.io/product-images/80460120/15.jpg,https://oleks-netizen.github.io/product-images/80460120/10.jpg,https://oleks-netizen.github.io/product-images/80460120/11.jpg,https://oleks-netizen.github.io/product-images/80460120/12.jpg,https://oleks-netizen.github.io/product-images/80460120/13.jpg,https://oleks-netizen.github.io/product-images/80460120/3.jpg,https://oleks-netizen.github.io/product-images/80460120/4.jpg,https://oleks-netizen.github.io/product-images/80460120/5.jpg,https://oleks-netizen.github.io/product-images/80460120/6.jpg,https://oleks-netizen.github.io/product-images/80460120/7.jpg,https://oleks-netizen.github.io/product-images/80460120/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/JD1107A/1.jpg,https://oleks-netizen.github.io/product-images/JD1107A/2.jpg,https://oleks-netizen.github.io/product-images/JD1107A/5.jpg,https://oleks-netizen.github.io/product-images/JD1107A/3.jpg</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>963_1_6</t>
+          <t>JD1107C</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/963_1_6/1.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/JD1107C/1.jpg,https://oleks-netizen.github.io/product-images/JD1107C/2.jpg,https://oleks-netizen.github.io/product-images/JD1107C/5.jpg,https://oleks-netizen.github.io/product-images/JD1107C/4.jpg</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>BN-BAG-10-1-choko</t>
+          <t>JD4012Q</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-BAG-10-1-choko/1.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-10-1-choko/2.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-10-1-choko/3.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-10-1-choko/4.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-10-1-choko/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/JD4012Q/1.jpg,https://oleks-netizen.github.io/product-images/JD4012Q/2.jpg,https://oleks-netizen.github.io/product-images/JD4012Q/11.jpg,https://oleks-netizen.github.io/product-images/JD4012Q/10.jpg,https://oleks-netizen.github.io/product-images/JD4012Q/4.jpg,https://oleks-netizen.github.io/product-images/JD4012Q/5.jpg,https://oleks-netizen.github.io/product-images/JD4012Q/6.jpg,https://oleks-netizen.github.io/product-images/JD4012Q/7.jpg,https://oleks-netizen.github.io/product-images/JD4012Q/8.jpg,https://oleks-netizen.github.io/product-images/JD4012Q/9.jpg</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>BN-BAG-10-choko</t>
+          <t>JD7055R</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-BAG-10-choko/1.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-10-choko/2.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-10-choko/3.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-10-choko/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/JD7055R/1.jpg,https://oleks-netizen.github.io/product-images/JD7055R/2.jpg,https://oleks-netizen.github.io/product-images/JD7055R/8.jpg,https://oleks-netizen.github.io/product-images/JD7055R/11.jpg,https://oleks-netizen.github.io/product-images/JD7055R/10.jpg,https://oleks-netizen.github.io/product-images/JD7055R/3.jpg,https://oleks-netizen.github.io/product-images/JD7055R/4.jpg,https://oleks-netizen.github.io/product-images/JD7055R/5.jpg,https://oleks-netizen.github.io/product-images/JD7055R/6.jpg,https://oleks-netizen.github.io/product-images/JD7055R/7.jpg</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>BN-BAG-12-choko</t>
+          <t>K10018bl-black</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-BAG-12-choko/1.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-12-choko/2.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-12-choko/5.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-12-choko/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K10018bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K10018bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K10018bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K10018bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K10018bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>BN-BAG-17-choko</t>
+          <t>K11318bl-black</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-BAG-17-choko/1.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-17-choko/2.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-17-choko/6.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-17-choko/4.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-17-choko/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K11318bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K11318bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K11318bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K11318bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>BN-BAG-19-choko</t>
+          <t>K11512be-beige</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-BAG-19-choko/1.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-19-choko/2.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-19-choko/5.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-19-choko/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K11512be-beige/1.jpg,https://oleks-netizen.github.io/product-images/K11512be-beige/2.jpg,https://oleks-netizen.github.io/product-images/K11512be-beige/6.jpg,https://oleks-netizen.github.io/product-images/K11512be-beige/4.jpg,https://oleks-netizen.github.io/product-images/K11512be-beige/5.jpg</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>BN-BAG-22-choko</t>
+          <t>K11512bl-black</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-BAG-22-choko/1.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-22-choko/2.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-22-choko/5.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-22-choko/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K11512bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K11512bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K11512bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K11512bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K11512bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>BN-BAG-24-choko</t>
+          <t>K11512w-white</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-BAG-24-choko/1.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-24-choko/3.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-24-choko/7.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-24-choko/4.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-24-choko/5.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-24-choko/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K11512w-white/1.jpg,https://oleks-netizen.github.io/product-images/K11512w-white/2.jpg,https://oleks-netizen.github.io/product-images/K11512w-white/6.jpg,https://oleks-netizen.github.io/product-images/K11512w-white/4.jpg,https://oleks-netizen.github.io/product-images/K11512w-white/5.jpg</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>BN-BAG-28-choko</t>
+          <t>K11512z-green</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-BAG-28-choko/1.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-28-choko/2.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-28-choko/7.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-28-choko/4.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-28-choko/5.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-28-choko/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K11512z-green/1.jpg,https://oleks-netizen.github.io/product-images/K11512z-green/2.jpg,https://oleks-netizen.github.io/product-images/K11512z-green/6.jpg,https://oleks-netizen.github.io/product-images/K11512z-green/4.jpg,https://oleks-netizen.github.io/product-images/K11512z-green/5.jpg</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>BN-BAG-3-choko</t>
+          <t>K12202bl-black</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-BAG-3-choko/1.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-3-choko/2.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-3-choko/3.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-3-choko/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K12202bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K12202bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K12202bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K12202bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K12202bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>BN-BAG-36-choko</t>
+          <t>K12504bl-black</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-BAG-36-choko/1.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-36-choko/2.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-36-choko/5.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-36-choko/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K12504bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K12504bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K12504bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K12504bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K12504bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>BN-BAG-61-choko-g</t>
+          <t>K12507bl-black</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-BAG-61-choko-g/1.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K12507bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K12507bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K12507bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K12507bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K12507bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>BN-BAG-63-p-choko</t>
+          <t>k12511bl-black</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko/1.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko/2.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko/10.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko/3.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko/5.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko/6.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko/7.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko/8.jpg,https://oleks-netizen.github.io/product-images/BN-BAG-63-p-choko/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/k12511bl-black/1.jpg,https://oleks-netizen.github.io/product-images/k12511bl-black/2.jpg,https://oleks-netizen.github.io/product-images/k12511bl-black/7.jpg,https://oleks-netizen.github.io/product-images/k12511bl-black/4.jpg,https://oleks-netizen.github.io/product-images/k12511bl-black/5.jpg,https://oleks-netizen.github.io/product-images/k12511bl-black/6.jpg</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>BN-GC-34-choko</t>
+          <t>K1607bl-black</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-GC-34-choko/2.jpg,https://oleks-netizen.github.io/product-images/BN-GC-34-choko/10.jpg,https://oleks-netizen.github.io/product-images/BN-GC-34-choko/3.jpg,https://oleks-netizen.github.io/product-images/BN-GC-34-choko/4.jpg,https://oleks-netizen.github.io/product-images/BN-GC-34-choko/5.jpg,https://oleks-netizen.github.io/product-images/BN-GC-34-choko/6.jpg,https://oleks-netizen.github.io/product-images/BN-GC-34-choko/7.jpg,https://oleks-netizen.github.io/product-images/BN-GC-34-choko/8.jpg,https://oleks-netizen.github.io/product-images/BN-GC-34-choko/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K1607bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K1607bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K1607bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K1607bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K1607bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>BN-KK-11-nn</t>
+          <t>K1608be-beige</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-KK-11-nn/1.jpg,https://oleks-netizen.github.io/product-images/BN-KK-11-nn/2.jpg,https://oleks-netizen.github.io/product-images/BN-KK-11-nn/9.jpg,https://oleks-netizen.github.io/product-images/BN-KK-11-nn/3.jpg,https://oleks-netizen.github.io/product-images/BN-KK-11-nn/4.jpg,https://oleks-netizen.github.io/product-images/BN-KK-11-nn/6.jpg,https://oleks-netizen.github.io/product-images/BN-KK-11-nn/7.jpg,https://oleks-netizen.github.io/product-images/BN-KK-11-nn/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K1608be-beige/1.jpg,https://oleks-netizen.github.io/product-images/K1608be-beige/2.jpg,https://oleks-netizen.github.io/product-images/K1608be-beige/6.jpg,https://oleks-netizen.github.io/product-images/K1608be-beige/4.jpg,https://oleks-netizen.github.io/product-images/K1608be-beige/5.jpg</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>BN-KL-7-g-kr</t>
+          <t>K1608bl-black</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BN-KL-7-g-kr/1.jpg,https://oleks-netizen.github.io/product-images/BN-KL-7-g-kr/2.jpg,https://oleks-netizen.github.io/product-images/BN-KL-7-g-kr/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K1608bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K1608bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K1608bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K1608bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K1608bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>CC602_BN</t>
+          <t>K16101bl-black</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/CC602_BN/1.jpg,https://oleks-netizen.github.io/product-images/CC602_BN/2.jpg,https://oleks-netizen.github.io/product-images/CC602_BN/7.jpg,https://oleks-netizen.github.io/product-images/CC602_BN/4.jpg,https://oleks-netizen.github.io/product-images/CC602_BN/5.jpg,https://oleks-netizen.github.io/product-images/CC602_BN/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K16101bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K16101bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K16101bl-black/7.jpg,https://oleks-netizen.github.io/product-images/K16101bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K16101bl-black/5.jpg,https://oleks-netizen.github.io/product-images/K16101bl-black/6.jpg</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -1401,57 +1401,57 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>CC602_CR_BRN</t>
+          <t>K17107bl-black</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/CC602_CR_BRN/1.jpg,https://oleks-netizen.github.io/product-images/CC602_CR_BRN/2.jpg,https://oleks-netizen.github.io/product-images/CC602_CR_BRN/4.jpg,https://oleks-netizen.github.io/product-images/CC602_CR_BRN/8.jpg,https://oleks-netizen.github.io/product-images/CC602_CR_BRN/5.jpg,https://oleks-netizen.github.io/product-images/CC602_CR_BRN/6.jpg,https://oleks-netizen.github.io/product-images/CC602_CR_BRN/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K17107bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K17107bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K17107bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K17107bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K17107bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>CC607_NPA_BLK</t>
+          <t>K17107w-white</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/CC607_NPA_BLK/1.jpg,https://oleks-netizen.github.io/product-images/CC607_NPA_BLK/2.jpg,https://oleks-netizen.github.io/product-images/CC607_NPA_BLK/7.jpg,https://oleks-netizen.github.io/product-images/CC607_NPA_BLK/4.jpg,https://oleks-netizen.github.io/product-images/CC607_NPA_BLK/5.jpg,https://oleks-netizen.github.io/product-images/CC607_NPA_BLK/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K17107w-white/1.jpg,https://oleks-netizen.github.io/product-images/K17107w-white/2.jpg,https://oleks-netizen.github.io/product-images/K17107w-white/6.jpg,https://oleks-netizen.github.io/product-images/K17107w-white/4.jpg,https://oleks-netizen.github.io/product-images/K17107w-white/5.jpg</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>FA-7778-4lx</t>
+          <t>K17108bl-black</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/FA-7778-4lx/1.jpg,https://oleks-netizen.github.io/product-images/FA-7778-4lx/2.jpg,https://oleks-netizen.github.io/product-images/FA-7778-4lx/8.jpg,https://oleks-netizen.github.io/product-images/FA-7778-4lx/4.jpg,https://oleks-netizen.github.io/product-images/FA-7778-4lx/5.jpg,https://oleks-netizen.github.io/product-images/FA-7778-4lx/6.jpg,https://oleks-netizen.github.io/product-images/FA-7778-4lx/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K17108bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K17108bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K17108bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K17108bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K17108bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>FC-1819-3md</t>
+          <t>K17109bl-black</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/FC-1819-3md/1.jpg,https://oleks-netizen.github.io/product-images/FC-1819-3md/2.jpg,https://oleks-netizen.github.io/product-images/FC-1819-3md/3.jpg,https://oleks-netizen.github.io/product-images/FC-1819-3md/6.jpg,https://oleks-netizen.github.io/product-images/FC-1819-3md/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K17109bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K17109bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K17109bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K17109bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K17109bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C69" t="n">
@@ -1461,132 +1461,132 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>GC-0041-4lx</t>
+          <t>K18005bl-black</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/GC-0041-4lx/1.jpg,https://oleks-netizen.github.io/product-images/GC-0041-4lx/2.jpg,https://oleks-netizen.github.io/product-images/GC-0041-4lx/10.jpg,https://oleks-netizen.github.io/product-images/GC-0041-4lx/4.jpg,https://oleks-netizen.github.io/product-images/GC-0041-4lx/5.jpg,https://oleks-netizen.github.io/product-images/GC-0041-4lx/6.jpg,https://oleks-netizen.github.io/product-images/GC-0041-4lx/7.jpg,https://oleks-netizen.github.io/product-images/GC-0041-4lx/8.jpg,https://oleks-netizen.github.io/product-images/GC-0041-4lx/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K18005bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K18005bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K18005bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K18005bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K18005bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>JCBBP 71 BLK_YELLOW</t>
+          <t>K18012bl-black</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/1.jpg,https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/2.jpg,https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/4.jpg,https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/10.jpg,https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/3.jpg,https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/6.jpg,https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/7.jpg,https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/8.jpg,https://oleks-netizen.github.io/product-images/JCBBP 71 BLK_YELLOW/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K18012bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K18012bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K18012bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K18012bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K18012bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>L21065-010</t>
+          <t>K188084bl-black</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21065-010/1.jpg,https://oleks-netizen.github.io/product-images/L21065-010/2.jpg,https://oleks-netizen.github.io/product-images/L21065-010/8.jpg,https://oleks-netizen.github.io/product-images/L21065-010/4.jpg,https://oleks-netizen.github.io/product-images/L21065-010/5.jpg,https://oleks-netizen.github.io/product-images/L21065-010/6.jpg,https://oleks-netizen.github.io/product-images/L21065-010/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K188084bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K188084bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K188084bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K188084bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K188084bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>L21065-038</t>
+          <t>K188084gr-gray</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21065-038/1.jpg,https://oleks-netizen.github.io/product-images/L21065-038/2.jpg,https://oleks-netizen.github.io/product-images/L21065-038/8.jpg,https://oleks-netizen.github.io/product-images/L21065-038/4.jpg,https://oleks-netizen.github.io/product-images/L21065-038/5.jpg,https://oleks-netizen.github.io/product-images/L21065-038/6.jpg,https://oleks-netizen.github.io/product-images/L21065-038/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K188084gr-gray/1.jpg,https://oleks-netizen.github.io/product-images/K188084gr-gray/2.jpg,https://oleks-netizen.github.io/product-images/K188084gr-gray/6.jpg,https://oleks-netizen.github.io/product-images/K188084gr-gray/4.jpg,https://oleks-netizen.github.io/product-images/K188084gr-gray/5.jpg</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>L21065-056</t>
+          <t>K18817bl-black</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21065-056/1.jpg,https://oleks-netizen.github.io/product-images/L21065-056/2.jpg,https://oleks-netizen.github.io/product-images/L21065-056/8.jpg,https://oleks-netizen.github.io/product-images/L21065-056/4.jpg,https://oleks-netizen.github.io/product-images/L21065-056/5.jpg,https://oleks-netizen.github.io/product-images/L21065-056/6.jpg,https://oleks-netizen.github.io/product-images/L21065-056/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K18817bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K18817bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K18817bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K18817bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K18817bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>L21065-058</t>
+          <t>K18868bl-black</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21065-058/1.jpg,https://oleks-netizen.github.io/product-images/L21065-058/2.jpg,https://oleks-netizen.github.io/product-images/L21065-058/8.jpg,https://oleks-netizen.github.io/product-images/L21065-058/4.jpg,https://oleks-netizen.github.io/product-images/L21065-058/5.jpg,https://oleks-netizen.github.io/product-images/L21065-058/6.jpg,https://oleks-netizen.github.io/product-images/L21065-058/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K18868bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K18868bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K18868bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K18868bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K18868bl-black/5.jpg</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>L21567-010</t>
+          <t>K45 BLK</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21567-010/1.jpg,https://oleks-netizen.github.io/product-images/L21567-010/2.jpg,https://oleks-netizen.github.io/product-images/L21567-010/8.jpg,https://oleks-netizen.github.io/product-images/L21567-010/4.jpg,https://oleks-netizen.github.io/product-images/L21567-010/5.jpg,https://oleks-netizen.github.io/product-images/L21567-010/6.jpg,https://oleks-netizen.github.io/product-images/L21567-010/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K45 BLK/1.jpg,https://oleks-netizen.github.io/product-images/K45 BLK/2.jpg,https://oleks-netizen.github.io/product-images/K45 BLK/6.jpg,https://oleks-netizen.github.io/product-images/K45 BLK/3.jpg,https://oleks-netizen.github.io/product-images/K45 BLK/5.jpg</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>L21567-025</t>
+          <t>K46 BLK</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21567-025/1.jpg,https://oleks-netizen.github.io/product-images/L21567-025/2.jpg,https://oleks-netizen.github.io/product-images/L21567-025/8.jpg,https://oleks-netizen.github.io/product-images/L21567-025/4.jpg,https://oleks-netizen.github.io/product-images/L21567-025/5.jpg,https://oleks-netizen.github.io/product-images/L21567-025/6.jpg,https://oleks-netizen.github.io/product-images/L21567-025/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K46 BLK/1.jpg</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>L21575-010</t>
+          <t>L20037-1</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21575-010/1.jpg,https://oleks-netizen.github.io/product-images/L21575-010/2.jpg,https://oleks-netizen.github.io/product-images/L21575-010/8.jpg,https://oleks-netizen.github.io/product-images/L21575-010/4.jpg,https://oleks-netizen.github.io/product-images/L21575-010/5.jpg,https://oleks-netizen.github.io/product-images/L21575-010/6.jpg,https://oleks-netizen.github.io/product-images/L21575-010/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20037-1/1.jpg,https://oleks-netizen.github.io/product-images/L20037-1/2.jpg,https://oleks-netizen.github.io/product-images/L20037-1/8.jpg,https://oleks-netizen.github.io/product-images/L20037-1/4.jpg,https://oleks-netizen.github.io/product-images/L20037-1/5.jpg,https://oleks-netizen.github.io/product-images/L20037-1/6.jpg,https://oleks-netizen.github.io/product-images/L20037-1/7.jpg</t>
         </is>
       </c>
       <c r="C78" t="n">
@@ -1596,12 +1596,12 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>L21575-038</t>
+          <t>L20037-40</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21575-038/1.jpg,https://oleks-netizen.github.io/product-images/L21575-038/2.jpg,https://oleks-netizen.github.io/product-images/L21575-038/8.jpg,https://oleks-netizen.github.io/product-images/L21575-038/4.jpg,https://oleks-netizen.github.io/product-images/L21575-038/5.jpg,https://oleks-netizen.github.io/product-images/L21575-038/6.jpg,https://oleks-netizen.github.io/product-images/L21575-038/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20037-40/1.jpg,https://oleks-netizen.github.io/product-images/L20037-40/2.jpg,https://oleks-netizen.github.io/product-images/L20037-40/3.jpg,https://oleks-netizen.github.io/product-images/L20037-40/8.jpg,https://oleks-netizen.github.io/product-images/L20037-40/5.jpg,https://oleks-netizen.github.io/product-images/L20037-40/6.jpg,https://oleks-netizen.github.io/product-images/L20037-40/7.jpg</t>
         </is>
       </c>
       <c r="C79" t="n">
@@ -1611,12 +1611,12 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>L21586-010</t>
+          <t>L20037-56</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21586-010/1.jpg,https://oleks-netizen.github.io/product-images/L21586-010/2.jpg,https://oleks-netizen.github.io/product-images/L21586-010/8.jpg,https://oleks-netizen.github.io/product-images/L21586-010/4.jpg,https://oleks-netizen.github.io/product-images/L21586-010/5.jpg,https://oleks-netizen.github.io/product-images/L21586-010/6.jpg,https://oleks-netizen.github.io/product-images/L21586-010/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20037-56/1.jpg,https://oleks-netizen.github.io/product-images/L20037-56/2.jpg,https://oleks-netizen.github.io/product-images/L20037-56/3.jpg,https://oleks-netizen.github.io/product-images/L20037-56/8.jpg,https://oleks-netizen.github.io/product-images/L20037-56/5.jpg,https://oleks-netizen.github.io/product-images/L20037-56/6.jpg,https://oleks-netizen.github.io/product-images/L20037-56/7.jpg</t>
         </is>
       </c>
       <c r="C80" t="n">
@@ -1626,12 +1626,12 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>L21586-025</t>
+          <t>L20066-1</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21586-025/1.jpg,https://oleks-netizen.github.io/product-images/L21586-025/2.jpg,https://oleks-netizen.github.io/product-images/L21586-025/8.jpg,https://oleks-netizen.github.io/product-images/L21586-025/4.jpg,https://oleks-netizen.github.io/product-images/L21586-025/5.jpg,https://oleks-netizen.github.io/product-images/L21586-025/6.jpg,https://oleks-netizen.github.io/product-images/L21586-025/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20066-1/1.jpg,https://oleks-netizen.github.io/product-images/L20066-1/2.jpg,https://oleks-netizen.github.io/product-images/L20066-1/3.jpg,https://oleks-netizen.github.io/product-images/L20066-1/8.jpg,https://oleks-netizen.github.io/product-images/L20066-1/5.jpg,https://oleks-netizen.github.io/product-images/L20066-1/6.jpg,https://oleks-netizen.github.io/product-images/L20066-1/7.jpg</t>
         </is>
       </c>
       <c r="C81" t="n">
@@ -1641,12 +1641,12 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>L21586-097</t>
+          <t>L20066-2</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L21586-097/1.jpg,https://oleks-netizen.github.io/product-images/L21586-097/2.jpg,https://oleks-netizen.github.io/product-images/L21586-097/8.jpg,https://oleks-netizen.github.io/product-images/L21586-097/4.jpg,https://oleks-netizen.github.io/product-images/L21586-097/5.jpg,https://oleks-netizen.github.io/product-images/L21586-097/6.jpg,https://oleks-netizen.github.io/product-images/L21586-097/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20066-2/1.jpg,https://oleks-netizen.github.io/product-images/L20066-2/2.jpg,https://oleks-netizen.github.io/product-images/L20066-2/3.jpg,https://oleks-netizen.github.io/product-images/L20066-2/8.jpg,https://oleks-netizen.github.io/product-images/L20066-2/5.jpg,https://oleks-netizen.github.io/product-images/L20066-2/6.jpg,https://oleks-netizen.github.io/product-images/L20066-2/7.jpg</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -1656,102 +1656,102 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>LC69004-01</t>
+          <t>L20066-6</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69004-01/1.jpg,https://oleks-netizen.github.io/product-images/LC69004-01/2.jpg,https://oleks-netizen.github.io/product-images/LC69004-01/9.jpg,https://oleks-netizen.github.io/product-images/LC69004-01/4.jpg,https://oleks-netizen.github.io/product-images/LC69004-01/5.jpg,https://oleks-netizen.github.io/product-images/LC69004-01/6.jpg,https://oleks-netizen.github.io/product-images/LC69004-01/7.jpg,https://oleks-netizen.github.io/product-images/LC69004-01/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20066-6/1.jpg,https://oleks-netizen.github.io/product-images/L20066-6/3.jpg,https://oleks-netizen.github.io/product-images/L20066-6/8.jpg,https://oleks-netizen.github.io/product-images/L20066-6/4.jpg,https://oleks-netizen.github.io/product-images/L20066-6/5.jpg,https://oleks-netizen.github.io/product-images/L20066-6/6.jpg,https://oleks-netizen.github.io/product-images/L20066-6/7.jpg</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>LC69004-02</t>
+          <t>L20138-1</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69004-02/1.jpg,https://oleks-netizen.github.io/product-images/LC69004-02/2.jpg,https://oleks-netizen.github.io/product-images/LC69004-02/9.jpg,https://oleks-netizen.github.io/product-images/LC69004-02/4.jpg,https://oleks-netizen.github.io/product-images/LC69004-02/5.jpg,https://oleks-netizen.github.io/product-images/LC69004-02/6.jpg,https://oleks-netizen.github.io/product-images/LC69004-02/7.jpg,https://oleks-netizen.github.io/product-images/LC69004-02/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20138-1/1.jpg,https://oleks-netizen.github.io/product-images/L20138-1/2.jpg,https://oleks-netizen.github.io/product-images/L20138-1/3.jpg,https://oleks-netizen.github.io/product-images/L20138-1/8.jpg,https://oleks-netizen.github.io/product-images/L20138-1/5.jpg,https://oleks-netizen.github.io/product-images/L20138-1/6.jpg,https://oleks-netizen.github.io/product-images/L20138-1/7.jpg</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>LC69004-03</t>
+          <t>L20138-15</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69004-03/1.jpg,https://oleks-netizen.github.io/product-images/LC69004-03/2.jpg,https://oleks-netizen.github.io/product-images/LC69004-03/9.jpg,https://oleks-netizen.github.io/product-images/LC69004-03/4.jpg,https://oleks-netizen.github.io/product-images/LC69004-03/5.jpg,https://oleks-netizen.github.io/product-images/LC69004-03/6.jpg,https://oleks-netizen.github.io/product-images/LC69004-03/7.jpg,https://oleks-netizen.github.io/product-images/LC69004-03/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20138-15/1.jpg,https://oleks-netizen.github.io/product-images/L20138-15/2.jpg,https://oleks-netizen.github.io/product-images/L20138-15/3.jpg,https://oleks-netizen.github.io/product-images/L20138-15/8.jpg,https://oleks-netizen.github.io/product-images/L20138-15/5.jpg,https://oleks-netizen.github.io/product-images/L20138-15/6.jpg,https://oleks-netizen.github.io/product-images/L20138-15/7.jpg</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>LC69004-04</t>
+          <t>L20138-2</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69004-04/1.jpg,https://oleks-netizen.github.io/product-images/LC69004-04/2.jpg,https://oleks-netizen.github.io/product-images/LC69004-04/9.jpg,https://oleks-netizen.github.io/product-images/LC69004-04/4.jpg,https://oleks-netizen.github.io/product-images/LC69004-04/5.jpg,https://oleks-netizen.github.io/product-images/LC69004-04/6.jpg,https://oleks-netizen.github.io/product-images/LC69004-04/7.jpg,https://oleks-netizen.github.io/product-images/LC69004-04/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20138-2/1.jpg,https://oleks-netizen.github.io/product-images/L20138-2/2.jpg,https://oleks-netizen.github.io/product-images/L20138-2/3.jpg,https://oleks-netizen.github.io/product-images/L20138-2/8.jpg,https://oleks-netizen.github.io/product-images/L20138-2/5.jpg,https://oleks-netizen.github.io/product-images/L20138-2/6.jpg,https://oleks-netizen.github.io/product-images/L20138-2/7.jpg</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>LC69033-01</t>
+          <t>L20711-1</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69033-01/1.jpg,https://oleks-netizen.github.io/product-images/LC69033-01/2.jpg,https://oleks-netizen.github.io/product-images/LC69033-01/9.jpg,https://oleks-netizen.github.io/product-images/LC69033-01/4.jpg,https://oleks-netizen.github.io/product-images/LC69033-01/5.jpg,https://oleks-netizen.github.io/product-images/LC69033-01/6.jpg,https://oleks-netizen.github.io/product-images/LC69033-01/7.jpg,https://oleks-netizen.github.io/product-images/LC69033-01/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20711-1/1.jpg,https://oleks-netizen.github.io/product-images/L20711-1/2.jpg,https://oleks-netizen.github.io/product-images/L20711-1/3.jpg,https://oleks-netizen.github.io/product-images/L20711-1/8.jpg,https://oleks-netizen.github.io/product-images/L20711-1/5.jpg,https://oleks-netizen.github.io/product-images/L20711-1/6.jpg,https://oleks-netizen.github.io/product-images/L20711-1/7.jpg</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>LC69033-05</t>
+          <t>L20711-56</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69033-05/1.jpg,https://oleks-netizen.github.io/product-images/LC69033-05/2.jpg,https://oleks-netizen.github.io/product-images/LC69033-05/9.jpg,https://oleks-netizen.github.io/product-images/LC69033-05/4.jpg,https://oleks-netizen.github.io/product-images/LC69033-05/5.jpg,https://oleks-netizen.github.io/product-images/LC69033-05/6.jpg,https://oleks-netizen.github.io/product-images/LC69033-05/7.jpg,https://oleks-netizen.github.io/product-images/LC69033-05/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20711-56/1.jpg,https://oleks-netizen.github.io/product-images/L20711-56/2.jpg,https://oleks-netizen.github.io/product-images/L20711-56/3.jpg,https://oleks-netizen.github.io/product-images/L20711-56/8.jpg,https://oleks-netizen.github.io/product-images/L20711-56/5.jpg,https://oleks-netizen.github.io/product-images/L20711-56/6.jpg,https://oleks-netizen.github.io/product-images/L20711-56/7.jpg</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>LC69033-28</t>
+          <t>L20711-80</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69033-28/1.jpg,https://oleks-netizen.github.io/product-images/LC69033-28/2.jpg,https://oleks-netizen.github.io/product-images/LC69033-28/3.jpg,https://oleks-netizen.github.io/product-images/LC69033-28/4.jpg,https://oleks-netizen.github.io/product-images/LC69033-28/5.jpg,https://oleks-netizen.github.io/product-images/LC69033-28/6.jpg,https://oleks-netizen.github.io/product-images/LC69033-28/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20711-80/1.jpg,https://oleks-netizen.github.io/product-images/L20711-80/2.jpg,https://oleks-netizen.github.io/product-images/L20711-80/3.jpg,https://oleks-netizen.github.io/product-images/L20711-80/8.jpg,https://oleks-netizen.github.io/product-images/L20711-80/5.jpg,https://oleks-netizen.github.io/product-images/L20711-80/6.jpg,https://oleks-netizen.github.io/product-images/L20711-80/7.jpg</t>
         </is>
       </c>
       <c r="C89" t="n">
@@ -1761,132 +1761,132 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>LC69033-41</t>
+          <t>L20712-1</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69033-41/1.jpg,https://oleks-netizen.github.io/product-images/LC69033-41/2.jpg,https://oleks-netizen.github.io/product-images/LC69033-41/9.jpg,https://oleks-netizen.github.io/product-images/LC69033-41/4.jpg,https://oleks-netizen.github.io/product-images/LC69033-41/5.jpg,https://oleks-netizen.github.io/product-images/LC69033-41/6.jpg,https://oleks-netizen.github.io/product-images/LC69033-41/7.jpg,https://oleks-netizen.github.io/product-images/LC69033-41/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20712-1/1.jpg,https://oleks-netizen.github.io/product-images/L20712-1/2.jpg,https://oleks-netizen.github.io/product-images/L20712-1/3.jpg,https://oleks-netizen.github.io/product-images/L20712-1/8.jpg,https://oleks-netizen.github.io/product-images/L20712-1/5.jpg,https://oleks-netizen.github.io/product-images/L20712-1/6.jpg,https://oleks-netizen.github.io/product-images/L20712-1/7.jpg</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>LC69033-71</t>
+          <t>L20712-2</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69033-71/1.jpg,https://oleks-netizen.github.io/product-images/LC69033-71/2.jpg,https://oleks-netizen.github.io/product-images/LC69033-71/3.jpg,https://oleks-netizen.github.io/product-images/LC69033-71/9.jpg,https://oleks-netizen.github.io/product-images/LC69033-71/4.jpg,https://oleks-netizen.github.io/product-images/LC69033-71/5.jpg,https://oleks-netizen.github.io/product-images/LC69033-71/6.jpg,https://oleks-netizen.github.io/product-images/LC69033-71/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L20712-2/1.jpg,https://oleks-netizen.github.io/product-images/L20712-2/2.jpg,https://oleks-netizen.github.io/product-images/L20712-2/3.jpg,https://oleks-netizen.github.io/product-images/L20712-2/8.jpg,https://oleks-netizen.github.io/product-images/L20712-2/5.jpg,https://oleks-netizen.github.io/product-images/L20712-2/6.jpg,https://oleks-netizen.github.io/product-images/L20712-2/7.jpg</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>LC69052-2035</t>
+          <t>L87026-01</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69052-2035/1.jpg,https://oleks-netizen.github.io/product-images/LC69052-2035/2.jpg,https://oleks-netizen.github.io/product-images/LC69052-2035/3.jpg,https://oleks-netizen.github.io/product-images/LC69052-2035/9.jpg,https://oleks-netizen.github.io/product-images/LC69052-2035/4.jpg,https://oleks-netizen.github.io/product-images/LC69052-2035/5.jpg,https://oleks-netizen.github.io/product-images/LC69052-2035/6.jpg,https://oleks-netizen.github.io/product-images/LC69052-2035/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L87026-01/1.jpg,https://oleks-netizen.github.io/product-images/L87026-01/2.jpg,https://oleks-netizen.github.io/product-images/L87026-01/3.jpg,https://oleks-netizen.github.io/product-images/L87026-01/10.jpg,https://oleks-netizen.github.io/product-images/L87026-01/5.jpg,https://oleks-netizen.github.io/product-images/L87026-01/6.jpg,https://oleks-netizen.github.io/product-images/L87026-01/7.jpg,https://oleks-netizen.github.io/product-images/L87026-01/8.jpg,https://oleks-netizen.github.io/product-images/L87026-01/9.jpg</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>LC69052-2036</t>
+          <t>L87026-130</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69052-2036/1.jpg,https://oleks-netizen.github.io/product-images/LC69052-2036/2.jpg,https://oleks-netizen.github.io/product-images/LC69052-2036/3.jpg,https://oleks-netizen.github.io/product-images/LC69052-2036/9.jpg,https://oleks-netizen.github.io/product-images/LC69052-2036/4.jpg,https://oleks-netizen.github.io/product-images/LC69052-2036/5.jpg,https://oleks-netizen.github.io/product-images/LC69052-2036/6.jpg,https://oleks-netizen.github.io/product-images/LC69052-2036/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L87026-130/1.jpg,https://oleks-netizen.github.io/product-images/L87026-130/2.jpg,https://oleks-netizen.github.io/product-images/L87026-130/3.jpg,https://oleks-netizen.github.io/product-images/L87026-130/10.jpg,https://oleks-netizen.github.io/product-images/L87026-130/5.jpg,https://oleks-netizen.github.io/product-images/L87026-130/6.jpg,https://oleks-netizen.github.io/product-images/L87026-130/7.jpg,https://oleks-netizen.github.io/product-images/L87026-130/8.jpg,https://oleks-netizen.github.io/product-images/L87026-130/9.jpg</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>LC69052-2058</t>
+          <t>L87026-152</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69052-2058/1.jpg,https://oleks-netizen.github.io/product-images/LC69052-2058/2.jpg,https://oleks-netizen.github.io/product-images/LC69052-2058/3.jpg,https://oleks-netizen.github.io/product-images/LC69052-2058/9.jpg,https://oleks-netizen.github.io/product-images/LC69052-2058/4.jpg,https://oleks-netizen.github.io/product-images/LC69052-2058/5.jpg,https://oleks-netizen.github.io/product-images/LC69052-2058/6.jpg,https://oleks-netizen.github.io/product-images/LC69052-2058/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L87026-152/1.jpg,https://oleks-netizen.github.io/product-images/L87026-152/2.jpg,https://oleks-netizen.github.io/product-images/L87026-152/3.jpg,https://oleks-netizen.github.io/product-images/L87026-152/10.jpg,https://oleks-netizen.github.io/product-images/L87026-152/5.jpg,https://oleks-netizen.github.io/product-images/L87026-152/6.jpg,https://oleks-netizen.github.io/product-images/L87026-152/7.jpg,https://oleks-netizen.github.io/product-images/L87026-152/8.jpg,https://oleks-netizen.github.io/product-images/L87026-152/9.jpg</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>LC69052-2259</t>
+          <t>L87110-01</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69052-2259/1.jpg,https://oleks-netizen.github.io/product-images/LC69052-2259/2.jpg,https://oleks-netizen.github.io/product-images/LC69052-2259/3.jpg,https://oleks-netizen.github.io/product-images/LC69052-2259/9.jpg,https://oleks-netizen.github.io/product-images/LC69052-2259/4.jpg,https://oleks-netizen.github.io/product-images/LC69052-2259/5.jpg,https://oleks-netizen.github.io/product-images/LC69052-2259/6.jpg,https://oleks-netizen.github.io/product-images/LC69052-2259/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L87110-01/1.jpg,https://oleks-netizen.github.io/product-images/L87110-01/2.jpg,https://oleks-netizen.github.io/product-images/L87110-01/10.jpg,https://oleks-netizen.github.io/product-images/L87110-01/4.jpg,https://oleks-netizen.github.io/product-images/L87110-01/5.jpg,https://oleks-netizen.github.io/product-images/L87110-01/6.jpg,https://oleks-netizen.github.io/product-images/L87110-01/7.jpg,https://oleks-netizen.github.io/product-images/L87110-01/8.jpg,https://oleks-netizen.github.io/product-images/L87110-01/9.jpg</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>LC69055-01</t>
+          <t>L87110-13</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69055-01/1.jpg,https://oleks-netizen.github.io/product-images/LC69055-01/2.jpg,https://oleks-netizen.github.io/product-images/LC69055-01/3.jpg,https://oleks-netizen.github.io/product-images/LC69055-01/9.jpg,https://oleks-netizen.github.io/product-images/LC69055-01/4.jpg,https://oleks-netizen.github.io/product-images/LC69055-01/5.jpg,https://oleks-netizen.github.io/product-images/LC69055-01/6.jpg,https://oleks-netizen.github.io/product-images/LC69055-01/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L87110-13/1.jpg,https://oleks-netizen.github.io/product-images/L87110-13/2.jpg,https://oleks-netizen.github.io/product-images/L87110-13/10.jpg,https://oleks-netizen.github.io/product-images/L87110-13/4.jpg,https://oleks-netizen.github.io/product-images/L87110-13/5.jpg,https://oleks-netizen.github.io/product-images/L87110-13/6.jpg,https://oleks-netizen.github.io/product-images/L87110-13/7.jpg,https://oleks-netizen.github.io/product-images/L87110-13/8.jpg,https://oleks-netizen.github.io/product-images/L87110-13/9.jpg</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>LC69055-26</t>
+          <t>L87110-22</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69055-26/1.jpg,https://oleks-netizen.github.io/product-images/LC69055-26/2.jpg,https://oleks-netizen.github.io/product-images/LC69055-26/9.jpg,https://oleks-netizen.github.io/product-images/LC69055-26/3.jpg,https://oleks-netizen.github.io/product-images/LC69055-26/4.jpg,https://oleks-netizen.github.io/product-images/LC69055-26/5.jpg,https://oleks-netizen.github.io/product-images/LC69055-26/6.jpg,https://oleks-netizen.github.io/product-images/LC69055-26/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L87110-22/1.jpg,https://oleks-netizen.github.io/product-images/L87110-22/2.jpg,https://oleks-netizen.github.io/product-images/L87110-22/10.jpg,https://oleks-netizen.github.io/product-images/L87110-22/4.jpg,https://oleks-netizen.github.io/product-images/L87110-22/5.jpg,https://oleks-netizen.github.io/product-images/L87110-22/6.jpg,https://oleks-netizen.github.io/product-images/L87110-22/7.jpg,https://oleks-netizen.github.io/product-images/L87110-22/8.jpg,https://oleks-netizen.github.io/product-images/L87110-22/9.jpg</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>LC69055-71</t>
+          <t>L87110-23</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69055-71/1.jpg,https://oleks-netizen.github.io/product-images/LC69055-71/2.jpg,https://oleks-netizen.github.io/product-images/LC69055-71/9.jpg,https://oleks-netizen.github.io/product-images/LC69055-71/3.jpg,https://oleks-netizen.github.io/product-images/LC69055-71/4.jpg,https://oleks-netizen.github.io/product-images/LC69055-71/5.jpg,https://oleks-netizen.github.io/product-images/LC69055-71/6.jpg,https://oleks-netizen.github.io/product-images/LC69055-71/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L87110-23/1.jpg,https://oleks-netizen.github.io/product-images/L87110-23/2.jpg,https://oleks-netizen.github.io/product-images/L87110-23/6.jpg,https://oleks-netizen.github.io/product-images/L87110-23/4.jpg,https://oleks-netizen.github.io/product-images/L87110-23/5.jpg,https://oleks-netizen.github.io/product-images/L87110-23/7.jpg,https://oleks-netizen.github.io/product-images/L87110-23/8.jpg,https://oleks-netizen.github.io/product-images/L87110-23/9.jpg</t>
         </is>
       </c>
       <c r="C98" t="n">
@@ -1896,57 +1896,57 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>LC69055-76</t>
+          <t>L87296-01</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69055-76/1.jpg,https://oleks-netizen.github.io/product-images/LC69055-76/2.jpg,https://oleks-netizen.github.io/product-images/LC69055-76/9.jpg,https://oleks-netizen.github.io/product-images/LC69055-76/3.jpg,https://oleks-netizen.github.io/product-images/LC69055-76/4.jpg,https://oleks-netizen.github.io/product-images/LC69055-76/5.jpg,https://oleks-netizen.github.io/product-images/LC69055-76/6.jpg,https://oleks-netizen.github.io/product-images/LC69055-76/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L87296-01/1.jpg,https://oleks-netizen.github.io/product-images/L87296-01/2.jpg,https://oleks-netizen.github.io/product-images/L87296-01/10.jpg,https://oleks-netizen.github.io/product-images/L87296-01/4.jpg,https://oleks-netizen.github.io/product-images/L87296-01/5.jpg,https://oleks-netizen.github.io/product-images/L87296-01/6.jpg,https://oleks-netizen.github.io/product-images/L87296-01/7.jpg,https://oleks-netizen.github.io/product-images/L87296-01/8.jpg,https://oleks-netizen.github.io/product-images/L87296-01/9.jpg</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>LC69055-84</t>
+          <t>L87296-13</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69055-84/1.jpg,https://oleks-netizen.github.io/product-images/LC69055-84/2.jpg,https://oleks-netizen.github.io/product-images/LC69055-84/9.jpg,https://oleks-netizen.github.io/product-images/LC69055-84/3.jpg,https://oleks-netizen.github.io/product-images/LC69055-84/4.jpg,https://oleks-netizen.github.io/product-images/LC69055-84/5.jpg,https://oleks-netizen.github.io/product-images/LC69055-84/6.jpg,https://oleks-netizen.github.io/product-images/LC69055-84/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L87296-13/1.jpg,https://oleks-netizen.github.io/product-images/L87296-13/2.jpg,https://oleks-netizen.github.io/product-images/L87296-13/10.jpg,https://oleks-netizen.github.io/product-images/L87296-13/4.jpg,https://oleks-netizen.github.io/product-images/L87296-13/5.jpg,https://oleks-netizen.github.io/product-images/L87296-13/6.jpg,https://oleks-netizen.github.io/product-images/L87296-13/7.jpg,https://oleks-netizen.github.io/product-images/L87296-13/8.jpg,https://oleks-netizen.github.io/product-images/L87296-13/9.jpg</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>LC69802-01</t>
+          <t>L87296-23</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69802-01/1.jpg,https://oleks-netizen.github.io/product-images/LC69802-01/2.jpg,https://oleks-netizen.github.io/product-images/LC69802-01/3.jpg,https://oleks-netizen.github.io/product-images/LC69802-01/9.jpg,https://oleks-netizen.github.io/product-images/LC69802-01/4.jpg,https://oleks-netizen.github.io/product-images/LC69802-01/5.jpg,https://oleks-netizen.github.io/product-images/LC69802-01/6.jpg,https://oleks-netizen.github.io/product-images/LC69802-01/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L87296-23/1.jpg,https://oleks-netizen.github.io/product-images/L87296-23/2.jpg,https://oleks-netizen.github.io/product-images/L87296-23/10.jpg,https://oleks-netizen.github.io/product-images/L87296-23/4.jpg,https://oleks-netizen.github.io/product-images/L87296-23/5.jpg,https://oleks-netizen.github.io/product-images/L87296-23/6.jpg,https://oleks-netizen.github.io/product-images/L87296-23/7.jpg,https://oleks-netizen.github.io/product-images/L87296-23/8.jpg,https://oleks-netizen.github.io/product-images/L87296-23/9.jpg</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>LC69802-12</t>
+          <t>L87296-33</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69802-12/1.jpg,https://oleks-netizen.github.io/product-images/LC69802-12/2.jpg,https://oleks-netizen.github.io/product-images/LC69802-12/3.jpg,https://oleks-netizen.github.io/product-images/LC69802-12/9.jpg,https://oleks-netizen.github.io/product-images/LC69802-12/4.jpg,https://oleks-netizen.github.io/product-images/LC69802-12/5.jpg,https://oleks-netizen.github.io/product-images/LC69802-12/6.jpg,https://oleks-netizen.github.io/product-images/LC69802-12/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L87296-33/1.jpg,https://oleks-netizen.github.io/product-images/L87296-33/2.jpg,https://oleks-netizen.github.io/product-images/L87296-33/4.jpg,https://oleks-netizen.github.io/product-images/L87296-33/5.jpg,https://oleks-netizen.github.io/product-images/L87296-33/6.jpg,https://oleks-netizen.github.io/product-images/L87296-33/7.jpg,https://oleks-netizen.github.io/product-images/L87296-33/8.jpg,https://oleks-netizen.github.io/product-images/L87296-33/9.jpg</t>
         </is>
       </c>
       <c r="C102" t="n">
@@ -1956,102 +1956,102 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>LC69802-25</t>
+          <t>L87454-01</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69802-25/1.jpg,https://oleks-netizen.github.io/product-images/LC69802-25/2.jpg,https://oleks-netizen.github.io/product-images/LC69802-25/9.jpg,https://oleks-netizen.github.io/product-images/LC69802-25/4.jpg,https://oleks-netizen.github.io/product-images/LC69802-25/5.jpg,https://oleks-netizen.github.io/product-images/LC69802-25/6.jpg,https://oleks-netizen.github.io/product-images/LC69802-25/7.jpg,https://oleks-netizen.github.io/product-images/LC69802-25/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L87454-01/1.jpg,https://oleks-netizen.github.io/product-images/L87454-01/2.jpg,https://oleks-netizen.github.io/product-images/L87454-01/7.jpg,https://oleks-netizen.github.io/product-images/L87454-01/4.jpg,https://oleks-netizen.github.io/product-images/L87454-01/5.jpg,https://oleks-netizen.github.io/product-images/L87454-01/6.jpg,https://oleks-netizen.github.io/product-images/L87454-01/9.jpg</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>LC69802-71</t>
+          <t>L87454-06</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69802-71/1.jpg,https://oleks-netizen.github.io/product-images/LC69802-71/2.jpg,https://oleks-netizen.github.io/product-images/LC69802-71/3.jpg,https://oleks-netizen.github.io/product-images/LC69802-71/9.jpg,https://oleks-netizen.github.io/product-images/LC69802-71/4.jpg,https://oleks-netizen.github.io/product-images/LC69802-71/5.jpg,https://oleks-netizen.github.io/product-images/LC69802-71/6.jpg,https://oleks-netizen.github.io/product-images/LC69802-71/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L87454-06/1.jpg,https://oleks-netizen.github.io/product-images/L87454-06/2.jpg,https://oleks-netizen.github.io/product-images/L87454-06/10.jpg,https://oleks-netizen.github.io/product-images/L87454-06/4.jpg,https://oleks-netizen.github.io/product-images/L87454-06/5.jpg,https://oleks-netizen.github.io/product-images/L87454-06/6.jpg,https://oleks-netizen.github.io/product-images/L87454-06/7.jpg,https://oleks-netizen.github.io/product-images/L87454-06/8.jpg,https://oleks-netizen.github.io/product-images/L87454-06/9.jpg</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>LC69855-2058</t>
+          <t>L87454-81</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69855-2058/1.jpg,https://oleks-netizen.github.io/product-images/LC69855-2058/2.jpg,https://oleks-netizen.github.io/product-images/LC69855-2058/3.jpg,https://oleks-netizen.github.io/product-images/LC69855-2058/9.jpg,https://oleks-netizen.github.io/product-images/LC69855-2058/4.jpg,https://oleks-netizen.github.io/product-images/LC69855-2058/5.jpg,https://oleks-netizen.github.io/product-images/LC69855-2058/6.jpg,https://oleks-netizen.github.io/product-images/LC69855-2058/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L87454-81/1.jpg,https://oleks-netizen.github.io/product-images/L87454-81/2.jpg,https://oleks-netizen.github.io/product-images/L87454-81/10.jpg,https://oleks-netizen.github.io/product-images/L87454-81/4.jpg,https://oleks-netizen.github.io/product-images/L87454-81/5.jpg,https://oleks-netizen.github.io/product-images/L87454-81/6.jpg,https://oleks-netizen.github.io/product-images/L87454-81/7.jpg,https://oleks-netizen.github.io/product-images/L87454-81/8.jpg,https://oleks-netizen.github.io/product-images/L87454-81/9.jpg</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>LC69855-2259</t>
+          <t>L87598-01</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69855-2259/1.jpg,https://oleks-netizen.github.io/product-images/LC69855-2259/2.jpg,https://oleks-netizen.github.io/product-images/LC69855-2259/8.jpg,https://oleks-netizen.github.io/product-images/LC69855-2259/4.jpg,https://oleks-netizen.github.io/product-images/LC69855-2259/5.jpg,https://oleks-netizen.github.io/product-images/LC69855-2259/6.jpg,https://oleks-netizen.github.io/product-images/LC69855-2259/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L87598-01/1.jpg,https://oleks-netizen.github.io/product-images/L87598-01/2.jpg,https://oleks-netizen.github.io/product-images/L87598-01/10.jpg,https://oleks-netizen.github.io/product-images/L87598-01/4.jpg,https://oleks-netizen.github.io/product-images/L87598-01/5.jpg,https://oleks-netizen.github.io/product-images/L87598-01/6.jpg,https://oleks-netizen.github.io/product-images/L87598-01/7.jpg,https://oleks-netizen.github.io/product-images/L87598-01/8.jpg,https://oleks-netizen.github.io/product-images/L87598-01/9.jpg</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>LC69855-2291</t>
+          <t>L87598-13</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC69855-2291/1.jpg,https://oleks-netizen.github.io/product-images/LC69855-2291/2.jpg,https://oleks-netizen.github.io/product-images/LC69855-2291/9.jpg,https://oleks-netizen.github.io/product-images/LC69855-2291/4.jpg,https://oleks-netizen.github.io/product-images/LC69855-2291/5.jpg,https://oleks-netizen.github.io/product-images/LC69855-2291/6.jpg,https://oleks-netizen.github.io/product-images/LC69855-2291/7.jpg,https://oleks-netizen.github.io/product-images/LC69855-2291/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L87598-13/1.jpg,https://oleks-netizen.github.io/product-images/L87598-13/2.jpg,https://oleks-netizen.github.io/product-images/L87598-13/3.jpg,https://oleks-netizen.github.io/product-images/L87598-13/10.jpg,https://oleks-netizen.github.io/product-images/L87598-13/5.jpg,https://oleks-netizen.github.io/product-images/L87598-13/6.jpg,https://oleks-netizen.github.io/product-images/L87598-13/7.jpg,https://oleks-netizen.github.io/product-images/L87598-13/8.jpg,https://oleks-netizen.github.io/product-images/L87598-13/9.jpg</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>RB-8033-4lx</t>
+          <t>L87598-23</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RB-8033-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RB-8033-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RB-8033-4lx/6.jpg,https://oleks-netizen.github.io/product-images/RB-8033-4lx/4.jpg,https://oleks-netizen.github.io/product-images/RB-8033-4lx/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L87598-23/1.jpg,https://oleks-netizen.github.io/product-images/L87598-23/2.jpg,https://oleks-netizen.github.io/product-images/L87598-23/3.jpg,https://oleks-netizen.github.io/product-images/L87598-23/10.jpg,https://oleks-netizen.github.io/product-images/L87598-23/5.jpg,https://oleks-netizen.github.io/product-images/L87598-23/6.jpg,https://oleks-netizen.github.io/product-images/L87598-23/7.jpg,https://oleks-netizen.github.io/product-images/L87598-23/8.jpg,https://oleks-netizen.github.io/product-images/L87598-23/9.jpg</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>RC-3990-3md</t>
+          <t>L87598-31</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RC-3990-3md/1.jpg,https://oleks-netizen.github.io/product-images/RC-3990-3md/2.jpg,https://oleks-netizen.github.io/product-images/RC-3990-3md/4.jpg,https://oleks-netizen.github.io/product-images/RC-3990-3md/10.jpg,https://oleks-netizen.github.io/product-images/RC-3990-3md/5.jpg,https://oleks-netizen.github.io/product-images/RC-3990-3md/6.jpg,https://oleks-netizen.github.io/product-images/RC-3990-3md/7.jpg,https://oleks-netizen.github.io/product-images/RC-3990-3md/8.jpg,https://oleks-netizen.github.io/product-images/RC-3990-3md/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L87598-31/1.jpg,https://oleks-netizen.github.io/product-images/L87598-31/2.jpg,https://oleks-netizen.github.io/product-images/L87598-31/3.jpg,https://oleks-netizen.github.io/product-images/L87598-31/10.jpg,https://oleks-netizen.github.io/product-images/L87598-31/5.jpg,https://oleks-netizen.github.io/product-images/L87598-31/6.jpg,https://oleks-netizen.github.io/product-images/L87598-31/7.jpg,https://oleks-netizen.github.io/product-images/L87598-31/8.jpg,https://oleks-netizen.github.io/product-images/L87598-31/9.jpg</t>
         </is>
       </c>
       <c r="C109" t="n">
@@ -2061,162 +2061,162 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>RC-60125-3md</t>
+          <t>L87640-01</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RC-60125-3md/1.jpg,https://oleks-netizen.github.io/product-images/RC-60125-3md/2.jpg,https://oleks-netizen.github.io/product-images/RC-60125-3md/7.jpg,https://oleks-netizen.github.io/product-images/RC-60125-3md/4.jpg,https://oleks-netizen.github.io/product-images/RC-60125-3md/5.jpg,https://oleks-netizen.github.io/product-images/RC-60125-3md/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L87640-01/1.jpg,https://oleks-netizen.github.io/product-images/L87640-01/2.jpg,https://oleks-netizen.github.io/product-images/L87640-01/3.jpg,https://oleks-netizen.github.io/product-images/L87640-01/6.jpg,https://oleks-netizen.github.io/product-images/L87640-01/5.jpg,https://oleks-netizen.github.io/product-images/L87640-01/7.jpg,https://oleks-netizen.github.io/product-images/L87640-01/8.jpg</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>RCc-1313-4lx</t>
+          <t>L87640-130</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RCc-1313-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RCc-1313-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RCc-1313-4lx/8.jpg,https://oleks-netizen.github.io/product-images/RCc-1313-4lx/3.jpg,https://oleks-netizen.github.io/product-images/RCc-1313-4lx/4.jpg,https://oleks-netizen.github.io/product-images/RCc-1313-4lx/5.jpg,https://oleks-netizen.github.io/product-images/RCc-1313-4lx/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L87640-130/1.jpg,https://oleks-netizen.github.io/product-images/L87640-130/2.jpg,https://oleks-netizen.github.io/product-images/L87640-130/3.jpg,https://oleks-netizen.github.io/product-images/L87640-130/4.jpg,https://oleks-netizen.github.io/product-images/L87640-130/5.jpg,https://oleks-netizen.github.io/product-images/L87640-130/6.jpg,https://oleks-netizen.github.io/product-images/L87640-130/7.jpg,https://oleks-netizen.github.io/product-images/L87640-130/8.jpg</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>RCh-1313-4lx</t>
+          <t>L87640-246</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RCh-1313-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RCh-1313-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RCh-1313-4lx/6.jpg,https://oleks-netizen.github.io/product-images/RCh-1313-4lx/3.jpg,https://oleks-netizen.github.io/product-images/RCh-1313-4lx/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L87640-246/1.jpg,https://oleks-netizen.github.io/product-images/L87640-246/2.jpg,https://oleks-netizen.github.io/product-images/L87640-246/9.jpg,https://oleks-netizen.github.io/product-images/L87640-246/4.jpg,https://oleks-netizen.github.io/product-images/L87640-246/5.jpg,https://oleks-netizen.github.io/product-images/L87640-246/6.jpg,https://oleks-netizen.github.io/product-images/L87640-246/7.jpg,https://oleks-netizen.github.io/product-images/L87640-246/8.jpg</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>RCj-0320-4lx</t>
+          <t>L87640-36</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RCj-0320-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RCj-0320-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RCj-0320-4lx/6.jpg,https://oleks-netizen.github.io/product-images/RCj-0320-4lx/4.jpg,https://oleks-netizen.github.io/product-images/RCj-0320-4lx/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L87640-36/1.jpg,https://oleks-netizen.github.io/product-images/L87640-36/2.jpg,https://oleks-netizen.github.io/product-images/L87640-36/9.jpg,https://oleks-netizen.github.io/product-images/L87640-36/4.jpg,https://oleks-netizen.github.io/product-images/L87640-36/5.jpg,https://oleks-netizen.github.io/product-images/L87640-36/6.jpg,https://oleks-netizen.github.io/product-images/L87640-36/7.jpg,https://oleks-netizen.github.io/product-images/L87640-36/8.jpg</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>RCj-1313-4lx</t>
+          <t>LC46019-1</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RCj-1313-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RCj-1313-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RCj-1313-4lx/6.jpg,https://oleks-netizen.github.io/product-images/RCj-1313-4lx/3.jpg,https://oleks-netizen.github.io/product-images/RCj-1313-4lx/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC46019-1/1.jpg,https://oleks-netizen.github.io/product-images/LC46019-1/2.jpg,https://oleks-netizen.github.io/product-images/LC46019-1/3.jpg,https://oleks-netizen.github.io/product-images/LC46019-1/4.jpg,https://oleks-netizen.github.io/product-images/LC46019-1/5.jpg,https://oleks-netizen.github.io/product-images/LC46019-1/6.jpg,https://oleks-netizen.github.io/product-images/LC46019-1/7.jpg,https://oleks-netizen.github.io/product-images/LC46019-1/8.jpg</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>RE-0001-4lx</t>
+          <t>LC46058-1</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RE-0001-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RE-0001-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RE-0001-4lx/9.jpg,https://oleks-netizen.github.io/product-images/RE-0001-4lx/4.jpg,https://oleks-netizen.github.io/product-images/RE-0001-4lx/5.jpg,https://oleks-netizen.github.io/product-images/RE-0001-4lx/6.jpg,https://oleks-netizen.github.io/product-images/RE-0001-4lx/7.jpg,https://oleks-netizen.github.io/product-images/RE-0001-4lx/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC46058-1/1.jpg,https://oleks-netizen.github.io/product-images/LC46058-1/2.jpg,https://oleks-netizen.github.io/product-images/LC46058-1/10.jpg,https://oleks-netizen.github.io/product-images/LC46058-1/4.jpg,https://oleks-netizen.github.io/product-images/LC46058-1/5.jpg,https://oleks-netizen.github.io/product-images/LC46058-1/6.jpg,https://oleks-netizen.github.io/product-images/LC46058-1/7.jpg,https://oleks-netizen.github.io/product-images/LC46058-1/8.jpg,https://oleks-netizen.github.io/product-images/LC46058-1/9.jpg</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>RE-60125-3md</t>
+          <t>LC46058-2</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RE-60125-3md/1.jpg,https://oleks-netizen.github.io/product-images/RE-60125-3md/2.jpg,https://oleks-netizen.github.io/product-images/RE-60125-3md/7.jpg,https://oleks-netizen.github.io/product-images/RE-60125-3md/3.jpg,https://oleks-netizen.github.io/product-images/RE-60125-3md/4.jpg,https://oleks-netizen.github.io/product-images/RE-60125-3md/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC46058-2/1.jpg,https://oleks-netizen.github.io/product-images/LC46058-2/2.jpg,https://oleks-netizen.github.io/product-images/LC46058-2/9.jpg,https://oleks-netizen.github.io/product-images/LC46058-2/4.jpg,https://oleks-netizen.github.io/product-images/LC46058-2/5.jpg,https://oleks-netizen.github.io/product-images/LC46058-2/6.jpg,https://oleks-netizen.github.io/product-images/LC46058-2/7.jpg,https://oleks-netizen.github.io/product-images/LC46058-2/8.jpg</t>
         </is>
       </c>
       <c r="C116" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>RK-60125-3md</t>
+          <t>LC46116-1</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RK-60125-3md/1.jpg,https://oleks-netizen.github.io/product-images/RK-60125-3md/2.jpg,https://oleks-netizen.github.io/product-images/RK-60125-3md/7.jpg,https://oleks-netizen.github.io/product-images/RK-60125-3md/4.jpg,https://oleks-netizen.github.io/product-images/RK-60125-3md/5.jpg,https://oleks-netizen.github.io/product-images/RK-60125-3md/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC46116-1/1.jpg,https://oleks-netizen.github.io/product-images/LC46116-1/2.jpg,https://oleks-netizen.github.io/product-images/LC46116-1/8.jpg,https://oleks-netizen.github.io/product-images/LC46116-1/4.jpg,https://oleks-netizen.github.io/product-images/LC46116-1/5.jpg,https://oleks-netizen.github.io/product-images/LC46116-1/6.jpg,https://oleks-netizen.github.io/product-images/LC46116-1/7.jpg</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>RY-1819-3md</t>
+          <t>LC46118-1</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RY-1819-3md/1.jpg,https://oleks-netizen.github.io/product-images/RY-1819-3md/7.jpg,https://oleks-netizen.github.io/product-images/RY-1819-3md/8.jpg,https://oleks-netizen.github.io/product-images/RY-1819-3md/3.jpg,https://oleks-netizen.github.io/product-images/RY-1819-3md/4.jpg,https://oleks-netizen.github.io/product-images/RY-1819-3md/5.jpg,https://oleks-netizen.github.io/product-images/RY-1819-3md/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC46118-1/1.jpg,https://oleks-netizen.github.io/product-images/LC46118-1/2.jpg,https://oleks-netizen.github.io/product-images/LC46118-1/3.jpg,https://oleks-netizen.github.io/product-images/LC46118-1/4.jpg,https://oleks-netizen.github.io/product-images/LC46118-1/5.jpg,https://oleks-netizen.github.io/product-images/LC46118-1/6.jpg,https://oleks-netizen.github.io/product-images/LC46118-1/7.jpg,https://oleks-netizen.github.io/product-images/LC46118-1/8.jpg</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>RА-60121-3md</t>
+          <t>LC46235-1</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RА-60121-3md/1.jpg,https://oleks-netizen.github.io/product-images/RА-60121-3md/2.jpg,https://oleks-netizen.github.io/product-images/RА-60121-3md/5.jpg,https://oleks-netizen.github.io/product-images/RА-60121-3md/9.jpg,https://oleks-netizen.github.io/product-images/RА-60121-3md/3.jpg,https://oleks-netizen.github.io/product-images/RА-60121-3md/4.jpg,https://oleks-netizen.github.io/product-images/RА-60121-3md/6.jpg,https://oleks-netizen.github.io/product-images/RА-60121-3md/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC46235-1/1.jpg,https://oleks-netizen.github.io/product-images/LC46235-1/2.jpg,https://oleks-netizen.github.io/product-images/LC46235-1/10.jpg,https://oleks-netizen.github.io/product-images/LC46235-1/3.jpg,https://oleks-netizen.github.io/product-images/LC46235-1/5.jpg,https://oleks-netizen.github.io/product-images/LC46235-1/6.jpg,https://oleks-netizen.github.io/product-images/LC46235-1/7.jpg,https://oleks-netizen.github.io/product-images/LC46235-1/8.jpg,https://oleks-netizen.github.io/product-images/LC46235-1/9.jpg</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>RЕ-60121-3md</t>
+          <t>LC46245-1</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RЕ-60121-3md/1.jpg,https://oleks-netizen.github.io/product-images/RЕ-60121-3md/2.jpg,https://oleks-netizen.github.io/product-images/RЕ-60121-3md/5.jpg,https://oleks-netizen.github.io/product-images/RЕ-60121-3md/9.jpg,https://oleks-netizen.github.io/product-images/RЕ-60121-3md/3.jpg,https://oleks-netizen.github.io/product-images/RЕ-60121-3md/4.jpg,https://oleks-netizen.github.io/product-images/RЕ-60121-3md/6.jpg,https://oleks-netizen.github.io/product-images/RЕ-60121-3md/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC46245-1/1.jpg,https://oleks-netizen.github.io/product-images/LC46245-1/2.jpg,https://oleks-netizen.github.io/product-images/LC46245-1/3.jpg,https://oleks-netizen.github.io/product-images/LC46245-1/4.jpg,https://oleks-netizen.github.io/product-images/LC46245-1/5.jpg,https://oleks-netizen.github.io/product-images/LC46245-1/6.jpg,https://oleks-netizen.github.io/product-images/LC46245-1/7.jpg,https://oleks-netizen.github.io/product-images/LC46245-1/8.jpg</t>
         </is>
       </c>
       <c r="C120" t="n">
@@ -2226,12 +2226,12 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>RК-60121-3md</t>
+          <t>LC46523-1</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RК-60121-3md/1.jpg,https://oleks-netizen.github.io/product-images/RК-60121-3md/2.jpg,https://oleks-netizen.github.io/product-images/RК-60121-3md/5.jpg,https://oleks-netizen.github.io/product-images/RК-60121-3md/9.jpg,https://oleks-netizen.github.io/product-images/RК-60121-3md/3.jpg,https://oleks-netizen.github.io/product-images/RК-60121-3md/4.jpg,https://oleks-netizen.github.io/product-images/RК-60121-3md/6.jpg,https://oleks-netizen.github.io/product-images/RК-60121-3md/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC46523-1/1.jpg,https://oleks-netizen.github.io/product-images/LC46523-1/2.jpg,https://oleks-netizen.github.io/product-images/LC46523-1/3.jpg,https://oleks-netizen.github.io/product-images/LC46523-1/4.jpg,https://oleks-netizen.github.io/product-images/LC46523-1/5.jpg,https://oleks-netizen.github.io/product-images/LC46523-1/6.jpg,https://oleks-netizen.github.io/product-images/LC46523-1/7.jpg,https://oleks-netizen.github.io/product-images/LC46523-1/8.jpg</t>
         </is>
       </c>
       <c r="C121" t="n">
@@ -2241,106 +2241,631 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>TW-Explorer-S-brown</t>
+          <t>LC46655-1</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-Explorer-S-brown/1.jpg,https://oleks-netizen.github.io/product-images/TW-Explorer-S-brown/2.jpg,https://oleks-netizen.github.io/product-images/TW-Explorer-S-brown/5.jpg,https://oleks-netizen.github.io/product-images/TW-Explorer-S-brown/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC46655-1/1.jpg,https://oleks-netizen.github.io/product-images/LC46655-1/2.jpg,https://oleks-netizen.github.io/product-images/LC46655-1/3.jpg,https://oleks-netizen.github.io/product-images/LC46655-1/4.jpg,https://oleks-netizen.github.io/product-images/LC46655-1/5.jpg,https://oleks-netizen.github.io/product-images/LC46655-1/6.jpg,https://oleks-netizen.github.io/product-images/LC46655-1/7.jpg,https://oleks-netizen.github.io/product-images/LC46655-1/8.jpg</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>TW-Explorer-S-dark-blue</t>
+          <t>LC46655-2</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-Explorer-S-dark-blue/1.jpg,https://oleks-netizen.github.io/product-images/TW-Explorer-S-dark-blue/2.jpg,https://oleks-netizen.github.io/product-images/TW-Explorer-S-dark-blue/5.jpg,https://oleks-netizen.github.io/product-images/TW-Explorer-S-dark-blue/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC46655-2/1.jpg,https://oleks-netizen.github.io/product-images/LC46655-2/2.jpg,https://oleks-netizen.github.io/product-images/LC46655-2/9.jpg,https://oleks-netizen.github.io/product-images/LC46655-2/4.jpg,https://oleks-netizen.github.io/product-images/LC46655-2/5.jpg,https://oleks-netizen.github.io/product-images/LC46655-2/6.jpg,https://oleks-netizen.github.io/product-images/LC46655-2/7.jpg,https://oleks-netizen.github.io/product-images/LC46655-2/8.jpg</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>TW-Lina-black-flo</t>
+          <t>LC46921-1</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-Lina-black-flo/1.jpg,https://oleks-netizen.github.io/product-images/TW-Lina-black-flo/9.jpg,https://oleks-netizen.github.io/product-images/TW-Lina-black-flo/3.jpg,https://oleks-netizen.github.io/product-images/TW-Lina-black-flo/4.jpg,https://oleks-netizen.github.io/product-images/TW-Lina-black-flo/5.jpg,https://oleks-netizen.github.io/product-images/TW-Lina-black-flo/6.jpg,https://oleks-netizen.github.io/product-images/TW-Lina-black-flo/7.jpg,https://oleks-netizen.github.io/product-images/TW-Lina-black-flo/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC46921-1/1.jpg,https://oleks-netizen.github.io/product-images/LC46921-1/2.jpg,https://oleks-netizen.github.io/product-images/LC46921-1/3.jpg,https://oleks-netizen.github.io/product-images/LC46921-1/4.jpg,https://oleks-netizen.github.io/product-images/LC46921-1/5.jpg,https://oleks-netizen.github.io/product-images/LC46921-1/6.jpg,https://oleks-netizen.github.io/product-images/LC46921-1/7.jpg,https://oleks-netizen.github.io/product-images/LC46921-1/8.jpg,https://oleks-netizen.github.io/product-images/LC46921-1/9.jpg</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>TW-Mini-bag-m-black</t>
+          <t>LC46921-2</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-Mini-bag-m-black/1.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC46921-2/1.jpg,https://oleks-netizen.github.io/product-images/LC46921-2/2.jpg,https://oleks-netizen.github.io/product-images/LC46921-2/3.jpg,https://oleks-netizen.github.io/product-images/LC46921-2/4.jpg,https://oleks-netizen.github.io/product-images/LC46921-2/5.jpg,https://oleks-netizen.github.io/product-images/LC46921-2/6.jpg,https://oleks-netizen.github.io/product-images/LC46921-2/7.jpg,https://oleks-netizen.github.io/product-images/LC46921-2/8.jpg,https://oleks-netizen.github.io/product-images/LC46921-2/9.jpg</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>TW-Nancy-1-caramel</t>
+          <t>LC46931-1</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-Nancy-1-caramel/1.jpg,https://oleks-netizen.github.io/product-images/TW-Nancy-1-caramel/2.jpg,https://oleks-netizen.github.io/product-images/TW-Nancy-1-caramel/7.jpg,https://oleks-netizen.github.io/product-images/TW-Nancy-1-caramel/3.jpg,https://oleks-netizen.github.io/product-images/TW-Nancy-1-caramel/4.jpg,https://oleks-netizen.github.io/product-images/TW-Nancy-1-caramel/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC46931-1/1.jpg,https://oleks-netizen.github.io/product-images/LC46931-1/2.jpg,https://oleks-netizen.github.io/product-images/LC46931-1/8.jpg,https://oleks-netizen.github.io/product-images/LC46931-1/4.jpg,https://oleks-netizen.github.io/product-images/LC46931-1/5.jpg,https://oleks-netizen.github.io/product-images/LC46931-1/6.jpg,https://oleks-netizen.github.io/product-images/LC46931-1/7.jpg</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>TW-Walker-mokko</t>
+          <t>LC46931-2</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/TW-Walker-mokko/1.jpg,https://oleks-netizen.github.io/product-images/TW-Walker-mokko/2.jpg,https://oleks-netizen.github.io/product-images/TW-Walker-mokko/5.jpg,https://oleks-netizen.github.io/product-images/TW-Walker-mokko/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC46931-2/1.jpg,https://oleks-netizen.github.io/product-images/LC46931-2/2.jpg,https://oleks-netizen.github.io/product-images/LC46931-2/3.jpg,https://oleks-netizen.github.io/product-images/LC46931-2/4.jpg,https://oleks-netizen.github.io/product-images/LC46931-2/5.jpg,https://oleks-netizen.github.io/product-images/LC46931-2/6.jpg,https://oleks-netizen.github.io/product-images/LC46931-2/7.jpg,https://oleks-netizen.github.io/product-images/LC46931-2/8.jpg</t>
         </is>
       </c>
       <c r="C127" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Y1311 45</t>
+          <t>LC89008-H1</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/Y1311 45/1.jpg,https://oleks-netizen.github.io/product-images/Y1311 45/2.jpg,https://oleks-netizen.github.io/product-images/Y1311 45/5.jpg,https://oleks-netizen.github.io/product-images/Y1311 45/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/LC89008-H1/1.jpg,https://oleks-netizen.github.io/product-images/LC89008-H1/2.jpg,https://oleks-netizen.github.io/product-images/LC89008-H1/7.jpg,https://oleks-netizen.github.io/product-images/LC89008-H1/4.jpg,https://oleks-netizen.github.io/product-images/LC89008-H1/5.jpg,https://oleks-netizen.github.io/product-images/LC89008-H1/6.jpg</t>
         </is>
       </c>
       <c r="C128" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>lim-354RAw</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/lim-354RAw/1.jpg,https://oleks-netizen.github.io/product-images/lim-354RAw/2.jpg,https://oleks-netizen.github.io/product-images/lim-354RAw/5.jpg,https://oleks-netizen.github.io/product-images/lim-354RAw/6.jpg,https://oleks-netizen.github.io/product-images/lim-354RAw/4.jpg</t>
+        </is>
+      </c>
+      <c r="C129" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>NB040A</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/NB040A/1.jpg,https://oleks-netizen.github.io/product-images/NB040A/2.jpg,https://oleks-netizen.github.io/product-images/NB040A/6.jpg,https://oleks-netizen.github.io/product-images/NB040A/4.jpg,https://oleks-netizen.github.io/product-images/NB040A/5.jpg</t>
+        </is>
+      </c>
+      <c r="C130" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>NB040B</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/NB040B/1.jpg,https://oleks-netizen.github.io/product-images/NB040B/2.jpg,https://oleks-netizen.github.io/product-images/NB040B/6.jpg,https://oleks-netizen.github.io/product-images/NB040B/3.jpg,https://oleks-netizen.github.io/product-images/NB040B/5.jpg</t>
+        </is>
+      </c>
+      <c r="C131" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>NB040C</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/NB040C/1.jpg,https://oleks-netizen.github.io/product-images/NB040C/2.jpg,https://oleks-netizen.github.io/product-images/NB040C/3.jpg,https://oleks-netizen.github.io/product-images/NB040C/6.jpg,https://oleks-netizen.github.io/product-images/NB040C/5.jpg</t>
+        </is>
+      </c>
+      <c r="C132" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>Nevada537moro</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/Nevada537moro/1.jpg,https://oleks-netizen.github.io/product-images/Nevada537moro/2.jpg,https://oleks-netizen.github.io/product-images/Nevada537moro/3.jpg,https://oleks-netizen.github.io/product-images/Nevada537moro/4.jpg</t>
+        </is>
+      </c>
+      <c r="C133" t="n">
         <v>4</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>NewRainbow1192nero</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/NewRainbow1192nero/1.jpg,https://oleks-netizen.github.io/product-images/NewRainbow1192nero/2.jpg,https://oleks-netizen.github.io/product-images/NewRainbow1192nero/7.jpg,https://oleks-netizen.github.io/product-images/NewRainbow1192nero/3.jpg,https://oleks-netizen.github.io/product-images/NewRainbow1192nero/4.jpg,https://oleks-netizen.github.io/product-images/NewRainbow1192nero/5.jpg</t>
+        </is>
+      </c>
+      <c r="C134" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>NewRainbow3435grigio</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/NewRainbow3435grigio/1.jpg,https://oleks-netizen.github.io/product-images/NewRainbow3435grigio/2.jpg,https://oleks-netizen.github.io/product-images/NewRainbow3435grigio/3.jpg,https://oleks-netizen.github.io/product-images/NewRainbow3435grigio/4.jpg,https://oleks-netizen.github.io/product-images/NewRainbow3435grigio/5.jpg,https://oleks-netizen.github.io/product-images/NewRainbow3435grigio/6.jpg</t>
+        </is>
+      </c>
+      <c r="C135" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>RA-0705-3mdL</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/RA-0705-3mdL/1.jpg,https://oleks-netizen.github.io/product-images/RA-0705-3mdL/2.jpg,https://oleks-netizen.github.io/product-images/RA-0705-3mdL/8.jpg,https://oleks-netizen.github.io/product-images/RA-0705-3mdL/4.jpg,https://oleks-netizen.github.io/product-images/RA-0705-3mdL/5.jpg,https://oleks-netizen.github.io/product-images/RA-0705-3mdL/6.jpg,https://oleks-netizen.github.io/product-images/RA-0705-3mdL/7.jpg</t>
+        </is>
+      </c>
+      <c r="C136" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>RA-5729-4sa</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/RA-5729-4sa/1.jpg,https://oleks-netizen.github.io/product-images/RA-5729-4sa/2.jpg,https://oleks-netizen.github.io/product-images/RA-5729-4sa/8.jpg,https://oleks-netizen.github.io/product-images/RA-5729-4sa/4.jpg,https://oleks-netizen.github.io/product-images/RA-5729-4sa/5.jpg,https://oleks-netizen.github.io/product-images/RA-5729-4sa/6.jpg,https://oleks-netizen.github.io/product-images/RA-5729-4sa/7.jpg</t>
+        </is>
+      </c>
+      <c r="C137" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>RB-1304-4lx</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/RB-1304-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RB-1304-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RB-1304-4lx/6.jpg,https://oleks-netizen.github.io/product-images/RB-1304-4lx/7.jpg,https://oleks-netizen.github.io/product-images/RB-1304-4lx/3.jpg,https://oleks-netizen.github.io/product-images/RB-1304-4lx/5.jpg</t>
+        </is>
+      </c>
+      <c r="C138" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>RC-1304-4lx</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/RC-1304-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RC-1304-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RC-1304-4lx/7.jpg,https://oleks-netizen.github.io/product-images/RC-1304-4lx/3.jpg,https://oleks-netizen.github.io/product-images/RC-1304-4lx/4.jpg,https://oleks-netizen.github.io/product-images/RC-1304-4lx/5.jpg</t>
+        </is>
+      </c>
+      <c r="C139" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>RC-1502-3md</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/RC-1502-3md/1.jpg,https://oleks-netizen.github.io/product-images/RC-1502-3md/2.jpg,https://oleks-netizen.github.io/product-images/RC-1502-3md/8.jpg,https://oleks-netizen.github.io/product-images/RC-1502-3md/4.jpg,https://oleks-netizen.github.io/product-images/RC-1502-3md/5.jpg,https://oleks-netizen.github.io/product-images/RC-1502-3md/6.jpg,https://oleks-netizen.github.io/product-images/RC-1502-3md/7.jpg</t>
+        </is>
+      </c>
+      <c r="C140" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>RC-1504-3md</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/RC-1504-3md/1.jpg,https://oleks-netizen.github.io/product-images/RC-1504-3md/3.jpg,https://oleks-netizen.github.io/product-images/RC-1504-3md/9.jpg,https://oleks-netizen.github.io/product-images/RC-1504-3md/4.jpg,https://oleks-netizen.github.io/product-images/RC-1504-3md/5.jpg,https://oleks-netizen.github.io/product-images/RC-1504-3md/6.jpg,https://oleks-netizen.github.io/product-images/RC-1504-3md/7.jpg,https://oleks-netizen.github.io/product-images/RC-1504-3md/8.jpg</t>
+        </is>
+      </c>
+      <c r="C141" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>RCs-7273-3md</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/RCs-7273-3md/1.jpg,https://oleks-netizen.github.io/product-images/RCs-7273-3md/2.jpg,https://oleks-netizen.github.io/product-images/RCs-7273-3md/3.jpg,https://oleks-netizen.github.io/product-images/RCs-7273-3md/9.jpg,https://oleks-netizen.github.io/product-images/RCs-7273-3md/4.jpg,https://oleks-netizen.github.io/product-images/RCs-7273-3md/5.jpg,https://oleks-netizen.github.io/product-images/RCs-7273-3md/6.jpg,https://oleks-netizen.github.io/product-images/RCs-7273-3md/8.jpg</t>
+        </is>
+      </c>
+      <c r="C142" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>RSw-6601-3md</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/RSw-6601-3md/1.jpg,https://oleks-netizen.github.io/product-images/RSw-6601-3md/2.jpg,https://oleks-netizen.github.io/product-images/RSw-6601-3md/7.jpg,https://oleks-netizen.github.io/product-images/RSw-6601-3md/3.jpg,https://oleks-netizen.github.io/product-images/RSw-6601-3md/4.jpg,https://oleks-netizen.github.io/product-images/RSw-6601-3md/6.jpg</t>
+        </is>
+      </c>
+      <c r="C143" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>RY-3450-4lx</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/RY-3450-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RY-3450-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RY-3450-4lx/8.jpg,https://oleks-netizen.github.io/product-images/RY-3450-4lx/4.jpg,https://oleks-netizen.github.io/product-images/RY-3450-4lx/5.jpg,https://oleks-netizen.github.io/product-images/RY-3450-4lx/6.jpg,https://oleks-netizen.github.io/product-images/RY-3450-4lx/7.jpg</t>
+        </is>
+      </c>
+      <c r="C144" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>RY-3451-4lx</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/RY-3451-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RY-3451-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RY-3451-4lx/3.jpg,https://oleks-netizen.github.io/product-images/RY-3451-4lx/9.jpg,https://oleks-netizen.github.io/product-images/RY-3451-4lx/4.jpg,https://oleks-netizen.github.io/product-images/RY-3451-4lx/5.jpg,https://oleks-netizen.github.io/product-images/RY-3451-4lx/6.jpg,https://oleks-netizen.github.io/product-images/RY-3451-4lx/7.jpg</t>
+        </is>
+      </c>
+      <c r="C145" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>RyE-4007-3md</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/RyE-4007-3md/1.jpg,https://oleks-netizen.github.io/product-images/RyE-4007-3md/2.jpg,https://oleks-netizen.github.io/product-images/RyE-4007-3md/7.jpg,https://oleks-netizen.github.io/product-images/RyE-4007-3md/3.jpg,https://oleks-netizen.github.io/product-images/RyE-4007-3md/4.jpg,https://oleks-netizen.github.io/product-images/RyE-4007-3md/5.jpg</t>
+        </is>
+      </c>
+      <c r="C146" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>RК-3990-3md</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/RК-3990-3md/1.jpg,https://oleks-netizen.github.io/product-images/RК-3990-3md/2.jpg,https://oleks-netizen.github.io/product-images/RК-3990-3md/4.jpg,https://oleks-netizen.github.io/product-images/RК-3990-3md/10.jpg,https://oleks-netizen.github.io/product-images/RК-3990-3md/5.jpg,https://oleks-netizen.github.io/product-images/RК-3990-3md/6.jpg,https://oleks-netizen.github.io/product-images/RК-3990-3md/7.jpg,https://oleks-netizen.github.io/product-images/RК-3990-3md/8.jpg,https://oleks-netizen.github.io/product-images/RК-3990-3md/9.jpg</t>
+        </is>
+      </c>
+      <c r="C147" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Swarovski1655Anero</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/Swarovski1655Anero/1.jpg,https://oleks-netizen.github.io/product-images/Swarovski1655Anero/2.jpg,https://oleks-netizen.github.io/product-images/Swarovski1655Anero/3.jpg,https://oleks-netizen.github.io/product-images/Swarovski1655Anero/4.jpg,https://oleks-netizen.github.io/product-images/Swarovski1655Anero/5.jpg</t>
+        </is>
+      </c>
+      <c r="C148" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>T0158A</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/T0158A/1.jpg,https://oleks-netizen.github.io/product-images/T0158A/2.jpg</t>
+        </is>
+      </c>
+      <c r="C149" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>TB019A</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TB019A/1.jpg,https://oleks-netizen.github.io/product-images/TB019A/2.jpg,https://oleks-netizen.github.io/product-images/TB019A/3.jpg,https://oleks-netizen.github.io/product-images/TB019A/4.jpg,https://oleks-netizen.github.io/product-images/TB019A/5.jpg,https://oleks-netizen.github.io/product-images/TB019A/6.jpg</t>
+        </is>
+      </c>
+      <c r="C150" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>TB019B</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TB019B/1.jpg,https://oleks-netizen.github.io/product-images/TB019B/7.jpg,https://oleks-netizen.github.io/product-images/TB019B/3.jpg,https://oleks-netizen.github.io/product-images/TB019B/4.jpg,https://oleks-netizen.github.io/product-images/TB019B/5.jpg,https://oleks-netizen.github.io/product-images/TB019B/6.jpg</t>
+        </is>
+      </c>
+      <c r="C151" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>TB019C</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TB019C/1.jpg,https://oleks-netizen.github.io/product-images/TB019C/2.jpg,https://oleks-netizen.github.io/product-images/TB019C/5.jpg,https://oleks-netizen.github.io/product-images/TB019C/8.jpg,https://oleks-netizen.github.io/product-images/TB019C/3.jpg,https://oleks-netizen.github.io/product-images/TB019C/4.jpg,https://oleks-netizen.github.io/product-images/TB019C/6.jpg</t>
+        </is>
+      </c>
+      <c r="C152" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>TB019J</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TB019J/1.jpg,https://oleks-netizen.github.io/product-images/TB019J/7.jpg,https://oleks-netizen.github.io/product-images/TB019J/3.jpg,https://oleks-netizen.github.io/product-images/TB019J/4.jpg,https://oleks-netizen.github.io/product-images/TB019J/5.jpg,https://oleks-netizen.github.io/product-images/TB019J/6.jpg</t>
+        </is>
+      </c>
+      <c r="C153" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>TB1063A</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TB1063A/1.jpg,https://oleks-netizen.github.io/product-images/TB1063A/2.jpg,https://oleks-netizen.github.io/product-images/TB1063A/3.jpg,https://oleks-netizen.github.io/product-images/TB1063A/4.jpg,https://oleks-netizen.github.io/product-images/TB1063A/5.jpg</t>
+        </is>
+      </c>
+      <c r="C154" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>TB1063C</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TB1063C/1.jpg,https://oleks-netizen.github.io/product-images/TB1063C/2.jpg,https://oleks-netizen.github.io/product-images/TB1063C/3.jpg,https://oleks-netizen.github.io/product-images/TB1063C/4.jpg,https://oleks-netizen.github.io/product-images/TB1063C/5.jpg</t>
+        </is>
+      </c>
+      <c r="C155" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>TB555A</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TB555A/1.jpg,https://oleks-netizen.github.io/product-images/TB555A/2.jpg,https://oleks-netizen.github.io/product-images/TB555A/3.jpg</t>
+        </is>
+      </c>
+      <c r="C156" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>TB555B</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TB555B/1.jpg,https://oleks-netizen.github.io/product-images/TB555B/2.jpg,https://oleks-netizen.github.io/product-images/TB555B/4.jpg</t>
+        </is>
+      </c>
+      <c r="C157" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>TB555C</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/TB555C/1.jpg,https://oleks-netizen.github.io/product-images/TB555C/2.jpg,https://oleks-netizen.github.io/product-images/TB555C/7.jpg,https://oleks-netizen.github.io/product-images/TB555C/3.jpg,https://oleks-netizen.github.io/product-images/TB555C/4.jpg,https://oleks-netizen.github.io/product-images/TB555C/5.jpg</t>
+        </is>
+      </c>
+      <c r="C158" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>VSL42 BLK ST BLUE</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/VSL42 BLK ST BLUE/1.jpg,https://oleks-netizen.github.io/product-images/VSL42 BLK ST BLUE/2.jpg,https://oleks-netizen.github.io/product-images/VSL42 BLK ST BLUE/8.jpg,https://oleks-netizen.github.io/product-images/VSL42 BLK ST BLUE/3.jpg,https://oleks-netizen.github.io/product-images/VSL42 BLK ST BLUE/4.jpg,https://oleks-netizen.github.io/product-images/VSL42 BLK ST BLUE/6.jpg,https://oleks-netizen.github.io/product-images/VSL42 BLK ST BLUE/7.jpg</t>
+        </is>
+      </c>
+      <c r="C159" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>VSL42 OIL TAN</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/VSL42 OIL TAN/1.jpg,https://oleks-netizen.github.io/product-images/VSL42 OIL TAN/2.jpg,https://oleks-netizen.github.io/product-images/VSL42 OIL TAN/8.jpg,https://oleks-netizen.github.io/product-images/VSL42 OIL TAN/3.jpg,https://oleks-netizen.github.io/product-images/VSL42 OIL TAN/4.jpg,https://oleks-netizen.github.io/product-images/VSL42 OIL TAN/6.jpg,https://oleks-netizen.github.io/product-images/VSL42 OIL TAN/7.jpg</t>
+        </is>
+      </c>
+      <c r="C160" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>Y60 BEIGE</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/Y60 BEIGE/1.jpg,https://oleks-netizen.github.io/product-images/Y60 BEIGE/2.jpg,https://oleks-netizen.github.io/product-images/Y60 BEIGE/3.jpg</t>
+        </is>
+      </c>
+      <c r="C161" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>Y60 BLK</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/Y60 BLK/1.jpg,https://oleks-netizen.github.io/product-images/Y60 BLK/2.jpg,https://oleks-netizen.github.io/product-images/Y60 BLK/3.jpg,https://oleks-netizen.github.io/product-images/Y60 BLK/4.jpg</t>
+        </is>
+      </c>
+      <c r="C162" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>ZА-3990-3md</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/ZА-3990-3md/1.jpg,https://oleks-netizen.github.io/product-images/ZА-3990-3md/2.jpg,https://oleks-netizen.github.io/product-images/ZА-3990-3md/4.jpg,https://oleks-netizen.github.io/product-images/ZА-3990-3md/10.jpg,https://oleks-netizen.github.io/product-images/ZА-3990-3md/3.jpg,https://oleks-netizen.github.io/product-images/ZА-3990-3md/6.jpg,https://oleks-netizen.github.io/product-images/ZА-3990-3md/7.jpg,https://oleks-netizen.github.io/product-images/ZА-3990-3md/8.jpg,https://oleks-netizen.github.io/product-images/ZА-3990-3md/9.jpg</t>
+        </is>
+      </c>
+      <c r="C163" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update 2026-02-28 16:53:56
</commit_message>
<xml_diff>
--- a/articles_summary.xlsx
+++ b/articles_summary.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C163"/>
+  <dimension ref="A1:C267"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,87 +441,87 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>11711719</t>
+          <t>00237</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/11711719/1.jpg,https://oleks-netizen.github.io/product-images/11711719/2.jpg,https://oleks-netizen.github.io/product-images/11711719/3.jpg,https://oleks-netizen.github.io/product-images/11711719/11.jpg,https://oleks-netizen.github.io/product-images/11711719/10.jpg,https://oleks-netizen.github.io/product-images/11711719/4.jpg,https://oleks-netizen.github.io/product-images/11711719/5.jpg,https://oleks-netizen.github.io/product-images/11711719/6.jpg,https://oleks-netizen.github.io/product-images/11711719/8.jpg,https://oleks-netizen.github.io/product-images/11711719/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/00237/1.jpg,https://oleks-netizen.github.io/product-images/00237/2.jpg,https://oleks-netizen.github.io/product-images/00237/3.jpg,https://oleks-netizen.github.io/product-images/00237/4.jpg,https://oleks-netizen.github.io/product-images/00237/5.jpg,https://oleks-netizen.github.io/product-images/00237/6.jpg,https://oleks-netizen.github.io/product-images/00237/7.jpg,https://oleks-netizen.github.io/product-images/00237/8.jpg,https://oleks-netizen.github.io/product-images/00237/9.jpg</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>11711719m</t>
+          <t>100v1genw91-white</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/11711719m/1.jpg,https://oleks-netizen.github.io/product-images/11711719m/2.jpg,https://oleks-netizen.github.io/product-images/11711719m/9.jpg,https://oleks-netizen.github.io/product-images/11711719m/3.jpg,https://oleks-netizen.github.io/product-images/11711719m/4.jpg,https://oleks-netizen.github.io/product-images/11711719m/5.jpg,https://oleks-netizen.github.io/product-images/11711719m/7.jpg,https://oleks-netizen.github.io/product-images/11711719m/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/100v1genw91-white/1.jpg,https://oleks-netizen.github.io/product-images/100v1genw91-white/2.jpg</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>11nero</t>
+          <t>11051</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/11nero/1.jpg,https://oleks-netizen.github.io/product-images/11nero/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/11051/1.jpg,https://oleks-netizen.github.io/product-images/11051/2.jpg,https://oleks-netizen.github.io/product-images/11051/12.jpg,https://oleks-netizen.github.io/product-images/11051/10.jpg,https://oleks-netizen.github.io/product-images/11051/11.jpg,https://oleks-netizen.github.io/product-images/11051/3.jpg,https://oleks-netizen.github.io/product-images/11051/5.jpg,https://oleks-netizen.github.io/product-images/11051/6.jpg,https://oleks-netizen.github.io/product-images/11051/7.jpg,https://oleks-netizen.github.io/product-images/11051/8.jpg,https://oleks-netizen.github.io/product-images/11051/9.jpg</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1352_1_2</t>
+          <t>110v1genw14</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/1352_1_2/1.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/110v1genw14/1.jpg,https://oleks-netizen.github.io/product-images/110v1genw14/2.jpg,https://oleks-netizen.github.io/product-images/110v1genw14/3.jpg</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1531_1_4</t>
+          <t>110v1genw64-black</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/1531_1_4/1.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/110v1genw64-black/1.jpg,https://oleks-netizen.github.io/product-images/110v1genw64-black/2.jpg</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1602060006</t>
+          <t>115v1fx90-black</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/1602060006/1.jpg,https://oleks-netizen.github.io/product-images/1602060006/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/115v1fx90-black/1.jpg,https://oleks-netizen.github.io/product-images/115v1fx90-black/2.jpg</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -531,27 +531,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>25000030m</t>
+          <t>115v1gen41</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/25000030m/1.jpg,https://oleks-netizen.github.io/product-images/25000030m/2.jpg,https://oleks-netizen.github.io/product-images/25000030m/16.jpg,https://oleks-netizen.github.io/product-images/25000030m/10.jpg,https://oleks-netizen.github.io/product-images/25000030m/11.jpg,https://oleks-netizen.github.io/product-images/25000030m/12.jpg,https://oleks-netizen.github.io/product-images/25000030m/13.jpg,https://oleks-netizen.github.io/product-images/25000030m/14.jpg,https://oleks-netizen.github.io/product-images/25000030m/15.jpg,https://oleks-netizen.github.io/product-images/25000030m/3.jpg,https://oleks-netizen.github.io/product-images/25000030m/4.jpg,https://oleks-netizen.github.io/product-images/25000030m/5.jpg,https://oleks-netizen.github.io/product-images/25000030m/6.jpg,https://oleks-netizen.github.io/product-images/25000030m/8.jpg,https://oleks-netizen.github.io/product-images/25000030m/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/115v1gen41/1.jpg,https://oleks-netizen.github.io/product-images/115v1gen41/2.jpg,https://oleks-netizen.github.io/product-images/115v1gen41/3.jpg</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>4041nero</t>
+          <t>115vfx82-black</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/4041nero/1.jpg,https://oleks-netizen.github.io/product-images/4041nero/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/115vfx82-black/1.jpg,https://oleks-netizen.github.io/product-images/115vfx82-black/2.jpg</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -561,1032 +561,1032 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>5196801</t>
+          <t>125v1genav9</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/5196801/1.jpg,https://oleks-netizen.github.io/product-images/5196801/2.jpg,https://oleks-netizen.github.io/product-images/5196801/7.jpg,https://oleks-netizen.github.io/product-images/5196801/11.jpg,https://oleks-netizen.github.io/product-images/5196801/10.jpg,https://oleks-netizen.github.io/product-images/5196801/4.jpg,https://oleks-netizen.github.io/product-images/5196801/5.jpg,https://oleks-netizen.github.io/product-images/5196801/6.jpg,https://oleks-netizen.github.io/product-images/5196801/8.jpg,https://oleks-netizen.github.io/product-images/5196801/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/125v1genav9/1.jpg,https://oleks-netizen.github.io/product-images/125v1genav9/2.jpg,https://oleks-netizen.github.io/product-images/125v1genav9/3.jpg,https://oleks-netizen.github.io/product-images/125v1genav9/4.jpg,https://oleks-netizen.github.io/product-images/125v1genav9/5.jpg</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>5228201</t>
+          <t>125vfx83-black</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/5228201/1.jpg,https://oleks-netizen.github.io/product-images/5228201/2.jpg,https://oleks-netizen.github.io/product-images/5228201/5.jpg,https://oleks-netizen.github.io/product-images/5228201/11.jpg,https://oleks-netizen.github.io/product-images/5228201/3.jpg,https://oleks-netizen.github.io/product-images/5228201/4.jpg,https://oleks-netizen.github.io/product-images/5228201/6.jpg,https://oleks-netizen.github.io/product-images/5228201/7.jpg,https://oleks-netizen.github.io/product-images/5228201/8.jpg,https://oleks-netizen.github.io/product-images/5228201/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/125vfx83-black/1.jpg,https://oleks-netizen.github.io/product-images/125vfx83-black/2.jpg</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>533670</t>
+          <t>13914</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/533670/1.jpg,https://oleks-netizen.github.io/product-images/533670/2.jpg,https://oleks-netizen.github.io/product-images/533670/7.jpg,https://oleks-netizen.github.io/product-images/533670/8.jpg,https://oleks-netizen.github.io/product-images/533670/3.jpg,https://oleks-netizen.github.io/product-images/533670/4.jpg,https://oleks-netizen.github.io/product-images/533670/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/13914/1.jpg,https://oleks-netizen.github.io/product-images/13914/2.jpg,https://oleks-netizen.github.io/product-images/13914/7.jpg,https://oleks-netizen.github.io/product-images/13914/3.jpg,https://oleks-netizen.github.io/product-images/13914/4.jpg,https://oleks-netizen.github.io/product-images/13914/6.jpg</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>538610</t>
+          <t>13928</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/538610/1.jpg,https://oleks-netizen.github.io/product-images/538610/2.jpg,https://oleks-netizen.github.io/product-images/538610/8.jpg,https://oleks-netizen.github.io/product-images/538610/3.jpg,https://oleks-netizen.github.io/product-images/538610/4.jpg,https://oleks-netizen.github.io/product-images/538610/6.jpg,https://oleks-netizen.github.io/product-images/538610/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/13928/1.jpg,https://oleks-netizen.github.io/product-images/13928/2.jpg,https://oleks-netizen.github.io/product-images/13928/6.jpg,https://oleks-netizen.github.io/product-images/13928/4.jpg,https://oleks-netizen.github.io/product-images/13928/5.jpg</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>77266501</t>
+          <t>13929</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/77266501/1.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/13929/1.jpg,https://oleks-netizen.github.io/product-images/13929/2.jpg,https://oleks-netizen.github.io/product-images/13929/6.jpg,https://oleks-netizen.github.io/product-images/13929/4.jpg,https://oleks-netizen.github.io/product-images/13929/5.jpg</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>80460064m</t>
+          <t>13960</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/80460064m/1.jpg,https://oleks-netizen.github.io/product-images/80460064m/2.jpg,https://oleks-netizen.github.io/product-images/80460064m/8.jpg,https://oleks-netizen.github.io/product-images/80460064m/15.jpg,https://oleks-netizen.github.io/product-images/80460064m/10.jpg,https://oleks-netizen.github.io/product-images/80460064m/11.jpg,https://oleks-netizen.github.io/product-images/80460064m/12.jpg,https://oleks-netizen.github.io/product-images/80460064m/13.jpg,https://oleks-netizen.github.io/product-images/80460064m/14.jpg,https://oleks-netizen.github.io/product-images/80460064m/3.jpg,https://oleks-netizen.github.io/product-images/80460064m/4.jpg,https://oleks-netizen.github.io/product-images/80460064m/5.jpg,https://oleks-netizen.github.io/product-images/80460064m/7.jpg,https://oleks-netizen.github.io/product-images/80460064m/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/13960/1.jpg,https://oleks-netizen.github.io/product-images/13960/2.jpg,https://oleks-netizen.github.io/product-images/13960/7.jpg,https://oleks-netizen.github.io/product-images/13960/3.jpg,https://oleks-netizen.github.io/product-images/13960/4.jpg,https://oleks-netizen.github.io/product-images/13960/5.jpg</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>80460101m</t>
+          <t>14050</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/80460101m/1.jpg,https://oleks-netizen.github.io/product-images/80460101m/2.jpg,https://oleks-netizen.github.io/product-images/80460101m/8.jpg,https://oleks-netizen.github.io/product-images/80460101m/17.jpg,https://oleks-netizen.github.io/product-images/80460101m/10.jpg,https://oleks-netizen.github.io/product-images/80460101m/11.jpg,https://oleks-netizen.github.io/product-images/80460101m/12.jpg,https://oleks-netizen.github.io/product-images/80460101m/13.jpg,https://oleks-netizen.github.io/product-images/80460101m/14.jpg,https://oleks-netizen.github.io/product-images/80460101m/15.jpg,https://oleks-netizen.github.io/product-images/80460101m/16.jpg,https://oleks-netizen.github.io/product-images/80460101m/3.jpg,https://oleks-netizen.github.io/product-images/80460101m/4.jpg,https://oleks-netizen.github.io/product-images/80460101m/5.jpg,https://oleks-netizen.github.io/product-images/80460101m/7.jpg,https://oleks-netizen.github.io/product-images/80460101m/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14050/1.jpg,https://oleks-netizen.github.io/product-images/14050/2.jpg,https://oleks-netizen.github.io/product-images/14050/6.jpg,https://oleks-netizen.github.io/product-images/14050/9.jpg,https://oleks-netizen.github.io/product-images/14050/3.jpg,https://oleks-netizen.github.io/product-images/14050/4.jpg,https://oleks-netizen.github.io/product-images/14050/5.jpg,https://oleks-netizen.github.io/product-images/14050/7.jpg</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>90421065m</t>
+          <t>14051</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/90421065m/1.jpg,https://oleks-netizen.github.io/product-images/90421065m/2.jpg,https://oleks-netizen.github.io/product-images/90421065m/15.jpg,https://oleks-netizen.github.io/product-images/90421065m/10.jpg,https://oleks-netizen.github.io/product-images/90421065m/11.jpg,https://oleks-netizen.github.io/product-images/90421065m/12.jpg,https://oleks-netizen.github.io/product-images/90421065m/13.jpg,https://oleks-netizen.github.io/product-images/90421065m/14.jpg,https://oleks-netizen.github.io/product-images/90421065m/3.jpg,https://oleks-netizen.github.io/product-images/90421065m/4.jpg,https://oleks-netizen.github.io/product-images/90421065m/6.jpg,https://oleks-netizen.github.io/product-images/90421065m/7.jpg,https://oleks-netizen.github.io/product-images/90421065m/8.jpg,https://oleks-netizen.github.io/product-images/90421065m/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14051/1.jpg,https://oleks-netizen.github.io/product-images/14051/2.jpg,https://oleks-netizen.github.io/product-images/14051/10.jpg,https://oleks-netizen.github.io/product-images/14051/3.jpg,https://oleks-netizen.github.io/product-images/14051/4.jpg,https://oleks-netizen.github.io/product-images/14051/5.jpg,https://oleks-netizen.github.io/product-images/14051/6.jpg,https://oleks-netizen.github.io/product-images/14051/7.jpg,https://oleks-netizen.github.io/product-images/14051/8.jpg</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Accademia1139nero</t>
+          <t>14052</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/Accademia1139nero/1.jpg,https://oleks-netizen.github.io/product-images/Accademia1139nero/2.jpg,https://oleks-netizen.github.io/product-images/Accademia1139nero/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14052/1.jpg,https://oleks-netizen.github.io/product-images/14052/2.jpg,https://oleks-netizen.github.io/product-images/14052/11.jpg,https://oleks-netizen.github.io/product-images/14052/3.jpg,https://oleks-netizen.github.io/product-images/14052/4.jpg,https://oleks-netizen.github.io/product-images/14052/5.jpg,https://oleks-netizen.github.io/product-images/14052/6.jpg,https://oleks-netizen.github.io/product-images/14052/7.jpg,https://oleks-netizen.github.io/product-images/14052/8.jpg,https://oleks-netizen.github.io/product-images/14052/9.jpg</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>ButC-1404-4lx</t>
+          <t>14053</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/ButC-1404-4lx/1.jpg,https://oleks-netizen.github.io/product-images/ButC-1404-4lx/2.jpg,https://oleks-netizen.github.io/product-images/ButC-1404-4lx/7.jpg,https://oleks-netizen.github.io/product-images/ButC-1404-4lx/4.jpg,https://oleks-netizen.github.io/product-images/ButC-1404-4lx/5.jpg,https://oleks-netizen.github.io/product-images/ButC-1404-4lx/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14053/1.jpg,https://oleks-netizen.github.io/product-images/14053/2.jpg,https://oleks-netizen.github.io/product-images/14053/5.jpg,https://oleks-netizen.github.io/product-images/14053/8.jpg,https://oleks-netizen.github.io/product-images/14053/3.jpg,https://oleks-netizen.github.io/product-images/14053/4.jpg,https://oleks-netizen.github.io/product-images/14053/6.jpg</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>BV38416-153</t>
+          <t>14055</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BV38416-153/1.jpg,https://oleks-netizen.github.io/product-images/BV38416-153/2.jpg,https://oleks-netizen.github.io/product-images/BV38416-153/3.jpg,https://oleks-netizen.github.io/product-images/BV38416-153/8.jpg,https://oleks-netizen.github.io/product-images/BV38416-153/5.jpg,https://oleks-netizen.github.io/product-images/BV38416-153/6.jpg,https://oleks-netizen.github.io/product-images/BV38416-153/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14055/1.jpg,https://oleks-netizen.github.io/product-images/14055/2.jpg,https://oleks-netizen.github.io/product-images/14055/5.jpg,https://oleks-netizen.github.io/product-images/14055/11.jpg,https://oleks-netizen.github.io/product-images/14055/10.jpg,https://oleks-netizen.github.io/product-images/14055/3.jpg,https://oleks-netizen.github.io/product-images/14055/4.jpg,https://oleks-netizen.github.io/product-images/14055/6.jpg,https://oleks-netizen.github.io/product-images/14055/7.jpg,https://oleks-netizen.github.io/product-images/14055/9.jpg</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>BV38601-1</t>
+          <t>14059</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BV38601-1/1.jpg,https://oleks-netizen.github.io/product-images/BV38601-1/2.jpg,https://oleks-netizen.github.io/product-images/BV38601-1/6.jpg,https://oleks-netizen.github.io/product-images/BV38601-1/4.jpg,https://oleks-netizen.github.io/product-images/BV38601-1/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14059/1.jpg,https://oleks-netizen.github.io/product-images/14059/2.jpg,https://oleks-netizen.github.io/product-images/14059/8.jpg,https://oleks-netizen.github.io/product-images/14059/3.jpg,https://oleks-netizen.github.io/product-images/14059/4.jpg,https://oleks-netizen.github.io/product-images/14059/5.jpg,https://oleks-netizen.github.io/product-images/14059/6.jpg</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>BV38753-1</t>
+          <t>14066</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/BV38753-1/1.jpg,https://oleks-netizen.github.io/product-images/BV38753-1/2.jpg,https://oleks-netizen.github.io/product-images/BV38753-1/8.jpg,https://oleks-netizen.github.io/product-images/BV38753-1/4.jpg,https://oleks-netizen.github.io/product-images/BV38753-1/5.jpg,https://oleks-netizen.github.io/product-images/BV38753-1/6.jpg,https://oleks-netizen.github.io/product-images/BV38753-1/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14066/1.jpg,https://oleks-netizen.github.io/product-images/14066/2.jpg,https://oleks-netizen.github.io/product-images/14066/14.jpg,https://oleks-netizen.github.io/product-images/14066/10.jpg,https://oleks-netizen.github.io/product-images/14066/11.jpg,https://oleks-netizen.github.io/product-images/14066/12.jpg,https://oleks-netizen.github.io/product-images/14066/13.jpg,https://oleks-netizen.github.io/product-images/14066/3.jpg,https://oleks-netizen.github.io/product-images/14066/4.jpg,https://oleks-netizen.github.io/product-images/14066/5.jpg,https://oleks-netizen.github.io/product-images/14066/6.jpg,https://oleks-netizen.github.io/product-images/14066/8.jpg,https://oleks-netizen.github.io/product-images/14066/9.jpg</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>C-3079A-black</t>
+          <t>14085</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/C-3079A-black/1.jpg,https://oleks-netizen.github.io/product-images/C-3079A-black/2.jpg,https://oleks-netizen.github.io/product-images/C-3079A-black/6.jpg,https://oleks-netizen.github.io/product-images/C-3079A-black/3.jpg,https://oleks-netizen.github.io/product-images/C-3079A-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14085/1.jpg,https://oleks-netizen.github.io/product-images/14085/2.jpg,https://oleks-netizen.github.io/product-images/14085/8.jpg,https://oleks-netizen.github.io/product-images/14085/16.jpg,https://oleks-netizen.github.io/product-images/14085/10.jpg,https://oleks-netizen.github.io/product-images/14085/11.jpg,https://oleks-netizen.github.io/product-images/14085/12.jpg,https://oleks-netizen.github.io/product-images/14085/13.jpg,https://oleks-netizen.github.io/product-images/14085/14.jpg,https://oleks-netizen.github.io/product-images/14085/3.jpg,https://oleks-netizen.github.io/product-images/14085/4.jpg,https://oleks-netizen.github.io/product-images/14085/5.jpg,https://oleks-netizen.github.io/product-images/14085/6.jpg,https://oleks-netizen.github.io/product-images/14085/7.jpg,https://oleks-netizen.github.io/product-images/14085/9.jpg</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Contatto9148nero</t>
+          <t>14088</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/Contatto9148nero/1.jpg,https://oleks-netizen.github.io/product-images/Contatto9148nero/2.jpg,https://oleks-netizen.github.io/product-images/Contatto9148nero/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14088/1.jpg,https://oleks-netizen.github.io/product-images/14088/2.jpg,https://oleks-netizen.github.io/product-images/14088/6.jpg,https://oleks-netizen.github.io/product-images/14088/19.jpg,https://oleks-netizen.github.io/product-images/14088/10.jpg,https://oleks-netizen.github.io/product-images/14088/11.jpg,https://oleks-netizen.github.io/product-images/14088/12.jpg,https://oleks-netizen.github.io/product-images/14088/13.jpg,https://oleks-netizen.github.io/product-images/14088/14.jpg,https://oleks-netizen.github.io/product-images/14088/15.jpg,https://oleks-netizen.github.io/product-images/14088/16.jpg,https://oleks-netizen.github.io/product-images/14088/17.jpg,https://oleks-netizen.github.io/product-images/14088/18.jpg,https://oleks-netizen.github.io/product-images/14088/3.jpg,https://oleks-netizen.github.io/product-images/14088/4.jpg,https://oleks-netizen.github.io/product-images/14088/5.jpg,https://oleks-netizen.github.io/product-images/14088/7.jpg,https://oleks-netizen.github.io/product-images/14088/9.jpg</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Cortina5051nero</t>
+          <t>14091</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/Cortina5051nero/1.jpg,https://oleks-netizen.github.io/product-images/Cortina5051nero/2.jpg,https://oleks-netizen.github.io/product-images/Cortina5051nero/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14091/1.jpg,https://oleks-netizen.github.io/product-images/14091/2.jpg,https://oleks-netizen.github.io/product-images/14091/19.jpg,https://oleks-netizen.github.io/product-images/14091/10.jpg,https://oleks-netizen.github.io/product-images/14091/11.jpg,https://oleks-netizen.github.io/product-images/14091/12.jpg,https://oleks-netizen.github.io/product-images/14091/13.jpg,https://oleks-netizen.github.io/product-images/14091/14.jpg,https://oleks-netizen.github.io/product-images/14091/15.jpg,https://oleks-netizen.github.io/product-images/14091/16.jpg,https://oleks-netizen.github.io/product-images/14091/17.jpg,https://oleks-netizen.github.io/product-images/14091/18.jpg,https://oleks-netizen.github.io/product-images/14091/3.jpg,https://oleks-netizen.github.io/product-images/14091/4.jpg,https://oleks-netizen.github.io/product-images/14091/5.jpg,https://oleks-netizen.github.io/product-images/14091/6.jpg,https://oleks-netizen.github.io/product-images/14091/7.jpg,https://oleks-netizen.github.io/product-images/14091/9.jpg</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Elit-1404-4lx</t>
+          <t>14114</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/Elit-1404-4lx/1.jpg,https://oleks-netizen.github.io/product-images/Elit-1404-4lx/2.jpg,https://oleks-netizen.github.io/product-images/Elit-1404-4lx/7.jpg,https://oleks-netizen.github.io/product-images/Elit-1404-4lx/4.jpg,https://oleks-netizen.github.io/product-images/Elit-1404-4lx/5.jpg,https://oleks-netizen.github.io/product-images/Elit-1404-4lx/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14114/1.jpg,https://oleks-netizen.github.io/product-images/14114/2.jpg,https://oleks-netizen.github.io/product-images/14114/6.jpg,https://oleks-netizen.github.io/product-images/14114/10.jpg,https://oleks-netizen.github.io/product-images/14114/4.jpg,https://oleks-netizen.github.io/product-images/14114/5.jpg,https://oleks-netizen.github.io/product-images/14114/7.jpg,https://oleks-netizen.github.io/product-images/14114/8.jpg,https://oleks-netizen.github.io/product-images/14114/9.jpg</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>FA-1819-3md</t>
+          <t>14135</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/FA-1819-3md/1.jpg,https://oleks-netizen.github.io/product-images/FA-1819-3md/2.jpg,https://oleks-netizen.github.io/product-images/FA-1819-3md/6.jpg,https://oleks-netizen.github.io/product-images/FA-1819-3md/4.jpg,https://oleks-netizen.github.io/product-images/FA-1819-3md/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14135/1.jpg,https://oleks-netizen.github.io/product-images/14135/2.jpg,https://oleks-netizen.github.io/product-images/14135/5.jpg,https://oleks-netizen.github.io/product-images/14135/12.jpg,https://oleks-netizen.github.io/product-images/14135/11.jpg,https://oleks-netizen.github.io/product-images/14135/3.jpg,https://oleks-netizen.github.io/product-images/14135/4.jpg,https://oleks-netizen.github.io/product-images/14135/6.jpg,https://oleks-netizen.github.io/product-images/14135/7.jpg,https://oleks-netizen.github.io/product-images/14135/8.jpg,https://oleks-netizen.github.io/product-images/14135/9.jpg</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>FA-8033-4lx</t>
+          <t>14155</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/FA-8033-4lx/1.jpg,https://oleks-netizen.github.io/product-images/FA-8033-4lx/2.jpg,https://oleks-netizen.github.io/product-images/FA-8033-4lx/6.jpg,https://oleks-netizen.github.io/product-images/FA-8033-4lx/4.jpg,https://oleks-netizen.github.io/product-images/FA-8033-4lx/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14155/1.jpg,https://oleks-netizen.github.io/product-images/14155/2.jpg,https://oleks-netizen.github.io/product-images/14155/9.jpg,https://oleks-netizen.github.io/product-images/14155/3.jpg,https://oleks-netizen.github.io/product-images/14155/4.jpg,https://oleks-netizen.github.io/product-images/14155/5.jpg,https://oleks-netizen.github.io/product-images/14155/7.jpg,https://oleks-netizen.github.io/product-images/14155/8.jpg</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>GA-1504-3md</t>
+          <t>14219</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/GA-1504-3md/1.jpg,https://oleks-netizen.github.io/product-images/GA-1504-3md/2.jpg,https://oleks-netizen.github.io/product-images/GA-1504-3md/5.jpg,https://oleks-netizen.github.io/product-images/GA-1504-3md/7.jpg,https://oleks-netizen.github.io/product-images/GA-1504-3md/4.jpg,https://oleks-netizen.github.io/product-images/GA-1504-3md/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14219/1.jpg,https://oleks-netizen.github.io/product-images/14219/2.jpg,https://oleks-netizen.github.io/product-images/14219/11.jpg,https://oleks-netizen.github.io/product-images/14219/10.jpg,https://oleks-netizen.github.io/product-images/14219/3.jpg,https://oleks-netizen.github.io/product-images/14219/4.jpg,https://oleks-netizen.github.io/product-images/14219/5.jpg,https://oleks-netizen.github.io/product-images/14219/7.jpg,https://oleks-netizen.github.io/product-images/14219/8.jpg,https://oleks-netizen.github.io/product-images/14219/9.jpg</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>GB-1302-3md</t>
+          <t>14223</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/GB-1302-3md/1.jpg,https://oleks-netizen.github.io/product-images/GB-1302-3md/2.jpg,https://oleks-netizen.github.io/product-images/GB-1302-3md/4.jpg,https://oleks-netizen.github.io/product-images/GB-1302-3md/7.jpg,https://oleks-netizen.github.io/product-images/GB-1302-3md/3.jpg,https://oleks-netizen.github.io/product-images/GB-1302-3md/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14223/1.jpg,https://oleks-netizen.github.io/product-images/14223/2.jpg,https://oleks-netizen.github.io/product-images/14223/5.jpg,https://oleks-netizen.github.io/product-images/14223/9.jpg,https://oleks-netizen.github.io/product-images/14223/3.jpg,https://oleks-netizen.github.io/product-images/14223/4.jpg,https://oleks-netizen.github.io/product-images/14223/6.jpg,https://oleks-netizen.github.io/product-images/14223/8.jpg</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>GC-1304-4lx</t>
+          <t>14224</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/GC-1304-4lx/1.jpg,https://oleks-netizen.github.io/product-images/GC-1304-4lx/2.jpg,https://oleks-netizen.github.io/product-images/GC-1304-4lx/5.jpg,https://oleks-netizen.github.io/product-images/GC-1304-4lx/7.jpg,https://oleks-netizen.github.io/product-images/GC-1304-4lx/4.jpg,https://oleks-netizen.github.io/product-images/GC-1304-4lx/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14224/1.jpg,https://oleks-netizen.github.io/product-images/14224/2.jpg,https://oleks-netizen.github.io/product-images/14224/5.jpg,https://oleks-netizen.github.io/product-images/14224/13.jpg,https://oleks-netizen.github.io/product-images/14224/10.jpg,https://oleks-netizen.github.io/product-images/14224/11.jpg,https://oleks-netizen.github.io/product-images/14224/12.jpg,https://oleks-netizen.github.io/product-images/14224/3.jpg,https://oleks-netizen.github.io/product-images/14224/4.jpg,https://oleks-netizen.github.io/product-images/14224/6.jpg,https://oleks-netizen.github.io/product-images/14224/7.jpg,https://oleks-netizen.github.io/product-images/14224/8.jpg</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>GE-3104-2lx</t>
+          <t>14225</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/GE-3104-2lx/1.jpg,https://oleks-netizen.github.io/product-images/GE-3104-2lx/2.jpg,https://oleks-netizen.github.io/product-images/GE-3104-2lx/3.jpg,https://oleks-netizen.github.io/product-images/GE-3104-2lx/6.jpg,https://oleks-netizen.github.io/product-images/GE-3104-2lx/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14225/1.jpg,https://oleks-netizen.github.io/product-images/14225/2.jpg,https://oleks-netizen.github.io/product-images/14225/3.jpg,https://oleks-netizen.github.io/product-images/14225/13.jpg,https://oleks-netizen.github.io/product-images/14225/11.jpg,https://oleks-netizen.github.io/product-images/14225/12.jpg,https://oleks-netizen.github.io/product-images/14225/4.jpg,https://oleks-netizen.github.io/product-images/14225/5.jpg,https://oleks-netizen.github.io/product-images/14225/6.jpg,https://oleks-netizen.github.io/product-images/14225/7.jpg,https://oleks-netizen.github.io/product-images/14225/8.jpg,https://oleks-netizen.github.io/product-images/14225/9.jpg</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>GX-8137-4lx</t>
+          <t>14227</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/GX-8137-4lx/1.jpg,https://oleks-netizen.github.io/product-images/GX-8137-4lx/2.jpg,https://oleks-netizen.github.io/product-images/GX-8137-4lx/9.jpg,https://oleks-netizen.github.io/product-images/GX-8137-4lx/3.jpg,https://oleks-netizen.github.io/product-images/GX-8137-4lx/4.jpg,https://oleks-netizen.github.io/product-images/GX-8137-4lx/5.jpg,https://oleks-netizen.github.io/product-images/GX-8137-4lx/7.jpg,https://oleks-netizen.github.io/product-images/GX-8137-4lx/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14227/1.jpg,https://oleks-netizen.github.io/product-images/14227/2.jpg,https://oleks-netizen.github.io/product-images/14227/5.jpg,https://oleks-netizen.github.io/product-images/14227/11.jpg,https://oleks-netizen.github.io/product-images/14227/10.jpg,https://oleks-netizen.github.io/product-images/14227/3.jpg,https://oleks-netizen.github.io/product-images/14227/4.jpg,https://oleks-netizen.github.io/product-images/14227/6.jpg,https://oleks-netizen.github.io/product-images/14227/7.jpg,https://oleks-netizen.github.io/product-images/14227/9.jpg</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>HB03334</t>
+          <t>14228</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/HB03334/1.jpg,https://oleks-netizen.github.io/product-images/HB03334/2.jpg,https://oleks-netizen.github.io/product-images/HB03334/3.jpg,https://oleks-netizen.github.io/product-images/HB03334/7.jpg,https://oleks-netizen.github.io/product-images/HB03334/4.jpg,https://oleks-netizen.github.io/product-images/HB03334/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14228/1.jpg,https://oleks-netizen.github.io/product-images/14228/2.jpg,https://oleks-netizen.github.io/product-images/14228/5.jpg,https://oleks-netizen.github.io/product-images/14228/8.jpg,https://oleks-netizen.github.io/product-images/14228/3.jpg,https://oleks-netizen.github.io/product-images/14228/4.jpg,https://oleks-netizen.github.io/product-images/14228/6.jpg</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Italico109nero</t>
+          <t>14230</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/Italico109nero/1.jpg,https://oleks-netizen.github.io/product-images/Italico109nero/4.jpg,https://oleks-netizen.github.io/product-images/Italico109nero/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14230/1.jpg,https://oleks-netizen.github.io/product-images/14230/2.jpg,https://oleks-netizen.github.io/product-images/14230/6.jpg,https://oleks-netizen.github.io/product-images/14230/11.jpg,https://oleks-netizen.github.io/product-images/14230/3.jpg,https://oleks-netizen.github.io/product-images/14230/4.jpg,https://oleks-netizen.github.io/product-images/14230/5.jpg,https://oleks-netizen.github.io/product-images/14230/7.jpg,https://oleks-netizen.github.io/product-images/14230/8.jpg,https://oleks-netizen.github.io/product-images/14230/9.jpg</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Italico1636cognac</t>
+          <t>14231</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/Italico1636cognac/1.jpg,https://oleks-netizen.github.io/product-images/Italico1636cognac/2.jpg,https://oleks-netizen.github.io/product-images/Italico1636cognac/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14231/1.jpg,https://oleks-netizen.github.io/product-images/14231/2.jpg,https://oleks-netizen.github.io/product-images/14231/11.jpg,https://oleks-netizen.github.io/product-images/14231/10.jpg,https://oleks-netizen.github.io/product-images/14231/3.jpg,https://oleks-netizen.github.io/product-images/14231/4.jpg,https://oleks-netizen.github.io/product-images/14231/5.jpg,https://oleks-netizen.github.io/product-images/14231/7.jpg,https://oleks-netizen.github.io/product-images/14231/8.jpg,https://oleks-netizen.github.io/product-images/14231/9.jpg</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Italico2367moro</t>
+          <t>14248</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/Italico2367moro/1.jpg,https://oleks-netizen.github.io/product-images/Italico2367moro/2.jpg,https://oleks-netizen.github.io/product-images/Italico2367moro/5.jpg,https://oleks-netizen.github.io/product-images/Italico2367moro/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14248/1.jpg,https://oleks-netizen.github.io/product-images/14248/2.jpg,https://oleks-netizen.github.io/product-images/14248/4.jpg,https://oleks-netizen.github.io/product-images/14248/12.jpg,https://oleks-netizen.github.io/product-images/14248/10.jpg,https://oleks-netizen.github.io/product-images/14248/11.jpg,https://oleks-netizen.github.io/product-images/14248/3.jpg,https://oleks-netizen.github.io/product-images/14248/5.jpg,https://oleks-netizen.github.io/product-images/14248/6.jpg,https://oleks-netizen.github.io/product-images/14248/7.jpg,https://oleks-netizen.github.io/product-images/14248/9.jpg</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Italico9188nero</t>
+          <t>14253</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/Italico9188nero/1.jpg,https://oleks-netizen.github.io/product-images/Italico9188nero/2.jpg,https://oleks-netizen.github.io/product-images/Italico9188nero/5.jpg,https://oleks-netizen.github.io/product-images/Italico9188nero/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14253/1.jpg,https://oleks-netizen.github.io/product-images/14253/2.jpg,https://oleks-netizen.github.io/product-images/14253/5.jpg,https://oleks-netizen.github.io/product-images/14253/15.jpg,https://oleks-netizen.github.io/product-images/14253/11.jpg,https://oleks-netizen.github.io/product-images/14253/12.jpg,https://oleks-netizen.github.io/product-images/14253/13.jpg,https://oleks-netizen.github.io/product-images/14253/14.jpg,https://oleks-netizen.github.io/product-images/14253/3.jpg,https://oleks-netizen.github.io/product-images/14253/4.jpg,https://oleks-netizen.github.io/product-images/14253/6.jpg,https://oleks-netizen.github.io/product-images/14253/7.jpg,https://oleks-netizen.github.io/product-images/14253/8.jpg,https://oleks-netizen.github.io/product-images/14253/9.jpg</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Italico9405nero</t>
+          <t>14254</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/Italico9405nero/1.jpg,https://oleks-netizen.github.io/product-images/Italico9405nero/2.jpg,https://oleks-netizen.github.io/product-images/Italico9405nero/5.jpg,https://oleks-netizen.github.io/product-images/Italico9405nero/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14254/1.jpg,https://oleks-netizen.github.io/product-images/14254/2.jpg,https://oleks-netizen.github.io/product-images/14254/14.jpg,https://oleks-netizen.github.io/product-images/14254/10.jpg,https://oleks-netizen.github.io/product-images/14254/11.jpg,https://oleks-netizen.github.io/product-images/14254/12.jpg,https://oleks-netizen.github.io/product-images/14254/13.jpg,https://oleks-netizen.github.io/product-images/14254/3.jpg,https://oleks-netizen.github.io/product-images/14254/4.jpg,https://oleks-netizen.github.io/product-images/14254/6.jpg,https://oleks-netizen.github.io/product-images/14254/7.jpg,https://oleks-netizen.github.io/product-images/14254/8.jpg,https://oleks-netizen.github.io/product-images/14254/9.jpg</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Italico954622moro</t>
+          <t>14346</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/Italico954622moro/1.jpg,https://oleks-netizen.github.io/product-images/Italico954622moro/2.jpg,https://oleks-netizen.github.io/product-images/Italico954622moro/5.jpg,https://oleks-netizen.github.io/product-images/Italico954622moro/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14346/1.jpg,https://oleks-netizen.github.io/product-images/14346/2.jpg,https://oleks-netizen.github.io/product-images/14346/3.jpg,https://oleks-netizen.github.io/product-images/14346/4.jpg,https://oleks-netizen.github.io/product-images/14346/5.jpg</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>JD1072A</t>
+          <t>14353</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/JD1072A/1.jpg,https://oleks-netizen.github.io/product-images/JD1072A/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14353/1.jpg,https://oleks-netizen.github.io/product-images/14353/2.jpg,https://oleks-netizen.github.io/product-images/14353/6.jpg,https://oleks-netizen.github.io/product-images/14353/14.jpg,https://oleks-netizen.github.io/product-images/14353/10.jpg,https://oleks-netizen.github.io/product-images/14353/11.jpg,https://oleks-netizen.github.io/product-images/14353/12.jpg,https://oleks-netizen.github.io/product-images/14353/13.jpg,https://oleks-netizen.github.io/product-images/14353/3.jpg,https://oleks-netizen.github.io/product-images/14353/4.jpg,https://oleks-netizen.github.io/product-images/14353/5.jpg,https://oleks-netizen.github.io/product-images/14353/8.jpg,https://oleks-netizen.github.io/product-images/14353/9.jpg</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>JD1072R</t>
+          <t>14365</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/JD1072R/1.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14365/1.jpg,https://oleks-netizen.github.io/product-images/14365/2.jpg,https://oleks-netizen.github.io/product-images/14365/6.jpg,https://oleks-netizen.github.io/product-images/14365/12.jpg,https://oleks-netizen.github.io/product-images/14365/11.jpg,https://oleks-netizen.github.io/product-images/14365/3.jpg,https://oleks-netizen.github.io/product-images/14365/4.jpg,https://oleks-netizen.github.io/product-images/14365/5.jpg,https://oleks-netizen.github.io/product-images/14365/7.jpg,https://oleks-netizen.github.io/product-images/14365/8.jpg,https://oleks-netizen.github.io/product-images/14365/9.jpg</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>JD1094A</t>
+          <t>14371</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/JD1094A/1.jpg,https://oleks-netizen.github.io/product-images/JD1094A/2.jpg,https://oleks-netizen.github.io/product-images/JD1094A/6.jpg,https://oleks-netizen.github.io/product-images/JD1094A/3.jpg,https://oleks-netizen.github.io/product-images/JD1094A/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14371/1.jpg,https://oleks-netizen.github.io/product-images/14371/2.jpg,https://oleks-netizen.github.io/product-images/14371/20.jpg,https://oleks-netizen.github.io/product-images/14371/10.jpg,https://oleks-netizen.github.io/product-images/14371/11.jpg,https://oleks-netizen.github.io/product-images/14371/12.jpg,https://oleks-netizen.github.io/product-images/14371/13.jpg,https://oleks-netizen.github.io/product-images/14371/14.jpg,https://oleks-netizen.github.io/product-images/14371/15.jpg,https://oleks-netizen.github.io/product-images/14371/16.jpg,https://oleks-netizen.github.io/product-images/14371/17.jpg,https://oleks-netizen.github.io/product-images/14371/18.jpg,https://oleks-netizen.github.io/product-images/14371/19.jpg,https://oleks-netizen.github.io/product-images/14371/3.jpg,https://oleks-netizen.github.io/product-images/14371/4.jpg,https://oleks-netizen.github.io/product-images/14371/5.jpg,https://oleks-netizen.github.io/product-images/14371/6.jpg,https://oleks-netizen.github.io/product-images/14371/7.jpg,https://oleks-netizen.github.io/product-images/14371/9.jpg</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>JD1097A</t>
+          <t>14376</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/JD1097A/1.jpg,https://oleks-netizen.github.io/product-images/JD1097A/2.jpg,https://oleks-netizen.github.io/product-images/JD1097A/5.jpg,https://oleks-netizen.github.io/product-images/JD1097A/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14376/1.jpg,https://oleks-netizen.github.io/product-images/14376/2.jpg,https://oleks-netizen.github.io/product-images/14376/4.jpg,https://oleks-netizen.github.io/product-images/14376/8.jpg,https://oleks-netizen.github.io/product-images/14376/3.jpg,https://oleks-netizen.github.io/product-images/14376/5.jpg,https://oleks-netizen.github.io/product-images/14376/7.jpg</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>JD1097C</t>
+          <t>14380</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/JD1097C/1.jpg,https://oleks-netizen.github.io/product-images/JD1097C/2.jpg,https://oleks-netizen.github.io/product-images/JD1097C/5.jpg,https://oleks-netizen.github.io/product-images/JD1097C/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14380/1.jpg,https://oleks-netizen.github.io/product-images/14380/2.jpg,https://oleks-netizen.github.io/product-images/14380/6.jpg,https://oleks-netizen.github.io/product-images/14380/10.jpg,https://oleks-netizen.github.io/product-images/14380/3.jpg,https://oleks-netizen.github.io/product-images/14380/4.jpg,https://oleks-netizen.github.io/product-images/14380/5.jpg,https://oleks-netizen.github.io/product-images/14380/7.jpg,https://oleks-netizen.github.io/product-images/14380/8.jpg</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>JD1105AL</t>
+          <t>14381</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/JD1105AL/1.jpg,https://oleks-netizen.github.io/product-images/JD1105AL/2.jpg,https://oleks-netizen.github.io/product-images/JD1105AL/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14381/1.jpg,https://oleks-netizen.github.io/product-images/14381/2.jpg,https://oleks-netizen.github.io/product-images/14381/9.jpg,https://oleks-netizen.github.io/product-images/14381/3.jpg,https://oleks-netizen.github.io/product-images/14381/4.jpg,https://oleks-netizen.github.io/product-images/14381/5.jpg,https://oleks-netizen.github.io/product-images/14381/6.jpg,https://oleks-netizen.github.io/product-images/14381/7.jpg</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>JD1105AS</t>
+          <t>14384</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/JD1105AS/1.jpg,https://oleks-netizen.github.io/product-images/JD1105AS/2.jpg,https://oleks-netizen.github.io/product-images/JD1105AS/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14384/1.jpg,https://oleks-netizen.github.io/product-images/14384/2.jpg,https://oleks-netizen.github.io/product-images/14384/7.jpg,https://oleks-netizen.github.io/product-images/14384/11.jpg,https://oleks-netizen.github.io/product-images/14384/3.jpg,https://oleks-netizen.github.io/product-images/14384/4.jpg,https://oleks-netizen.github.io/product-images/14384/5.jpg,https://oleks-netizen.github.io/product-images/14384/6.jpg,https://oleks-netizen.github.io/product-images/14384/8.jpg,https://oleks-netizen.github.io/product-images/14384/9.jpg</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>JD1107A</t>
+          <t>14397</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/JD1107A/1.jpg,https://oleks-netizen.github.io/product-images/JD1107A/2.jpg,https://oleks-netizen.github.io/product-images/JD1107A/5.jpg,https://oleks-netizen.github.io/product-images/JD1107A/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14397/1.jpg,https://oleks-netizen.github.io/product-images/14397/2.jpg,https://oleks-netizen.github.io/product-images/14397/12.jpg,https://oleks-netizen.github.io/product-images/14397/10.jpg,https://oleks-netizen.github.io/product-images/14397/11.jpg,https://oleks-netizen.github.io/product-images/14397/3.jpg,https://oleks-netizen.github.io/product-images/14397/4.jpg,https://oleks-netizen.github.io/product-images/14397/6.jpg,https://oleks-netizen.github.io/product-images/14397/7.jpg,https://oleks-netizen.github.io/product-images/14397/8.jpg,https://oleks-netizen.github.io/product-images/14397/9.jpg</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>JD1107C</t>
+          <t>14398</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/JD1107C/1.jpg,https://oleks-netizen.github.io/product-images/JD1107C/2.jpg,https://oleks-netizen.github.io/product-images/JD1107C/5.jpg,https://oleks-netizen.github.io/product-images/JD1107C/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14398/1.jpg,https://oleks-netizen.github.io/product-images/14398/2.jpg,https://oleks-netizen.github.io/product-images/14398/17.jpg,https://oleks-netizen.github.io/product-images/14398/10.jpg,https://oleks-netizen.github.io/product-images/14398/11.jpg,https://oleks-netizen.github.io/product-images/14398/12.jpg,https://oleks-netizen.github.io/product-images/14398/13.jpg,https://oleks-netizen.github.io/product-images/14398/15.jpg,https://oleks-netizen.github.io/product-images/14398/16.jpg,https://oleks-netizen.github.io/product-images/14398/3.jpg,https://oleks-netizen.github.io/product-images/14398/4.jpg,https://oleks-netizen.github.io/product-images/14398/5.jpg,https://oleks-netizen.github.io/product-images/14398/6.jpg,https://oleks-netizen.github.io/product-images/14398/7.jpg,https://oleks-netizen.github.io/product-images/14398/8.jpg,https://oleks-netizen.github.io/product-images/14398/9.jpg</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>JD4012Q</t>
+          <t>14404</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/JD4012Q/1.jpg,https://oleks-netizen.github.io/product-images/JD4012Q/2.jpg,https://oleks-netizen.github.io/product-images/JD4012Q/11.jpg,https://oleks-netizen.github.io/product-images/JD4012Q/10.jpg,https://oleks-netizen.github.io/product-images/JD4012Q/4.jpg,https://oleks-netizen.github.io/product-images/JD4012Q/5.jpg,https://oleks-netizen.github.io/product-images/JD4012Q/6.jpg,https://oleks-netizen.github.io/product-images/JD4012Q/7.jpg,https://oleks-netizen.github.io/product-images/JD4012Q/8.jpg,https://oleks-netizen.github.io/product-images/JD4012Q/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14404/1.jpg,https://oleks-netizen.github.io/product-images/14404/2.jpg,https://oleks-netizen.github.io/product-images/14404/14.jpg,https://oleks-netizen.github.io/product-images/14404/11.jpg,https://oleks-netizen.github.io/product-images/14404/12.jpg,https://oleks-netizen.github.io/product-images/14404/13.jpg,https://oleks-netizen.github.io/product-images/14404/3.jpg,https://oleks-netizen.github.io/product-images/14404/4.jpg,https://oleks-netizen.github.io/product-images/14404/5.jpg,https://oleks-netizen.github.io/product-images/14404/6.jpg,https://oleks-netizen.github.io/product-images/14404/7.jpg,https://oleks-netizen.github.io/product-images/14404/8.jpg,https://oleks-netizen.github.io/product-images/14404/9.jpg</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>JD7055R</t>
+          <t>14406</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/JD7055R/1.jpg,https://oleks-netizen.github.io/product-images/JD7055R/2.jpg,https://oleks-netizen.github.io/product-images/JD7055R/8.jpg,https://oleks-netizen.github.io/product-images/JD7055R/11.jpg,https://oleks-netizen.github.io/product-images/JD7055R/10.jpg,https://oleks-netizen.github.io/product-images/JD7055R/3.jpg,https://oleks-netizen.github.io/product-images/JD7055R/4.jpg,https://oleks-netizen.github.io/product-images/JD7055R/5.jpg,https://oleks-netizen.github.io/product-images/JD7055R/6.jpg,https://oleks-netizen.github.io/product-images/JD7055R/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14406/1.jpg,https://oleks-netizen.github.io/product-images/14406/2.jpg,https://oleks-netizen.github.io/product-images/14406/13.jpg,https://oleks-netizen.github.io/product-images/14406/11.jpg,https://oleks-netizen.github.io/product-images/14406/12.jpg,https://oleks-netizen.github.io/product-images/14406/3.jpg,https://oleks-netizen.github.io/product-images/14406/4.jpg,https://oleks-netizen.github.io/product-images/14406/5.jpg,https://oleks-netizen.github.io/product-images/14406/6.jpg,https://oleks-netizen.github.io/product-images/14406/7.jpg,https://oleks-netizen.github.io/product-images/14406/8.jpg,https://oleks-netizen.github.io/product-images/14406/9.jpg</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>K10018bl-black</t>
+          <t>14407</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K10018bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K10018bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K10018bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K10018bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K10018bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14407/1.jpg,https://oleks-netizen.github.io/product-images/14407/2.jpg,https://oleks-netizen.github.io/product-images/14407/12.jpg,https://oleks-netizen.github.io/product-images/14407/10.jpg,https://oleks-netizen.github.io/product-images/14407/11.jpg,https://oleks-netizen.github.io/product-images/14407/3.jpg,https://oleks-netizen.github.io/product-images/14407/4.jpg,https://oleks-netizen.github.io/product-images/14407/5.jpg,https://oleks-netizen.github.io/product-images/14407/6.jpg,https://oleks-netizen.github.io/product-images/14407/8.jpg,https://oleks-netizen.github.io/product-images/14407/9.jpg</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>K11318bl-black</t>
+          <t>14420</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K11318bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K11318bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K11318bl-black/3.jpg,https://oleks-netizen.github.io/product-images/K11318bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14420/1.jpg,https://oleks-netizen.github.io/product-images/14420/2.jpg,https://oleks-netizen.github.io/product-images/14420/13.jpg,https://oleks-netizen.github.io/product-images/14420/10.jpg,https://oleks-netizen.github.io/product-images/14420/11.jpg,https://oleks-netizen.github.io/product-images/14420/3.jpg,https://oleks-netizen.github.io/product-images/14420/4.jpg,https://oleks-netizen.github.io/product-images/14420/5.jpg,https://oleks-netizen.github.io/product-images/14420/6.jpg,https://oleks-netizen.github.io/product-images/14420/7.jpg,https://oleks-netizen.github.io/product-images/14420/8.jpg,https://oleks-netizen.github.io/product-images/14420/9.jpg</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>K11512be-beige</t>
+          <t>14422</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K11512be-beige/1.jpg,https://oleks-netizen.github.io/product-images/K11512be-beige/2.jpg,https://oleks-netizen.github.io/product-images/K11512be-beige/6.jpg,https://oleks-netizen.github.io/product-images/K11512be-beige/4.jpg,https://oleks-netizen.github.io/product-images/K11512be-beige/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14422/1.jpg,https://oleks-netizen.github.io/product-images/14422/2.jpg,https://oleks-netizen.github.io/product-images/14422/10.jpg,https://oleks-netizen.github.io/product-images/14422/3.jpg,https://oleks-netizen.github.io/product-images/14422/4.jpg,https://oleks-netizen.github.io/product-images/14422/5.jpg,https://oleks-netizen.github.io/product-images/14422/6.jpg,https://oleks-netizen.github.io/product-images/14422/7.jpg,https://oleks-netizen.github.io/product-images/14422/9.jpg</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>K11512bl-black</t>
+          <t>14429</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K11512bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K11512bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K11512bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K11512bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K11512bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14429/1.jpg,https://oleks-netizen.github.io/product-images/14429/2.jpg,https://oleks-netizen.github.io/product-images/14429/13.jpg,https://oleks-netizen.github.io/product-images/14429/10.jpg,https://oleks-netizen.github.io/product-images/14429/12.jpg,https://oleks-netizen.github.io/product-images/14429/3.jpg,https://oleks-netizen.github.io/product-images/14429/4.jpg,https://oleks-netizen.github.io/product-images/14429/5.jpg,https://oleks-netizen.github.io/product-images/14429/6.jpg,https://oleks-netizen.github.io/product-images/14429/7.jpg,https://oleks-netizen.github.io/product-images/14429/8.jpg,https://oleks-netizen.github.io/product-images/14429/9.jpg</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>K11512w-white</t>
+          <t>14436</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K11512w-white/1.jpg,https://oleks-netizen.github.io/product-images/K11512w-white/2.jpg,https://oleks-netizen.github.io/product-images/K11512w-white/6.jpg,https://oleks-netizen.github.io/product-images/K11512w-white/4.jpg,https://oleks-netizen.github.io/product-images/K11512w-white/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14436/1.jpg,https://oleks-netizen.github.io/product-images/14436/2.jpg,https://oleks-netizen.github.io/product-images/14436/11.jpg,https://oleks-netizen.github.io/product-images/14436/10.jpg,https://oleks-netizen.github.io/product-images/14436/3.jpg,https://oleks-netizen.github.io/product-images/14436/4.jpg,https://oleks-netizen.github.io/product-images/14436/5.jpg,https://oleks-netizen.github.io/product-images/14436/6.jpg,https://oleks-netizen.github.io/product-images/14436/8.jpg,https://oleks-netizen.github.io/product-images/14436/9.jpg</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>K11512z-green</t>
+          <t>14437</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K11512z-green/1.jpg,https://oleks-netizen.github.io/product-images/K11512z-green/2.jpg,https://oleks-netizen.github.io/product-images/K11512z-green/6.jpg,https://oleks-netizen.github.io/product-images/K11512z-green/4.jpg,https://oleks-netizen.github.io/product-images/K11512z-green/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14437/1.jpg,https://oleks-netizen.github.io/product-images/14437/2.jpg,https://oleks-netizen.github.io/product-images/14437/12.jpg,https://oleks-netizen.github.io/product-images/14437/10.jpg,https://oleks-netizen.github.io/product-images/14437/11.jpg,https://oleks-netizen.github.io/product-images/14437/3.jpg,https://oleks-netizen.github.io/product-images/14437/4.jpg,https://oleks-netizen.github.io/product-images/14437/5.jpg,https://oleks-netizen.github.io/product-images/14437/6.jpg,https://oleks-netizen.github.io/product-images/14437/7.jpg,https://oleks-netizen.github.io/product-images/14437/9.jpg</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>K12202bl-black</t>
+          <t>14439</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K12202bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K12202bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K12202bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K12202bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K12202bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14439/1.jpg,https://oleks-netizen.github.io/product-images/14439/2.jpg,https://oleks-netizen.github.io/product-images/14439/7.jpg,https://oleks-netizen.github.io/product-images/14439/9.jpg,https://oleks-netizen.github.io/product-images/14439/3.jpg,https://oleks-netizen.github.io/product-images/14439/4.jpg,https://oleks-netizen.github.io/product-images/14439/5.jpg,https://oleks-netizen.github.io/product-images/14439/6.jpg</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>K12504bl-black</t>
+          <t>14445</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K12504bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K12504bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K12504bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K12504bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K12504bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14445/1.jpg,https://oleks-netizen.github.io/product-images/14445/2.jpg,https://oleks-netizen.github.io/product-images/14445/12.jpg,https://oleks-netizen.github.io/product-images/14445/11.jpg,https://oleks-netizen.github.io/product-images/14445/3.jpg,https://oleks-netizen.github.io/product-images/14445/4.jpg,https://oleks-netizen.github.io/product-images/14445/5.jpg,https://oleks-netizen.github.io/product-images/14445/6.jpg,https://oleks-netizen.github.io/product-images/14445/7.jpg,https://oleks-netizen.github.io/product-images/14445/8.jpg,https://oleks-netizen.github.io/product-images/14445/9.jpg</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>K12507bl-black</t>
+          <t>14446</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K12507bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K12507bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K12507bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K12507bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K12507bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14446/1.jpg,https://oleks-netizen.github.io/product-images/14446/2.jpg,https://oleks-netizen.github.io/product-images/14446/9.jpg,https://oleks-netizen.github.io/product-images/14446/3.jpg,https://oleks-netizen.github.io/product-images/14446/4.jpg,https://oleks-netizen.github.io/product-images/14446/5.jpg,https://oleks-netizen.github.io/product-images/14446/6.jpg,https://oleks-netizen.github.io/product-images/14446/7.jpg</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>k12511bl-black</t>
+          <t>14448</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/k12511bl-black/1.jpg,https://oleks-netizen.github.io/product-images/k12511bl-black/2.jpg,https://oleks-netizen.github.io/product-images/k12511bl-black/7.jpg,https://oleks-netizen.github.io/product-images/k12511bl-black/4.jpg,https://oleks-netizen.github.io/product-images/k12511bl-black/5.jpg,https://oleks-netizen.github.io/product-images/k12511bl-black/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14448/1.jpg,https://oleks-netizen.github.io/product-images/14448/2.jpg,https://oleks-netizen.github.io/product-images/14448/13.jpg,https://oleks-netizen.github.io/product-images/14448/10.jpg,https://oleks-netizen.github.io/product-images/14448/12.jpg,https://oleks-netizen.github.io/product-images/14448/3.jpg,https://oleks-netizen.github.io/product-images/14448/4.jpg,https://oleks-netizen.github.io/product-images/14448/5.jpg,https://oleks-netizen.github.io/product-images/14448/6.jpg,https://oleks-netizen.github.io/product-images/14448/7.jpg,https://oleks-netizen.github.io/product-images/14448/8.jpg,https://oleks-netizen.github.io/product-images/14448/9.jpg</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>K1607bl-black</t>
+          <t>14449</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K1607bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K1607bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K1607bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K1607bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K1607bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14449/1.jpg,https://oleks-netizen.github.io/product-images/14449/2.jpg,https://oleks-netizen.github.io/product-images/14449/12.jpg,https://oleks-netizen.github.io/product-images/14449/10.jpg,https://oleks-netizen.github.io/product-images/14449/11.jpg,https://oleks-netizen.github.io/product-images/14449/3.jpg,https://oleks-netizen.github.io/product-images/14449/4.jpg,https://oleks-netizen.github.io/product-images/14449/5.jpg,https://oleks-netizen.github.io/product-images/14449/7.jpg,https://oleks-netizen.github.io/product-images/14449/8.jpg,https://oleks-netizen.github.io/product-images/14449/9.jpg</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>K1608be-beige</t>
+          <t>14452</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K1608be-beige/1.jpg,https://oleks-netizen.github.io/product-images/K1608be-beige/2.jpg,https://oleks-netizen.github.io/product-images/K1608be-beige/6.jpg,https://oleks-netizen.github.io/product-images/K1608be-beige/4.jpg,https://oleks-netizen.github.io/product-images/K1608be-beige/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14452/1.jpg,https://oleks-netizen.github.io/product-images/14452/2.jpg,https://oleks-netizen.github.io/product-images/14452/15.jpg,https://oleks-netizen.github.io/product-images/14452/10.jpg,https://oleks-netizen.github.io/product-images/14452/11.jpg,https://oleks-netizen.github.io/product-images/14452/12.jpg,https://oleks-netizen.github.io/product-images/14452/13.jpg,https://oleks-netizen.github.io/product-images/14452/3.jpg,https://oleks-netizen.github.io/product-images/14452/4.jpg,https://oleks-netizen.github.io/product-images/14452/5.jpg,https://oleks-netizen.github.io/product-images/14452/6.jpg,https://oleks-netizen.github.io/product-images/14452/7.jpg,https://oleks-netizen.github.io/product-images/14452/8.jpg,https://oleks-netizen.github.io/product-images/14452/9.jpg</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>K1608bl-black</t>
+          <t>14455</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K1608bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K1608bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K1608bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K1608bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K1608bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14455/1.jpg,https://oleks-netizen.github.io/product-images/14455/2.jpg,https://oleks-netizen.github.io/product-images/14455/10.jpg,https://oleks-netizen.github.io/product-images/14455/3.jpg,https://oleks-netizen.github.io/product-images/14455/4.jpg,https://oleks-netizen.github.io/product-images/14455/6.jpg,https://oleks-netizen.github.io/product-images/14455/7.jpg,https://oleks-netizen.github.io/product-images/14455/8.jpg,https://oleks-netizen.github.io/product-images/14455/9.jpg</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>K16101bl-black</t>
+          <t>14459</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K16101bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K16101bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K16101bl-black/7.jpg,https://oleks-netizen.github.io/product-images/K16101bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K16101bl-black/5.jpg,https://oleks-netizen.github.io/product-images/K16101bl-black/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14459/1.jpg,https://oleks-netizen.github.io/product-images/14459/2.jpg,https://oleks-netizen.github.io/product-images/14459/10.jpg,https://oleks-netizen.github.io/product-images/14459/3.jpg,https://oleks-netizen.github.io/product-images/14459/4.jpg,https://oleks-netizen.github.io/product-images/14459/5.jpg,https://oleks-netizen.github.io/product-images/14459/6.jpg,https://oleks-netizen.github.io/product-images/14459/7.jpg,https://oleks-netizen.github.io/product-images/14459/8.jpg</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>K17107bl-black</t>
+          <t>14462</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K17107bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K17107bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K17107bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K17107bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K17107bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14462/1.jpg,https://oleks-netizen.github.io/product-images/14462/2.jpg,https://oleks-netizen.github.io/product-images/14462/8.jpg,https://oleks-netizen.github.io/product-images/14462/11.jpg,https://oleks-netizen.github.io/product-images/14462/3.jpg,https://oleks-netizen.github.io/product-images/14462/4.jpg,https://oleks-netizen.github.io/product-images/14462/5.jpg,https://oleks-netizen.github.io/product-images/14462/6.jpg,https://oleks-netizen.github.io/product-images/14462/7.jpg,https://oleks-netizen.github.io/product-images/14462/9.jpg</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>K17107w-white</t>
+          <t>14463</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K17107w-white/1.jpg,https://oleks-netizen.github.io/product-images/K17107w-white/2.jpg,https://oleks-netizen.github.io/product-images/K17107w-white/6.jpg,https://oleks-netizen.github.io/product-images/K17107w-white/4.jpg,https://oleks-netizen.github.io/product-images/K17107w-white/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14463/1.jpg,https://oleks-netizen.github.io/product-images/14463/2.jpg,https://oleks-netizen.github.io/product-images/14463/4.jpg,https://oleks-netizen.github.io/product-images/14463/9.jpg,https://oleks-netizen.github.io/product-images/14463/3.jpg,https://oleks-netizen.github.io/product-images/14463/5.jpg,https://oleks-netizen.github.io/product-images/14463/6.jpg,https://oleks-netizen.github.io/product-images/14463/7.jpg</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>K17108bl-black</t>
+          <t>14464</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K17108bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K17108bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K17108bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K17108bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K17108bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14464/1.jpg,https://oleks-netizen.github.io/product-images/14464/2.jpg,https://oleks-netizen.github.io/product-images/14464/16.jpg,https://oleks-netizen.github.io/product-images/14464/11.jpg,https://oleks-netizen.github.io/product-images/14464/12.jpg,https://oleks-netizen.github.io/product-images/14464/13.jpg,https://oleks-netizen.github.io/product-images/14464/14.jpg,https://oleks-netizen.github.io/product-images/14464/15.jpg,https://oleks-netizen.github.io/product-images/14464/3.jpg,https://oleks-netizen.github.io/product-images/14464/4.jpg,https://oleks-netizen.github.io/product-images/14464/5.jpg,https://oleks-netizen.github.io/product-images/14464/6.jpg,https://oleks-netizen.github.io/product-images/14464/7.jpg,https://oleks-netizen.github.io/product-images/14464/8.jpg,https://oleks-netizen.github.io/product-images/14464/9.jpg</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>K17109bl-black</t>
+          <t>14467</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K17109bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K17109bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K17109bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K17109bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K17109bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14467/1.jpg,https://oleks-netizen.github.io/product-images/14467/2.jpg,https://oleks-netizen.github.io/product-images/14467/13.jpg,https://oleks-netizen.github.io/product-images/14467/10.jpg,https://oleks-netizen.github.io/product-images/14467/12.jpg,https://oleks-netizen.github.io/product-images/14467/3.jpg,https://oleks-netizen.github.io/product-images/14467/4.jpg,https://oleks-netizen.github.io/product-images/14467/5.jpg,https://oleks-netizen.github.io/product-images/14467/6.jpg,https://oleks-netizen.github.io/product-images/14467/7.jpg,https://oleks-netizen.github.io/product-images/14467/8.jpg,https://oleks-netizen.github.io/product-images/14467/9.jpg</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>K18005bl-black</t>
+          <t>14473</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K18005bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K18005bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K18005bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K18005bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K18005bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14473/1.jpg,https://oleks-netizen.github.io/product-images/14473/2.jpg,https://oleks-netizen.github.io/product-images/14473/6.jpg,https://oleks-netizen.github.io/product-images/14473/11.jpg,https://oleks-netizen.github.io/product-images/14473/3.jpg,https://oleks-netizen.github.io/product-images/14473/4.jpg,https://oleks-netizen.github.io/product-images/14473/5.jpg,https://oleks-netizen.github.io/product-images/14473/7.jpg,https://oleks-netizen.github.io/product-images/14473/8.jpg,https://oleks-netizen.github.io/product-images/14473/9.jpg</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>K18012bl-black</t>
+          <t>14474</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K18012bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K18012bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K18012bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K18012bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K18012bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14474/1.jpg,https://oleks-netizen.github.io/product-images/14474/2.jpg,https://oleks-netizen.github.io/product-images/14474/6.jpg,https://oleks-netizen.github.io/product-images/14474/11.jpg,https://oleks-netizen.github.io/product-images/14474/10.jpg,https://oleks-netizen.github.io/product-images/14474/3.jpg,https://oleks-netizen.github.io/product-images/14474/4.jpg,https://oleks-netizen.github.io/product-images/14474/5.jpg,https://oleks-netizen.github.io/product-images/14474/8.jpg,https://oleks-netizen.github.io/product-images/14474/9.jpg</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>K188084bl-black</t>
+          <t>14478</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K188084bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K188084bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K188084bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K188084bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K188084bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14478/1.jpg,https://oleks-netizen.github.io/product-images/14478/2.jpg,https://oleks-netizen.github.io/product-images/14478/7.jpg,https://oleks-netizen.github.io/product-images/14478/11.jpg,https://oleks-netizen.github.io/product-images/14478/10.jpg,https://oleks-netizen.github.io/product-images/14478/3.jpg,https://oleks-netizen.github.io/product-images/14478/4.jpg,https://oleks-netizen.github.io/product-images/14478/5.jpg,https://oleks-netizen.github.io/product-images/14478/6.jpg,https://oleks-netizen.github.io/product-images/14478/8.jpg</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>K188084gr-gray</t>
+          <t>14479</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K188084gr-gray/1.jpg,https://oleks-netizen.github.io/product-images/K188084gr-gray/2.jpg,https://oleks-netizen.github.io/product-images/K188084gr-gray/6.jpg,https://oleks-netizen.github.io/product-images/K188084gr-gray/4.jpg,https://oleks-netizen.github.io/product-images/K188084gr-gray/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14479/1.jpg,https://oleks-netizen.github.io/product-images/14479/2.jpg,https://oleks-netizen.github.io/product-images/14479/11.jpg,https://oleks-netizen.github.io/product-images/14479/10.jpg,https://oleks-netizen.github.io/product-images/14479/3.jpg,https://oleks-netizen.github.io/product-images/14479/4.jpg,https://oleks-netizen.github.io/product-images/14479/5.jpg,https://oleks-netizen.github.io/product-images/14479/6.jpg,https://oleks-netizen.github.io/product-images/14479/8.jpg,https://oleks-netizen.github.io/product-images/14479/9.jpg</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>K18817bl-black</t>
+          <t>14484</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K18817bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K18817bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K18817bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K18817bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K18817bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14484/1.jpg,https://oleks-netizen.github.io/product-images/14484/2.jpg,https://oleks-netizen.github.io/product-images/14484/14.jpg,https://oleks-netizen.github.io/product-images/14484/10.jpg,https://oleks-netizen.github.io/product-images/14484/11.jpg,https://oleks-netizen.github.io/product-images/14484/12.jpg,https://oleks-netizen.github.io/product-images/14484/3.jpg,https://oleks-netizen.github.io/product-images/14484/4.jpg,https://oleks-netizen.github.io/product-images/14484/5.jpg,https://oleks-netizen.github.io/product-images/14484/6.jpg,https://oleks-netizen.github.io/product-images/14484/7.jpg,https://oleks-netizen.github.io/product-images/14484/8.jpg,https://oleks-netizen.github.io/product-images/14484/9.jpg</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>K18868bl-black</t>
+          <t>14497</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K18868bl-black/1.jpg,https://oleks-netizen.github.io/product-images/K18868bl-black/2.jpg,https://oleks-netizen.github.io/product-images/K18868bl-black/6.jpg,https://oleks-netizen.github.io/product-images/K18868bl-black/4.jpg,https://oleks-netizen.github.io/product-images/K18868bl-black/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14497/1.jpg,https://oleks-netizen.github.io/product-images/14497/2.jpg,https://oleks-netizen.github.io/product-images/14497/13.jpg,https://oleks-netizen.github.io/product-images/14497/11.jpg,https://oleks-netizen.github.io/product-images/14497/12.jpg,https://oleks-netizen.github.io/product-images/14497/3.jpg,https://oleks-netizen.github.io/product-images/14497/4.jpg,https://oleks-netizen.github.io/product-images/14497/5.jpg,https://oleks-netizen.github.io/product-images/14497/6.jpg,https://oleks-netizen.github.io/product-images/14497/7.jpg,https://oleks-netizen.github.io/product-images/14497/8.jpg,https://oleks-netizen.github.io/product-images/14497/9.jpg</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>K45 BLK</t>
+          <t>14499</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K45 BLK/1.jpg,https://oleks-netizen.github.io/product-images/K45 BLK/2.jpg,https://oleks-netizen.github.io/product-images/K45 BLK/6.jpg,https://oleks-netizen.github.io/product-images/K45 BLK/3.jpg,https://oleks-netizen.github.io/product-images/K45 BLK/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14499/1.jpg,https://oleks-netizen.github.io/product-images/14499/2.jpg,https://oleks-netizen.github.io/product-images/14499/10.jpg,https://oleks-netizen.github.io/product-images/14499/3.jpg,https://oleks-netizen.github.io/product-images/14499/4.jpg,https://oleks-netizen.github.io/product-images/14499/5.jpg,https://oleks-netizen.github.io/product-images/14499/6.jpg,https://oleks-netizen.github.io/product-images/14499/8.jpg,https://oleks-netizen.github.io/product-images/14499/9.jpg</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>K46 BLK</t>
+          <t>14500</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K46 BLK/1.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14500/1.jpg,https://oleks-netizen.github.io/product-images/14500/2.jpg,https://oleks-netizen.github.io/product-images/14500/8.jpg,https://oleks-netizen.github.io/product-images/14500/10.jpg,https://oleks-netizen.github.io/product-images/14500/3.jpg,https://oleks-netizen.github.io/product-images/14500/4.jpg,https://oleks-netizen.github.io/product-images/14500/6.jpg,https://oleks-netizen.github.io/product-images/14500/7.jpg,https://oleks-netizen.github.io/product-images/14500/9.jpg</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>L20037-1</t>
+          <t>14501</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20037-1/1.jpg,https://oleks-netizen.github.io/product-images/L20037-1/2.jpg,https://oleks-netizen.github.io/product-images/L20037-1/8.jpg,https://oleks-netizen.github.io/product-images/L20037-1/4.jpg,https://oleks-netizen.github.io/product-images/L20037-1/5.jpg,https://oleks-netizen.github.io/product-images/L20037-1/6.jpg,https://oleks-netizen.github.io/product-images/L20037-1/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14501/1.jpg,https://oleks-netizen.github.io/product-images/14501/2.jpg,https://oleks-netizen.github.io/product-images/14501/5.jpg,https://oleks-netizen.github.io/product-images/14501/8.jpg,https://oleks-netizen.github.io/product-images/14501/3.jpg,https://oleks-netizen.github.io/product-images/14501/4.jpg,https://oleks-netizen.github.io/product-images/14501/6.jpg</t>
         </is>
       </c>
       <c r="C78" t="n">
@@ -1596,72 +1596,72 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>L20037-40</t>
+          <t>14509</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20037-40/1.jpg,https://oleks-netizen.github.io/product-images/L20037-40/2.jpg,https://oleks-netizen.github.io/product-images/L20037-40/3.jpg,https://oleks-netizen.github.io/product-images/L20037-40/8.jpg,https://oleks-netizen.github.io/product-images/L20037-40/5.jpg,https://oleks-netizen.github.io/product-images/L20037-40/6.jpg,https://oleks-netizen.github.io/product-images/L20037-40/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14509/1.jpg,https://oleks-netizen.github.io/product-images/14509/2.jpg,https://oleks-netizen.github.io/product-images/14509/10.jpg,https://oleks-netizen.github.io/product-images/14509/3.jpg,https://oleks-netizen.github.io/product-images/14509/4.jpg,https://oleks-netizen.github.io/product-images/14509/5.jpg,https://oleks-netizen.github.io/product-images/14509/6.jpg,https://oleks-netizen.github.io/product-images/14509/8.jpg,https://oleks-netizen.github.io/product-images/14509/9.jpg</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>L20037-56</t>
+          <t>14512</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20037-56/1.jpg,https://oleks-netizen.github.io/product-images/L20037-56/2.jpg,https://oleks-netizen.github.io/product-images/L20037-56/3.jpg,https://oleks-netizen.github.io/product-images/L20037-56/8.jpg,https://oleks-netizen.github.io/product-images/L20037-56/5.jpg,https://oleks-netizen.github.io/product-images/L20037-56/6.jpg,https://oleks-netizen.github.io/product-images/L20037-56/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14512/1.jpg,https://oleks-netizen.github.io/product-images/14512/2.jpg,https://oleks-netizen.github.io/product-images/14512/5.jpg,https://oleks-netizen.github.io/product-images/14512/9.jpg,https://oleks-netizen.github.io/product-images/14512/3.jpg,https://oleks-netizen.github.io/product-images/14512/4.jpg,https://oleks-netizen.github.io/product-images/14512/6.jpg,https://oleks-netizen.github.io/product-images/14512/7.jpg</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>L20066-1</t>
+          <t>14515</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20066-1/1.jpg,https://oleks-netizen.github.io/product-images/L20066-1/2.jpg,https://oleks-netizen.github.io/product-images/L20066-1/3.jpg,https://oleks-netizen.github.io/product-images/L20066-1/8.jpg,https://oleks-netizen.github.io/product-images/L20066-1/5.jpg,https://oleks-netizen.github.io/product-images/L20066-1/6.jpg,https://oleks-netizen.github.io/product-images/L20066-1/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14515/1.jpg,https://oleks-netizen.github.io/product-images/14515/2.jpg,https://oleks-netizen.github.io/product-images/14515/5.jpg,https://oleks-netizen.github.io/product-images/14515/9.jpg,https://oleks-netizen.github.io/product-images/14515/3.jpg,https://oleks-netizen.github.io/product-images/14515/4.jpg,https://oleks-netizen.github.io/product-images/14515/6.jpg,https://oleks-netizen.github.io/product-images/14515/7.jpg</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>L20066-2</t>
+          <t>14516</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20066-2/1.jpg,https://oleks-netizen.github.io/product-images/L20066-2/2.jpg,https://oleks-netizen.github.io/product-images/L20066-2/3.jpg,https://oleks-netizen.github.io/product-images/L20066-2/8.jpg,https://oleks-netizen.github.io/product-images/L20066-2/5.jpg,https://oleks-netizen.github.io/product-images/L20066-2/6.jpg,https://oleks-netizen.github.io/product-images/L20066-2/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14516/1.jpg,https://oleks-netizen.github.io/product-images/14516/2.jpg,https://oleks-netizen.github.io/product-images/14516/6.jpg,https://oleks-netizen.github.io/product-images/14516/10.jpg,https://oleks-netizen.github.io/product-images/14516/3.jpg,https://oleks-netizen.github.io/product-images/14516/4.jpg,https://oleks-netizen.github.io/product-images/14516/5.jpg,https://oleks-netizen.github.io/product-images/14516/7.jpg,https://oleks-netizen.github.io/product-images/14516/9.jpg</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>L20066-6</t>
+          <t>14531</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20066-6/1.jpg,https://oleks-netizen.github.io/product-images/L20066-6/3.jpg,https://oleks-netizen.github.io/product-images/L20066-6/8.jpg,https://oleks-netizen.github.io/product-images/L20066-6/4.jpg,https://oleks-netizen.github.io/product-images/L20066-6/5.jpg,https://oleks-netizen.github.io/product-images/L20066-6/6.jpg,https://oleks-netizen.github.io/product-images/L20066-6/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14531/1.jpg,https://oleks-netizen.github.io/product-images/14531/2.jpg,https://oleks-netizen.github.io/product-images/14531/4.jpg,https://oleks-netizen.github.io/product-images/14531/8.jpg,https://oleks-netizen.github.io/product-images/14531/3.jpg,https://oleks-netizen.github.io/product-images/14531/5.jpg,https://oleks-netizen.github.io/product-images/14531/6.jpg</t>
         </is>
       </c>
       <c r="C83" t="n">
@@ -1671,252 +1671,252 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>L20138-1</t>
+          <t>14532</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20138-1/1.jpg,https://oleks-netizen.github.io/product-images/L20138-1/2.jpg,https://oleks-netizen.github.io/product-images/L20138-1/3.jpg,https://oleks-netizen.github.io/product-images/L20138-1/8.jpg,https://oleks-netizen.github.io/product-images/L20138-1/5.jpg,https://oleks-netizen.github.io/product-images/L20138-1/6.jpg,https://oleks-netizen.github.io/product-images/L20138-1/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14532/1.jpg,https://oleks-netizen.github.io/product-images/14532/2.jpg,https://oleks-netizen.github.io/product-images/14532/9.jpg,https://oleks-netizen.github.io/product-images/14532/3.jpg,https://oleks-netizen.github.io/product-images/14532/4.jpg,https://oleks-netizen.github.io/product-images/14532/5.jpg,https://oleks-netizen.github.io/product-images/14532/7.jpg,https://oleks-netizen.github.io/product-images/14532/8.jpg</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>L20138-15</t>
+          <t>14534</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20138-15/1.jpg,https://oleks-netizen.github.io/product-images/L20138-15/2.jpg,https://oleks-netizen.github.io/product-images/L20138-15/3.jpg,https://oleks-netizen.github.io/product-images/L20138-15/8.jpg,https://oleks-netizen.github.io/product-images/L20138-15/5.jpg,https://oleks-netizen.github.io/product-images/L20138-15/6.jpg,https://oleks-netizen.github.io/product-images/L20138-15/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14534/1.jpg,https://oleks-netizen.github.io/product-images/14534/2.jpg,https://oleks-netizen.github.io/product-images/14534/14.jpg,https://oleks-netizen.github.io/product-images/14534/11.jpg,https://oleks-netizen.github.io/product-images/14534/12.jpg,https://oleks-netizen.github.io/product-images/14534/13.jpg,https://oleks-netizen.github.io/product-images/14534/3.jpg,https://oleks-netizen.github.io/product-images/14534/4.jpg,https://oleks-netizen.github.io/product-images/14534/5.jpg,https://oleks-netizen.github.io/product-images/14534/6.jpg,https://oleks-netizen.github.io/product-images/14534/7.jpg,https://oleks-netizen.github.io/product-images/14534/8.jpg,https://oleks-netizen.github.io/product-images/14534/9.jpg</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>L20138-2</t>
+          <t>14536</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20138-2/1.jpg,https://oleks-netizen.github.io/product-images/L20138-2/2.jpg,https://oleks-netizen.github.io/product-images/L20138-2/3.jpg,https://oleks-netizen.github.io/product-images/L20138-2/8.jpg,https://oleks-netizen.github.io/product-images/L20138-2/5.jpg,https://oleks-netizen.github.io/product-images/L20138-2/6.jpg,https://oleks-netizen.github.io/product-images/L20138-2/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14536/1.jpg,https://oleks-netizen.github.io/product-images/14536/2.jpg,https://oleks-netizen.github.io/product-images/14536/3.jpg,https://oleks-netizen.github.io/product-images/14536/11.jpg,https://oleks-netizen.github.io/product-images/14536/10.jpg,https://oleks-netizen.github.io/product-images/14536/4.jpg,https://oleks-netizen.github.io/product-images/14536/5.jpg,https://oleks-netizen.github.io/product-images/14536/6.jpg,https://oleks-netizen.github.io/product-images/14536/8.jpg,https://oleks-netizen.github.io/product-images/14536/9.jpg</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>L20711-1</t>
+          <t>14563</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20711-1/1.jpg,https://oleks-netizen.github.io/product-images/L20711-1/2.jpg,https://oleks-netizen.github.io/product-images/L20711-1/3.jpg,https://oleks-netizen.github.io/product-images/L20711-1/8.jpg,https://oleks-netizen.github.io/product-images/L20711-1/5.jpg,https://oleks-netizen.github.io/product-images/L20711-1/6.jpg,https://oleks-netizen.github.io/product-images/L20711-1/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14563/1.jpg,https://oleks-netizen.github.io/product-images/14563/2.jpg,https://oleks-netizen.github.io/product-images/14563/13.jpg,https://oleks-netizen.github.io/product-images/14563/10.jpg,https://oleks-netizen.github.io/product-images/14563/12.jpg,https://oleks-netizen.github.io/product-images/14563/3.jpg,https://oleks-netizen.github.io/product-images/14563/4.jpg,https://oleks-netizen.github.io/product-images/14563/5.jpg,https://oleks-netizen.github.io/product-images/14563/6.jpg,https://oleks-netizen.github.io/product-images/14563/7.jpg,https://oleks-netizen.github.io/product-images/14563/8.jpg,https://oleks-netizen.github.io/product-images/14563/9.jpg</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>L20711-56</t>
+          <t>14567</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20711-56/1.jpg,https://oleks-netizen.github.io/product-images/L20711-56/2.jpg,https://oleks-netizen.github.io/product-images/L20711-56/3.jpg,https://oleks-netizen.github.io/product-images/L20711-56/8.jpg,https://oleks-netizen.github.io/product-images/L20711-56/5.jpg,https://oleks-netizen.github.io/product-images/L20711-56/6.jpg,https://oleks-netizen.github.io/product-images/L20711-56/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14567/1.jpg,https://oleks-netizen.github.io/product-images/14567/2.jpg,https://oleks-netizen.github.io/product-images/14567/11.jpg,https://oleks-netizen.github.io/product-images/14567/3.jpg,https://oleks-netizen.github.io/product-images/14567/4.jpg,https://oleks-netizen.github.io/product-images/14567/5.jpg,https://oleks-netizen.github.io/product-images/14567/6.jpg,https://oleks-netizen.github.io/product-images/14567/7.jpg,https://oleks-netizen.github.io/product-images/14567/8.jpg,https://oleks-netizen.github.io/product-images/14567/9.jpg</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>L20711-80</t>
+          <t>14580</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20711-80/1.jpg,https://oleks-netizen.github.io/product-images/L20711-80/2.jpg,https://oleks-netizen.github.io/product-images/L20711-80/3.jpg,https://oleks-netizen.github.io/product-images/L20711-80/8.jpg,https://oleks-netizen.github.io/product-images/L20711-80/5.jpg,https://oleks-netizen.github.io/product-images/L20711-80/6.jpg,https://oleks-netizen.github.io/product-images/L20711-80/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14580/1.jpg,https://oleks-netizen.github.io/product-images/14580/2.jpg,https://oleks-netizen.github.io/product-images/14580/12.jpg,https://oleks-netizen.github.io/product-images/14580/10.jpg,https://oleks-netizen.github.io/product-images/14580/11.jpg,https://oleks-netizen.github.io/product-images/14580/3.jpg,https://oleks-netizen.github.io/product-images/14580/4.jpg,https://oleks-netizen.github.io/product-images/14580/6.jpg,https://oleks-netizen.github.io/product-images/14580/7.jpg,https://oleks-netizen.github.io/product-images/14580/8.jpg,https://oleks-netizen.github.io/product-images/14580/9.jpg</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>L20712-1</t>
+          <t>14581</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20712-1/1.jpg,https://oleks-netizen.github.io/product-images/L20712-1/2.jpg,https://oleks-netizen.github.io/product-images/L20712-1/3.jpg,https://oleks-netizen.github.io/product-images/L20712-1/8.jpg,https://oleks-netizen.github.io/product-images/L20712-1/5.jpg,https://oleks-netizen.github.io/product-images/L20712-1/6.jpg,https://oleks-netizen.github.io/product-images/L20712-1/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14581/1.jpg,https://oleks-netizen.github.io/product-images/14581/2.jpg,https://oleks-netizen.github.io/product-images/14581/13.jpg,https://oleks-netizen.github.io/product-images/14581/10.jpg,https://oleks-netizen.github.io/product-images/14581/11.jpg,https://oleks-netizen.github.io/product-images/14581/12.jpg,https://oleks-netizen.github.io/product-images/14581/3.jpg,https://oleks-netizen.github.io/product-images/14581/4.jpg,https://oleks-netizen.github.io/product-images/14581/5.jpg,https://oleks-netizen.github.io/product-images/14581/6.jpg,https://oleks-netizen.github.io/product-images/14581/8.jpg,https://oleks-netizen.github.io/product-images/14581/9.jpg</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>L20712-2</t>
+          <t>14585</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L20712-2/1.jpg,https://oleks-netizen.github.io/product-images/L20712-2/2.jpg,https://oleks-netizen.github.io/product-images/L20712-2/3.jpg,https://oleks-netizen.github.io/product-images/L20712-2/8.jpg,https://oleks-netizen.github.io/product-images/L20712-2/5.jpg,https://oleks-netizen.github.io/product-images/L20712-2/6.jpg,https://oleks-netizen.github.io/product-images/L20712-2/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14585/1.jpg,https://oleks-netizen.github.io/product-images/14585/2.jpg,https://oleks-netizen.github.io/product-images/14585/10.jpg,https://oleks-netizen.github.io/product-images/14585/3.jpg,https://oleks-netizen.github.io/product-images/14585/4.jpg,https://oleks-netizen.github.io/product-images/14585/5.jpg,https://oleks-netizen.github.io/product-images/14585/6.jpg,https://oleks-netizen.github.io/product-images/14585/7.jpg,https://oleks-netizen.github.io/product-images/14585/9.jpg</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>L87026-01</t>
+          <t>14588</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L87026-01/1.jpg,https://oleks-netizen.github.io/product-images/L87026-01/2.jpg,https://oleks-netizen.github.io/product-images/L87026-01/3.jpg,https://oleks-netizen.github.io/product-images/L87026-01/10.jpg,https://oleks-netizen.github.io/product-images/L87026-01/5.jpg,https://oleks-netizen.github.io/product-images/L87026-01/6.jpg,https://oleks-netizen.github.io/product-images/L87026-01/7.jpg,https://oleks-netizen.github.io/product-images/L87026-01/8.jpg,https://oleks-netizen.github.io/product-images/L87026-01/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14588/1.jpg,https://oleks-netizen.github.io/product-images/14588/2.jpg,https://oleks-netizen.github.io/product-images/14588/12.jpg,https://oleks-netizen.github.io/product-images/14588/10.jpg,https://oleks-netizen.github.io/product-images/14588/11.jpg,https://oleks-netizen.github.io/product-images/14588/3.jpg,https://oleks-netizen.github.io/product-images/14588/4.jpg,https://oleks-netizen.github.io/product-images/14588/5.jpg,https://oleks-netizen.github.io/product-images/14588/6.jpg,https://oleks-netizen.github.io/product-images/14588/8.jpg,https://oleks-netizen.github.io/product-images/14588/9.jpg</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>L87026-130</t>
+          <t>14590</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L87026-130/1.jpg,https://oleks-netizen.github.io/product-images/L87026-130/2.jpg,https://oleks-netizen.github.io/product-images/L87026-130/3.jpg,https://oleks-netizen.github.io/product-images/L87026-130/10.jpg,https://oleks-netizen.github.io/product-images/L87026-130/5.jpg,https://oleks-netizen.github.io/product-images/L87026-130/6.jpg,https://oleks-netizen.github.io/product-images/L87026-130/7.jpg,https://oleks-netizen.github.io/product-images/L87026-130/8.jpg,https://oleks-netizen.github.io/product-images/L87026-130/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14590/1.jpg,https://oleks-netizen.github.io/product-images/14590/2.jpg,https://oleks-netizen.github.io/product-images/14590/11.jpg,https://oleks-netizen.github.io/product-images/14590/10.jpg,https://oleks-netizen.github.io/product-images/14590/3.jpg,https://oleks-netizen.github.io/product-images/14590/4.jpg,https://oleks-netizen.github.io/product-images/14590/5.jpg,https://oleks-netizen.github.io/product-images/14590/7.jpg,https://oleks-netizen.github.io/product-images/14590/8.jpg,https://oleks-netizen.github.io/product-images/14590/9.jpg</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>L87026-152</t>
+          <t>14591</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L87026-152/1.jpg,https://oleks-netizen.github.io/product-images/L87026-152/2.jpg,https://oleks-netizen.github.io/product-images/L87026-152/3.jpg,https://oleks-netizen.github.io/product-images/L87026-152/10.jpg,https://oleks-netizen.github.io/product-images/L87026-152/5.jpg,https://oleks-netizen.github.io/product-images/L87026-152/6.jpg,https://oleks-netizen.github.io/product-images/L87026-152/7.jpg,https://oleks-netizen.github.io/product-images/L87026-152/8.jpg,https://oleks-netizen.github.io/product-images/L87026-152/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14591/1.jpg,https://oleks-netizen.github.io/product-images/14591/2.jpg,https://oleks-netizen.github.io/product-images/14591/11.jpg,https://oleks-netizen.github.io/product-images/14591/10.jpg,https://oleks-netizen.github.io/product-images/14591/3.jpg,https://oleks-netizen.github.io/product-images/14591/4.jpg,https://oleks-netizen.github.io/product-images/14591/5.jpg,https://oleks-netizen.github.io/product-images/14591/6.jpg,https://oleks-netizen.github.io/product-images/14591/7.jpg,https://oleks-netizen.github.io/product-images/14591/9.jpg</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>L87110-01</t>
+          <t>14595</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L87110-01/1.jpg,https://oleks-netizen.github.io/product-images/L87110-01/2.jpg,https://oleks-netizen.github.io/product-images/L87110-01/10.jpg,https://oleks-netizen.github.io/product-images/L87110-01/4.jpg,https://oleks-netizen.github.io/product-images/L87110-01/5.jpg,https://oleks-netizen.github.io/product-images/L87110-01/6.jpg,https://oleks-netizen.github.io/product-images/L87110-01/7.jpg,https://oleks-netizen.github.io/product-images/L87110-01/8.jpg,https://oleks-netizen.github.io/product-images/L87110-01/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14595/1.jpg,https://oleks-netizen.github.io/product-images/14595/2.jpg,https://oleks-netizen.github.io/product-images/14595/12.jpg,https://oleks-netizen.github.io/product-images/14595/13.jpg,https://oleks-netizen.github.io/product-images/14595/11.jpg,https://oleks-netizen.github.io/product-images/14595/3.jpg,https://oleks-netizen.github.io/product-images/14595/4.jpg,https://oleks-netizen.github.io/product-images/14595/5.jpg,https://oleks-netizen.github.io/product-images/14595/6.jpg,https://oleks-netizen.github.io/product-images/14595/7.jpg,https://oleks-netizen.github.io/product-images/14595/8.jpg,https://oleks-netizen.github.io/product-images/14595/9.jpg</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>L87110-13</t>
+          <t>14596</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L87110-13/1.jpg,https://oleks-netizen.github.io/product-images/L87110-13/2.jpg,https://oleks-netizen.github.io/product-images/L87110-13/10.jpg,https://oleks-netizen.github.io/product-images/L87110-13/4.jpg,https://oleks-netizen.github.io/product-images/L87110-13/5.jpg,https://oleks-netizen.github.io/product-images/L87110-13/6.jpg,https://oleks-netizen.github.io/product-images/L87110-13/7.jpg,https://oleks-netizen.github.io/product-images/L87110-13/8.jpg,https://oleks-netizen.github.io/product-images/L87110-13/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14596/1.jpg,https://oleks-netizen.github.io/product-images/14596/2.jpg,https://oleks-netizen.github.io/product-images/14596/5.jpg,https://oleks-netizen.github.io/product-images/14596/7.jpg,https://oleks-netizen.github.io/product-images/14596/3.jpg,https://oleks-netizen.github.io/product-images/14596/4.jpg</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>L87110-22</t>
+          <t>14597</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L87110-22/1.jpg,https://oleks-netizen.github.io/product-images/L87110-22/2.jpg,https://oleks-netizen.github.io/product-images/L87110-22/10.jpg,https://oleks-netizen.github.io/product-images/L87110-22/4.jpg,https://oleks-netizen.github.io/product-images/L87110-22/5.jpg,https://oleks-netizen.github.io/product-images/L87110-22/6.jpg,https://oleks-netizen.github.io/product-images/L87110-22/7.jpg,https://oleks-netizen.github.io/product-images/L87110-22/8.jpg,https://oleks-netizen.github.io/product-images/L87110-22/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14597/1.jpg,https://oleks-netizen.github.io/product-images/14597/2.jpg,https://oleks-netizen.github.io/product-images/14597/6.jpg,https://oleks-netizen.github.io/product-images/14597/12.jpg,https://oleks-netizen.github.io/product-images/14597/11.jpg,https://oleks-netizen.github.io/product-images/14597/3.jpg,https://oleks-netizen.github.io/product-images/14597/4.jpg,https://oleks-netizen.github.io/product-images/14597/5.jpg,https://oleks-netizen.github.io/product-images/14597/7.jpg,https://oleks-netizen.github.io/product-images/14597/8.jpg,https://oleks-netizen.github.io/product-images/14597/9.jpg</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>L87110-23</t>
+          <t>14598</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L87110-23/1.jpg,https://oleks-netizen.github.io/product-images/L87110-23/2.jpg,https://oleks-netizen.github.io/product-images/L87110-23/6.jpg,https://oleks-netizen.github.io/product-images/L87110-23/4.jpg,https://oleks-netizen.github.io/product-images/L87110-23/5.jpg,https://oleks-netizen.github.io/product-images/L87110-23/7.jpg,https://oleks-netizen.github.io/product-images/L87110-23/8.jpg,https://oleks-netizen.github.io/product-images/L87110-23/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14598/1.jpg,https://oleks-netizen.github.io/product-images/14598/2.jpg,https://oleks-netizen.github.io/product-images/14598/3.jpg,https://oleks-netizen.github.io/product-images/14598/14.jpg,https://oleks-netizen.github.io/product-images/14598/11.jpg,https://oleks-netizen.github.io/product-images/14598/12.jpg,https://oleks-netizen.github.io/product-images/14598/13.jpg,https://oleks-netizen.github.io/product-images/14598/4.jpg,https://oleks-netizen.github.io/product-images/14598/5.jpg,https://oleks-netizen.github.io/product-images/14598/6.jpg,https://oleks-netizen.github.io/product-images/14598/7.jpg,https://oleks-netizen.github.io/product-images/14598/8.jpg,https://oleks-netizen.github.io/product-images/14598/9.jpg</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>L87296-01</t>
+          <t>14602</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L87296-01/1.jpg,https://oleks-netizen.github.io/product-images/L87296-01/2.jpg,https://oleks-netizen.github.io/product-images/L87296-01/10.jpg,https://oleks-netizen.github.io/product-images/L87296-01/4.jpg,https://oleks-netizen.github.io/product-images/L87296-01/5.jpg,https://oleks-netizen.github.io/product-images/L87296-01/6.jpg,https://oleks-netizen.github.io/product-images/L87296-01/7.jpg,https://oleks-netizen.github.io/product-images/L87296-01/8.jpg,https://oleks-netizen.github.io/product-images/L87296-01/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14602/1.jpg,https://oleks-netizen.github.io/product-images/14602/2.jpg,https://oleks-netizen.github.io/product-images/14602/10.jpg,https://oleks-netizen.github.io/product-images/14602/11.jpg,https://oleks-netizen.github.io/product-images/14602/12.jpg,https://oleks-netizen.github.io/product-images/14602/13.jpg,https://oleks-netizen.github.io/product-images/14602/14.jpg,https://oleks-netizen.github.io/product-images/14602/15.jpg,https://oleks-netizen.github.io/product-images/14602/16.jpg,https://oleks-netizen.github.io/product-images/14602/17.jpg,https://oleks-netizen.github.io/product-images/14602/18.jpg,https://oleks-netizen.github.io/product-images/14602/3.jpg,https://oleks-netizen.github.io/product-images/14602/4.jpg,https://oleks-netizen.github.io/product-images/14602/5.jpg,https://oleks-netizen.github.io/product-images/14602/6.jpg,https://oleks-netizen.github.io/product-images/14602/7.jpg,https://oleks-netizen.github.io/product-images/14602/8.jpg,https://oleks-netizen.github.io/product-images/14602/9.jpg</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>L87296-13</t>
+          <t>14603</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L87296-13/1.jpg,https://oleks-netizen.github.io/product-images/L87296-13/2.jpg,https://oleks-netizen.github.io/product-images/L87296-13/10.jpg,https://oleks-netizen.github.io/product-images/L87296-13/4.jpg,https://oleks-netizen.github.io/product-images/L87296-13/5.jpg,https://oleks-netizen.github.io/product-images/L87296-13/6.jpg,https://oleks-netizen.github.io/product-images/L87296-13/7.jpg,https://oleks-netizen.github.io/product-images/L87296-13/8.jpg,https://oleks-netizen.github.io/product-images/L87296-13/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14603/1.jpg,https://oleks-netizen.github.io/product-images/14603/2.jpg,https://oleks-netizen.github.io/product-images/14603/10.jpg,https://oleks-netizen.github.io/product-images/14603/3.jpg,https://oleks-netizen.github.io/product-images/14603/4.jpg,https://oleks-netizen.github.io/product-images/14603/5.jpg,https://oleks-netizen.github.io/product-images/14603/6.jpg,https://oleks-netizen.github.io/product-images/14603/8.jpg,https://oleks-netizen.github.io/product-images/14603/9.jpg</t>
         </is>
       </c>
       <c r="C100" t="n">
@@ -1926,207 +1926,207 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>L87296-23</t>
+          <t>14604</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L87296-23/1.jpg,https://oleks-netizen.github.io/product-images/L87296-23/2.jpg,https://oleks-netizen.github.io/product-images/L87296-23/10.jpg,https://oleks-netizen.github.io/product-images/L87296-23/4.jpg,https://oleks-netizen.github.io/product-images/L87296-23/5.jpg,https://oleks-netizen.github.io/product-images/L87296-23/6.jpg,https://oleks-netizen.github.io/product-images/L87296-23/7.jpg,https://oleks-netizen.github.io/product-images/L87296-23/8.jpg,https://oleks-netizen.github.io/product-images/L87296-23/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14604/1.jpg,https://oleks-netizen.github.io/product-images/14604/2.jpg,https://oleks-netizen.github.io/product-images/14604/12.jpg,https://oleks-netizen.github.io/product-images/14604/10.jpg,https://oleks-netizen.github.io/product-images/14604/11.jpg,https://oleks-netizen.github.io/product-images/14604/3.jpg,https://oleks-netizen.github.io/product-images/14604/4.jpg,https://oleks-netizen.github.io/product-images/14604/5.jpg,https://oleks-netizen.github.io/product-images/14604/6.jpg,https://oleks-netizen.github.io/product-images/14604/7.jpg,https://oleks-netizen.github.io/product-images/14604/9.jpg</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>L87296-33</t>
+          <t>14607</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L87296-33/1.jpg,https://oleks-netizen.github.io/product-images/L87296-33/2.jpg,https://oleks-netizen.github.io/product-images/L87296-33/4.jpg,https://oleks-netizen.github.io/product-images/L87296-33/5.jpg,https://oleks-netizen.github.io/product-images/L87296-33/6.jpg,https://oleks-netizen.github.io/product-images/L87296-33/7.jpg,https://oleks-netizen.github.io/product-images/L87296-33/8.jpg,https://oleks-netizen.github.io/product-images/L87296-33/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14607/10.jpg,https://oleks-netizen.github.io/product-images/14607/11.jpg,https://oleks-netizen.github.io/product-images/14607/12.jpg,https://oleks-netizen.github.io/product-images/14607/1.jpg,https://oleks-netizen.github.io/product-images/14607/2.jpg,https://oleks-netizen.github.io/product-images/14607/3.jpg,https://oleks-netizen.github.io/product-images/14607/4.jpg,https://oleks-netizen.github.io/product-images/14607/5.jpg,https://oleks-netizen.github.io/product-images/14607/6.jpg,https://oleks-netizen.github.io/product-images/14607/7.jpg,https://oleks-netizen.github.io/product-images/14607/8.jpg,https://oleks-netizen.github.io/product-images/14607/9.jpg</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>L87454-01</t>
+          <t>14609</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L87454-01/1.jpg,https://oleks-netizen.github.io/product-images/L87454-01/2.jpg,https://oleks-netizen.github.io/product-images/L87454-01/7.jpg,https://oleks-netizen.github.io/product-images/L87454-01/4.jpg,https://oleks-netizen.github.io/product-images/L87454-01/5.jpg,https://oleks-netizen.github.io/product-images/L87454-01/6.jpg,https://oleks-netizen.github.io/product-images/L87454-01/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14609/1.jpg,https://oleks-netizen.github.io/product-images/14609/2.jpg,https://oleks-netizen.github.io/product-images/14609/5.jpg,https://oleks-netizen.github.io/product-images/14609/9.jpg,https://oleks-netizen.github.io/product-images/14609/3.jpg,https://oleks-netizen.github.io/product-images/14609/4.jpg,https://oleks-netizen.github.io/product-images/14609/7.jpg,https://oleks-netizen.github.io/product-images/14609/8.jpg</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>L87454-06</t>
+          <t>14615</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L87454-06/1.jpg,https://oleks-netizen.github.io/product-images/L87454-06/2.jpg,https://oleks-netizen.github.io/product-images/L87454-06/10.jpg,https://oleks-netizen.github.io/product-images/L87454-06/4.jpg,https://oleks-netizen.github.io/product-images/L87454-06/5.jpg,https://oleks-netizen.github.io/product-images/L87454-06/6.jpg,https://oleks-netizen.github.io/product-images/L87454-06/7.jpg,https://oleks-netizen.github.io/product-images/L87454-06/8.jpg,https://oleks-netizen.github.io/product-images/L87454-06/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14615/1.jpg,https://oleks-netizen.github.io/product-images/14615/2.jpg,https://oleks-netizen.github.io/product-images/14615/5.jpg,https://oleks-netizen.github.io/product-images/14615/8.jpg,https://oleks-netizen.github.io/product-images/14615/3.jpg,https://oleks-netizen.github.io/product-images/14615/4.jpg,https://oleks-netizen.github.io/product-images/14615/6.jpg</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>L87454-81</t>
+          <t>14627</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L87454-81/1.jpg,https://oleks-netizen.github.io/product-images/L87454-81/2.jpg,https://oleks-netizen.github.io/product-images/L87454-81/10.jpg,https://oleks-netizen.github.io/product-images/L87454-81/4.jpg,https://oleks-netizen.github.io/product-images/L87454-81/5.jpg,https://oleks-netizen.github.io/product-images/L87454-81/6.jpg,https://oleks-netizen.github.io/product-images/L87454-81/7.jpg,https://oleks-netizen.github.io/product-images/L87454-81/8.jpg,https://oleks-netizen.github.io/product-images/L87454-81/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14627/1.jpg,https://oleks-netizen.github.io/product-images/14627/2.jpg,https://oleks-netizen.github.io/product-images/14627/6.jpg,https://oleks-netizen.github.io/product-images/14627/9.jpg,https://oleks-netizen.github.io/product-images/14627/3.jpg,https://oleks-netizen.github.io/product-images/14627/4.jpg,https://oleks-netizen.github.io/product-images/14627/5.jpg,https://oleks-netizen.github.io/product-images/14627/8.jpg</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>L87598-01</t>
+          <t>14645</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L87598-01/1.jpg,https://oleks-netizen.github.io/product-images/L87598-01/2.jpg,https://oleks-netizen.github.io/product-images/L87598-01/10.jpg,https://oleks-netizen.github.io/product-images/L87598-01/4.jpg,https://oleks-netizen.github.io/product-images/L87598-01/5.jpg,https://oleks-netizen.github.io/product-images/L87598-01/6.jpg,https://oleks-netizen.github.io/product-images/L87598-01/7.jpg,https://oleks-netizen.github.io/product-images/L87598-01/8.jpg,https://oleks-netizen.github.io/product-images/L87598-01/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14645/1.jpg,https://oleks-netizen.github.io/product-images/14645/2.jpg,https://oleks-netizen.github.io/product-images/14645/7.jpg,https://oleks-netizen.github.io/product-images/14645/3.jpg,https://oleks-netizen.github.io/product-images/14645/4.jpg,https://oleks-netizen.github.io/product-images/14645/5.jpg</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>L87598-13</t>
+          <t>14648</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L87598-13/1.jpg,https://oleks-netizen.github.io/product-images/L87598-13/2.jpg,https://oleks-netizen.github.io/product-images/L87598-13/3.jpg,https://oleks-netizen.github.io/product-images/L87598-13/10.jpg,https://oleks-netizen.github.io/product-images/L87598-13/5.jpg,https://oleks-netizen.github.io/product-images/L87598-13/6.jpg,https://oleks-netizen.github.io/product-images/L87598-13/7.jpg,https://oleks-netizen.github.io/product-images/L87598-13/8.jpg,https://oleks-netizen.github.io/product-images/L87598-13/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14648/1.jpg,https://oleks-netizen.github.io/product-images/14648/2.jpg,https://oleks-netizen.github.io/product-images/14648/4.jpg,https://oleks-netizen.github.io/product-images/14648/12.jpg,https://oleks-netizen.github.io/product-images/14648/11.jpg,https://oleks-netizen.github.io/product-images/14648/3.jpg,https://oleks-netizen.github.io/product-images/14648/5.jpg,https://oleks-netizen.github.io/product-images/14648/6.jpg,https://oleks-netizen.github.io/product-images/14648/7.jpg,https://oleks-netizen.github.io/product-images/14648/8.jpg,https://oleks-netizen.github.io/product-images/14648/9.jpg</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>L87598-23</t>
+          <t>14680</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L87598-23/1.jpg,https://oleks-netizen.github.io/product-images/L87598-23/2.jpg,https://oleks-netizen.github.io/product-images/L87598-23/3.jpg,https://oleks-netizen.github.io/product-images/L87598-23/10.jpg,https://oleks-netizen.github.io/product-images/L87598-23/5.jpg,https://oleks-netizen.github.io/product-images/L87598-23/6.jpg,https://oleks-netizen.github.io/product-images/L87598-23/7.jpg,https://oleks-netizen.github.io/product-images/L87598-23/8.jpg,https://oleks-netizen.github.io/product-images/L87598-23/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14680/1.jpg,https://oleks-netizen.github.io/product-images/14680/2.jpg,https://oleks-netizen.github.io/product-images/14680/23.jpg,https://oleks-netizen.github.io/product-images/14680/10.jpg,https://oleks-netizen.github.io/product-images/14680/11.jpg,https://oleks-netizen.github.io/product-images/14680/12.jpg,https://oleks-netizen.github.io/product-images/14680/13.jpg,https://oleks-netizen.github.io/product-images/14680/14.jpg,https://oleks-netizen.github.io/product-images/14680/15.jpg,https://oleks-netizen.github.io/product-images/14680/16.jpg,https://oleks-netizen.github.io/product-images/14680/17.jpg,https://oleks-netizen.github.io/product-images/14680/18.jpg,https://oleks-netizen.github.io/product-images/14680/19.jpg,https://oleks-netizen.github.io/product-images/14680/20.jpg,https://oleks-netizen.github.io/product-images/14680/21.jpg,https://oleks-netizen.github.io/product-images/14680/22.jpg,https://oleks-netizen.github.io/product-images/14680/3.jpg,https://oleks-netizen.github.io/product-images/14680/4.jpg,https://oleks-netizen.github.io/product-images/14680/6.jpg,https://oleks-netizen.github.io/product-images/14680/7.jpg,https://oleks-netizen.github.io/product-images/14680/8.jpg,https://oleks-netizen.github.io/product-images/14680/9.jpg</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>L87598-31</t>
+          <t>14681</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L87598-31/1.jpg,https://oleks-netizen.github.io/product-images/L87598-31/2.jpg,https://oleks-netizen.github.io/product-images/L87598-31/3.jpg,https://oleks-netizen.github.io/product-images/L87598-31/10.jpg,https://oleks-netizen.github.io/product-images/L87598-31/5.jpg,https://oleks-netizen.github.io/product-images/L87598-31/6.jpg,https://oleks-netizen.github.io/product-images/L87598-31/7.jpg,https://oleks-netizen.github.io/product-images/L87598-31/8.jpg,https://oleks-netizen.github.io/product-images/L87598-31/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14681/1.jpg,https://oleks-netizen.github.io/product-images/14681/2.jpg,https://oleks-netizen.github.io/product-images/14681/15.jpg,https://oleks-netizen.github.io/product-images/14681/10.jpg,https://oleks-netizen.github.io/product-images/14681/11.jpg,https://oleks-netizen.github.io/product-images/14681/12.jpg,https://oleks-netizen.github.io/product-images/14681/13.jpg,https://oleks-netizen.github.io/product-images/14681/3.jpg,https://oleks-netizen.github.io/product-images/14681/4.jpg,https://oleks-netizen.github.io/product-images/14681/5.jpg,https://oleks-netizen.github.io/product-images/14681/6.jpg,https://oleks-netizen.github.io/product-images/14681/7.jpg,https://oleks-netizen.github.io/product-images/14681/8.jpg,https://oleks-netizen.github.io/product-images/14681/9.jpg</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>L87640-01</t>
+          <t>14682</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L87640-01/1.jpg,https://oleks-netizen.github.io/product-images/L87640-01/2.jpg,https://oleks-netizen.github.io/product-images/L87640-01/3.jpg,https://oleks-netizen.github.io/product-images/L87640-01/6.jpg,https://oleks-netizen.github.io/product-images/L87640-01/5.jpg,https://oleks-netizen.github.io/product-images/L87640-01/7.jpg,https://oleks-netizen.github.io/product-images/L87640-01/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14682/1.jpg,https://oleks-netizen.github.io/product-images/14682/2.jpg,https://oleks-netizen.github.io/product-images/14682/24.jpg,https://oleks-netizen.github.io/product-images/14682/10.jpg,https://oleks-netizen.github.io/product-images/14682/11.jpg,https://oleks-netizen.github.io/product-images/14682/12.jpg,https://oleks-netizen.github.io/product-images/14682/13.jpg,https://oleks-netizen.github.io/product-images/14682/14.jpg,https://oleks-netizen.github.io/product-images/14682/15.jpg,https://oleks-netizen.github.io/product-images/14682/17.jpg,https://oleks-netizen.github.io/product-images/14682/18.jpg,https://oleks-netizen.github.io/product-images/14682/19.jpg,https://oleks-netizen.github.io/product-images/14682/20.jpg,https://oleks-netizen.github.io/product-images/14682/21.jpg,https://oleks-netizen.github.io/product-images/14682/22.jpg,https://oleks-netizen.github.io/product-images/14682/23.jpg,https://oleks-netizen.github.io/product-images/14682/3.jpg,https://oleks-netizen.github.io/product-images/14682/4.jpg,https://oleks-netizen.github.io/product-images/14682/5.jpg,https://oleks-netizen.github.io/product-images/14682/6.jpg,https://oleks-netizen.github.io/product-images/14682/7.jpg,https://oleks-netizen.github.io/product-images/14682/8.jpg,https://oleks-netizen.github.io/product-images/14682/9.jpg</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>7</v>
+        <v>23</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>L87640-130</t>
+          <t>14683</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L87640-130/1.jpg,https://oleks-netizen.github.io/product-images/L87640-130/2.jpg,https://oleks-netizen.github.io/product-images/L87640-130/3.jpg,https://oleks-netizen.github.io/product-images/L87640-130/4.jpg,https://oleks-netizen.github.io/product-images/L87640-130/5.jpg,https://oleks-netizen.github.io/product-images/L87640-130/6.jpg,https://oleks-netizen.github.io/product-images/L87640-130/7.jpg,https://oleks-netizen.github.io/product-images/L87640-130/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14683/1.jpg,https://oleks-netizen.github.io/product-images/14683/2.jpg,https://oleks-netizen.github.io/product-images/14683/8.jpg,https://oleks-netizen.github.io/product-images/14683/3.jpg,https://oleks-netizen.github.io/product-images/14683/4.jpg,https://oleks-netizen.github.io/product-images/14683/5.jpg,https://oleks-netizen.github.io/product-images/14683/7.jpg</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>L87640-246</t>
+          <t>14686</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L87640-246/1.jpg,https://oleks-netizen.github.io/product-images/L87640-246/2.jpg,https://oleks-netizen.github.io/product-images/L87640-246/9.jpg,https://oleks-netizen.github.io/product-images/L87640-246/4.jpg,https://oleks-netizen.github.io/product-images/L87640-246/5.jpg,https://oleks-netizen.github.io/product-images/L87640-246/6.jpg,https://oleks-netizen.github.io/product-images/L87640-246/7.jpg,https://oleks-netizen.github.io/product-images/L87640-246/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14686/1.jpg,https://oleks-netizen.github.io/product-images/14686/2.jpg,https://oleks-netizen.github.io/product-images/14686/14.jpg,https://oleks-netizen.github.io/product-images/14686/10.jpg,https://oleks-netizen.github.io/product-images/14686/11.jpg,https://oleks-netizen.github.io/product-images/14686/13.jpg,https://oleks-netizen.github.io/product-images/14686/3.jpg,https://oleks-netizen.github.io/product-images/14686/4.jpg,https://oleks-netizen.github.io/product-images/14686/5.jpg,https://oleks-netizen.github.io/product-images/14686/6.jpg,https://oleks-netizen.github.io/product-images/14686/7.jpg,https://oleks-netizen.github.io/product-images/14686/8.jpg,https://oleks-netizen.github.io/product-images/14686/9.jpg</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>L87640-36</t>
+          <t>14687</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L87640-36/1.jpg,https://oleks-netizen.github.io/product-images/L87640-36/2.jpg,https://oleks-netizen.github.io/product-images/L87640-36/9.jpg,https://oleks-netizen.github.io/product-images/L87640-36/4.jpg,https://oleks-netizen.github.io/product-images/L87640-36/5.jpg,https://oleks-netizen.github.io/product-images/L87640-36/6.jpg,https://oleks-netizen.github.io/product-images/L87640-36/7.jpg,https://oleks-netizen.github.io/product-images/L87640-36/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14687/1.jpg,https://oleks-netizen.github.io/product-images/14687/2.jpg,https://oleks-netizen.github.io/product-images/14687/3.jpg,https://oleks-netizen.github.io/product-images/14687/17.jpg,https://oleks-netizen.github.io/product-images/14687/10.jpg,https://oleks-netizen.github.io/product-images/14687/11.jpg,https://oleks-netizen.github.io/product-images/14687/12.jpg,https://oleks-netizen.github.io/product-images/14687/13.jpg,https://oleks-netizen.github.io/product-images/14687/15.jpg,https://oleks-netizen.github.io/product-images/14687/16.jpg,https://oleks-netizen.github.io/product-images/14687/4.jpg,https://oleks-netizen.github.io/product-images/14687/5.jpg,https://oleks-netizen.github.io/product-images/14687/6.jpg,https://oleks-netizen.github.io/product-images/14687/7.jpg,https://oleks-netizen.github.io/product-images/14687/8.jpg,https://oleks-netizen.github.io/product-images/14687/9.jpg</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>LC46019-1</t>
+          <t>14689</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC46019-1/1.jpg,https://oleks-netizen.github.io/product-images/LC46019-1/2.jpg,https://oleks-netizen.github.io/product-images/LC46019-1/3.jpg,https://oleks-netizen.github.io/product-images/LC46019-1/4.jpg,https://oleks-netizen.github.io/product-images/LC46019-1/5.jpg,https://oleks-netizen.github.io/product-images/LC46019-1/6.jpg,https://oleks-netizen.github.io/product-images/LC46019-1/7.jpg,https://oleks-netizen.github.io/product-images/LC46019-1/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14689/1.jpg,https://oleks-netizen.github.io/product-images/14689/2.jpg,https://oleks-netizen.github.io/product-images/14689/9.jpg,https://oleks-netizen.github.io/product-images/14689/4.jpg,https://oleks-netizen.github.io/product-images/14689/5.jpg,https://oleks-netizen.github.io/product-images/14689/6.jpg,https://oleks-netizen.github.io/product-images/14689/7.jpg,https://oleks-netizen.github.io/product-images/14689/8.jpg</t>
         </is>
       </c>
       <c r="C114" t="n">
@@ -2136,27 +2136,27 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>LC46058-1</t>
+          <t>14752</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC46058-1/1.jpg,https://oleks-netizen.github.io/product-images/LC46058-1/2.jpg,https://oleks-netizen.github.io/product-images/LC46058-1/10.jpg,https://oleks-netizen.github.io/product-images/LC46058-1/4.jpg,https://oleks-netizen.github.io/product-images/LC46058-1/5.jpg,https://oleks-netizen.github.io/product-images/LC46058-1/6.jpg,https://oleks-netizen.github.io/product-images/LC46058-1/7.jpg,https://oleks-netizen.github.io/product-images/LC46058-1/8.jpg,https://oleks-netizen.github.io/product-images/LC46058-1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14752/1.jpg,https://oleks-netizen.github.io/product-images/14752/2.jpg,https://oleks-netizen.github.io/product-images/14752/11.jpg,https://oleks-netizen.github.io/product-images/14752/14.jpg,https://oleks-netizen.github.io/product-images/14752/12.jpg,https://oleks-netizen.github.io/product-images/14752/13.jpg,https://oleks-netizen.github.io/product-images/14752/3.jpg,https://oleks-netizen.github.io/product-images/14752/4.jpg,https://oleks-netizen.github.io/product-images/14752/5.jpg,https://oleks-netizen.github.io/product-images/14752/6.jpg,https://oleks-netizen.github.io/product-images/14752/7.jpg,https://oleks-netizen.github.io/product-images/14752/8.jpg,https://oleks-netizen.github.io/product-images/14752/9.jpg</t>
         </is>
       </c>
       <c r="C115" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>LC46058-2</t>
+          <t>14776</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC46058-2/1.jpg,https://oleks-netizen.github.io/product-images/LC46058-2/2.jpg,https://oleks-netizen.github.io/product-images/LC46058-2/9.jpg,https://oleks-netizen.github.io/product-images/LC46058-2/4.jpg,https://oleks-netizen.github.io/product-images/LC46058-2/5.jpg,https://oleks-netizen.github.io/product-images/LC46058-2/6.jpg,https://oleks-netizen.github.io/product-images/LC46058-2/7.jpg,https://oleks-netizen.github.io/product-images/LC46058-2/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14776/1.jpg,https://oleks-netizen.github.io/product-images/14776/2.jpg,https://oleks-netizen.github.io/product-images/14776/9.jpg,https://oleks-netizen.github.io/product-images/14776/3.jpg,https://oleks-netizen.github.io/product-images/14776/4.jpg,https://oleks-netizen.github.io/product-images/14776/5.jpg,https://oleks-netizen.github.io/product-images/14776/6.jpg,https://oleks-netizen.github.io/product-images/14776/7.jpg</t>
         </is>
       </c>
       <c r="C116" t="n">
@@ -2166,342 +2166,342 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>LC46116-1</t>
+          <t>14779</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC46116-1/1.jpg,https://oleks-netizen.github.io/product-images/LC46116-1/2.jpg,https://oleks-netizen.github.io/product-images/LC46116-1/8.jpg,https://oleks-netizen.github.io/product-images/LC46116-1/4.jpg,https://oleks-netizen.github.io/product-images/LC46116-1/5.jpg,https://oleks-netizen.github.io/product-images/LC46116-1/6.jpg,https://oleks-netizen.github.io/product-images/LC46116-1/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14779/1.jpg,https://oleks-netizen.github.io/product-images/14779/2.jpg,https://oleks-netizen.github.io/product-images/14779/9.jpg,https://oleks-netizen.github.io/product-images/14779/3.jpg,https://oleks-netizen.github.io/product-images/14779/4.jpg,https://oleks-netizen.github.io/product-images/14779/5.jpg,https://oleks-netizen.github.io/product-images/14779/6.jpg,https://oleks-netizen.github.io/product-images/14779/8.jpg</t>
         </is>
       </c>
       <c r="C117" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>LC46118-1</t>
+          <t>14893</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC46118-1/1.jpg,https://oleks-netizen.github.io/product-images/LC46118-1/2.jpg,https://oleks-netizen.github.io/product-images/LC46118-1/3.jpg,https://oleks-netizen.github.io/product-images/LC46118-1/4.jpg,https://oleks-netizen.github.io/product-images/LC46118-1/5.jpg,https://oleks-netizen.github.io/product-images/LC46118-1/6.jpg,https://oleks-netizen.github.io/product-images/LC46118-1/7.jpg,https://oleks-netizen.github.io/product-images/LC46118-1/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14893/1.jpg,https://oleks-netizen.github.io/product-images/14893/2.jpg,https://oleks-netizen.github.io/product-images/14893/10.jpg,https://oleks-netizen.github.io/product-images/14893/3.jpg,https://oleks-netizen.github.io/product-images/14893/4.jpg,https://oleks-netizen.github.io/product-images/14893/5.jpg,https://oleks-netizen.github.io/product-images/14893/6.jpg,https://oleks-netizen.github.io/product-images/14893/8.jpg,https://oleks-netizen.github.io/product-images/14893/9.jpg</t>
         </is>
       </c>
       <c r="C118" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>LC46235-1</t>
+          <t>14894</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC46235-1/1.jpg,https://oleks-netizen.github.io/product-images/LC46235-1/2.jpg,https://oleks-netizen.github.io/product-images/LC46235-1/10.jpg,https://oleks-netizen.github.io/product-images/LC46235-1/3.jpg,https://oleks-netizen.github.io/product-images/LC46235-1/5.jpg,https://oleks-netizen.github.io/product-images/LC46235-1/6.jpg,https://oleks-netizen.github.io/product-images/LC46235-1/7.jpg,https://oleks-netizen.github.io/product-images/LC46235-1/8.jpg,https://oleks-netizen.github.io/product-images/LC46235-1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14894/1.jpg,https://oleks-netizen.github.io/product-images/14894/2.jpg,https://oleks-netizen.github.io/product-images/14894/10.jpg,https://oleks-netizen.github.io/product-images/14894/11.jpg,https://oleks-netizen.github.io/product-images/14894/12.jpg,https://oleks-netizen.github.io/product-images/14894/13.jpg,https://oleks-netizen.github.io/product-images/14894/3.jpg,https://oleks-netizen.github.io/product-images/14894/4.jpg,https://oleks-netizen.github.io/product-images/14894/5.jpg,https://oleks-netizen.github.io/product-images/14894/6.jpg,https://oleks-netizen.github.io/product-images/14894/7.jpg,https://oleks-netizen.github.io/product-images/14894/8.jpg,https://oleks-netizen.github.io/product-images/14894/9.jpg</t>
         </is>
       </c>
       <c r="C119" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>LC46245-1</t>
+          <t>14906</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC46245-1/1.jpg,https://oleks-netizen.github.io/product-images/LC46245-1/2.jpg,https://oleks-netizen.github.io/product-images/LC46245-1/3.jpg,https://oleks-netizen.github.io/product-images/LC46245-1/4.jpg,https://oleks-netizen.github.io/product-images/LC46245-1/5.jpg,https://oleks-netizen.github.io/product-images/LC46245-1/6.jpg,https://oleks-netizen.github.io/product-images/LC46245-1/7.jpg,https://oleks-netizen.github.io/product-images/LC46245-1/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14906/1.jpg,https://oleks-netizen.github.io/product-images/14906/2.jpg,https://oleks-netizen.github.io/product-images/14906/3.jpg,https://oleks-netizen.github.io/product-images/14906/4.jpg,https://oleks-netizen.github.io/product-images/14906/5.jpg,https://oleks-netizen.github.io/product-images/14906/6.jpg,https://oleks-netizen.github.io/product-images/14906/7.jpg</t>
         </is>
       </c>
       <c r="C120" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>LC46523-1</t>
+          <t>14911</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC46523-1/1.jpg,https://oleks-netizen.github.io/product-images/LC46523-1/2.jpg,https://oleks-netizen.github.io/product-images/LC46523-1/3.jpg,https://oleks-netizen.github.io/product-images/LC46523-1/4.jpg,https://oleks-netizen.github.io/product-images/LC46523-1/5.jpg,https://oleks-netizen.github.io/product-images/LC46523-1/6.jpg,https://oleks-netizen.github.io/product-images/LC46523-1/7.jpg,https://oleks-netizen.github.io/product-images/LC46523-1/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14911/1.jpg,https://oleks-netizen.github.io/product-images/14911/2.jpg,https://oleks-netizen.github.io/product-images/14911/7.jpg,https://oleks-netizen.github.io/product-images/14911/14.jpg,https://oleks-netizen.github.io/product-images/14911/10.jpg,https://oleks-netizen.github.io/product-images/14911/11.jpg,https://oleks-netizen.github.io/product-images/14911/12.jpg,https://oleks-netizen.github.io/product-images/14911/13.jpg,https://oleks-netizen.github.io/product-images/14911/3.jpg,https://oleks-netizen.github.io/product-images/14911/4.jpg,https://oleks-netizen.github.io/product-images/14911/5.jpg,https://oleks-netizen.github.io/product-images/14911/6.jpg,https://oleks-netizen.github.io/product-images/14911/8.jpg</t>
         </is>
       </c>
       <c r="C121" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>LC46655-1</t>
+          <t>14912</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC46655-1/1.jpg,https://oleks-netizen.github.io/product-images/LC46655-1/2.jpg,https://oleks-netizen.github.io/product-images/LC46655-1/3.jpg,https://oleks-netizen.github.io/product-images/LC46655-1/4.jpg,https://oleks-netizen.github.io/product-images/LC46655-1/5.jpg,https://oleks-netizen.github.io/product-images/LC46655-1/6.jpg,https://oleks-netizen.github.io/product-images/LC46655-1/7.jpg,https://oleks-netizen.github.io/product-images/LC46655-1/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14912/1.jpg,https://oleks-netizen.github.io/product-images/14912/2.jpg,https://oleks-netizen.github.io/product-images/14912/9.jpg,https://oleks-netizen.github.io/product-images/14912/14.jpg,https://oleks-netizen.github.io/product-images/14912/10.jpg,https://oleks-netizen.github.io/product-images/14912/11.jpg,https://oleks-netizen.github.io/product-images/14912/12.jpg,https://oleks-netizen.github.io/product-images/14912/3.jpg,https://oleks-netizen.github.io/product-images/14912/4.jpg,https://oleks-netizen.github.io/product-images/14912/5.jpg,https://oleks-netizen.github.io/product-images/14912/6.jpg,https://oleks-netizen.github.io/product-images/14912/7.jpg,https://oleks-netizen.github.io/product-images/14912/8.jpg</t>
         </is>
       </c>
       <c r="C122" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>LC46655-2</t>
+          <t>14913</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC46655-2/1.jpg,https://oleks-netizen.github.io/product-images/LC46655-2/2.jpg,https://oleks-netizen.github.io/product-images/LC46655-2/9.jpg,https://oleks-netizen.github.io/product-images/LC46655-2/4.jpg,https://oleks-netizen.github.io/product-images/LC46655-2/5.jpg,https://oleks-netizen.github.io/product-images/LC46655-2/6.jpg,https://oleks-netizen.github.io/product-images/LC46655-2/7.jpg,https://oleks-netizen.github.io/product-images/LC46655-2/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14913/1.jpg,https://oleks-netizen.github.io/product-images/14913/2.jpg,https://oleks-netizen.github.io/product-images/14913/3.jpg,https://oleks-netizen.github.io/product-images/14913/15.jpg,https://oleks-netizen.github.io/product-images/14913/10.jpg,https://oleks-netizen.github.io/product-images/14913/12.jpg,https://oleks-netizen.github.io/product-images/14913/13.jpg,https://oleks-netizen.github.io/product-images/14913/14.jpg,https://oleks-netizen.github.io/product-images/14913/4.jpg,https://oleks-netizen.github.io/product-images/14913/5.jpg,https://oleks-netizen.github.io/product-images/14913/6.jpg,https://oleks-netizen.github.io/product-images/14913/7.jpg,https://oleks-netizen.github.io/product-images/14913/8.jpg,https://oleks-netizen.github.io/product-images/14913/9.jpg</t>
         </is>
       </c>
       <c r="C123" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>LC46921-1</t>
+          <t>14916</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC46921-1/1.jpg,https://oleks-netizen.github.io/product-images/LC46921-1/2.jpg,https://oleks-netizen.github.io/product-images/LC46921-1/3.jpg,https://oleks-netizen.github.io/product-images/LC46921-1/4.jpg,https://oleks-netizen.github.io/product-images/LC46921-1/5.jpg,https://oleks-netizen.github.io/product-images/LC46921-1/6.jpg,https://oleks-netizen.github.io/product-images/LC46921-1/7.jpg,https://oleks-netizen.github.io/product-images/LC46921-1/8.jpg,https://oleks-netizen.github.io/product-images/LC46921-1/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14916/1.jpg,https://oleks-netizen.github.io/product-images/14916/2.jpg,https://oleks-netizen.github.io/product-images/14916/3.jpg,https://oleks-netizen.github.io/product-images/14916/11.jpg,https://oleks-netizen.github.io/product-images/14916/10.jpg,https://oleks-netizen.github.io/product-images/14916/4.jpg,https://oleks-netizen.github.io/product-images/14916/5.jpg,https://oleks-netizen.github.io/product-images/14916/7.jpg,https://oleks-netizen.github.io/product-images/14916/8.jpg,https://oleks-netizen.github.io/product-images/14916/9.jpg</t>
         </is>
       </c>
       <c r="C124" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>LC46921-2</t>
+          <t>14917</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC46921-2/1.jpg,https://oleks-netizen.github.io/product-images/LC46921-2/2.jpg,https://oleks-netizen.github.io/product-images/LC46921-2/3.jpg,https://oleks-netizen.github.io/product-images/LC46921-2/4.jpg,https://oleks-netizen.github.io/product-images/LC46921-2/5.jpg,https://oleks-netizen.github.io/product-images/LC46921-2/6.jpg,https://oleks-netizen.github.io/product-images/LC46921-2/7.jpg,https://oleks-netizen.github.io/product-images/LC46921-2/8.jpg,https://oleks-netizen.github.io/product-images/LC46921-2/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14917/1.jpg,https://oleks-netizen.github.io/product-images/14917/2.jpg,https://oleks-netizen.github.io/product-images/14917/6.jpg,https://oleks-netizen.github.io/product-images/14917/14.jpg,https://oleks-netizen.github.io/product-images/14917/11.jpg,https://oleks-netizen.github.io/product-images/14917/12.jpg,https://oleks-netizen.github.io/product-images/14917/13.jpg,https://oleks-netizen.github.io/product-images/14917/3.jpg,https://oleks-netizen.github.io/product-images/14917/4.jpg,https://oleks-netizen.github.io/product-images/14917/5.jpg,https://oleks-netizen.github.io/product-images/14917/7.jpg,https://oleks-netizen.github.io/product-images/14917/8.jpg,https://oleks-netizen.github.io/product-images/14917/9.jpg</t>
         </is>
       </c>
       <c r="C125" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>LC46931-1</t>
+          <t>14918</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC46931-1/1.jpg,https://oleks-netizen.github.io/product-images/LC46931-1/2.jpg,https://oleks-netizen.github.io/product-images/LC46931-1/8.jpg,https://oleks-netizen.github.io/product-images/LC46931-1/4.jpg,https://oleks-netizen.github.io/product-images/LC46931-1/5.jpg,https://oleks-netizen.github.io/product-images/LC46931-1/6.jpg,https://oleks-netizen.github.io/product-images/LC46931-1/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14918/1.jpg,https://oleks-netizen.github.io/product-images/14918/2.jpg,https://oleks-netizen.github.io/product-images/14918/5.jpg,https://oleks-netizen.github.io/product-images/14918/9.jpg,https://oleks-netizen.github.io/product-images/14918/3.jpg,https://oleks-netizen.github.io/product-images/14918/4.jpg,https://oleks-netizen.github.io/product-images/14918/7.jpg,https://oleks-netizen.github.io/product-images/14918/8.jpg</t>
         </is>
       </c>
       <c r="C126" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>LC46931-2</t>
+          <t>14919</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC46931-2/1.jpg,https://oleks-netizen.github.io/product-images/LC46931-2/2.jpg,https://oleks-netizen.github.io/product-images/LC46931-2/3.jpg,https://oleks-netizen.github.io/product-images/LC46931-2/4.jpg,https://oleks-netizen.github.io/product-images/LC46931-2/5.jpg,https://oleks-netizen.github.io/product-images/LC46931-2/6.jpg,https://oleks-netizen.github.io/product-images/LC46931-2/7.jpg,https://oleks-netizen.github.io/product-images/LC46931-2/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14919/1.jpg,https://oleks-netizen.github.io/product-images/14919/2.jpg,https://oleks-netizen.github.io/product-images/14919/5.jpg,https://oleks-netizen.github.io/product-images/14919/4.jpg</t>
         </is>
       </c>
       <c r="C127" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>LC89008-H1</t>
+          <t>14923</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/LC89008-H1/1.jpg,https://oleks-netizen.github.io/product-images/LC89008-H1/2.jpg,https://oleks-netizen.github.io/product-images/LC89008-H1/7.jpg,https://oleks-netizen.github.io/product-images/LC89008-H1/4.jpg,https://oleks-netizen.github.io/product-images/LC89008-H1/5.jpg,https://oleks-netizen.github.io/product-images/LC89008-H1/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14923/1.jpg,https://oleks-netizen.github.io/product-images/14923/2.jpg,https://oleks-netizen.github.io/product-images/14923/3.jpg,https://oleks-netizen.github.io/product-images/14923/4.jpg,https://oleks-netizen.github.io/product-images/14923/5.jpg,https://oleks-netizen.github.io/product-images/14923/6.jpg,https://oleks-netizen.github.io/product-images/14923/7.jpg,https://oleks-netizen.github.io/product-images/14923/8.jpg</t>
         </is>
       </c>
       <c r="C128" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>lim-354RAw</t>
+          <t>14924</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/lim-354RAw/1.jpg,https://oleks-netizen.github.io/product-images/lim-354RAw/2.jpg,https://oleks-netizen.github.io/product-images/lim-354RAw/5.jpg,https://oleks-netizen.github.io/product-images/lim-354RAw/6.jpg,https://oleks-netizen.github.io/product-images/lim-354RAw/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14924/1.jpg,https://oleks-netizen.github.io/product-images/14924/2.jpg,https://oleks-netizen.github.io/product-images/14924/9.jpg,https://oleks-netizen.github.io/product-images/14924/10.jpg,https://oleks-netizen.github.io/product-images/14924/3.jpg,https://oleks-netizen.github.io/product-images/14924/4.jpg,https://oleks-netizen.github.io/product-images/14924/6.jpg,https://oleks-netizen.github.io/product-images/14924/7.jpg,https://oleks-netizen.github.io/product-images/14924/8.jpg</t>
         </is>
       </c>
       <c r="C129" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>NB040A</t>
+          <t>14925</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/NB040A/1.jpg,https://oleks-netizen.github.io/product-images/NB040A/2.jpg,https://oleks-netizen.github.io/product-images/NB040A/6.jpg,https://oleks-netizen.github.io/product-images/NB040A/4.jpg,https://oleks-netizen.github.io/product-images/NB040A/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14925/1.jpg,https://oleks-netizen.github.io/product-images/14925/2.jpg,https://oleks-netizen.github.io/product-images/14925/8.jpg,https://oleks-netizen.github.io/product-images/14925/10.jpg,https://oleks-netizen.github.io/product-images/14925/3.jpg,https://oleks-netizen.github.io/product-images/14925/4.jpg,https://oleks-netizen.github.io/product-images/14925/5.jpg,https://oleks-netizen.github.io/product-images/14925/6.jpg,https://oleks-netizen.github.io/product-images/14925/9.jpg</t>
         </is>
       </c>
       <c r="C130" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>NB040B</t>
+          <t>14926</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/NB040B/1.jpg,https://oleks-netizen.github.io/product-images/NB040B/2.jpg,https://oleks-netizen.github.io/product-images/NB040B/6.jpg,https://oleks-netizen.github.io/product-images/NB040B/3.jpg,https://oleks-netizen.github.io/product-images/NB040B/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14926/1.jpg,https://oleks-netizen.github.io/product-images/14926/2.jpg,https://oleks-netizen.github.io/product-images/14926/9.jpg,https://oleks-netizen.github.io/product-images/14926/3.jpg,https://oleks-netizen.github.io/product-images/14926/4.jpg,https://oleks-netizen.github.io/product-images/14926/6.jpg,https://oleks-netizen.github.io/product-images/14926/7.jpg,https://oleks-netizen.github.io/product-images/14926/8.jpg</t>
         </is>
       </c>
       <c r="C131" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>NB040C</t>
+          <t>14927</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/NB040C/1.jpg,https://oleks-netizen.github.io/product-images/NB040C/2.jpg,https://oleks-netizen.github.io/product-images/NB040C/3.jpg,https://oleks-netizen.github.io/product-images/NB040C/6.jpg,https://oleks-netizen.github.io/product-images/NB040C/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14927/1.jpg,https://oleks-netizen.github.io/product-images/14927/2.jpg,https://oleks-netizen.github.io/product-images/14927/9.jpg,https://oleks-netizen.github.io/product-images/14927/12.jpg,https://oleks-netizen.github.io/product-images/14927/11.jpg,https://oleks-netizen.github.io/product-images/14927/3.jpg,https://oleks-netizen.github.io/product-images/14927/4.jpg,https://oleks-netizen.github.io/product-images/14927/5.jpg,https://oleks-netizen.github.io/product-images/14927/6.jpg,https://oleks-netizen.github.io/product-images/14927/7.jpg,https://oleks-netizen.github.io/product-images/14927/8.jpg</t>
         </is>
       </c>
       <c r="C132" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Nevada537moro</t>
+          <t>14934</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/Nevada537moro/1.jpg,https://oleks-netizen.github.io/product-images/Nevada537moro/2.jpg,https://oleks-netizen.github.io/product-images/Nevada537moro/3.jpg,https://oleks-netizen.github.io/product-images/Nevada537moro/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14934/1.jpg,https://oleks-netizen.github.io/product-images/14934/2.jpg,https://oleks-netizen.github.io/product-images/14934/14.jpg,https://oleks-netizen.github.io/product-images/14934/10.jpg,https://oleks-netizen.github.io/product-images/14934/11.jpg,https://oleks-netizen.github.io/product-images/14934/12.jpg,https://oleks-netizen.github.io/product-images/14934/13.jpg,https://oleks-netizen.github.io/product-images/14934/3.jpg,https://oleks-netizen.github.io/product-images/14934/4.jpg,https://oleks-netizen.github.io/product-images/14934/5.jpg,https://oleks-netizen.github.io/product-images/14934/6.jpg,https://oleks-netizen.github.io/product-images/14934/7.jpg,https://oleks-netizen.github.io/product-images/14934/8.jpg</t>
         </is>
       </c>
       <c r="C133" t="n">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>NewRainbow1192nero</t>
+          <t>14935</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/NewRainbow1192nero/1.jpg,https://oleks-netizen.github.io/product-images/NewRainbow1192nero/2.jpg,https://oleks-netizen.github.io/product-images/NewRainbow1192nero/7.jpg,https://oleks-netizen.github.io/product-images/NewRainbow1192nero/3.jpg,https://oleks-netizen.github.io/product-images/NewRainbow1192nero/4.jpg,https://oleks-netizen.github.io/product-images/NewRainbow1192nero/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14935/1.jpg,https://oleks-netizen.github.io/product-images/14935/2.jpg,https://oleks-netizen.github.io/product-images/14935/11.jpg,https://oleks-netizen.github.io/product-images/14935/12.jpg,https://oleks-netizen.github.io/product-images/14935/10.jpg,https://oleks-netizen.github.io/product-images/14935/3.jpg,https://oleks-netizen.github.io/product-images/14935/4.jpg,https://oleks-netizen.github.io/product-images/14935/5.jpg,https://oleks-netizen.github.io/product-images/14935/7.jpg,https://oleks-netizen.github.io/product-images/14935/8.jpg,https://oleks-netizen.github.io/product-images/14935/9.jpg</t>
         </is>
       </c>
       <c r="C134" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>NewRainbow3435grigio</t>
+          <t>14963</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/NewRainbow3435grigio/1.jpg,https://oleks-netizen.github.io/product-images/NewRainbow3435grigio/2.jpg,https://oleks-netizen.github.io/product-images/NewRainbow3435grigio/3.jpg,https://oleks-netizen.github.io/product-images/NewRainbow3435grigio/4.jpg,https://oleks-netizen.github.io/product-images/NewRainbow3435grigio/5.jpg,https://oleks-netizen.github.io/product-images/NewRainbow3435grigio/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14963/1.jpg,https://oleks-netizen.github.io/product-images/14963/2.jpg,https://oleks-netizen.github.io/product-images/14963/9.jpg,https://oleks-netizen.github.io/product-images/14963/3.jpg,https://oleks-netizen.github.io/product-images/14963/4.jpg,https://oleks-netizen.github.io/product-images/14963/6.jpg,https://oleks-netizen.github.io/product-images/14963/7.jpg,https://oleks-netizen.github.io/product-images/14963/8.jpg</t>
         </is>
       </c>
       <c r="C135" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>RA-0705-3mdL</t>
+          <t>14964</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RA-0705-3mdL/1.jpg,https://oleks-netizen.github.io/product-images/RA-0705-3mdL/2.jpg,https://oleks-netizen.github.io/product-images/RA-0705-3mdL/8.jpg,https://oleks-netizen.github.io/product-images/RA-0705-3mdL/4.jpg,https://oleks-netizen.github.io/product-images/RA-0705-3mdL/5.jpg,https://oleks-netizen.github.io/product-images/RA-0705-3mdL/6.jpg,https://oleks-netizen.github.io/product-images/RA-0705-3mdL/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14964/1.jpg,https://oleks-netizen.github.io/product-images/14964/2.jpg,https://oleks-netizen.github.io/product-images/14964/3.jpg,https://oleks-netizen.github.io/product-images/14964/4.jpg,https://oleks-netizen.github.io/product-images/14964/5.jpg,https://oleks-netizen.github.io/product-images/14964/6.jpg,https://oleks-netizen.github.io/product-images/14964/7.jpg,https://oleks-netizen.github.io/product-images/14964/8.jpg</t>
         </is>
       </c>
       <c r="C136" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>RA-5729-4sa</t>
+          <t>16134</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RA-5729-4sa/1.jpg,https://oleks-netizen.github.io/product-images/RA-5729-4sa/2.jpg,https://oleks-netizen.github.io/product-images/RA-5729-4sa/8.jpg,https://oleks-netizen.github.io/product-images/RA-5729-4sa/4.jpg,https://oleks-netizen.github.io/product-images/RA-5729-4sa/5.jpg,https://oleks-netizen.github.io/product-images/RA-5729-4sa/6.jpg,https://oleks-netizen.github.io/product-images/RA-5729-4sa/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/16134/1.jpg,https://oleks-netizen.github.io/product-images/16134/2.jpg,https://oleks-netizen.github.io/product-images/16134/6.jpg,https://oleks-netizen.github.io/product-images/16134/4.jpg,https://oleks-netizen.github.io/product-images/16134/5.jpg</t>
         </is>
       </c>
       <c r="C137" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>RB-1304-4lx</t>
+          <t>16142</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RB-1304-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RB-1304-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RB-1304-4lx/6.jpg,https://oleks-netizen.github.io/product-images/RB-1304-4lx/7.jpg,https://oleks-netizen.github.io/product-images/RB-1304-4lx/3.jpg,https://oleks-netizen.github.io/product-images/RB-1304-4lx/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/16142/1.jpg,https://oleks-netizen.github.io/product-images/16142/2.jpg,https://oleks-netizen.github.io/product-images/16142/6.jpg,https://oleks-netizen.github.io/product-images/16142/3.jpg,https://oleks-netizen.github.io/product-images/16142/4.jpg</t>
         </is>
       </c>
       <c r="C138" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>RC-1304-4lx</t>
+          <t>16169</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RC-1304-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RC-1304-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RC-1304-4lx/7.jpg,https://oleks-netizen.github.io/product-images/RC-1304-4lx/3.jpg,https://oleks-netizen.github.io/product-images/RC-1304-4lx/4.jpg,https://oleks-netizen.github.io/product-images/RC-1304-4lx/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/16169/1.jpg,https://oleks-netizen.github.io/product-images/16169/2.jpg,https://oleks-netizen.github.io/product-images/16169/7.jpg,https://oleks-netizen.github.io/product-images/16169/3.jpg,https://oleks-netizen.github.io/product-images/16169/4.jpg,https://oleks-netizen.github.io/product-images/16169/5.jpg</t>
         </is>
       </c>
       <c r="C139" t="n">
@@ -2511,12 +2511,12 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>RC-1502-3md</t>
+          <t>16206</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RC-1502-3md/1.jpg,https://oleks-netizen.github.io/product-images/RC-1502-3md/2.jpg,https://oleks-netizen.github.io/product-images/RC-1502-3md/8.jpg,https://oleks-netizen.github.io/product-images/RC-1502-3md/4.jpg,https://oleks-netizen.github.io/product-images/RC-1502-3md/5.jpg,https://oleks-netizen.github.io/product-images/RC-1502-3md/6.jpg,https://oleks-netizen.github.io/product-images/RC-1502-3md/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/16206/1.jpg,https://oleks-netizen.github.io/product-images/16206/2.jpg,https://oleks-netizen.github.io/product-images/16206/8.jpg,https://oleks-netizen.github.io/product-images/16206/3.jpg,https://oleks-netizen.github.io/product-images/16206/4.jpg,https://oleks-netizen.github.io/product-images/16206/5.jpg,https://oleks-netizen.github.io/product-images/16206/7.jpg</t>
         </is>
       </c>
       <c r="C140" t="n">
@@ -2526,42 +2526,42 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>RC-1504-3md</t>
+          <t>17086</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RC-1504-3md/1.jpg,https://oleks-netizen.github.io/product-images/RC-1504-3md/3.jpg,https://oleks-netizen.github.io/product-images/RC-1504-3md/9.jpg,https://oleks-netizen.github.io/product-images/RC-1504-3md/4.jpg,https://oleks-netizen.github.io/product-images/RC-1504-3md/5.jpg,https://oleks-netizen.github.io/product-images/RC-1504-3md/6.jpg,https://oleks-netizen.github.io/product-images/RC-1504-3md/7.jpg,https://oleks-netizen.github.io/product-images/RC-1504-3md/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/17086/1.jpg,https://oleks-netizen.github.io/product-images/17086/2.jpg,https://oleks-netizen.github.io/product-images/17086/7.jpg,https://oleks-netizen.github.io/product-images/17086/4.jpg,https://oleks-netizen.github.io/product-images/17086/5.jpg,https://oleks-netizen.github.io/product-images/17086/6.jpg</t>
         </is>
       </c>
       <c r="C141" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>RCs-7273-3md</t>
+          <t>17098</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RCs-7273-3md/1.jpg,https://oleks-netizen.github.io/product-images/RCs-7273-3md/2.jpg,https://oleks-netizen.github.io/product-images/RCs-7273-3md/3.jpg,https://oleks-netizen.github.io/product-images/RCs-7273-3md/9.jpg,https://oleks-netizen.github.io/product-images/RCs-7273-3md/4.jpg,https://oleks-netizen.github.io/product-images/RCs-7273-3md/5.jpg,https://oleks-netizen.github.io/product-images/RCs-7273-3md/6.jpg,https://oleks-netizen.github.io/product-images/RCs-7273-3md/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/17098/1.jpg,https://oleks-netizen.github.io/product-images/17098/2.jpg,https://oleks-netizen.github.io/product-images/17098/5.jpg,https://oleks-netizen.github.io/product-images/17098/3.jpg</t>
         </is>
       </c>
       <c r="C142" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>RSw-6601-3md</t>
+          <t>17229</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RSw-6601-3md/1.jpg,https://oleks-netizen.github.io/product-images/RSw-6601-3md/2.jpg,https://oleks-netizen.github.io/product-images/RSw-6601-3md/7.jpg,https://oleks-netizen.github.io/product-images/RSw-6601-3md/3.jpg,https://oleks-netizen.github.io/product-images/RSw-6601-3md/4.jpg,https://oleks-netizen.github.io/product-images/RSw-6601-3md/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/17229/1.jpg,https://oleks-netizen.github.io/product-images/17229/2.jpg,https://oleks-netizen.github.io/product-images/17229/7.jpg,https://oleks-netizen.github.io/product-images/17229/3.jpg,https://oleks-netizen.github.io/product-images/17229/4.jpg,https://oleks-netizen.github.io/product-images/17229/5.jpg</t>
         </is>
       </c>
       <c r="C143" t="n">
@@ -2571,301 +2571,1861 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>RY-3450-4lx</t>
+          <t>17238</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RY-3450-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RY-3450-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RY-3450-4lx/8.jpg,https://oleks-netizen.github.io/product-images/RY-3450-4lx/4.jpg,https://oleks-netizen.github.io/product-images/RY-3450-4lx/5.jpg,https://oleks-netizen.github.io/product-images/RY-3450-4lx/6.jpg,https://oleks-netizen.github.io/product-images/RY-3450-4lx/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/17238/1.jpg,https://oleks-netizen.github.io/product-images/17238/2.jpg,https://oleks-netizen.github.io/product-images/17238/7.jpg,https://oleks-netizen.github.io/product-images/17238/3.jpg,https://oleks-netizen.github.io/product-images/17238/4.jpg,https://oleks-netizen.github.io/product-images/17238/5.jpg</t>
         </is>
       </c>
       <c r="C144" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>RY-3451-4lx</t>
+          <t>17248</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RY-3451-4lx/1.jpg,https://oleks-netizen.github.io/product-images/RY-3451-4lx/2.jpg,https://oleks-netizen.github.io/product-images/RY-3451-4lx/3.jpg,https://oleks-netizen.github.io/product-images/RY-3451-4lx/9.jpg,https://oleks-netizen.github.io/product-images/RY-3451-4lx/4.jpg,https://oleks-netizen.github.io/product-images/RY-3451-4lx/5.jpg,https://oleks-netizen.github.io/product-images/RY-3451-4lx/6.jpg,https://oleks-netizen.github.io/product-images/RY-3451-4lx/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/17248/1.jpg,https://oleks-netizen.github.io/product-images/17248/2.jpg,https://oleks-netizen.github.io/product-images/17248/8.jpg,https://oleks-netizen.github.io/product-images/17248/3.jpg,https://oleks-netizen.github.io/product-images/17248/4.jpg,https://oleks-netizen.github.io/product-images/17248/6.jpg,https://oleks-netizen.github.io/product-images/17248/7.jpg</t>
         </is>
       </c>
       <c r="C145" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>RyE-4007-3md</t>
+          <t>18004</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RyE-4007-3md/1.jpg,https://oleks-netizen.github.io/product-images/RyE-4007-3md/2.jpg,https://oleks-netizen.github.io/product-images/RyE-4007-3md/7.jpg,https://oleks-netizen.github.io/product-images/RyE-4007-3md/3.jpg,https://oleks-netizen.github.io/product-images/RyE-4007-3md/4.jpg,https://oleks-netizen.github.io/product-images/RyE-4007-3md/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18004/1.jpg,https://oleks-netizen.github.io/product-images/18004/2.jpg,https://oleks-netizen.github.io/product-images/18004/11.jpg,https://oleks-netizen.github.io/product-images/18004/10.jpg,https://oleks-netizen.github.io/product-images/18004/3.jpg,https://oleks-netizen.github.io/product-images/18004/4.jpg,https://oleks-netizen.github.io/product-images/18004/5.jpg,https://oleks-netizen.github.io/product-images/18004/7.jpg,https://oleks-netizen.github.io/product-images/18004/8.jpg,https://oleks-netizen.github.io/product-images/18004/9.jpg</t>
         </is>
       </c>
       <c r="C146" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>RК-3990-3md</t>
+          <t>18012</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/RК-3990-3md/1.jpg,https://oleks-netizen.github.io/product-images/RК-3990-3md/2.jpg,https://oleks-netizen.github.io/product-images/RК-3990-3md/4.jpg,https://oleks-netizen.github.io/product-images/RК-3990-3md/10.jpg,https://oleks-netizen.github.io/product-images/RК-3990-3md/5.jpg,https://oleks-netizen.github.io/product-images/RК-3990-3md/6.jpg,https://oleks-netizen.github.io/product-images/RК-3990-3md/7.jpg,https://oleks-netizen.github.io/product-images/RК-3990-3md/8.jpg,https://oleks-netizen.github.io/product-images/RК-3990-3md/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18012/1.jpg,https://oleks-netizen.github.io/product-images/18012/2.jpg,https://oleks-netizen.github.io/product-images/18012/5.jpg,https://oleks-netizen.github.io/product-images/18012/3.jpg</t>
         </is>
       </c>
       <c r="C147" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Swarovski1655Anero</t>
+          <t>18018</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/Swarovski1655Anero/1.jpg,https://oleks-netizen.github.io/product-images/Swarovski1655Anero/2.jpg,https://oleks-netizen.github.io/product-images/Swarovski1655Anero/3.jpg,https://oleks-netizen.github.io/product-images/Swarovski1655Anero/4.jpg,https://oleks-netizen.github.io/product-images/Swarovski1655Anero/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18018/1.jpg,https://oleks-netizen.github.io/product-images/18018/2.jpg,https://oleks-netizen.github.io/product-images/18018/13.jpg,https://oleks-netizen.github.io/product-images/18018/10.jpg,https://oleks-netizen.github.io/product-images/18018/11.jpg,https://oleks-netizen.github.io/product-images/18018/12.jpg,https://oleks-netizen.github.io/product-images/18018/3.jpg,https://oleks-netizen.github.io/product-images/18018/5.jpg,https://oleks-netizen.github.io/product-images/18018/6.jpg,https://oleks-netizen.github.io/product-images/18018/7.jpg,https://oleks-netizen.github.io/product-images/18018/8.jpg,https://oleks-netizen.github.io/product-images/18018/9.jpg</t>
         </is>
       </c>
       <c r="C148" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>T0158A</t>
+          <t>18070</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/T0158A/1.jpg,https://oleks-netizen.github.io/product-images/T0158A/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18070/1.jpg,https://oleks-netizen.github.io/product-images/18070/2.jpg,https://oleks-netizen.github.io/product-images/18070/11.jpg,https://oleks-netizen.github.io/product-images/18070/10.jpg,https://oleks-netizen.github.io/product-images/18070/3.jpg,https://oleks-netizen.github.io/product-images/18070/4.jpg,https://oleks-netizen.github.io/product-images/18070/5.jpg,https://oleks-netizen.github.io/product-images/18070/7.jpg,https://oleks-netizen.github.io/product-images/18070/8.jpg,https://oleks-netizen.github.io/product-images/18070/9.jpg</t>
         </is>
       </c>
       <c r="C149" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>TB019A</t>
+          <t>18092</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/TB019A/1.jpg,https://oleks-netizen.github.io/product-images/TB019A/2.jpg,https://oleks-netizen.github.io/product-images/TB019A/3.jpg,https://oleks-netizen.github.io/product-images/TB019A/4.jpg,https://oleks-netizen.github.io/product-images/TB019A/5.jpg,https://oleks-netizen.github.io/product-images/TB019A/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18092/1.jpg,https://oleks-netizen.github.io/product-images/18092/2.jpg,https://oleks-netizen.github.io/product-images/18092/3.jpg,https://oleks-netizen.github.io/product-images/18092/4.jpg,https://oleks-netizen.github.io/product-images/18092/5.jpg,https://oleks-netizen.github.io/product-images/18092/6.jpg,https://oleks-netizen.github.io/product-images/18092/7.jpg,https://oleks-netizen.github.io/product-images/18092/8.jpg,https://oleks-netizen.github.io/product-images/18092/9.jpg</t>
         </is>
       </c>
       <c r="C150" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>TB019B</t>
+          <t>18097</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/TB019B/1.jpg,https://oleks-netizen.github.io/product-images/TB019B/7.jpg,https://oleks-netizen.github.io/product-images/TB019B/3.jpg,https://oleks-netizen.github.io/product-images/TB019B/4.jpg,https://oleks-netizen.github.io/product-images/TB019B/5.jpg,https://oleks-netizen.github.io/product-images/TB019B/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18097/10.jpg,https://oleks-netizen.github.io/product-images/18097/1.jpg,https://oleks-netizen.github.io/product-images/18097/2.jpg,https://oleks-netizen.github.io/product-images/18097/3.jpg,https://oleks-netizen.github.io/product-images/18097/4.jpg,https://oleks-netizen.github.io/product-images/18097/5.jpg,https://oleks-netizen.github.io/product-images/18097/6.jpg,https://oleks-netizen.github.io/product-images/18097/7.jpg,https://oleks-netizen.github.io/product-images/18097/8.jpg,https://oleks-netizen.github.io/product-images/18097/9.jpg</t>
         </is>
       </c>
       <c r="C151" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>TB019C</t>
+          <t>18103</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/TB019C/1.jpg,https://oleks-netizen.github.io/product-images/TB019C/2.jpg,https://oleks-netizen.github.io/product-images/TB019C/5.jpg,https://oleks-netizen.github.io/product-images/TB019C/8.jpg,https://oleks-netizen.github.io/product-images/TB019C/3.jpg,https://oleks-netizen.github.io/product-images/TB019C/4.jpg,https://oleks-netizen.github.io/product-images/TB019C/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18103/10.jpg,https://oleks-netizen.github.io/product-images/18103/11.jpg,https://oleks-netizen.github.io/product-images/18103/1.jpg,https://oleks-netizen.github.io/product-images/18103/2.jpg,https://oleks-netizen.github.io/product-images/18103/3.jpg,https://oleks-netizen.github.io/product-images/18103/4.jpg,https://oleks-netizen.github.io/product-images/18103/5.jpg,https://oleks-netizen.github.io/product-images/18103/6.jpg,https://oleks-netizen.github.io/product-images/18103/7.jpg,https://oleks-netizen.github.io/product-images/18103/8.jpg,https://oleks-netizen.github.io/product-images/18103/9.jpg</t>
         </is>
       </c>
       <c r="C152" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>TB019J</t>
+          <t>18169</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/TB019J/1.jpg,https://oleks-netizen.github.io/product-images/TB019J/7.jpg,https://oleks-netizen.github.io/product-images/TB019J/3.jpg,https://oleks-netizen.github.io/product-images/TB019J/4.jpg,https://oleks-netizen.github.io/product-images/TB019J/5.jpg,https://oleks-netizen.github.io/product-images/TB019J/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18169/1.jpg,https://oleks-netizen.github.io/product-images/18169/2.jpg,https://oleks-netizen.github.io/product-images/18169/3.jpg,https://oleks-netizen.github.io/product-images/18169/4.jpg,https://oleks-netizen.github.io/product-images/18169/5.jpg,https://oleks-netizen.github.io/product-images/18169/6.jpg,https://oleks-netizen.github.io/product-images/18169/7.jpg,https://oleks-netizen.github.io/product-images/18169/8.jpg,https://oleks-netizen.github.io/product-images/18169/9.jpg</t>
         </is>
       </c>
       <c r="C153" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>TB1063A</t>
+          <t>18171</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/TB1063A/1.jpg,https://oleks-netizen.github.io/product-images/TB1063A/2.jpg,https://oleks-netizen.github.io/product-images/TB1063A/3.jpg,https://oleks-netizen.github.io/product-images/TB1063A/4.jpg,https://oleks-netizen.github.io/product-images/TB1063A/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18171/10.jpg,https://oleks-netizen.github.io/product-images/18171/11.jpg,https://oleks-netizen.github.io/product-images/18171/12.jpg,https://oleks-netizen.github.io/product-images/18171/1.jpg,https://oleks-netizen.github.io/product-images/18171/2.jpg,https://oleks-netizen.github.io/product-images/18171/3.jpg,https://oleks-netizen.github.io/product-images/18171/4.jpg,https://oleks-netizen.github.io/product-images/18171/5.jpg,https://oleks-netizen.github.io/product-images/18171/6.jpg,https://oleks-netizen.github.io/product-images/18171/7.jpg,https://oleks-netizen.github.io/product-images/18171/8.jpg,https://oleks-netizen.github.io/product-images/18171/9.jpg</t>
         </is>
       </c>
       <c r="C154" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>TB1063C</t>
+          <t>18178</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/TB1063C/1.jpg,https://oleks-netizen.github.io/product-images/TB1063C/2.jpg,https://oleks-netizen.github.io/product-images/TB1063C/3.jpg,https://oleks-netizen.github.io/product-images/TB1063C/4.jpg,https://oleks-netizen.github.io/product-images/TB1063C/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18178/10.jpg,https://oleks-netizen.github.io/product-images/18178/11.jpg,https://oleks-netizen.github.io/product-images/18178/12.jpg,https://oleks-netizen.github.io/product-images/18178/1.jpg,https://oleks-netizen.github.io/product-images/18178/2.jpg,https://oleks-netizen.github.io/product-images/18178/3.jpg,https://oleks-netizen.github.io/product-images/18178/4.jpg,https://oleks-netizen.github.io/product-images/18178/5.jpg,https://oleks-netizen.github.io/product-images/18178/6.jpg,https://oleks-netizen.github.io/product-images/18178/7.jpg,https://oleks-netizen.github.io/product-images/18178/8.jpg,https://oleks-netizen.github.io/product-images/18178/9.jpg</t>
         </is>
       </c>
       <c r="C155" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>TB555A</t>
+          <t>18203</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/TB555A/1.jpg,https://oleks-netizen.github.io/product-images/TB555A/2.jpg,https://oleks-netizen.github.io/product-images/TB555A/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18203/10.jpg,https://oleks-netizen.github.io/product-images/18203/11.jpg,https://oleks-netizen.github.io/product-images/18203/1.jpg,https://oleks-netizen.github.io/product-images/18203/2.jpg,https://oleks-netizen.github.io/product-images/18203/3.jpg,https://oleks-netizen.github.io/product-images/18203/4.jpg,https://oleks-netizen.github.io/product-images/18203/5.jpg,https://oleks-netizen.github.io/product-images/18203/6.jpg,https://oleks-netizen.github.io/product-images/18203/7.jpg,https://oleks-netizen.github.io/product-images/18203/8.jpg,https://oleks-netizen.github.io/product-images/18203/9.jpg</t>
         </is>
       </c>
       <c r="C156" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>TB555B</t>
+          <t>18235</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/TB555B/1.jpg,https://oleks-netizen.github.io/product-images/TB555B/2.jpg,https://oleks-netizen.github.io/product-images/TB555B/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18235/10.jpg,https://oleks-netizen.github.io/product-images/18235/11.jpg,https://oleks-netizen.github.io/product-images/18235/12.jpg,https://oleks-netizen.github.io/product-images/18235/13.jpg,https://oleks-netizen.github.io/product-images/18235/1.jpg,https://oleks-netizen.github.io/product-images/18235/2.jpg,https://oleks-netizen.github.io/product-images/18235/3.jpg,https://oleks-netizen.github.io/product-images/18235/4.jpg,https://oleks-netizen.github.io/product-images/18235/5.jpg,https://oleks-netizen.github.io/product-images/18235/6.jpg,https://oleks-netizen.github.io/product-images/18235/7.jpg,https://oleks-netizen.github.io/product-images/18235/8.jpg,https://oleks-netizen.github.io/product-images/18235/9.jpg</t>
         </is>
       </c>
       <c r="C157" t="n">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>TB555C</t>
+          <t>18236</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/TB555C/1.jpg,https://oleks-netizen.github.io/product-images/TB555C/2.jpg,https://oleks-netizen.github.io/product-images/TB555C/7.jpg,https://oleks-netizen.github.io/product-images/TB555C/3.jpg,https://oleks-netizen.github.io/product-images/TB555C/4.jpg,https://oleks-netizen.github.io/product-images/TB555C/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18236/10.jpg,https://oleks-netizen.github.io/product-images/18236/11.jpg,https://oleks-netizen.github.io/product-images/18236/12.jpg,https://oleks-netizen.github.io/product-images/18236/1.jpg,https://oleks-netizen.github.io/product-images/18236/2.jpg,https://oleks-netizen.github.io/product-images/18236/3.jpg,https://oleks-netizen.github.io/product-images/18236/4.jpg,https://oleks-netizen.github.io/product-images/18236/5.jpg,https://oleks-netizen.github.io/product-images/18236/6.jpg,https://oleks-netizen.github.io/product-images/18236/7.jpg,https://oleks-netizen.github.io/product-images/18236/8.jpg,https://oleks-netizen.github.io/product-images/18236/9.jpg</t>
         </is>
       </c>
       <c r="C158" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>VSL42 BLK ST BLUE</t>
+          <t>18239</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/VSL42 BLK ST BLUE/1.jpg,https://oleks-netizen.github.io/product-images/VSL42 BLK ST BLUE/2.jpg,https://oleks-netizen.github.io/product-images/VSL42 BLK ST BLUE/8.jpg,https://oleks-netizen.github.io/product-images/VSL42 BLK ST BLUE/3.jpg,https://oleks-netizen.github.io/product-images/VSL42 BLK ST BLUE/4.jpg,https://oleks-netizen.github.io/product-images/VSL42 BLK ST BLUE/6.jpg,https://oleks-netizen.github.io/product-images/VSL42 BLK ST BLUE/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18239/10.jpg,https://oleks-netizen.github.io/product-images/18239/11.jpg,https://oleks-netizen.github.io/product-images/18239/12.jpg,https://oleks-netizen.github.io/product-images/18239/13.jpg,https://oleks-netizen.github.io/product-images/18239/1.jpg,https://oleks-netizen.github.io/product-images/18239/2.jpg,https://oleks-netizen.github.io/product-images/18239/3.jpg,https://oleks-netizen.github.io/product-images/18239/4.jpg,https://oleks-netizen.github.io/product-images/18239/5.jpg,https://oleks-netizen.github.io/product-images/18239/6.jpg,https://oleks-netizen.github.io/product-images/18239/7.jpg,https://oleks-netizen.github.io/product-images/18239/8.jpg,https://oleks-netizen.github.io/product-images/18239/9.jpg</t>
         </is>
       </c>
       <c r="C159" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>VSL42 OIL TAN</t>
+          <t>18293</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/VSL42 OIL TAN/1.jpg,https://oleks-netizen.github.io/product-images/VSL42 OIL TAN/2.jpg,https://oleks-netizen.github.io/product-images/VSL42 OIL TAN/8.jpg,https://oleks-netizen.github.io/product-images/VSL42 OIL TAN/3.jpg,https://oleks-netizen.github.io/product-images/VSL42 OIL TAN/4.jpg,https://oleks-netizen.github.io/product-images/VSL42 OIL TAN/6.jpg,https://oleks-netizen.github.io/product-images/VSL42 OIL TAN/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18293/10.jpg,https://oleks-netizen.github.io/product-images/18293/11.jpg,https://oleks-netizen.github.io/product-images/18293/12.jpg,https://oleks-netizen.github.io/product-images/18293/1.jpg,https://oleks-netizen.github.io/product-images/18293/2.jpg,https://oleks-netizen.github.io/product-images/18293/3.jpg,https://oleks-netizen.github.io/product-images/18293/4.jpg,https://oleks-netizen.github.io/product-images/18293/5.jpg,https://oleks-netizen.github.io/product-images/18293/6.jpg,https://oleks-netizen.github.io/product-images/18293/7.jpg,https://oleks-netizen.github.io/product-images/18293/8.jpg,https://oleks-netizen.github.io/product-images/18293/9.jpg</t>
         </is>
       </c>
       <c r="C160" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Y60 BEIGE</t>
+          <t>18309</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/Y60 BEIGE/1.jpg,https://oleks-netizen.github.io/product-images/Y60 BEIGE/2.jpg,https://oleks-netizen.github.io/product-images/Y60 BEIGE/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18309/1.jpg,https://oleks-netizen.github.io/product-images/18309/2.jpg,https://oleks-netizen.github.io/product-images/18309/7.jpg,https://oleks-netizen.github.io/product-images/18309/4.jpg,https://oleks-netizen.github.io/product-images/18309/5.jpg,https://oleks-netizen.github.io/product-images/18309/6.jpg</t>
         </is>
       </c>
       <c r="C161" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Y60 BLK</t>
+          <t>18327</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/Y60 BLK/1.jpg,https://oleks-netizen.github.io/product-images/Y60 BLK/2.jpg,https://oleks-netizen.github.io/product-images/Y60 BLK/3.jpg,https://oleks-netizen.github.io/product-images/Y60 BLK/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18327/1.jpg,https://oleks-netizen.github.io/product-images/18327/2.jpg,https://oleks-netizen.github.io/product-images/18327/9.jpg,https://oleks-netizen.github.io/product-images/18327/3.jpg,https://oleks-netizen.github.io/product-images/18327/4.jpg,https://oleks-netizen.github.io/product-images/18327/5.jpg,https://oleks-netizen.github.io/product-images/18327/7.jpg,https://oleks-netizen.github.io/product-images/18327/8.jpg</t>
         </is>
       </c>
       <c r="C162" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>ZА-3990-3md</t>
+          <t>18331</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/ZА-3990-3md/1.jpg,https://oleks-netizen.github.io/product-images/ZА-3990-3md/2.jpg,https://oleks-netizen.github.io/product-images/ZА-3990-3md/4.jpg,https://oleks-netizen.github.io/product-images/ZА-3990-3md/10.jpg,https://oleks-netizen.github.io/product-images/ZА-3990-3md/3.jpg,https://oleks-netizen.github.io/product-images/ZА-3990-3md/6.jpg,https://oleks-netizen.github.io/product-images/ZА-3990-3md/7.jpg,https://oleks-netizen.github.io/product-images/ZА-3990-3md/8.jpg,https://oleks-netizen.github.io/product-images/ZА-3990-3md/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18331/1.jpg,https://oleks-netizen.github.io/product-images/18331/2.jpg,https://oleks-netizen.github.io/product-images/18331/7.jpg,https://oleks-netizen.github.io/product-images/18331/3.jpg,https://oleks-netizen.github.io/product-images/18331/5.jpg,https://oleks-netizen.github.io/product-images/18331/6.jpg</t>
         </is>
       </c>
       <c r="C163" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>18345</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/18345/1.jpg,https://oleks-netizen.github.io/product-images/18345/2.jpg,https://oleks-netizen.github.io/product-images/18345/9.jpg,https://oleks-netizen.github.io/product-images/18345/3.jpg,https://oleks-netizen.github.io/product-images/18345/4.jpg,https://oleks-netizen.github.io/product-images/18345/5.jpg,https://oleks-netizen.github.io/product-images/18345/7.jpg,https://oleks-netizen.github.io/product-images/18345/8.jpg</t>
+        </is>
+      </c>
+      <c r="C164" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>18347</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/18347/1.jpg,https://oleks-netizen.github.io/product-images/18347/2.jpg,https://oleks-netizen.github.io/product-images/18347/8.jpg,https://oleks-netizen.github.io/product-images/18347/3.jpg,https://oleks-netizen.github.io/product-images/18347/4.jpg,https://oleks-netizen.github.io/product-images/18347/5.jpg,https://oleks-netizen.github.io/product-images/18347/6.jpg</t>
+        </is>
+      </c>
+      <c r="C165" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>18376</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/18376/1.jpg,https://oleks-netizen.github.io/product-images/18376/2.jpg,https://oleks-netizen.github.io/product-images/18376/8.jpg,https://oleks-netizen.github.io/product-images/18376/3.jpg,https://oleks-netizen.github.io/product-images/18376/4.jpg,https://oleks-netizen.github.io/product-images/18376/5.jpg,https://oleks-netizen.github.io/product-images/18376/7.jpg</t>
+        </is>
+      </c>
+      <c r="C166" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>18382</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/18382/1.jpg,https://oleks-netizen.github.io/product-images/18382/2.jpg,https://oleks-netizen.github.io/product-images/18382/8.jpg,https://oleks-netizen.github.io/product-images/18382/3.jpg,https://oleks-netizen.github.io/product-images/18382/4.jpg,https://oleks-netizen.github.io/product-images/18382/5.jpg,https://oleks-netizen.github.io/product-images/18382/7.jpg</t>
+        </is>
+      </c>
+      <c r="C167" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>18398</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/18398/1.jpg,https://oleks-netizen.github.io/product-images/18398/2.jpg,https://oleks-netizen.github.io/product-images/18398/7.jpg,https://oleks-netizen.github.io/product-images/18398/3.jpg,https://oleks-netizen.github.io/product-images/18398/4.jpg,https://oleks-netizen.github.io/product-images/18398/5.jpg</t>
+        </is>
+      </c>
+      <c r="C168" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>18400</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/18400/1.jpg,https://oleks-netizen.github.io/product-images/18400/2.jpg,https://oleks-netizen.github.io/product-images/18400/7.jpg,https://oleks-netizen.github.io/product-images/18400/4.jpg,https://oleks-netizen.github.io/product-images/18400/5.jpg,https://oleks-netizen.github.io/product-images/18400/6.jpg</t>
+        </is>
+      </c>
+      <c r="C169" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>18404</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/18404/1.jpg,https://oleks-netizen.github.io/product-images/18404/2.jpg,https://oleks-netizen.github.io/product-images/18404/6.jpg,https://oleks-netizen.github.io/product-images/18404/4.jpg,https://oleks-netizen.github.io/product-images/18404/5.jpg</t>
+        </is>
+      </c>
+      <c r="C170" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>18411</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/18411/1.jpg,https://oleks-netizen.github.io/product-images/18411/2.jpg,https://oleks-netizen.github.io/product-images/18411/6.jpg,https://oleks-netizen.github.io/product-images/18411/4.jpg,https://oleks-netizen.github.io/product-images/18411/5.jpg</t>
+        </is>
+      </c>
+      <c r="C171" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>18483</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/18483/1.jpg,https://oleks-netizen.github.io/product-images/18483/2.jpg,https://oleks-netizen.github.io/product-images/18483/8.jpg,https://oleks-netizen.github.io/product-images/18483/3.jpg,https://oleks-netizen.github.io/product-images/18483/4.jpg,https://oleks-netizen.github.io/product-images/18483/5.jpg,https://oleks-netizen.github.io/product-images/18483/7.jpg</t>
+        </is>
+      </c>
+      <c r="C172" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>18803</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/18803/1.jpg,https://oleks-netizen.github.io/product-images/18803/2.jpg,https://oleks-netizen.github.io/product-images/18803/7.jpg,https://oleks-netizen.github.io/product-images/18803/3.jpg,https://oleks-netizen.github.io/product-images/18803/4.jpg,https://oleks-netizen.github.io/product-images/18803/5.jpg</t>
+        </is>
+      </c>
+      <c r="C173" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>18813</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/18813/1.jpg,https://oleks-netizen.github.io/product-images/18813/2.jpg,https://oleks-netizen.github.io/product-images/18813/11.jpg,https://oleks-netizen.github.io/product-images/18813/10.jpg,https://oleks-netizen.github.io/product-images/18813/3.jpg,https://oleks-netizen.github.io/product-images/18813/4.jpg,https://oleks-netizen.github.io/product-images/18813/5.jpg,https://oleks-netizen.github.io/product-images/18813/7.jpg,https://oleks-netizen.github.io/product-images/18813/8.jpg,https://oleks-netizen.github.io/product-images/18813/9.jpg</t>
+        </is>
+      </c>
+      <c r="C174" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>18815</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/18815/1.jpg,https://oleks-netizen.github.io/product-images/18815/2.jpg,https://oleks-netizen.github.io/product-images/18815/8.jpg,https://oleks-netizen.github.io/product-images/18815/3.jpg,https://oleks-netizen.github.io/product-images/18815/4.jpg,https://oleks-netizen.github.io/product-images/18815/5.jpg,https://oleks-netizen.github.io/product-images/18815/6.jpg</t>
+        </is>
+      </c>
+      <c r="C175" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>18822</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/18822/1.jpg,https://oleks-netizen.github.io/product-images/18822/2.jpg,https://oleks-netizen.github.io/product-images/18822/10.jpg,https://oleks-netizen.github.io/product-images/18822/3.jpg,https://oleks-netizen.github.io/product-images/18822/4.jpg,https://oleks-netizen.github.io/product-images/18822/5.jpg,https://oleks-netizen.github.io/product-images/18822/6.jpg,https://oleks-netizen.github.io/product-images/18822/8.jpg,https://oleks-netizen.github.io/product-images/18822/9.jpg</t>
+        </is>
+      </c>
+      <c r="C176" t="n">
         <v>9</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>18825</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/18825/1.jpg,https://oleks-netizen.github.io/product-images/18825/2.jpg,https://oleks-netizen.github.io/product-images/18825/9.jpg,https://oleks-netizen.github.io/product-images/18825/3.jpg,https://oleks-netizen.github.io/product-images/18825/4.jpg,https://oleks-netizen.github.io/product-images/18825/5.jpg,https://oleks-netizen.github.io/product-images/18825/7.jpg,https://oleks-netizen.github.io/product-images/18825/8.jpg</t>
+        </is>
+      </c>
+      <c r="C177" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>18831</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/18831/1.jpg,https://oleks-netizen.github.io/product-images/18831/2.jpg,https://oleks-netizen.github.io/product-images/18831/7.jpg,https://oleks-netizen.github.io/product-images/18831/3.jpg,https://oleks-netizen.github.io/product-images/18831/4.jpg,https://oleks-netizen.github.io/product-images/18831/5.jpg</t>
+        </is>
+      </c>
+      <c r="C178" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>18836</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/18836/1.jpg,https://oleks-netizen.github.io/product-images/18836/2.jpg,https://oleks-netizen.github.io/product-images/18836/7.jpg,https://oleks-netizen.github.io/product-images/18836/3.jpg,https://oleks-netizen.github.io/product-images/18836/4.jpg,https://oleks-netizen.github.io/product-images/18836/6.jpg</t>
+        </is>
+      </c>
+      <c r="C179" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>18837</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/18837/1.jpg,https://oleks-netizen.github.io/product-images/18837/2.jpg,https://oleks-netizen.github.io/product-images/18837/9.jpg,https://oleks-netizen.github.io/product-images/18837/3.jpg,https://oleks-netizen.github.io/product-images/18837/4.jpg,https://oleks-netizen.github.io/product-images/18837/5.jpg,https://oleks-netizen.github.io/product-images/18837/6.jpg,https://oleks-netizen.github.io/product-images/18837/8.jpg</t>
+        </is>
+      </c>
+      <c r="C180" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>18840</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/18840/1.jpg,https://oleks-netizen.github.io/product-images/18840/2.jpg,https://oleks-netizen.github.io/product-images/18840/7.jpg,https://oleks-netizen.github.io/product-images/18840/3.jpg,https://oleks-netizen.github.io/product-images/18840/4.jpg,https://oleks-netizen.github.io/product-images/18840/5.jpg</t>
+        </is>
+      </c>
+      <c r="C181" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>18867</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/18867/1.jpg,https://oleks-netizen.github.io/product-images/18867/2.jpg,https://oleks-netizen.github.io/product-images/18867/7.jpg,https://oleks-netizen.github.io/product-images/18867/3.jpg,https://oleks-netizen.github.io/product-images/18867/4.jpg,https://oleks-netizen.github.io/product-images/18867/5.jpg</t>
+        </is>
+      </c>
+      <c r="C182" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>18870</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/18870/1.jpg,https://oleks-netizen.github.io/product-images/18870/2.jpg,https://oleks-netizen.github.io/product-images/18870/9.jpg,https://oleks-netizen.github.io/product-images/18870/3.jpg,https://oleks-netizen.github.io/product-images/18870/4.jpg,https://oleks-netizen.github.io/product-images/18870/5.jpg,https://oleks-netizen.github.io/product-images/18870/6.jpg,https://oleks-netizen.github.io/product-images/18870/8.jpg</t>
+        </is>
+      </c>
+      <c r="C183" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>18871</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/18871/1.jpg,https://oleks-netizen.github.io/product-images/18871/2.jpg,https://oleks-netizen.github.io/product-images/18871/7.jpg,https://oleks-netizen.github.io/product-images/18871/3.jpg,https://oleks-netizen.github.io/product-images/18871/4.jpg,https://oleks-netizen.github.io/product-images/18871/6.jpg</t>
+        </is>
+      </c>
+      <c r="C184" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>18877</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/18877/1.jpg,https://oleks-netizen.github.io/product-images/18877/2.jpg,https://oleks-netizen.github.io/product-images/18877/9.jpg,https://oleks-netizen.github.io/product-images/18877/3.jpg,https://oleks-netizen.github.io/product-images/18877/4.jpg,https://oleks-netizen.github.io/product-images/18877/5.jpg,https://oleks-netizen.github.io/product-images/18877/6.jpg,https://oleks-netizen.github.io/product-images/18877/8.jpg</t>
+        </is>
+      </c>
+      <c r="C185" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>18959</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/18959/1.jpg,https://oleks-netizen.github.io/product-images/18959/2.jpg,https://oleks-netizen.github.io/product-images/18959/7.jpg,https://oleks-netizen.github.io/product-images/18959/3.jpg,https://oleks-netizen.github.io/product-images/18959/4.jpg,https://oleks-netizen.github.io/product-images/18959/5.jpg</t>
+        </is>
+      </c>
+      <c r="C186" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>18966</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/18966/1.jpg,https://oleks-netizen.github.io/product-images/18966/2.jpg,https://oleks-netizen.github.io/product-images/18966/6.jpg,https://oleks-netizen.github.io/product-images/18966/4.jpg,https://oleks-netizen.github.io/product-images/18966/5.jpg</t>
+        </is>
+      </c>
+      <c r="C187" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>19016</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/19016/1.jpg,https://oleks-netizen.github.io/product-images/19016/2.jpg,https://oleks-netizen.github.io/product-images/19016/6.jpg,https://oleks-netizen.github.io/product-images/19016/3.jpg,https://oleks-netizen.github.io/product-images/19016/5.jpg</t>
+        </is>
+      </c>
+      <c r="C188" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>19049</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/19049/1.jpg,https://oleks-netizen.github.io/product-images/19049/2.jpg,https://oleks-netizen.github.io/product-images/19049/6.jpg,https://oleks-netizen.github.io/product-images/19049/4.jpg,https://oleks-netizen.github.io/product-images/19049/5.jpg</t>
+        </is>
+      </c>
+      <c r="C189" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>19058</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/19058/1.jpg,https://oleks-netizen.github.io/product-images/19058/2.jpg,https://oleks-netizen.github.io/product-images/19058/3.jpg</t>
+        </is>
+      </c>
+      <c r="C190" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>19061</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/19061/1.jpg,https://oleks-netizen.github.io/product-images/19061/2.jpg,https://oleks-netizen.github.io/product-images/19061/3.jpg,https://oleks-netizen.github.io/product-images/19061/4.jpg,https://oleks-netizen.github.io/product-images/19061/5.jpg</t>
+        </is>
+      </c>
+      <c r="C191" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>19082</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/19082/1.jpg,https://oleks-netizen.github.io/product-images/19082/2.jpg,https://oleks-netizen.github.io/product-images/19082/3.jpg</t>
+        </is>
+      </c>
+      <c r="C192" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>20040</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20040/1.jpg,https://oleks-netizen.github.io/product-images/20040/2.jpg,https://oleks-netizen.github.io/product-images/20040/3.jpg,https://oleks-netizen.github.io/product-images/20040/11.jpg,https://oleks-netizen.github.io/product-images/20040/10.jpg,https://oleks-netizen.github.io/product-images/20040/4.jpg,https://oleks-netizen.github.io/product-images/20040/5.jpg,https://oleks-netizen.github.io/product-images/20040/6.jpg,https://oleks-netizen.github.io/product-images/20040/8.jpg,https://oleks-netizen.github.io/product-images/20040/9.jpg</t>
+        </is>
+      </c>
+      <c r="C193" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>20041</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20041/1.jpg,https://oleks-netizen.github.io/product-images/20041/2.jpg,https://oleks-netizen.github.io/product-images/20041/3.jpg,https://oleks-netizen.github.io/product-images/20041/4.jpg,https://oleks-netizen.github.io/product-images/20041/5.jpg,https://oleks-netizen.github.io/product-images/20041/6.jpg,https://oleks-netizen.github.io/product-images/20041/7.jpg,https://oleks-netizen.github.io/product-images/20041/8.jpg,https://oleks-netizen.github.io/product-images/20041/9.jpg</t>
+        </is>
+      </c>
+      <c r="C194" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>20042</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20042/1.jpg,https://oleks-netizen.github.io/product-images/20042/2.jpg,https://oleks-netizen.github.io/product-images/20042/17.jpg,https://oleks-netizen.github.io/product-images/20042/10.jpg,https://oleks-netizen.github.io/product-images/20042/11.jpg,https://oleks-netizen.github.io/product-images/20042/12.jpg,https://oleks-netizen.github.io/product-images/20042/13.jpg,https://oleks-netizen.github.io/product-images/20042/14.jpg,https://oleks-netizen.github.io/product-images/20042/15.jpg,https://oleks-netizen.github.io/product-images/20042/16.jpg,https://oleks-netizen.github.io/product-images/20042/4.jpg,https://oleks-netizen.github.io/product-images/20042/5.jpg,https://oleks-netizen.github.io/product-images/20042/6.jpg,https://oleks-netizen.github.io/product-images/20042/7.jpg,https://oleks-netizen.github.io/product-images/20042/8.jpg,https://oleks-netizen.github.io/product-images/20042/9.jpg</t>
+        </is>
+      </c>
+      <c r="C195" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>20047</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20047/1.jpg,https://oleks-netizen.github.io/product-images/20047/2.jpg,https://oleks-netizen.github.io/product-images/20047/14.jpg,https://oleks-netizen.github.io/product-images/20047/10.jpg,https://oleks-netizen.github.io/product-images/20047/11.jpg,https://oleks-netizen.github.io/product-images/20047/12.jpg,https://oleks-netizen.github.io/product-images/20047/13.jpg,https://oleks-netizen.github.io/product-images/20047/3.jpg,https://oleks-netizen.github.io/product-images/20047/4.jpg,https://oleks-netizen.github.io/product-images/20047/5.jpg,https://oleks-netizen.github.io/product-images/20047/7.jpg,https://oleks-netizen.github.io/product-images/20047/8.jpg,https://oleks-netizen.github.io/product-images/20047/9.jpg</t>
+        </is>
+      </c>
+      <c r="C196" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>20069</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20069/10.jpg,https://oleks-netizen.github.io/product-images/20069/11.jpg,https://oleks-netizen.github.io/product-images/20069/12.jpg,https://oleks-netizen.github.io/product-images/20069/1.jpg,https://oleks-netizen.github.io/product-images/20069/2.jpg,https://oleks-netizen.github.io/product-images/20069/3.jpg,https://oleks-netizen.github.io/product-images/20069/4.jpg,https://oleks-netizen.github.io/product-images/20069/5.jpg,https://oleks-netizen.github.io/product-images/20069/6.jpg,https://oleks-netizen.github.io/product-images/20069/7.jpg,https://oleks-netizen.github.io/product-images/20069/8.jpg,https://oleks-netizen.github.io/product-images/20069/9.jpg</t>
+        </is>
+      </c>
+      <c r="C197" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>20075</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20075/1.jpg,https://oleks-netizen.github.io/product-images/20075/2.jpg,https://oleks-netizen.github.io/product-images/20075/11.jpg,https://oleks-netizen.github.io/product-images/20075/13.jpg,https://oleks-netizen.github.io/product-images/20075/12.jpg,https://oleks-netizen.github.io/product-images/20075/3.jpg,https://oleks-netizen.github.io/product-images/20075/4.jpg,https://oleks-netizen.github.io/product-images/20075/5.jpg,https://oleks-netizen.github.io/product-images/20075/6.jpg,https://oleks-netizen.github.io/product-images/20075/7.jpg,https://oleks-netizen.github.io/product-images/20075/8.jpg,https://oleks-netizen.github.io/product-images/20075/9.jpg</t>
+        </is>
+      </c>
+      <c r="C198" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>20080</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20080/1.jpg,https://oleks-netizen.github.io/product-images/20080/2.jpg,https://oleks-netizen.github.io/product-images/20080/6.jpg,https://oleks-netizen.github.io/product-images/20080/8.jpg,https://oleks-netizen.github.io/product-images/20080/3.jpg,https://oleks-netizen.github.io/product-images/20080/4.jpg,https://oleks-netizen.github.io/product-images/20080/5.jpg</t>
+        </is>
+      </c>
+      <c r="C199" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>20083</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20083/1.jpg,https://oleks-netizen.github.io/product-images/20083/2.jpg,https://oleks-netizen.github.io/product-images/20083/13.jpg,https://oleks-netizen.github.io/product-images/20083/10.jpg,https://oleks-netizen.github.io/product-images/20083/11.jpg,https://oleks-netizen.github.io/product-images/20083/12.jpg,https://oleks-netizen.github.io/product-images/20083/3.jpg,https://oleks-netizen.github.io/product-images/20083/4.jpg,https://oleks-netizen.github.io/product-images/20083/5.jpg,https://oleks-netizen.github.io/product-images/20083/6.jpg,https://oleks-netizen.github.io/product-images/20083/7.jpg,https://oleks-netizen.github.io/product-images/20083/8.jpg</t>
+        </is>
+      </c>
+      <c r="C200" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>20084</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20084/1.jpg,https://oleks-netizen.github.io/product-images/20084/2.jpg,https://oleks-netizen.github.io/product-images/20084/3.jpg,https://oleks-netizen.github.io/product-images/20084/4.jpg,https://oleks-netizen.github.io/product-images/20084/5.jpg,https://oleks-netizen.github.io/product-images/20084/6.jpg</t>
+        </is>
+      </c>
+      <c r="C201" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>20121</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20121/1.jpg,https://oleks-netizen.github.io/product-images/20121/2.jpg,https://oleks-netizen.github.io/product-images/20121/8.jpg,https://oleks-netizen.github.io/product-images/20121/3.jpg,https://oleks-netizen.github.io/product-images/20121/4.jpg,https://oleks-netizen.github.io/product-images/20121/5.jpg,https://oleks-netizen.github.io/product-images/20121/6.jpg</t>
+        </is>
+      </c>
+      <c r="C202" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>20126</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20126/1.jpg,https://oleks-netizen.github.io/product-images/20126/2.jpg,https://oleks-netizen.github.io/product-images/20126/3.jpg,https://oleks-netizen.github.io/product-images/20126/4.jpg,https://oleks-netizen.github.io/product-images/20126/5.jpg,https://oleks-netizen.github.io/product-images/20126/6.jpg</t>
+        </is>
+      </c>
+      <c r="C203" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>20131</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20131/1.jpg,https://oleks-netizen.github.io/product-images/20131/2.jpg,https://oleks-netizen.github.io/product-images/20131/3.jpg,https://oleks-netizen.github.io/product-images/20131/4.jpg</t>
+        </is>
+      </c>
+      <c r="C204" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>20136</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20136/1.jpg,https://oleks-netizen.github.io/product-images/20136/2.jpg,https://oleks-netizen.github.io/product-images/20136/7.jpg,https://oleks-netizen.github.io/product-images/20136/3.jpg,https://oleks-netizen.github.io/product-images/20136/4.jpg,https://oleks-netizen.github.io/product-images/20136/5.jpg</t>
+        </is>
+      </c>
+      <c r="C205" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>20193</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20193/1.jpg,https://oleks-netizen.github.io/product-images/20193/2.jpg,https://oleks-netizen.github.io/product-images/20193/3.jpg,https://oleks-netizen.github.io/product-images/20193/4.jpg,https://oleks-netizen.github.io/product-images/20193/5.jpg,https://oleks-netizen.github.io/product-images/20193/6.jpg,https://oleks-netizen.github.io/product-images/20193/7.jpg,https://oleks-netizen.github.io/product-images/20193/8.jpg,https://oleks-netizen.github.io/product-images/20193/9.jpg</t>
+        </is>
+      </c>
+      <c r="C206" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>20218</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20218/1.jpg,https://oleks-netizen.github.io/product-images/20218/2.jpg,https://oleks-netizen.github.io/product-images/20218/3.jpg,https://oleks-netizen.github.io/product-images/20218/4.jpg,https://oleks-netizen.github.io/product-images/20218/5.jpg,https://oleks-netizen.github.io/product-images/20218/6.jpg,https://oleks-netizen.github.io/product-images/20218/7.jpg,https://oleks-netizen.github.io/product-images/20218/8.jpg</t>
+        </is>
+      </c>
+      <c r="C207" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>20221</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20221/1.jpg,https://oleks-netizen.github.io/product-images/20221/2.jpg,https://oleks-netizen.github.io/product-images/20221/3.jpg,https://oleks-netizen.github.io/product-images/20221/4.jpg,https://oleks-netizen.github.io/product-images/20221/5.jpg,https://oleks-netizen.github.io/product-images/20221/6.jpg,https://oleks-netizen.github.io/product-images/20221/7.jpg,https://oleks-netizen.github.io/product-images/20221/8.jpg,https://oleks-netizen.github.io/product-images/20221/9.jpg</t>
+        </is>
+      </c>
+      <c r="C208" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>20222</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20222/10.jpg,https://oleks-netizen.github.io/product-images/20222/11.jpg,https://oleks-netizen.github.io/product-images/20222/1.jpg,https://oleks-netizen.github.io/product-images/20222/2.jpg,https://oleks-netizen.github.io/product-images/20222/3.jpg,https://oleks-netizen.github.io/product-images/20222/4.jpg,https://oleks-netizen.github.io/product-images/20222/5.jpg,https://oleks-netizen.github.io/product-images/20222/6.jpg,https://oleks-netizen.github.io/product-images/20222/7.jpg,https://oleks-netizen.github.io/product-images/20222/8.jpg,https://oleks-netizen.github.io/product-images/20222/9.jpg</t>
+        </is>
+      </c>
+      <c r="C209" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>20231</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20231/1.jpg,https://oleks-netizen.github.io/product-images/20231/2.jpg,https://oleks-netizen.github.io/product-images/20231/8.jpg,https://oleks-netizen.github.io/product-images/20231/10.jpg,https://oleks-netizen.github.io/product-images/20231/3.jpg,https://oleks-netizen.github.io/product-images/20231/4.jpg,https://oleks-netizen.github.io/product-images/20231/5.jpg,https://oleks-netizen.github.io/product-images/20231/6.jpg,https://oleks-netizen.github.io/product-images/20231/7.jpg</t>
+        </is>
+      </c>
+      <c r="C210" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>20237</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20237/1.jpg,https://oleks-netizen.github.io/product-images/20237/2.jpg,https://oleks-netizen.github.io/product-images/20237/7.jpg,https://oleks-netizen.github.io/product-images/20237/11.jpg,https://oleks-netizen.github.io/product-images/20237/10.jpg,https://oleks-netizen.github.io/product-images/20237/3.jpg,https://oleks-netizen.github.io/product-images/20237/4.jpg,https://oleks-netizen.github.io/product-images/20237/6.jpg,https://oleks-netizen.github.io/product-images/20237/8.jpg,https://oleks-netizen.github.io/product-images/20237/9.jpg</t>
+        </is>
+      </c>
+      <c r="C211" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>20238</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20238/1.jpg,https://oleks-netizen.github.io/product-images/20238/2.jpg,https://oleks-netizen.github.io/product-images/20238/13.jpg,https://oleks-netizen.github.io/product-images/20238/11.jpg,https://oleks-netizen.github.io/product-images/20238/12.jpg,https://oleks-netizen.github.io/product-images/20238/3.jpg,https://oleks-netizen.github.io/product-images/20238/4.jpg,https://oleks-netizen.github.io/product-images/20238/5.jpg,https://oleks-netizen.github.io/product-images/20238/6.jpg,https://oleks-netizen.github.io/product-images/20238/7.jpg,https://oleks-netizen.github.io/product-images/20238/8.jpg,https://oleks-netizen.github.io/product-images/20238/9.jpg</t>
+        </is>
+      </c>
+      <c r="C212" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>20245</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20245/1.jpg,https://oleks-netizen.github.io/product-images/20245/2.jpg,https://oleks-netizen.github.io/product-images/20245/11.jpg,https://oleks-netizen.github.io/product-images/20245/10.jpg,https://oleks-netizen.github.io/product-images/20245/3.jpg,https://oleks-netizen.github.io/product-images/20245/4.jpg,https://oleks-netizen.github.io/product-images/20245/5.jpg,https://oleks-netizen.github.io/product-images/20245/7.jpg,https://oleks-netizen.github.io/product-images/20245/8.jpg,https://oleks-netizen.github.io/product-images/20245/9.jpg</t>
+        </is>
+      </c>
+      <c r="C213" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>20256</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20256/1.jpg,https://oleks-netizen.github.io/product-images/20256/2.jpg,https://oleks-netizen.github.io/product-images/20256/3.jpg,https://oleks-netizen.github.io/product-images/20256/4.jpg,https://oleks-netizen.github.io/product-images/20256/5.jpg,https://oleks-netizen.github.io/product-images/20256/6.jpg,https://oleks-netizen.github.io/product-images/20256/7.jpg,https://oleks-netizen.github.io/product-images/20256/8.jpg</t>
+        </is>
+      </c>
+      <c r="C214" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>20262</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20262/1.jpg,https://oleks-netizen.github.io/product-images/20262/2.jpg,https://oleks-netizen.github.io/product-images/20262/3.jpg,https://oleks-netizen.github.io/product-images/20262/4.jpg,https://oleks-netizen.github.io/product-images/20262/5.jpg,https://oleks-netizen.github.io/product-images/20262/6.jpg,https://oleks-netizen.github.io/product-images/20262/7.jpg,https://oleks-netizen.github.io/product-images/20262/8.jpg,https://oleks-netizen.github.io/product-images/20262/9.jpg</t>
+        </is>
+      </c>
+      <c r="C215" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>20263</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20263/1.jpg,https://oleks-netizen.github.io/product-images/20263/2.jpg,https://oleks-netizen.github.io/product-images/20263/3.jpg,https://oleks-netizen.github.io/product-images/20263/4.jpg,https://oleks-netizen.github.io/product-images/20263/5.jpg,https://oleks-netizen.github.io/product-images/20263/6.jpg,https://oleks-netizen.github.io/product-images/20263/7.jpg,https://oleks-netizen.github.io/product-images/20263/8.jpg,https://oleks-netizen.github.io/product-images/20263/9.jpg</t>
+        </is>
+      </c>
+      <c r="C216" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>20269</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20269/1.jpg,https://oleks-netizen.github.io/product-images/20269/2.jpg,https://oleks-netizen.github.io/product-images/20269/3.jpg,https://oleks-netizen.github.io/product-images/20269/4.jpg,https://oleks-netizen.github.io/product-images/20269/5.jpg,https://oleks-netizen.github.io/product-images/20269/6.jpg,https://oleks-netizen.github.io/product-images/20269/7.jpg,https://oleks-netizen.github.io/product-images/20269/8.jpg</t>
+        </is>
+      </c>
+      <c r="C217" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>20270</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20270/1.jpg,https://oleks-netizen.github.io/product-images/20270/2.jpg,https://oleks-netizen.github.io/product-images/20270/3.jpg,https://oleks-netizen.github.io/product-images/20270/4.jpg,https://oleks-netizen.github.io/product-images/20270/5.jpg,https://oleks-netizen.github.io/product-images/20270/6.jpg,https://oleks-netizen.github.io/product-images/20270/7.jpg,https://oleks-netizen.github.io/product-images/20270/8.jpg</t>
+        </is>
+      </c>
+      <c r="C218" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>20277</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20277/1.jpg,https://oleks-netizen.github.io/product-images/20277/2.jpg,https://oleks-netizen.github.io/product-images/20277/3.jpg,https://oleks-netizen.github.io/product-images/20277/4.jpg,https://oleks-netizen.github.io/product-images/20277/5.jpg,https://oleks-netizen.github.io/product-images/20277/6.jpg,https://oleks-netizen.github.io/product-images/20277/7.jpg,https://oleks-netizen.github.io/product-images/20277/8.jpg</t>
+        </is>
+      </c>
+      <c r="C219" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>20279</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20279/1.jpg,https://oleks-netizen.github.io/product-images/20279/2.jpg,https://oleks-netizen.github.io/product-images/20279/3.jpg,https://oleks-netizen.github.io/product-images/20279/4.jpg,https://oleks-netizen.github.io/product-images/20279/5.jpg,https://oleks-netizen.github.io/product-images/20279/6.jpg,https://oleks-netizen.github.io/product-images/20279/7.jpg,https://oleks-netizen.github.io/product-images/20279/8.jpg</t>
+        </is>
+      </c>
+      <c r="C220" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>20289</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20289/1.jpg,https://oleks-netizen.github.io/product-images/20289/2.jpg,https://oleks-netizen.github.io/product-images/20289/3.jpg,https://oleks-netizen.github.io/product-images/20289/4.jpg,https://oleks-netizen.github.io/product-images/20289/5.jpg,https://oleks-netizen.github.io/product-images/20289/6.jpg</t>
+        </is>
+      </c>
+      <c r="C221" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>20309</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20309/1.jpg,https://oleks-netizen.github.io/product-images/20309/2.jpg,https://oleks-netizen.github.io/product-images/20309/3.jpg,https://oleks-netizen.github.io/product-images/20309/4.jpg,https://oleks-netizen.github.io/product-images/20309/5.jpg,https://oleks-netizen.github.io/product-images/20309/6.jpg,https://oleks-netizen.github.io/product-images/20309/7.jpg,https://oleks-netizen.github.io/product-images/20309/8.jpg,https://oleks-netizen.github.io/product-images/20309/9.jpg</t>
+        </is>
+      </c>
+      <c r="C222" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>20312</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20312/1.jpg,https://oleks-netizen.github.io/product-images/20312/2.jpg,https://oleks-netizen.github.io/product-images/20312/3.jpg,https://oleks-netizen.github.io/product-images/20312/4.jpg,https://oleks-netizen.github.io/product-images/20312/5.jpg,https://oleks-netizen.github.io/product-images/20312/6.jpg,https://oleks-netizen.github.io/product-images/20312/7.jpg,https://oleks-netizen.github.io/product-images/20312/8.jpg</t>
+        </is>
+      </c>
+      <c r="C223" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>20314</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20314/1.jpg,https://oleks-netizen.github.io/product-images/20314/2.jpg,https://oleks-netizen.github.io/product-images/20314/3.jpg,https://oleks-netizen.github.io/product-images/20314/4.jpg,https://oleks-netizen.github.io/product-images/20314/5.jpg,https://oleks-netizen.github.io/product-images/20314/6.jpg,https://oleks-netizen.github.io/product-images/20314/7.jpg,https://oleks-netizen.github.io/product-images/20314/8.jpg</t>
+        </is>
+      </c>
+      <c r="C224" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>20416</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20416/10.jpg,https://oleks-netizen.github.io/product-images/20416/1.jpg,https://oleks-netizen.github.io/product-images/20416/2.jpg,https://oleks-netizen.github.io/product-images/20416/3.jpg,https://oleks-netizen.github.io/product-images/20416/4.jpg,https://oleks-netizen.github.io/product-images/20416/5.jpg,https://oleks-netizen.github.io/product-images/20416/6.jpg,https://oleks-netizen.github.io/product-images/20416/7.jpg,https://oleks-netizen.github.io/product-images/20416/8.jpg,https://oleks-netizen.github.io/product-images/20416/9.jpg</t>
+        </is>
+      </c>
+      <c r="C225" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>20441</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20441/1.jpg,https://oleks-netizen.github.io/product-images/20441/2.jpg,https://oleks-netizen.github.io/product-images/20441/3.jpg,https://oleks-netizen.github.io/product-images/20441/4.jpg,https://oleks-netizen.github.io/product-images/20441/5.jpg,https://oleks-netizen.github.io/product-images/20441/6.jpg,https://oleks-netizen.github.io/product-images/20441/7.jpg,https://oleks-netizen.github.io/product-images/20441/8.jpg,https://oleks-netizen.github.io/product-images/20441/9.jpg</t>
+        </is>
+      </c>
+      <c r="C226" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>20442</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20442/10.jpg,https://oleks-netizen.github.io/product-images/20442/1.jpg,https://oleks-netizen.github.io/product-images/20442/2.jpg,https://oleks-netizen.github.io/product-images/20442/3.jpg,https://oleks-netizen.github.io/product-images/20442/4.jpg,https://oleks-netizen.github.io/product-images/20442/5.jpg,https://oleks-netizen.github.io/product-images/20442/6.jpg,https://oleks-netizen.github.io/product-images/20442/7.jpg,https://oleks-netizen.github.io/product-images/20442/8.jpg,https://oleks-netizen.github.io/product-images/20442/9.jpg</t>
+        </is>
+      </c>
+      <c r="C227" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>20451</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/20451/1.jpg,https://oleks-netizen.github.io/product-images/20451/2.jpg,https://oleks-netizen.github.io/product-images/20451/3.jpg,https://oleks-netizen.github.io/product-images/20451/4.jpg,https://oleks-netizen.github.io/product-images/20451/5.jpg,https://oleks-netizen.github.io/product-images/20451/6.jpg,https://oleks-netizen.github.io/product-images/20451/7.jpg</t>
+        </is>
+      </c>
+      <c r="C228" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>21246</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/21246/1.jpg,https://oleks-netizen.github.io/product-images/21246/2.jpg,https://oleks-netizen.github.io/product-images/21246/3.jpg,https://oleks-netizen.github.io/product-images/21246/4.jpg,https://oleks-netizen.github.io/product-images/21246/5.jpg,https://oleks-netizen.github.io/product-images/21246/6.jpg,https://oleks-netizen.github.io/product-images/21246/7.jpg,https://oleks-netizen.github.io/product-images/21246/8.jpg,https://oleks-netizen.github.io/product-images/21246/9.jpg</t>
+        </is>
+      </c>
+      <c r="C229" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>21258</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/21258/10.jpg,https://oleks-netizen.github.io/product-images/21258/11.jpg,https://oleks-netizen.github.io/product-images/21258/1.jpg,https://oleks-netizen.github.io/product-images/21258/2.jpg,https://oleks-netizen.github.io/product-images/21258/3.jpg,https://oleks-netizen.github.io/product-images/21258/4.jpg,https://oleks-netizen.github.io/product-images/21258/5.jpg,https://oleks-netizen.github.io/product-images/21258/6.jpg,https://oleks-netizen.github.io/product-images/21258/7.jpg,https://oleks-netizen.github.io/product-images/21258/8.jpg,https://oleks-netizen.github.io/product-images/21258/9.jpg</t>
+        </is>
+      </c>
+      <c r="C230" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>21264</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/21264/10.jpg,https://oleks-netizen.github.io/product-images/21264/11.jpg,https://oleks-netizen.github.io/product-images/21264/1.jpg,https://oleks-netizen.github.io/product-images/21264/2.jpg,https://oleks-netizen.github.io/product-images/21264/3.jpg,https://oleks-netizen.github.io/product-images/21264/4.jpg,https://oleks-netizen.github.io/product-images/21264/5.jpg,https://oleks-netizen.github.io/product-images/21264/6.jpg,https://oleks-netizen.github.io/product-images/21264/7.jpg,https://oleks-netizen.github.io/product-images/21264/8.jpg,https://oleks-netizen.github.io/product-images/21264/9.jpg</t>
+        </is>
+      </c>
+      <c r="C231" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>21265</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/21265/10.jpg,https://oleks-netizen.github.io/product-images/21265/11.jpg,https://oleks-netizen.github.io/product-images/21265/1.jpg,https://oleks-netizen.github.io/product-images/21265/2.jpg,https://oleks-netizen.github.io/product-images/21265/3.jpg,https://oleks-netizen.github.io/product-images/21265/4.jpg,https://oleks-netizen.github.io/product-images/21265/5.jpg,https://oleks-netizen.github.io/product-images/21265/6.jpg,https://oleks-netizen.github.io/product-images/21265/7.jpg,https://oleks-netizen.github.io/product-images/21265/8.jpg,https://oleks-netizen.github.io/product-images/21265/9.jpg</t>
+        </is>
+      </c>
+      <c r="C232" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>21266</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/21266/10.jpg,https://oleks-netizen.github.io/product-images/21266/1.jpg,https://oleks-netizen.github.io/product-images/21266/2.jpg,https://oleks-netizen.github.io/product-images/21266/3.jpg,https://oleks-netizen.github.io/product-images/21266/4.jpg,https://oleks-netizen.github.io/product-images/21266/5.jpg,https://oleks-netizen.github.io/product-images/21266/6.jpg,https://oleks-netizen.github.io/product-images/21266/7.jpg,https://oleks-netizen.github.io/product-images/21266/8.jpg,https://oleks-netizen.github.io/product-images/21266/9.jpg</t>
+        </is>
+      </c>
+      <c r="C233" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>21274</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/21274/10.jpg,https://oleks-netizen.github.io/product-images/21274/1.jpg,https://oleks-netizen.github.io/product-images/21274/2.jpg,https://oleks-netizen.github.io/product-images/21274/3.jpg,https://oleks-netizen.github.io/product-images/21274/4.jpg,https://oleks-netizen.github.io/product-images/21274/5.jpg,https://oleks-netizen.github.io/product-images/21274/6.jpg,https://oleks-netizen.github.io/product-images/21274/7.jpg,https://oleks-netizen.github.io/product-images/21274/8.jpg,https://oleks-netizen.github.io/product-images/21274/9.jpg</t>
+        </is>
+      </c>
+      <c r="C234" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>21276</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/21276/1.jpg,https://oleks-netizen.github.io/product-images/21276/2.jpg,https://oleks-netizen.github.io/product-images/21276/12.jpg,https://oleks-netizen.github.io/product-images/21276/10.jpg,https://oleks-netizen.github.io/product-images/21276/11.jpg,https://oleks-netizen.github.io/product-images/21276/3.jpg,https://oleks-netizen.github.io/product-images/21276/4.jpg,https://oleks-netizen.github.io/product-images/21276/5.jpg,https://oleks-netizen.github.io/product-images/21276/6.jpg,https://oleks-netizen.github.io/product-images/21276/8.jpg,https://oleks-netizen.github.io/product-images/21276/9.jpg</t>
+        </is>
+      </c>
+      <c r="C235" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>21301</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/21301/10.jpg,https://oleks-netizen.github.io/product-images/21301/11.jpg,https://oleks-netizen.github.io/product-images/21301/1.jpg,https://oleks-netizen.github.io/product-images/21301/2.jpg,https://oleks-netizen.github.io/product-images/21301/3.jpg,https://oleks-netizen.github.io/product-images/21301/4.jpg,https://oleks-netizen.github.io/product-images/21301/5.jpg,https://oleks-netizen.github.io/product-images/21301/6.jpg,https://oleks-netizen.github.io/product-images/21301/7.jpg,https://oleks-netizen.github.io/product-images/21301/8.jpg,https://oleks-netizen.github.io/product-images/21301/9.jpg</t>
+        </is>
+      </c>
+      <c r="C236" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>21482</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/21482/10.jpg,https://oleks-netizen.github.io/product-images/21482/1.jpg,https://oleks-netizen.github.io/product-images/21482/2.jpg,https://oleks-netizen.github.io/product-images/21482/3.jpg,https://oleks-netizen.github.io/product-images/21482/4.jpg,https://oleks-netizen.github.io/product-images/21482/5.jpg,https://oleks-netizen.github.io/product-images/21482/6.jpg,https://oleks-netizen.github.io/product-images/21482/7.jpg,https://oleks-netizen.github.io/product-images/21482/8.jpg,https://oleks-netizen.github.io/product-images/21482/9.jpg</t>
+        </is>
+      </c>
+      <c r="C237" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>22078</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/22078/1.jpg,https://oleks-netizen.github.io/product-images/22078/2.jpg,https://oleks-netizen.github.io/product-images/22078/12.jpg,https://oleks-netizen.github.io/product-images/22078/10.jpg,https://oleks-netizen.github.io/product-images/22078/11.jpg,https://oleks-netizen.github.io/product-images/22078/3.jpg,https://oleks-netizen.github.io/product-images/22078/4.jpg,https://oleks-netizen.github.io/product-images/22078/5.jpg,https://oleks-netizen.github.io/product-images/22078/6.jpg,https://oleks-netizen.github.io/product-images/22078/8.jpg,https://oleks-netizen.github.io/product-images/22078/9.jpg</t>
+        </is>
+      </c>
+      <c r="C238" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>22082</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/22082/10.jpg,https://oleks-netizen.github.io/product-images/22082/1.jpg,https://oleks-netizen.github.io/product-images/22082/2.jpg,https://oleks-netizen.github.io/product-images/22082/3.jpg,https://oleks-netizen.github.io/product-images/22082/4.jpg,https://oleks-netizen.github.io/product-images/22082/5.jpg,https://oleks-netizen.github.io/product-images/22082/6.jpg,https://oleks-netizen.github.io/product-images/22082/7.jpg,https://oleks-netizen.github.io/product-images/22082/8.jpg,https://oleks-netizen.github.io/product-images/22082/9.jpg</t>
+        </is>
+      </c>
+      <c r="C239" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>22087</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/22087/10.jpg,https://oleks-netizen.github.io/product-images/22087/11.jpg,https://oleks-netizen.github.io/product-images/22087/1.jpg,https://oleks-netizen.github.io/product-images/22087/2.jpg,https://oleks-netizen.github.io/product-images/22087/3.jpg,https://oleks-netizen.github.io/product-images/22087/4.jpg,https://oleks-netizen.github.io/product-images/22087/5.jpg,https://oleks-netizen.github.io/product-images/22087/6.jpg,https://oleks-netizen.github.io/product-images/22087/7.jpg,https://oleks-netizen.github.io/product-images/22087/8.jpg,https://oleks-netizen.github.io/product-images/22087/9.jpg</t>
+        </is>
+      </c>
+      <c r="C240" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>22088</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/22088/10.jpg,https://oleks-netizen.github.io/product-images/22088/1.jpg,https://oleks-netizen.github.io/product-images/22088/2.jpg,https://oleks-netizen.github.io/product-images/22088/3.jpg,https://oleks-netizen.github.io/product-images/22088/4.jpg,https://oleks-netizen.github.io/product-images/22088/5.jpg,https://oleks-netizen.github.io/product-images/22088/6.jpg,https://oleks-netizen.github.io/product-images/22088/7.jpg,https://oleks-netizen.github.io/product-images/22088/8.jpg,https://oleks-netizen.github.io/product-images/22088/9.jpg</t>
+        </is>
+      </c>
+      <c r="C241" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>22094</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/22094/10.jpg,https://oleks-netizen.github.io/product-images/22094/11.jpg,https://oleks-netizen.github.io/product-images/22094/1.jpg,https://oleks-netizen.github.io/product-images/22094/2.jpg,https://oleks-netizen.github.io/product-images/22094/3.jpg,https://oleks-netizen.github.io/product-images/22094/4.jpg,https://oleks-netizen.github.io/product-images/22094/5.jpg,https://oleks-netizen.github.io/product-images/22094/6.jpg,https://oleks-netizen.github.io/product-images/22094/7.jpg,https://oleks-netizen.github.io/product-images/22094/8.jpg,https://oleks-netizen.github.io/product-images/22094/9.jpg</t>
+        </is>
+      </c>
+      <c r="C242" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>22116</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/22116/10.jpg,https://oleks-netizen.github.io/product-images/22116/1.jpg,https://oleks-netizen.github.io/product-images/22116/2.jpg,https://oleks-netizen.github.io/product-images/22116/3.jpg,https://oleks-netizen.github.io/product-images/22116/4.jpg,https://oleks-netizen.github.io/product-images/22116/5.jpg,https://oleks-netizen.github.io/product-images/22116/6.jpg,https://oleks-netizen.github.io/product-images/22116/7.jpg,https://oleks-netizen.github.io/product-images/22116/8.jpg,https://oleks-netizen.github.io/product-images/22116/9.jpg</t>
+        </is>
+      </c>
+      <c r="C243" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>22125</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/22125/10.jpg,https://oleks-netizen.github.io/product-images/22125/1.jpg,https://oleks-netizen.github.io/product-images/22125/2.jpg,https://oleks-netizen.github.io/product-images/22125/3.jpg,https://oleks-netizen.github.io/product-images/22125/4.jpg,https://oleks-netizen.github.io/product-images/22125/5.jpg,https://oleks-netizen.github.io/product-images/22125/6.jpg,https://oleks-netizen.github.io/product-images/22125/7.jpg,https://oleks-netizen.github.io/product-images/22125/8.jpg,https://oleks-netizen.github.io/product-images/22125/9.jpg</t>
+        </is>
+      </c>
+      <c r="C244" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>Cv1gnn16-115</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/Cv1gnn16-115/1.jpg,https://oleks-netizen.github.io/product-images/Cv1gnn16-115/2.jpg</t>
+        </is>
+      </c>
+      <c r="C245" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>Cv1gnn28-125</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/Cv1gnn28-125/1.jpg,https://oleks-netizen.github.io/product-images/Cv1gnn28-125/2.jpg</t>
+        </is>
+      </c>
+      <c r="C246" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>CV1gnn38-115</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/CV1gnn38-115/1.jpg,https://oleks-netizen.github.io/product-images/CV1gnn38-115/2.jpg</t>
+        </is>
+      </c>
+      <c r="C247" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>G853-035146</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/G853-035146/1.jpg,https://oleks-netizen.github.io/product-images/G853-035146/2.jpg,https://oleks-netizen.github.io/product-images/G853-035146/12.jpg,https://oleks-netizen.github.io/product-images/G853-035146/10.jpg,https://oleks-netizen.github.io/product-images/G853-035146/11.jpg,https://oleks-netizen.github.io/product-images/G853-035146/4.jpg,https://oleks-netizen.github.io/product-images/G853-035146/5.jpg,https://oleks-netizen.github.io/product-images/G853-035146/6.jpg,https://oleks-netizen.github.io/product-images/G853-035146/7.jpg,https://oleks-netizen.github.io/product-images/G853-035146/8.jpg,https://oleks-netizen.github.io/product-images/G853-035146/9.jpg</t>
+        </is>
+      </c>
+      <c r="C248" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>JBNC39MN TAN</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/JBNC39MN TAN/1.jpg,https://oleks-netizen.github.io/product-images/JBNC39MN TAN/2.jpg,https://oleks-netizen.github.io/product-images/JBNC39MN TAN/6.jpg,https://oleks-netizen.github.io/product-images/JBNC39MN TAN/7.jpg,https://oleks-netizen.github.io/product-images/JBNC39MN TAN/3.jpg,https://oleks-netizen.github.io/product-images/JBNC39MN TAN/5.jpg</t>
+        </is>
+      </c>
+      <c r="C249" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>k1001b-black</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/k1001b-black/1.jpg,https://oleks-netizen.github.io/product-images/k1001b-black/2.jpg,https://oleks-netizen.github.io/product-images/k1001b-black/9.jpg,https://oleks-netizen.github.io/product-images/k1001b-black/3.jpg,https://oleks-netizen.github.io/product-images/k1001b-black/4.jpg,https://oleks-netizen.github.io/product-images/k1001b-black/5.jpg,https://oleks-netizen.github.io/product-images/k1001b-black/6.jpg,https://oleks-netizen.github.io/product-images/k1001b-black/8.jpg</t>
+        </is>
+      </c>
+      <c r="C250" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>K11031-black</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/K11031-black/1.jpg,https://oleks-netizen.github.io/product-images/K11031-black/2.jpg,https://oleks-netizen.github.io/product-images/K11031-black/9.jpg,https://oleks-netizen.github.io/product-images/K11031-black/4.jpg,https://oleks-netizen.github.io/product-images/K11031-black/5.jpg,https://oleks-netizen.github.io/product-images/K11031-black/6.jpg,https://oleks-netizen.github.io/product-images/K11031-black/7.jpg,https://oleks-netizen.github.io/product-images/K11031-black/8.jpg</t>
+        </is>
+      </c>
+      <c r="C251" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>K11031-dark brown</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/K11031-dark brown/1.jpg,https://oleks-netizen.github.io/product-images/K11031-dark brown/2.jpg,https://oleks-netizen.github.io/product-images/K11031-dark brown/3.jpg,https://oleks-netizen.github.io/product-images/K11031-dark brown/4.jpg,https://oleks-netizen.github.io/product-images/K11031-dark brown/5.jpg,https://oleks-netizen.github.io/product-images/K11031-dark brown/6.jpg,https://oleks-netizen.github.io/product-images/K11031-dark brown/7.jpg</t>
+        </is>
+      </c>
+      <c r="C252" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>k11120a-black</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/k11120a-black/1.jpg,https://oleks-netizen.github.io/product-images/k11120a-black/2.jpg,https://oleks-netizen.github.io/product-images/k11120a-black/3.jpg,https://oleks-netizen.github.io/product-images/k11120a-black/4.jpg,https://oleks-netizen.github.io/product-images/k11120a-black/5.jpg,https://oleks-netizen.github.io/product-images/k11120a-black/6.jpg,https://oleks-netizen.github.io/product-images/k11120a-black/7.jpg,https://oleks-netizen.github.io/product-images/k11120a-black/8.jpg</t>
+        </is>
+      </c>
+      <c r="C253" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>K12335-blue</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/K12335-blue/1.jpg,https://oleks-netizen.github.io/product-images/K12335-blue/2.jpg,https://oleks-netizen.github.io/product-images/K12335-blue/9.jpg,https://oleks-netizen.github.io/product-images/K12335-blue/3.jpg,https://oleks-netizen.github.io/product-images/K12335-blue/4.jpg,https://oleks-netizen.github.io/product-images/K12335-blue/5.jpg,https://oleks-netizen.github.io/product-images/K12335-blue/6.jpg,https://oleks-netizen.github.io/product-images/K12335-blue/7.jpg</t>
+        </is>
+      </c>
+      <c r="C254" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>K12335-red</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/K12335-red/1.jpg,https://oleks-netizen.github.io/product-images/K12335-red/2.jpg,https://oleks-netizen.github.io/product-images/K12335-red/9.jpg,https://oleks-netizen.github.io/product-images/K12335-red/3.jpg,https://oleks-netizen.github.io/product-images/K12335-red/4.jpg,https://oleks-netizen.github.io/product-images/K12335-red/5.jpg,https://oleks-netizen.github.io/product-images/K12335-red/6.jpg,https://oleks-netizen.github.io/product-images/K12335-red/8.jpg</t>
+        </is>
+      </c>
+      <c r="C255" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>K1a0001-bordo</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/K1a0001-bordo/1.jpg,https://oleks-netizen.github.io/product-images/K1a0001-bordo/2.jpg,https://oleks-netizen.github.io/product-images/K1a0001-bordo/9.jpg,https://oleks-netizen.github.io/product-images/K1a0001-bordo/3.jpg,https://oleks-netizen.github.io/product-images/K1a0001-bordo/4.jpg,https://oleks-netizen.github.io/product-images/K1a0001-bordo/5.jpg,https://oleks-netizen.github.io/product-images/K1a0001-bordo/7.jpg,https://oleks-netizen.github.io/product-images/K1a0001-bordo/8.jpg</t>
+        </is>
+      </c>
+      <c r="C256" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>K1b837-green</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/K1b837-green/1.jpg,https://oleks-netizen.github.io/product-images/K1b837-green/2.jpg,https://oleks-netizen.github.io/product-images/K1b837-green/9.jpg,https://oleks-netizen.github.io/product-images/K1b837-green/4.jpg,https://oleks-netizen.github.io/product-images/K1b837-green/5.jpg,https://oleks-netizen.github.io/product-images/K1b837-green/6.jpg,https://oleks-netizen.github.io/product-images/K1b837-green/7.jpg,https://oleks-netizen.github.io/product-images/K1b837-green/8.jpg</t>
+        </is>
+      </c>
+      <c r="C257" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>L346-020388</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L346-020388/1.jpg,https://oleks-netizen.github.io/product-images/L346-020388/2.jpg,https://oleks-netizen.github.io/product-images/L346-020388/5.jpg,https://oleks-netizen.github.io/product-images/L346-020388/10.jpg,https://oleks-netizen.github.io/product-images/L346-020388/3.jpg,https://oleks-netizen.github.io/product-images/L346-020388/4.jpg,https://oleks-netizen.github.io/product-images/L346-020388/7.jpg,https://oleks-netizen.github.io/product-images/L346-020388/8.jpg,https://oleks-netizen.github.io/product-images/L346-020388/9.jpg</t>
+        </is>
+      </c>
+      <c r="C258" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>L501-040010</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L501-040010/1.jpg,https://oleks-netizen.github.io/product-images/L501-040010/2.jpg,https://oleks-netizen.github.io/product-images/L501-040010/9.jpg,https://oleks-netizen.github.io/product-images/L501-040010/4.jpg,https://oleks-netizen.github.io/product-images/L501-040010/5.jpg,https://oleks-netizen.github.io/product-images/L501-040010/6.jpg,https://oleks-netizen.github.io/product-images/L501-040010/7.jpg,https://oleks-netizen.github.io/product-images/L501-040010/8.jpg</t>
+        </is>
+      </c>
+      <c r="C259" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>L754-028148</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L754-028148/10.jpg,https://oleks-netizen.github.io/product-images/L754-028148/11.jpg,https://oleks-netizen.github.io/product-images/L754-028148/12.jpg,https://oleks-netizen.github.io/product-images/L754-028148/1.jpg,https://oleks-netizen.github.io/product-images/L754-028148/2.jpg,https://oleks-netizen.github.io/product-images/L754-028148/3.jpg,https://oleks-netizen.github.io/product-images/L754-028148/4.jpg,https://oleks-netizen.github.io/product-images/L754-028148/5.jpg,https://oleks-netizen.github.io/product-images/L754-028148/6.jpg,https://oleks-netizen.github.io/product-images/L754-028148/7.jpg,https://oleks-netizen.github.io/product-images/L754-028148/8.jpg,https://oleks-netizen.github.io/product-images/L754-028148/9.jpg</t>
+        </is>
+      </c>
+      <c r="C260" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>L891-037263</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L891-037263/1.jpg,https://oleks-netizen.github.io/product-images/L891-037263/2.jpg,https://oleks-netizen.github.io/product-images/L891-037263/5.jpg,https://oleks-netizen.github.io/product-images/L891-037263/14.jpg,https://oleks-netizen.github.io/product-images/L891-037263/10.jpg,https://oleks-netizen.github.io/product-images/L891-037263/11.jpg,https://oleks-netizen.github.io/product-images/L891-037263/12.jpg,https://oleks-netizen.github.io/product-images/L891-037263/13.jpg,https://oleks-netizen.github.io/product-images/L891-037263/4.jpg,https://oleks-netizen.github.io/product-images/L891-037263/6.jpg,https://oleks-netizen.github.io/product-images/L891-037263/7.jpg,https://oleks-netizen.github.io/product-images/L891-037263/8.jpg,https://oleks-netizen.github.io/product-images/L891-037263/9.jpg</t>
+        </is>
+      </c>
+      <c r="C261" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>L902-038857</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L902-038857/1.jpg,https://oleks-netizen.github.io/product-images/L902-038857/2.jpg,https://oleks-netizen.github.io/product-images/L902-038857/9.jpg,https://oleks-netizen.github.io/product-images/L902-038857/4.jpg,https://oleks-netizen.github.io/product-images/L902-038857/5.jpg,https://oleks-netizen.github.io/product-images/L902-038857/6.jpg,https://oleks-netizen.github.io/product-images/L902-038857/7.jpg,https://oleks-netizen.github.io/product-images/L902-038857/8.jpg</t>
+        </is>
+      </c>
+      <c r="C262" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>L908-039595</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L908-039595/1.jpg,https://oleks-netizen.github.io/product-images/L908-039595/2.jpg,https://oleks-netizen.github.io/product-images/L908-039595/6.jpg,https://oleks-netizen.github.io/product-images/L908-039595/16.jpg,https://oleks-netizen.github.io/product-images/L908-039595/10.jpg,https://oleks-netizen.github.io/product-images/L908-039595/11.jpg,https://oleks-netizen.github.io/product-images/L908-039595/12.jpg,https://oleks-netizen.github.io/product-images/L908-039595/13.jpg,https://oleks-netizen.github.io/product-images/L908-039595/14.jpg,https://oleks-netizen.github.io/product-images/L908-039595/15.jpg,https://oleks-netizen.github.io/product-images/L908-039595/3.jpg,https://oleks-netizen.github.io/product-images/L908-039595/4.jpg,https://oleks-netizen.github.io/product-images/L908-039595/5.jpg,https://oleks-netizen.github.io/product-images/L908-039595/8.jpg,https://oleks-netizen.github.io/product-images/L908-039595/9.jpg</t>
+        </is>
+      </c>
+      <c r="C263" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>L926-039984</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/L926-039984/1.jpg,https://oleks-netizen.github.io/product-images/L926-039984/2.jpg,https://oleks-netizen.github.io/product-images/L926-039984/10.jpg,https://oleks-netizen.github.io/product-images/L926-039984/4.jpg,https://oleks-netizen.github.io/product-images/L926-039984/5.jpg,https://oleks-netizen.github.io/product-images/L926-039984/6.jpg,https://oleks-netizen.github.io/product-images/L926-039984/7.jpg,https://oleks-netizen.github.io/product-images/L926-039984/8.jpg,https://oleks-netizen.github.io/product-images/L926-039984/9.jpg</t>
+        </is>
+      </c>
+      <c r="C264" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>V1115GX19-brown</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/V1115GX19-brown/1.jpg,https://oleks-netizen.github.io/product-images/V1115GX19-brown/2.jpg</t>
+        </is>
+      </c>
+      <c r="C265" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>V1125GX11-black</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/V1125GX11-black/1.jpg,https://oleks-netizen.github.io/product-images/V1125GX11-black/2.jpg</t>
+        </is>
+      </c>
+      <c r="C266" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>V1WLT07-yellow</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>https://oleks-netizen.github.io/product-images/V1WLT07-yellow/1.jpg,https://oleks-netizen.github.io/product-images/V1WLT07-yellow/2.jpg,https://oleks-netizen.github.io/product-images/V1WLT07-yellow/3.jpg,https://oleks-netizen.github.io/product-images/V1WLT07-yellow/4.jpg,https://oleks-netizen.github.io/product-images/V1WLT07-yellow/5.jpg</t>
+        </is>
+      </c>
+      <c r="C267" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto update 2026-02-28 18:11:41
</commit_message>
<xml_diff>
--- a/articles_summary.xlsx
+++ b/articles_summary.xlsx
@@ -446,7 +446,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/00237/1.jpg,https://oleks-netizen.github.io/product-images/00237/2.jpg,https://oleks-netizen.github.io/product-images/00237/3.jpg,https://oleks-netizen.github.io/product-images/00237/4.jpg,https://oleks-netizen.github.io/product-images/00237/5.jpg,https://oleks-netizen.github.io/product-images/00237/6.jpg,https://oleks-netizen.github.io/product-images/00237/7.jpg,https://oleks-netizen.github.io/product-images/00237/8.jpg,https://oleks-netizen.github.io/product-images/00237/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/00237/01.jpg,https://oleks-netizen.github.io/product-images/00237/02.jpg,https://oleks-netizen.github.io/product-images/00237/03.jpg,https://oleks-netizen.github.io/product-images/00237/04.jpg,https://oleks-netizen.github.io/product-images/00237/05.jpg,https://oleks-netizen.github.io/product-images/00237/06.jpg,https://oleks-netizen.github.io/product-images/00237/07.jpg,https://oleks-netizen.github.io/product-images/00237/08.jpg,https://oleks-netizen.github.io/product-images/00237/09.jpg</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -461,7 +461,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/100v1genw91-white/1.jpg,https://oleks-netizen.github.io/product-images/100v1genw91-white/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/100v1genw91-white/01.jpg,https://oleks-netizen.github.io/product-images/100v1genw91-white/02.jpg</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -476,7 +476,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/11051/1.jpg,https://oleks-netizen.github.io/product-images/11051/2.jpg,https://oleks-netizen.github.io/product-images/11051/12.jpg,https://oleks-netizen.github.io/product-images/11051/10.jpg,https://oleks-netizen.github.io/product-images/11051/11.jpg,https://oleks-netizen.github.io/product-images/11051/3.jpg,https://oleks-netizen.github.io/product-images/11051/5.jpg,https://oleks-netizen.github.io/product-images/11051/6.jpg,https://oleks-netizen.github.io/product-images/11051/7.jpg,https://oleks-netizen.github.io/product-images/11051/8.jpg,https://oleks-netizen.github.io/product-images/11051/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/11051/01.jpg,https://oleks-netizen.github.io/product-images/11051/02.jpg,https://oleks-netizen.github.io/product-images/11051/12.jpg,https://oleks-netizen.github.io/product-images/11051/10.jpg,https://oleks-netizen.github.io/product-images/11051/11.jpg,https://oleks-netizen.github.io/product-images/11051/03.jpg,https://oleks-netizen.github.io/product-images/11051/05.jpg,https://oleks-netizen.github.io/product-images/11051/06.jpg,https://oleks-netizen.github.io/product-images/11051/07.jpg,https://oleks-netizen.github.io/product-images/11051/08.jpg,https://oleks-netizen.github.io/product-images/11051/09.jpg</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -491,7 +491,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/110v1genw14/1.jpg,https://oleks-netizen.github.io/product-images/110v1genw14/2.jpg,https://oleks-netizen.github.io/product-images/110v1genw14/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/110v1genw14/01.jpg,https://oleks-netizen.github.io/product-images/110v1genw14/02.jpg,https://oleks-netizen.github.io/product-images/110v1genw14/03.jpg</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -506,7 +506,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/110v1genw64-black/1.jpg,https://oleks-netizen.github.io/product-images/110v1genw64-black/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/110v1genw64-black/01.jpg,https://oleks-netizen.github.io/product-images/110v1genw64-black/02.jpg</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -521,7 +521,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/115v1fx90-black/1.jpg,https://oleks-netizen.github.io/product-images/115v1fx90-black/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/115v1fx90-black/01.jpg,https://oleks-netizen.github.io/product-images/115v1fx90-black/02.jpg</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -536,7 +536,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/115v1gen41/1.jpg,https://oleks-netizen.github.io/product-images/115v1gen41/2.jpg,https://oleks-netizen.github.io/product-images/115v1gen41/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/115v1gen41/01.jpg,https://oleks-netizen.github.io/product-images/115v1gen41/02.jpg,https://oleks-netizen.github.io/product-images/115v1gen41/03.jpg</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -551,7 +551,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/115vfx82-black/1.jpg,https://oleks-netizen.github.io/product-images/115vfx82-black/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/115vfx82-black/01.jpg,https://oleks-netizen.github.io/product-images/115vfx82-black/02.jpg</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -566,7 +566,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/125v1genav9/1.jpg,https://oleks-netizen.github.io/product-images/125v1genav9/2.jpg,https://oleks-netizen.github.io/product-images/125v1genav9/3.jpg,https://oleks-netizen.github.io/product-images/125v1genav9/4.jpg,https://oleks-netizen.github.io/product-images/125v1genav9/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/125v1genav9/01.jpg,https://oleks-netizen.github.io/product-images/125v1genav9/02.jpg,https://oleks-netizen.github.io/product-images/125v1genav9/03.jpg,https://oleks-netizen.github.io/product-images/125v1genav9/04.jpg,https://oleks-netizen.github.io/product-images/125v1genav9/05.jpg</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -581,7 +581,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/125vfx83-black/1.jpg,https://oleks-netizen.github.io/product-images/125vfx83-black/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/125vfx83-black/01.jpg,https://oleks-netizen.github.io/product-images/125vfx83-black/02.jpg</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -596,7 +596,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/13914/1.jpg,https://oleks-netizen.github.io/product-images/13914/2.jpg,https://oleks-netizen.github.io/product-images/13914/7.jpg,https://oleks-netizen.github.io/product-images/13914/3.jpg,https://oleks-netizen.github.io/product-images/13914/4.jpg,https://oleks-netizen.github.io/product-images/13914/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/13914/01.jpg,https://oleks-netizen.github.io/product-images/13914/02.jpg,https://oleks-netizen.github.io/product-images/13914/07.jpg,https://oleks-netizen.github.io/product-images/13914/03.jpg,https://oleks-netizen.github.io/product-images/13914/04.jpg,https://oleks-netizen.github.io/product-images/13914/06.jpg</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -611,7 +611,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/13928/1.jpg,https://oleks-netizen.github.io/product-images/13928/2.jpg,https://oleks-netizen.github.io/product-images/13928/6.jpg,https://oleks-netizen.github.io/product-images/13928/4.jpg,https://oleks-netizen.github.io/product-images/13928/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/13928/01.jpg,https://oleks-netizen.github.io/product-images/13928/02.jpg,https://oleks-netizen.github.io/product-images/13928/06.jpg,https://oleks-netizen.github.io/product-images/13928/04.jpg,https://oleks-netizen.github.io/product-images/13928/05.jpg</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -626,7 +626,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/13929/1.jpg,https://oleks-netizen.github.io/product-images/13929/2.jpg,https://oleks-netizen.github.io/product-images/13929/6.jpg,https://oleks-netizen.github.io/product-images/13929/4.jpg,https://oleks-netizen.github.io/product-images/13929/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/13929/01.jpg,https://oleks-netizen.github.io/product-images/13929/02.jpg,https://oleks-netizen.github.io/product-images/13929/06.jpg,https://oleks-netizen.github.io/product-images/13929/04.jpg,https://oleks-netizen.github.io/product-images/13929/05.jpg</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -641,7 +641,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/13960/1.jpg,https://oleks-netizen.github.io/product-images/13960/2.jpg,https://oleks-netizen.github.io/product-images/13960/7.jpg,https://oleks-netizen.github.io/product-images/13960/3.jpg,https://oleks-netizen.github.io/product-images/13960/4.jpg,https://oleks-netizen.github.io/product-images/13960/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/13960/01.jpg,https://oleks-netizen.github.io/product-images/13960/02.jpg,https://oleks-netizen.github.io/product-images/13960/07.jpg,https://oleks-netizen.github.io/product-images/13960/03.jpg,https://oleks-netizen.github.io/product-images/13960/04.jpg,https://oleks-netizen.github.io/product-images/13960/05.jpg</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -656,7 +656,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14050/1.jpg,https://oleks-netizen.github.io/product-images/14050/2.jpg,https://oleks-netizen.github.io/product-images/14050/6.jpg,https://oleks-netizen.github.io/product-images/14050/9.jpg,https://oleks-netizen.github.io/product-images/14050/3.jpg,https://oleks-netizen.github.io/product-images/14050/4.jpg,https://oleks-netizen.github.io/product-images/14050/5.jpg,https://oleks-netizen.github.io/product-images/14050/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14050/01.jpg,https://oleks-netizen.github.io/product-images/14050/02.jpg,https://oleks-netizen.github.io/product-images/14050/06.jpg,https://oleks-netizen.github.io/product-images/14050/09.jpg,https://oleks-netizen.github.io/product-images/14050/03.jpg,https://oleks-netizen.github.io/product-images/14050/04.jpg,https://oleks-netizen.github.io/product-images/14050/05.jpg,https://oleks-netizen.github.io/product-images/14050/07.jpg</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -671,7 +671,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14051/1.jpg,https://oleks-netizen.github.io/product-images/14051/2.jpg,https://oleks-netizen.github.io/product-images/14051/10.jpg,https://oleks-netizen.github.io/product-images/14051/3.jpg,https://oleks-netizen.github.io/product-images/14051/4.jpg,https://oleks-netizen.github.io/product-images/14051/5.jpg,https://oleks-netizen.github.io/product-images/14051/6.jpg,https://oleks-netizen.github.io/product-images/14051/7.jpg,https://oleks-netizen.github.io/product-images/14051/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14051/01.jpg,https://oleks-netizen.github.io/product-images/14051/02.jpg,https://oleks-netizen.github.io/product-images/14051/10.jpg,https://oleks-netizen.github.io/product-images/14051/03.jpg,https://oleks-netizen.github.io/product-images/14051/04.jpg,https://oleks-netizen.github.io/product-images/14051/05.jpg,https://oleks-netizen.github.io/product-images/14051/06.jpg,https://oleks-netizen.github.io/product-images/14051/07.jpg,https://oleks-netizen.github.io/product-images/14051/08.jpg</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -686,7 +686,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14052/1.jpg,https://oleks-netizen.github.io/product-images/14052/2.jpg,https://oleks-netizen.github.io/product-images/14052/11.jpg,https://oleks-netizen.github.io/product-images/14052/3.jpg,https://oleks-netizen.github.io/product-images/14052/4.jpg,https://oleks-netizen.github.io/product-images/14052/5.jpg,https://oleks-netizen.github.io/product-images/14052/6.jpg,https://oleks-netizen.github.io/product-images/14052/7.jpg,https://oleks-netizen.github.io/product-images/14052/8.jpg,https://oleks-netizen.github.io/product-images/14052/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14052/01.jpg,https://oleks-netizen.github.io/product-images/14052/02.jpg,https://oleks-netizen.github.io/product-images/14052/11.jpg,https://oleks-netizen.github.io/product-images/14052/03.jpg,https://oleks-netizen.github.io/product-images/14052/04.jpg,https://oleks-netizen.github.io/product-images/14052/05.jpg,https://oleks-netizen.github.io/product-images/14052/06.jpg,https://oleks-netizen.github.io/product-images/14052/07.jpg,https://oleks-netizen.github.io/product-images/14052/08.jpg,https://oleks-netizen.github.io/product-images/14052/09.jpg</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -701,7 +701,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14053/1.jpg,https://oleks-netizen.github.io/product-images/14053/2.jpg,https://oleks-netizen.github.io/product-images/14053/5.jpg,https://oleks-netizen.github.io/product-images/14053/8.jpg,https://oleks-netizen.github.io/product-images/14053/3.jpg,https://oleks-netizen.github.io/product-images/14053/4.jpg,https://oleks-netizen.github.io/product-images/14053/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14053/01.jpg,https://oleks-netizen.github.io/product-images/14053/02.jpg,https://oleks-netizen.github.io/product-images/14053/05.jpg,https://oleks-netizen.github.io/product-images/14053/08.jpg,https://oleks-netizen.github.io/product-images/14053/03.jpg,https://oleks-netizen.github.io/product-images/14053/04.jpg,https://oleks-netizen.github.io/product-images/14053/06.jpg</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -716,7 +716,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14055/1.jpg,https://oleks-netizen.github.io/product-images/14055/2.jpg,https://oleks-netizen.github.io/product-images/14055/5.jpg,https://oleks-netizen.github.io/product-images/14055/11.jpg,https://oleks-netizen.github.io/product-images/14055/10.jpg,https://oleks-netizen.github.io/product-images/14055/3.jpg,https://oleks-netizen.github.io/product-images/14055/4.jpg,https://oleks-netizen.github.io/product-images/14055/6.jpg,https://oleks-netizen.github.io/product-images/14055/7.jpg,https://oleks-netizen.github.io/product-images/14055/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14055/01.jpg,https://oleks-netizen.github.io/product-images/14055/02.jpg,https://oleks-netizen.github.io/product-images/14055/05.jpg,https://oleks-netizen.github.io/product-images/14055/11.jpg,https://oleks-netizen.github.io/product-images/14055/10.jpg,https://oleks-netizen.github.io/product-images/14055/03.jpg,https://oleks-netizen.github.io/product-images/14055/04.jpg,https://oleks-netizen.github.io/product-images/14055/06.jpg,https://oleks-netizen.github.io/product-images/14055/07.jpg,https://oleks-netizen.github.io/product-images/14055/09.jpg</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -731,7 +731,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14059/1.jpg,https://oleks-netizen.github.io/product-images/14059/2.jpg,https://oleks-netizen.github.io/product-images/14059/8.jpg,https://oleks-netizen.github.io/product-images/14059/3.jpg,https://oleks-netizen.github.io/product-images/14059/4.jpg,https://oleks-netizen.github.io/product-images/14059/5.jpg,https://oleks-netizen.github.io/product-images/14059/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14059/01.jpg,https://oleks-netizen.github.io/product-images/14059/02.jpg,https://oleks-netizen.github.io/product-images/14059/08.jpg,https://oleks-netizen.github.io/product-images/14059/03.jpg,https://oleks-netizen.github.io/product-images/14059/04.jpg,https://oleks-netizen.github.io/product-images/14059/05.jpg,https://oleks-netizen.github.io/product-images/14059/06.jpg</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -746,7 +746,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14066/1.jpg,https://oleks-netizen.github.io/product-images/14066/2.jpg,https://oleks-netizen.github.io/product-images/14066/14.jpg,https://oleks-netizen.github.io/product-images/14066/10.jpg,https://oleks-netizen.github.io/product-images/14066/11.jpg,https://oleks-netizen.github.io/product-images/14066/12.jpg,https://oleks-netizen.github.io/product-images/14066/13.jpg,https://oleks-netizen.github.io/product-images/14066/3.jpg,https://oleks-netizen.github.io/product-images/14066/4.jpg,https://oleks-netizen.github.io/product-images/14066/5.jpg,https://oleks-netizen.github.io/product-images/14066/6.jpg,https://oleks-netizen.github.io/product-images/14066/8.jpg,https://oleks-netizen.github.io/product-images/14066/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14066/01.jpg,https://oleks-netizen.github.io/product-images/14066/02.jpg,https://oleks-netizen.github.io/product-images/14066/14.jpg,https://oleks-netizen.github.io/product-images/14066/10.jpg,https://oleks-netizen.github.io/product-images/14066/11.jpg,https://oleks-netizen.github.io/product-images/14066/12.jpg,https://oleks-netizen.github.io/product-images/14066/13.jpg,https://oleks-netizen.github.io/product-images/14066/03.jpg,https://oleks-netizen.github.io/product-images/14066/04.jpg,https://oleks-netizen.github.io/product-images/14066/05.jpg,https://oleks-netizen.github.io/product-images/14066/06.jpg,https://oleks-netizen.github.io/product-images/14066/08.jpg,https://oleks-netizen.github.io/product-images/14066/09.jpg</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -761,7 +761,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14085/1.jpg,https://oleks-netizen.github.io/product-images/14085/2.jpg,https://oleks-netizen.github.io/product-images/14085/8.jpg,https://oleks-netizen.github.io/product-images/14085/16.jpg,https://oleks-netizen.github.io/product-images/14085/10.jpg,https://oleks-netizen.github.io/product-images/14085/11.jpg,https://oleks-netizen.github.io/product-images/14085/12.jpg,https://oleks-netizen.github.io/product-images/14085/13.jpg,https://oleks-netizen.github.io/product-images/14085/14.jpg,https://oleks-netizen.github.io/product-images/14085/3.jpg,https://oleks-netizen.github.io/product-images/14085/4.jpg,https://oleks-netizen.github.io/product-images/14085/5.jpg,https://oleks-netizen.github.io/product-images/14085/6.jpg,https://oleks-netizen.github.io/product-images/14085/7.jpg,https://oleks-netizen.github.io/product-images/14085/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14085/01.jpg,https://oleks-netizen.github.io/product-images/14085/02.jpg,https://oleks-netizen.github.io/product-images/14085/08.jpg,https://oleks-netizen.github.io/product-images/14085/16.jpg,https://oleks-netizen.github.io/product-images/14085/10.jpg,https://oleks-netizen.github.io/product-images/14085/11.jpg,https://oleks-netizen.github.io/product-images/14085/12.jpg,https://oleks-netizen.github.io/product-images/14085/13.jpg,https://oleks-netizen.github.io/product-images/14085/14.jpg,https://oleks-netizen.github.io/product-images/14085/03.jpg,https://oleks-netizen.github.io/product-images/14085/04.jpg,https://oleks-netizen.github.io/product-images/14085/05.jpg,https://oleks-netizen.github.io/product-images/14085/06.jpg,https://oleks-netizen.github.io/product-images/14085/07.jpg,https://oleks-netizen.github.io/product-images/14085/09.jpg</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -776,7 +776,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14088/1.jpg,https://oleks-netizen.github.io/product-images/14088/2.jpg,https://oleks-netizen.github.io/product-images/14088/6.jpg,https://oleks-netizen.github.io/product-images/14088/19.jpg,https://oleks-netizen.github.io/product-images/14088/10.jpg,https://oleks-netizen.github.io/product-images/14088/11.jpg,https://oleks-netizen.github.io/product-images/14088/12.jpg,https://oleks-netizen.github.io/product-images/14088/13.jpg,https://oleks-netizen.github.io/product-images/14088/14.jpg,https://oleks-netizen.github.io/product-images/14088/15.jpg,https://oleks-netizen.github.io/product-images/14088/16.jpg,https://oleks-netizen.github.io/product-images/14088/17.jpg,https://oleks-netizen.github.io/product-images/14088/18.jpg,https://oleks-netizen.github.io/product-images/14088/3.jpg,https://oleks-netizen.github.io/product-images/14088/4.jpg,https://oleks-netizen.github.io/product-images/14088/5.jpg,https://oleks-netizen.github.io/product-images/14088/7.jpg,https://oleks-netizen.github.io/product-images/14088/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14088/01.jpg,https://oleks-netizen.github.io/product-images/14088/02.jpg,https://oleks-netizen.github.io/product-images/14088/06.jpg,https://oleks-netizen.github.io/product-images/14088/19.jpg,https://oleks-netizen.github.io/product-images/14088/10.jpg,https://oleks-netizen.github.io/product-images/14088/11.jpg,https://oleks-netizen.github.io/product-images/14088/12.jpg,https://oleks-netizen.github.io/product-images/14088/13.jpg,https://oleks-netizen.github.io/product-images/14088/14.jpg,https://oleks-netizen.github.io/product-images/14088/15.jpg,https://oleks-netizen.github.io/product-images/14088/16.jpg,https://oleks-netizen.github.io/product-images/14088/17.jpg,https://oleks-netizen.github.io/product-images/14088/18.jpg,https://oleks-netizen.github.io/product-images/14088/03.jpg,https://oleks-netizen.github.io/product-images/14088/04.jpg,https://oleks-netizen.github.io/product-images/14088/05.jpg,https://oleks-netizen.github.io/product-images/14088/07.jpg,https://oleks-netizen.github.io/product-images/14088/09.jpg</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -791,7 +791,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14091/1.jpg,https://oleks-netizen.github.io/product-images/14091/2.jpg,https://oleks-netizen.github.io/product-images/14091/19.jpg,https://oleks-netizen.github.io/product-images/14091/10.jpg,https://oleks-netizen.github.io/product-images/14091/11.jpg,https://oleks-netizen.github.io/product-images/14091/12.jpg,https://oleks-netizen.github.io/product-images/14091/13.jpg,https://oleks-netizen.github.io/product-images/14091/14.jpg,https://oleks-netizen.github.io/product-images/14091/15.jpg,https://oleks-netizen.github.io/product-images/14091/16.jpg,https://oleks-netizen.github.io/product-images/14091/17.jpg,https://oleks-netizen.github.io/product-images/14091/18.jpg,https://oleks-netizen.github.io/product-images/14091/3.jpg,https://oleks-netizen.github.io/product-images/14091/4.jpg,https://oleks-netizen.github.io/product-images/14091/5.jpg,https://oleks-netizen.github.io/product-images/14091/6.jpg,https://oleks-netizen.github.io/product-images/14091/7.jpg,https://oleks-netizen.github.io/product-images/14091/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14091/01.jpg,https://oleks-netizen.github.io/product-images/14091/02.jpg,https://oleks-netizen.github.io/product-images/14091/19.jpg,https://oleks-netizen.github.io/product-images/14091/10.jpg,https://oleks-netizen.github.io/product-images/14091/11.jpg,https://oleks-netizen.github.io/product-images/14091/12.jpg,https://oleks-netizen.github.io/product-images/14091/13.jpg,https://oleks-netizen.github.io/product-images/14091/14.jpg,https://oleks-netizen.github.io/product-images/14091/15.jpg,https://oleks-netizen.github.io/product-images/14091/16.jpg,https://oleks-netizen.github.io/product-images/14091/17.jpg,https://oleks-netizen.github.io/product-images/14091/18.jpg,https://oleks-netizen.github.io/product-images/14091/03.jpg,https://oleks-netizen.github.io/product-images/14091/04.jpg,https://oleks-netizen.github.io/product-images/14091/05.jpg,https://oleks-netizen.github.io/product-images/14091/06.jpg,https://oleks-netizen.github.io/product-images/14091/07.jpg,https://oleks-netizen.github.io/product-images/14091/09.jpg</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -806,7 +806,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14114/1.jpg,https://oleks-netizen.github.io/product-images/14114/2.jpg,https://oleks-netizen.github.io/product-images/14114/6.jpg,https://oleks-netizen.github.io/product-images/14114/10.jpg,https://oleks-netizen.github.io/product-images/14114/4.jpg,https://oleks-netizen.github.io/product-images/14114/5.jpg,https://oleks-netizen.github.io/product-images/14114/7.jpg,https://oleks-netizen.github.io/product-images/14114/8.jpg,https://oleks-netizen.github.io/product-images/14114/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14114/01.jpg,https://oleks-netizen.github.io/product-images/14114/02.jpg,https://oleks-netizen.github.io/product-images/14114/06.jpg,https://oleks-netizen.github.io/product-images/14114/10.jpg,https://oleks-netizen.github.io/product-images/14114/04.jpg,https://oleks-netizen.github.io/product-images/14114/05.jpg,https://oleks-netizen.github.io/product-images/14114/07.jpg,https://oleks-netizen.github.io/product-images/14114/08.jpg,https://oleks-netizen.github.io/product-images/14114/09.jpg</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -821,7 +821,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14135/1.jpg,https://oleks-netizen.github.io/product-images/14135/2.jpg,https://oleks-netizen.github.io/product-images/14135/5.jpg,https://oleks-netizen.github.io/product-images/14135/12.jpg,https://oleks-netizen.github.io/product-images/14135/11.jpg,https://oleks-netizen.github.io/product-images/14135/3.jpg,https://oleks-netizen.github.io/product-images/14135/4.jpg,https://oleks-netizen.github.io/product-images/14135/6.jpg,https://oleks-netizen.github.io/product-images/14135/7.jpg,https://oleks-netizen.github.io/product-images/14135/8.jpg,https://oleks-netizen.github.io/product-images/14135/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14135/01.jpg,https://oleks-netizen.github.io/product-images/14135/02.jpg,https://oleks-netizen.github.io/product-images/14135/05.jpg,https://oleks-netizen.github.io/product-images/14135/12.jpg,https://oleks-netizen.github.io/product-images/14135/11.jpg,https://oleks-netizen.github.io/product-images/14135/03.jpg,https://oleks-netizen.github.io/product-images/14135/04.jpg,https://oleks-netizen.github.io/product-images/14135/06.jpg,https://oleks-netizen.github.io/product-images/14135/07.jpg,https://oleks-netizen.github.io/product-images/14135/08.jpg,https://oleks-netizen.github.io/product-images/14135/09.jpg</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -836,7 +836,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14155/1.jpg,https://oleks-netizen.github.io/product-images/14155/2.jpg,https://oleks-netizen.github.io/product-images/14155/9.jpg,https://oleks-netizen.github.io/product-images/14155/3.jpg,https://oleks-netizen.github.io/product-images/14155/4.jpg,https://oleks-netizen.github.io/product-images/14155/5.jpg,https://oleks-netizen.github.io/product-images/14155/7.jpg,https://oleks-netizen.github.io/product-images/14155/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14155/01.jpg,https://oleks-netizen.github.io/product-images/14155/02.jpg,https://oleks-netizen.github.io/product-images/14155/09.jpg,https://oleks-netizen.github.io/product-images/14155/03.jpg,https://oleks-netizen.github.io/product-images/14155/04.jpg,https://oleks-netizen.github.io/product-images/14155/05.jpg,https://oleks-netizen.github.io/product-images/14155/07.jpg,https://oleks-netizen.github.io/product-images/14155/08.jpg</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -851,7 +851,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14219/1.jpg,https://oleks-netizen.github.io/product-images/14219/2.jpg,https://oleks-netizen.github.io/product-images/14219/11.jpg,https://oleks-netizen.github.io/product-images/14219/10.jpg,https://oleks-netizen.github.io/product-images/14219/3.jpg,https://oleks-netizen.github.io/product-images/14219/4.jpg,https://oleks-netizen.github.io/product-images/14219/5.jpg,https://oleks-netizen.github.io/product-images/14219/7.jpg,https://oleks-netizen.github.io/product-images/14219/8.jpg,https://oleks-netizen.github.io/product-images/14219/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14219/01.jpg,https://oleks-netizen.github.io/product-images/14219/02.jpg,https://oleks-netizen.github.io/product-images/14219/11.jpg,https://oleks-netizen.github.io/product-images/14219/10.jpg,https://oleks-netizen.github.io/product-images/14219/03.jpg,https://oleks-netizen.github.io/product-images/14219/04.jpg,https://oleks-netizen.github.io/product-images/14219/05.jpg,https://oleks-netizen.github.io/product-images/14219/07.jpg,https://oleks-netizen.github.io/product-images/14219/08.jpg,https://oleks-netizen.github.io/product-images/14219/09.jpg</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -866,7 +866,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14223/1.jpg,https://oleks-netizen.github.io/product-images/14223/2.jpg,https://oleks-netizen.github.io/product-images/14223/5.jpg,https://oleks-netizen.github.io/product-images/14223/9.jpg,https://oleks-netizen.github.io/product-images/14223/3.jpg,https://oleks-netizen.github.io/product-images/14223/4.jpg,https://oleks-netizen.github.io/product-images/14223/6.jpg,https://oleks-netizen.github.io/product-images/14223/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14223/01.jpg,https://oleks-netizen.github.io/product-images/14223/02.jpg,https://oleks-netizen.github.io/product-images/14223/05.jpg,https://oleks-netizen.github.io/product-images/14223/09.jpg,https://oleks-netizen.github.io/product-images/14223/03.jpg,https://oleks-netizen.github.io/product-images/14223/04.jpg,https://oleks-netizen.github.io/product-images/14223/06.jpg,https://oleks-netizen.github.io/product-images/14223/08.jpg</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -881,7 +881,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14224/1.jpg,https://oleks-netizen.github.io/product-images/14224/2.jpg,https://oleks-netizen.github.io/product-images/14224/5.jpg,https://oleks-netizen.github.io/product-images/14224/13.jpg,https://oleks-netizen.github.io/product-images/14224/10.jpg,https://oleks-netizen.github.io/product-images/14224/11.jpg,https://oleks-netizen.github.io/product-images/14224/12.jpg,https://oleks-netizen.github.io/product-images/14224/3.jpg,https://oleks-netizen.github.io/product-images/14224/4.jpg,https://oleks-netizen.github.io/product-images/14224/6.jpg,https://oleks-netizen.github.io/product-images/14224/7.jpg,https://oleks-netizen.github.io/product-images/14224/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14224/01.jpg,https://oleks-netizen.github.io/product-images/14224/02.jpg,https://oleks-netizen.github.io/product-images/14224/05.jpg,https://oleks-netizen.github.io/product-images/14224/13.jpg,https://oleks-netizen.github.io/product-images/14224/10.jpg,https://oleks-netizen.github.io/product-images/14224/11.jpg,https://oleks-netizen.github.io/product-images/14224/12.jpg,https://oleks-netizen.github.io/product-images/14224/03.jpg,https://oleks-netizen.github.io/product-images/14224/04.jpg,https://oleks-netizen.github.io/product-images/14224/06.jpg,https://oleks-netizen.github.io/product-images/14224/07.jpg,https://oleks-netizen.github.io/product-images/14224/08.jpg</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -896,7 +896,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14225/1.jpg,https://oleks-netizen.github.io/product-images/14225/2.jpg,https://oleks-netizen.github.io/product-images/14225/3.jpg,https://oleks-netizen.github.io/product-images/14225/13.jpg,https://oleks-netizen.github.io/product-images/14225/11.jpg,https://oleks-netizen.github.io/product-images/14225/12.jpg,https://oleks-netizen.github.io/product-images/14225/4.jpg,https://oleks-netizen.github.io/product-images/14225/5.jpg,https://oleks-netizen.github.io/product-images/14225/6.jpg,https://oleks-netizen.github.io/product-images/14225/7.jpg,https://oleks-netizen.github.io/product-images/14225/8.jpg,https://oleks-netizen.github.io/product-images/14225/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14225/01.jpg,https://oleks-netizen.github.io/product-images/14225/02.jpg,https://oleks-netizen.github.io/product-images/14225/03.jpg,https://oleks-netizen.github.io/product-images/14225/13.jpg,https://oleks-netizen.github.io/product-images/14225/11.jpg,https://oleks-netizen.github.io/product-images/14225/12.jpg,https://oleks-netizen.github.io/product-images/14225/04.jpg,https://oleks-netizen.github.io/product-images/14225/05.jpg,https://oleks-netizen.github.io/product-images/14225/06.jpg,https://oleks-netizen.github.io/product-images/14225/07.jpg,https://oleks-netizen.github.io/product-images/14225/08.jpg,https://oleks-netizen.github.io/product-images/14225/09.jpg</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -911,7 +911,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14227/1.jpg,https://oleks-netizen.github.io/product-images/14227/2.jpg,https://oleks-netizen.github.io/product-images/14227/5.jpg,https://oleks-netizen.github.io/product-images/14227/11.jpg,https://oleks-netizen.github.io/product-images/14227/10.jpg,https://oleks-netizen.github.io/product-images/14227/3.jpg,https://oleks-netizen.github.io/product-images/14227/4.jpg,https://oleks-netizen.github.io/product-images/14227/6.jpg,https://oleks-netizen.github.io/product-images/14227/7.jpg,https://oleks-netizen.github.io/product-images/14227/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14227/01.jpg,https://oleks-netizen.github.io/product-images/14227/02.jpg,https://oleks-netizen.github.io/product-images/14227/05.jpg,https://oleks-netizen.github.io/product-images/14227/11.jpg,https://oleks-netizen.github.io/product-images/14227/10.jpg,https://oleks-netizen.github.io/product-images/14227/03.jpg,https://oleks-netizen.github.io/product-images/14227/04.jpg,https://oleks-netizen.github.io/product-images/14227/06.jpg,https://oleks-netizen.github.io/product-images/14227/07.jpg,https://oleks-netizen.github.io/product-images/14227/09.jpg</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -926,7 +926,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14228/1.jpg,https://oleks-netizen.github.io/product-images/14228/2.jpg,https://oleks-netizen.github.io/product-images/14228/5.jpg,https://oleks-netizen.github.io/product-images/14228/8.jpg,https://oleks-netizen.github.io/product-images/14228/3.jpg,https://oleks-netizen.github.io/product-images/14228/4.jpg,https://oleks-netizen.github.io/product-images/14228/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14228/01.jpg,https://oleks-netizen.github.io/product-images/14228/02.jpg,https://oleks-netizen.github.io/product-images/14228/05.jpg,https://oleks-netizen.github.io/product-images/14228/08.jpg,https://oleks-netizen.github.io/product-images/14228/03.jpg,https://oleks-netizen.github.io/product-images/14228/04.jpg,https://oleks-netizen.github.io/product-images/14228/06.jpg</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -941,7 +941,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14230/1.jpg,https://oleks-netizen.github.io/product-images/14230/2.jpg,https://oleks-netizen.github.io/product-images/14230/6.jpg,https://oleks-netizen.github.io/product-images/14230/11.jpg,https://oleks-netizen.github.io/product-images/14230/3.jpg,https://oleks-netizen.github.io/product-images/14230/4.jpg,https://oleks-netizen.github.io/product-images/14230/5.jpg,https://oleks-netizen.github.io/product-images/14230/7.jpg,https://oleks-netizen.github.io/product-images/14230/8.jpg,https://oleks-netizen.github.io/product-images/14230/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14230/01.jpg,https://oleks-netizen.github.io/product-images/14230/02.jpg,https://oleks-netizen.github.io/product-images/14230/06.jpg,https://oleks-netizen.github.io/product-images/14230/11.jpg,https://oleks-netizen.github.io/product-images/14230/03.jpg,https://oleks-netizen.github.io/product-images/14230/04.jpg,https://oleks-netizen.github.io/product-images/14230/05.jpg,https://oleks-netizen.github.io/product-images/14230/07.jpg,https://oleks-netizen.github.io/product-images/14230/08.jpg,https://oleks-netizen.github.io/product-images/14230/09.jpg</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -956,7 +956,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14231/1.jpg,https://oleks-netizen.github.io/product-images/14231/2.jpg,https://oleks-netizen.github.io/product-images/14231/11.jpg,https://oleks-netizen.github.io/product-images/14231/10.jpg,https://oleks-netizen.github.io/product-images/14231/3.jpg,https://oleks-netizen.github.io/product-images/14231/4.jpg,https://oleks-netizen.github.io/product-images/14231/5.jpg,https://oleks-netizen.github.io/product-images/14231/7.jpg,https://oleks-netizen.github.io/product-images/14231/8.jpg,https://oleks-netizen.github.io/product-images/14231/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14231/01.jpg,https://oleks-netizen.github.io/product-images/14231/02.jpg,https://oleks-netizen.github.io/product-images/14231/11.jpg,https://oleks-netizen.github.io/product-images/14231/10.jpg,https://oleks-netizen.github.io/product-images/14231/03.jpg,https://oleks-netizen.github.io/product-images/14231/04.jpg,https://oleks-netizen.github.io/product-images/14231/05.jpg,https://oleks-netizen.github.io/product-images/14231/07.jpg,https://oleks-netizen.github.io/product-images/14231/08.jpg,https://oleks-netizen.github.io/product-images/14231/09.jpg</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -971,7 +971,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14248/1.jpg,https://oleks-netizen.github.io/product-images/14248/2.jpg,https://oleks-netizen.github.io/product-images/14248/4.jpg,https://oleks-netizen.github.io/product-images/14248/12.jpg,https://oleks-netizen.github.io/product-images/14248/10.jpg,https://oleks-netizen.github.io/product-images/14248/11.jpg,https://oleks-netizen.github.io/product-images/14248/3.jpg,https://oleks-netizen.github.io/product-images/14248/5.jpg,https://oleks-netizen.github.io/product-images/14248/6.jpg,https://oleks-netizen.github.io/product-images/14248/7.jpg,https://oleks-netizen.github.io/product-images/14248/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14248/01.jpg,https://oleks-netizen.github.io/product-images/14248/02.jpg,https://oleks-netizen.github.io/product-images/14248/04.jpg,https://oleks-netizen.github.io/product-images/14248/12.jpg,https://oleks-netizen.github.io/product-images/14248/10.jpg,https://oleks-netizen.github.io/product-images/14248/11.jpg,https://oleks-netizen.github.io/product-images/14248/03.jpg,https://oleks-netizen.github.io/product-images/14248/05.jpg,https://oleks-netizen.github.io/product-images/14248/06.jpg,https://oleks-netizen.github.io/product-images/14248/07.jpg,https://oleks-netizen.github.io/product-images/14248/09.jpg</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -986,7 +986,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14253/1.jpg,https://oleks-netizen.github.io/product-images/14253/2.jpg,https://oleks-netizen.github.io/product-images/14253/5.jpg,https://oleks-netizen.github.io/product-images/14253/15.jpg,https://oleks-netizen.github.io/product-images/14253/11.jpg,https://oleks-netizen.github.io/product-images/14253/12.jpg,https://oleks-netizen.github.io/product-images/14253/13.jpg,https://oleks-netizen.github.io/product-images/14253/14.jpg,https://oleks-netizen.github.io/product-images/14253/3.jpg,https://oleks-netizen.github.io/product-images/14253/4.jpg,https://oleks-netizen.github.io/product-images/14253/6.jpg,https://oleks-netizen.github.io/product-images/14253/7.jpg,https://oleks-netizen.github.io/product-images/14253/8.jpg,https://oleks-netizen.github.io/product-images/14253/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14253/01.jpg,https://oleks-netizen.github.io/product-images/14253/02.jpg,https://oleks-netizen.github.io/product-images/14253/05.jpg,https://oleks-netizen.github.io/product-images/14253/15.jpg,https://oleks-netizen.github.io/product-images/14253/11.jpg,https://oleks-netizen.github.io/product-images/14253/12.jpg,https://oleks-netizen.github.io/product-images/14253/13.jpg,https://oleks-netizen.github.io/product-images/14253/14.jpg,https://oleks-netizen.github.io/product-images/14253/03.jpg,https://oleks-netizen.github.io/product-images/14253/04.jpg,https://oleks-netizen.github.io/product-images/14253/06.jpg,https://oleks-netizen.github.io/product-images/14253/07.jpg,https://oleks-netizen.github.io/product-images/14253/08.jpg,https://oleks-netizen.github.io/product-images/14253/09.jpg</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14254/1.jpg,https://oleks-netizen.github.io/product-images/14254/2.jpg,https://oleks-netizen.github.io/product-images/14254/14.jpg,https://oleks-netizen.github.io/product-images/14254/10.jpg,https://oleks-netizen.github.io/product-images/14254/11.jpg,https://oleks-netizen.github.io/product-images/14254/12.jpg,https://oleks-netizen.github.io/product-images/14254/13.jpg,https://oleks-netizen.github.io/product-images/14254/3.jpg,https://oleks-netizen.github.io/product-images/14254/4.jpg,https://oleks-netizen.github.io/product-images/14254/6.jpg,https://oleks-netizen.github.io/product-images/14254/7.jpg,https://oleks-netizen.github.io/product-images/14254/8.jpg,https://oleks-netizen.github.io/product-images/14254/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14254/01.jpg,https://oleks-netizen.github.io/product-images/14254/02.jpg,https://oleks-netizen.github.io/product-images/14254/14.jpg,https://oleks-netizen.github.io/product-images/14254/10.jpg,https://oleks-netizen.github.io/product-images/14254/11.jpg,https://oleks-netizen.github.io/product-images/14254/12.jpg,https://oleks-netizen.github.io/product-images/14254/13.jpg,https://oleks-netizen.github.io/product-images/14254/03.jpg,https://oleks-netizen.github.io/product-images/14254/04.jpg,https://oleks-netizen.github.io/product-images/14254/06.jpg,https://oleks-netizen.github.io/product-images/14254/07.jpg,https://oleks-netizen.github.io/product-images/14254/08.jpg,https://oleks-netizen.github.io/product-images/14254/09.jpg</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -1016,7 +1016,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14346/1.jpg,https://oleks-netizen.github.io/product-images/14346/2.jpg,https://oleks-netizen.github.io/product-images/14346/3.jpg,https://oleks-netizen.github.io/product-images/14346/4.jpg,https://oleks-netizen.github.io/product-images/14346/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14346/01.jpg,https://oleks-netizen.github.io/product-images/14346/02.jpg,https://oleks-netizen.github.io/product-images/14346/03.jpg,https://oleks-netizen.github.io/product-images/14346/04.jpg,https://oleks-netizen.github.io/product-images/14346/05.jpg</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -1031,7 +1031,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14353/1.jpg,https://oleks-netizen.github.io/product-images/14353/2.jpg,https://oleks-netizen.github.io/product-images/14353/6.jpg,https://oleks-netizen.github.io/product-images/14353/14.jpg,https://oleks-netizen.github.io/product-images/14353/10.jpg,https://oleks-netizen.github.io/product-images/14353/11.jpg,https://oleks-netizen.github.io/product-images/14353/12.jpg,https://oleks-netizen.github.io/product-images/14353/13.jpg,https://oleks-netizen.github.io/product-images/14353/3.jpg,https://oleks-netizen.github.io/product-images/14353/4.jpg,https://oleks-netizen.github.io/product-images/14353/5.jpg,https://oleks-netizen.github.io/product-images/14353/8.jpg,https://oleks-netizen.github.io/product-images/14353/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14353/01.jpg,https://oleks-netizen.github.io/product-images/14353/02.jpg,https://oleks-netizen.github.io/product-images/14353/06.jpg,https://oleks-netizen.github.io/product-images/14353/14.jpg,https://oleks-netizen.github.io/product-images/14353/10.jpg,https://oleks-netizen.github.io/product-images/14353/11.jpg,https://oleks-netizen.github.io/product-images/14353/12.jpg,https://oleks-netizen.github.io/product-images/14353/13.jpg,https://oleks-netizen.github.io/product-images/14353/03.jpg,https://oleks-netizen.github.io/product-images/14353/04.jpg,https://oleks-netizen.github.io/product-images/14353/05.jpg,https://oleks-netizen.github.io/product-images/14353/08.jpg,https://oleks-netizen.github.io/product-images/14353/09.jpg</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14365/1.jpg,https://oleks-netizen.github.io/product-images/14365/2.jpg,https://oleks-netizen.github.io/product-images/14365/6.jpg,https://oleks-netizen.github.io/product-images/14365/12.jpg,https://oleks-netizen.github.io/product-images/14365/11.jpg,https://oleks-netizen.github.io/product-images/14365/3.jpg,https://oleks-netizen.github.io/product-images/14365/4.jpg,https://oleks-netizen.github.io/product-images/14365/5.jpg,https://oleks-netizen.github.io/product-images/14365/7.jpg,https://oleks-netizen.github.io/product-images/14365/8.jpg,https://oleks-netizen.github.io/product-images/14365/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14365/01.jpg,https://oleks-netizen.github.io/product-images/14365/02.jpg,https://oleks-netizen.github.io/product-images/14365/06.jpg,https://oleks-netizen.github.io/product-images/14365/12.jpg,https://oleks-netizen.github.io/product-images/14365/11.jpg,https://oleks-netizen.github.io/product-images/14365/03.jpg,https://oleks-netizen.github.io/product-images/14365/04.jpg,https://oleks-netizen.github.io/product-images/14365/05.jpg,https://oleks-netizen.github.io/product-images/14365/07.jpg,https://oleks-netizen.github.io/product-images/14365/08.jpg,https://oleks-netizen.github.io/product-images/14365/09.jpg</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -1061,7 +1061,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14371/1.jpg,https://oleks-netizen.github.io/product-images/14371/2.jpg,https://oleks-netizen.github.io/product-images/14371/20.jpg,https://oleks-netizen.github.io/product-images/14371/10.jpg,https://oleks-netizen.github.io/product-images/14371/11.jpg,https://oleks-netizen.github.io/product-images/14371/12.jpg,https://oleks-netizen.github.io/product-images/14371/13.jpg,https://oleks-netizen.github.io/product-images/14371/14.jpg,https://oleks-netizen.github.io/product-images/14371/15.jpg,https://oleks-netizen.github.io/product-images/14371/16.jpg,https://oleks-netizen.github.io/product-images/14371/17.jpg,https://oleks-netizen.github.io/product-images/14371/18.jpg,https://oleks-netizen.github.io/product-images/14371/19.jpg,https://oleks-netizen.github.io/product-images/14371/3.jpg,https://oleks-netizen.github.io/product-images/14371/4.jpg,https://oleks-netizen.github.io/product-images/14371/5.jpg,https://oleks-netizen.github.io/product-images/14371/6.jpg,https://oleks-netizen.github.io/product-images/14371/7.jpg,https://oleks-netizen.github.io/product-images/14371/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14371/01.jpg,https://oleks-netizen.github.io/product-images/14371/02.jpg,https://oleks-netizen.github.io/product-images/14371/20.jpg,https://oleks-netizen.github.io/product-images/14371/10.jpg,https://oleks-netizen.github.io/product-images/14371/11.jpg,https://oleks-netizen.github.io/product-images/14371/12.jpg,https://oleks-netizen.github.io/product-images/14371/13.jpg,https://oleks-netizen.github.io/product-images/14371/14.jpg,https://oleks-netizen.github.io/product-images/14371/15.jpg,https://oleks-netizen.github.io/product-images/14371/16.jpg,https://oleks-netizen.github.io/product-images/14371/17.jpg,https://oleks-netizen.github.io/product-images/14371/18.jpg,https://oleks-netizen.github.io/product-images/14371/19.jpg,https://oleks-netizen.github.io/product-images/14371/03.jpg,https://oleks-netizen.github.io/product-images/14371/04.jpg,https://oleks-netizen.github.io/product-images/14371/05.jpg,https://oleks-netizen.github.io/product-images/14371/06.jpg,https://oleks-netizen.github.io/product-images/14371/07.jpg,https://oleks-netizen.github.io/product-images/14371/09.jpg</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -1076,7 +1076,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14376/1.jpg,https://oleks-netizen.github.io/product-images/14376/2.jpg,https://oleks-netizen.github.io/product-images/14376/4.jpg,https://oleks-netizen.github.io/product-images/14376/8.jpg,https://oleks-netizen.github.io/product-images/14376/3.jpg,https://oleks-netizen.github.io/product-images/14376/5.jpg,https://oleks-netizen.github.io/product-images/14376/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14376/01.jpg,https://oleks-netizen.github.io/product-images/14376/02.jpg,https://oleks-netizen.github.io/product-images/14376/04.jpg,https://oleks-netizen.github.io/product-images/14376/08.jpg,https://oleks-netizen.github.io/product-images/14376/03.jpg,https://oleks-netizen.github.io/product-images/14376/05.jpg,https://oleks-netizen.github.io/product-images/14376/07.jpg</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1091,7 +1091,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14380/1.jpg,https://oleks-netizen.github.io/product-images/14380/2.jpg,https://oleks-netizen.github.io/product-images/14380/6.jpg,https://oleks-netizen.github.io/product-images/14380/10.jpg,https://oleks-netizen.github.io/product-images/14380/3.jpg,https://oleks-netizen.github.io/product-images/14380/4.jpg,https://oleks-netizen.github.io/product-images/14380/5.jpg,https://oleks-netizen.github.io/product-images/14380/7.jpg,https://oleks-netizen.github.io/product-images/14380/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14380/01.jpg,https://oleks-netizen.github.io/product-images/14380/02.jpg,https://oleks-netizen.github.io/product-images/14380/06.jpg,https://oleks-netizen.github.io/product-images/14380/10.jpg,https://oleks-netizen.github.io/product-images/14380/03.jpg,https://oleks-netizen.github.io/product-images/14380/04.jpg,https://oleks-netizen.github.io/product-images/14380/05.jpg,https://oleks-netizen.github.io/product-images/14380/07.jpg,https://oleks-netizen.github.io/product-images/14380/08.jpg</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1106,7 +1106,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14381/1.jpg,https://oleks-netizen.github.io/product-images/14381/2.jpg,https://oleks-netizen.github.io/product-images/14381/9.jpg,https://oleks-netizen.github.io/product-images/14381/3.jpg,https://oleks-netizen.github.io/product-images/14381/4.jpg,https://oleks-netizen.github.io/product-images/14381/5.jpg,https://oleks-netizen.github.io/product-images/14381/6.jpg,https://oleks-netizen.github.io/product-images/14381/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14381/01.jpg,https://oleks-netizen.github.io/product-images/14381/02.jpg,https://oleks-netizen.github.io/product-images/14381/09.jpg,https://oleks-netizen.github.io/product-images/14381/03.jpg,https://oleks-netizen.github.io/product-images/14381/04.jpg,https://oleks-netizen.github.io/product-images/14381/05.jpg,https://oleks-netizen.github.io/product-images/14381/06.jpg,https://oleks-netizen.github.io/product-images/14381/07.jpg</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14384/1.jpg,https://oleks-netizen.github.io/product-images/14384/2.jpg,https://oleks-netizen.github.io/product-images/14384/7.jpg,https://oleks-netizen.github.io/product-images/14384/11.jpg,https://oleks-netizen.github.io/product-images/14384/3.jpg,https://oleks-netizen.github.io/product-images/14384/4.jpg,https://oleks-netizen.github.io/product-images/14384/5.jpg,https://oleks-netizen.github.io/product-images/14384/6.jpg,https://oleks-netizen.github.io/product-images/14384/8.jpg,https://oleks-netizen.github.io/product-images/14384/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14384/01.jpg,https://oleks-netizen.github.io/product-images/14384/02.jpg,https://oleks-netizen.github.io/product-images/14384/07.jpg,https://oleks-netizen.github.io/product-images/14384/11.jpg,https://oleks-netizen.github.io/product-images/14384/03.jpg,https://oleks-netizen.github.io/product-images/14384/04.jpg,https://oleks-netizen.github.io/product-images/14384/05.jpg,https://oleks-netizen.github.io/product-images/14384/06.jpg,https://oleks-netizen.github.io/product-images/14384/08.jpg,https://oleks-netizen.github.io/product-images/14384/09.jpg</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1136,7 +1136,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14397/1.jpg,https://oleks-netizen.github.io/product-images/14397/2.jpg,https://oleks-netizen.github.io/product-images/14397/12.jpg,https://oleks-netizen.github.io/product-images/14397/10.jpg,https://oleks-netizen.github.io/product-images/14397/11.jpg,https://oleks-netizen.github.io/product-images/14397/3.jpg,https://oleks-netizen.github.io/product-images/14397/4.jpg,https://oleks-netizen.github.io/product-images/14397/6.jpg,https://oleks-netizen.github.io/product-images/14397/7.jpg,https://oleks-netizen.github.io/product-images/14397/8.jpg,https://oleks-netizen.github.io/product-images/14397/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14397/01.jpg,https://oleks-netizen.github.io/product-images/14397/02.jpg,https://oleks-netizen.github.io/product-images/14397/12.jpg,https://oleks-netizen.github.io/product-images/14397/10.jpg,https://oleks-netizen.github.io/product-images/14397/11.jpg,https://oleks-netizen.github.io/product-images/14397/03.jpg,https://oleks-netizen.github.io/product-images/14397/04.jpg,https://oleks-netizen.github.io/product-images/14397/06.jpg,https://oleks-netizen.github.io/product-images/14397/07.jpg,https://oleks-netizen.github.io/product-images/14397/08.jpg,https://oleks-netizen.github.io/product-images/14397/09.jpg</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1151,7 +1151,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14398/1.jpg,https://oleks-netizen.github.io/product-images/14398/2.jpg,https://oleks-netizen.github.io/product-images/14398/17.jpg,https://oleks-netizen.github.io/product-images/14398/10.jpg,https://oleks-netizen.github.io/product-images/14398/11.jpg,https://oleks-netizen.github.io/product-images/14398/12.jpg,https://oleks-netizen.github.io/product-images/14398/13.jpg,https://oleks-netizen.github.io/product-images/14398/15.jpg,https://oleks-netizen.github.io/product-images/14398/16.jpg,https://oleks-netizen.github.io/product-images/14398/3.jpg,https://oleks-netizen.github.io/product-images/14398/4.jpg,https://oleks-netizen.github.io/product-images/14398/5.jpg,https://oleks-netizen.github.io/product-images/14398/6.jpg,https://oleks-netizen.github.io/product-images/14398/7.jpg,https://oleks-netizen.github.io/product-images/14398/8.jpg,https://oleks-netizen.github.io/product-images/14398/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14398/01.jpg,https://oleks-netizen.github.io/product-images/14398/02.jpg,https://oleks-netizen.github.io/product-images/14398/17.jpg,https://oleks-netizen.github.io/product-images/14398/10.jpg,https://oleks-netizen.github.io/product-images/14398/11.jpg,https://oleks-netizen.github.io/product-images/14398/12.jpg,https://oleks-netizen.github.io/product-images/14398/13.jpg,https://oleks-netizen.github.io/product-images/14398/15.jpg,https://oleks-netizen.github.io/product-images/14398/16.jpg,https://oleks-netizen.github.io/product-images/14398/03.jpg,https://oleks-netizen.github.io/product-images/14398/04.jpg,https://oleks-netizen.github.io/product-images/14398/05.jpg,https://oleks-netizen.github.io/product-images/14398/06.jpg,https://oleks-netizen.github.io/product-images/14398/07.jpg,https://oleks-netizen.github.io/product-images/14398/08.jpg,https://oleks-netizen.github.io/product-images/14398/09.jpg</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1166,7 +1166,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14404/1.jpg,https://oleks-netizen.github.io/product-images/14404/2.jpg,https://oleks-netizen.github.io/product-images/14404/14.jpg,https://oleks-netizen.github.io/product-images/14404/11.jpg,https://oleks-netizen.github.io/product-images/14404/12.jpg,https://oleks-netizen.github.io/product-images/14404/13.jpg,https://oleks-netizen.github.io/product-images/14404/3.jpg,https://oleks-netizen.github.io/product-images/14404/4.jpg,https://oleks-netizen.github.io/product-images/14404/5.jpg,https://oleks-netizen.github.io/product-images/14404/6.jpg,https://oleks-netizen.github.io/product-images/14404/7.jpg,https://oleks-netizen.github.io/product-images/14404/8.jpg,https://oleks-netizen.github.io/product-images/14404/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14404/01.jpg,https://oleks-netizen.github.io/product-images/14404/02.jpg,https://oleks-netizen.github.io/product-images/14404/14.jpg,https://oleks-netizen.github.io/product-images/14404/11.jpg,https://oleks-netizen.github.io/product-images/14404/12.jpg,https://oleks-netizen.github.io/product-images/14404/13.jpg,https://oleks-netizen.github.io/product-images/14404/03.jpg,https://oleks-netizen.github.io/product-images/14404/04.jpg,https://oleks-netizen.github.io/product-images/14404/05.jpg,https://oleks-netizen.github.io/product-images/14404/06.jpg,https://oleks-netizen.github.io/product-images/14404/07.jpg,https://oleks-netizen.github.io/product-images/14404/08.jpg,https://oleks-netizen.github.io/product-images/14404/09.jpg</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14406/1.jpg,https://oleks-netizen.github.io/product-images/14406/2.jpg,https://oleks-netizen.github.io/product-images/14406/13.jpg,https://oleks-netizen.github.io/product-images/14406/11.jpg,https://oleks-netizen.github.io/product-images/14406/12.jpg,https://oleks-netizen.github.io/product-images/14406/3.jpg,https://oleks-netizen.github.io/product-images/14406/4.jpg,https://oleks-netizen.github.io/product-images/14406/5.jpg,https://oleks-netizen.github.io/product-images/14406/6.jpg,https://oleks-netizen.github.io/product-images/14406/7.jpg,https://oleks-netizen.github.io/product-images/14406/8.jpg,https://oleks-netizen.github.io/product-images/14406/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14406/01.jpg,https://oleks-netizen.github.io/product-images/14406/02.jpg,https://oleks-netizen.github.io/product-images/14406/13.jpg,https://oleks-netizen.github.io/product-images/14406/11.jpg,https://oleks-netizen.github.io/product-images/14406/12.jpg,https://oleks-netizen.github.io/product-images/14406/03.jpg,https://oleks-netizen.github.io/product-images/14406/04.jpg,https://oleks-netizen.github.io/product-images/14406/05.jpg,https://oleks-netizen.github.io/product-images/14406/06.jpg,https://oleks-netizen.github.io/product-images/14406/07.jpg,https://oleks-netizen.github.io/product-images/14406/08.jpg,https://oleks-netizen.github.io/product-images/14406/09.jpg</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1196,7 +1196,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14407/1.jpg,https://oleks-netizen.github.io/product-images/14407/2.jpg,https://oleks-netizen.github.io/product-images/14407/12.jpg,https://oleks-netizen.github.io/product-images/14407/10.jpg,https://oleks-netizen.github.io/product-images/14407/11.jpg,https://oleks-netizen.github.io/product-images/14407/3.jpg,https://oleks-netizen.github.io/product-images/14407/4.jpg,https://oleks-netizen.github.io/product-images/14407/5.jpg,https://oleks-netizen.github.io/product-images/14407/6.jpg,https://oleks-netizen.github.io/product-images/14407/8.jpg,https://oleks-netizen.github.io/product-images/14407/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14407/01.jpg,https://oleks-netizen.github.io/product-images/14407/02.jpg,https://oleks-netizen.github.io/product-images/14407/12.jpg,https://oleks-netizen.github.io/product-images/14407/10.jpg,https://oleks-netizen.github.io/product-images/14407/11.jpg,https://oleks-netizen.github.io/product-images/14407/03.jpg,https://oleks-netizen.github.io/product-images/14407/04.jpg,https://oleks-netizen.github.io/product-images/14407/05.jpg,https://oleks-netizen.github.io/product-images/14407/06.jpg,https://oleks-netizen.github.io/product-images/14407/08.jpg,https://oleks-netizen.github.io/product-images/14407/09.jpg</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1211,7 +1211,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14420/1.jpg,https://oleks-netizen.github.io/product-images/14420/2.jpg,https://oleks-netizen.github.io/product-images/14420/13.jpg,https://oleks-netizen.github.io/product-images/14420/10.jpg,https://oleks-netizen.github.io/product-images/14420/11.jpg,https://oleks-netizen.github.io/product-images/14420/3.jpg,https://oleks-netizen.github.io/product-images/14420/4.jpg,https://oleks-netizen.github.io/product-images/14420/5.jpg,https://oleks-netizen.github.io/product-images/14420/6.jpg,https://oleks-netizen.github.io/product-images/14420/7.jpg,https://oleks-netizen.github.io/product-images/14420/8.jpg,https://oleks-netizen.github.io/product-images/14420/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14420/01.jpg,https://oleks-netizen.github.io/product-images/14420/02.jpg,https://oleks-netizen.github.io/product-images/14420/13.jpg,https://oleks-netizen.github.io/product-images/14420/10.jpg,https://oleks-netizen.github.io/product-images/14420/11.jpg,https://oleks-netizen.github.io/product-images/14420/03.jpg,https://oleks-netizen.github.io/product-images/14420/04.jpg,https://oleks-netizen.github.io/product-images/14420/05.jpg,https://oleks-netizen.github.io/product-images/14420/06.jpg,https://oleks-netizen.github.io/product-images/14420/07.jpg,https://oleks-netizen.github.io/product-images/14420/08.jpg,https://oleks-netizen.github.io/product-images/14420/09.jpg</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14422/1.jpg,https://oleks-netizen.github.io/product-images/14422/2.jpg,https://oleks-netizen.github.io/product-images/14422/10.jpg,https://oleks-netizen.github.io/product-images/14422/3.jpg,https://oleks-netizen.github.io/product-images/14422/4.jpg,https://oleks-netizen.github.io/product-images/14422/5.jpg,https://oleks-netizen.github.io/product-images/14422/6.jpg,https://oleks-netizen.github.io/product-images/14422/7.jpg,https://oleks-netizen.github.io/product-images/14422/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14422/01.jpg,https://oleks-netizen.github.io/product-images/14422/02.jpg,https://oleks-netizen.github.io/product-images/14422/10.jpg,https://oleks-netizen.github.io/product-images/14422/03.jpg,https://oleks-netizen.github.io/product-images/14422/04.jpg,https://oleks-netizen.github.io/product-images/14422/05.jpg,https://oleks-netizen.github.io/product-images/14422/06.jpg,https://oleks-netizen.github.io/product-images/14422/07.jpg,https://oleks-netizen.github.io/product-images/14422/09.jpg</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14429/1.jpg,https://oleks-netizen.github.io/product-images/14429/2.jpg,https://oleks-netizen.github.io/product-images/14429/13.jpg,https://oleks-netizen.github.io/product-images/14429/10.jpg,https://oleks-netizen.github.io/product-images/14429/12.jpg,https://oleks-netizen.github.io/product-images/14429/3.jpg,https://oleks-netizen.github.io/product-images/14429/4.jpg,https://oleks-netizen.github.io/product-images/14429/5.jpg,https://oleks-netizen.github.io/product-images/14429/6.jpg,https://oleks-netizen.github.io/product-images/14429/7.jpg,https://oleks-netizen.github.io/product-images/14429/8.jpg,https://oleks-netizen.github.io/product-images/14429/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14429/01.jpg,https://oleks-netizen.github.io/product-images/14429/02.jpg,https://oleks-netizen.github.io/product-images/14429/13.jpg,https://oleks-netizen.github.io/product-images/14429/10.jpg,https://oleks-netizen.github.io/product-images/14429/12.jpg,https://oleks-netizen.github.io/product-images/14429/03.jpg,https://oleks-netizen.github.io/product-images/14429/04.jpg,https://oleks-netizen.github.io/product-images/14429/05.jpg,https://oleks-netizen.github.io/product-images/14429/06.jpg,https://oleks-netizen.github.io/product-images/14429/07.jpg,https://oleks-netizen.github.io/product-images/14429/08.jpg,https://oleks-netizen.github.io/product-images/14429/09.jpg</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -1256,7 +1256,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14436/1.jpg,https://oleks-netizen.github.io/product-images/14436/2.jpg,https://oleks-netizen.github.io/product-images/14436/11.jpg,https://oleks-netizen.github.io/product-images/14436/10.jpg,https://oleks-netizen.github.io/product-images/14436/3.jpg,https://oleks-netizen.github.io/product-images/14436/4.jpg,https://oleks-netizen.github.io/product-images/14436/5.jpg,https://oleks-netizen.github.io/product-images/14436/6.jpg,https://oleks-netizen.github.io/product-images/14436/8.jpg,https://oleks-netizen.github.io/product-images/14436/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14436/01.jpg,https://oleks-netizen.github.io/product-images/14436/02.jpg,https://oleks-netizen.github.io/product-images/14436/11.jpg,https://oleks-netizen.github.io/product-images/14436/10.jpg,https://oleks-netizen.github.io/product-images/14436/03.jpg,https://oleks-netizen.github.io/product-images/14436/04.jpg,https://oleks-netizen.github.io/product-images/14436/05.jpg,https://oleks-netizen.github.io/product-images/14436/06.jpg,https://oleks-netizen.github.io/product-images/14436/08.jpg,https://oleks-netizen.github.io/product-images/14436/09.jpg</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -1271,7 +1271,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14437/1.jpg,https://oleks-netizen.github.io/product-images/14437/2.jpg,https://oleks-netizen.github.io/product-images/14437/12.jpg,https://oleks-netizen.github.io/product-images/14437/10.jpg,https://oleks-netizen.github.io/product-images/14437/11.jpg,https://oleks-netizen.github.io/product-images/14437/3.jpg,https://oleks-netizen.github.io/product-images/14437/4.jpg,https://oleks-netizen.github.io/product-images/14437/5.jpg,https://oleks-netizen.github.io/product-images/14437/6.jpg,https://oleks-netizen.github.io/product-images/14437/7.jpg,https://oleks-netizen.github.io/product-images/14437/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14437/01.jpg,https://oleks-netizen.github.io/product-images/14437/02.jpg,https://oleks-netizen.github.io/product-images/14437/12.jpg,https://oleks-netizen.github.io/product-images/14437/10.jpg,https://oleks-netizen.github.io/product-images/14437/11.jpg,https://oleks-netizen.github.io/product-images/14437/03.jpg,https://oleks-netizen.github.io/product-images/14437/04.jpg,https://oleks-netizen.github.io/product-images/14437/05.jpg,https://oleks-netizen.github.io/product-images/14437/06.jpg,https://oleks-netizen.github.io/product-images/14437/07.jpg,https://oleks-netizen.github.io/product-images/14437/09.jpg</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -1286,7 +1286,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14439/1.jpg,https://oleks-netizen.github.io/product-images/14439/2.jpg,https://oleks-netizen.github.io/product-images/14439/7.jpg,https://oleks-netizen.github.io/product-images/14439/9.jpg,https://oleks-netizen.github.io/product-images/14439/3.jpg,https://oleks-netizen.github.io/product-images/14439/4.jpg,https://oleks-netizen.github.io/product-images/14439/5.jpg,https://oleks-netizen.github.io/product-images/14439/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14439/01.jpg,https://oleks-netizen.github.io/product-images/14439/02.jpg,https://oleks-netizen.github.io/product-images/14439/07.jpg,https://oleks-netizen.github.io/product-images/14439/09.jpg,https://oleks-netizen.github.io/product-images/14439/03.jpg,https://oleks-netizen.github.io/product-images/14439/04.jpg,https://oleks-netizen.github.io/product-images/14439/05.jpg,https://oleks-netizen.github.io/product-images/14439/06.jpg</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -1301,7 +1301,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14445/1.jpg,https://oleks-netizen.github.io/product-images/14445/2.jpg,https://oleks-netizen.github.io/product-images/14445/12.jpg,https://oleks-netizen.github.io/product-images/14445/11.jpg,https://oleks-netizen.github.io/product-images/14445/3.jpg,https://oleks-netizen.github.io/product-images/14445/4.jpg,https://oleks-netizen.github.io/product-images/14445/5.jpg,https://oleks-netizen.github.io/product-images/14445/6.jpg,https://oleks-netizen.github.io/product-images/14445/7.jpg,https://oleks-netizen.github.io/product-images/14445/8.jpg,https://oleks-netizen.github.io/product-images/14445/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14445/01.jpg,https://oleks-netizen.github.io/product-images/14445/02.jpg,https://oleks-netizen.github.io/product-images/14445/12.jpg,https://oleks-netizen.github.io/product-images/14445/11.jpg,https://oleks-netizen.github.io/product-images/14445/03.jpg,https://oleks-netizen.github.io/product-images/14445/04.jpg,https://oleks-netizen.github.io/product-images/14445/05.jpg,https://oleks-netizen.github.io/product-images/14445/06.jpg,https://oleks-netizen.github.io/product-images/14445/07.jpg,https://oleks-netizen.github.io/product-images/14445/08.jpg,https://oleks-netizen.github.io/product-images/14445/09.jpg</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -1316,7 +1316,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14446/1.jpg,https://oleks-netizen.github.io/product-images/14446/2.jpg,https://oleks-netizen.github.io/product-images/14446/9.jpg,https://oleks-netizen.github.io/product-images/14446/3.jpg,https://oleks-netizen.github.io/product-images/14446/4.jpg,https://oleks-netizen.github.io/product-images/14446/5.jpg,https://oleks-netizen.github.io/product-images/14446/6.jpg,https://oleks-netizen.github.io/product-images/14446/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14446/01.jpg,https://oleks-netizen.github.io/product-images/14446/02.jpg,https://oleks-netizen.github.io/product-images/14446/09.jpg,https://oleks-netizen.github.io/product-images/14446/03.jpg,https://oleks-netizen.github.io/product-images/14446/04.jpg,https://oleks-netizen.github.io/product-images/14446/05.jpg,https://oleks-netizen.github.io/product-images/14446/06.jpg,https://oleks-netizen.github.io/product-images/14446/07.jpg</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -1331,7 +1331,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14448/1.jpg,https://oleks-netizen.github.io/product-images/14448/2.jpg,https://oleks-netizen.github.io/product-images/14448/13.jpg,https://oleks-netizen.github.io/product-images/14448/10.jpg,https://oleks-netizen.github.io/product-images/14448/12.jpg,https://oleks-netizen.github.io/product-images/14448/3.jpg,https://oleks-netizen.github.io/product-images/14448/4.jpg,https://oleks-netizen.github.io/product-images/14448/5.jpg,https://oleks-netizen.github.io/product-images/14448/6.jpg,https://oleks-netizen.github.io/product-images/14448/7.jpg,https://oleks-netizen.github.io/product-images/14448/8.jpg,https://oleks-netizen.github.io/product-images/14448/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14448/01.jpg,https://oleks-netizen.github.io/product-images/14448/02.jpg,https://oleks-netizen.github.io/product-images/14448/13.jpg,https://oleks-netizen.github.io/product-images/14448/10.jpg,https://oleks-netizen.github.io/product-images/14448/12.jpg,https://oleks-netizen.github.io/product-images/14448/03.jpg,https://oleks-netizen.github.io/product-images/14448/04.jpg,https://oleks-netizen.github.io/product-images/14448/05.jpg,https://oleks-netizen.github.io/product-images/14448/06.jpg,https://oleks-netizen.github.io/product-images/14448/07.jpg,https://oleks-netizen.github.io/product-images/14448/08.jpg,https://oleks-netizen.github.io/product-images/14448/09.jpg</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -1346,7 +1346,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14449/1.jpg,https://oleks-netizen.github.io/product-images/14449/2.jpg,https://oleks-netizen.github.io/product-images/14449/12.jpg,https://oleks-netizen.github.io/product-images/14449/10.jpg,https://oleks-netizen.github.io/product-images/14449/11.jpg,https://oleks-netizen.github.io/product-images/14449/3.jpg,https://oleks-netizen.github.io/product-images/14449/4.jpg,https://oleks-netizen.github.io/product-images/14449/5.jpg,https://oleks-netizen.github.io/product-images/14449/7.jpg,https://oleks-netizen.github.io/product-images/14449/8.jpg,https://oleks-netizen.github.io/product-images/14449/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14449/01.jpg,https://oleks-netizen.github.io/product-images/14449/02.jpg,https://oleks-netizen.github.io/product-images/14449/12.jpg,https://oleks-netizen.github.io/product-images/14449/10.jpg,https://oleks-netizen.github.io/product-images/14449/11.jpg,https://oleks-netizen.github.io/product-images/14449/03.jpg,https://oleks-netizen.github.io/product-images/14449/04.jpg,https://oleks-netizen.github.io/product-images/14449/05.jpg,https://oleks-netizen.github.io/product-images/14449/07.jpg,https://oleks-netizen.github.io/product-images/14449/08.jpg,https://oleks-netizen.github.io/product-images/14449/09.jpg</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -1361,7 +1361,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14452/1.jpg,https://oleks-netizen.github.io/product-images/14452/2.jpg,https://oleks-netizen.github.io/product-images/14452/15.jpg,https://oleks-netizen.github.io/product-images/14452/10.jpg,https://oleks-netizen.github.io/product-images/14452/11.jpg,https://oleks-netizen.github.io/product-images/14452/12.jpg,https://oleks-netizen.github.io/product-images/14452/13.jpg,https://oleks-netizen.github.io/product-images/14452/3.jpg,https://oleks-netizen.github.io/product-images/14452/4.jpg,https://oleks-netizen.github.io/product-images/14452/5.jpg,https://oleks-netizen.github.io/product-images/14452/6.jpg,https://oleks-netizen.github.io/product-images/14452/7.jpg,https://oleks-netizen.github.io/product-images/14452/8.jpg,https://oleks-netizen.github.io/product-images/14452/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14452/01.jpg,https://oleks-netizen.github.io/product-images/14452/02.jpg,https://oleks-netizen.github.io/product-images/14452/15.jpg,https://oleks-netizen.github.io/product-images/14452/10.jpg,https://oleks-netizen.github.io/product-images/14452/11.jpg,https://oleks-netizen.github.io/product-images/14452/12.jpg,https://oleks-netizen.github.io/product-images/14452/13.jpg,https://oleks-netizen.github.io/product-images/14452/03.jpg,https://oleks-netizen.github.io/product-images/14452/04.jpg,https://oleks-netizen.github.io/product-images/14452/05.jpg,https://oleks-netizen.github.io/product-images/14452/06.jpg,https://oleks-netizen.github.io/product-images/14452/07.jpg,https://oleks-netizen.github.io/product-images/14452/08.jpg,https://oleks-netizen.github.io/product-images/14452/09.jpg</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -1376,7 +1376,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14455/1.jpg,https://oleks-netizen.github.io/product-images/14455/2.jpg,https://oleks-netizen.github.io/product-images/14455/10.jpg,https://oleks-netizen.github.io/product-images/14455/3.jpg,https://oleks-netizen.github.io/product-images/14455/4.jpg,https://oleks-netizen.github.io/product-images/14455/6.jpg,https://oleks-netizen.github.io/product-images/14455/7.jpg,https://oleks-netizen.github.io/product-images/14455/8.jpg,https://oleks-netizen.github.io/product-images/14455/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14455/01.jpg,https://oleks-netizen.github.io/product-images/14455/02.jpg,https://oleks-netizen.github.io/product-images/14455/10.jpg,https://oleks-netizen.github.io/product-images/14455/03.jpg,https://oleks-netizen.github.io/product-images/14455/04.jpg,https://oleks-netizen.github.io/product-images/14455/06.jpg,https://oleks-netizen.github.io/product-images/14455/07.jpg,https://oleks-netizen.github.io/product-images/14455/08.jpg,https://oleks-netizen.github.io/product-images/14455/09.jpg</t>
         </is>
       </c>
       <c r="C64" t="n">
@@ -1391,7 +1391,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14459/1.jpg,https://oleks-netizen.github.io/product-images/14459/2.jpg,https://oleks-netizen.github.io/product-images/14459/10.jpg,https://oleks-netizen.github.io/product-images/14459/3.jpg,https://oleks-netizen.github.io/product-images/14459/4.jpg,https://oleks-netizen.github.io/product-images/14459/5.jpg,https://oleks-netizen.github.io/product-images/14459/6.jpg,https://oleks-netizen.github.io/product-images/14459/7.jpg,https://oleks-netizen.github.io/product-images/14459/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14459/01.jpg,https://oleks-netizen.github.io/product-images/14459/02.jpg,https://oleks-netizen.github.io/product-images/14459/10.jpg,https://oleks-netizen.github.io/product-images/14459/03.jpg,https://oleks-netizen.github.io/product-images/14459/04.jpg,https://oleks-netizen.github.io/product-images/14459/05.jpg,https://oleks-netizen.github.io/product-images/14459/06.jpg,https://oleks-netizen.github.io/product-images/14459/07.jpg,https://oleks-netizen.github.io/product-images/14459/08.jpg</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -1406,7 +1406,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14462/1.jpg,https://oleks-netizen.github.io/product-images/14462/2.jpg,https://oleks-netizen.github.io/product-images/14462/8.jpg,https://oleks-netizen.github.io/product-images/14462/11.jpg,https://oleks-netizen.github.io/product-images/14462/3.jpg,https://oleks-netizen.github.io/product-images/14462/4.jpg,https://oleks-netizen.github.io/product-images/14462/5.jpg,https://oleks-netizen.github.io/product-images/14462/6.jpg,https://oleks-netizen.github.io/product-images/14462/7.jpg,https://oleks-netizen.github.io/product-images/14462/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14462/01.jpg,https://oleks-netizen.github.io/product-images/14462/02.jpg,https://oleks-netizen.github.io/product-images/14462/08.jpg,https://oleks-netizen.github.io/product-images/14462/11.jpg,https://oleks-netizen.github.io/product-images/14462/03.jpg,https://oleks-netizen.github.io/product-images/14462/04.jpg,https://oleks-netizen.github.io/product-images/14462/05.jpg,https://oleks-netizen.github.io/product-images/14462/06.jpg,https://oleks-netizen.github.io/product-images/14462/07.jpg,https://oleks-netizen.github.io/product-images/14462/09.jpg</t>
         </is>
       </c>
       <c r="C66" t="n">
@@ -1421,7 +1421,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14463/1.jpg,https://oleks-netizen.github.io/product-images/14463/2.jpg,https://oleks-netizen.github.io/product-images/14463/4.jpg,https://oleks-netizen.github.io/product-images/14463/9.jpg,https://oleks-netizen.github.io/product-images/14463/3.jpg,https://oleks-netizen.github.io/product-images/14463/5.jpg,https://oleks-netizen.github.io/product-images/14463/6.jpg,https://oleks-netizen.github.io/product-images/14463/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14463/01.jpg,https://oleks-netizen.github.io/product-images/14463/02.jpg,https://oleks-netizen.github.io/product-images/14463/04.jpg,https://oleks-netizen.github.io/product-images/14463/09.jpg,https://oleks-netizen.github.io/product-images/14463/03.jpg,https://oleks-netizen.github.io/product-images/14463/05.jpg,https://oleks-netizen.github.io/product-images/14463/06.jpg,https://oleks-netizen.github.io/product-images/14463/07.jpg</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -1436,7 +1436,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14464/1.jpg,https://oleks-netizen.github.io/product-images/14464/2.jpg,https://oleks-netizen.github.io/product-images/14464/16.jpg,https://oleks-netizen.github.io/product-images/14464/11.jpg,https://oleks-netizen.github.io/product-images/14464/12.jpg,https://oleks-netizen.github.io/product-images/14464/13.jpg,https://oleks-netizen.github.io/product-images/14464/14.jpg,https://oleks-netizen.github.io/product-images/14464/15.jpg,https://oleks-netizen.github.io/product-images/14464/3.jpg,https://oleks-netizen.github.io/product-images/14464/4.jpg,https://oleks-netizen.github.io/product-images/14464/5.jpg,https://oleks-netizen.github.io/product-images/14464/6.jpg,https://oleks-netizen.github.io/product-images/14464/7.jpg,https://oleks-netizen.github.io/product-images/14464/8.jpg,https://oleks-netizen.github.io/product-images/14464/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14464/01.jpg,https://oleks-netizen.github.io/product-images/14464/02.jpg,https://oleks-netizen.github.io/product-images/14464/16.jpg,https://oleks-netizen.github.io/product-images/14464/11.jpg,https://oleks-netizen.github.io/product-images/14464/12.jpg,https://oleks-netizen.github.io/product-images/14464/13.jpg,https://oleks-netizen.github.io/product-images/14464/14.jpg,https://oleks-netizen.github.io/product-images/14464/15.jpg,https://oleks-netizen.github.io/product-images/14464/03.jpg,https://oleks-netizen.github.io/product-images/14464/04.jpg,https://oleks-netizen.github.io/product-images/14464/05.jpg,https://oleks-netizen.github.io/product-images/14464/06.jpg,https://oleks-netizen.github.io/product-images/14464/07.jpg,https://oleks-netizen.github.io/product-images/14464/08.jpg,https://oleks-netizen.github.io/product-images/14464/09.jpg</t>
         </is>
       </c>
       <c r="C68" t="n">
@@ -1451,7 +1451,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14467/1.jpg,https://oleks-netizen.github.io/product-images/14467/2.jpg,https://oleks-netizen.github.io/product-images/14467/13.jpg,https://oleks-netizen.github.io/product-images/14467/10.jpg,https://oleks-netizen.github.io/product-images/14467/12.jpg,https://oleks-netizen.github.io/product-images/14467/3.jpg,https://oleks-netizen.github.io/product-images/14467/4.jpg,https://oleks-netizen.github.io/product-images/14467/5.jpg,https://oleks-netizen.github.io/product-images/14467/6.jpg,https://oleks-netizen.github.io/product-images/14467/7.jpg,https://oleks-netizen.github.io/product-images/14467/8.jpg,https://oleks-netizen.github.io/product-images/14467/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14467/01.jpg,https://oleks-netizen.github.io/product-images/14467/02.jpg,https://oleks-netizen.github.io/product-images/14467/13.jpg,https://oleks-netizen.github.io/product-images/14467/10.jpg,https://oleks-netizen.github.io/product-images/14467/12.jpg,https://oleks-netizen.github.io/product-images/14467/03.jpg,https://oleks-netizen.github.io/product-images/14467/04.jpg,https://oleks-netizen.github.io/product-images/14467/05.jpg,https://oleks-netizen.github.io/product-images/14467/06.jpg,https://oleks-netizen.github.io/product-images/14467/07.jpg,https://oleks-netizen.github.io/product-images/14467/08.jpg,https://oleks-netizen.github.io/product-images/14467/09.jpg</t>
         </is>
       </c>
       <c r="C69" t="n">
@@ -1466,7 +1466,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14473/1.jpg,https://oleks-netizen.github.io/product-images/14473/2.jpg,https://oleks-netizen.github.io/product-images/14473/6.jpg,https://oleks-netizen.github.io/product-images/14473/11.jpg,https://oleks-netizen.github.io/product-images/14473/3.jpg,https://oleks-netizen.github.io/product-images/14473/4.jpg,https://oleks-netizen.github.io/product-images/14473/5.jpg,https://oleks-netizen.github.io/product-images/14473/7.jpg,https://oleks-netizen.github.io/product-images/14473/8.jpg,https://oleks-netizen.github.io/product-images/14473/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14473/01.jpg,https://oleks-netizen.github.io/product-images/14473/02.jpg,https://oleks-netizen.github.io/product-images/14473/06.jpg,https://oleks-netizen.github.io/product-images/14473/11.jpg,https://oleks-netizen.github.io/product-images/14473/03.jpg,https://oleks-netizen.github.io/product-images/14473/04.jpg,https://oleks-netizen.github.io/product-images/14473/05.jpg,https://oleks-netizen.github.io/product-images/14473/07.jpg,https://oleks-netizen.github.io/product-images/14473/08.jpg,https://oleks-netizen.github.io/product-images/14473/09.jpg</t>
         </is>
       </c>
       <c r="C70" t="n">
@@ -1481,7 +1481,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14474/1.jpg,https://oleks-netizen.github.io/product-images/14474/2.jpg,https://oleks-netizen.github.io/product-images/14474/6.jpg,https://oleks-netizen.github.io/product-images/14474/11.jpg,https://oleks-netizen.github.io/product-images/14474/10.jpg,https://oleks-netizen.github.io/product-images/14474/3.jpg,https://oleks-netizen.github.io/product-images/14474/4.jpg,https://oleks-netizen.github.io/product-images/14474/5.jpg,https://oleks-netizen.github.io/product-images/14474/8.jpg,https://oleks-netizen.github.io/product-images/14474/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14474/01.jpg,https://oleks-netizen.github.io/product-images/14474/02.jpg,https://oleks-netizen.github.io/product-images/14474/06.jpg,https://oleks-netizen.github.io/product-images/14474/11.jpg,https://oleks-netizen.github.io/product-images/14474/10.jpg,https://oleks-netizen.github.io/product-images/14474/03.jpg,https://oleks-netizen.github.io/product-images/14474/04.jpg,https://oleks-netizen.github.io/product-images/14474/05.jpg,https://oleks-netizen.github.io/product-images/14474/08.jpg,https://oleks-netizen.github.io/product-images/14474/09.jpg</t>
         </is>
       </c>
       <c r="C71" t="n">
@@ -1496,7 +1496,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14478/1.jpg,https://oleks-netizen.github.io/product-images/14478/2.jpg,https://oleks-netizen.github.io/product-images/14478/7.jpg,https://oleks-netizen.github.io/product-images/14478/11.jpg,https://oleks-netizen.github.io/product-images/14478/10.jpg,https://oleks-netizen.github.io/product-images/14478/3.jpg,https://oleks-netizen.github.io/product-images/14478/4.jpg,https://oleks-netizen.github.io/product-images/14478/5.jpg,https://oleks-netizen.github.io/product-images/14478/6.jpg,https://oleks-netizen.github.io/product-images/14478/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14478/01.jpg,https://oleks-netizen.github.io/product-images/14478/02.jpg,https://oleks-netizen.github.io/product-images/14478/07.jpg,https://oleks-netizen.github.io/product-images/14478/11.jpg,https://oleks-netizen.github.io/product-images/14478/10.jpg,https://oleks-netizen.github.io/product-images/14478/03.jpg,https://oleks-netizen.github.io/product-images/14478/04.jpg,https://oleks-netizen.github.io/product-images/14478/05.jpg,https://oleks-netizen.github.io/product-images/14478/06.jpg,https://oleks-netizen.github.io/product-images/14478/08.jpg</t>
         </is>
       </c>
       <c r="C72" t="n">
@@ -1511,7 +1511,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14479/1.jpg,https://oleks-netizen.github.io/product-images/14479/2.jpg,https://oleks-netizen.github.io/product-images/14479/11.jpg,https://oleks-netizen.github.io/product-images/14479/10.jpg,https://oleks-netizen.github.io/product-images/14479/3.jpg,https://oleks-netizen.github.io/product-images/14479/4.jpg,https://oleks-netizen.github.io/product-images/14479/5.jpg,https://oleks-netizen.github.io/product-images/14479/6.jpg,https://oleks-netizen.github.io/product-images/14479/8.jpg,https://oleks-netizen.github.io/product-images/14479/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14479/01.jpg,https://oleks-netizen.github.io/product-images/14479/02.jpg,https://oleks-netizen.github.io/product-images/14479/11.jpg,https://oleks-netizen.github.io/product-images/14479/10.jpg,https://oleks-netizen.github.io/product-images/14479/03.jpg,https://oleks-netizen.github.io/product-images/14479/04.jpg,https://oleks-netizen.github.io/product-images/14479/05.jpg,https://oleks-netizen.github.io/product-images/14479/06.jpg,https://oleks-netizen.github.io/product-images/14479/08.jpg,https://oleks-netizen.github.io/product-images/14479/09.jpg</t>
         </is>
       </c>
       <c r="C73" t="n">
@@ -1526,7 +1526,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14484/1.jpg,https://oleks-netizen.github.io/product-images/14484/2.jpg,https://oleks-netizen.github.io/product-images/14484/14.jpg,https://oleks-netizen.github.io/product-images/14484/10.jpg,https://oleks-netizen.github.io/product-images/14484/11.jpg,https://oleks-netizen.github.io/product-images/14484/12.jpg,https://oleks-netizen.github.io/product-images/14484/3.jpg,https://oleks-netizen.github.io/product-images/14484/4.jpg,https://oleks-netizen.github.io/product-images/14484/5.jpg,https://oleks-netizen.github.io/product-images/14484/6.jpg,https://oleks-netizen.github.io/product-images/14484/7.jpg,https://oleks-netizen.github.io/product-images/14484/8.jpg,https://oleks-netizen.github.io/product-images/14484/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14484/01.jpg,https://oleks-netizen.github.io/product-images/14484/02.jpg,https://oleks-netizen.github.io/product-images/14484/14.jpg,https://oleks-netizen.github.io/product-images/14484/10.jpg,https://oleks-netizen.github.io/product-images/14484/11.jpg,https://oleks-netizen.github.io/product-images/14484/12.jpg,https://oleks-netizen.github.io/product-images/14484/03.jpg,https://oleks-netizen.github.io/product-images/14484/04.jpg,https://oleks-netizen.github.io/product-images/14484/05.jpg,https://oleks-netizen.github.io/product-images/14484/06.jpg,https://oleks-netizen.github.io/product-images/14484/07.jpg,https://oleks-netizen.github.io/product-images/14484/08.jpg,https://oleks-netizen.github.io/product-images/14484/09.jpg</t>
         </is>
       </c>
       <c r="C74" t="n">
@@ -1541,7 +1541,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14497/1.jpg,https://oleks-netizen.github.io/product-images/14497/2.jpg,https://oleks-netizen.github.io/product-images/14497/13.jpg,https://oleks-netizen.github.io/product-images/14497/11.jpg,https://oleks-netizen.github.io/product-images/14497/12.jpg,https://oleks-netizen.github.io/product-images/14497/3.jpg,https://oleks-netizen.github.io/product-images/14497/4.jpg,https://oleks-netizen.github.io/product-images/14497/5.jpg,https://oleks-netizen.github.io/product-images/14497/6.jpg,https://oleks-netizen.github.io/product-images/14497/7.jpg,https://oleks-netizen.github.io/product-images/14497/8.jpg,https://oleks-netizen.github.io/product-images/14497/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14497/01.jpg,https://oleks-netizen.github.io/product-images/14497/02.jpg,https://oleks-netizen.github.io/product-images/14497/13.jpg,https://oleks-netizen.github.io/product-images/14497/11.jpg,https://oleks-netizen.github.io/product-images/14497/12.jpg,https://oleks-netizen.github.io/product-images/14497/03.jpg,https://oleks-netizen.github.io/product-images/14497/04.jpg,https://oleks-netizen.github.io/product-images/14497/05.jpg,https://oleks-netizen.github.io/product-images/14497/06.jpg,https://oleks-netizen.github.io/product-images/14497/07.jpg,https://oleks-netizen.github.io/product-images/14497/08.jpg,https://oleks-netizen.github.io/product-images/14497/09.jpg</t>
         </is>
       </c>
       <c r="C75" t="n">
@@ -1556,7 +1556,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14499/1.jpg,https://oleks-netizen.github.io/product-images/14499/2.jpg,https://oleks-netizen.github.io/product-images/14499/10.jpg,https://oleks-netizen.github.io/product-images/14499/3.jpg,https://oleks-netizen.github.io/product-images/14499/4.jpg,https://oleks-netizen.github.io/product-images/14499/5.jpg,https://oleks-netizen.github.io/product-images/14499/6.jpg,https://oleks-netizen.github.io/product-images/14499/8.jpg,https://oleks-netizen.github.io/product-images/14499/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14499/01.jpg,https://oleks-netizen.github.io/product-images/14499/02.jpg,https://oleks-netizen.github.io/product-images/14499/10.jpg,https://oleks-netizen.github.io/product-images/14499/03.jpg,https://oleks-netizen.github.io/product-images/14499/04.jpg,https://oleks-netizen.github.io/product-images/14499/05.jpg,https://oleks-netizen.github.io/product-images/14499/06.jpg,https://oleks-netizen.github.io/product-images/14499/08.jpg,https://oleks-netizen.github.io/product-images/14499/09.jpg</t>
         </is>
       </c>
       <c r="C76" t="n">
@@ -1571,7 +1571,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14500/1.jpg,https://oleks-netizen.github.io/product-images/14500/2.jpg,https://oleks-netizen.github.io/product-images/14500/8.jpg,https://oleks-netizen.github.io/product-images/14500/10.jpg,https://oleks-netizen.github.io/product-images/14500/3.jpg,https://oleks-netizen.github.io/product-images/14500/4.jpg,https://oleks-netizen.github.io/product-images/14500/6.jpg,https://oleks-netizen.github.io/product-images/14500/7.jpg,https://oleks-netizen.github.io/product-images/14500/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14500/01.jpg,https://oleks-netizen.github.io/product-images/14500/02.jpg,https://oleks-netizen.github.io/product-images/14500/08.jpg,https://oleks-netizen.github.io/product-images/14500/10.jpg,https://oleks-netizen.github.io/product-images/14500/03.jpg,https://oleks-netizen.github.io/product-images/14500/04.jpg,https://oleks-netizen.github.io/product-images/14500/06.jpg,https://oleks-netizen.github.io/product-images/14500/07.jpg,https://oleks-netizen.github.io/product-images/14500/09.jpg</t>
         </is>
       </c>
       <c r="C77" t="n">
@@ -1586,7 +1586,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14501/1.jpg,https://oleks-netizen.github.io/product-images/14501/2.jpg,https://oleks-netizen.github.io/product-images/14501/5.jpg,https://oleks-netizen.github.io/product-images/14501/8.jpg,https://oleks-netizen.github.io/product-images/14501/3.jpg,https://oleks-netizen.github.io/product-images/14501/4.jpg,https://oleks-netizen.github.io/product-images/14501/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14501/01.jpg,https://oleks-netizen.github.io/product-images/14501/02.jpg,https://oleks-netizen.github.io/product-images/14501/05.jpg,https://oleks-netizen.github.io/product-images/14501/08.jpg,https://oleks-netizen.github.io/product-images/14501/03.jpg,https://oleks-netizen.github.io/product-images/14501/04.jpg,https://oleks-netizen.github.io/product-images/14501/06.jpg</t>
         </is>
       </c>
       <c r="C78" t="n">
@@ -1601,7 +1601,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14509/1.jpg,https://oleks-netizen.github.io/product-images/14509/2.jpg,https://oleks-netizen.github.io/product-images/14509/10.jpg,https://oleks-netizen.github.io/product-images/14509/3.jpg,https://oleks-netizen.github.io/product-images/14509/4.jpg,https://oleks-netizen.github.io/product-images/14509/5.jpg,https://oleks-netizen.github.io/product-images/14509/6.jpg,https://oleks-netizen.github.io/product-images/14509/8.jpg,https://oleks-netizen.github.io/product-images/14509/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14509/01.jpg,https://oleks-netizen.github.io/product-images/14509/02.jpg,https://oleks-netizen.github.io/product-images/14509/10.jpg,https://oleks-netizen.github.io/product-images/14509/03.jpg,https://oleks-netizen.github.io/product-images/14509/04.jpg,https://oleks-netizen.github.io/product-images/14509/05.jpg,https://oleks-netizen.github.io/product-images/14509/06.jpg,https://oleks-netizen.github.io/product-images/14509/08.jpg,https://oleks-netizen.github.io/product-images/14509/09.jpg</t>
         </is>
       </c>
       <c r="C79" t="n">
@@ -1616,7 +1616,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14512/1.jpg,https://oleks-netizen.github.io/product-images/14512/2.jpg,https://oleks-netizen.github.io/product-images/14512/5.jpg,https://oleks-netizen.github.io/product-images/14512/9.jpg,https://oleks-netizen.github.io/product-images/14512/3.jpg,https://oleks-netizen.github.io/product-images/14512/4.jpg,https://oleks-netizen.github.io/product-images/14512/6.jpg,https://oleks-netizen.github.io/product-images/14512/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14512/01.jpg,https://oleks-netizen.github.io/product-images/14512/02.jpg,https://oleks-netizen.github.io/product-images/14512/05.jpg,https://oleks-netizen.github.io/product-images/14512/09.jpg,https://oleks-netizen.github.io/product-images/14512/03.jpg,https://oleks-netizen.github.io/product-images/14512/04.jpg,https://oleks-netizen.github.io/product-images/14512/06.jpg,https://oleks-netizen.github.io/product-images/14512/07.jpg</t>
         </is>
       </c>
       <c r="C80" t="n">
@@ -1631,7 +1631,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14515/1.jpg,https://oleks-netizen.github.io/product-images/14515/2.jpg,https://oleks-netizen.github.io/product-images/14515/5.jpg,https://oleks-netizen.github.io/product-images/14515/9.jpg,https://oleks-netizen.github.io/product-images/14515/3.jpg,https://oleks-netizen.github.io/product-images/14515/4.jpg,https://oleks-netizen.github.io/product-images/14515/6.jpg,https://oleks-netizen.github.io/product-images/14515/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14515/01.jpg,https://oleks-netizen.github.io/product-images/14515/02.jpg,https://oleks-netizen.github.io/product-images/14515/05.jpg,https://oleks-netizen.github.io/product-images/14515/09.jpg,https://oleks-netizen.github.io/product-images/14515/03.jpg,https://oleks-netizen.github.io/product-images/14515/04.jpg,https://oleks-netizen.github.io/product-images/14515/06.jpg,https://oleks-netizen.github.io/product-images/14515/07.jpg</t>
         </is>
       </c>
       <c r="C81" t="n">
@@ -1646,7 +1646,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14516/1.jpg,https://oleks-netizen.github.io/product-images/14516/2.jpg,https://oleks-netizen.github.io/product-images/14516/6.jpg,https://oleks-netizen.github.io/product-images/14516/10.jpg,https://oleks-netizen.github.io/product-images/14516/3.jpg,https://oleks-netizen.github.io/product-images/14516/4.jpg,https://oleks-netizen.github.io/product-images/14516/5.jpg,https://oleks-netizen.github.io/product-images/14516/7.jpg,https://oleks-netizen.github.io/product-images/14516/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14516/01.jpg,https://oleks-netizen.github.io/product-images/14516/02.jpg,https://oleks-netizen.github.io/product-images/14516/06.jpg,https://oleks-netizen.github.io/product-images/14516/10.jpg,https://oleks-netizen.github.io/product-images/14516/03.jpg,https://oleks-netizen.github.io/product-images/14516/04.jpg,https://oleks-netizen.github.io/product-images/14516/05.jpg,https://oleks-netizen.github.io/product-images/14516/07.jpg,https://oleks-netizen.github.io/product-images/14516/09.jpg</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -1661,7 +1661,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14531/1.jpg,https://oleks-netizen.github.io/product-images/14531/2.jpg,https://oleks-netizen.github.io/product-images/14531/4.jpg,https://oleks-netizen.github.io/product-images/14531/8.jpg,https://oleks-netizen.github.io/product-images/14531/3.jpg,https://oleks-netizen.github.io/product-images/14531/5.jpg,https://oleks-netizen.github.io/product-images/14531/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14531/01.jpg,https://oleks-netizen.github.io/product-images/14531/02.jpg,https://oleks-netizen.github.io/product-images/14531/04.jpg,https://oleks-netizen.github.io/product-images/14531/08.jpg,https://oleks-netizen.github.io/product-images/14531/03.jpg,https://oleks-netizen.github.io/product-images/14531/05.jpg,https://oleks-netizen.github.io/product-images/14531/06.jpg</t>
         </is>
       </c>
       <c r="C83" t="n">
@@ -1676,7 +1676,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14532/1.jpg,https://oleks-netizen.github.io/product-images/14532/2.jpg,https://oleks-netizen.github.io/product-images/14532/9.jpg,https://oleks-netizen.github.io/product-images/14532/3.jpg,https://oleks-netizen.github.io/product-images/14532/4.jpg,https://oleks-netizen.github.io/product-images/14532/5.jpg,https://oleks-netizen.github.io/product-images/14532/7.jpg,https://oleks-netizen.github.io/product-images/14532/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14532/01.jpg,https://oleks-netizen.github.io/product-images/14532/02.jpg,https://oleks-netizen.github.io/product-images/14532/09.jpg,https://oleks-netizen.github.io/product-images/14532/03.jpg,https://oleks-netizen.github.io/product-images/14532/04.jpg,https://oleks-netizen.github.io/product-images/14532/05.jpg,https://oleks-netizen.github.io/product-images/14532/07.jpg,https://oleks-netizen.github.io/product-images/14532/08.jpg</t>
         </is>
       </c>
       <c r="C84" t="n">
@@ -1691,7 +1691,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14534/1.jpg,https://oleks-netizen.github.io/product-images/14534/2.jpg,https://oleks-netizen.github.io/product-images/14534/14.jpg,https://oleks-netizen.github.io/product-images/14534/11.jpg,https://oleks-netizen.github.io/product-images/14534/12.jpg,https://oleks-netizen.github.io/product-images/14534/13.jpg,https://oleks-netizen.github.io/product-images/14534/3.jpg,https://oleks-netizen.github.io/product-images/14534/4.jpg,https://oleks-netizen.github.io/product-images/14534/5.jpg,https://oleks-netizen.github.io/product-images/14534/6.jpg,https://oleks-netizen.github.io/product-images/14534/7.jpg,https://oleks-netizen.github.io/product-images/14534/8.jpg,https://oleks-netizen.github.io/product-images/14534/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14534/01.jpg,https://oleks-netizen.github.io/product-images/14534/02.jpg,https://oleks-netizen.github.io/product-images/14534/14.jpg,https://oleks-netizen.github.io/product-images/14534/11.jpg,https://oleks-netizen.github.io/product-images/14534/12.jpg,https://oleks-netizen.github.io/product-images/14534/13.jpg,https://oleks-netizen.github.io/product-images/14534/03.jpg,https://oleks-netizen.github.io/product-images/14534/04.jpg,https://oleks-netizen.github.io/product-images/14534/05.jpg,https://oleks-netizen.github.io/product-images/14534/06.jpg,https://oleks-netizen.github.io/product-images/14534/07.jpg,https://oleks-netizen.github.io/product-images/14534/08.jpg,https://oleks-netizen.github.io/product-images/14534/09.jpg</t>
         </is>
       </c>
       <c r="C85" t="n">
@@ -1706,7 +1706,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14536/1.jpg,https://oleks-netizen.github.io/product-images/14536/2.jpg,https://oleks-netizen.github.io/product-images/14536/3.jpg,https://oleks-netizen.github.io/product-images/14536/11.jpg,https://oleks-netizen.github.io/product-images/14536/10.jpg,https://oleks-netizen.github.io/product-images/14536/4.jpg,https://oleks-netizen.github.io/product-images/14536/5.jpg,https://oleks-netizen.github.io/product-images/14536/6.jpg,https://oleks-netizen.github.io/product-images/14536/8.jpg,https://oleks-netizen.github.io/product-images/14536/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14536/01.jpg,https://oleks-netizen.github.io/product-images/14536/02.jpg,https://oleks-netizen.github.io/product-images/14536/03.jpg,https://oleks-netizen.github.io/product-images/14536/11.jpg,https://oleks-netizen.github.io/product-images/14536/10.jpg,https://oleks-netizen.github.io/product-images/14536/04.jpg,https://oleks-netizen.github.io/product-images/14536/05.jpg,https://oleks-netizen.github.io/product-images/14536/06.jpg,https://oleks-netizen.github.io/product-images/14536/08.jpg,https://oleks-netizen.github.io/product-images/14536/09.jpg</t>
         </is>
       </c>
       <c r="C86" t="n">
@@ -1721,7 +1721,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14563/1.jpg,https://oleks-netizen.github.io/product-images/14563/2.jpg,https://oleks-netizen.github.io/product-images/14563/13.jpg,https://oleks-netizen.github.io/product-images/14563/10.jpg,https://oleks-netizen.github.io/product-images/14563/12.jpg,https://oleks-netizen.github.io/product-images/14563/3.jpg,https://oleks-netizen.github.io/product-images/14563/4.jpg,https://oleks-netizen.github.io/product-images/14563/5.jpg,https://oleks-netizen.github.io/product-images/14563/6.jpg,https://oleks-netizen.github.io/product-images/14563/7.jpg,https://oleks-netizen.github.io/product-images/14563/8.jpg,https://oleks-netizen.github.io/product-images/14563/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14563/01.jpg,https://oleks-netizen.github.io/product-images/14563/02.jpg,https://oleks-netizen.github.io/product-images/14563/13.jpg,https://oleks-netizen.github.io/product-images/14563/10.jpg,https://oleks-netizen.github.io/product-images/14563/12.jpg,https://oleks-netizen.github.io/product-images/14563/03.jpg,https://oleks-netizen.github.io/product-images/14563/04.jpg,https://oleks-netizen.github.io/product-images/14563/05.jpg,https://oleks-netizen.github.io/product-images/14563/06.jpg,https://oleks-netizen.github.io/product-images/14563/07.jpg,https://oleks-netizen.github.io/product-images/14563/08.jpg,https://oleks-netizen.github.io/product-images/14563/09.jpg</t>
         </is>
       </c>
       <c r="C87" t="n">
@@ -1736,7 +1736,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14567/1.jpg,https://oleks-netizen.github.io/product-images/14567/2.jpg,https://oleks-netizen.github.io/product-images/14567/11.jpg,https://oleks-netizen.github.io/product-images/14567/3.jpg,https://oleks-netizen.github.io/product-images/14567/4.jpg,https://oleks-netizen.github.io/product-images/14567/5.jpg,https://oleks-netizen.github.io/product-images/14567/6.jpg,https://oleks-netizen.github.io/product-images/14567/7.jpg,https://oleks-netizen.github.io/product-images/14567/8.jpg,https://oleks-netizen.github.io/product-images/14567/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14567/01.jpg,https://oleks-netizen.github.io/product-images/14567/02.jpg,https://oleks-netizen.github.io/product-images/14567/11.jpg,https://oleks-netizen.github.io/product-images/14567/03.jpg,https://oleks-netizen.github.io/product-images/14567/04.jpg,https://oleks-netizen.github.io/product-images/14567/05.jpg,https://oleks-netizen.github.io/product-images/14567/06.jpg,https://oleks-netizen.github.io/product-images/14567/07.jpg,https://oleks-netizen.github.io/product-images/14567/08.jpg,https://oleks-netizen.github.io/product-images/14567/09.jpg</t>
         </is>
       </c>
       <c r="C88" t="n">
@@ -1751,7 +1751,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14580/1.jpg,https://oleks-netizen.github.io/product-images/14580/2.jpg,https://oleks-netizen.github.io/product-images/14580/12.jpg,https://oleks-netizen.github.io/product-images/14580/10.jpg,https://oleks-netizen.github.io/product-images/14580/11.jpg,https://oleks-netizen.github.io/product-images/14580/3.jpg,https://oleks-netizen.github.io/product-images/14580/4.jpg,https://oleks-netizen.github.io/product-images/14580/6.jpg,https://oleks-netizen.github.io/product-images/14580/7.jpg,https://oleks-netizen.github.io/product-images/14580/8.jpg,https://oleks-netizen.github.io/product-images/14580/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14580/01.jpg,https://oleks-netizen.github.io/product-images/14580/02.jpg,https://oleks-netizen.github.io/product-images/14580/12.jpg,https://oleks-netizen.github.io/product-images/14580/10.jpg,https://oleks-netizen.github.io/product-images/14580/11.jpg,https://oleks-netizen.github.io/product-images/14580/03.jpg,https://oleks-netizen.github.io/product-images/14580/04.jpg,https://oleks-netizen.github.io/product-images/14580/06.jpg,https://oleks-netizen.github.io/product-images/14580/07.jpg,https://oleks-netizen.github.io/product-images/14580/08.jpg,https://oleks-netizen.github.io/product-images/14580/09.jpg</t>
         </is>
       </c>
       <c r="C89" t="n">
@@ -1766,7 +1766,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14581/1.jpg,https://oleks-netizen.github.io/product-images/14581/2.jpg,https://oleks-netizen.github.io/product-images/14581/13.jpg,https://oleks-netizen.github.io/product-images/14581/10.jpg,https://oleks-netizen.github.io/product-images/14581/11.jpg,https://oleks-netizen.github.io/product-images/14581/12.jpg,https://oleks-netizen.github.io/product-images/14581/3.jpg,https://oleks-netizen.github.io/product-images/14581/4.jpg,https://oleks-netizen.github.io/product-images/14581/5.jpg,https://oleks-netizen.github.io/product-images/14581/6.jpg,https://oleks-netizen.github.io/product-images/14581/8.jpg,https://oleks-netizen.github.io/product-images/14581/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14581/01.jpg,https://oleks-netizen.github.io/product-images/14581/02.jpg,https://oleks-netizen.github.io/product-images/14581/13.jpg,https://oleks-netizen.github.io/product-images/14581/10.jpg,https://oleks-netizen.github.io/product-images/14581/11.jpg,https://oleks-netizen.github.io/product-images/14581/12.jpg,https://oleks-netizen.github.io/product-images/14581/03.jpg,https://oleks-netizen.github.io/product-images/14581/04.jpg,https://oleks-netizen.github.io/product-images/14581/05.jpg,https://oleks-netizen.github.io/product-images/14581/06.jpg,https://oleks-netizen.github.io/product-images/14581/08.jpg,https://oleks-netizen.github.io/product-images/14581/09.jpg</t>
         </is>
       </c>
       <c r="C90" t="n">
@@ -1781,7 +1781,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14585/1.jpg,https://oleks-netizen.github.io/product-images/14585/2.jpg,https://oleks-netizen.github.io/product-images/14585/10.jpg,https://oleks-netizen.github.io/product-images/14585/3.jpg,https://oleks-netizen.github.io/product-images/14585/4.jpg,https://oleks-netizen.github.io/product-images/14585/5.jpg,https://oleks-netizen.github.io/product-images/14585/6.jpg,https://oleks-netizen.github.io/product-images/14585/7.jpg,https://oleks-netizen.github.io/product-images/14585/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14585/01.jpg,https://oleks-netizen.github.io/product-images/14585/02.jpg,https://oleks-netizen.github.io/product-images/14585/10.jpg,https://oleks-netizen.github.io/product-images/14585/03.jpg,https://oleks-netizen.github.io/product-images/14585/04.jpg,https://oleks-netizen.github.io/product-images/14585/05.jpg,https://oleks-netizen.github.io/product-images/14585/06.jpg,https://oleks-netizen.github.io/product-images/14585/07.jpg,https://oleks-netizen.github.io/product-images/14585/09.jpg</t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -1796,7 +1796,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14588/1.jpg,https://oleks-netizen.github.io/product-images/14588/2.jpg,https://oleks-netizen.github.io/product-images/14588/12.jpg,https://oleks-netizen.github.io/product-images/14588/10.jpg,https://oleks-netizen.github.io/product-images/14588/11.jpg,https://oleks-netizen.github.io/product-images/14588/3.jpg,https://oleks-netizen.github.io/product-images/14588/4.jpg,https://oleks-netizen.github.io/product-images/14588/5.jpg,https://oleks-netizen.github.io/product-images/14588/6.jpg,https://oleks-netizen.github.io/product-images/14588/8.jpg,https://oleks-netizen.github.io/product-images/14588/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14588/01.jpg,https://oleks-netizen.github.io/product-images/14588/02.jpg,https://oleks-netizen.github.io/product-images/14588/12.jpg,https://oleks-netizen.github.io/product-images/14588/10.jpg,https://oleks-netizen.github.io/product-images/14588/11.jpg,https://oleks-netizen.github.io/product-images/14588/03.jpg,https://oleks-netizen.github.io/product-images/14588/04.jpg,https://oleks-netizen.github.io/product-images/14588/05.jpg,https://oleks-netizen.github.io/product-images/14588/06.jpg,https://oleks-netizen.github.io/product-images/14588/08.jpg,https://oleks-netizen.github.io/product-images/14588/09.jpg</t>
         </is>
       </c>
       <c r="C92" t="n">
@@ -1811,7 +1811,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14590/1.jpg,https://oleks-netizen.github.io/product-images/14590/2.jpg,https://oleks-netizen.github.io/product-images/14590/11.jpg,https://oleks-netizen.github.io/product-images/14590/10.jpg,https://oleks-netizen.github.io/product-images/14590/3.jpg,https://oleks-netizen.github.io/product-images/14590/4.jpg,https://oleks-netizen.github.io/product-images/14590/5.jpg,https://oleks-netizen.github.io/product-images/14590/7.jpg,https://oleks-netizen.github.io/product-images/14590/8.jpg,https://oleks-netizen.github.io/product-images/14590/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14590/01.jpg,https://oleks-netizen.github.io/product-images/14590/02.jpg,https://oleks-netizen.github.io/product-images/14590/11.jpg,https://oleks-netizen.github.io/product-images/14590/10.jpg,https://oleks-netizen.github.io/product-images/14590/03.jpg,https://oleks-netizen.github.io/product-images/14590/04.jpg,https://oleks-netizen.github.io/product-images/14590/05.jpg,https://oleks-netizen.github.io/product-images/14590/07.jpg,https://oleks-netizen.github.io/product-images/14590/08.jpg,https://oleks-netizen.github.io/product-images/14590/09.jpg</t>
         </is>
       </c>
       <c r="C93" t="n">
@@ -1826,7 +1826,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14591/1.jpg,https://oleks-netizen.github.io/product-images/14591/2.jpg,https://oleks-netizen.github.io/product-images/14591/11.jpg,https://oleks-netizen.github.io/product-images/14591/10.jpg,https://oleks-netizen.github.io/product-images/14591/3.jpg,https://oleks-netizen.github.io/product-images/14591/4.jpg,https://oleks-netizen.github.io/product-images/14591/5.jpg,https://oleks-netizen.github.io/product-images/14591/6.jpg,https://oleks-netizen.github.io/product-images/14591/7.jpg,https://oleks-netizen.github.io/product-images/14591/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14591/01.jpg,https://oleks-netizen.github.io/product-images/14591/02.jpg,https://oleks-netizen.github.io/product-images/14591/11.jpg,https://oleks-netizen.github.io/product-images/14591/10.jpg,https://oleks-netizen.github.io/product-images/14591/03.jpg,https://oleks-netizen.github.io/product-images/14591/04.jpg,https://oleks-netizen.github.io/product-images/14591/05.jpg,https://oleks-netizen.github.io/product-images/14591/06.jpg,https://oleks-netizen.github.io/product-images/14591/07.jpg,https://oleks-netizen.github.io/product-images/14591/09.jpg</t>
         </is>
       </c>
       <c r="C94" t="n">
@@ -1841,7 +1841,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14595/1.jpg,https://oleks-netizen.github.io/product-images/14595/2.jpg,https://oleks-netizen.github.io/product-images/14595/12.jpg,https://oleks-netizen.github.io/product-images/14595/13.jpg,https://oleks-netizen.github.io/product-images/14595/11.jpg,https://oleks-netizen.github.io/product-images/14595/3.jpg,https://oleks-netizen.github.io/product-images/14595/4.jpg,https://oleks-netizen.github.io/product-images/14595/5.jpg,https://oleks-netizen.github.io/product-images/14595/6.jpg,https://oleks-netizen.github.io/product-images/14595/7.jpg,https://oleks-netizen.github.io/product-images/14595/8.jpg,https://oleks-netizen.github.io/product-images/14595/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14595/01.jpg,https://oleks-netizen.github.io/product-images/14595/02.jpg,https://oleks-netizen.github.io/product-images/14595/12.jpg,https://oleks-netizen.github.io/product-images/14595/13.jpg,https://oleks-netizen.github.io/product-images/14595/11.jpg,https://oleks-netizen.github.io/product-images/14595/03.jpg,https://oleks-netizen.github.io/product-images/14595/04.jpg,https://oleks-netizen.github.io/product-images/14595/05.jpg,https://oleks-netizen.github.io/product-images/14595/06.jpg,https://oleks-netizen.github.io/product-images/14595/07.jpg,https://oleks-netizen.github.io/product-images/14595/08.jpg,https://oleks-netizen.github.io/product-images/14595/09.jpg</t>
         </is>
       </c>
       <c r="C95" t="n">
@@ -1856,7 +1856,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14596/1.jpg,https://oleks-netizen.github.io/product-images/14596/2.jpg,https://oleks-netizen.github.io/product-images/14596/5.jpg,https://oleks-netizen.github.io/product-images/14596/7.jpg,https://oleks-netizen.github.io/product-images/14596/3.jpg,https://oleks-netizen.github.io/product-images/14596/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14596/01.jpg,https://oleks-netizen.github.io/product-images/14596/02.jpg,https://oleks-netizen.github.io/product-images/14596/05.jpg,https://oleks-netizen.github.io/product-images/14596/07.jpg,https://oleks-netizen.github.io/product-images/14596/03.jpg,https://oleks-netizen.github.io/product-images/14596/04.jpg</t>
         </is>
       </c>
       <c r="C96" t="n">
@@ -1871,7 +1871,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14597/1.jpg,https://oleks-netizen.github.io/product-images/14597/2.jpg,https://oleks-netizen.github.io/product-images/14597/6.jpg,https://oleks-netizen.github.io/product-images/14597/12.jpg,https://oleks-netizen.github.io/product-images/14597/11.jpg,https://oleks-netizen.github.io/product-images/14597/3.jpg,https://oleks-netizen.github.io/product-images/14597/4.jpg,https://oleks-netizen.github.io/product-images/14597/5.jpg,https://oleks-netizen.github.io/product-images/14597/7.jpg,https://oleks-netizen.github.io/product-images/14597/8.jpg,https://oleks-netizen.github.io/product-images/14597/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14597/01.jpg,https://oleks-netizen.github.io/product-images/14597/02.jpg,https://oleks-netizen.github.io/product-images/14597/06.jpg,https://oleks-netizen.github.io/product-images/14597/12.jpg,https://oleks-netizen.github.io/product-images/14597/11.jpg,https://oleks-netizen.github.io/product-images/14597/03.jpg,https://oleks-netizen.github.io/product-images/14597/04.jpg,https://oleks-netizen.github.io/product-images/14597/05.jpg,https://oleks-netizen.github.io/product-images/14597/07.jpg,https://oleks-netizen.github.io/product-images/14597/08.jpg,https://oleks-netizen.github.io/product-images/14597/09.jpg</t>
         </is>
       </c>
       <c r="C97" t="n">
@@ -1886,7 +1886,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14598/1.jpg,https://oleks-netizen.github.io/product-images/14598/2.jpg,https://oleks-netizen.github.io/product-images/14598/3.jpg,https://oleks-netizen.github.io/product-images/14598/14.jpg,https://oleks-netizen.github.io/product-images/14598/11.jpg,https://oleks-netizen.github.io/product-images/14598/12.jpg,https://oleks-netizen.github.io/product-images/14598/13.jpg,https://oleks-netizen.github.io/product-images/14598/4.jpg,https://oleks-netizen.github.io/product-images/14598/5.jpg,https://oleks-netizen.github.io/product-images/14598/6.jpg,https://oleks-netizen.github.io/product-images/14598/7.jpg,https://oleks-netizen.github.io/product-images/14598/8.jpg,https://oleks-netizen.github.io/product-images/14598/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14598/01.jpg,https://oleks-netizen.github.io/product-images/14598/02.jpg,https://oleks-netizen.github.io/product-images/14598/03.jpg,https://oleks-netizen.github.io/product-images/14598/14.jpg,https://oleks-netizen.github.io/product-images/14598/11.jpg,https://oleks-netizen.github.io/product-images/14598/12.jpg,https://oleks-netizen.github.io/product-images/14598/13.jpg,https://oleks-netizen.github.io/product-images/14598/04.jpg,https://oleks-netizen.github.io/product-images/14598/05.jpg,https://oleks-netizen.github.io/product-images/14598/06.jpg,https://oleks-netizen.github.io/product-images/14598/07.jpg,https://oleks-netizen.github.io/product-images/14598/08.jpg,https://oleks-netizen.github.io/product-images/14598/09.jpg</t>
         </is>
       </c>
       <c r="C98" t="n">
@@ -1901,7 +1901,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14602/1.jpg,https://oleks-netizen.github.io/product-images/14602/2.jpg,https://oleks-netizen.github.io/product-images/14602/10.jpg,https://oleks-netizen.github.io/product-images/14602/11.jpg,https://oleks-netizen.github.io/product-images/14602/12.jpg,https://oleks-netizen.github.io/product-images/14602/13.jpg,https://oleks-netizen.github.io/product-images/14602/14.jpg,https://oleks-netizen.github.io/product-images/14602/15.jpg,https://oleks-netizen.github.io/product-images/14602/16.jpg,https://oleks-netizen.github.io/product-images/14602/17.jpg,https://oleks-netizen.github.io/product-images/14602/18.jpg,https://oleks-netizen.github.io/product-images/14602/3.jpg,https://oleks-netizen.github.io/product-images/14602/4.jpg,https://oleks-netizen.github.io/product-images/14602/5.jpg,https://oleks-netizen.github.io/product-images/14602/6.jpg,https://oleks-netizen.github.io/product-images/14602/7.jpg,https://oleks-netizen.github.io/product-images/14602/8.jpg,https://oleks-netizen.github.io/product-images/14602/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14602/01.jpg,https://oleks-netizen.github.io/product-images/14602/02.jpg,https://oleks-netizen.github.io/product-images/14602/10.jpg,https://oleks-netizen.github.io/product-images/14602/11.jpg,https://oleks-netizen.github.io/product-images/14602/12.jpg,https://oleks-netizen.github.io/product-images/14602/13.jpg,https://oleks-netizen.github.io/product-images/14602/14.jpg,https://oleks-netizen.github.io/product-images/14602/15.jpg,https://oleks-netizen.github.io/product-images/14602/16.jpg,https://oleks-netizen.github.io/product-images/14602/17.jpg,https://oleks-netizen.github.io/product-images/14602/18.jpg,https://oleks-netizen.github.io/product-images/14602/03.jpg,https://oleks-netizen.github.io/product-images/14602/04.jpg,https://oleks-netizen.github.io/product-images/14602/05.jpg,https://oleks-netizen.github.io/product-images/14602/06.jpg,https://oleks-netizen.github.io/product-images/14602/07.jpg,https://oleks-netizen.github.io/product-images/14602/08.jpg,https://oleks-netizen.github.io/product-images/14602/09.jpg</t>
         </is>
       </c>
       <c r="C99" t="n">
@@ -1916,7 +1916,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14603/1.jpg,https://oleks-netizen.github.io/product-images/14603/2.jpg,https://oleks-netizen.github.io/product-images/14603/10.jpg,https://oleks-netizen.github.io/product-images/14603/3.jpg,https://oleks-netizen.github.io/product-images/14603/4.jpg,https://oleks-netizen.github.io/product-images/14603/5.jpg,https://oleks-netizen.github.io/product-images/14603/6.jpg,https://oleks-netizen.github.io/product-images/14603/8.jpg,https://oleks-netizen.github.io/product-images/14603/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14603/01.jpg,https://oleks-netizen.github.io/product-images/14603/02.jpg,https://oleks-netizen.github.io/product-images/14603/10.jpg,https://oleks-netizen.github.io/product-images/14603/03.jpg,https://oleks-netizen.github.io/product-images/14603/04.jpg,https://oleks-netizen.github.io/product-images/14603/05.jpg,https://oleks-netizen.github.io/product-images/14603/06.jpg,https://oleks-netizen.github.io/product-images/14603/08.jpg,https://oleks-netizen.github.io/product-images/14603/09.jpg</t>
         </is>
       </c>
       <c r="C100" t="n">
@@ -1931,7 +1931,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14604/1.jpg,https://oleks-netizen.github.io/product-images/14604/2.jpg,https://oleks-netizen.github.io/product-images/14604/12.jpg,https://oleks-netizen.github.io/product-images/14604/10.jpg,https://oleks-netizen.github.io/product-images/14604/11.jpg,https://oleks-netizen.github.io/product-images/14604/3.jpg,https://oleks-netizen.github.io/product-images/14604/4.jpg,https://oleks-netizen.github.io/product-images/14604/5.jpg,https://oleks-netizen.github.io/product-images/14604/6.jpg,https://oleks-netizen.github.io/product-images/14604/7.jpg,https://oleks-netizen.github.io/product-images/14604/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14604/01.jpg,https://oleks-netizen.github.io/product-images/14604/02.jpg,https://oleks-netizen.github.io/product-images/14604/12.jpg,https://oleks-netizen.github.io/product-images/14604/10.jpg,https://oleks-netizen.github.io/product-images/14604/11.jpg,https://oleks-netizen.github.io/product-images/14604/03.jpg,https://oleks-netizen.github.io/product-images/14604/04.jpg,https://oleks-netizen.github.io/product-images/14604/05.jpg,https://oleks-netizen.github.io/product-images/14604/06.jpg,https://oleks-netizen.github.io/product-images/14604/07.jpg,https://oleks-netizen.github.io/product-images/14604/09.jpg</t>
         </is>
       </c>
       <c r="C101" t="n">
@@ -1946,7 +1946,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14607/10.jpg,https://oleks-netizen.github.io/product-images/14607/11.jpg,https://oleks-netizen.github.io/product-images/14607/12.jpg,https://oleks-netizen.github.io/product-images/14607/1.jpg,https://oleks-netizen.github.io/product-images/14607/2.jpg,https://oleks-netizen.github.io/product-images/14607/3.jpg,https://oleks-netizen.github.io/product-images/14607/4.jpg,https://oleks-netizen.github.io/product-images/14607/5.jpg,https://oleks-netizen.github.io/product-images/14607/6.jpg,https://oleks-netizen.github.io/product-images/14607/7.jpg,https://oleks-netizen.github.io/product-images/14607/8.jpg,https://oleks-netizen.github.io/product-images/14607/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14607/10.jpg,https://oleks-netizen.github.io/product-images/14607/11.jpg,https://oleks-netizen.github.io/product-images/14607/12.jpg,https://oleks-netizen.github.io/product-images/14607/01.jpg,https://oleks-netizen.github.io/product-images/14607/02.jpg,https://oleks-netizen.github.io/product-images/14607/03.jpg,https://oleks-netizen.github.io/product-images/14607/04.jpg,https://oleks-netizen.github.io/product-images/14607/05.jpg,https://oleks-netizen.github.io/product-images/14607/06.jpg,https://oleks-netizen.github.io/product-images/14607/07.jpg,https://oleks-netizen.github.io/product-images/14607/08.jpg,https://oleks-netizen.github.io/product-images/14607/09.jpg</t>
         </is>
       </c>
       <c r="C102" t="n">
@@ -1961,7 +1961,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14609/1.jpg,https://oleks-netizen.github.io/product-images/14609/2.jpg,https://oleks-netizen.github.io/product-images/14609/5.jpg,https://oleks-netizen.github.io/product-images/14609/9.jpg,https://oleks-netizen.github.io/product-images/14609/3.jpg,https://oleks-netizen.github.io/product-images/14609/4.jpg,https://oleks-netizen.github.io/product-images/14609/7.jpg,https://oleks-netizen.github.io/product-images/14609/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14609/01.jpg,https://oleks-netizen.github.io/product-images/14609/02.jpg,https://oleks-netizen.github.io/product-images/14609/05.jpg,https://oleks-netizen.github.io/product-images/14609/09.jpg,https://oleks-netizen.github.io/product-images/14609/03.jpg,https://oleks-netizen.github.io/product-images/14609/04.jpg,https://oleks-netizen.github.io/product-images/14609/07.jpg,https://oleks-netizen.github.io/product-images/14609/08.jpg</t>
         </is>
       </c>
       <c r="C103" t="n">
@@ -1976,7 +1976,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14615/1.jpg,https://oleks-netizen.github.io/product-images/14615/2.jpg,https://oleks-netizen.github.io/product-images/14615/5.jpg,https://oleks-netizen.github.io/product-images/14615/8.jpg,https://oleks-netizen.github.io/product-images/14615/3.jpg,https://oleks-netizen.github.io/product-images/14615/4.jpg,https://oleks-netizen.github.io/product-images/14615/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14615/01.jpg,https://oleks-netizen.github.io/product-images/14615/02.jpg,https://oleks-netizen.github.io/product-images/14615/05.jpg,https://oleks-netizen.github.io/product-images/14615/08.jpg,https://oleks-netizen.github.io/product-images/14615/03.jpg,https://oleks-netizen.github.io/product-images/14615/04.jpg,https://oleks-netizen.github.io/product-images/14615/06.jpg</t>
         </is>
       </c>
       <c r="C104" t="n">
@@ -1991,7 +1991,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14627/1.jpg,https://oleks-netizen.github.io/product-images/14627/2.jpg,https://oleks-netizen.github.io/product-images/14627/6.jpg,https://oleks-netizen.github.io/product-images/14627/9.jpg,https://oleks-netizen.github.io/product-images/14627/3.jpg,https://oleks-netizen.github.io/product-images/14627/4.jpg,https://oleks-netizen.github.io/product-images/14627/5.jpg,https://oleks-netizen.github.io/product-images/14627/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14627/01.jpg,https://oleks-netizen.github.io/product-images/14627/02.jpg,https://oleks-netizen.github.io/product-images/14627/06.jpg,https://oleks-netizen.github.io/product-images/14627/09.jpg,https://oleks-netizen.github.io/product-images/14627/03.jpg,https://oleks-netizen.github.io/product-images/14627/04.jpg,https://oleks-netizen.github.io/product-images/14627/05.jpg,https://oleks-netizen.github.io/product-images/14627/08.jpg</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -2006,7 +2006,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14645/1.jpg,https://oleks-netizen.github.io/product-images/14645/2.jpg,https://oleks-netizen.github.io/product-images/14645/7.jpg,https://oleks-netizen.github.io/product-images/14645/3.jpg,https://oleks-netizen.github.io/product-images/14645/4.jpg,https://oleks-netizen.github.io/product-images/14645/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14645/01.jpg,https://oleks-netizen.github.io/product-images/14645/02.jpg,https://oleks-netizen.github.io/product-images/14645/07.jpg,https://oleks-netizen.github.io/product-images/14645/03.jpg,https://oleks-netizen.github.io/product-images/14645/04.jpg,https://oleks-netizen.github.io/product-images/14645/05.jpg</t>
         </is>
       </c>
       <c r="C106" t="n">
@@ -2021,7 +2021,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14648/1.jpg,https://oleks-netizen.github.io/product-images/14648/2.jpg,https://oleks-netizen.github.io/product-images/14648/4.jpg,https://oleks-netizen.github.io/product-images/14648/12.jpg,https://oleks-netizen.github.io/product-images/14648/11.jpg,https://oleks-netizen.github.io/product-images/14648/3.jpg,https://oleks-netizen.github.io/product-images/14648/5.jpg,https://oleks-netizen.github.io/product-images/14648/6.jpg,https://oleks-netizen.github.io/product-images/14648/7.jpg,https://oleks-netizen.github.io/product-images/14648/8.jpg,https://oleks-netizen.github.io/product-images/14648/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14648/01.jpg,https://oleks-netizen.github.io/product-images/14648/02.jpg,https://oleks-netizen.github.io/product-images/14648/04.jpg,https://oleks-netizen.github.io/product-images/14648/12.jpg,https://oleks-netizen.github.io/product-images/14648/11.jpg,https://oleks-netizen.github.io/product-images/14648/03.jpg,https://oleks-netizen.github.io/product-images/14648/05.jpg,https://oleks-netizen.github.io/product-images/14648/06.jpg,https://oleks-netizen.github.io/product-images/14648/07.jpg,https://oleks-netizen.github.io/product-images/14648/08.jpg,https://oleks-netizen.github.io/product-images/14648/09.jpg</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -2036,7 +2036,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14680/1.jpg,https://oleks-netizen.github.io/product-images/14680/2.jpg,https://oleks-netizen.github.io/product-images/14680/23.jpg,https://oleks-netizen.github.io/product-images/14680/10.jpg,https://oleks-netizen.github.io/product-images/14680/11.jpg,https://oleks-netizen.github.io/product-images/14680/12.jpg,https://oleks-netizen.github.io/product-images/14680/13.jpg,https://oleks-netizen.github.io/product-images/14680/14.jpg,https://oleks-netizen.github.io/product-images/14680/15.jpg,https://oleks-netizen.github.io/product-images/14680/16.jpg,https://oleks-netizen.github.io/product-images/14680/17.jpg,https://oleks-netizen.github.io/product-images/14680/18.jpg,https://oleks-netizen.github.io/product-images/14680/19.jpg,https://oleks-netizen.github.io/product-images/14680/20.jpg,https://oleks-netizen.github.io/product-images/14680/21.jpg,https://oleks-netizen.github.io/product-images/14680/22.jpg,https://oleks-netizen.github.io/product-images/14680/3.jpg,https://oleks-netizen.github.io/product-images/14680/4.jpg,https://oleks-netizen.github.io/product-images/14680/6.jpg,https://oleks-netizen.github.io/product-images/14680/7.jpg,https://oleks-netizen.github.io/product-images/14680/8.jpg,https://oleks-netizen.github.io/product-images/14680/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14680/01.jpg,https://oleks-netizen.github.io/product-images/14680/02.jpg,https://oleks-netizen.github.io/product-images/14680/23.jpg,https://oleks-netizen.github.io/product-images/14680/10.jpg,https://oleks-netizen.github.io/product-images/14680/11.jpg,https://oleks-netizen.github.io/product-images/14680/12.jpg,https://oleks-netizen.github.io/product-images/14680/13.jpg,https://oleks-netizen.github.io/product-images/14680/14.jpg,https://oleks-netizen.github.io/product-images/14680/15.jpg,https://oleks-netizen.github.io/product-images/14680/16.jpg,https://oleks-netizen.github.io/product-images/14680/17.jpg,https://oleks-netizen.github.io/product-images/14680/18.jpg,https://oleks-netizen.github.io/product-images/14680/19.jpg,https://oleks-netizen.github.io/product-images/14680/20.jpg,https://oleks-netizen.github.io/product-images/14680/21.jpg,https://oleks-netizen.github.io/product-images/14680/22.jpg,https://oleks-netizen.github.io/product-images/14680/03.jpg,https://oleks-netizen.github.io/product-images/14680/04.jpg,https://oleks-netizen.github.io/product-images/14680/06.jpg,https://oleks-netizen.github.io/product-images/14680/07.jpg,https://oleks-netizen.github.io/product-images/14680/08.jpg,https://oleks-netizen.github.io/product-images/14680/09.jpg</t>
         </is>
       </c>
       <c r="C108" t="n">
@@ -2051,7 +2051,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14681/1.jpg,https://oleks-netizen.github.io/product-images/14681/2.jpg,https://oleks-netizen.github.io/product-images/14681/15.jpg,https://oleks-netizen.github.io/product-images/14681/10.jpg,https://oleks-netizen.github.io/product-images/14681/11.jpg,https://oleks-netizen.github.io/product-images/14681/12.jpg,https://oleks-netizen.github.io/product-images/14681/13.jpg,https://oleks-netizen.github.io/product-images/14681/3.jpg,https://oleks-netizen.github.io/product-images/14681/4.jpg,https://oleks-netizen.github.io/product-images/14681/5.jpg,https://oleks-netizen.github.io/product-images/14681/6.jpg,https://oleks-netizen.github.io/product-images/14681/7.jpg,https://oleks-netizen.github.io/product-images/14681/8.jpg,https://oleks-netizen.github.io/product-images/14681/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14681/01.jpg,https://oleks-netizen.github.io/product-images/14681/02.jpg,https://oleks-netizen.github.io/product-images/14681/15.jpg,https://oleks-netizen.github.io/product-images/14681/10.jpg,https://oleks-netizen.github.io/product-images/14681/11.jpg,https://oleks-netizen.github.io/product-images/14681/12.jpg,https://oleks-netizen.github.io/product-images/14681/13.jpg,https://oleks-netizen.github.io/product-images/14681/03.jpg,https://oleks-netizen.github.io/product-images/14681/04.jpg,https://oleks-netizen.github.io/product-images/14681/05.jpg,https://oleks-netizen.github.io/product-images/14681/06.jpg,https://oleks-netizen.github.io/product-images/14681/07.jpg,https://oleks-netizen.github.io/product-images/14681/08.jpg,https://oleks-netizen.github.io/product-images/14681/09.jpg</t>
         </is>
       </c>
       <c r="C109" t="n">
@@ -2066,7 +2066,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14682/1.jpg,https://oleks-netizen.github.io/product-images/14682/2.jpg,https://oleks-netizen.github.io/product-images/14682/24.jpg,https://oleks-netizen.github.io/product-images/14682/10.jpg,https://oleks-netizen.github.io/product-images/14682/11.jpg,https://oleks-netizen.github.io/product-images/14682/12.jpg,https://oleks-netizen.github.io/product-images/14682/13.jpg,https://oleks-netizen.github.io/product-images/14682/14.jpg,https://oleks-netizen.github.io/product-images/14682/15.jpg,https://oleks-netizen.github.io/product-images/14682/17.jpg,https://oleks-netizen.github.io/product-images/14682/18.jpg,https://oleks-netizen.github.io/product-images/14682/19.jpg,https://oleks-netizen.github.io/product-images/14682/20.jpg,https://oleks-netizen.github.io/product-images/14682/21.jpg,https://oleks-netizen.github.io/product-images/14682/22.jpg,https://oleks-netizen.github.io/product-images/14682/23.jpg,https://oleks-netizen.github.io/product-images/14682/3.jpg,https://oleks-netizen.github.io/product-images/14682/4.jpg,https://oleks-netizen.github.io/product-images/14682/5.jpg,https://oleks-netizen.github.io/product-images/14682/6.jpg,https://oleks-netizen.github.io/product-images/14682/7.jpg,https://oleks-netizen.github.io/product-images/14682/8.jpg,https://oleks-netizen.github.io/product-images/14682/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14682/01.jpg,https://oleks-netizen.github.io/product-images/14682/02.jpg,https://oleks-netizen.github.io/product-images/14682/24.jpg,https://oleks-netizen.github.io/product-images/14682/10.jpg,https://oleks-netizen.github.io/product-images/14682/11.jpg,https://oleks-netizen.github.io/product-images/14682/12.jpg,https://oleks-netizen.github.io/product-images/14682/13.jpg,https://oleks-netizen.github.io/product-images/14682/14.jpg,https://oleks-netizen.github.io/product-images/14682/15.jpg,https://oleks-netizen.github.io/product-images/14682/17.jpg,https://oleks-netizen.github.io/product-images/14682/18.jpg,https://oleks-netizen.github.io/product-images/14682/19.jpg,https://oleks-netizen.github.io/product-images/14682/20.jpg,https://oleks-netizen.github.io/product-images/14682/21.jpg,https://oleks-netizen.github.io/product-images/14682/22.jpg,https://oleks-netizen.github.io/product-images/14682/23.jpg,https://oleks-netizen.github.io/product-images/14682/03.jpg,https://oleks-netizen.github.io/product-images/14682/04.jpg,https://oleks-netizen.github.io/product-images/14682/05.jpg,https://oleks-netizen.github.io/product-images/14682/06.jpg,https://oleks-netizen.github.io/product-images/14682/07.jpg,https://oleks-netizen.github.io/product-images/14682/08.jpg,https://oleks-netizen.github.io/product-images/14682/09.jpg</t>
         </is>
       </c>
       <c r="C110" t="n">
@@ -2081,7 +2081,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14683/1.jpg,https://oleks-netizen.github.io/product-images/14683/2.jpg,https://oleks-netizen.github.io/product-images/14683/8.jpg,https://oleks-netizen.github.io/product-images/14683/3.jpg,https://oleks-netizen.github.io/product-images/14683/4.jpg,https://oleks-netizen.github.io/product-images/14683/5.jpg,https://oleks-netizen.github.io/product-images/14683/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14683/01.jpg,https://oleks-netizen.github.io/product-images/14683/02.jpg,https://oleks-netizen.github.io/product-images/14683/08.jpg,https://oleks-netizen.github.io/product-images/14683/03.jpg,https://oleks-netizen.github.io/product-images/14683/04.jpg,https://oleks-netizen.github.io/product-images/14683/05.jpg,https://oleks-netizen.github.io/product-images/14683/07.jpg</t>
         </is>
       </c>
       <c r="C111" t="n">
@@ -2096,7 +2096,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14686/1.jpg,https://oleks-netizen.github.io/product-images/14686/2.jpg,https://oleks-netizen.github.io/product-images/14686/14.jpg,https://oleks-netizen.github.io/product-images/14686/10.jpg,https://oleks-netizen.github.io/product-images/14686/11.jpg,https://oleks-netizen.github.io/product-images/14686/13.jpg,https://oleks-netizen.github.io/product-images/14686/3.jpg,https://oleks-netizen.github.io/product-images/14686/4.jpg,https://oleks-netizen.github.io/product-images/14686/5.jpg,https://oleks-netizen.github.io/product-images/14686/6.jpg,https://oleks-netizen.github.io/product-images/14686/7.jpg,https://oleks-netizen.github.io/product-images/14686/8.jpg,https://oleks-netizen.github.io/product-images/14686/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14686/01.jpg,https://oleks-netizen.github.io/product-images/14686/02.jpg,https://oleks-netizen.github.io/product-images/14686/14.jpg,https://oleks-netizen.github.io/product-images/14686/10.jpg,https://oleks-netizen.github.io/product-images/14686/11.jpg,https://oleks-netizen.github.io/product-images/14686/13.jpg,https://oleks-netizen.github.io/product-images/14686/03.jpg,https://oleks-netizen.github.io/product-images/14686/04.jpg,https://oleks-netizen.github.io/product-images/14686/05.jpg,https://oleks-netizen.github.io/product-images/14686/06.jpg,https://oleks-netizen.github.io/product-images/14686/07.jpg,https://oleks-netizen.github.io/product-images/14686/08.jpg,https://oleks-netizen.github.io/product-images/14686/09.jpg</t>
         </is>
       </c>
       <c r="C112" t="n">
@@ -2111,7 +2111,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14687/1.jpg,https://oleks-netizen.github.io/product-images/14687/2.jpg,https://oleks-netizen.github.io/product-images/14687/3.jpg,https://oleks-netizen.github.io/product-images/14687/17.jpg,https://oleks-netizen.github.io/product-images/14687/10.jpg,https://oleks-netizen.github.io/product-images/14687/11.jpg,https://oleks-netizen.github.io/product-images/14687/12.jpg,https://oleks-netizen.github.io/product-images/14687/13.jpg,https://oleks-netizen.github.io/product-images/14687/15.jpg,https://oleks-netizen.github.io/product-images/14687/16.jpg,https://oleks-netizen.github.io/product-images/14687/4.jpg,https://oleks-netizen.github.io/product-images/14687/5.jpg,https://oleks-netizen.github.io/product-images/14687/6.jpg,https://oleks-netizen.github.io/product-images/14687/7.jpg,https://oleks-netizen.github.io/product-images/14687/8.jpg,https://oleks-netizen.github.io/product-images/14687/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14687/01.jpg,https://oleks-netizen.github.io/product-images/14687/02.jpg,https://oleks-netizen.github.io/product-images/14687/03.jpg,https://oleks-netizen.github.io/product-images/14687/17.jpg,https://oleks-netizen.github.io/product-images/14687/10.jpg,https://oleks-netizen.github.io/product-images/14687/11.jpg,https://oleks-netizen.github.io/product-images/14687/12.jpg,https://oleks-netizen.github.io/product-images/14687/13.jpg,https://oleks-netizen.github.io/product-images/14687/15.jpg,https://oleks-netizen.github.io/product-images/14687/16.jpg,https://oleks-netizen.github.io/product-images/14687/04.jpg,https://oleks-netizen.github.io/product-images/14687/05.jpg,https://oleks-netizen.github.io/product-images/14687/06.jpg,https://oleks-netizen.github.io/product-images/14687/07.jpg,https://oleks-netizen.github.io/product-images/14687/08.jpg,https://oleks-netizen.github.io/product-images/14687/09.jpg</t>
         </is>
       </c>
       <c r="C113" t="n">
@@ -2126,7 +2126,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14689/1.jpg,https://oleks-netizen.github.io/product-images/14689/2.jpg,https://oleks-netizen.github.io/product-images/14689/9.jpg,https://oleks-netizen.github.io/product-images/14689/4.jpg,https://oleks-netizen.github.io/product-images/14689/5.jpg,https://oleks-netizen.github.io/product-images/14689/6.jpg,https://oleks-netizen.github.io/product-images/14689/7.jpg,https://oleks-netizen.github.io/product-images/14689/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14689/01.jpg,https://oleks-netizen.github.io/product-images/14689/02.jpg,https://oleks-netizen.github.io/product-images/14689/09.jpg,https://oleks-netizen.github.io/product-images/14689/04.jpg,https://oleks-netizen.github.io/product-images/14689/05.jpg,https://oleks-netizen.github.io/product-images/14689/06.jpg,https://oleks-netizen.github.io/product-images/14689/07.jpg,https://oleks-netizen.github.io/product-images/14689/08.jpg</t>
         </is>
       </c>
       <c r="C114" t="n">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14752/1.jpg,https://oleks-netizen.github.io/product-images/14752/2.jpg,https://oleks-netizen.github.io/product-images/14752/11.jpg,https://oleks-netizen.github.io/product-images/14752/14.jpg,https://oleks-netizen.github.io/product-images/14752/12.jpg,https://oleks-netizen.github.io/product-images/14752/13.jpg,https://oleks-netizen.github.io/product-images/14752/3.jpg,https://oleks-netizen.github.io/product-images/14752/4.jpg,https://oleks-netizen.github.io/product-images/14752/5.jpg,https://oleks-netizen.github.io/product-images/14752/6.jpg,https://oleks-netizen.github.io/product-images/14752/7.jpg,https://oleks-netizen.github.io/product-images/14752/8.jpg,https://oleks-netizen.github.io/product-images/14752/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14752/01.jpg,https://oleks-netizen.github.io/product-images/14752/02.jpg,https://oleks-netizen.github.io/product-images/14752/11.jpg,https://oleks-netizen.github.io/product-images/14752/14.jpg,https://oleks-netizen.github.io/product-images/14752/12.jpg,https://oleks-netizen.github.io/product-images/14752/13.jpg,https://oleks-netizen.github.io/product-images/14752/03.jpg,https://oleks-netizen.github.io/product-images/14752/04.jpg,https://oleks-netizen.github.io/product-images/14752/05.jpg,https://oleks-netizen.github.io/product-images/14752/06.jpg,https://oleks-netizen.github.io/product-images/14752/07.jpg,https://oleks-netizen.github.io/product-images/14752/08.jpg,https://oleks-netizen.github.io/product-images/14752/09.jpg</t>
         </is>
       </c>
       <c r="C115" t="n">
@@ -2156,7 +2156,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14776/1.jpg,https://oleks-netizen.github.io/product-images/14776/2.jpg,https://oleks-netizen.github.io/product-images/14776/9.jpg,https://oleks-netizen.github.io/product-images/14776/3.jpg,https://oleks-netizen.github.io/product-images/14776/4.jpg,https://oleks-netizen.github.io/product-images/14776/5.jpg,https://oleks-netizen.github.io/product-images/14776/6.jpg,https://oleks-netizen.github.io/product-images/14776/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14776/01.jpg,https://oleks-netizen.github.io/product-images/14776/02.jpg,https://oleks-netizen.github.io/product-images/14776/09.jpg,https://oleks-netizen.github.io/product-images/14776/03.jpg,https://oleks-netizen.github.io/product-images/14776/04.jpg,https://oleks-netizen.github.io/product-images/14776/05.jpg,https://oleks-netizen.github.io/product-images/14776/06.jpg,https://oleks-netizen.github.io/product-images/14776/07.jpg</t>
         </is>
       </c>
       <c r="C116" t="n">
@@ -2171,7 +2171,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14779/1.jpg,https://oleks-netizen.github.io/product-images/14779/2.jpg,https://oleks-netizen.github.io/product-images/14779/9.jpg,https://oleks-netizen.github.io/product-images/14779/3.jpg,https://oleks-netizen.github.io/product-images/14779/4.jpg,https://oleks-netizen.github.io/product-images/14779/5.jpg,https://oleks-netizen.github.io/product-images/14779/6.jpg,https://oleks-netizen.github.io/product-images/14779/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14779/01.jpg,https://oleks-netizen.github.io/product-images/14779/02.jpg,https://oleks-netizen.github.io/product-images/14779/09.jpg,https://oleks-netizen.github.io/product-images/14779/03.jpg,https://oleks-netizen.github.io/product-images/14779/04.jpg,https://oleks-netizen.github.io/product-images/14779/05.jpg,https://oleks-netizen.github.io/product-images/14779/06.jpg,https://oleks-netizen.github.io/product-images/14779/08.jpg</t>
         </is>
       </c>
       <c r="C117" t="n">
@@ -2186,7 +2186,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14893/1.jpg,https://oleks-netizen.github.io/product-images/14893/2.jpg,https://oleks-netizen.github.io/product-images/14893/10.jpg,https://oleks-netizen.github.io/product-images/14893/3.jpg,https://oleks-netizen.github.io/product-images/14893/4.jpg,https://oleks-netizen.github.io/product-images/14893/5.jpg,https://oleks-netizen.github.io/product-images/14893/6.jpg,https://oleks-netizen.github.io/product-images/14893/8.jpg,https://oleks-netizen.github.io/product-images/14893/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14893/01.jpg,https://oleks-netizen.github.io/product-images/14893/02.jpg,https://oleks-netizen.github.io/product-images/14893/10.jpg,https://oleks-netizen.github.io/product-images/14893/03.jpg,https://oleks-netizen.github.io/product-images/14893/04.jpg,https://oleks-netizen.github.io/product-images/14893/05.jpg,https://oleks-netizen.github.io/product-images/14893/06.jpg,https://oleks-netizen.github.io/product-images/14893/08.jpg,https://oleks-netizen.github.io/product-images/14893/09.jpg</t>
         </is>
       </c>
       <c r="C118" t="n">
@@ -2201,7 +2201,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14894/1.jpg,https://oleks-netizen.github.io/product-images/14894/2.jpg,https://oleks-netizen.github.io/product-images/14894/10.jpg,https://oleks-netizen.github.io/product-images/14894/11.jpg,https://oleks-netizen.github.io/product-images/14894/12.jpg,https://oleks-netizen.github.io/product-images/14894/13.jpg,https://oleks-netizen.github.io/product-images/14894/3.jpg,https://oleks-netizen.github.io/product-images/14894/4.jpg,https://oleks-netizen.github.io/product-images/14894/5.jpg,https://oleks-netizen.github.io/product-images/14894/6.jpg,https://oleks-netizen.github.io/product-images/14894/7.jpg,https://oleks-netizen.github.io/product-images/14894/8.jpg,https://oleks-netizen.github.io/product-images/14894/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14894/01.jpg,https://oleks-netizen.github.io/product-images/14894/02.jpg,https://oleks-netizen.github.io/product-images/14894/10.jpg,https://oleks-netizen.github.io/product-images/14894/11.jpg,https://oleks-netizen.github.io/product-images/14894/12.jpg,https://oleks-netizen.github.io/product-images/14894/13.jpg,https://oleks-netizen.github.io/product-images/14894/03.jpg,https://oleks-netizen.github.io/product-images/14894/04.jpg,https://oleks-netizen.github.io/product-images/14894/05.jpg,https://oleks-netizen.github.io/product-images/14894/06.jpg,https://oleks-netizen.github.io/product-images/14894/07.jpg,https://oleks-netizen.github.io/product-images/14894/08.jpg,https://oleks-netizen.github.io/product-images/14894/09.jpg</t>
         </is>
       </c>
       <c r="C119" t="n">
@@ -2216,7 +2216,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14906/1.jpg,https://oleks-netizen.github.io/product-images/14906/2.jpg,https://oleks-netizen.github.io/product-images/14906/3.jpg,https://oleks-netizen.github.io/product-images/14906/4.jpg,https://oleks-netizen.github.io/product-images/14906/5.jpg,https://oleks-netizen.github.io/product-images/14906/6.jpg,https://oleks-netizen.github.io/product-images/14906/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14906/01.jpg,https://oleks-netizen.github.io/product-images/14906/02.jpg,https://oleks-netizen.github.io/product-images/14906/03.jpg,https://oleks-netizen.github.io/product-images/14906/04.jpg,https://oleks-netizen.github.io/product-images/14906/05.jpg,https://oleks-netizen.github.io/product-images/14906/06.jpg,https://oleks-netizen.github.io/product-images/14906/07.jpg</t>
         </is>
       </c>
       <c r="C120" t="n">
@@ -2231,7 +2231,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14911/1.jpg,https://oleks-netizen.github.io/product-images/14911/2.jpg,https://oleks-netizen.github.io/product-images/14911/7.jpg,https://oleks-netizen.github.io/product-images/14911/14.jpg,https://oleks-netizen.github.io/product-images/14911/10.jpg,https://oleks-netizen.github.io/product-images/14911/11.jpg,https://oleks-netizen.github.io/product-images/14911/12.jpg,https://oleks-netizen.github.io/product-images/14911/13.jpg,https://oleks-netizen.github.io/product-images/14911/3.jpg,https://oleks-netizen.github.io/product-images/14911/4.jpg,https://oleks-netizen.github.io/product-images/14911/5.jpg,https://oleks-netizen.github.io/product-images/14911/6.jpg,https://oleks-netizen.github.io/product-images/14911/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14911/01.jpg,https://oleks-netizen.github.io/product-images/14911/02.jpg,https://oleks-netizen.github.io/product-images/14911/07.jpg,https://oleks-netizen.github.io/product-images/14911/14.jpg,https://oleks-netizen.github.io/product-images/14911/10.jpg,https://oleks-netizen.github.io/product-images/14911/11.jpg,https://oleks-netizen.github.io/product-images/14911/12.jpg,https://oleks-netizen.github.io/product-images/14911/13.jpg,https://oleks-netizen.github.io/product-images/14911/03.jpg,https://oleks-netizen.github.io/product-images/14911/04.jpg,https://oleks-netizen.github.io/product-images/14911/05.jpg,https://oleks-netizen.github.io/product-images/14911/06.jpg,https://oleks-netizen.github.io/product-images/14911/08.jpg</t>
         </is>
       </c>
       <c r="C121" t="n">
@@ -2246,7 +2246,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14912/1.jpg,https://oleks-netizen.github.io/product-images/14912/2.jpg,https://oleks-netizen.github.io/product-images/14912/9.jpg,https://oleks-netizen.github.io/product-images/14912/14.jpg,https://oleks-netizen.github.io/product-images/14912/10.jpg,https://oleks-netizen.github.io/product-images/14912/11.jpg,https://oleks-netizen.github.io/product-images/14912/12.jpg,https://oleks-netizen.github.io/product-images/14912/3.jpg,https://oleks-netizen.github.io/product-images/14912/4.jpg,https://oleks-netizen.github.io/product-images/14912/5.jpg,https://oleks-netizen.github.io/product-images/14912/6.jpg,https://oleks-netizen.github.io/product-images/14912/7.jpg,https://oleks-netizen.github.io/product-images/14912/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14912/01.jpg,https://oleks-netizen.github.io/product-images/14912/02.jpg,https://oleks-netizen.github.io/product-images/14912/09.jpg,https://oleks-netizen.github.io/product-images/14912/14.jpg,https://oleks-netizen.github.io/product-images/14912/10.jpg,https://oleks-netizen.github.io/product-images/14912/11.jpg,https://oleks-netizen.github.io/product-images/14912/12.jpg,https://oleks-netizen.github.io/product-images/14912/03.jpg,https://oleks-netizen.github.io/product-images/14912/04.jpg,https://oleks-netizen.github.io/product-images/14912/05.jpg,https://oleks-netizen.github.io/product-images/14912/06.jpg,https://oleks-netizen.github.io/product-images/14912/07.jpg,https://oleks-netizen.github.io/product-images/14912/08.jpg</t>
         </is>
       </c>
       <c r="C122" t="n">
@@ -2261,7 +2261,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14913/1.jpg,https://oleks-netizen.github.io/product-images/14913/2.jpg,https://oleks-netizen.github.io/product-images/14913/3.jpg,https://oleks-netizen.github.io/product-images/14913/15.jpg,https://oleks-netizen.github.io/product-images/14913/10.jpg,https://oleks-netizen.github.io/product-images/14913/12.jpg,https://oleks-netizen.github.io/product-images/14913/13.jpg,https://oleks-netizen.github.io/product-images/14913/14.jpg,https://oleks-netizen.github.io/product-images/14913/4.jpg,https://oleks-netizen.github.io/product-images/14913/5.jpg,https://oleks-netizen.github.io/product-images/14913/6.jpg,https://oleks-netizen.github.io/product-images/14913/7.jpg,https://oleks-netizen.github.io/product-images/14913/8.jpg,https://oleks-netizen.github.io/product-images/14913/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14913/01.jpg,https://oleks-netizen.github.io/product-images/14913/02.jpg,https://oleks-netizen.github.io/product-images/14913/03.jpg,https://oleks-netizen.github.io/product-images/14913/15.jpg,https://oleks-netizen.github.io/product-images/14913/10.jpg,https://oleks-netizen.github.io/product-images/14913/12.jpg,https://oleks-netizen.github.io/product-images/14913/13.jpg,https://oleks-netizen.github.io/product-images/14913/14.jpg,https://oleks-netizen.github.io/product-images/14913/04.jpg,https://oleks-netizen.github.io/product-images/14913/05.jpg,https://oleks-netizen.github.io/product-images/14913/06.jpg,https://oleks-netizen.github.io/product-images/14913/07.jpg,https://oleks-netizen.github.io/product-images/14913/08.jpg,https://oleks-netizen.github.io/product-images/14913/09.jpg</t>
         </is>
       </c>
       <c r="C123" t="n">
@@ -2276,7 +2276,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14916/1.jpg,https://oleks-netizen.github.io/product-images/14916/2.jpg,https://oleks-netizen.github.io/product-images/14916/3.jpg,https://oleks-netizen.github.io/product-images/14916/11.jpg,https://oleks-netizen.github.io/product-images/14916/10.jpg,https://oleks-netizen.github.io/product-images/14916/4.jpg,https://oleks-netizen.github.io/product-images/14916/5.jpg,https://oleks-netizen.github.io/product-images/14916/7.jpg,https://oleks-netizen.github.io/product-images/14916/8.jpg,https://oleks-netizen.github.io/product-images/14916/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14916/01.jpg,https://oleks-netizen.github.io/product-images/14916/02.jpg,https://oleks-netizen.github.io/product-images/14916/03.jpg,https://oleks-netizen.github.io/product-images/14916/11.jpg,https://oleks-netizen.github.io/product-images/14916/10.jpg,https://oleks-netizen.github.io/product-images/14916/04.jpg,https://oleks-netizen.github.io/product-images/14916/05.jpg,https://oleks-netizen.github.io/product-images/14916/07.jpg,https://oleks-netizen.github.io/product-images/14916/08.jpg,https://oleks-netizen.github.io/product-images/14916/09.jpg</t>
         </is>
       </c>
       <c r="C124" t="n">
@@ -2291,7 +2291,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14917/1.jpg,https://oleks-netizen.github.io/product-images/14917/2.jpg,https://oleks-netizen.github.io/product-images/14917/6.jpg,https://oleks-netizen.github.io/product-images/14917/14.jpg,https://oleks-netizen.github.io/product-images/14917/11.jpg,https://oleks-netizen.github.io/product-images/14917/12.jpg,https://oleks-netizen.github.io/product-images/14917/13.jpg,https://oleks-netizen.github.io/product-images/14917/3.jpg,https://oleks-netizen.github.io/product-images/14917/4.jpg,https://oleks-netizen.github.io/product-images/14917/5.jpg,https://oleks-netizen.github.io/product-images/14917/7.jpg,https://oleks-netizen.github.io/product-images/14917/8.jpg,https://oleks-netizen.github.io/product-images/14917/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14917/01.jpg,https://oleks-netizen.github.io/product-images/14917/02.jpg,https://oleks-netizen.github.io/product-images/14917/06.jpg,https://oleks-netizen.github.io/product-images/14917/14.jpg,https://oleks-netizen.github.io/product-images/14917/11.jpg,https://oleks-netizen.github.io/product-images/14917/12.jpg,https://oleks-netizen.github.io/product-images/14917/13.jpg,https://oleks-netizen.github.io/product-images/14917/03.jpg,https://oleks-netizen.github.io/product-images/14917/04.jpg,https://oleks-netizen.github.io/product-images/14917/05.jpg,https://oleks-netizen.github.io/product-images/14917/07.jpg,https://oleks-netizen.github.io/product-images/14917/08.jpg,https://oleks-netizen.github.io/product-images/14917/09.jpg</t>
         </is>
       </c>
       <c r="C125" t="n">
@@ -2306,7 +2306,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14918/1.jpg,https://oleks-netizen.github.io/product-images/14918/2.jpg,https://oleks-netizen.github.io/product-images/14918/5.jpg,https://oleks-netizen.github.io/product-images/14918/9.jpg,https://oleks-netizen.github.io/product-images/14918/3.jpg,https://oleks-netizen.github.io/product-images/14918/4.jpg,https://oleks-netizen.github.io/product-images/14918/7.jpg,https://oleks-netizen.github.io/product-images/14918/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14918/01.jpg,https://oleks-netizen.github.io/product-images/14918/02.jpg,https://oleks-netizen.github.io/product-images/14918/05.jpg,https://oleks-netizen.github.io/product-images/14918/09.jpg,https://oleks-netizen.github.io/product-images/14918/03.jpg,https://oleks-netizen.github.io/product-images/14918/04.jpg,https://oleks-netizen.github.io/product-images/14918/07.jpg,https://oleks-netizen.github.io/product-images/14918/08.jpg</t>
         </is>
       </c>
       <c r="C126" t="n">
@@ -2321,7 +2321,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14919/1.jpg,https://oleks-netizen.github.io/product-images/14919/2.jpg,https://oleks-netizen.github.io/product-images/14919/5.jpg,https://oleks-netizen.github.io/product-images/14919/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14919/01.jpg,https://oleks-netizen.github.io/product-images/14919/02.jpg,https://oleks-netizen.github.io/product-images/14919/05.jpg,https://oleks-netizen.github.io/product-images/14919/04.jpg</t>
         </is>
       </c>
       <c r="C127" t="n">
@@ -2336,7 +2336,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14923/1.jpg,https://oleks-netizen.github.io/product-images/14923/2.jpg,https://oleks-netizen.github.io/product-images/14923/3.jpg,https://oleks-netizen.github.io/product-images/14923/4.jpg,https://oleks-netizen.github.io/product-images/14923/5.jpg,https://oleks-netizen.github.io/product-images/14923/6.jpg,https://oleks-netizen.github.io/product-images/14923/7.jpg,https://oleks-netizen.github.io/product-images/14923/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14923/01.jpg,https://oleks-netizen.github.io/product-images/14923/02.jpg,https://oleks-netizen.github.io/product-images/14923/03.jpg,https://oleks-netizen.github.io/product-images/14923/04.jpg,https://oleks-netizen.github.io/product-images/14923/05.jpg,https://oleks-netizen.github.io/product-images/14923/06.jpg,https://oleks-netizen.github.io/product-images/14923/07.jpg,https://oleks-netizen.github.io/product-images/14923/08.jpg</t>
         </is>
       </c>
       <c r="C128" t="n">
@@ -2351,7 +2351,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14924/1.jpg,https://oleks-netizen.github.io/product-images/14924/2.jpg,https://oleks-netizen.github.io/product-images/14924/9.jpg,https://oleks-netizen.github.io/product-images/14924/10.jpg,https://oleks-netizen.github.io/product-images/14924/3.jpg,https://oleks-netizen.github.io/product-images/14924/4.jpg,https://oleks-netizen.github.io/product-images/14924/6.jpg,https://oleks-netizen.github.io/product-images/14924/7.jpg,https://oleks-netizen.github.io/product-images/14924/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14924/01.jpg,https://oleks-netizen.github.io/product-images/14924/02.jpg,https://oleks-netizen.github.io/product-images/14924/09.jpg,https://oleks-netizen.github.io/product-images/14924/10.jpg,https://oleks-netizen.github.io/product-images/14924/03.jpg,https://oleks-netizen.github.io/product-images/14924/04.jpg,https://oleks-netizen.github.io/product-images/14924/06.jpg,https://oleks-netizen.github.io/product-images/14924/07.jpg,https://oleks-netizen.github.io/product-images/14924/08.jpg</t>
         </is>
       </c>
       <c r="C129" t="n">
@@ -2366,7 +2366,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14925/1.jpg,https://oleks-netizen.github.io/product-images/14925/2.jpg,https://oleks-netizen.github.io/product-images/14925/8.jpg,https://oleks-netizen.github.io/product-images/14925/10.jpg,https://oleks-netizen.github.io/product-images/14925/3.jpg,https://oleks-netizen.github.io/product-images/14925/4.jpg,https://oleks-netizen.github.io/product-images/14925/5.jpg,https://oleks-netizen.github.io/product-images/14925/6.jpg,https://oleks-netizen.github.io/product-images/14925/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14925/01.jpg,https://oleks-netizen.github.io/product-images/14925/02.jpg,https://oleks-netizen.github.io/product-images/14925/08.jpg,https://oleks-netizen.github.io/product-images/14925/10.jpg,https://oleks-netizen.github.io/product-images/14925/03.jpg,https://oleks-netizen.github.io/product-images/14925/04.jpg,https://oleks-netizen.github.io/product-images/14925/05.jpg,https://oleks-netizen.github.io/product-images/14925/06.jpg,https://oleks-netizen.github.io/product-images/14925/09.jpg</t>
         </is>
       </c>
       <c r="C130" t="n">
@@ -2381,7 +2381,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14926/1.jpg,https://oleks-netizen.github.io/product-images/14926/2.jpg,https://oleks-netizen.github.io/product-images/14926/9.jpg,https://oleks-netizen.github.io/product-images/14926/3.jpg,https://oleks-netizen.github.io/product-images/14926/4.jpg,https://oleks-netizen.github.io/product-images/14926/6.jpg,https://oleks-netizen.github.io/product-images/14926/7.jpg,https://oleks-netizen.github.io/product-images/14926/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14926/01.jpg,https://oleks-netizen.github.io/product-images/14926/02.jpg,https://oleks-netizen.github.io/product-images/14926/09.jpg,https://oleks-netizen.github.io/product-images/14926/03.jpg,https://oleks-netizen.github.io/product-images/14926/04.jpg,https://oleks-netizen.github.io/product-images/14926/06.jpg,https://oleks-netizen.github.io/product-images/14926/07.jpg,https://oleks-netizen.github.io/product-images/14926/08.jpg</t>
         </is>
       </c>
       <c r="C131" t="n">
@@ -2396,7 +2396,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14927/1.jpg,https://oleks-netizen.github.io/product-images/14927/2.jpg,https://oleks-netizen.github.io/product-images/14927/9.jpg,https://oleks-netizen.github.io/product-images/14927/12.jpg,https://oleks-netizen.github.io/product-images/14927/11.jpg,https://oleks-netizen.github.io/product-images/14927/3.jpg,https://oleks-netizen.github.io/product-images/14927/4.jpg,https://oleks-netizen.github.io/product-images/14927/5.jpg,https://oleks-netizen.github.io/product-images/14927/6.jpg,https://oleks-netizen.github.io/product-images/14927/7.jpg,https://oleks-netizen.github.io/product-images/14927/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14927/01.jpg,https://oleks-netizen.github.io/product-images/14927/02.jpg,https://oleks-netizen.github.io/product-images/14927/09.jpg,https://oleks-netizen.github.io/product-images/14927/12.jpg,https://oleks-netizen.github.io/product-images/14927/11.jpg,https://oleks-netizen.github.io/product-images/14927/03.jpg,https://oleks-netizen.github.io/product-images/14927/04.jpg,https://oleks-netizen.github.io/product-images/14927/05.jpg,https://oleks-netizen.github.io/product-images/14927/06.jpg,https://oleks-netizen.github.io/product-images/14927/07.jpg,https://oleks-netizen.github.io/product-images/14927/08.jpg</t>
         </is>
       </c>
       <c r="C132" t="n">
@@ -2411,7 +2411,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14934/1.jpg,https://oleks-netizen.github.io/product-images/14934/2.jpg,https://oleks-netizen.github.io/product-images/14934/14.jpg,https://oleks-netizen.github.io/product-images/14934/10.jpg,https://oleks-netizen.github.io/product-images/14934/11.jpg,https://oleks-netizen.github.io/product-images/14934/12.jpg,https://oleks-netizen.github.io/product-images/14934/13.jpg,https://oleks-netizen.github.io/product-images/14934/3.jpg,https://oleks-netizen.github.io/product-images/14934/4.jpg,https://oleks-netizen.github.io/product-images/14934/5.jpg,https://oleks-netizen.github.io/product-images/14934/6.jpg,https://oleks-netizen.github.io/product-images/14934/7.jpg,https://oleks-netizen.github.io/product-images/14934/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14934/01.jpg,https://oleks-netizen.github.io/product-images/14934/02.jpg,https://oleks-netizen.github.io/product-images/14934/14.jpg,https://oleks-netizen.github.io/product-images/14934/10.jpg,https://oleks-netizen.github.io/product-images/14934/11.jpg,https://oleks-netizen.github.io/product-images/14934/12.jpg,https://oleks-netizen.github.io/product-images/14934/13.jpg,https://oleks-netizen.github.io/product-images/14934/03.jpg,https://oleks-netizen.github.io/product-images/14934/04.jpg,https://oleks-netizen.github.io/product-images/14934/05.jpg,https://oleks-netizen.github.io/product-images/14934/06.jpg,https://oleks-netizen.github.io/product-images/14934/07.jpg,https://oleks-netizen.github.io/product-images/14934/08.jpg</t>
         </is>
       </c>
       <c r="C133" t="n">
@@ -2426,7 +2426,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14935/1.jpg,https://oleks-netizen.github.io/product-images/14935/2.jpg,https://oleks-netizen.github.io/product-images/14935/11.jpg,https://oleks-netizen.github.io/product-images/14935/12.jpg,https://oleks-netizen.github.io/product-images/14935/10.jpg,https://oleks-netizen.github.io/product-images/14935/3.jpg,https://oleks-netizen.github.io/product-images/14935/4.jpg,https://oleks-netizen.github.io/product-images/14935/5.jpg,https://oleks-netizen.github.io/product-images/14935/7.jpg,https://oleks-netizen.github.io/product-images/14935/8.jpg,https://oleks-netizen.github.io/product-images/14935/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14935/01.jpg,https://oleks-netizen.github.io/product-images/14935/02.jpg,https://oleks-netizen.github.io/product-images/14935/11.jpg,https://oleks-netizen.github.io/product-images/14935/12.jpg,https://oleks-netizen.github.io/product-images/14935/10.jpg,https://oleks-netizen.github.io/product-images/14935/03.jpg,https://oleks-netizen.github.io/product-images/14935/04.jpg,https://oleks-netizen.github.io/product-images/14935/05.jpg,https://oleks-netizen.github.io/product-images/14935/07.jpg,https://oleks-netizen.github.io/product-images/14935/08.jpg,https://oleks-netizen.github.io/product-images/14935/09.jpg</t>
         </is>
       </c>
       <c r="C134" t="n">
@@ -2441,7 +2441,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14963/1.jpg,https://oleks-netizen.github.io/product-images/14963/2.jpg,https://oleks-netizen.github.io/product-images/14963/9.jpg,https://oleks-netizen.github.io/product-images/14963/3.jpg,https://oleks-netizen.github.io/product-images/14963/4.jpg,https://oleks-netizen.github.io/product-images/14963/6.jpg,https://oleks-netizen.github.io/product-images/14963/7.jpg,https://oleks-netizen.github.io/product-images/14963/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14963/01.jpg,https://oleks-netizen.github.io/product-images/14963/02.jpg,https://oleks-netizen.github.io/product-images/14963/09.jpg,https://oleks-netizen.github.io/product-images/14963/03.jpg,https://oleks-netizen.github.io/product-images/14963/04.jpg,https://oleks-netizen.github.io/product-images/14963/06.jpg,https://oleks-netizen.github.io/product-images/14963/07.jpg,https://oleks-netizen.github.io/product-images/14963/08.jpg</t>
         </is>
       </c>
       <c r="C135" t="n">
@@ -2456,7 +2456,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/14964/1.jpg,https://oleks-netizen.github.io/product-images/14964/2.jpg,https://oleks-netizen.github.io/product-images/14964/3.jpg,https://oleks-netizen.github.io/product-images/14964/4.jpg,https://oleks-netizen.github.io/product-images/14964/5.jpg,https://oleks-netizen.github.io/product-images/14964/6.jpg,https://oleks-netizen.github.io/product-images/14964/7.jpg,https://oleks-netizen.github.io/product-images/14964/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/14964/01.jpg,https://oleks-netizen.github.io/product-images/14964/02.jpg,https://oleks-netizen.github.io/product-images/14964/03.jpg,https://oleks-netizen.github.io/product-images/14964/04.jpg,https://oleks-netizen.github.io/product-images/14964/05.jpg,https://oleks-netizen.github.io/product-images/14964/06.jpg,https://oleks-netizen.github.io/product-images/14964/07.jpg,https://oleks-netizen.github.io/product-images/14964/08.jpg</t>
         </is>
       </c>
       <c r="C136" t="n">
@@ -2471,7 +2471,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/16134/1.jpg,https://oleks-netizen.github.io/product-images/16134/2.jpg,https://oleks-netizen.github.io/product-images/16134/6.jpg,https://oleks-netizen.github.io/product-images/16134/4.jpg,https://oleks-netizen.github.io/product-images/16134/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/16134/01.jpg,https://oleks-netizen.github.io/product-images/16134/02.jpg,https://oleks-netizen.github.io/product-images/16134/06.jpg,https://oleks-netizen.github.io/product-images/16134/04.jpg,https://oleks-netizen.github.io/product-images/16134/05.jpg</t>
         </is>
       </c>
       <c r="C137" t="n">
@@ -2486,7 +2486,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/16142/1.jpg,https://oleks-netizen.github.io/product-images/16142/2.jpg,https://oleks-netizen.github.io/product-images/16142/6.jpg,https://oleks-netizen.github.io/product-images/16142/3.jpg,https://oleks-netizen.github.io/product-images/16142/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/16142/01.jpg,https://oleks-netizen.github.io/product-images/16142/02.jpg,https://oleks-netizen.github.io/product-images/16142/06.jpg,https://oleks-netizen.github.io/product-images/16142/03.jpg,https://oleks-netizen.github.io/product-images/16142/04.jpg</t>
         </is>
       </c>
       <c r="C138" t="n">
@@ -2501,7 +2501,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/16169/1.jpg,https://oleks-netizen.github.io/product-images/16169/2.jpg,https://oleks-netizen.github.io/product-images/16169/7.jpg,https://oleks-netizen.github.io/product-images/16169/3.jpg,https://oleks-netizen.github.io/product-images/16169/4.jpg,https://oleks-netizen.github.io/product-images/16169/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/16169/01.jpg,https://oleks-netizen.github.io/product-images/16169/02.jpg,https://oleks-netizen.github.io/product-images/16169/07.jpg,https://oleks-netizen.github.io/product-images/16169/03.jpg,https://oleks-netizen.github.io/product-images/16169/04.jpg,https://oleks-netizen.github.io/product-images/16169/05.jpg</t>
         </is>
       </c>
       <c r="C139" t="n">
@@ -2516,7 +2516,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/16206/1.jpg,https://oleks-netizen.github.io/product-images/16206/2.jpg,https://oleks-netizen.github.io/product-images/16206/8.jpg,https://oleks-netizen.github.io/product-images/16206/3.jpg,https://oleks-netizen.github.io/product-images/16206/4.jpg,https://oleks-netizen.github.io/product-images/16206/5.jpg,https://oleks-netizen.github.io/product-images/16206/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/16206/01.jpg,https://oleks-netizen.github.io/product-images/16206/02.jpg,https://oleks-netizen.github.io/product-images/16206/08.jpg,https://oleks-netizen.github.io/product-images/16206/03.jpg,https://oleks-netizen.github.io/product-images/16206/04.jpg,https://oleks-netizen.github.io/product-images/16206/05.jpg,https://oleks-netizen.github.io/product-images/16206/07.jpg</t>
         </is>
       </c>
       <c r="C140" t="n">
@@ -2531,7 +2531,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/17086/1.jpg,https://oleks-netizen.github.io/product-images/17086/2.jpg,https://oleks-netizen.github.io/product-images/17086/7.jpg,https://oleks-netizen.github.io/product-images/17086/4.jpg,https://oleks-netizen.github.io/product-images/17086/5.jpg,https://oleks-netizen.github.io/product-images/17086/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/17086/01.jpg,https://oleks-netizen.github.io/product-images/17086/02.jpg,https://oleks-netizen.github.io/product-images/17086/07.jpg,https://oleks-netizen.github.io/product-images/17086/04.jpg,https://oleks-netizen.github.io/product-images/17086/05.jpg,https://oleks-netizen.github.io/product-images/17086/06.jpg</t>
         </is>
       </c>
       <c r="C141" t="n">
@@ -2546,7 +2546,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/17098/1.jpg,https://oleks-netizen.github.io/product-images/17098/2.jpg,https://oleks-netizen.github.io/product-images/17098/5.jpg,https://oleks-netizen.github.io/product-images/17098/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/17098/01.jpg,https://oleks-netizen.github.io/product-images/17098/02.jpg,https://oleks-netizen.github.io/product-images/17098/05.jpg,https://oleks-netizen.github.io/product-images/17098/03.jpg</t>
         </is>
       </c>
       <c r="C142" t="n">
@@ -2561,7 +2561,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/17229/1.jpg,https://oleks-netizen.github.io/product-images/17229/2.jpg,https://oleks-netizen.github.io/product-images/17229/7.jpg,https://oleks-netizen.github.io/product-images/17229/3.jpg,https://oleks-netizen.github.io/product-images/17229/4.jpg,https://oleks-netizen.github.io/product-images/17229/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/17229/01.jpg,https://oleks-netizen.github.io/product-images/17229/02.jpg,https://oleks-netizen.github.io/product-images/17229/07.jpg,https://oleks-netizen.github.io/product-images/17229/03.jpg,https://oleks-netizen.github.io/product-images/17229/04.jpg,https://oleks-netizen.github.io/product-images/17229/05.jpg</t>
         </is>
       </c>
       <c r="C143" t="n">
@@ -2576,7 +2576,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/17238/1.jpg,https://oleks-netizen.github.io/product-images/17238/2.jpg,https://oleks-netizen.github.io/product-images/17238/7.jpg,https://oleks-netizen.github.io/product-images/17238/3.jpg,https://oleks-netizen.github.io/product-images/17238/4.jpg,https://oleks-netizen.github.io/product-images/17238/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/17238/01.jpg,https://oleks-netizen.github.io/product-images/17238/02.jpg,https://oleks-netizen.github.io/product-images/17238/07.jpg,https://oleks-netizen.github.io/product-images/17238/03.jpg,https://oleks-netizen.github.io/product-images/17238/04.jpg,https://oleks-netizen.github.io/product-images/17238/05.jpg</t>
         </is>
       </c>
       <c r="C144" t="n">
@@ -2591,7 +2591,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/17248/1.jpg,https://oleks-netizen.github.io/product-images/17248/2.jpg,https://oleks-netizen.github.io/product-images/17248/8.jpg,https://oleks-netizen.github.io/product-images/17248/3.jpg,https://oleks-netizen.github.io/product-images/17248/4.jpg,https://oleks-netizen.github.io/product-images/17248/6.jpg,https://oleks-netizen.github.io/product-images/17248/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/17248/01.jpg,https://oleks-netizen.github.io/product-images/17248/02.jpg,https://oleks-netizen.github.io/product-images/17248/08.jpg,https://oleks-netizen.github.io/product-images/17248/03.jpg,https://oleks-netizen.github.io/product-images/17248/04.jpg,https://oleks-netizen.github.io/product-images/17248/06.jpg,https://oleks-netizen.github.io/product-images/17248/07.jpg</t>
         </is>
       </c>
       <c r="C145" t="n">
@@ -2606,7 +2606,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18004/1.jpg,https://oleks-netizen.github.io/product-images/18004/2.jpg,https://oleks-netizen.github.io/product-images/18004/11.jpg,https://oleks-netizen.github.io/product-images/18004/10.jpg,https://oleks-netizen.github.io/product-images/18004/3.jpg,https://oleks-netizen.github.io/product-images/18004/4.jpg,https://oleks-netizen.github.io/product-images/18004/5.jpg,https://oleks-netizen.github.io/product-images/18004/7.jpg,https://oleks-netizen.github.io/product-images/18004/8.jpg,https://oleks-netizen.github.io/product-images/18004/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18004/01.jpg,https://oleks-netizen.github.io/product-images/18004/02.jpg,https://oleks-netizen.github.io/product-images/18004/11.jpg,https://oleks-netizen.github.io/product-images/18004/10.jpg,https://oleks-netizen.github.io/product-images/18004/03.jpg,https://oleks-netizen.github.io/product-images/18004/04.jpg,https://oleks-netizen.github.io/product-images/18004/05.jpg,https://oleks-netizen.github.io/product-images/18004/07.jpg,https://oleks-netizen.github.io/product-images/18004/08.jpg,https://oleks-netizen.github.io/product-images/18004/09.jpg</t>
         </is>
       </c>
       <c r="C146" t="n">
@@ -2621,7 +2621,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18012/1.jpg,https://oleks-netizen.github.io/product-images/18012/2.jpg,https://oleks-netizen.github.io/product-images/18012/5.jpg,https://oleks-netizen.github.io/product-images/18012/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18012/01.jpg,https://oleks-netizen.github.io/product-images/18012/02.jpg,https://oleks-netizen.github.io/product-images/18012/05.jpg,https://oleks-netizen.github.io/product-images/18012/03.jpg</t>
         </is>
       </c>
       <c r="C147" t="n">
@@ -2636,7 +2636,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18018/1.jpg,https://oleks-netizen.github.io/product-images/18018/2.jpg,https://oleks-netizen.github.io/product-images/18018/13.jpg,https://oleks-netizen.github.io/product-images/18018/10.jpg,https://oleks-netizen.github.io/product-images/18018/11.jpg,https://oleks-netizen.github.io/product-images/18018/12.jpg,https://oleks-netizen.github.io/product-images/18018/3.jpg,https://oleks-netizen.github.io/product-images/18018/5.jpg,https://oleks-netizen.github.io/product-images/18018/6.jpg,https://oleks-netizen.github.io/product-images/18018/7.jpg,https://oleks-netizen.github.io/product-images/18018/8.jpg,https://oleks-netizen.github.io/product-images/18018/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18018/01.jpg,https://oleks-netizen.github.io/product-images/18018/02.jpg,https://oleks-netizen.github.io/product-images/18018/13.jpg,https://oleks-netizen.github.io/product-images/18018/10.jpg,https://oleks-netizen.github.io/product-images/18018/11.jpg,https://oleks-netizen.github.io/product-images/18018/12.jpg,https://oleks-netizen.github.io/product-images/18018/03.jpg,https://oleks-netizen.github.io/product-images/18018/05.jpg,https://oleks-netizen.github.io/product-images/18018/06.jpg,https://oleks-netizen.github.io/product-images/18018/07.jpg,https://oleks-netizen.github.io/product-images/18018/08.jpg,https://oleks-netizen.github.io/product-images/18018/09.jpg</t>
         </is>
       </c>
       <c r="C148" t="n">
@@ -2651,7 +2651,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18070/1.jpg,https://oleks-netizen.github.io/product-images/18070/2.jpg,https://oleks-netizen.github.io/product-images/18070/11.jpg,https://oleks-netizen.github.io/product-images/18070/10.jpg,https://oleks-netizen.github.io/product-images/18070/3.jpg,https://oleks-netizen.github.io/product-images/18070/4.jpg,https://oleks-netizen.github.io/product-images/18070/5.jpg,https://oleks-netizen.github.io/product-images/18070/7.jpg,https://oleks-netizen.github.io/product-images/18070/8.jpg,https://oleks-netizen.github.io/product-images/18070/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18070/01.jpg,https://oleks-netizen.github.io/product-images/18070/02.jpg,https://oleks-netizen.github.io/product-images/18070/11.jpg,https://oleks-netizen.github.io/product-images/18070/10.jpg,https://oleks-netizen.github.io/product-images/18070/03.jpg,https://oleks-netizen.github.io/product-images/18070/04.jpg,https://oleks-netizen.github.io/product-images/18070/05.jpg,https://oleks-netizen.github.io/product-images/18070/07.jpg,https://oleks-netizen.github.io/product-images/18070/08.jpg,https://oleks-netizen.github.io/product-images/18070/09.jpg</t>
         </is>
       </c>
       <c r="C149" t="n">
@@ -2666,7 +2666,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18092/1.jpg,https://oleks-netizen.github.io/product-images/18092/2.jpg,https://oleks-netizen.github.io/product-images/18092/3.jpg,https://oleks-netizen.github.io/product-images/18092/4.jpg,https://oleks-netizen.github.io/product-images/18092/5.jpg,https://oleks-netizen.github.io/product-images/18092/6.jpg,https://oleks-netizen.github.io/product-images/18092/7.jpg,https://oleks-netizen.github.io/product-images/18092/8.jpg,https://oleks-netizen.github.io/product-images/18092/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18092/01.jpg,https://oleks-netizen.github.io/product-images/18092/02.jpg,https://oleks-netizen.github.io/product-images/18092/03.jpg,https://oleks-netizen.github.io/product-images/18092/04.jpg,https://oleks-netizen.github.io/product-images/18092/05.jpg,https://oleks-netizen.github.io/product-images/18092/06.jpg,https://oleks-netizen.github.io/product-images/18092/07.jpg,https://oleks-netizen.github.io/product-images/18092/08.jpg,https://oleks-netizen.github.io/product-images/18092/09.jpg</t>
         </is>
       </c>
       <c r="C150" t="n">
@@ -2681,7 +2681,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18097/10.jpg,https://oleks-netizen.github.io/product-images/18097/1.jpg,https://oleks-netizen.github.io/product-images/18097/2.jpg,https://oleks-netizen.github.io/product-images/18097/3.jpg,https://oleks-netizen.github.io/product-images/18097/4.jpg,https://oleks-netizen.github.io/product-images/18097/5.jpg,https://oleks-netizen.github.io/product-images/18097/6.jpg,https://oleks-netizen.github.io/product-images/18097/7.jpg,https://oleks-netizen.github.io/product-images/18097/8.jpg,https://oleks-netizen.github.io/product-images/18097/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18097/10.jpg,https://oleks-netizen.github.io/product-images/18097/01.jpg,https://oleks-netizen.github.io/product-images/18097/02.jpg,https://oleks-netizen.github.io/product-images/18097/03.jpg,https://oleks-netizen.github.io/product-images/18097/04.jpg,https://oleks-netizen.github.io/product-images/18097/05.jpg,https://oleks-netizen.github.io/product-images/18097/06.jpg,https://oleks-netizen.github.io/product-images/18097/07.jpg,https://oleks-netizen.github.io/product-images/18097/08.jpg,https://oleks-netizen.github.io/product-images/18097/09.jpg</t>
         </is>
       </c>
       <c r="C151" t="n">
@@ -2696,7 +2696,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18103/10.jpg,https://oleks-netizen.github.io/product-images/18103/11.jpg,https://oleks-netizen.github.io/product-images/18103/1.jpg,https://oleks-netizen.github.io/product-images/18103/2.jpg,https://oleks-netizen.github.io/product-images/18103/3.jpg,https://oleks-netizen.github.io/product-images/18103/4.jpg,https://oleks-netizen.github.io/product-images/18103/5.jpg,https://oleks-netizen.github.io/product-images/18103/6.jpg,https://oleks-netizen.github.io/product-images/18103/7.jpg,https://oleks-netizen.github.io/product-images/18103/8.jpg,https://oleks-netizen.github.io/product-images/18103/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18103/10.jpg,https://oleks-netizen.github.io/product-images/18103/11.jpg,https://oleks-netizen.github.io/product-images/18103/01.jpg,https://oleks-netizen.github.io/product-images/18103/02.jpg,https://oleks-netizen.github.io/product-images/18103/03.jpg,https://oleks-netizen.github.io/product-images/18103/04.jpg,https://oleks-netizen.github.io/product-images/18103/05.jpg,https://oleks-netizen.github.io/product-images/18103/06.jpg,https://oleks-netizen.github.io/product-images/18103/07.jpg,https://oleks-netizen.github.io/product-images/18103/08.jpg,https://oleks-netizen.github.io/product-images/18103/09.jpg</t>
         </is>
       </c>
       <c r="C152" t="n">
@@ -2711,7 +2711,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18169/1.jpg,https://oleks-netizen.github.io/product-images/18169/2.jpg,https://oleks-netizen.github.io/product-images/18169/3.jpg,https://oleks-netizen.github.io/product-images/18169/4.jpg,https://oleks-netizen.github.io/product-images/18169/5.jpg,https://oleks-netizen.github.io/product-images/18169/6.jpg,https://oleks-netizen.github.io/product-images/18169/7.jpg,https://oleks-netizen.github.io/product-images/18169/8.jpg,https://oleks-netizen.github.io/product-images/18169/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18169/01.jpg,https://oleks-netizen.github.io/product-images/18169/02.jpg,https://oleks-netizen.github.io/product-images/18169/03.jpg,https://oleks-netizen.github.io/product-images/18169/04.jpg,https://oleks-netizen.github.io/product-images/18169/05.jpg,https://oleks-netizen.github.io/product-images/18169/06.jpg,https://oleks-netizen.github.io/product-images/18169/07.jpg,https://oleks-netizen.github.io/product-images/18169/08.jpg,https://oleks-netizen.github.io/product-images/18169/09.jpg</t>
         </is>
       </c>
       <c r="C153" t="n">
@@ -2726,7 +2726,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18171/10.jpg,https://oleks-netizen.github.io/product-images/18171/11.jpg,https://oleks-netizen.github.io/product-images/18171/12.jpg,https://oleks-netizen.github.io/product-images/18171/1.jpg,https://oleks-netizen.github.io/product-images/18171/2.jpg,https://oleks-netizen.github.io/product-images/18171/3.jpg,https://oleks-netizen.github.io/product-images/18171/4.jpg,https://oleks-netizen.github.io/product-images/18171/5.jpg,https://oleks-netizen.github.io/product-images/18171/6.jpg,https://oleks-netizen.github.io/product-images/18171/7.jpg,https://oleks-netizen.github.io/product-images/18171/8.jpg,https://oleks-netizen.github.io/product-images/18171/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18171/10.jpg,https://oleks-netizen.github.io/product-images/18171/11.jpg,https://oleks-netizen.github.io/product-images/18171/12.jpg,https://oleks-netizen.github.io/product-images/18171/01.jpg,https://oleks-netizen.github.io/product-images/18171/02.jpg,https://oleks-netizen.github.io/product-images/18171/03.jpg,https://oleks-netizen.github.io/product-images/18171/04.jpg,https://oleks-netizen.github.io/product-images/18171/05.jpg,https://oleks-netizen.github.io/product-images/18171/06.jpg,https://oleks-netizen.github.io/product-images/18171/07.jpg,https://oleks-netizen.github.io/product-images/18171/08.jpg,https://oleks-netizen.github.io/product-images/18171/09.jpg</t>
         </is>
       </c>
       <c r="C154" t="n">
@@ -2741,7 +2741,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18178/10.jpg,https://oleks-netizen.github.io/product-images/18178/11.jpg,https://oleks-netizen.github.io/product-images/18178/12.jpg,https://oleks-netizen.github.io/product-images/18178/1.jpg,https://oleks-netizen.github.io/product-images/18178/2.jpg,https://oleks-netizen.github.io/product-images/18178/3.jpg,https://oleks-netizen.github.io/product-images/18178/4.jpg,https://oleks-netizen.github.io/product-images/18178/5.jpg,https://oleks-netizen.github.io/product-images/18178/6.jpg,https://oleks-netizen.github.io/product-images/18178/7.jpg,https://oleks-netizen.github.io/product-images/18178/8.jpg,https://oleks-netizen.github.io/product-images/18178/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18178/10.jpg,https://oleks-netizen.github.io/product-images/18178/11.jpg,https://oleks-netizen.github.io/product-images/18178/12.jpg,https://oleks-netizen.github.io/product-images/18178/01.jpg,https://oleks-netizen.github.io/product-images/18178/02.jpg,https://oleks-netizen.github.io/product-images/18178/03.jpg,https://oleks-netizen.github.io/product-images/18178/04.jpg,https://oleks-netizen.github.io/product-images/18178/05.jpg,https://oleks-netizen.github.io/product-images/18178/06.jpg,https://oleks-netizen.github.io/product-images/18178/07.jpg,https://oleks-netizen.github.io/product-images/18178/08.jpg,https://oleks-netizen.github.io/product-images/18178/09.jpg</t>
         </is>
       </c>
       <c r="C155" t="n">
@@ -2756,7 +2756,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18203/10.jpg,https://oleks-netizen.github.io/product-images/18203/11.jpg,https://oleks-netizen.github.io/product-images/18203/1.jpg,https://oleks-netizen.github.io/product-images/18203/2.jpg,https://oleks-netizen.github.io/product-images/18203/3.jpg,https://oleks-netizen.github.io/product-images/18203/4.jpg,https://oleks-netizen.github.io/product-images/18203/5.jpg,https://oleks-netizen.github.io/product-images/18203/6.jpg,https://oleks-netizen.github.io/product-images/18203/7.jpg,https://oleks-netizen.github.io/product-images/18203/8.jpg,https://oleks-netizen.github.io/product-images/18203/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18203/10.jpg,https://oleks-netizen.github.io/product-images/18203/11.jpg,https://oleks-netizen.github.io/product-images/18203/01.jpg,https://oleks-netizen.github.io/product-images/18203/02.jpg,https://oleks-netizen.github.io/product-images/18203/03.jpg,https://oleks-netizen.github.io/product-images/18203/04.jpg,https://oleks-netizen.github.io/product-images/18203/05.jpg,https://oleks-netizen.github.io/product-images/18203/06.jpg,https://oleks-netizen.github.io/product-images/18203/07.jpg,https://oleks-netizen.github.io/product-images/18203/08.jpg,https://oleks-netizen.github.io/product-images/18203/09.jpg</t>
         </is>
       </c>
       <c r="C156" t="n">
@@ -2771,7 +2771,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18235/10.jpg,https://oleks-netizen.github.io/product-images/18235/11.jpg,https://oleks-netizen.github.io/product-images/18235/12.jpg,https://oleks-netizen.github.io/product-images/18235/13.jpg,https://oleks-netizen.github.io/product-images/18235/1.jpg,https://oleks-netizen.github.io/product-images/18235/2.jpg,https://oleks-netizen.github.io/product-images/18235/3.jpg,https://oleks-netizen.github.io/product-images/18235/4.jpg,https://oleks-netizen.github.io/product-images/18235/5.jpg,https://oleks-netizen.github.io/product-images/18235/6.jpg,https://oleks-netizen.github.io/product-images/18235/7.jpg,https://oleks-netizen.github.io/product-images/18235/8.jpg,https://oleks-netizen.github.io/product-images/18235/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18235/10.jpg,https://oleks-netizen.github.io/product-images/18235/11.jpg,https://oleks-netizen.github.io/product-images/18235/12.jpg,https://oleks-netizen.github.io/product-images/18235/13.jpg,https://oleks-netizen.github.io/product-images/18235/01.jpg,https://oleks-netizen.github.io/product-images/18235/02.jpg,https://oleks-netizen.github.io/product-images/18235/03.jpg,https://oleks-netizen.github.io/product-images/18235/04.jpg,https://oleks-netizen.github.io/product-images/18235/05.jpg,https://oleks-netizen.github.io/product-images/18235/06.jpg,https://oleks-netizen.github.io/product-images/18235/07.jpg,https://oleks-netizen.github.io/product-images/18235/08.jpg,https://oleks-netizen.github.io/product-images/18235/09.jpg</t>
         </is>
       </c>
       <c r="C157" t="n">
@@ -2786,7 +2786,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18236/10.jpg,https://oleks-netizen.github.io/product-images/18236/11.jpg,https://oleks-netizen.github.io/product-images/18236/12.jpg,https://oleks-netizen.github.io/product-images/18236/1.jpg,https://oleks-netizen.github.io/product-images/18236/2.jpg,https://oleks-netizen.github.io/product-images/18236/3.jpg,https://oleks-netizen.github.io/product-images/18236/4.jpg,https://oleks-netizen.github.io/product-images/18236/5.jpg,https://oleks-netizen.github.io/product-images/18236/6.jpg,https://oleks-netizen.github.io/product-images/18236/7.jpg,https://oleks-netizen.github.io/product-images/18236/8.jpg,https://oleks-netizen.github.io/product-images/18236/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18236/10.jpg,https://oleks-netizen.github.io/product-images/18236/11.jpg,https://oleks-netizen.github.io/product-images/18236/12.jpg,https://oleks-netizen.github.io/product-images/18236/01.jpg,https://oleks-netizen.github.io/product-images/18236/02.jpg,https://oleks-netizen.github.io/product-images/18236/03.jpg,https://oleks-netizen.github.io/product-images/18236/04.jpg,https://oleks-netizen.github.io/product-images/18236/05.jpg,https://oleks-netizen.github.io/product-images/18236/06.jpg,https://oleks-netizen.github.io/product-images/18236/07.jpg,https://oleks-netizen.github.io/product-images/18236/08.jpg,https://oleks-netizen.github.io/product-images/18236/09.jpg</t>
         </is>
       </c>
       <c r="C158" t="n">
@@ -2801,7 +2801,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18239/10.jpg,https://oleks-netizen.github.io/product-images/18239/11.jpg,https://oleks-netizen.github.io/product-images/18239/12.jpg,https://oleks-netizen.github.io/product-images/18239/13.jpg,https://oleks-netizen.github.io/product-images/18239/1.jpg,https://oleks-netizen.github.io/product-images/18239/2.jpg,https://oleks-netizen.github.io/product-images/18239/3.jpg,https://oleks-netizen.github.io/product-images/18239/4.jpg,https://oleks-netizen.github.io/product-images/18239/5.jpg,https://oleks-netizen.github.io/product-images/18239/6.jpg,https://oleks-netizen.github.io/product-images/18239/7.jpg,https://oleks-netizen.github.io/product-images/18239/8.jpg,https://oleks-netizen.github.io/product-images/18239/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18239/10.jpg,https://oleks-netizen.github.io/product-images/18239/11.jpg,https://oleks-netizen.github.io/product-images/18239/12.jpg,https://oleks-netizen.github.io/product-images/18239/13.jpg,https://oleks-netizen.github.io/product-images/18239/01.jpg,https://oleks-netizen.github.io/product-images/18239/02.jpg,https://oleks-netizen.github.io/product-images/18239/03.jpg,https://oleks-netizen.github.io/product-images/18239/04.jpg,https://oleks-netizen.github.io/product-images/18239/05.jpg,https://oleks-netizen.github.io/product-images/18239/06.jpg,https://oleks-netizen.github.io/product-images/18239/07.jpg,https://oleks-netizen.github.io/product-images/18239/08.jpg,https://oleks-netizen.github.io/product-images/18239/09.jpg</t>
         </is>
       </c>
       <c r="C159" t="n">
@@ -2816,7 +2816,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18293/10.jpg,https://oleks-netizen.github.io/product-images/18293/11.jpg,https://oleks-netizen.github.io/product-images/18293/12.jpg,https://oleks-netizen.github.io/product-images/18293/1.jpg,https://oleks-netizen.github.io/product-images/18293/2.jpg,https://oleks-netizen.github.io/product-images/18293/3.jpg,https://oleks-netizen.github.io/product-images/18293/4.jpg,https://oleks-netizen.github.io/product-images/18293/5.jpg,https://oleks-netizen.github.io/product-images/18293/6.jpg,https://oleks-netizen.github.io/product-images/18293/7.jpg,https://oleks-netizen.github.io/product-images/18293/8.jpg,https://oleks-netizen.github.io/product-images/18293/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18293/10.jpg,https://oleks-netizen.github.io/product-images/18293/11.jpg,https://oleks-netizen.github.io/product-images/18293/12.jpg,https://oleks-netizen.github.io/product-images/18293/01.jpg,https://oleks-netizen.github.io/product-images/18293/02.jpg,https://oleks-netizen.github.io/product-images/18293/03.jpg,https://oleks-netizen.github.io/product-images/18293/04.jpg,https://oleks-netizen.github.io/product-images/18293/05.jpg,https://oleks-netizen.github.io/product-images/18293/06.jpg,https://oleks-netizen.github.io/product-images/18293/07.jpg,https://oleks-netizen.github.io/product-images/18293/08.jpg,https://oleks-netizen.github.io/product-images/18293/09.jpg</t>
         </is>
       </c>
       <c r="C160" t="n">
@@ -2831,7 +2831,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18309/1.jpg,https://oleks-netizen.github.io/product-images/18309/2.jpg,https://oleks-netizen.github.io/product-images/18309/7.jpg,https://oleks-netizen.github.io/product-images/18309/4.jpg,https://oleks-netizen.github.io/product-images/18309/5.jpg,https://oleks-netizen.github.io/product-images/18309/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18309/01.jpg,https://oleks-netizen.github.io/product-images/18309/02.jpg,https://oleks-netizen.github.io/product-images/18309/07.jpg,https://oleks-netizen.github.io/product-images/18309/04.jpg,https://oleks-netizen.github.io/product-images/18309/05.jpg,https://oleks-netizen.github.io/product-images/18309/06.jpg</t>
         </is>
       </c>
       <c r="C161" t="n">
@@ -2846,7 +2846,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18327/1.jpg,https://oleks-netizen.github.io/product-images/18327/2.jpg,https://oleks-netizen.github.io/product-images/18327/9.jpg,https://oleks-netizen.github.io/product-images/18327/3.jpg,https://oleks-netizen.github.io/product-images/18327/4.jpg,https://oleks-netizen.github.io/product-images/18327/5.jpg,https://oleks-netizen.github.io/product-images/18327/7.jpg,https://oleks-netizen.github.io/product-images/18327/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18327/01.jpg,https://oleks-netizen.github.io/product-images/18327/02.jpg,https://oleks-netizen.github.io/product-images/18327/09.jpg,https://oleks-netizen.github.io/product-images/18327/03.jpg,https://oleks-netizen.github.io/product-images/18327/04.jpg,https://oleks-netizen.github.io/product-images/18327/05.jpg,https://oleks-netizen.github.io/product-images/18327/07.jpg,https://oleks-netizen.github.io/product-images/18327/08.jpg</t>
         </is>
       </c>
       <c r="C162" t="n">
@@ -2861,7 +2861,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18331/1.jpg,https://oleks-netizen.github.io/product-images/18331/2.jpg,https://oleks-netizen.github.io/product-images/18331/7.jpg,https://oleks-netizen.github.io/product-images/18331/3.jpg,https://oleks-netizen.github.io/product-images/18331/5.jpg,https://oleks-netizen.github.io/product-images/18331/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18331/01.jpg,https://oleks-netizen.github.io/product-images/18331/02.jpg,https://oleks-netizen.github.io/product-images/18331/07.jpg,https://oleks-netizen.github.io/product-images/18331/03.jpg,https://oleks-netizen.github.io/product-images/18331/05.jpg,https://oleks-netizen.github.io/product-images/18331/06.jpg</t>
         </is>
       </c>
       <c r="C163" t="n">
@@ -2876,7 +2876,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18345/1.jpg,https://oleks-netizen.github.io/product-images/18345/2.jpg,https://oleks-netizen.github.io/product-images/18345/9.jpg,https://oleks-netizen.github.io/product-images/18345/3.jpg,https://oleks-netizen.github.io/product-images/18345/4.jpg,https://oleks-netizen.github.io/product-images/18345/5.jpg,https://oleks-netizen.github.io/product-images/18345/7.jpg,https://oleks-netizen.github.io/product-images/18345/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18345/01.jpg,https://oleks-netizen.github.io/product-images/18345/02.jpg,https://oleks-netizen.github.io/product-images/18345/09.jpg,https://oleks-netizen.github.io/product-images/18345/03.jpg,https://oleks-netizen.github.io/product-images/18345/04.jpg,https://oleks-netizen.github.io/product-images/18345/05.jpg,https://oleks-netizen.github.io/product-images/18345/07.jpg,https://oleks-netizen.github.io/product-images/18345/08.jpg</t>
         </is>
       </c>
       <c r="C164" t="n">
@@ -2891,7 +2891,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18347/1.jpg,https://oleks-netizen.github.io/product-images/18347/2.jpg,https://oleks-netizen.github.io/product-images/18347/8.jpg,https://oleks-netizen.github.io/product-images/18347/3.jpg,https://oleks-netizen.github.io/product-images/18347/4.jpg,https://oleks-netizen.github.io/product-images/18347/5.jpg,https://oleks-netizen.github.io/product-images/18347/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18347/01.jpg,https://oleks-netizen.github.io/product-images/18347/02.jpg,https://oleks-netizen.github.io/product-images/18347/08.jpg,https://oleks-netizen.github.io/product-images/18347/03.jpg,https://oleks-netizen.github.io/product-images/18347/04.jpg,https://oleks-netizen.github.io/product-images/18347/05.jpg,https://oleks-netizen.github.io/product-images/18347/06.jpg</t>
         </is>
       </c>
       <c r="C165" t="n">
@@ -2906,7 +2906,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18376/1.jpg,https://oleks-netizen.github.io/product-images/18376/2.jpg,https://oleks-netizen.github.io/product-images/18376/8.jpg,https://oleks-netizen.github.io/product-images/18376/3.jpg,https://oleks-netizen.github.io/product-images/18376/4.jpg,https://oleks-netizen.github.io/product-images/18376/5.jpg,https://oleks-netizen.github.io/product-images/18376/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18376/01.jpg,https://oleks-netizen.github.io/product-images/18376/02.jpg,https://oleks-netizen.github.io/product-images/18376/08.jpg,https://oleks-netizen.github.io/product-images/18376/03.jpg,https://oleks-netizen.github.io/product-images/18376/04.jpg,https://oleks-netizen.github.io/product-images/18376/05.jpg,https://oleks-netizen.github.io/product-images/18376/07.jpg</t>
         </is>
       </c>
       <c r="C166" t="n">
@@ -2921,7 +2921,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18382/1.jpg,https://oleks-netizen.github.io/product-images/18382/2.jpg,https://oleks-netizen.github.io/product-images/18382/8.jpg,https://oleks-netizen.github.io/product-images/18382/3.jpg,https://oleks-netizen.github.io/product-images/18382/4.jpg,https://oleks-netizen.github.io/product-images/18382/5.jpg,https://oleks-netizen.github.io/product-images/18382/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18382/01.jpg,https://oleks-netizen.github.io/product-images/18382/02.jpg,https://oleks-netizen.github.io/product-images/18382/08.jpg,https://oleks-netizen.github.io/product-images/18382/03.jpg,https://oleks-netizen.github.io/product-images/18382/04.jpg,https://oleks-netizen.github.io/product-images/18382/05.jpg,https://oleks-netizen.github.io/product-images/18382/07.jpg</t>
         </is>
       </c>
       <c r="C167" t="n">
@@ -2936,7 +2936,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18398/1.jpg,https://oleks-netizen.github.io/product-images/18398/2.jpg,https://oleks-netizen.github.io/product-images/18398/7.jpg,https://oleks-netizen.github.io/product-images/18398/3.jpg,https://oleks-netizen.github.io/product-images/18398/4.jpg,https://oleks-netizen.github.io/product-images/18398/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18398/01.jpg,https://oleks-netizen.github.io/product-images/18398/02.jpg,https://oleks-netizen.github.io/product-images/18398/07.jpg,https://oleks-netizen.github.io/product-images/18398/03.jpg,https://oleks-netizen.github.io/product-images/18398/04.jpg,https://oleks-netizen.github.io/product-images/18398/05.jpg</t>
         </is>
       </c>
       <c r="C168" t="n">
@@ -2951,7 +2951,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18400/1.jpg,https://oleks-netizen.github.io/product-images/18400/2.jpg,https://oleks-netizen.github.io/product-images/18400/7.jpg,https://oleks-netizen.github.io/product-images/18400/4.jpg,https://oleks-netizen.github.io/product-images/18400/5.jpg,https://oleks-netizen.github.io/product-images/18400/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18400/01.jpg,https://oleks-netizen.github.io/product-images/18400/02.jpg,https://oleks-netizen.github.io/product-images/18400/07.jpg,https://oleks-netizen.github.io/product-images/18400/04.jpg,https://oleks-netizen.github.io/product-images/18400/05.jpg,https://oleks-netizen.github.io/product-images/18400/06.jpg</t>
         </is>
       </c>
       <c r="C169" t="n">
@@ -2966,7 +2966,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18404/1.jpg,https://oleks-netizen.github.io/product-images/18404/2.jpg,https://oleks-netizen.github.io/product-images/18404/6.jpg,https://oleks-netizen.github.io/product-images/18404/4.jpg,https://oleks-netizen.github.io/product-images/18404/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18404/01.jpg,https://oleks-netizen.github.io/product-images/18404/02.jpg,https://oleks-netizen.github.io/product-images/18404/06.jpg,https://oleks-netizen.github.io/product-images/18404/04.jpg,https://oleks-netizen.github.io/product-images/18404/05.jpg</t>
         </is>
       </c>
       <c r="C170" t="n">
@@ -2981,7 +2981,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18411/1.jpg,https://oleks-netizen.github.io/product-images/18411/2.jpg,https://oleks-netizen.github.io/product-images/18411/6.jpg,https://oleks-netizen.github.io/product-images/18411/4.jpg,https://oleks-netizen.github.io/product-images/18411/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18411/01.jpg,https://oleks-netizen.github.io/product-images/18411/02.jpg,https://oleks-netizen.github.io/product-images/18411/06.jpg,https://oleks-netizen.github.io/product-images/18411/04.jpg,https://oleks-netizen.github.io/product-images/18411/05.jpg</t>
         </is>
       </c>
       <c r="C171" t="n">
@@ -2996,7 +2996,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18483/1.jpg,https://oleks-netizen.github.io/product-images/18483/2.jpg,https://oleks-netizen.github.io/product-images/18483/8.jpg,https://oleks-netizen.github.io/product-images/18483/3.jpg,https://oleks-netizen.github.io/product-images/18483/4.jpg,https://oleks-netizen.github.io/product-images/18483/5.jpg,https://oleks-netizen.github.io/product-images/18483/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18483/01.jpg,https://oleks-netizen.github.io/product-images/18483/02.jpg,https://oleks-netizen.github.io/product-images/18483/08.jpg,https://oleks-netizen.github.io/product-images/18483/03.jpg,https://oleks-netizen.github.io/product-images/18483/04.jpg,https://oleks-netizen.github.io/product-images/18483/05.jpg,https://oleks-netizen.github.io/product-images/18483/07.jpg</t>
         </is>
       </c>
       <c r="C172" t="n">
@@ -3011,7 +3011,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18803/1.jpg,https://oleks-netizen.github.io/product-images/18803/2.jpg,https://oleks-netizen.github.io/product-images/18803/7.jpg,https://oleks-netizen.github.io/product-images/18803/3.jpg,https://oleks-netizen.github.io/product-images/18803/4.jpg,https://oleks-netizen.github.io/product-images/18803/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18803/01.jpg,https://oleks-netizen.github.io/product-images/18803/02.jpg,https://oleks-netizen.github.io/product-images/18803/07.jpg,https://oleks-netizen.github.io/product-images/18803/03.jpg,https://oleks-netizen.github.io/product-images/18803/04.jpg,https://oleks-netizen.github.io/product-images/18803/05.jpg</t>
         </is>
       </c>
       <c r="C173" t="n">
@@ -3026,7 +3026,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18813/1.jpg,https://oleks-netizen.github.io/product-images/18813/2.jpg,https://oleks-netizen.github.io/product-images/18813/11.jpg,https://oleks-netizen.github.io/product-images/18813/10.jpg,https://oleks-netizen.github.io/product-images/18813/3.jpg,https://oleks-netizen.github.io/product-images/18813/4.jpg,https://oleks-netizen.github.io/product-images/18813/5.jpg,https://oleks-netizen.github.io/product-images/18813/7.jpg,https://oleks-netizen.github.io/product-images/18813/8.jpg,https://oleks-netizen.github.io/product-images/18813/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18813/01.jpg,https://oleks-netizen.github.io/product-images/18813/02.jpg,https://oleks-netizen.github.io/product-images/18813/11.jpg,https://oleks-netizen.github.io/product-images/18813/10.jpg,https://oleks-netizen.github.io/product-images/18813/03.jpg,https://oleks-netizen.github.io/product-images/18813/04.jpg,https://oleks-netizen.github.io/product-images/18813/05.jpg,https://oleks-netizen.github.io/product-images/18813/07.jpg,https://oleks-netizen.github.io/product-images/18813/08.jpg,https://oleks-netizen.github.io/product-images/18813/09.jpg</t>
         </is>
       </c>
       <c r="C174" t="n">
@@ -3041,7 +3041,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18815/1.jpg,https://oleks-netizen.github.io/product-images/18815/2.jpg,https://oleks-netizen.github.io/product-images/18815/8.jpg,https://oleks-netizen.github.io/product-images/18815/3.jpg,https://oleks-netizen.github.io/product-images/18815/4.jpg,https://oleks-netizen.github.io/product-images/18815/5.jpg,https://oleks-netizen.github.io/product-images/18815/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18815/01.jpg,https://oleks-netizen.github.io/product-images/18815/02.jpg,https://oleks-netizen.github.io/product-images/18815/08.jpg,https://oleks-netizen.github.io/product-images/18815/03.jpg,https://oleks-netizen.github.io/product-images/18815/04.jpg,https://oleks-netizen.github.io/product-images/18815/05.jpg,https://oleks-netizen.github.io/product-images/18815/06.jpg</t>
         </is>
       </c>
       <c r="C175" t="n">
@@ -3056,7 +3056,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18822/1.jpg,https://oleks-netizen.github.io/product-images/18822/2.jpg,https://oleks-netizen.github.io/product-images/18822/10.jpg,https://oleks-netizen.github.io/product-images/18822/3.jpg,https://oleks-netizen.github.io/product-images/18822/4.jpg,https://oleks-netizen.github.io/product-images/18822/5.jpg,https://oleks-netizen.github.io/product-images/18822/6.jpg,https://oleks-netizen.github.io/product-images/18822/8.jpg,https://oleks-netizen.github.io/product-images/18822/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18822/01.jpg,https://oleks-netizen.github.io/product-images/18822/02.jpg,https://oleks-netizen.github.io/product-images/18822/10.jpg,https://oleks-netizen.github.io/product-images/18822/03.jpg,https://oleks-netizen.github.io/product-images/18822/04.jpg,https://oleks-netizen.github.io/product-images/18822/05.jpg,https://oleks-netizen.github.io/product-images/18822/06.jpg,https://oleks-netizen.github.io/product-images/18822/08.jpg,https://oleks-netizen.github.io/product-images/18822/09.jpg</t>
         </is>
       </c>
       <c r="C176" t="n">
@@ -3071,7 +3071,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18825/1.jpg,https://oleks-netizen.github.io/product-images/18825/2.jpg,https://oleks-netizen.github.io/product-images/18825/9.jpg,https://oleks-netizen.github.io/product-images/18825/3.jpg,https://oleks-netizen.github.io/product-images/18825/4.jpg,https://oleks-netizen.github.io/product-images/18825/5.jpg,https://oleks-netizen.github.io/product-images/18825/7.jpg,https://oleks-netizen.github.io/product-images/18825/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18825/01.jpg,https://oleks-netizen.github.io/product-images/18825/02.jpg,https://oleks-netizen.github.io/product-images/18825/09.jpg,https://oleks-netizen.github.io/product-images/18825/03.jpg,https://oleks-netizen.github.io/product-images/18825/04.jpg,https://oleks-netizen.github.io/product-images/18825/05.jpg,https://oleks-netizen.github.io/product-images/18825/07.jpg,https://oleks-netizen.github.io/product-images/18825/08.jpg</t>
         </is>
       </c>
       <c r="C177" t="n">
@@ -3086,7 +3086,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18831/1.jpg,https://oleks-netizen.github.io/product-images/18831/2.jpg,https://oleks-netizen.github.io/product-images/18831/7.jpg,https://oleks-netizen.github.io/product-images/18831/3.jpg,https://oleks-netizen.github.io/product-images/18831/4.jpg,https://oleks-netizen.github.io/product-images/18831/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18831/01.jpg,https://oleks-netizen.github.io/product-images/18831/02.jpg,https://oleks-netizen.github.io/product-images/18831/07.jpg,https://oleks-netizen.github.io/product-images/18831/03.jpg,https://oleks-netizen.github.io/product-images/18831/04.jpg,https://oleks-netizen.github.io/product-images/18831/05.jpg</t>
         </is>
       </c>
       <c r="C178" t="n">
@@ -3101,7 +3101,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18836/1.jpg,https://oleks-netizen.github.io/product-images/18836/2.jpg,https://oleks-netizen.github.io/product-images/18836/7.jpg,https://oleks-netizen.github.io/product-images/18836/3.jpg,https://oleks-netizen.github.io/product-images/18836/4.jpg,https://oleks-netizen.github.io/product-images/18836/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18836/01.jpg,https://oleks-netizen.github.io/product-images/18836/02.jpg,https://oleks-netizen.github.io/product-images/18836/07.jpg,https://oleks-netizen.github.io/product-images/18836/03.jpg,https://oleks-netizen.github.io/product-images/18836/04.jpg,https://oleks-netizen.github.io/product-images/18836/06.jpg</t>
         </is>
       </c>
       <c r="C179" t="n">
@@ -3116,7 +3116,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18837/1.jpg,https://oleks-netizen.github.io/product-images/18837/2.jpg,https://oleks-netizen.github.io/product-images/18837/9.jpg,https://oleks-netizen.github.io/product-images/18837/3.jpg,https://oleks-netizen.github.io/product-images/18837/4.jpg,https://oleks-netizen.github.io/product-images/18837/5.jpg,https://oleks-netizen.github.io/product-images/18837/6.jpg,https://oleks-netizen.github.io/product-images/18837/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18837/01.jpg,https://oleks-netizen.github.io/product-images/18837/02.jpg,https://oleks-netizen.github.io/product-images/18837/09.jpg,https://oleks-netizen.github.io/product-images/18837/03.jpg,https://oleks-netizen.github.io/product-images/18837/04.jpg,https://oleks-netizen.github.io/product-images/18837/05.jpg,https://oleks-netizen.github.io/product-images/18837/06.jpg,https://oleks-netizen.github.io/product-images/18837/08.jpg</t>
         </is>
       </c>
       <c r="C180" t="n">
@@ -3131,7 +3131,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18840/1.jpg,https://oleks-netizen.github.io/product-images/18840/2.jpg,https://oleks-netizen.github.io/product-images/18840/7.jpg,https://oleks-netizen.github.io/product-images/18840/3.jpg,https://oleks-netizen.github.io/product-images/18840/4.jpg,https://oleks-netizen.github.io/product-images/18840/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18840/01.jpg,https://oleks-netizen.github.io/product-images/18840/02.jpg,https://oleks-netizen.github.io/product-images/18840/07.jpg,https://oleks-netizen.github.io/product-images/18840/03.jpg,https://oleks-netizen.github.io/product-images/18840/04.jpg,https://oleks-netizen.github.io/product-images/18840/05.jpg</t>
         </is>
       </c>
       <c r="C181" t="n">
@@ -3146,7 +3146,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18867/1.jpg,https://oleks-netizen.github.io/product-images/18867/2.jpg,https://oleks-netizen.github.io/product-images/18867/7.jpg,https://oleks-netizen.github.io/product-images/18867/3.jpg,https://oleks-netizen.github.io/product-images/18867/4.jpg,https://oleks-netizen.github.io/product-images/18867/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18867/01.jpg,https://oleks-netizen.github.io/product-images/18867/02.jpg,https://oleks-netizen.github.io/product-images/18867/07.jpg,https://oleks-netizen.github.io/product-images/18867/03.jpg,https://oleks-netizen.github.io/product-images/18867/04.jpg,https://oleks-netizen.github.io/product-images/18867/05.jpg</t>
         </is>
       </c>
       <c r="C182" t="n">
@@ -3161,7 +3161,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18870/1.jpg,https://oleks-netizen.github.io/product-images/18870/2.jpg,https://oleks-netizen.github.io/product-images/18870/9.jpg,https://oleks-netizen.github.io/product-images/18870/3.jpg,https://oleks-netizen.github.io/product-images/18870/4.jpg,https://oleks-netizen.github.io/product-images/18870/5.jpg,https://oleks-netizen.github.io/product-images/18870/6.jpg,https://oleks-netizen.github.io/product-images/18870/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18870/01.jpg,https://oleks-netizen.github.io/product-images/18870/02.jpg,https://oleks-netizen.github.io/product-images/18870/09.jpg,https://oleks-netizen.github.io/product-images/18870/03.jpg,https://oleks-netizen.github.io/product-images/18870/04.jpg,https://oleks-netizen.github.io/product-images/18870/05.jpg,https://oleks-netizen.github.io/product-images/18870/06.jpg,https://oleks-netizen.github.io/product-images/18870/08.jpg</t>
         </is>
       </c>
       <c r="C183" t="n">
@@ -3176,7 +3176,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18871/1.jpg,https://oleks-netizen.github.io/product-images/18871/2.jpg,https://oleks-netizen.github.io/product-images/18871/7.jpg,https://oleks-netizen.github.io/product-images/18871/3.jpg,https://oleks-netizen.github.io/product-images/18871/4.jpg,https://oleks-netizen.github.io/product-images/18871/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18871/01.jpg,https://oleks-netizen.github.io/product-images/18871/02.jpg,https://oleks-netizen.github.io/product-images/18871/07.jpg,https://oleks-netizen.github.io/product-images/18871/03.jpg,https://oleks-netizen.github.io/product-images/18871/04.jpg,https://oleks-netizen.github.io/product-images/18871/06.jpg</t>
         </is>
       </c>
       <c r="C184" t="n">
@@ -3191,7 +3191,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18877/1.jpg,https://oleks-netizen.github.io/product-images/18877/2.jpg,https://oleks-netizen.github.io/product-images/18877/9.jpg,https://oleks-netizen.github.io/product-images/18877/3.jpg,https://oleks-netizen.github.io/product-images/18877/4.jpg,https://oleks-netizen.github.io/product-images/18877/5.jpg,https://oleks-netizen.github.io/product-images/18877/6.jpg,https://oleks-netizen.github.io/product-images/18877/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18877/01.jpg,https://oleks-netizen.github.io/product-images/18877/02.jpg,https://oleks-netizen.github.io/product-images/18877/09.jpg,https://oleks-netizen.github.io/product-images/18877/03.jpg,https://oleks-netizen.github.io/product-images/18877/04.jpg,https://oleks-netizen.github.io/product-images/18877/05.jpg,https://oleks-netizen.github.io/product-images/18877/06.jpg,https://oleks-netizen.github.io/product-images/18877/08.jpg</t>
         </is>
       </c>
       <c r="C185" t="n">
@@ -3206,7 +3206,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18959/1.jpg,https://oleks-netizen.github.io/product-images/18959/2.jpg,https://oleks-netizen.github.io/product-images/18959/7.jpg,https://oleks-netizen.github.io/product-images/18959/3.jpg,https://oleks-netizen.github.io/product-images/18959/4.jpg,https://oleks-netizen.github.io/product-images/18959/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18959/01.jpg,https://oleks-netizen.github.io/product-images/18959/02.jpg,https://oleks-netizen.github.io/product-images/18959/07.jpg,https://oleks-netizen.github.io/product-images/18959/03.jpg,https://oleks-netizen.github.io/product-images/18959/04.jpg,https://oleks-netizen.github.io/product-images/18959/05.jpg</t>
         </is>
       </c>
       <c r="C186" t="n">
@@ -3221,7 +3221,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/18966/1.jpg,https://oleks-netizen.github.io/product-images/18966/2.jpg,https://oleks-netizen.github.io/product-images/18966/6.jpg,https://oleks-netizen.github.io/product-images/18966/4.jpg,https://oleks-netizen.github.io/product-images/18966/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/18966/01.jpg,https://oleks-netizen.github.io/product-images/18966/02.jpg,https://oleks-netizen.github.io/product-images/18966/06.jpg,https://oleks-netizen.github.io/product-images/18966/04.jpg,https://oleks-netizen.github.io/product-images/18966/05.jpg</t>
         </is>
       </c>
       <c r="C187" t="n">
@@ -3236,7 +3236,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/19016/1.jpg,https://oleks-netizen.github.io/product-images/19016/2.jpg,https://oleks-netizen.github.io/product-images/19016/6.jpg,https://oleks-netizen.github.io/product-images/19016/3.jpg,https://oleks-netizen.github.io/product-images/19016/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/19016/01.jpg,https://oleks-netizen.github.io/product-images/19016/02.jpg,https://oleks-netizen.github.io/product-images/19016/06.jpg,https://oleks-netizen.github.io/product-images/19016/03.jpg,https://oleks-netizen.github.io/product-images/19016/05.jpg</t>
         </is>
       </c>
       <c r="C188" t="n">
@@ -3251,7 +3251,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/19049/1.jpg,https://oleks-netizen.github.io/product-images/19049/2.jpg,https://oleks-netizen.github.io/product-images/19049/6.jpg,https://oleks-netizen.github.io/product-images/19049/4.jpg,https://oleks-netizen.github.io/product-images/19049/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/19049/01.jpg,https://oleks-netizen.github.io/product-images/19049/02.jpg,https://oleks-netizen.github.io/product-images/19049/06.jpg,https://oleks-netizen.github.io/product-images/19049/04.jpg,https://oleks-netizen.github.io/product-images/19049/05.jpg</t>
         </is>
       </c>
       <c r="C189" t="n">
@@ -3266,7 +3266,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/19058/1.jpg,https://oleks-netizen.github.io/product-images/19058/2.jpg,https://oleks-netizen.github.io/product-images/19058/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/19058/01.jpg,https://oleks-netizen.github.io/product-images/19058/02.jpg,https://oleks-netizen.github.io/product-images/19058/03.jpg</t>
         </is>
       </c>
       <c r="C190" t="n">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/19061/1.jpg,https://oleks-netizen.github.io/product-images/19061/2.jpg,https://oleks-netizen.github.io/product-images/19061/3.jpg,https://oleks-netizen.github.io/product-images/19061/4.jpg,https://oleks-netizen.github.io/product-images/19061/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/19061/01.jpg,https://oleks-netizen.github.io/product-images/19061/02.jpg,https://oleks-netizen.github.io/product-images/19061/03.jpg,https://oleks-netizen.github.io/product-images/19061/04.jpg,https://oleks-netizen.github.io/product-images/19061/05.jpg</t>
         </is>
       </c>
       <c r="C191" t="n">
@@ -3296,7 +3296,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/19082/1.jpg,https://oleks-netizen.github.io/product-images/19082/2.jpg,https://oleks-netizen.github.io/product-images/19082/3.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/19082/01.jpg,https://oleks-netizen.github.io/product-images/19082/02.jpg,https://oleks-netizen.github.io/product-images/19082/03.jpg</t>
         </is>
       </c>
       <c r="C192" t="n">
@@ -3311,7 +3311,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20040/1.jpg,https://oleks-netizen.github.io/product-images/20040/2.jpg,https://oleks-netizen.github.io/product-images/20040/3.jpg,https://oleks-netizen.github.io/product-images/20040/11.jpg,https://oleks-netizen.github.io/product-images/20040/10.jpg,https://oleks-netizen.github.io/product-images/20040/4.jpg,https://oleks-netizen.github.io/product-images/20040/5.jpg,https://oleks-netizen.github.io/product-images/20040/6.jpg,https://oleks-netizen.github.io/product-images/20040/8.jpg,https://oleks-netizen.github.io/product-images/20040/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20040/01.jpg,https://oleks-netizen.github.io/product-images/20040/02.jpg,https://oleks-netizen.github.io/product-images/20040/03.jpg,https://oleks-netizen.github.io/product-images/20040/11.jpg,https://oleks-netizen.github.io/product-images/20040/10.jpg,https://oleks-netizen.github.io/product-images/20040/04.jpg,https://oleks-netizen.github.io/product-images/20040/05.jpg,https://oleks-netizen.github.io/product-images/20040/06.jpg,https://oleks-netizen.github.io/product-images/20040/08.jpg,https://oleks-netizen.github.io/product-images/20040/09.jpg</t>
         </is>
       </c>
       <c r="C193" t="n">
@@ -3326,7 +3326,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20041/1.jpg,https://oleks-netizen.github.io/product-images/20041/2.jpg,https://oleks-netizen.github.io/product-images/20041/3.jpg,https://oleks-netizen.github.io/product-images/20041/4.jpg,https://oleks-netizen.github.io/product-images/20041/5.jpg,https://oleks-netizen.github.io/product-images/20041/6.jpg,https://oleks-netizen.github.io/product-images/20041/7.jpg,https://oleks-netizen.github.io/product-images/20041/8.jpg,https://oleks-netizen.github.io/product-images/20041/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20041/01.jpg,https://oleks-netizen.github.io/product-images/20041/02.jpg,https://oleks-netizen.github.io/product-images/20041/03.jpg,https://oleks-netizen.github.io/product-images/20041/04.jpg,https://oleks-netizen.github.io/product-images/20041/05.jpg,https://oleks-netizen.github.io/product-images/20041/06.jpg,https://oleks-netizen.github.io/product-images/20041/07.jpg,https://oleks-netizen.github.io/product-images/20041/08.jpg,https://oleks-netizen.github.io/product-images/20041/09.jpg</t>
         </is>
       </c>
       <c r="C194" t="n">
@@ -3341,7 +3341,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20042/1.jpg,https://oleks-netizen.github.io/product-images/20042/2.jpg,https://oleks-netizen.github.io/product-images/20042/17.jpg,https://oleks-netizen.github.io/product-images/20042/10.jpg,https://oleks-netizen.github.io/product-images/20042/11.jpg,https://oleks-netizen.github.io/product-images/20042/12.jpg,https://oleks-netizen.github.io/product-images/20042/13.jpg,https://oleks-netizen.github.io/product-images/20042/14.jpg,https://oleks-netizen.github.io/product-images/20042/15.jpg,https://oleks-netizen.github.io/product-images/20042/16.jpg,https://oleks-netizen.github.io/product-images/20042/4.jpg,https://oleks-netizen.github.io/product-images/20042/5.jpg,https://oleks-netizen.github.io/product-images/20042/6.jpg,https://oleks-netizen.github.io/product-images/20042/7.jpg,https://oleks-netizen.github.io/product-images/20042/8.jpg,https://oleks-netizen.github.io/product-images/20042/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20042/01.jpg,https://oleks-netizen.github.io/product-images/20042/02.jpg,https://oleks-netizen.github.io/product-images/20042/17.jpg,https://oleks-netizen.github.io/product-images/20042/10.jpg,https://oleks-netizen.github.io/product-images/20042/11.jpg,https://oleks-netizen.github.io/product-images/20042/12.jpg,https://oleks-netizen.github.io/product-images/20042/13.jpg,https://oleks-netizen.github.io/product-images/20042/14.jpg,https://oleks-netizen.github.io/product-images/20042/15.jpg,https://oleks-netizen.github.io/product-images/20042/16.jpg,https://oleks-netizen.github.io/product-images/20042/04.jpg,https://oleks-netizen.github.io/product-images/20042/05.jpg,https://oleks-netizen.github.io/product-images/20042/06.jpg,https://oleks-netizen.github.io/product-images/20042/07.jpg,https://oleks-netizen.github.io/product-images/20042/08.jpg,https://oleks-netizen.github.io/product-images/20042/09.jpg</t>
         </is>
       </c>
       <c r="C195" t="n">
@@ -3356,7 +3356,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20047/1.jpg,https://oleks-netizen.github.io/product-images/20047/2.jpg,https://oleks-netizen.github.io/product-images/20047/14.jpg,https://oleks-netizen.github.io/product-images/20047/10.jpg,https://oleks-netizen.github.io/product-images/20047/11.jpg,https://oleks-netizen.github.io/product-images/20047/12.jpg,https://oleks-netizen.github.io/product-images/20047/13.jpg,https://oleks-netizen.github.io/product-images/20047/3.jpg,https://oleks-netizen.github.io/product-images/20047/4.jpg,https://oleks-netizen.github.io/product-images/20047/5.jpg,https://oleks-netizen.github.io/product-images/20047/7.jpg,https://oleks-netizen.github.io/product-images/20047/8.jpg,https://oleks-netizen.github.io/product-images/20047/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20047/01.jpg,https://oleks-netizen.github.io/product-images/20047/02.jpg,https://oleks-netizen.github.io/product-images/20047/14.jpg,https://oleks-netizen.github.io/product-images/20047/10.jpg,https://oleks-netizen.github.io/product-images/20047/11.jpg,https://oleks-netizen.github.io/product-images/20047/12.jpg,https://oleks-netizen.github.io/product-images/20047/13.jpg,https://oleks-netizen.github.io/product-images/20047/03.jpg,https://oleks-netizen.github.io/product-images/20047/04.jpg,https://oleks-netizen.github.io/product-images/20047/05.jpg,https://oleks-netizen.github.io/product-images/20047/07.jpg,https://oleks-netizen.github.io/product-images/20047/08.jpg,https://oleks-netizen.github.io/product-images/20047/09.jpg</t>
         </is>
       </c>
       <c r="C196" t="n">
@@ -3371,7 +3371,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20069/10.jpg,https://oleks-netizen.github.io/product-images/20069/11.jpg,https://oleks-netizen.github.io/product-images/20069/12.jpg,https://oleks-netizen.github.io/product-images/20069/1.jpg,https://oleks-netizen.github.io/product-images/20069/2.jpg,https://oleks-netizen.github.io/product-images/20069/3.jpg,https://oleks-netizen.github.io/product-images/20069/4.jpg,https://oleks-netizen.github.io/product-images/20069/5.jpg,https://oleks-netizen.github.io/product-images/20069/6.jpg,https://oleks-netizen.github.io/product-images/20069/7.jpg,https://oleks-netizen.github.io/product-images/20069/8.jpg,https://oleks-netizen.github.io/product-images/20069/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20069/10.jpg,https://oleks-netizen.github.io/product-images/20069/11.jpg,https://oleks-netizen.github.io/product-images/20069/12.jpg,https://oleks-netizen.github.io/product-images/20069/01.jpg,https://oleks-netizen.github.io/product-images/20069/02.jpg,https://oleks-netizen.github.io/product-images/20069/03.jpg,https://oleks-netizen.github.io/product-images/20069/04.jpg,https://oleks-netizen.github.io/product-images/20069/05.jpg,https://oleks-netizen.github.io/product-images/20069/06.jpg,https://oleks-netizen.github.io/product-images/20069/07.jpg,https://oleks-netizen.github.io/product-images/20069/08.jpg,https://oleks-netizen.github.io/product-images/20069/09.jpg</t>
         </is>
       </c>
       <c r="C197" t="n">
@@ -3386,7 +3386,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20075/1.jpg,https://oleks-netizen.github.io/product-images/20075/2.jpg,https://oleks-netizen.github.io/product-images/20075/11.jpg,https://oleks-netizen.github.io/product-images/20075/13.jpg,https://oleks-netizen.github.io/product-images/20075/12.jpg,https://oleks-netizen.github.io/product-images/20075/3.jpg,https://oleks-netizen.github.io/product-images/20075/4.jpg,https://oleks-netizen.github.io/product-images/20075/5.jpg,https://oleks-netizen.github.io/product-images/20075/6.jpg,https://oleks-netizen.github.io/product-images/20075/7.jpg,https://oleks-netizen.github.io/product-images/20075/8.jpg,https://oleks-netizen.github.io/product-images/20075/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20075/01.jpg,https://oleks-netizen.github.io/product-images/20075/02.jpg,https://oleks-netizen.github.io/product-images/20075/11.jpg,https://oleks-netizen.github.io/product-images/20075/13.jpg,https://oleks-netizen.github.io/product-images/20075/12.jpg,https://oleks-netizen.github.io/product-images/20075/03.jpg,https://oleks-netizen.github.io/product-images/20075/04.jpg,https://oleks-netizen.github.io/product-images/20075/05.jpg,https://oleks-netizen.github.io/product-images/20075/06.jpg,https://oleks-netizen.github.io/product-images/20075/07.jpg,https://oleks-netizen.github.io/product-images/20075/08.jpg,https://oleks-netizen.github.io/product-images/20075/09.jpg</t>
         </is>
       </c>
       <c r="C198" t="n">
@@ -3401,7 +3401,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20080/1.jpg,https://oleks-netizen.github.io/product-images/20080/2.jpg,https://oleks-netizen.github.io/product-images/20080/6.jpg,https://oleks-netizen.github.io/product-images/20080/8.jpg,https://oleks-netizen.github.io/product-images/20080/3.jpg,https://oleks-netizen.github.io/product-images/20080/4.jpg,https://oleks-netizen.github.io/product-images/20080/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20080/01.jpg,https://oleks-netizen.github.io/product-images/20080/02.jpg,https://oleks-netizen.github.io/product-images/20080/06.jpg,https://oleks-netizen.github.io/product-images/20080/08.jpg,https://oleks-netizen.github.io/product-images/20080/03.jpg,https://oleks-netizen.github.io/product-images/20080/04.jpg,https://oleks-netizen.github.io/product-images/20080/05.jpg</t>
         </is>
       </c>
       <c r="C199" t="n">
@@ -3416,7 +3416,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20083/1.jpg,https://oleks-netizen.github.io/product-images/20083/2.jpg,https://oleks-netizen.github.io/product-images/20083/13.jpg,https://oleks-netizen.github.io/product-images/20083/10.jpg,https://oleks-netizen.github.io/product-images/20083/11.jpg,https://oleks-netizen.github.io/product-images/20083/12.jpg,https://oleks-netizen.github.io/product-images/20083/3.jpg,https://oleks-netizen.github.io/product-images/20083/4.jpg,https://oleks-netizen.github.io/product-images/20083/5.jpg,https://oleks-netizen.github.io/product-images/20083/6.jpg,https://oleks-netizen.github.io/product-images/20083/7.jpg,https://oleks-netizen.github.io/product-images/20083/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20083/01.jpg,https://oleks-netizen.github.io/product-images/20083/02.jpg,https://oleks-netizen.github.io/product-images/20083/13.jpg,https://oleks-netizen.github.io/product-images/20083/10.jpg,https://oleks-netizen.github.io/product-images/20083/11.jpg,https://oleks-netizen.github.io/product-images/20083/12.jpg,https://oleks-netizen.github.io/product-images/20083/03.jpg,https://oleks-netizen.github.io/product-images/20083/04.jpg,https://oleks-netizen.github.io/product-images/20083/05.jpg,https://oleks-netizen.github.io/product-images/20083/06.jpg,https://oleks-netizen.github.io/product-images/20083/07.jpg,https://oleks-netizen.github.io/product-images/20083/08.jpg</t>
         </is>
       </c>
       <c r="C200" t="n">
@@ -3431,7 +3431,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20084/1.jpg,https://oleks-netizen.github.io/product-images/20084/2.jpg,https://oleks-netizen.github.io/product-images/20084/3.jpg,https://oleks-netizen.github.io/product-images/20084/4.jpg,https://oleks-netizen.github.io/product-images/20084/5.jpg,https://oleks-netizen.github.io/product-images/20084/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20084/01.jpg,https://oleks-netizen.github.io/product-images/20084/02.jpg,https://oleks-netizen.github.io/product-images/20084/03.jpg,https://oleks-netizen.github.io/product-images/20084/04.jpg,https://oleks-netizen.github.io/product-images/20084/05.jpg,https://oleks-netizen.github.io/product-images/20084/06.jpg</t>
         </is>
       </c>
       <c r="C201" t="n">
@@ -3446,7 +3446,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20121/1.jpg,https://oleks-netizen.github.io/product-images/20121/2.jpg,https://oleks-netizen.github.io/product-images/20121/8.jpg,https://oleks-netizen.github.io/product-images/20121/3.jpg,https://oleks-netizen.github.io/product-images/20121/4.jpg,https://oleks-netizen.github.io/product-images/20121/5.jpg,https://oleks-netizen.github.io/product-images/20121/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20121/01.jpg,https://oleks-netizen.github.io/product-images/20121/02.jpg,https://oleks-netizen.github.io/product-images/20121/08.jpg,https://oleks-netizen.github.io/product-images/20121/03.jpg,https://oleks-netizen.github.io/product-images/20121/04.jpg,https://oleks-netizen.github.io/product-images/20121/05.jpg,https://oleks-netizen.github.io/product-images/20121/06.jpg</t>
         </is>
       </c>
       <c r="C202" t="n">
@@ -3461,7 +3461,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20126/1.jpg,https://oleks-netizen.github.io/product-images/20126/2.jpg,https://oleks-netizen.github.io/product-images/20126/3.jpg,https://oleks-netizen.github.io/product-images/20126/4.jpg,https://oleks-netizen.github.io/product-images/20126/5.jpg,https://oleks-netizen.github.io/product-images/20126/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20126/01.jpg,https://oleks-netizen.github.io/product-images/20126/02.jpg,https://oleks-netizen.github.io/product-images/20126/03.jpg,https://oleks-netizen.github.io/product-images/20126/04.jpg,https://oleks-netizen.github.io/product-images/20126/05.jpg,https://oleks-netizen.github.io/product-images/20126/06.jpg</t>
         </is>
       </c>
       <c r="C203" t="n">
@@ -3476,7 +3476,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20131/1.jpg,https://oleks-netizen.github.io/product-images/20131/2.jpg,https://oleks-netizen.github.io/product-images/20131/3.jpg,https://oleks-netizen.github.io/product-images/20131/4.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20131/01.jpg,https://oleks-netizen.github.io/product-images/20131/02.jpg,https://oleks-netizen.github.io/product-images/20131/03.jpg,https://oleks-netizen.github.io/product-images/20131/04.jpg</t>
         </is>
       </c>
       <c r="C204" t="n">
@@ -3491,7 +3491,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20136/1.jpg,https://oleks-netizen.github.io/product-images/20136/2.jpg,https://oleks-netizen.github.io/product-images/20136/7.jpg,https://oleks-netizen.github.io/product-images/20136/3.jpg,https://oleks-netizen.github.io/product-images/20136/4.jpg,https://oleks-netizen.github.io/product-images/20136/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20136/01.jpg,https://oleks-netizen.github.io/product-images/20136/02.jpg,https://oleks-netizen.github.io/product-images/20136/07.jpg,https://oleks-netizen.github.io/product-images/20136/03.jpg,https://oleks-netizen.github.io/product-images/20136/04.jpg,https://oleks-netizen.github.io/product-images/20136/05.jpg</t>
         </is>
       </c>
       <c r="C205" t="n">
@@ -3506,7 +3506,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20193/1.jpg,https://oleks-netizen.github.io/product-images/20193/2.jpg,https://oleks-netizen.github.io/product-images/20193/3.jpg,https://oleks-netizen.github.io/product-images/20193/4.jpg,https://oleks-netizen.github.io/product-images/20193/5.jpg,https://oleks-netizen.github.io/product-images/20193/6.jpg,https://oleks-netizen.github.io/product-images/20193/7.jpg,https://oleks-netizen.github.io/product-images/20193/8.jpg,https://oleks-netizen.github.io/product-images/20193/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20193/01.jpg,https://oleks-netizen.github.io/product-images/20193/02.jpg,https://oleks-netizen.github.io/product-images/20193/03.jpg,https://oleks-netizen.github.io/product-images/20193/04.jpg,https://oleks-netizen.github.io/product-images/20193/05.jpg,https://oleks-netizen.github.io/product-images/20193/06.jpg,https://oleks-netizen.github.io/product-images/20193/07.jpg,https://oleks-netizen.github.io/product-images/20193/08.jpg,https://oleks-netizen.github.io/product-images/20193/09.jpg</t>
         </is>
       </c>
       <c r="C206" t="n">
@@ -3521,7 +3521,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20218/1.jpg,https://oleks-netizen.github.io/product-images/20218/2.jpg,https://oleks-netizen.github.io/product-images/20218/3.jpg,https://oleks-netizen.github.io/product-images/20218/4.jpg,https://oleks-netizen.github.io/product-images/20218/5.jpg,https://oleks-netizen.github.io/product-images/20218/6.jpg,https://oleks-netizen.github.io/product-images/20218/7.jpg,https://oleks-netizen.github.io/product-images/20218/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20218/01.jpg,https://oleks-netizen.github.io/product-images/20218/02.jpg,https://oleks-netizen.github.io/product-images/20218/03.jpg,https://oleks-netizen.github.io/product-images/20218/04.jpg,https://oleks-netizen.github.io/product-images/20218/05.jpg,https://oleks-netizen.github.io/product-images/20218/06.jpg,https://oleks-netizen.github.io/product-images/20218/07.jpg,https://oleks-netizen.github.io/product-images/20218/08.jpg</t>
         </is>
       </c>
       <c r="C207" t="n">
@@ -3536,7 +3536,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20221/1.jpg,https://oleks-netizen.github.io/product-images/20221/2.jpg,https://oleks-netizen.github.io/product-images/20221/3.jpg,https://oleks-netizen.github.io/product-images/20221/4.jpg,https://oleks-netizen.github.io/product-images/20221/5.jpg,https://oleks-netizen.github.io/product-images/20221/6.jpg,https://oleks-netizen.github.io/product-images/20221/7.jpg,https://oleks-netizen.github.io/product-images/20221/8.jpg,https://oleks-netizen.github.io/product-images/20221/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20221/01.jpg,https://oleks-netizen.github.io/product-images/20221/02.jpg,https://oleks-netizen.github.io/product-images/20221/03.jpg,https://oleks-netizen.github.io/product-images/20221/04.jpg,https://oleks-netizen.github.io/product-images/20221/05.jpg,https://oleks-netizen.github.io/product-images/20221/06.jpg,https://oleks-netizen.github.io/product-images/20221/07.jpg,https://oleks-netizen.github.io/product-images/20221/08.jpg,https://oleks-netizen.github.io/product-images/20221/09.jpg</t>
         </is>
       </c>
       <c r="C208" t="n">
@@ -3551,7 +3551,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20222/10.jpg,https://oleks-netizen.github.io/product-images/20222/11.jpg,https://oleks-netizen.github.io/product-images/20222/1.jpg,https://oleks-netizen.github.io/product-images/20222/2.jpg,https://oleks-netizen.github.io/product-images/20222/3.jpg,https://oleks-netizen.github.io/product-images/20222/4.jpg,https://oleks-netizen.github.io/product-images/20222/5.jpg,https://oleks-netizen.github.io/product-images/20222/6.jpg,https://oleks-netizen.github.io/product-images/20222/7.jpg,https://oleks-netizen.github.io/product-images/20222/8.jpg,https://oleks-netizen.github.io/product-images/20222/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20222/10.jpg,https://oleks-netizen.github.io/product-images/20222/11.jpg,https://oleks-netizen.github.io/product-images/20222/01.jpg,https://oleks-netizen.github.io/product-images/20222/02.jpg,https://oleks-netizen.github.io/product-images/20222/03.jpg,https://oleks-netizen.github.io/product-images/20222/04.jpg,https://oleks-netizen.github.io/product-images/20222/05.jpg,https://oleks-netizen.github.io/product-images/20222/06.jpg,https://oleks-netizen.github.io/product-images/20222/07.jpg,https://oleks-netizen.github.io/product-images/20222/08.jpg,https://oleks-netizen.github.io/product-images/20222/09.jpg</t>
         </is>
       </c>
       <c r="C209" t="n">
@@ -3566,7 +3566,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20231/1.jpg,https://oleks-netizen.github.io/product-images/20231/2.jpg,https://oleks-netizen.github.io/product-images/20231/8.jpg,https://oleks-netizen.github.io/product-images/20231/10.jpg,https://oleks-netizen.github.io/product-images/20231/3.jpg,https://oleks-netizen.github.io/product-images/20231/4.jpg,https://oleks-netizen.github.io/product-images/20231/5.jpg,https://oleks-netizen.github.io/product-images/20231/6.jpg,https://oleks-netizen.github.io/product-images/20231/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20231/01.jpg,https://oleks-netizen.github.io/product-images/20231/02.jpg,https://oleks-netizen.github.io/product-images/20231/08.jpg,https://oleks-netizen.github.io/product-images/20231/10.jpg,https://oleks-netizen.github.io/product-images/20231/03.jpg,https://oleks-netizen.github.io/product-images/20231/04.jpg,https://oleks-netizen.github.io/product-images/20231/05.jpg,https://oleks-netizen.github.io/product-images/20231/06.jpg,https://oleks-netizen.github.io/product-images/20231/07.jpg</t>
         </is>
       </c>
       <c r="C210" t="n">
@@ -3581,7 +3581,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20237/1.jpg,https://oleks-netizen.github.io/product-images/20237/2.jpg,https://oleks-netizen.github.io/product-images/20237/7.jpg,https://oleks-netizen.github.io/product-images/20237/11.jpg,https://oleks-netizen.github.io/product-images/20237/10.jpg,https://oleks-netizen.github.io/product-images/20237/3.jpg,https://oleks-netizen.github.io/product-images/20237/4.jpg,https://oleks-netizen.github.io/product-images/20237/6.jpg,https://oleks-netizen.github.io/product-images/20237/8.jpg,https://oleks-netizen.github.io/product-images/20237/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20237/01.jpg,https://oleks-netizen.github.io/product-images/20237/02.jpg,https://oleks-netizen.github.io/product-images/20237/07.jpg,https://oleks-netizen.github.io/product-images/20237/11.jpg,https://oleks-netizen.github.io/product-images/20237/10.jpg,https://oleks-netizen.github.io/product-images/20237/03.jpg,https://oleks-netizen.github.io/product-images/20237/04.jpg,https://oleks-netizen.github.io/product-images/20237/06.jpg,https://oleks-netizen.github.io/product-images/20237/08.jpg,https://oleks-netizen.github.io/product-images/20237/09.jpg</t>
         </is>
       </c>
       <c r="C211" t="n">
@@ -3596,7 +3596,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20238/1.jpg,https://oleks-netizen.github.io/product-images/20238/2.jpg,https://oleks-netizen.github.io/product-images/20238/13.jpg,https://oleks-netizen.github.io/product-images/20238/11.jpg,https://oleks-netizen.github.io/product-images/20238/12.jpg,https://oleks-netizen.github.io/product-images/20238/3.jpg,https://oleks-netizen.github.io/product-images/20238/4.jpg,https://oleks-netizen.github.io/product-images/20238/5.jpg,https://oleks-netizen.github.io/product-images/20238/6.jpg,https://oleks-netizen.github.io/product-images/20238/7.jpg,https://oleks-netizen.github.io/product-images/20238/8.jpg,https://oleks-netizen.github.io/product-images/20238/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20238/01.jpg,https://oleks-netizen.github.io/product-images/20238/02.jpg,https://oleks-netizen.github.io/product-images/20238/13.jpg,https://oleks-netizen.github.io/product-images/20238/11.jpg,https://oleks-netizen.github.io/product-images/20238/12.jpg,https://oleks-netizen.github.io/product-images/20238/03.jpg,https://oleks-netizen.github.io/product-images/20238/04.jpg,https://oleks-netizen.github.io/product-images/20238/05.jpg,https://oleks-netizen.github.io/product-images/20238/06.jpg,https://oleks-netizen.github.io/product-images/20238/07.jpg,https://oleks-netizen.github.io/product-images/20238/08.jpg,https://oleks-netizen.github.io/product-images/20238/09.jpg</t>
         </is>
       </c>
       <c r="C212" t="n">
@@ -3611,7 +3611,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20245/1.jpg,https://oleks-netizen.github.io/product-images/20245/2.jpg,https://oleks-netizen.github.io/product-images/20245/11.jpg,https://oleks-netizen.github.io/product-images/20245/10.jpg,https://oleks-netizen.github.io/product-images/20245/3.jpg,https://oleks-netizen.github.io/product-images/20245/4.jpg,https://oleks-netizen.github.io/product-images/20245/5.jpg,https://oleks-netizen.github.io/product-images/20245/7.jpg,https://oleks-netizen.github.io/product-images/20245/8.jpg,https://oleks-netizen.github.io/product-images/20245/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20245/01.jpg,https://oleks-netizen.github.io/product-images/20245/02.jpg,https://oleks-netizen.github.io/product-images/20245/11.jpg,https://oleks-netizen.github.io/product-images/20245/10.jpg,https://oleks-netizen.github.io/product-images/20245/03.jpg,https://oleks-netizen.github.io/product-images/20245/04.jpg,https://oleks-netizen.github.io/product-images/20245/05.jpg,https://oleks-netizen.github.io/product-images/20245/07.jpg,https://oleks-netizen.github.io/product-images/20245/08.jpg,https://oleks-netizen.github.io/product-images/20245/09.jpg</t>
         </is>
       </c>
       <c r="C213" t="n">
@@ -3626,7 +3626,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20256/1.jpg,https://oleks-netizen.github.io/product-images/20256/2.jpg,https://oleks-netizen.github.io/product-images/20256/3.jpg,https://oleks-netizen.github.io/product-images/20256/4.jpg,https://oleks-netizen.github.io/product-images/20256/5.jpg,https://oleks-netizen.github.io/product-images/20256/6.jpg,https://oleks-netizen.github.io/product-images/20256/7.jpg,https://oleks-netizen.github.io/product-images/20256/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20256/01.jpg,https://oleks-netizen.github.io/product-images/20256/02.jpg,https://oleks-netizen.github.io/product-images/20256/03.jpg,https://oleks-netizen.github.io/product-images/20256/04.jpg,https://oleks-netizen.github.io/product-images/20256/05.jpg,https://oleks-netizen.github.io/product-images/20256/06.jpg,https://oleks-netizen.github.io/product-images/20256/07.jpg,https://oleks-netizen.github.io/product-images/20256/08.jpg</t>
         </is>
       </c>
       <c r="C214" t="n">
@@ -3641,7 +3641,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20262/1.jpg,https://oleks-netizen.github.io/product-images/20262/2.jpg,https://oleks-netizen.github.io/product-images/20262/3.jpg,https://oleks-netizen.github.io/product-images/20262/4.jpg,https://oleks-netizen.github.io/product-images/20262/5.jpg,https://oleks-netizen.github.io/product-images/20262/6.jpg,https://oleks-netizen.github.io/product-images/20262/7.jpg,https://oleks-netizen.github.io/product-images/20262/8.jpg,https://oleks-netizen.github.io/product-images/20262/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20262/01.jpg,https://oleks-netizen.github.io/product-images/20262/02.jpg,https://oleks-netizen.github.io/product-images/20262/03.jpg,https://oleks-netizen.github.io/product-images/20262/04.jpg,https://oleks-netizen.github.io/product-images/20262/05.jpg,https://oleks-netizen.github.io/product-images/20262/06.jpg,https://oleks-netizen.github.io/product-images/20262/07.jpg,https://oleks-netizen.github.io/product-images/20262/08.jpg,https://oleks-netizen.github.io/product-images/20262/09.jpg</t>
         </is>
       </c>
       <c r="C215" t="n">
@@ -3656,7 +3656,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20263/1.jpg,https://oleks-netizen.github.io/product-images/20263/2.jpg,https://oleks-netizen.github.io/product-images/20263/3.jpg,https://oleks-netizen.github.io/product-images/20263/4.jpg,https://oleks-netizen.github.io/product-images/20263/5.jpg,https://oleks-netizen.github.io/product-images/20263/6.jpg,https://oleks-netizen.github.io/product-images/20263/7.jpg,https://oleks-netizen.github.io/product-images/20263/8.jpg,https://oleks-netizen.github.io/product-images/20263/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20263/01.jpg,https://oleks-netizen.github.io/product-images/20263/02.jpg,https://oleks-netizen.github.io/product-images/20263/03.jpg,https://oleks-netizen.github.io/product-images/20263/04.jpg,https://oleks-netizen.github.io/product-images/20263/05.jpg,https://oleks-netizen.github.io/product-images/20263/06.jpg,https://oleks-netizen.github.io/product-images/20263/07.jpg,https://oleks-netizen.github.io/product-images/20263/08.jpg,https://oleks-netizen.github.io/product-images/20263/09.jpg</t>
         </is>
       </c>
       <c r="C216" t="n">
@@ -3671,7 +3671,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20269/1.jpg,https://oleks-netizen.github.io/product-images/20269/2.jpg,https://oleks-netizen.github.io/product-images/20269/3.jpg,https://oleks-netizen.github.io/product-images/20269/4.jpg,https://oleks-netizen.github.io/product-images/20269/5.jpg,https://oleks-netizen.github.io/product-images/20269/6.jpg,https://oleks-netizen.github.io/product-images/20269/7.jpg,https://oleks-netizen.github.io/product-images/20269/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20269/01.jpg,https://oleks-netizen.github.io/product-images/20269/02.jpg,https://oleks-netizen.github.io/product-images/20269/03.jpg,https://oleks-netizen.github.io/product-images/20269/04.jpg,https://oleks-netizen.github.io/product-images/20269/05.jpg,https://oleks-netizen.github.io/product-images/20269/06.jpg,https://oleks-netizen.github.io/product-images/20269/07.jpg,https://oleks-netizen.github.io/product-images/20269/08.jpg</t>
         </is>
       </c>
       <c r="C217" t="n">
@@ -3686,7 +3686,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20270/1.jpg,https://oleks-netizen.github.io/product-images/20270/2.jpg,https://oleks-netizen.github.io/product-images/20270/3.jpg,https://oleks-netizen.github.io/product-images/20270/4.jpg,https://oleks-netizen.github.io/product-images/20270/5.jpg,https://oleks-netizen.github.io/product-images/20270/6.jpg,https://oleks-netizen.github.io/product-images/20270/7.jpg,https://oleks-netizen.github.io/product-images/20270/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20270/01.jpg,https://oleks-netizen.github.io/product-images/20270/02.jpg,https://oleks-netizen.github.io/product-images/20270/03.jpg,https://oleks-netizen.github.io/product-images/20270/04.jpg,https://oleks-netizen.github.io/product-images/20270/05.jpg,https://oleks-netizen.github.io/product-images/20270/06.jpg,https://oleks-netizen.github.io/product-images/20270/07.jpg,https://oleks-netizen.github.io/product-images/20270/08.jpg</t>
         </is>
       </c>
       <c r="C218" t="n">
@@ -3701,7 +3701,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20277/1.jpg,https://oleks-netizen.github.io/product-images/20277/2.jpg,https://oleks-netizen.github.io/product-images/20277/3.jpg,https://oleks-netizen.github.io/product-images/20277/4.jpg,https://oleks-netizen.github.io/product-images/20277/5.jpg,https://oleks-netizen.github.io/product-images/20277/6.jpg,https://oleks-netizen.github.io/product-images/20277/7.jpg,https://oleks-netizen.github.io/product-images/20277/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20277/01.jpg,https://oleks-netizen.github.io/product-images/20277/02.jpg,https://oleks-netizen.github.io/product-images/20277/03.jpg,https://oleks-netizen.github.io/product-images/20277/04.jpg,https://oleks-netizen.github.io/product-images/20277/05.jpg,https://oleks-netizen.github.io/product-images/20277/06.jpg,https://oleks-netizen.github.io/product-images/20277/07.jpg,https://oleks-netizen.github.io/product-images/20277/08.jpg</t>
         </is>
       </c>
       <c r="C219" t="n">
@@ -3716,7 +3716,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20279/1.jpg,https://oleks-netizen.github.io/product-images/20279/2.jpg,https://oleks-netizen.github.io/product-images/20279/3.jpg,https://oleks-netizen.github.io/product-images/20279/4.jpg,https://oleks-netizen.github.io/product-images/20279/5.jpg,https://oleks-netizen.github.io/product-images/20279/6.jpg,https://oleks-netizen.github.io/product-images/20279/7.jpg,https://oleks-netizen.github.io/product-images/20279/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20279/01.jpg,https://oleks-netizen.github.io/product-images/20279/02.jpg,https://oleks-netizen.github.io/product-images/20279/03.jpg,https://oleks-netizen.github.io/product-images/20279/04.jpg,https://oleks-netizen.github.io/product-images/20279/05.jpg,https://oleks-netizen.github.io/product-images/20279/06.jpg,https://oleks-netizen.github.io/product-images/20279/07.jpg,https://oleks-netizen.github.io/product-images/20279/08.jpg</t>
         </is>
       </c>
       <c r="C220" t="n">
@@ -3731,7 +3731,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20289/1.jpg,https://oleks-netizen.github.io/product-images/20289/2.jpg,https://oleks-netizen.github.io/product-images/20289/3.jpg,https://oleks-netizen.github.io/product-images/20289/4.jpg,https://oleks-netizen.github.io/product-images/20289/5.jpg,https://oleks-netizen.github.io/product-images/20289/6.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20289/01.jpg,https://oleks-netizen.github.io/product-images/20289/02.jpg,https://oleks-netizen.github.io/product-images/20289/03.jpg,https://oleks-netizen.github.io/product-images/20289/04.jpg,https://oleks-netizen.github.io/product-images/20289/05.jpg,https://oleks-netizen.github.io/product-images/20289/06.jpg</t>
         </is>
       </c>
       <c r="C221" t="n">
@@ -3746,7 +3746,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20309/1.jpg,https://oleks-netizen.github.io/product-images/20309/2.jpg,https://oleks-netizen.github.io/product-images/20309/3.jpg,https://oleks-netizen.github.io/product-images/20309/4.jpg,https://oleks-netizen.github.io/product-images/20309/5.jpg,https://oleks-netizen.github.io/product-images/20309/6.jpg,https://oleks-netizen.github.io/product-images/20309/7.jpg,https://oleks-netizen.github.io/product-images/20309/8.jpg,https://oleks-netizen.github.io/product-images/20309/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20309/01.jpg,https://oleks-netizen.github.io/product-images/20309/02.jpg,https://oleks-netizen.github.io/product-images/20309/03.jpg,https://oleks-netizen.github.io/product-images/20309/04.jpg,https://oleks-netizen.github.io/product-images/20309/05.jpg,https://oleks-netizen.github.io/product-images/20309/06.jpg,https://oleks-netizen.github.io/product-images/20309/07.jpg,https://oleks-netizen.github.io/product-images/20309/08.jpg,https://oleks-netizen.github.io/product-images/20309/09.jpg</t>
         </is>
       </c>
       <c r="C222" t="n">
@@ -3761,7 +3761,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20312/1.jpg,https://oleks-netizen.github.io/product-images/20312/2.jpg,https://oleks-netizen.github.io/product-images/20312/3.jpg,https://oleks-netizen.github.io/product-images/20312/4.jpg,https://oleks-netizen.github.io/product-images/20312/5.jpg,https://oleks-netizen.github.io/product-images/20312/6.jpg,https://oleks-netizen.github.io/product-images/20312/7.jpg,https://oleks-netizen.github.io/product-images/20312/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20312/01.jpg,https://oleks-netizen.github.io/product-images/20312/02.jpg,https://oleks-netizen.github.io/product-images/20312/03.jpg,https://oleks-netizen.github.io/product-images/20312/04.jpg,https://oleks-netizen.github.io/product-images/20312/05.jpg,https://oleks-netizen.github.io/product-images/20312/06.jpg,https://oleks-netizen.github.io/product-images/20312/07.jpg,https://oleks-netizen.github.io/product-images/20312/08.jpg</t>
         </is>
       </c>
       <c r="C223" t="n">
@@ -3776,7 +3776,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20314/1.jpg,https://oleks-netizen.github.io/product-images/20314/2.jpg,https://oleks-netizen.github.io/product-images/20314/3.jpg,https://oleks-netizen.github.io/product-images/20314/4.jpg,https://oleks-netizen.github.io/product-images/20314/5.jpg,https://oleks-netizen.github.io/product-images/20314/6.jpg,https://oleks-netizen.github.io/product-images/20314/7.jpg,https://oleks-netizen.github.io/product-images/20314/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20314/01.jpg,https://oleks-netizen.github.io/product-images/20314/02.jpg,https://oleks-netizen.github.io/product-images/20314/03.jpg,https://oleks-netizen.github.io/product-images/20314/04.jpg,https://oleks-netizen.github.io/product-images/20314/05.jpg,https://oleks-netizen.github.io/product-images/20314/06.jpg,https://oleks-netizen.github.io/product-images/20314/07.jpg,https://oleks-netizen.github.io/product-images/20314/08.jpg</t>
         </is>
       </c>
       <c r="C224" t="n">
@@ -3791,7 +3791,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20416/10.jpg,https://oleks-netizen.github.io/product-images/20416/1.jpg,https://oleks-netizen.github.io/product-images/20416/2.jpg,https://oleks-netizen.github.io/product-images/20416/3.jpg,https://oleks-netizen.github.io/product-images/20416/4.jpg,https://oleks-netizen.github.io/product-images/20416/5.jpg,https://oleks-netizen.github.io/product-images/20416/6.jpg,https://oleks-netizen.github.io/product-images/20416/7.jpg,https://oleks-netizen.github.io/product-images/20416/8.jpg,https://oleks-netizen.github.io/product-images/20416/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20416/10.jpg,https://oleks-netizen.github.io/product-images/20416/01.jpg,https://oleks-netizen.github.io/product-images/20416/02.jpg,https://oleks-netizen.github.io/product-images/20416/03.jpg,https://oleks-netizen.github.io/product-images/20416/04.jpg,https://oleks-netizen.github.io/product-images/20416/05.jpg,https://oleks-netizen.github.io/product-images/20416/06.jpg,https://oleks-netizen.github.io/product-images/20416/07.jpg,https://oleks-netizen.github.io/product-images/20416/08.jpg,https://oleks-netizen.github.io/product-images/20416/09.jpg</t>
         </is>
       </c>
       <c r="C225" t="n">
@@ -3806,7 +3806,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20441/1.jpg,https://oleks-netizen.github.io/product-images/20441/2.jpg,https://oleks-netizen.github.io/product-images/20441/3.jpg,https://oleks-netizen.github.io/product-images/20441/4.jpg,https://oleks-netizen.github.io/product-images/20441/5.jpg,https://oleks-netizen.github.io/product-images/20441/6.jpg,https://oleks-netizen.github.io/product-images/20441/7.jpg,https://oleks-netizen.github.io/product-images/20441/8.jpg,https://oleks-netizen.github.io/product-images/20441/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20441/01.jpg,https://oleks-netizen.github.io/product-images/20441/02.jpg,https://oleks-netizen.github.io/product-images/20441/03.jpg,https://oleks-netizen.github.io/product-images/20441/04.jpg,https://oleks-netizen.github.io/product-images/20441/05.jpg,https://oleks-netizen.github.io/product-images/20441/06.jpg,https://oleks-netizen.github.io/product-images/20441/07.jpg,https://oleks-netizen.github.io/product-images/20441/08.jpg,https://oleks-netizen.github.io/product-images/20441/09.jpg</t>
         </is>
       </c>
       <c r="C226" t="n">
@@ -3821,7 +3821,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20442/10.jpg,https://oleks-netizen.github.io/product-images/20442/1.jpg,https://oleks-netizen.github.io/product-images/20442/2.jpg,https://oleks-netizen.github.io/product-images/20442/3.jpg,https://oleks-netizen.github.io/product-images/20442/4.jpg,https://oleks-netizen.github.io/product-images/20442/5.jpg,https://oleks-netizen.github.io/product-images/20442/6.jpg,https://oleks-netizen.github.io/product-images/20442/7.jpg,https://oleks-netizen.github.io/product-images/20442/8.jpg,https://oleks-netizen.github.io/product-images/20442/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20442/10.jpg,https://oleks-netizen.github.io/product-images/20442/01.jpg,https://oleks-netizen.github.io/product-images/20442/02.jpg,https://oleks-netizen.github.io/product-images/20442/03.jpg,https://oleks-netizen.github.io/product-images/20442/04.jpg,https://oleks-netizen.github.io/product-images/20442/05.jpg,https://oleks-netizen.github.io/product-images/20442/06.jpg,https://oleks-netizen.github.io/product-images/20442/07.jpg,https://oleks-netizen.github.io/product-images/20442/08.jpg,https://oleks-netizen.github.io/product-images/20442/09.jpg</t>
         </is>
       </c>
       <c r="C227" t="n">
@@ -3836,7 +3836,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/20451/1.jpg,https://oleks-netizen.github.io/product-images/20451/2.jpg,https://oleks-netizen.github.io/product-images/20451/3.jpg,https://oleks-netizen.github.io/product-images/20451/4.jpg,https://oleks-netizen.github.io/product-images/20451/5.jpg,https://oleks-netizen.github.io/product-images/20451/6.jpg,https://oleks-netizen.github.io/product-images/20451/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/20451/01.jpg,https://oleks-netizen.github.io/product-images/20451/02.jpg,https://oleks-netizen.github.io/product-images/20451/03.jpg,https://oleks-netizen.github.io/product-images/20451/04.jpg,https://oleks-netizen.github.io/product-images/20451/05.jpg,https://oleks-netizen.github.io/product-images/20451/06.jpg,https://oleks-netizen.github.io/product-images/20451/07.jpg</t>
         </is>
       </c>
       <c r="C228" t="n">
@@ -3851,7 +3851,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/21246/1.jpg,https://oleks-netizen.github.io/product-images/21246/2.jpg,https://oleks-netizen.github.io/product-images/21246/3.jpg,https://oleks-netizen.github.io/product-images/21246/4.jpg,https://oleks-netizen.github.io/product-images/21246/5.jpg,https://oleks-netizen.github.io/product-images/21246/6.jpg,https://oleks-netizen.github.io/product-images/21246/7.jpg,https://oleks-netizen.github.io/product-images/21246/8.jpg,https://oleks-netizen.github.io/product-images/21246/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/21246/01.jpg,https://oleks-netizen.github.io/product-images/21246/02.jpg,https://oleks-netizen.github.io/product-images/21246/03.jpg,https://oleks-netizen.github.io/product-images/21246/04.jpg,https://oleks-netizen.github.io/product-images/21246/05.jpg,https://oleks-netizen.github.io/product-images/21246/06.jpg,https://oleks-netizen.github.io/product-images/21246/07.jpg,https://oleks-netizen.github.io/product-images/21246/08.jpg,https://oleks-netizen.github.io/product-images/21246/09.jpg</t>
         </is>
       </c>
       <c r="C229" t="n">
@@ -3866,7 +3866,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/21258/10.jpg,https://oleks-netizen.github.io/product-images/21258/11.jpg,https://oleks-netizen.github.io/product-images/21258/1.jpg,https://oleks-netizen.github.io/product-images/21258/2.jpg,https://oleks-netizen.github.io/product-images/21258/3.jpg,https://oleks-netizen.github.io/product-images/21258/4.jpg,https://oleks-netizen.github.io/product-images/21258/5.jpg,https://oleks-netizen.github.io/product-images/21258/6.jpg,https://oleks-netizen.github.io/product-images/21258/7.jpg,https://oleks-netizen.github.io/product-images/21258/8.jpg,https://oleks-netizen.github.io/product-images/21258/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/21258/10.jpg,https://oleks-netizen.github.io/product-images/21258/11.jpg,https://oleks-netizen.github.io/product-images/21258/01.jpg,https://oleks-netizen.github.io/product-images/21258/02.jpg,https://oleks-netizen.github.io/product-images/21258/03.jpg,https://oleks-netizen.github.io/product-images/21258/04.jpg,https://oleks-netizen.github.io/product-images/21258/05.jpg,https://oleks-netizen.github.io/product-images/21258/06.jpg,https://oleks-netizen.github.io/product-images/21258/07.jpg,https://oleks-netizen.github.io/product-images/21258/08.jpg,https://oleks-netizen.github.io/product-images/21258/09.jpg</t>
         </is>
       </c>
       <c r="C230" t="n">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/21264/10.jpg,https://oleks-netizen.github.io/product-images/21264/11.jpg,https://oleks-netizen.github.io/product-images/21264/1.jpg,https://oleks-netizen.github.io/product-images/21264/2.jpg,https://oleks-netizen.github.io/product-images/21264/3.jpg,https://oleks-netizen.github.io/product-images/21264/4.jpg,https://oleks-netizen.github.io/product-images/21264/5.jpg,https://oleks-netizen.github.io/product-images/21264/6.jpg,https://oleks-netizen.github.io/product-images/21264/7.jpg,https://oleks-netizen.github.io/product-images/21264/8.jpg,https://oleks-netizen.github.io/product-images/21264/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/21264/10.jpg,https://oleks-netizen.github.io/product-images/21264/11.jpg,https://oleks-netizen.github.io/product-images/21264/01.jpg,https://oleks-netizen.github.io/product-images/21264/02.jpg,https://oleks-netizen.github.io/product-images/21264/03.jpg,https://oleks-netizen.github.io/product-images/21264/04.jpg,https://oleks-netizen.github.io/product-images/21264/05.jpg,https://oleks-netizen.github.io/product-images/21264/06.jpg,https://oleks-netizen.github.io/product-images/21264/07.jpg,https://oleks-netizen.github.io/product-images/21264/08.jpg,https://oleks-netizen.github.io/product-images/21264/09.jpg</t>
         </is>
       </c>
       <c r="C231" t="n">
@@ -3896,7 +3896,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/21265/10.jpg,https://oleks-netizen.github.io/product-images/21265/11.jpg,https://oleks-netizen.github.io/product-images/21265/1.jpg,https://oleks-netizen.github.io/product-images/21265/2.jpg,https://oleks-netizen.github.io/product-images/21265/3.jpg,https://oleks-netizen.github.io/product-images/21265/4.jpg,https://oleks-netizen.github.io/product-images/21265/5.jpg,https://oleks-netizen.github.io/product-images/21265/6.jpg,https://oleks-netizen.github.io/product-images/21265/7.jpg,https://oleks-netizen.github.io/product-images/21265/8.jpg,https://oleks-netizen.github.io/product-images/21265/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/21265/10.jpg,https://oleks-netizen.github.io/product-images/21265/11.jpg,https://oleks-netizen.github.io/product-images/21265/01.jpg,https://oleks-netizen.github.io/product-images/21265/02.jpg,https://oleks-netizen.github.io/product-images/21265/03.jpg,https://oleks-netizen.github.io/product-images/21265/04.jpg,https://oleks-netizen.github.io/product-images/21265/05.jpg,https://oleks-netizen.github.io/product-images/21265/06.jpg,https://oleks-netizen.github.io/product-images/21265/07.jpg,https://oleks-netizen.github.io/product-images/21265/08.jpg,https://oleks-netizen.github.io/product-images/21265/09.jpg</t>
         </is>
       </c>
       <c r="C232" t="n">
@@ -3911,7 +3911,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/21266/10.jpg,https://oleks-netizen.github.io/product-images/21266/1.jpg,https://oleks-netizen.github.io/product-images/21266/2.jpg,https://oleks-netizen.github.io/product-images/21266/3.jpg,https://oleks-netizen.github.io/product-images/21266/4.jpg,https://oleks-netizen.github.io/product-images/21266/5.jpg,https://oleks-netizen.github.io/product-images/21266/6.jpg,https://oleks-netizen.github.io/product-images/21266/7.jpg,https://oleks-netizen.github.io/product-images/21266/8.jpg,https://oleks-netizen.github.io/product-images/21266/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/21266/10.jpg,https://oleks-netizen.github.io/product-images/21266/01.jpg,https://oleks-netizen.github.io/product-images/21266/02.jpg,https://oleks-netizen.github.io/product-images/21266/03.jpg,https://oleks-netizen.github.io/product-images/21266/04.jpg,https://oleks-netizen.github.io/product-images/21266/05.jpg,https://oleks-netizen.github.io/product-images/21266/06.jpg,https://oleks-netizen.github.io/product-images/21266/07.jpg,https://oleks-netizen.github.io/product-images/21266/08.jpg,https://oleks-netizen.github.io/product-images/21266/09.jpg</t>
         </is>
       </c>
       <c r="C233" t="n">
@@ -3926,7 +3926,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/21274/10.jpg,https://oleks-netizen.github.io/product-images/21274/1.jpg,https://oleks-netizen.github.io/product-images/21274/2.jpg,https://oleks-netizen.github.io/product-images/21274/3.jpg,https://oleks-netizen.github.io/product-images/21274/4.jpg,https://oleks-netizen.github.io/product-images/21274/5.jpg,https://oleks-netizen.github.io/product-images/21274/6.jpg,https://oleks-netizen.github.io/product-images/21274/7.jpg,https://oleks-netizen.github.io/product-images/21274/8.jpg,https://oleks-netizen.github.io/product-images/21274/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/21274/10.jpg,https://oleks-netizen.github.io/product-images/21274/01.jpg,https://oleks-netizen.github.io/product-images/21274/02.jpg,https://oleks-netizen.github.io/product-images/21274/03.jpg,https://oleks-netizen.github.io/product-images/21274/04.jpg,https://oleks-netizen.github.io/product-images/21274/05.jpg,https://oleks-netizen.github.io/product-images/21274/06.jpg,https://oleks-netizen.github.io/product-images/21274/07.jpg,https://oleks-netizen.github.io/product-images/21274/08.jpg,https://oleks-netizen.github.io/product-images/21274/09.jpg</t>
         </is>
       </c>
       <c r="C234" t="n">
@@ -3941,7 +3941,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/21276/1.jpg,https://oleks-netizen.github.io/product-images/21276/2.jpg,https://oleks-netizen.github.io/product-images/21276/12.jpg,https://oleks-netizen.github.io/product-images/21276/10.jpg,https://oleks-netizen.github.io/product-images/21276/11.jpg,https://oleks-netizen.github.io/product-images/21276/3.jpg,https://oleks-netizen.github.io/product-images/21276/4.jpg,https://oleks-netizen.github.io/product-images/21276/5.jpg,https://oleks-netizen.github.io/product-images/21276/6.jpg,https://oleks-netizen.github.io/product-images/21276/8.jpg,https://oleks-netizen.github.io/product-images/21276/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/21276/01.jpg,https://oleks-netizen.github.io/product-images/21276/02.jpg,https://oleks-netizen.github.io/product-images/21276/12.jpg,https://oleks-netizen.github.io/product-images/21276/10.jpg,https://oleks-netizen.github.io/product-images/21276/11.jpg,https://oleks-netizen.github.io/product-images/21276/03.jpg,https://oleks-netizen.github.io/product-images/21276/04.jpg,https://oleks-netizen.github.io/product-images/21276/05.jpg,https://oleks-netizen.github.io/product-images/21276/06.jpg,https://oleks-netizen.github.io/product-images/21276/08.jpg,https://oleks-netizen.github.io/product-images/21276/09.jpg</t>
         </is>
       </c>
       <c r="C235" t="n">
@@ -3956,7 +3956,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/21301/10.jpg,https://oleks-netizen.github.io/product-images/21301/11.jpg,https://oleks-netizen.github.io/product-images/21301/1.jpg,https://oleks-netizen.github.io/product-images/21301/2.jpg,https://oleks-netizen.github.io/product-images/21301/3.jpg,https://oleks-netizen.github.io/product-images/21301/4.jpg,https://oleks-netizen.github.io/product-images/21301/5.jpg,https://oleks-netizen.github.io/product-images/21301/6.jpg,https://oleks-netizen.github.io/product-images/21301/7.jpg,https://oleks-netizen.github.io/product-images/21301/8.jpg,https://oleks-netizen.github.io/product-images/21301/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/21301/10.jpg,https://oleks-netizen.github.io/product-images/21301/11.jpg,https://oleks-netizen.github.io/product-images/21301/01.jpg,https://oleks-netizen.github.io/product-images/21301/02.jpg,https://oleks-netizen.github.io/product-images/21301/03.jpg,https://oleks-netizen.github.io/product-images/21301/04.jpg,https://oleks-netizen.github.io/product-images/21301/05.jpg,https://oleks-netizen.github.io/product-images/21301/06.jpg,https://oleks-netizen.github.io/product-images/21301/07.jpg,https://oleks-netizen.github.io/product-images/21301/08.jpg,https://oleks-netizen.github.io/product-images/21301/09.jpg</t>
         </is>
       </c>
       <c r="C236" t="n">
@@ -3971,7 +3971,7 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/21482/10.jpg,https://oleks-netizen.github.io/product-images/21482/1.jpg,https://oleks-netizen.github.io/product-images/21482/2.jpg,https://oleks-netizen.github.io/product-images/21482/3.jpg,https://oleks-netizen.github.io/product-images/21482/4.jpg,https://oleks-netizen.github.io/product-images/21482/5.jpg,https://oleks-netizen.github.io/product-images/21482/6.jpg,https://oleks-netizen.github.io/product-images/21482/7.jpg,https://oleks-netizen.github.io/product-images/21482/8.jpg,https://oleks-netizen.github.io/product-images/21482/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/21482/10.jpg,https://oleks-netizen.github.io/product-images/21482/01.jpg,https://oleks-netizen.github.io/product-images/21482/02.jpg,https://oleks-netizen.github.io/product-images/21482/03.jpg,https://oleks-netizen.github.io/product-images/21482/04.jpg,https://oleks-netizen.github.io/product-images/21482/05.jpg,https://oleks-netizen.github.io/product-images/21482/06.jpg,https://oleks-netizen.github.io/product-images/21482/07.jpg,https://oleks-netizen.github.io/product-images/21482/08.jpg,https://oleks-netizen.github.io/product-images/21482/09.jpg</t>
         </is>
       </c>
       <c r="C237" t="n">
@@ -3986,7 +3986,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/22078/1.jpg,https://oleks-netizen.github.io/product-images/22078/2.jpg,https://oleks-netizen.github.io/product-images/22078/12.jpg,https://oleks-netizen.github.io/product-images/22078/10.jpg,https://oleks-netizen.github.io/product-images/22078/11.jpg,https://oleks-netizen.github.io/product-images/22078/3.jpg,https://oleks-netizen.github.io/product-images/22078/4.jpg,https://oleks-netizen.github.io/product-images/22078/5.jpg,https://oleks-netizen.github.io/product-images/22078/6.jpg,https://oleks-netizen.github.io/product-images/22078/8.jpg,https://oleks-netizen.github.io/product-images/22078/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/22078/01.jpg,https://oleks-netizen.github.io/product-images/22078/02.jpg,https://oleks-netizen.github.io/product-images/22078/12.jpg,https://oleks-netizen.github.io/product-images/22078/10.jpg,https://oleks-netizen.github.io/product-images/22078/11.jpg,https://oleks-netizen.github.io/product-images/22078/03.jpg,https://oleks-netizen.github.io/product-images/22078/04.jpg,https://oleks-netizen.github.io/product-images/22078/05.jpg,https://oleks-netizen.github.io/product-images/22078/06.jpg,https://oleks-netizen.github.io/product-images/22078/08.jpg,https://oleks-netizen.github.io/product-images/22078/09.jpg</t>
         </is>
       </c>
       <c r="C238" t="n">
@@ -4001,7 +4001,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/22082/10.jpg,https://oleks-netizen.github.io/product-images/22082/1.jpg,https://oleks-netizen.github.io/product-images/22082/2.jpg,https://oleks-netizen.github.io/product-images/22082/3.jpg,https://oleks-netizen.github.io/product-images/22082/4.jpg,https://oleks-netizen.github.io/product-images/22082/5.jpg,https://oleks-netizen.github.io/product-images/22082/6.jpg,https://oleks-netizen.github.io/product-images/22082/7.jpg,https://oleks-netizen.github.io/product-images/22082/8.jpg,https://oleks-netizen.github.io/product-images/22082/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/22082/10.jpg,https://oleks-netizen.github.io/product-images/22082/01.jpg,https://oleks-netizen.github.io/product-images/22082/02.jpg,https://oleks-netizen.github.io/product-images/22082/03.jpg,https://oleks-netizen.github.io/product-images/22082/04.jpg,https://oleks-netizen.github.io/product-images/22082/05.jpg,https://oleks-netizen.github.io/product-images/22082/06.jpg,https://oleks-netizen.github.io/product-images/22082/07.jpg,https://oleks-netizen.github.io/product-images/22082/08.jpg,https://oleks-netizen.github.io/product-images/22082/09.jpg</t>
         </is>
       </c>
       <c r="C239" t="n">
@@ -4016,7 +4016,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/22087/10.jpg,https://oleks-netizen.github.io/product-images/22087/11.jpg,https://oleks-netizen.github.io/product-images/22087/1.jpg,https://oleks-netizen.github.io/product-images/22087/2.jpg,https://oleks-netizen.github.io/product-images/22087/3.jpg,https://oleks-netizen.github.io/product-images/22087/4.jpg,https://oleks-netizen.github.io/product-images/22087/5.jpg,https://oleks-netizen.github.io/product-images/22087/6.jpg,https://oleks-netizen.github.io/product-images/22087/7.jpg,https://oleks-netizen.github.io/product-images/22087/8.jpg,https://oleks-netizen.github.io/product-images/22087/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/22087/10.jpg,https://oleks-netizen.github.io/product-images/22087/11.jpg,https://oleks-netizen.github.io/product-images/22087/01.jpg,https://oleks-netizen.github.io/product-images/22087/02.jpg,https://oleks-netizen.github.io/product-images/22087/03.jpg,https://oleks-netizen.github.io/product-images/22087/04.jpg,https://oleks-netizen.github.io/product-images/22087/05.jpg,https://oleks-netizen.github.io/product-images/22087/06.jpg,https://oleks-netizen.github.io/product-images/22087/07.jpg,https://oleks-netizen.github.io/product-images/22087/08.jpg,https://oleks-netizen.github.io/product-images/22087/09.jpg</t>
         </is>
       </c>
       <c r="C240" t="n">
@@ -4031,7 +4031,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/22088/10.jpg,https://oleks-netizen.github.io/product-images/22088/1.jpg,https://oleks-netizen.github.io/product-images/22088/2.jpg,https://oleks-netizen.github.io/product-images/22088/3.jpg,https://oleks-netizen.github.io/product-images/22088/4.jpg,https://oleks-netizen.github.io/product-images/22088/5.jpg,https://oleks-netizen.github.io/product-images/22088/6.jpg,https://oleks-netizen.github.io/product-images/22088/7.jpg,https://oleks-netizen.github.io/product-images/22088/8.jpg,https://oleks-netizen.github.io/product-images/22088/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/22088/10.jpg,https://oleks-netizen.github.io/product-images/22088/01.jpg,https://oleks-netizen.github.io/product-images/22088/02.jpg,https://oleks-netizen.github.io/product-images/22088/03.jpg,https://oleks-netizen.github.io/product-images/22088/04.jpg,https://oleks-netizen.github.io/product-images/22088/05.jpg,https://oleks-netizen.github.io/product-images/22088/06.jpg,https://oleks-netizen.github.io/product-images/22088/07.jpg,https://oleks-netizen.github.io/product-images/22088/08.jpg,https://oleks-netizen.github.io/product-images/22088/09.jpg</t>
         </is>
       </c>
       <c r="C241" t="n">
@@ -4046,7 +4046,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/22094/10.jpg,https://oleks-netizen.github.io/product-images/22094/11.jpg,https://oleks-netizen.github.io/product-images/22094/1.jpg,https://oleks-netizen.github.io/product-images/22094/2.jpg,https://oleks-netizen.github.io/product-images/22094/3.jpg,https://oleks-netizen.github.io/product-images/22094/4.jpg,https://oleks-netizen.github.io/product-images/22094/5.jpg,https://oleks-netizen.github.io/product-images/22094/6.jpg,https://oleks-netizen.github.io/product-images/22094/7.jpg,https://oleks-netizen.github.io/product-images/22094/8.jpg,https://oleks-netizen.github.io/product-images/22094/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/22094/10.jpg,https://oleks-netizen.github.io/product-images/22094/11.jpg,https://oleks-netizen.github.io/product-images/22094/01.jpg,https://oleks-netizen.github.io/product-images/22094/02.jpg,https://oleks-netizen.github.io/product-images/22094/03.jpg,https://oleks-netizen.github.io/product-images/22094/04.jpg,https://oleks-netizen.github.io/product-images/22094/05.jpg,https://oleks-netizen.github.io/product-images/22094/06.jpg,https://oleks-netizen.github.io/product-images/22094/07.jpg,https://oleks-netizen.github.io/product-images/22094/08.jpg,https://oleks-netizen.github.io/product-images/22094/09.jpg</t>
         </is>
       </c>
       <c r="C242" t="n">
@@ -4061,7 +4061,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/22116/10.jpg,https://oleks-netizen.github.io/product-images/22116/1.jpg,https://oleks-netizen.github.io/product-images/22116/2.jpg,https://oleks-netizen.github.io/product-images/22116/3.jpg,https://oleks-netizen.github.io/product-images/22116/4.jpg,https://oleks-netizen.github.io/product-images/22116/5.jpg,https://oleks-netizen.github.io/product-images/22116/6.jpg,https://oleks-netizen.github.io/product-images/22116/7.jpg,https://oleks-netizen.github.io/product-images/22116/8.jpg,https://oleks-netizen.github.io/product-images/22116/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/22116/10.jpg,https://oleks-netizen.github.io/product-images/22116/01.jpg,https://oleks-netizen.github.io/product-images/22116/02.jpg,https://oleks-netizen.github.io/product-images/22116/03.jpg,https://oleks-netizen.github.io/product-images/22116/04.jpg,https://oleks-netizen.github.io/product-images/22116/05.jpg,https://oleks-netizen.github.io/product-images/22116/06.jpg,https://oleks-netizen.github.io/product-images/22116/07.jpg,https://oleks-netizen.github.io/product-images/22116/08.jpg,https://oleks-netizen.github.io/product-images/22116/09.jpg</t>
         </is>
       </c>
       <c r="C243" t="n">
@@ -4076,7 +4076,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/22125/10.jpg,https://oleks-netizen.github.io/product-images/22125/1.jpg,https://oleks-netizen.github.io/product-images/22125/2.jpg,https://oleks-netizen.github.io/product-images/22125/3.jpg,https://oleks-netizen.github.io/product-images/22125/4.jpg,https://oleks-netizen.github.io/product-images/22125/5.jpg,https://oleks-netizen.github.io/product-images/22125/6.jpg,https://oleks-netizen.github.io/product-images/22125/7.jpg,https://oleks-netizen.github.io/product-images/22125/8.jpg,https://oleks-netizen.github.io/product-images/22125/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/22125/10.jpg,https://oleks-netizen.github.io/product-images/22125/01.jpg,https://oleks-netizen.github.io/product-images/22125/02.jpg,https://oleks-netizen.github.io/product-images/22125/03.jpg,https://oleks-netizen.github.io/product-images/22125/04.jpg,https://oleks-netizen.github.io/product-images/22125/05.jpg,https://oleks-netizen.github.io/product-images/22125/06.jpg,https://oleks-netizen.github.io/product-images/22125/07.jpg,https://oleks-netizen.github.io/product-images/22125/08.jpg,https://oleks-netizen.github.io/product-images/22125/09.jpg</t>
         </is>
       </c>
       <c r="C244" t="n">
@@ -4091,7 +4091,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/Cv1gnn16-115/1.jpg,https://oleks-netizen.github.io/product-images/Cv1gnn16-115/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/Cv1gnn16-115/01.jpg,https://oleks-netizen.github.io/product-images/Cv1gnn16-115/02.jpg</t>
         </is>
       </c>
       <c r="C245" t="n">
@@ -4106,7 +4106,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/Cv1gnn28-125/1.jpg,https://oleks-netizen.github.io/product-images/Cv1gnn28-125/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/Cv1gnn28-125/01.jpg,https://oleks-netizen.github.io/product-images/Cv1gnn28-125/02.jpg</t>
         </is>
       </c>
       <c r="C246" t="n">
@@ -4121,7 +4121,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/CV1gnn38-115/1.jpg,https://oleks-netizen.github.io/product-images/CV1gnn38-115/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/CV1gnn38-115/01.jpg,https://oleks-netizen.github.io/product-images/CV1gnn38-115/02.jpg</t>
         </is>
       </c>
       <c r="C247" t="n">
@@ -4136,7 +4136,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/G853-035146/1.jpg,https://oleks-netizen.github.io/product-images/G853-035146/2.jpg,https://oleks-netizen.github.io/product-images/G853-035146/12.jpg,https://oleks-netizen.github.io/product-images/G853-035146/10.jpg,https://oleks-netizen.github.io/product-images/G853-035146/11.jpg,https://oleks-netizen.github.io/product-images/G853-035146/4.jpg,https://oleks-netizen.github.io/product-images/G853-035146/5.jpg,https://oleks-netizen.github.io/product-images/G853-035146/6.jpg,https://oleks-netizen.github.io/product-images/G853-035146/7.jpg,https://oleks-netizen.github.io/product-images/G853-035146/8.jpg,https://oleks-netizen.github.io/product-images/G853-035146/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/G853-035146/01.jpg,https://oleks-netizen.github.io/product-images/G853-035146/02.jpg,https://oleks-netizen.github.io/product-images/G853-035146/12.jpg,https://oleks-netizen.github.io/product-images/G853-035146/10.jpg,https://oleks-netizen.github.io/product-images/G853-035146/11.jpg,https://oleks-netizen.github.io/product-images/G853-035146/04.jpg,https://oleks-netizen.github.io/product-images/G853-035146/05.jpg,https://oleks-netizen.github.io/product-images/G853-035146/06.jpg,https://oleks-netizen.github.io/product-images/G853-035146/07.jpg,https://oleks-netizen.github.io/product-images/G853-035146/08.jpg,https://oleks-netizen.github.io/product-images/G853-035146/09.jpg</t>
         </is>
       </c>
       <c r="C248" t="n">
@@ -4151,7 +4151,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/JBNC39MN TAN/1.jpg,https://oleks-netizen.github.io/product-images/JBNC39MN TAN/2.jpg,https://oleks-netizen.github.io/product-images/JBNC39MN TAN/6.jpg,https://oleks-netizen.github.io/product-images/JBNC39MN TAN/7.jpg,https://oleks-netizen.github.io/product-images/JBNC39MN TAN/3.jpg,https://oleks-netizen.github.io/product-images/JBNC39MN TAN/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/JBNC39MN TAN/01.jpg,https://oleks-netizen.github.io/product-images/JBNC39MN TAN/02.jpg,https://oleks-netizen.github.io/product-images/JBNC39MN TAN/06.jpg,https://oleks-netizen.github.io/product-images/JBNC39MN TAN/07.jpg,https://oleks-netizen.github.io/product-images/JBNC39MN TAN/03.jpg,https://oleks-netizen.github.io/product-images/JBNC39MN TAN/05.jpg</t>
         </is>
       </c>
       <c r="C249" t="n">
@@ -4166,7 +4166,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/k1001b-black/1.jpg,https://oleks-netizen.github.io/product-images/k1001b-black/2.jpg,https://oleks-netizen.github.io/product-images/k1001b-black/9.jpg,https://oleks-netizen.github.io/product-images/k1001b-black/3.jpg,https://oleks-netizen.github.io/product-images/k1001b-black/4.jpg,https://oleks-netizen.github.io/product-images/k1001b-black/5.jpg,https://oleks-netizen.github.io/product-images/k1001b-black/6.jpg,https://oleks-netizen.github.io/product-images/k1001b-black/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/k1001b-black/01.jpg,https://oleks-netizen.github.io/product-images/k1001b-black/02.jpg,https://oleks-netizen.github.io/product-images/k1001b-black/09.jpg,https://oleks-netizen.github.io/product-images/k1001b-black/03.jpg,https://oleks-netizen.github.io/product-images/k1001b-black/04.jpg,https://oleks-netizen.github.io/product-images/k1001b-black/05.jpg,https://oleks-netizen.github.io/product-images/k1001b-black/06.jpg,https://oleks-netizen.github.io/product-images/k1001b-black/08.jpg</t>
         </is>
       </c>
       <c r="C250" t="n">
@@ -4181,7 +4181,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K11031-black/1.jpg,https://oleks-netizen.github.io/product-images/K11031-black/2.jpg,https://oleks-netizen.github.io/product-images/K11031-black/9.jpg,https://oleks-netizen.github.io/product-images/K11031-black/4.jpg,https://oleks-netizen.github.io/product-images/K11031-black/5.jpg,https://oleks-netizen.github.io/product-images/K11031-black/6.jpg,https://oleks-netizen.github.io/product-images/K11031-black/7.jpg,https://oleks-netizen.github.io/product-images/K11031-black/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K11031-black/01.jpg,https://oleks-netizen.github.io/product-images/K11031-black/02.jpg,https://oleks-netizen.github.io/product-images/K11031-black/09.jpg,https://oleks-netizen.github.io/product-images/K11031-black/04.jpg,https://oleks-netizen.github.io/product-images/K11031-black/05.jpg,https://oleks-netizen.github.io/product-images/K11031-black/06.jpg,https://oleks-netizen.github.io/product-images/K11031-black/07.jpg,https://oleks-netizen.github.io/product-images/K11031-black/08.jpg</t>
         </is>
       </c>
       <c r="C251" t="n">
@@ -4196,7 +4196,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K11031-dark brown/1.jpg,https://oleks-netizen.github.io/product-images/K11031-dark brown/2.jpg,https://oleks-netizen.github.io/product-images/K11031-dark brown/3.jpg,https://oleks-netizen.github.io/product-images/K11031-dark brown/4.jpg,https://oleks-netizen.github.io/product-images/K11031-dark brown/5.jpg,https://oleks-netizen.github.io/product-images/K11031-dark brown/6.jpg,https://oleks-netizen.github.io/product-images/K11031-dark brown/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K11031-dark brown/01.jpg,https://oleks-netizen.github.io/product-images/K11031-dark brown/02.jpg,https://oleks-netizen.github.io/product-images/K11031-dark brown/03.jpg,https://oleks-netizen.github.io/product-images/K11031-dark brown/04.jpg,https://oleks-netizen.github.io/product-images/K11031-dark brown/05.jpg,https://oleks-netizen.github.io/product-images/K11031-dark brown/06.jpg,https://oleks-netizen.github.io/product-images/K11031-dark brown/07.jpg</t>
         </is>
       </c>
       <c r="C252" t="n">
@@ -4211,7 +4211,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/k11120a-black/1.jpg,https://oleks-netizen.github.io/product-images/k11120a-black/2.jpg,https://oleks-netizen.github.io/product-images/k11120a-black/3.jpg,https://oleks-netizen.github.io/product-images/k11120a-black/4.jpg,https://oleks-netizen.github.io/product-images/k11120a-black/5.jpg,https://oleks-netizen.github.io/product-images/k11120a-black/6.jpg,https://oleks-netizen.github.io/product-images/k11120a-black/7.jpg,https://oleks-netizen.github.io/product-images/k11120a-black/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/k11120a-black/01.jpg,https://oleks-netizen.github.io/product-images/k11120a-black/02.jpg,https://oleks-netizen.github.io/product-images/k11120a-black/03.jpg,https://oleks-netizen.github.io/product-images/k11120a-black/04.jpg,https://oleks-netizen.github.io/product-images/k11120a-black/05.jpg,https://oleks-netizen.github.io/product-images/k11120a-black/06.jpg,https://oleks-netizen.github.io/product-images/k11120a-black/07.jpg,https://oleks-netizen.github.io/product-images/k11120a-black/08.jpg</t>
         </is>
       </c>
       <c r="C253" t="n">
@@ -4226,7 +4226,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K12335-blue/1.jpg,https://oleks-netizen.github.io/product-images/K12335-blue/2.jpg,https://oleks-netizen.github.io/product-images/K12335-blue/9.jpg,https://oleks-netizen.github.io/product-images/K12335-blue/3.jpg,https://oleks-netizen.github.io/product-images/K12335-blue/4.jpg,https://oleks-netizen.github.io/product-images/K12335-blue/5.jpg,https://oleks-netizen.github.io/product-images/K12335-blue/6.jpg,https://oleks-netizen.github.io/product-images/K12335-blue/7.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K12335-blue/01.jpg,https://oleks-netizen.github.io/product-images/K12335-blue/02.jpg,https://oleks-netizen.github.io/product-images/K12335-blue/09.jpg,https://oleks-netizen.github.io/product-images/K12335-blue/03.jpg,https://oleks-netizen.github.io/product-images/K12335-blue/04.jpg,https://oleks-netizen.github.io/product-images/K12335-blue/05.jpg,https://oleks-netizen.github.io/product-images/K12335-blue/06.jpg,https://oleks-netizen.github.io/product-images/K12335-blue/07.jpg</t>
         </is>
       </c>
       <c r="C254" t="n">
@@ -4241,7 +4241,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K12335-red/1.jpg,https://oleks-netizen.github.io/product-images/K12335-red/2.jpg,https://oleks-netizen.github.io/product-images/K12335-red/9.jpg,https://oleks-netizen.github.io/product-images/K12335-red/3.jpg,https://oleks-netizen.github.io/product-images/K12335-red/4.jpg,https://oleks-netizen.github.io/product-images/K12335-red/5.jpg,https://oleks-netizen.github.io/product-images/K12335-red/6.jpg,https://oleks-netizen.github.io/product-images/K12335-red/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K12335-red/01.jpg,https://oleks-netizen.github.io/product-images/K12335-red/02.jpg,https://oleks-netizen.github.io/product-images/K12335-red/09.jpg,https://oleks-netizen.github.io/product-images/K12335-red/03.jpg,https://oleks-netizen.github.io/product-images/K12335-red/04.jpg,https://oleks-netizen.github.io/product-images/K12335-red/05.jpg,https://oleks-netizen.github.io/product-images/K12335-red/06.jpg,https://oleks-netizen.github.io/product-images/K12335-red/08.jpg</t>
         </is>
       </c>
       <c r="C255" t="n">
@@ -4256,7 +4256,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K1a0001-bordo/1.jpg,https://oleks-netizen.github.io/product-images/K1a0001-bordo/2.jpg,https://oleks-netizen.github.io/product-images/K1a0001-bordo/9.jpg,https://oleks-netizen.github.io/product-images/K1a0001-bordo/3.jpg,https://oleks-netizen.github.io/product-images/K1a0001-bordo/4.jpg,https://oleks-netizen.github.io/product-images/K1a0001-bordo/5.jpg,https://oleks-netizen.github.io/product-images/K1a0001-bordo/7.jpg,https://oleks-netizen.github.io/product-images/K1a0001-bordo/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K1a0001-bordo/01.jpg,https://oleks-netizen.github.io/product-images/K1a0001-bordo/02.jpg,https://oleks-netizen.github.io/product-images/K1a0001-bordo/09.jpg,https://oleks-netizen.github.io/product-images/K1a0001-bordo/03.jpg,https://oleks-netizen.github.io/product-images/K1a0001-bordo/04.jpg,https://oleks-netizen.github.io/product-images/K1a0001-bordo/05.jpg,https://oleks-netizen.github.io/product-images/K1a0001-bordo/07.jpg,https://oleks-netizen.github.io/product-images/K1a0001-bordo/08.jpg</t>
         </is>
       </c>
       <c r="C256" t="n">
@@ -4271,7 +4271,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/K1b837-green/1.jpg,https://oleks-netizen.github.io/product-images/K1b837-green/2.jpg,https://oleks-netizen.github.io/product-images/K1b837-green/9.jpg,https://oleks-netizen.github.io/product-images/K1b837-green/4.jpg,https://oleks-netizen.github.io/product-images/K1b837-green/5.jpg,https://oleks-netizen.github.io/product-images/K1b837-green/6.jpg,https://oleks-netizen.github.io/product-images/K1b837-green/7.jpg,https://oleks-netizen.github.io/product-images/K1b837-green/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/K1b837-green/01.jpg,https://oleks-netizen.github.io/product-images/K1b837-green/02.jpg,https://oleks-netizen.github.io/product-images/K1b837-green/09.jpg,https://oleks-netizen.github.io/product-images/K1b837-green/04.jpg,https://oleks-netizen.github.io/product-images/K1b837-green/05.jpg,https://oleks-netizen.github.io/product-images/K1b837-green/06.jpg,https://oleks-netizen.github.io/product-images/K1b837-green/07.jpg,https://oleks-netizen.github.io/product-images/K1b837-green/08.jpg</t>
         </is>
       </c>
       <c r="C257" t="n">
@@ -4286,7 +4286,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L346-020388/1.jpg,https://oleks-netizen.github.io/product-images/L346-020388/2.jpg,https://oleks-netizen.github.io/product-images/L346-020388/5.jpg,https://oleks-netizen.github.io/product-images/L346-020388/10.jpg,https://oleks-netizen.github.io/product-images/L346-020388/3.jpg,https://oleks-netizen.github.io/product-images/L346-020388/4.jpg,https://oleks-netizen.github.io/product-images/L346-020388/7.jpg,https://oleks-netizen.github.io/product-images/L346-020388/8.jpg,https://oleks-netizen.github.io/product-images/L346-020388/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L346-020388/01.jpg,https://oleks-netizen.github.io/product-images/L346-020388/02.jpg,https://oleks-netizen.github.io/product-images/L346-020388/05.jpg,https://oleks-netizen.github.io/product-images/L346-020388/10.jpg,https://oleks-netizen.github.io/product-images/L346-020388/03.jpg,https://oleks-netizen.github.io/product-images/L346-020388/04.jpg,https://oleks-netizen.github.io/product-images/L346-020388/07.jpg,https://oleks-netizen.github.io/product-images/L346-020388/08.jpg,https://oleks-netizen.github.io/product-images/L346-020388/09.jpg</t>
         </is>
       </c>
       <c r="C258" t="n">
@@ -4301,7 +4301,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L501-040010/1.jpg,https://oleks-netizen.github.io/product-images/L501-040010/2.jpg,https://oleks-netizen.github.io/product-images/L501-040010/9.jpg,https://oleks-netizen.github.io/product-images/L501-040010/4.jpg,https://oleks-netizen.github.io/product-images/L501-040010/5.jpg,https://oleks-netizen.github.io/product-images/L501-040010/6.jpg,https://oleks-netizen.github.io/product-images/L501-040010/7.jpg,https://oleks-netizen.github.io/product-images/L501-040010/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L501-040010/01.jpg,https://oleks-netizen.github.io/product-images/L501-040010/02.jpg,https://oleks-netizen.github.io/product-images/L501-040010/09.jpg,https://oleks-netizen.github.io/product-images/L501-040010/04.jpg,https://oleks-netizen.github.io/product-images/L501-040010/05.jpg,https://oleks-netizen.github.io/product-images/L501-040010/06.jpg,https://oleks-netizen.github.io/product-images/L501-040010/07.jpg,https://oleks-netizen.github.io/product-images/L501-040010/08.jpg</t>
         </is>
       </c>
       <c r="C259" t="n">
@@ -4316,7 +4316,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L754-028148/10.jpg,https://oleks-netizen.github.io/product-images/L754-028148/11.jpg,https://oleks-netizen.github.io/product-images/L754-028148/12.jpg,https://oleks-netizen.github.io/product-images/L754-028148/1.jpg,https://oleks-netizen.github.io/product-images/L754-028148/2.jpg,https://oleks-netizen.github.io/product-images/L754-028148/3.jpg,https://oleks-netizen.github.io/product-images/L754-028148/4.jpg,https://oleks-netizen.github.io/product-images/L754-028148/5.jpg,https://oleks-netizen.github.io/product-images/L754-028148/6.jpg,https://oleks-netizen.github.io/product-images/L754-028148/7.jpg,https://oleks-netizen.github.io/product-images/L754-028148/8.jpg,https://oleks-netizen.github.io/product-images/L754-028148/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L754-028148/10.jpg,https://oleks-netizen.github.io/product-images/L754-028148/11.jpg,https://oleks-netizen.github.io/product-images/L754-028148/12.jpg,https://oleks-netizen.github.io/product-images/L754-028148/01.jpg,https://oleks-netizen.github.io/product-images/L754-028148/02.jpg,https://oleks-netizen.github.io/product-images/L754-028148/03.jpg,https://oleks-netizen.github.io/product-images/L754-028148/04.jpg,https://oleks-netizen.github.io/product-images/L754-028148/05.jpg,https://oleks-netizen.github.io/product-images/L754-028148/06.jpg,https://oleks-netizen.github.io/product-images/L754-028148/07.jpg,https://oleks-netizen.github.io/product-images/L754-028148/08.jpg,https://oleks-netizen.github.io/product-images/L754-028148/09.jpg</t>
         </is>
       </c>
       <c r="C260" t="n">
@@ -4331,7 +4331,7 @@
       </c>
       <c r="B261" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L891-037263/1.jpg,https://oleks-netizen.github.io/product-images/L891-037263/2.jpg,https://oleks-netizen.github.io/product-images/L891-037263/5.jpg,https://oleks-netizen.github.io/product-images/L891-037263/14.jpg,https://oleks-netizen.github.io/product-images/L891-037263/10.jpg,https://oleks-netizen.github.io/product-images/L891-037263/11.jpg,https://oleks-netizen.github.io/product-images/L891-037263/12.jpg,https://oleks-netizen.github.io/product-images/L891-037263/13.jpg,https://oleks-netizen.github.io/product-images/L891-037263/4.jpg,https://oleks-netizen.github.io/product-images/L891-037263/6.jpg,https://oleks-netizen.github.io/product-images/L891-037263/7.jpg,https://oleks-netizen.github.io/product-images/L891-037263/8.jpg,https://oleks-netizen.github.io/product-images/L891-037263/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L891-037263/01.jpg,https://oleks-netizen.github.io/product-images/L891-037263/02.jpg,https://oleks-netizen.github.io/product-images/L891-037263/05.jpg,https://oleks-netizen.github.io/product-images/L891-037263/14.jpg,https://oleks-netizen.github.io/product-images/L891-037263/10.jpg,https://oleks-netizen.github.io/product-images/L891-037263/11.jpg,https://oleks-netizen.github.io/product-images/L891-037263/12.jpg,https://oleks-netizen.github.io/product-images/L891-037263/13.jpg,https://oleks-netizen.github.io/product-images/L891-037263/04.jpg,https://oleks-netizen.github.io/product-images/L891-037263/06.jpg,https://oleks-netizen.github.io/product-images/L891-037263/07.jpg,https://oleks-netizen.github.io/product-images/L891-037263/08.jpg,https://oleks-netizen.github.io/product-images/L891-037263/09.jpg</t>
         </is>
       </c>
       <c r="C261" t="n">
@@ -4346,7 +4346,7 @@
       </c>
       <c r="B262" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L902-038857/1.jpg,https://oleks-netizen.github.io/product-images/L902-038857/2.jpg,https://oleks-netizen.github.io/product-images/L902-038857/9.jpg,https://oleks-netizen.github.io/product-images/L902-038857/4.jpg,https://oleks-netizen.github.io/product-images/L902-038857/5.jpg,https://oleks-netizen.github.io/product-images/L902-038857/6.jpg,https://oleks-netizen.github.io/product-images/L902-038857/7.jpg,https://oleks-netizen.github.io/product-images/L902-038857/8.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L902-038857/01.jpg,https://oleks-netizen.github.io/product-images/L902-038857/02.jpg,https://oleks-netizen.github.io/product-images/L902-038857/09.jpg,https://oleks-netizen.github.io/product-images/L902-038857/04.jpg,https://oleks-netizen.github.io/product-images/L902-038857/05.jpg,https://oleks-netizen.github.io/product-images/L902-038857/06.jpg,https://oleks-netizen.github.io/product-images/L902-038857/07.jpg,https://oleks-netizen.github.io/product-images/L902-038857/08.jpg</t>
         </is>
       </c>
       <c r="C262" t="n">
@@ -4361,7 +4361,7 @@
       </c>
       <c r="B263" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L908-039595/1.jpg,https://oleks-netizen.github.io/product-images/L908-039595/2.jpg,https://oleks-netizen.github.io/product-images/L908-039595/6.jpg,https://oleks-netizen.github.io/product-images/L908-039595/16.jpg,https://oleks-netizen.github.io/product-images/L908-039595/10.jpg,https://oleks-netizen.github.io/product-images/L908-039595/11.jpg,https://oleks-netizen.github.io/product-images/L908-039595/12.jpg,https://oleks-netizen.github.io/product-images/L908-039595/13.jpg,https://oleks-netizen.github.io/product-images/L908-039595/14.jpg,https://oleks-netizen.github.io/product-images/L908-039595/15.jpg,https://oleks-netizen.github.io/product-images/L908-039595/3.jpg,https://oleks-netizen.github.io/product-images/L908-039595/4.jpg,https://oleks-netizen.github.io/product-images/L908-039595/5.jpg,https://oleks-netizen.github.io/product-images/L908-039595/8.jpg,https://oleks-netizen.github.io/product-images/L908-039595/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L908-039595/01.jpg,https://oleks-netizen.github.io/product-images/L908-039595/02.jpg,https://oleks-netizen.github.io/product-images/L908-039595/06.jpg,https://oleks-netizen.github.io/product-images/L908-039595/16.jpg,https://oleks-netizen.github.io/product-images/L908-039595/10.jpg,https://oleks-netizen.github.io/product-images/L908-039595/11.jpg,https://oleks-netizen.github.io/product-images/L908-039595/12.jpg,https://oleks-netizen.github.io/product-images/L908-039595/13.jpg,https://oleks-netizen.github.io/product-images/L908-039595/14.jpg,https://oleks-netizen.github.io/product-images/L908-039595/15.jpg,https://oleks-netizen.github.io/product-images/L908-039595/03.jpg,https://oleks-netizen.github.io/product-images/L908-039595/04.jpg,https://oleks-netizen.github.io/product-images/L908-039595/05.jpg,https://oleks-netizen.github.io/product-images/L908-039595/08.jpg,https://oleks-netizen.github.io/product-images/L908-039595/09.jpg</t>
         </is>
       </c>
       <c r="C263" t="n">
@@ -4376,7 +4376,7 @@
       </c>
       <c r="B264" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/L926-039984/1.jpg,https://oleks-netizen.github.io/product-images/L926-039984/2.jpg,https://oleks-netizen.github.io/product-images/L926-039984/10.jpg,https://oleks-netizen.github.io/product-images/L926-039984/4.jpg,https://oleks-netizen.github.io/product-images/L926-039984/5.jpg,https://oleks-netizen.github.io/product-images/L926-039984/6.jpg,https://oleks-netizen.github.io/product-images/L926-039984/7.jpg,https://oleks-netizen.github.io/product-images/L926-039984/8.jpg,https://oleks-netizen.github.io/product-images/L926-039984/9.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/L926-039984/01.jpg,https://oleks-netizen.github.io/product-images/L926-039984/02.jpg,https://oleks-netizen.github.io/product-images/L926-039984/10.jpg,https://oleks-netizen.github.io/product-images/L926-039984/04.jpg,https://oleks-netizen.github.io/product-images/L926-039984/05.jpg,https://oleks-netizen.github.io/product-images/L926-039984/06.jpg,https://oleks-netizen.github.io/product-images/L926-039984/07.jpg,https://oleks-netizen.github.io/product-images/L926-039984/08.jpg,https://oleks-netizen.github.io/product-images/L926-039984/09.jpg</t>
         </is>
       </c>
       <c r="C264" t="n">
@@ -4391,7 +4391,7 @@
       </c>
       <c r="B265" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/V1115GX19-brown/1.jpg,https://oleks-netizen.github.io/product-images/V1115GX19-brown/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/V1115GX19-brown/01.jpg,https://oleks-netizen.github.io/product-images/V1115GX19-brown/02.jpg</t>
         </is>
       </c>
       <c r="C265" t="n">
@@ -4406,7 +4406,7 @@
       </c>
       <c r="B266" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/V1125GX11-black/1.jpg,https://oleks-netizen.github.io/product-images/V1125GX11-black/2.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/V1125GX11-black/01.jpg,https://oleks-netizen.github.io/product-images/V1125GX11-black/02.jpg</t>
         </is>
       </c>
       <c r="C266" t="n">
@@ -4421,7 +4421,7 @@
       </c>
       <c r="B267" t="inlineStr">
         <is>
-          <t>https://oleks-netizen.github.io/product-images/V1WLT07-yellow/1.jpg,https://oleks-netizen.github.io/product-images/V1WLT07-yellow/2.jpg,https://oleks-netizen.github.io/product-images/V1WLT07-yellow/3.jpg,https://oleks-netizen.github.io/product-images/V1WLT07-yellow/4.jpg,https://oleks-netizen.github.io/product-images/V1WLT07-yellow/5.jpg</t>
+          <t>https://oleks-netizen.github.io/product-images/V1WLT07-yellow/01.jpg,https://oleks-netizen.github.io/product-images/V1WLT07-yellow/02.jpg,https://oleks-netizen.github.io/product-images/V1WLT07-yellow/03.jpg,https://oleks-netizen.github.io/product-images/V1WLT07-yellow/04.jpg,https://oleks-netizen.github.io/product-images/V1WLT07-yellow/05.jpg</t>
         </is>
       </c>
       <c r="C267" t="n">

</xml_diff>